<commit_message>
up tc huy dk
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -5,20 +5,21 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University_IT\Tạm\Kiểm Thử Phần Mềm\event-manager-javafx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University_IT\Tam\KiemThuPhanMem\event-manager-javafx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3202CD2-F17F-49B4-AB8D-6E90F124D35D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8A899B-20BA-492F-8BCA-5D07D47F73C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="821" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="97" r:id="rId1"/>
     <sheet name="Samples" sheetId="122" r:id="rId2"/>
-    <sheet name="Test Report" sheetId="107" r:id="rId3"/>
+    <sheet name="Samples2" sheetId="123" r:id="rId3"/>
+    <sheet name="Test Report" sheetId="107" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="Access">[1]Validation!$E$2:$E$223</definedName>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="168">
   <si>
     <t>TC1</t>
   </si>
@@ -665,6 +666,40 @@
   </si>
   <si>
     <t>1.2</t>
+  </si>
+  <si>
+    <t>Đăng ký tham gia</t>
+  </si>
+  <si>
+    <t>1. Đăng ký tham gia sự kiện</t>
+  </si>
+  <si>
+    <t>2. Hủy đăng ký</t>
+  </si>
+  <si>
+    <t>Kiểm tra hủy đăng ký trong thời gian cho phép</t>
+  </si>
+  <si>
+    <t>Kiểm tra hủy đăng ký trong thời gian không cho phép</t>
+  </si>
+  <si>
+    <t>1: User đăng nhập thành công vào hệ thống
+2: User đăng ký một sự kiện bất kỳ
+3: Sau đó truy cập vào trang Sự kiện đã đăng ký
+4: Chọn sự kiện và nhấn Hủy đăng ký(trong vòng 48h)
+5: Xác nhận hủy đăng ký
+6: Hiển thị thông báo hủy đăng ký sự kiện thành công(sự kiện đã được xóa khỏi danh sách sự kiện đã đăng ký)</t>
+  </si>
+  <si>
+    <t>1: User đăng nhập thành công vào hệ thống
+2: User đăng ký một sự kiện bất kỳ
+3: Sau đó truy cập vào trang Sự kiện đã đăng ký
+4: Chọn sự kiện và nhấn Hủy đăng ký(sau 48h)
+5: Xác nhận hủy đăng ký
+6: Hiển thị thông báo lỗi không thể hủy đăng ký sự kiện này</t>
+  </si>
+  <si>
+    <t>1.3</t>
   </si>
 </sst>
 </file>
@@ -857,7 +892,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -1350,6 +1385,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1357,7 +1405,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1583,9 +1631,6 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1661,6 +1706,21 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1673,6 +1733,42 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1691,12 +1787,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1706,9 +1796,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1721,9 +1808,6 @@
     <xf numFmtId="0" fontId="15" fillId="5" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1731,49 +1815,26 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2097,8 +2158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H72"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView showGridLines="0" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -2107,8 +2168,8 @@
     <col min="2" max="2" width="14.125" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.25" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.5" style="105" customWidth="1"/>
-    <col min="6" max="6" width="23.875" style="112" customWidth="1"/>
+    <col min="5" max="5" width="32.5" style="104" customWidth="1"/>
+    <col min="6" max="6" width="23.875" style="111" customWidth="1"/>
     <col min="7" max="7" width="20.5" style="1" customWidth="1"/>
     <col min="8" max="8" width="26.625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
@@ -2121,8 +2182,8 @@
       </c>
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="111"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="110"/>
       <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:8">
@@ -2134,8 +2195,8 @@
         <v>1</v>
       </c>
       <c r="D3" s="28"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="111"/>
+      <c r="E3" s="103"/>
+      <c r="F3" s="110"/>
       <c r="G3" s="25"/>
     </row>
     <row r="4" spans="1:8">
@@ -2147,8 +2208,8 @@
         <v>45731</v>
       </c>
       <c r="D4" s="11"/>
-      <c r="E4" s="104"/>
-      <c r="F4" s="111"/>
+      <c r="E4" s="103"/>
+      <c r="F4" s="110"/>
       <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:8" ht="15" thickBot="1">
@@ -2156,8 +2217,8 @@
       <c r="B5" s="27"/>
       <c r="C5" s="28"/>
       <c r="D5" s="28"/>
-      <c r="E5" s="104"/>
-      <c r="F5" s="111"/>
+      <c r="E5" s="103"/>
+      <c r="F5" s="110"/>
       <c r="G5" s="25"/>
     </row>
     <row r="6" spans="1:8" ht="14.25" customHeight="1" thickBot="1">
@@ -2165,12 +2226,12 @@
       <c r="B6" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="115" t="s">
+      <c r="C6" s="114" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="115"/>
-      <c r="E6" s="116"/>
-      <c r="F6" s="111"/>
+      <c r="D6" s="114"/>
+      <c r="E6" s="115"/>
+      <c r="F6" s="110"/>
       <c r="G6" s="25"/>
     </row>
     <row r="7" spans="1:8">
@@ -2178,12 +2239,12 @@
       <c r="B7" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="115" t="s">
+      <c r="C7" s="114" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="115"/>
-      <c r="E7" s="116"/>
-      <c r="F7" s="111"/>
+      <c r="D7" s="114"/>
+      <c r="E7" s="115"/>
+      <c r="F7" s="110"/>
       <c r="G7" s="25"/>
     </row>
     <row r="8" spans="1:8">
@@ -2191,8 +2252,8 @@
       <c r="B8" s="27"/>
       <c r="C8" s="25"/>
       <c r="D8" s="25"/>
-      <c r="E8" s="104"/>
-      <c r="F8" s="111"/>
+      <c r="E8" s="103"/>
+      <c r="F8" s="110"/>
       <c r="G8" s="25"/>
     </row>
     <row r="9" spans="1:8">
@@ -2201,7 +2262,7 @@
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
       <c r="E9" s="64"/>
-      <c r="F9" s="111"/>
+      <c r="F9" s="110"/>
       <c r="G9" s="25"/>
     </row>
     <row r="10" spans="1:8">
@@ -2240,10 +2301,10 @@
         <v>40</v>
       </c>
       <c r="D12" s="40"/>
-      <c r="E12" s="103" t="s">
+      <c r="E12" s="102" t="s">
         <v>69</v>
       </c>
-      <c r="F12" s="113" t="s">
+      <c r="F12" s="112" t="s">
         <v>44</v>
       </c>
       <c r="G12" s="40"/>
@@ -2257,10 +2318,10 @@
         <v>40</v>
       </c>
       <c r="D13" s="38"/>
-      <c r="E13" s="103" t="s">
+      <c r="E13" s="102" t="s">
         <v>68</v>
       </c>
-      <c r="F13" s="113" t="s">
+      <c r="F13" s="112" t="s">
         <v>44</v>
       </c>
       <c r="G13" s="40"/>
@@ -2274,10 +2335,10 @@
         <v>40</v>
       </c>
       <c r="D14" s="40"/>
-      <c r="E14" s="103" t="s">
+      <c r="E14" s="102" t="s">
         <v>153</v>
       </c>
-      <c r="F14" s="113" t="s">
+      <c r="F14" s="112" t="s">
         <v>44</v>
       </c>
       <c r="G14" s="40"/>
@@ -2291,10 +2352,10 @@
         <v>40</v>
       </c>
       <c r="D15" s="40"/>
-      <c r="E15" s="103" t="s">
+      <c r="E15" s="102" t="s">
         <v>115</v>
       </c>
-      <c r="F15" s="113" t="s">
+      <c r="F15" s="112" t="s">
         <v>44</v>
       </c>
       <c r="G15" s="40"/>
@@ -2308,10 +2369,10 @@
         <v>40</v>
       </c>
       <c r="D16" s="40"/>
-      <c r="E16" s="103" t="s">
+      <c r="E16" s="102" t="s">
         <v>116</v>
       </c>
-      <c r="F16" s="113" t="s">
+      <c r="F16" s="112" t="s">
         <v>44</v>
       </c>
       <c r="G16" s="40"/>
@@ -2325,10 +2386,10 @@
         <v>40</v>
       </c>
       <c r="D17" s="40"/>
-      <c r="E17" s="103" t="s">
+      <c r="E17" s="102" t="s">
         <v>117</v>
       </c>
-      <c r="F17" s="113" t="s">
+      <c r="F17" s="112" t="s">
         <v>44</v>
       </c>
       <c r="G17" s="40"/>
@@ -2342,10 +2403,10 @@
         <v>40</v>
       </c>
       <c r="D18" s="40"/>
-      <c r="E18" s="103" t="s">
+      <c r="E18" s="102" t="s">
         <v>118</v>
       </c>
-      <c r="F18" s="113" t="s">
+      <c r="F18" s="112" t="s">
         <v>44</v>
       </c>
       <c r="G18" s="40"/>
@@ -2359,10 +2420,10 @@
         <v>40</v>
       </c>
       <c r="D19" s="40"/>
-      <c r="E19" s="103" t="s">
+      <c r="E19" s="102" t="s">
         <v>62</v>
       </c>
-      <c r="F19" s="113" t="s">
+      <c r="F19" s="112" t="s">
         <v>44</v>
       </c>
       <c r="G19" s="40"/>
@@ -2376,10 +2437,10 @@
         <v>40</v>
       </c>
       <c r="D20" s="40"/>
-      <c r="E20" s="103" t="s">
+      <c r="E20" s="102" t="s">
         <v>119</v>
       </c>
-      <c r="F20" s="113" t="s">
+      <c r="F20" s="112" t="s">
         <v>44</v>
       </c>
       <c r="G20" s="40"/>
@@ -2393,10 +2454,10 @@
         <v>40</v>
       </c>
       <c r="D21" s="40"/>
-      <c r="E21" s="103" t="s">
+      <c r="E21" s="102" t="s">
         <v>63</v>
       </c>
-      <c r="F21" s="113" t="s">
+      <c r="F21" s="112" t="s">
         <v>44</v>
       </c>
       <c r="G21" s="40"/>
@@ -2410,10 +2471,10 @@
         <v>40</v>
       </c>
       <c r="D22" s="40"/>
-      <c r="E22" s="103" t="s">
+      <c r="E22" s="102" t="s">
         <v>64</v>
       </c>
-      <c r="F22" s="113" t="s">
+      <c r="F22" s="112" t="s">
         <v>44</v>
       </c>
       <c r="G22" s="40"/>
@@ -2427,10 +2488,10 @@
         <v>40</v>
       </c>
       <c r="D23" s="40"/>
-      <c r="E23" s="103" t="s">
+      <c r="E23" s="102" t="s">
         <v>65</v>
       </c>
-      <c r="F23" s="113" t="s">
+      <c r="F23" s="112" t="s">
         <v>44</v>
       </c>
       <c r="G23" s="40"/>
@@ -2444,10 +2505,10 @@
         <v>40</v>
       </c>
       <c r="D24" s="40"/>
-      <c r="E24" s="103" t="s">
+      <c r="E24" s="102" t="s">
         <v>66</v>
       </c>
-      <c r="F24" s="113" t="s">
+      <c r="F24" s="112" t="s">
         <v>44</v>
       </c>
       <c r="G24" s="40"/>
@@ -2460,15 +2521,15 @@
       <c r="C25" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="102"/>
-      <c r="E25" s="103" t="s">
+      <c r="D25" s="101"/>
+      <c r="E25" s="102" t="s">
         <v>103</v>
       </c>
-      <c r="F25" s="113" t="s">
+      <c r="F25" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="G25" s="102"/>
-      <c r="H25" s="108"/>
+      <c r="G25" s="101"/>
+      <c r="H25" s="107"/>
     </row>
     <row r="26" spans="2:8" s="34" customFormat="1" ht="38.25">
       <c r="B26" s="36">
@@ -2477,15 +2538,15 @@
       <c r="C26" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="102"/>
-      <c r="E26" s="107" t="s">
+      <c r="D26" s="101"/>
+      <c r="E26" s="106" t="s">
         <v>67</v>
       </c>
-      <c r="F26" s="113" t="s">
+      <c r="F26" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="G26" s="102"/>
-      <c r="H26" s="108"/>
+      <c r="G26" s="101"/>
+      <c r="H26" s="107"/>
     </row>
     <row r="27" spans="2:8" s="34" customFormat="1" ht="25.5">
       <c r="B27" s="36">
@@ -2494,15 +2555,15 @@
       <c r="C27" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="102"/>
-      <c r="E27" s="107" t="s">
+      <c r="D27" s="101"/>
+      <c r="E27" s="106" t="s">
         <v>107</v>
       </c>
-      <c r="F27" s="113" t="s">
+      <c r="F27" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="G27" s="102"/>
-      <c r="H27" s="108"/>
+      <c r="G27" s="101"/>
+      <c r="H27" s="107"/>
     </row>
     <row r="28" spans="2:8" s="34" customFormat="1">
       <c r="B28" s="36">
@@ -2511,15 +2572,15 @@
       <c r="C28" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="102"/>
-      <c r="E28" s="107" t="s">
+      <c r="D28" s="101"/>
+      <c r="E28" s="106" t="s">
         <v>108</v>
       </c>
-      <c r="F28" s="113" t="s">
+      <c r="F28" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="G28" s="102"/>
-      <c r="H28" s="108"/>
+      <c r="G28" s="101"/>
+      <c r="H28" s="107"/>
     </row>
     <row r="29" spans="2:8" s="34" customFormat="1">
       <c r="B29" s="36">
@@ -2528,15 +2589,15 @@
       <c r="C29" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="102"/>
-      <c r="E29" s="107" t="s">
+      <c r="D29" s="101"/>
+      <c r="E29" s="106" t="s">
         <v>109</v>
       </c>
-      <c r="F29" s="113" t="s">
+      <c r="F29" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="G29" s="102"/>
-      <c r="H29" s="108"/>
+      <c r="G29" s="101"/>
+      <c r="H29" s="107"/>
     </row>
     <row r="30" spans="2:8" s="34" customFormat="1">
       <c r="B30" s="36">
@@ -2545,15 +2606,15 @@
       <c r="C30" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="102"/>
-      <c r="E30" s="107" t="s">
+      <c r="D30" s="101"/>
+      <c r="E30" s="106" t="s">
         <v>110</v>
       </c>
-      <c r="F30" s="113" t="s">
+      <c r="F30" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="G30" s="102"/>
-      <c r="H30" s="108"/>
+      <c r="G30" s="101"/>
+      <c r="H30" s="107"/>
     </row>
     <row r="31" spans="2:8" s="34" customFormat="1" ht="25.5">
       <c r="B31" s="36">
@@ -2562,15 +2623,15 @@
       <c r="C31" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="D31" s="102"/>
-      <c r="E31" s="107" t="s">
+      <c r="D31" s="101"/>
+      <c r="E31" s="106" t="s">
         <v>111</v>
       </c>
-      <c r="F31" s="113" t="s">
+      <c r="F31" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="G31" s="102"/>
-      <c r="H31" s="108"/>
+      <c r="G31" s="101"/>
+      <c r="H31" s="107"/>
     </row>
     <row r="32" spans="2:8" s="34" customFormat="1" ht="38.25">
       <c r="B32" s="36">
@@ -2579,15 +2640,15 @@
       <c r="C32" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="D32" s="102"/>
-      <c r="E32" s="107" t="s">
+      <c r="D32" s="101"/>
+      <c r="E32" s="106" t="s">
         <v>112</v>
       </c>
-      <c r="F32" s="113" t="s">
+      <c r="F32" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="G32" s="102"/>
-      <c r="H32" s="108"/>
+      <c r="G32" s="101"/>
+      <c r="H32" s="107"/>
     </row>
     <row r="33" spans="2:8" s="34" customFormat="1" ht="25.5">
       <c r="B33" s="36">
@@ -2596,15 +2657,15 @@
       <c r="C33" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="102"/>
-      <c r="E33" s="107" t="s">
+      <c r="D33" s="101"/>
+      <c r="E33" s="106" t="s">
         <v>113</v>
       </c>
-      <c r="F33" s="113" t="s">
+      <c r="F33" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="G33" s="102"/>
-      <c r="H33" s="108"/>
+      <c r="G33" s="101"/>
+      <c r="H33" s="107"/>
     </row>
     <row r="34" spans="2:8" s="34" customFormat="1">
       <c r="B34" s="36">
@@ -2613,15 +2674,15 @@
       <c r="C34" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="D34" s="102"/>
-      <c r="E34" s="107" t="s">
+      <c r="D34" s="101"/>
+      <c r="E34" s="106" t="s">
         <v>114</v>
       </c>
-      <c r="F34" s="113" t="s">
+      <c r="F34" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="102"/>
-      <c r="H34" s="108"/>
+      <c r="G34" s="101"/>
+      <c r="H34" s="107"/>
     </row>
     <row r="35" spans="2:8" s="34" customFormat="1" ht="25.5">
       <c r="B35" s="36">
@@ -2630,15 +2691,15 @@
       <c r="C35" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="D35" s="102"/>
-      <c r="E35" s="107" t="s">
+      <c r="D35" s="101"/>
+      <c r="E35" s="106" t="s">
         <v>137</v>
       </c>
-      <c r="F35" s="113" t="s">
+      <c r="F35" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="G35" s="102"/>
-      <c r="H35" s="108"/>
+      <c r="G35" s="101"/>
+      <c r="H35" s="107"/>
     </row>
     <row r="36" spans="2:8" s="34" customFormat="1">
       <c r="B36" s="36">
@@ -2647,15 +2708,15 @@
       <c r="C36" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="D36" s="102"/>
-      <c r="E36" s="107" t="s">
+      <c r="D36" s="101"/>
+      <c r="E36" s="106" t="s">
         <v>138</v>
       </c>
-      <c r="F36" s="113" t="s">
+      <c r="F36" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="G36" s="102"/>
-      <c r="H36" s="108"/>
+      <c r="G36" s="101"/>
+      <c r="H36" s="107"/>
     </row>
     <row r="37" spans="2:8" s="34" customFormat="1" ht="25.5">
       <c r="B37" s="36">
@@ -2664,15 +2725,15 @@
       <c r="C37" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="D37" s="102"/>
-      <c r="E37" s="107" t="s">
+      <c r="D37" s="101"/>
+      <c r="E37" s="106" t="s">
         <v>139</v>
       </c>
-      <c r="F37" s="113" t="s">
+      <c r="F37" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="G37" s="102"/>
-      <c r="H37" s="108"/>
+      <c r="G37" s="101"/>
+      <c r="H37" s="107"/>
     </row>
     <row r="38" spans="2:8" s="34" customFormat="1" ht="25.5">
       <c r="B38" s="36">
@@ -2681,15 +2742,15 @@
       <c r="C38" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="D38" s="102"/>
-      <c r="E38" s="107" t="s">
+      <c r="D38" s="101"/>
+      <c r="E38" s="106" t="s">
         <v>140</v>
       </c>
-      <c r="F38" s="113" t="s">
+      <c r="F38" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="G38" s="102"/>
-      <c r="H38" s="108"/>
+      <c r="G38" s="101"/>
+      <c r="H38" s="107"/>
     </row>
     <row r="39" spans="2:8" s="34" customFormat="1" ht="25.5">
       <c r="B39" s="36">
@@ -2698,15 +2759,15 @@
       <c r="C39" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="D39" s="102"/>
-      <c r="E39" s="107" t="s">
+      <c r="D39" s="101"/>
+      <c r="E39" s="106" t="s">
         <v>141</v>
       </c>
-      <c r="F39" s="113" t="s">
+      <c r="F39" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="G39" s="102"/>
-      <c r="H39" s="108"/>
+      <c r="G39" s="101"/>
+      <c r="H39" s="107"/>
     </row>
     <row r="40" spans="2:8" s="34" customFormat="1" ht="25.5">
       <c r="B40" s="36">
@@ -2715,15 +2776,15 @@
       <c r="C40" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="D40" s="102"/>
-      <c r="E40" s="107" t="s">
+      <c r="D40" s="101"/>
+      <c r="E40" s="106" t="s">
         <v>142</v>
       </c>
-      <c r="F40" s="113" t="s">
+      <c r="F40" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="G40" s="102"/>
-      <c r="H40" s="108"/>
+      <c r="G40" s="101"/>
+      <c r="H40" s="107"/>
     </row>
     <row r="41" spans="2:8" s="34" customFormat="1" ht="25.5">
       <c r="B41" s="36">
@@ -2732,15 +2793,15 @@
       <c r="C41" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="D41" s="102"/>
-      <c r="E41" s="107" t="s">
+      <c r="D41" s="101"/>
+      <c r="E41" s="106" t="s">
         <v>135</v>
       </c>
-      <c r="F41" s="113" t="s">
+      <c r="F41" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="G41" s="102"/>
-      <c r="H41" s="108"/>
+      <c r="G41" s="101"/>
+      <c r="H41" s="107"/>
     </row>
     <row r="42" spans="2:8" s="34" customFormat="1" ht="25.5">
       <c r="B42" s="36">
@@ -2749,15 +2810,15 @@
       <c r="C42" s="37" t="s">
         <v>159</v>
       </c>
-      <c r="D42" s="102"/>
-      <c r="E42" s="107" t="s">
+      <c r="D42" s="101"/>
+      <c r="E42" s="106" t="s">
         <v>158</v>
       </c>
-      <c r="F42" s="113" t="s">
+      <c r="F42" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="G42" s="102"/>
-      <c r="H42" s="108"/>
+      <c r="G42" s="101"/>
+      <c r="H42" s="107"/>
     </row>
     <row r="43" spans="2:8" s="34" customFormat="1" ht="25.5">
       <c r="B43" s="36">
@@ -2766,15 +2827,15 @@
       <c r="C43" s="37" t="s">
         <v>159</v>
       </c>
-      <c r="D43" s="102"/>
-      <c r="E43" s="107" t="s">
+      <c r="D43" s="101"/>
+      <c r="E43" s="106" t="s">
         <v>154</v>
       </c>
-      <c r="F43" s="113" t="s">
+      <c r="F43" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="G43" s="102"/>
-      <c r="H43" s="108"/>
+      <c r="G43" s="101"/>
+      <c r="H43" s="107"/>
     </row>
     <row r="44" spans="2:8" s="34" customFormat="1">
       <c r="B44" s="36">
@@ -2783,15 +2844,15 @@
       <c r="C44" s="37" t="s">
         <v>159</v>
       </c>
-      <c r="D44" s="102"/>
-      <c r="E44" s="107" t="s">
+      <c r="D44" s="101"/>
+      <c r="E44" s="106" t="s">
         <v>155</v>
       </c>
-      <c r="F44" s="113" t="s">
+      <c r="F44" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="G44" s="102"/>
-      <c r="H44" s="108"/>
+      <c r="G44" s="101"/>
+      <c r="H44" s="107"/>
     </row>
     <row r="45" spans="2:8" s="34" customFormat="1">
       <c r="B45" s="36">
@@ -2800,15 +2861,15 @@
       <c r="C45" s="37" t="s">
         <v>159</v>
       </c>
-      <c r="D45" s="102"/>
-      <c r="E45" s="107" t="s">
+      <c r="D45" s="101"/>
+      <c r="E45" s="106" t="s">
         <v>156</v>
       </c>
-      <c r="F45" s="113" t="s">
+      <c r="F45" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="G45" s="102"/>
-      <c r="H45" s="108"/>
+      <c r="G45" s="101"/>
+      <c r="H45" s="107"/>
     </row>
     <row r="46" spans="2:8" s="34" customFormat="1">
       <c r="B46" s="36">
@@ -2817,247 +2878,263 @@
       <c r="C46" s="37" t="s">
         <v>159</v>
       </c>
-      <c r="D46" s="102"/>
-      <c r="E46" s="107" t="s">
+      <c r="D46" s="101"/>
+      <c r="E46" s="106" t="s">
         <v>157</v>
       </c>
-      <c r="F46" s="113" t="s">
+      <c r="F46" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="G46" s="102"/>
-      <c r="H46" s="108"/>
-    </row>
-    <row r="47" spans="2:8" s="34" customFormat="1">
-      <c r="B47" s="36"/>
-      <c r="C47" s="37"/>
-      <c r="D47" s="102"/>
-      <c r="E47" s="107"/>
-      <c r="F47" s="113"/>
-      <c r="G47" s="102"/>
-      <c r="H47" s="108"/>
-    </row>
-    <row r="48" spans="2:8" s="34" customFormat="1">
-      <c r="B48" s="36"/>
-      <c r="C48" s="37"/>
-      <c r="D48" s="102"/>
-      <c r="E48" s="107"/>
-      <c r="F48" s="113"/>
-      <c r="G48" s="102"/>
-      <c r="H48" s="108"/>
+      <c r="G46" s="101"/>
+      <c r="H46" s="107"/>
+    </row>
+    <row r="47" spans="2:8" s="34" customFormat="1" ht="25.5">
+      <c r="B47" s="36">
+        <v>45746</v>
+      </c>
+      <c r="C47" s="37" t="s">
+        <v>167</v>
+      </c>
+      <c r="D47" s="101"/>
+      <c r="E47" s="106" t="s">
+        <v>163</v>
+      </c>
+      <c r="F47" s="112" t="s">
+        <v>44</v>
+      </c>
+      <c r="G47" s="101"/>
+      <c r="H47" s="107"/>
+    </row>
+    <row r="48" spans="2:8" s="34" customFormat="1" ht="25.5">
+      <c r="B48" s="36">
+        <v>45746</v>
+      </c>
+      <c r="C48" s="37" t="s">
+        <v>167</v>
+      </c>
+      <c r="D48" s="101"/>
+      <c r="E48" s="106" t="s">
+        <v>164</v>
+      </c>
+      <c r="F48" s="112" t="s">
+        <v>44</v>
+      </c>
+      <c r="G48" s="101"/>
+      <c r="H48" s="107"/>
     </row>
     <row r="49" spans="2:8" s="34" customFormat="1">
       <c r="B49" s="36"/>
       <c r="C49" s="37"/>
-      <c r="D49" s="102"/>
-      <c r="E49" s="107"/>
-      <c r="F49" s="113"/>
-      <c r="G49" s="102"/>
-      <c r="H49" s="108"/>
+      <c r="D49" s="101"/>
+      <c r="E49" s="106"/>
+      <c r="F49" s="112"/>
+      <c r="G49" s="101"/>
+      <c r="H49" s="107"/>
     </row>
     <row r="50" spans="2:8" s="34" customFormat="1">
       <c r="B50" s="36"/>
       <c r="C50" s="37"/>
-      <c r="D50" s="102"/>
-      <c r="E50" s="107"/>
-      <c r="F50" s="113"/>
-      <c r="G50" s="102"/>
-      <c r="H50" s="108"/>
+      <c r="D50" s="101"/>
+      <c r="E50" s="106"/>
+      <c r="F50" s="112"/>
+      <c r="G50" s="101"/>
+      <c r="H50" s="107"/>
     </row>
     <row r="51" spans="2:8" s="34" customFormat="1">
       <c r="B51" s="36"/>
       <c r="C51" s="37"/>
-      <c r="D51" s="102"/>
-      <c r="E51" s="107"/>
-      <c r="F51" s="113"/>
-      <c r="G51" s="102"/>
-      <c r="H51" s="108"/>
+      <c r="D51" s="101"/>
+      <c r="E51" s="106"/>
+      <c r="F51" s="112"/>
+      <c r="G51" s="101"/>
+      <c r="H51" s="107"/>
     </row>
     <row r="52" spans="2:8" s="34" customFormat="1">
       <c r="B52" s="36"/>
       <c r="C52" s="37"/>
-      <c r="D52" s="102"/>
-      <c r="E52" s="107"/>
-      <c r="F52" s="113"/>
-      <c r="G52" s="102"/>
-      <c r="H52" s="108"/>
+      <c r="D52" s="101"/>
+      <c r="E52" s="106"/>
+      <c r="F52" s="112"/>
+      <c r="G52" s="101"/>
+      <c r="H52" s="107"/>
     </row>
     <row r="53" spans="2:8" s="34" customFormat="1">
       <c r="B53" s="36"/>
       <c r="C53" s="37"/>
-      <c r="D53" s="102"/>
-      <c r="E53" s="107"/>
-      <c r="F53" s="113"/>
-      <c r="G53" s="102"/>
-      <c r="H53" s="108"/>
+      <c r="D53" s="101"/>
+      <c r="E53" s="106"/>
+      <c r="F53" s="112"/>
+      <c r="G53" s="101"/>
+      <c r="H53" s="107"/>
     </row>
     <row r="54" spans="2:8" s="34" customFormat="1">
       <c r="B54" s="36"/>
       <c r="C54" s="37"/>
-      <c r="D54" s="102"/>
-      <c r="E54" s="107"/>
-      <c r="F54" s="113"/>
-      <c r="G54" s="102"/>
-      <c r="H54" s="108"/>
+      <c r="D54" s="101"/>
+      <c r="E54" s="106"/>
+      <c r="F54" s="112"/>
+      <c r="G54" s="101"/>
+      <c r="H54" s="107"/>
     </row>
     <row r="55" spans="2:8" s="34" customFormat="1">
       <c r="B55" s="36"/>
       <c r="C55" s="37"/>
-      <c r="D55" s="102"/>
-      <c r="E55" s="107"/>
-      <c r="F55" s="113"/>
-      <c r="G55" s="102"/>
-      <c r="H55" s="108"/>
+      <c r="D55" s="101"/>
+      <c r="E55" s="106"/>
+      <c r="F55" s="112"/>
+      <c r="G55" s="101"/>
+      <c r="H55" s="107"/>
     </row>
     <row r="56" spans="2:8" s="34" customFormat="1">
       <c r="B56" s="36"/>
       <c r="C56" s="37"/>
-      <c r="D56" s="102"/>
-      <c r="E56" s="107"/>
-      <c r="F56" s="113"/>
-      <c r="G56" s="102"/>
-      <c r="H56" s="108"/>
+      <c r="D56" s="101"/>
+      <c r="E56" s="106"/>
+      <c r="F56" s="112"/>
+      <c r="G56" s="101"/>
+      <c r="H56" s="107"/>
     </row>
     <row r="57" spans="2:8" s="34" customFormat="1">
       <c r="B57" s="36"/>
       <c r="C57" s="37"/>
-      <c r="D57" s="102"/>
-      <c r="E57" s="107"/>
-      <c r="F57" s="113"/>
-      <c r="G57" s="102"/>
-      <c r="H57" s="108"/>
+      <c r="D57" s="101"/>
+      <c r="E57" s="106"/>
+      <c r="F57" s="112"/>
+      <c r="G57" s="101"/>
+      <c r="H57" s="107"/>
     </row>
     <row r="58" spans="2:8" s="34" customFormat="1">
       <c r="B58" s="36"/>
       <c r="C58" s="37"/>
-      <c r="D58" s="102"/>
-      <c r="E58" s="107"/>
-      <c r="F58" s="113"/>
-      <c r="G58" s="102"/>
-      <c r="H58" s="108"/>
+      <c r="D58" s="101"/>
+      <c r="E58" s="106"/>
+      <c r="F58" s="112"/>
+      <c r="G58" s="101"/>
+      <c r="H58" s="107"/>
     </row>
     <row r="59" spans="2:8" s="34" customFormat="1">
       <c r="B59" s="36"/>
       <c r="C59" s="37"/>
-      <c r="D59" s="102"/>
-      <c r="E59" s="107"/>
-      <c r="F59" s="113"/>
-      <c r="G59" s="102"/>
-      <c r="H59" s="108"/>
+      <c r="D59" s="101"/>
+      <c r="E59" s="106"/>
+      <c r="F59" s="112"/>
+      <c r="G59" s="101"/>
+      <c r="H59" s="107"/>
     </row>
     <row r="60" spans="2:8" s="34" customFormat="1">
       <c r="B60" s="36"/>
       <c r="C60" s="37"/>
-      <c r="D60" s="102"/>
-      <c r="E60" s="107"/>
-      <c r="F60" s="113"/>
-      <c r="G60" s="102"/>
-      <c r="H60" s="108"/>
+      <c r="D60" s="101"/>
+      <c r="E60" s="106"/>
+      <c r="F60" s="112"/>
+      <c r="G60" s="101"/>
+      <c r="H60" s="107"/>
     </row>
     <row r="61" spans="2:8" s="34" customFormat="1">
       <c r="B61" s="36"/>
       <c r="C61" s="37"/>
-      <c r="D61" s="102"/>
-      <c r="E61" s="107"/>
-      <c r="F61" s="113"/>
-      <c r="G61" s="102"/>
-      <c r="H61" s="108"/>
+      <c r="D61" s="101"/>
+      <c r="E61" s="106"/>
+      <c r="F61" s="112"/>
+      <c r="G61" s="101"/>
+      <c r="H61" s="107"/>
     </row>
     <row r="62" spans="2:8" s="34" customFormat="1">
       <c r="B62" s="36"/>
       <c r="C62" s="37"/>
-      <c r="D62" s="102"/>
-      <c r="E62" s="107"/>
-      <c r="F62" s="113"/>
-      <c r="G62" s="102"/>
-      <c r="H62" s="108"/>
+      <c r="D62" s="101"/>
+      <c r="E62" s="106"/>
+      <c r="F62" s="112"/>
+      <c r="G62" s="101"/>
+      <c r="H62" s="107"/>
     </row>
     <row r="63" spans="2:8" s="34" customFormat="1">
       <c r="B63" s="36"/>
       <c r="C63" s="37"/>
-      <c r="D63" s="102"/>
-      <c r="E63" s="107"/>
-      <c r="F63" s="113"/>
-      <c r="G63" s="102"/>
-      <c r="H63" s="108"/>
+      <c r="D63" s="101"/>
+      <c r="E63" s="106"/>
+      <c r="F63" s="112"/>
+      <c r="G63" s="101"/>
+      <c r="H63" s="107"/>
     </row>
     <row r="64" spans="2:8" s="34" customFormat="1">
       <c r="B64" s="36"/>
       <c r="C64" s="37"/>
-      <c r="D64" s="102"/>
-      <c r="E64" s="107"/>
-      <c r="F64" s="113"/>
-      <c r="G64" s="102"/>
-      <c r="H64" s="108"/>
+      <c r="D64" s="101"/>
+      <c r="E64" s="106"/>
+      <c r="F64" s="112"/>
+      <c r="G64" s="101"/>
+      <c r="H64" s="107"/>
     </row>
     <row r="65" spans="2:8" s="34" customFormat="1">
       <c r="B65" s="36"/>
       <c r="C65" s="37"/>
-      <c r="D65" s="102"/>
-      <c r="E65" s="107"/>
-      <c r="F65" s="113"/>
-      <c r="G65" s="102"/>
-      <c r="H65" s="108"/>
+      <c r="D65" s="101"/>
+      <c r="E65" s="106"/>
+      <c r="F65" s="112"/>
+      <c r="G65" s="101"/>
+      <c r="H65" s="107"/>
     </row>
     <row r="66" spans="2:8" s="34" customFormat="1">
       <c r="B66" s="36"/>
       <c r="C66" s="37"/>
-      <c r="D66" s="102"/>
-      <c r="E66" s="107"/>
-      <c r="F66" s="113"/>
-      <c r="G66" s="102"/>
-      <c r="H66" s="108"/>
+      <c r="D66" s="101"/>
+      <c r="E66" s="106"/>
+      <c r="F66" s="112"/>
+      <c r="G66" s="101"/>
+      <c r="H66" s="107"/>
     </row>
     <row r="67" spans="2:8" s="34" customFormat="1">
       <c r="B67" s="36"/>
       <c r="C67" s="37"/>
-      <c r="D67" s="102"/>
-      <c r="E67" s="107"/>
-      <c r="F67" s="113"/>
-      <c r="G67" s="102"/>
-      <c r="H67" s="108"/>
+      <c r="D67" s="101"/>
+      <c r="E67" s="106"/>
+      <c r="F67" s="112"/>
+      <c r="G67" s="101"/>
+      <c r="H67" s="107"/>
     </row>
     <row r="68" spans="2:8" s="34" customFormat="1">
       <c r="B68" s="36"/>
       <c r="C68" s="37"/>
-      <c r="D68" s="102"/>
-      <c r="E68" s="107"/>
-      <c r="F68" s="113"/>
-      <c r="G68" s="102"/>
-      <c r="H68" s="108"/>
+      <c r="D68" s="101"/>
+      <c r="E68" s="106"/>
+      <c r="F68" s="112"/>
+      <c r="G68" s="101"/>
+      <c r="H68" s="107"/>
     </row>
     <row r="69" spans="2:8" s="34" customFormat="1">
       <c r="B69" s="36"/>
       <c r="C69" s="37"/>
-      <c r="D69" s="102"/>
-      <c r="E69" s="107"/>
-      <c r="F69" s="113"/>
-      <c r="G69" s="102"/>
-      <c r="H69" s="108"/>
+      <c r="D69" s="101"/>
+      <c r="E69" s="106"/>
+      <c r="F69" s="112"/>
+      <c r="G69" s="101"/>
+      <c r="H69" s="107"/>
     </row>
     <row r="70" spans="2:8" s="34" customFormat="1">
       <c r="B70" s="36"/>
       <c r="C70" s="37"/>
-      <c r="D70" s="102"/>
-      <c r="E70" s="107"/>
-      <c r="F70" s="113"/>
-      <c r="G70" s="102"/>
-      <c r="H70" s="108"/>
+      <c r="D70" s="101"/>
+      <c r="E70" s="106"/>
+      <c r="F70" s="112"/>
+      <c r="G70" s="101"/>
+      <c r="H70" s="107"/>
     </row>
     <row r="71" spans="2:8" s="34" customFormat="1">
       <c r="B71" s="36"/>
       <c r="C71" s="37"/>
-      <c r="D71" s="102"/>
-      <c r="E71" s="107"/>
-      <c r="F71" s="113"/>
-      <c r="G71" s="102"/>
-      <c r="H71" s="108"/>
+      <c r="D71" s="101"/>
+      <c r="E71" s="106"/>
+      <c r="F71" s="112"/>
+      <c r="G71" s="101"/>
+      <c r="H71" s="107"/>
     </row>
     <row r="72" spans="2:8" s="34" customFormat="1">
-      <c r="B72" s="110"/>
-      <c r="C72" s="109"/>
+      <c r="B72" s="109"/>
+      <c r="C72" s="108"/>
       <c r="D72" s="43"/>
-      <c r="E72" s="106"/>
-      <c r="F72" s="114"/>
+      <c r="E72" s="105"/>
+      <c r="F72" s="113"/>
       <c r="G72" s="43"/>
       <c r="H72" s="44"/>
     </row>
@@ -3080,10 +3157,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K79"/>
+  <dimension ref="A1:L95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="85" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36:F36"/>
+    <sheetView topLeftCell="A30" zoomScale="85" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" outlineLevelRow="1"/>
@@ -3102,27 +3179,27 @@
       <c r="A1" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
-      <c r="D1" s="121"/>
+      <c r="B1" s="137"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
-      <c r="I1" s="92"/>
+      <c r="I1" s="91"/>
       <c r="J1" s="6"/>
       <c r="K1" s="7"/>
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="122"/>
-      <c r="C2" s="122"/>
-      <c r="D2" s="122"/>
+      <c r="B2" s="138"/>
+      <c r="C2" s="138"/>
+      <c r="D2" s="138"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
-      <c r="I2" s="92"/>
+      <c r="I2" s="91"/>
       <c r="J2" s="6"/>
       <c r="K2" s="7"/>
     </row>
@@ -3130,51 +3207,51 @@
       <c r="A3" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="114" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="115"/>
-      <c r="D3" s="116"/>
+      <c r="C3" s="114"/>
+      <c r="D3" s="115"/>
       <c r="E3" s="61"/>
       <c r="F3" s="61"/>
       <c r="G3" s="61"/>
-      <c r="H3" s="131"/>
-      <c r="I3" s="131"/>
-      <c r="J3" s="131"/>
+      <c r="H3" s="145"/>
+      <c r="I3" s="145"/>
+      <c r="J3" s="145"/>
       <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="12.75">
       <c r="A4" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="133" t="s">
+      <c r="B4" s="146" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="134"/>
-      <c r="D4" s="135"/>
+      <c r="C4" s="147"/>
+      <c r="D4" s="148"/>
       <c r="E4" s="61"/>
       <c r="F4" s="61"/>
       <c r="G4" s="61"/>
-      <c r="H4" s="131"/>
-      <c r="I4" s="131"/>
-      <c r="J4" s="131"/>
+      <c r="H4" s="145"/>
+      <c r="I4" s="145"/>
+      <c r="J4" s="145"/>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" s="71" customFormat="1" ht="25.5">
       <c r="A5" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="124" t="s">
+      <c r="B5" s="140" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="125"/>
-      <c r="D5" s="126"/>
+      <c r="C5" s="141"/>
+      <c r="D5" s="142"/>
       <c r="E5" s="69"/>
       <c r="F5" s="69"/>
       <c r="G5" s="69"/>
-      <c r="H5" s="130"/>
-      <c r="I5" s="130"/>
-      <c r="J5" s="130"/>
+      <c r="H5" s="144"/>
+      <c r="I5" s="144"/>
+      <c r="J5" s="144"/>
       <c r="K5" s="70"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
@@ -3195,9 +3272,9 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="131"/>
-      <c r="I6" s="131"/>
-      <c r="J6" s="131"/>
+      <c r="H6" s="145"/>
+      <c r="I6" s="145"/>
+      <c r="J6" s="145"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -3218,89 +3295,89 @@
       <c r="E7" s="62"/>
       <c r="F7" s="62"/>
       <c r="G7" s="62"/>
-      <c r="H7" s="131"/>
-      <c r="I7" s="131"/>
-      <c r="J7" s="131"/>
+      <c r="H7" s="145"/>
+      <c r="I7" s="145"/>
+      <c r="J7" s="145"/>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="123"/>
-      <c r="B8" s="123"/>
-      <c r="C8" s="123"/>
-      <c r="D8" s="123"/>
+      <c r="A8" s="139"/>
+      <c r="B8" s="139"/>
+      <c r="C8" s="139"/>
+      <c r="D8" s="139"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
-      <c r="I8" s="93"/>
-      <c r="J8" s="93"/>
+      <c r="I8" s="92"/>
+      <c r="J8" s="92"/>
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" s="73" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="140" t="s">
+      <c r="A9" s="128" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="141" t="s">
+      <c r="B9" s="152" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="140" t="s">
+      <c r="C9" s="128" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="147" t="s">
+      <c r="D9" s="129" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="148"/>
-      <c r="F9" s="148"/>
-      <c r="G9" s="149"/>
-      <c r="H9" s="136" t="s">
+      <c r="E9" s="130"/>
+      <c r="F9" s="130"/>
+      <c r="G9" s="131"/>
+      <c r="H9" s="149" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="132" t="s">
+      <c r="I9" s="125" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="132" t="s">
+      <c r="J9" s="125" t="s">
         <v>32</v>
       </c>
       <c r="K9" s="72"/>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="132"/>
-      <c r="B10" s="142"/>
-      <c r="C10" s="132"/>
-      <c r="D10" s="137"/>
-      <c r="E10" s="150"/>
-      <c r="F10" s="150"/>
-      <c r="G10" s="151"/>
-      <c r="H10" s="137"/>
-      <c r="I10" s="132"/>
-      <c r="J10" s="132"/>
+      <c r="A10" s="125"/>
+      <c r="B10" s="153"/>
+      <c r="C10" s="125"/>
+      <c r="D10" s="132"/>
+      <c r="E10" s="133"/>
+      <c r="F10" s="133"/>
+      <c r="G10" s="134"/>
+      <c r="H10" s="132"/>
+      <c r="I10" s="125"/>
+      <c r="J10" s="125"/>
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" s="74" customFormat="1" ht="15">
-      <c r="A11" s="138"/>
-      <c r="B11" s="138"/>
-      <c r="C11" s="138"/>
-      <c r="D11" s="138"/>
-      <c r="E11" s="138"/>
-      <c r="F11" s="138"/>
-      <c r="G11" s="138"/>
-      <c r="H11" s="138"/>
-      <c r="I11" s="138"/>
-      <c r="J11" s="139"/>
+      <c r="A11" s="150"/>
+      <c r="B11" s="150"/>
+      <c r="C11" s="150"/>
+      <c r="D11" s="150"/>
+      <c r="E11" s="150"/>
+      <c r="F11" s="150"/>
+      <c r="G11" s="150"/>
+      <c r="H11" s="150"/>
+      <c r="I11" s="150"/>
+      <c r="J11" s="151"/>
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A12" s="127" t="s">
+      <c r="A12" s="135" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="128"/>
-      <c r="C12" s="128"/>
-      <c r="D12" s="128"/>
-      <c r="E12" s="128"/>
-      <c r="F12" s="128"/>
-      <c r="G12" s="128"/>
-      <c r="H12" s="128"/>
-      <c r="I12" s="128"/>
-      <c r="J12" s="129"/>
+      <c r="B12" s="136"/>
+      <c r="C12" s="136"/>
+      <c r="D12" s="136"/>
+      <c r="E12" s="136"/>
+      <c r="F12" s="136"/>
+      <c r="G12" s="136"/>
+      <c r="H12" s="136"/>
+      <c r="I12" s="136"/>
+      <c r="J12" s="143"/>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" ht="102.75" customHeight="1" outlineLevel="1">
       <c r="A13" s="78" t="s">
@@ -3312,9 +3389,9 @@
       <c r="C13" s="77" t="s">
         <v>85</v>
       </c>
-      <c r="D13" s="145"/>
-      <c r="E13" s="146"/>
-      <c r="F13" s="146"/>
+      <c r="D13" s="116"/>
+      <c r="E13" s="117"/>
+      <c r="F13" s="117"/>
       <c r="G13" s="76"/>
       <c r="H13" s="90"/>
       <c r="I13" s="77"/>
@@ -3330,9 +3407,9 @@
       <c r="C14" s="77" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="145"/>
-      <c r="E14" s="146"/>
-      <c r="F14" s="146"/>
+      <c r="D14" s="116"/>
+      <c r="E14" s="117"/>
+      <c r="F14" s="117"/>
       <c r="G14" s="76"/>
       <c r="H14" s="90"/>
       <c r="I14" s="77"/>
@@ -3348,9 +3425,9 @@
       <c r="C15" s="77" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="145"/>
-      <c r="E15" s="146"/>
-      <c r="F15" s="146"/>
+      <c r="D15" s="116"/>
+      <c r="E15" s="117"/>
+      <c r="F15" s="117"/>
       <c r="G15" s="76"/>
       <c r="H15" s="90"/>
       <c r="I15" s="77"/>
@@ -3366,9 +3443,9 @@
       <c r="C16" s="77" t="s">
         <v>95</v>
       </c>
-      <c r="D16" s="145"/>
-      <c r="E16" s="146"/>
-      <c r="F16" s="146"/>
+      <c r="D16" s="116"/>
+      <c r="E16" s="117"/>
+      <c r="F16" s="117"/>
       <c r="G16" s="76"/>
       <c r="H16" s="90"/>
       <c r="I16" s="77"/>
@@ -3384,9 +3461,9 @@
       <c r="C17" s="77" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="145"/>
-      <c r="E17" s="146"/>
-      <c r="F17" s="146"/>
+      <c r="D17" s="116"/>
+      <c r="E17" s="117"/>
+      <c r="F17" s="117"/>
       <c r="G17" s="76"/>
       <c r="H17" s="90"/>
       <c r="I17" s="77"/>
@@ -3402,56 +3479,56 @@
       <c r="C18" s="77" t="s">
         <v>93</v>
       </c>
-      <c r="D18" s="145"/>
-      <c r="E18" s="146"/>
-      <c r="F18" s="146"/>
+      <c r="D18" s="116"/>
+      <c r="E18" s="117"/>
+      <c r="F18" s="117"/>
       <c r="G18" s="76"/>
       <c r="H18" s="90"/>
       <c r="I18" s="77"/>
       <c r="J18" s="75"/>
     </row>
-    <row r="19" spans="1:10" s="101" customFormat="1" ht="91.5" customHeight="1" outlineLevel="1">
+    <row r="19" spans="1:10" s="100" customFormat="1" ht="91.5" customHeight="1" outlineLevel="1">
       <c r="A19" s="78" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="94" t="s">
+      <c r="B19" s="93" t="s">
         <v>97</v>
       </c>
       <c r="C19" s="87" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="152"/>
-      <c r="E19" s="153"/>
-      <c r="F19" s="154"/>
+      <c r="D19" s="118"/>
+      <c r="E19" s="119"/>
+      <c r="F19" s="120"/>
       <c r="G19" s="77"/>
       <c r="H19" s="77"/>
       <c r="I19" s="77"/>
       <c r="J19" s="75"/>
     </row>
-    <row r="20" spans="1:10" s="101" customFormat="1" ht="107.25" customHeight="1" outlineLevel="1">
+    <row r="20" spans="1:10" s="100" customFormat="1" ht="107.25" customHeight="1" outlineLevel="1">
       <c r="A20" s="78" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="94" t="s">
+      <c r="B20" s="93" t="s">
         <v>100</v>
       </c>
       <c r="C20" s="77" t="s">
         <v>102</v>
       </c>
-      <c r="D20" s="152"/>
-      <c r="E20" s="153"/>
-      <c r="F20" s="154"/>
+      <c r="D20" s="118"/>
+      <c r="E20" s="119"/>
+      <c r="F20" s="120"/>
       <c r="G20" s="77"/>
       <c r="H20" s="77"/>
       <c r="I20" s="77"/>
       <c r="J20" s="75"/>
     </row>
     <row r="21" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A21" s="127" t="s">
+      <c r="A21" s="135" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="128"/>
-      <c r="C21" s="128"/>
+      <c r="B21" s="136"/>
+      <c r="C21" s="136"/>
       <c r="D21" s="88"/>
       <c r="E21" s="88"/>
       <c r="F21" s="88"/>
@@ -3461,7 +3538,7 @@
       <c r="J21" s="89"/>
     </row>
     <row r="22" spans="1:10" s="4" customFormat="1" ht="57" customHeight="1" outlineLevel="1">
-      <c r="A22" s="95" t="s">
+      <c r="A22" s="94" t="s">
         <v>0</v>
       </c>
       <c r="B22" s="86" t="s">
@@ -3470,16 +3547,16 @@
       <c r="C22" s="87" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="143"/>
-      <c r="E22" s="144"/>
-      <c r="F22" s="144"/>
-      <c r="G22" s="96"/>
-      <c r="H22" s="97"/>
+      <c r="D22" s="126"/>
+      <c r="E22" s="127"/>
+      <c r="F22" s="127"/>
+      <c r="G22" s="95"/>
+      <c r="H22" s="96"/>
       <c r="I22" s="87"/>
-      <c r="J22" s="98"/>
+      <c r="J22" s="97"/>
     </row>
     <row r="23" spans="1:10" s="4" customFormat="1" ht="83.25" customHeight="1" outlineLevel="1">
-      <c r="A23" s="95" t="s">
+      <c r="A23" s="94" t="s">
         <v>1</v>
       </c>
       <c r="B23" s="86" t="s">
@@ -3488,16 +3565,16 @@
       <c r="C23" s="87" t="s">
         <v>72</v>
       </c>
-      <c r="D23" s="143"/>
-      <c r="E23" s="144"/>
-      <c r="F23" s="144"/>
-      <c r="G23" s="96"/>
-      <c r="H23" s="97"/>
+      <c r="D23" s="126"/>
+      <c r="E23" s="127"/>
+      <c r="F23" s="127"/>
+      <c r="G23" s="95"/>
+      <c r="H23" s="96"/>
       <c r="I23" s="87"/>
-      <c r="J23" s="98"/>
+      <c r="J23" s="97"/>
     </row>
     <row r="24" spans="1:10" s="4" customFormat="1" ht="68.25" customHeight="1" outlineLevel="1">
-      <c r="A24" s="95" t="s">
+      <c r="A24" s="94" t="s">
         <v>2</v>
       </c>
       <c r="B24" s="86" t="s">
@@ -3506,217 +3583,217 @@
       <c r="C24" s="87" t="s">
         <v>75</v>
       </c>
-      <c r="D24" s="143"/>
-      <c r="E24" s="144"/>
-      <c r="F24" s="144"/>
-      <c r="G24" s="96"/>
-      <c r="H24" s="97"/>
+      <c r="D24" s="126"/>
+      <c r="E24" s="127"/>
+      <c r="F24" s="127"/>
+      <c r="G24" s="95"/>
+      <c r="H24" s="96"/>
       <c r="I24" s="87"/>
-      <c r="J24" s="98"/>
-    </row>
-    <row r="25" spans="1:10" s="101" customFormat="1" ht="83.25" customHeight="1" outlineLevel="1">
+      <c r="J24" s="97"/>
+    </row>
+    <row r="25" spans="1:10" s="100" customFormat="1" ht="83.25" customHeight="1" outlineLevel="1">
       <c r="A25" s="78" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="94" t="s">
+      <c r="B25" s="93" t="s">
         <v>76</v>
       </c>
       <c r="C25" s="87" t="s">
         <v>77</v>
       </c>
-      <c r="D25" s="152"/>
-      <c r="E25" s="153"/>
-      <c r="F25" s="154"/>
+      <c r="D25" s="118"/>
+      <c r="E25" s="119"/>
+      <c r="F25" s="120"/>
       <c r="G25" s="77"/>
       <c r="H25" s="77"/>
       <c r="I25" s="77"/>
       <c r="J25" s="75"/>
     </row>
-    <row r="26" spans="1:10" s="101" customFormat="1" ht="68.25" customHeight="1" outlineLevel="1">
+    <row r="26" spans="1:10" s="100" customFormat="1" ht="68.25" customHeight="1" outlineLevel="1">
       <c r="A26" s="78" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="94" t="s">
+      <c r="B26" s="93" t="s">
         <v>96</v>
       </c>
       <c r="C26" s="87" t="s">
         <v>99</v>
       </c>
-      <c r="D26" s="152"/>
-      <c r="E26" s="153"/>
-      <c r="F26" s="154"/>
+      <c r="D26" s="118"/>
+      <c r="E26" s="119"/>
+      <c r="F26" s="120"/>
       <c r="G26" s="77"/>
       <c r="H26" s="77"/>
       <c r="I26" s="77"/>
       <c r="J26" s="75"/>
     </row>
-    <row r="27" spans="1:10" s="101" customFormat="1" ht="69.75" customHeight="1" outlineLevel="1">
+    <row r="27" spans="1:10" s="100" customFormat="1" ht="69.75" customHeight="1" outlineLevel="1">
       <c r="A27" s="78" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="94" t="s">
+      <c r="B27" s="93" t="s">
         <v>49</v>
       </c>
       <c r="C27" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="152"/>
-      <c r="E27" s="153"/>
-      <c r="F27" s="154"/>
+      <c r="D27" s="118"/>
+      <c r="E27" s="119"/>
+      <c r="F27" s="120"/>
       <c r="G27" s="77"/>
       <c r="H27" s="77"/>
       <c r="I27" s="77"/>
       <c r="J27" s="75"/>
     </row>
-    <row r="28" spans="1:10" s="101" customFormat="1" ht="80.25" customHeight="1" outlineLevel="1">
+    <row r="28" spans="1:10" s="100" customFormat="1" ht="80.25" customHeight="1" outlineLevel="1">
       <c r="A28" s="78" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="94" t="s">
+      <c r="B28" s="93" t="s">
         <v>78</v>
       </c>
       <c r="C28" s="77" t="s">
         <v>79</v>
       </c>
-      <c r="D28" s="152"/>
-      <c r="E28" s="153"/>
-      <c r="F28" s="154"/>
+      <c r="D28" s="118"/>
+      <c r="E28" s="119"/>
+      <c r="F28" s="120"/>
       <c r="G28" s="77"/>
       <c r="H28" s="77"/>
       <c r="I28" s="77"/>
       <c r="J28" s="75"/>
     </row>
-    <row r="29" spans="1:10" s="101" customFormat="1" ht="46.5" customHeight="1" outlineLevel="1">
+    <row r="29" spans="1:10" s="100" customFormat="1" ht="46.5" customHeight="1" outlineLevel="1">
       <c r="A29" s="78" t="s">
         <v>71</v>
       </c>
-      <c r="B29" s="94" t="s">
+      <c r="B29" s="93" t="s">
         <v>60</v>
       </c>
       <c r="C29" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="152"/>
-      <c r="E29" s="153"/>
-      <c r="F29" s="154"/>
+      <c r="D29" s="118"/>
+      <c r="E29" s="119"/>
+      <c r="F29" s="120"/>
       <c r="G29" s="77"/>
       <c r="H29" s="77"/>
       <c r="I29" s="77"/>
       <c r="J29" s="75"/>
     </row>
-    <row r="30" spans="1:10" s="101" customFormat="1" ht="108.75" customHeight="1" outlineLevel="1">
+    <row r="30" spans="1:10" s="100" customFormat="1" ht="108.75" customHeight="1" outlineLevel="1">
       <c r="A30" s="78" t="s">
         <v>104</v>
       </c>
-      <c r="B30" s="94" t="s">
+      <c r="B30" s="93" t="s">
         <v>51</v>
       </c>
       <c r="C30" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="D30" s="152"/>
-      <c r="E30" s="153"/>
-      <c r="F30" s="154"/>
+      <c r="D30" s="118"/>
+      <c r="E30" s="119"/>
+      <c r="F30" s="120"/>
       <c r="G30" s="77"/>
       <c r="H30" s="77"/>
       <c r="I30" s="77"/>
       <c r="J30" s="75"/>
     </row>
-    <row r="31" spans="1:10" s="101" customFormat="1" ht="46.5" customHeight="1" outlineLevel="1">
+    <row r="31" spans="1:10" s="100" customFormat="1" ht="46.5" customHeight="1" outlineLevel="1">
       <c r="A31" s="78" t="s">
         <v>105</v>
       </c>
-      <c r="B31" s="94" t="s">
+      <c r="B31" s="93" t="s">
         <v>59</v>
       </c>
       <c r="C31" s="77" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="152"/>
-      <c r="E31" s="153"/>
-      <c r="F31" s="154"/>
+      <c r="D31" s="118"/>
+      <c r="E31" s="119"/>
+      <c r="F31" s="120"/>
       <c r="G31" s="77"/>
       <c r="H31" s="77"/>
       <c r="I31" s="77"/>
       <c r="J31" s="75"/>
     </row>
-    <row r="32" spans="1:10" s="101" customFormat="1" ht="107.25" customHeight="1" outlineLevel="1">
+    <row r="32" spans="1:10" s="100" customFormat="1" ht="107.25" customHeight="1" outlineLevel="1">
       <c r="A32" s="78" t="s">
         <v>106</v>
       </c>
-      <c r="B32" s="94" t="s">
+      <c r="B32" s="93" t="s">
         <v>58</v>
       </c>
       <c r="C32" s="77" t="s">
         <v>101</v>
       </c>
-      <c r="D32" s="152"/>
-      <c r="E32" s="153"/>
-      <c r="F32" s="154"/>
+      <c r="D32" s="118"/>
+      <c r="E32" s="119"/>
+      <c r="F32" s="120"/>
       <c r="G32" s="77"/>
       <c r="H32" s="77"/>
       <c r="I32" s="77"/>
       <c r="J32" s="75"/>
     </row>
     <row r="33" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A33" s="117" t="s">
+      <c r="A33" s="121" t="s">
         <v>81</v>
       </c>
-      <c r="B33" s="118"/>
-      <c r="C33" s="118"/>
-      <c r="D33" s="99"/>
-      <c r="E33" s="99"/>
-      <c r="F33" s="99"/>
-      <c r="G33" s="99"/>
-      <c r="H33" s="99"/>
-      <c r="I33" s="99"/>
-      <c r="J33" s="100"/>
+      <c r="B33" s="122"/>
+      <c r="C33" s="122"/>
+      <c r="D33" s="98"/>
+      <c r="E33" s="98"/>
+      <c r="F33" s="98"/>
+      <c r="G33" s="98"/>
+      <c r="H33" s="98"/>
+      <c r="I33" s="98"/>
+      <c r="J33" s="99"/>
     </row>
     <row r="34" spans="1:10" s="4" customFormat="1" ht="57" customHeight="1" outlineLevel="1">
       <c r="A34" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B34" s="94" t="s">
+      <c r="B34" s="93" t="s">
         <v>83</v>
       </c>
       <c r="C34" s="77" t="s">
         <v>84</v>
       </c>
-      <c r="D34" s="119"/>
-      <c r="E34" s="120"/>
-      <c r="F34" s="120"/>
+      <c r="D34" s="123"/>
+      <c r="E34" s="124"/>
+      <c r="F34" s="124"/>
       <c r="G34" s="76"/>
       <c r="H34" s="83"/>
       <c r="I34" s="77"/>
       <c r="J34" s="75"/>
     </row>
     <row r="35" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A35" s="117" t="s">
+      <c r="A35" s="121" t="s">
         <v>82</v>
       </c>
-      <c r="B35" s="118"/>
-      <c r="C35" s="118"/>
-      <c r="D35" s="99"/>
-      <c r="E35" s="99"/>
-      <c r="F35" s="99"/>
-      <c r="G35" s="99"/>
-      <c r="H35" s="99"/>
-      <c r="I35" s="99"/>
-      <c r="J35" s="100"/>
+      <c r="B35" s="122"/>
+      <c r="C35" s="122"/>
+      <c r="D35" s="98"/>
+      <c r="E35" s="98"/>
+      <c r="F35" s="98"/>
+      <c r="G35" s="98"/>
+      <c r="H35" s="98"/>
+      <c r="I35" s="98"/>
+      <c r="J35" s="99"/>
     </row>
     <row r="36" spans="1:10" s="4" customFormat="1" ht="116.25" customHeight="1" outlineLevel="1">
       <c r="A36" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B36" s="94" t="s">
+      <c r="B36" s="93" t="s">
         <v>143</v>
       </c>
       <c r="C36" s="77" t="s">
         <v>146</v>
       </c>
-      <c r="D36" s="119"/>
-      <c r="E36" s="120"/>
-      <c r="F36" s="120"/>
+      <c r="D36" s="123"/>
+      <c r="E36" s="124"/>
+      <c r="F36" s="124"/>
       <c r="G36" s="76"/>
       <c r="H36" s="83"/>
       <c r="I36" s="77"/>
@@ -3732,9 +3809,9 @@
       <c r="C37" s="77" t="s">
         <v>148</v>
       </c>
-      <c r="D37" s="119"/>
-      <c r="E37" s="120"/>
-      <c r="F37" s="120"/>
+      <c r="D37" s="123"/>
+      <c r="E37" s="124"/>
+      <c r="F37" s="124"/>
       <c r="G37" s="76"/>
       <c r="H37" s="83"/>
       <c r="I37" s="77"/>
@@ -3744,15 +3821,15 @@
       <c r="A38" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="B38" s="94" t="s">
+      <c r="B38" s="93" t="s">
         <v>145</v>
       </c>
       <c r="C38" s="77" t="s">
         <v>147</v>
       </c>
-      <c r="D38" s="119"/>
-      <c r="E38" s="120"/>
-      <c r="F38" s="120"/>
+      <c r="D38" s="123"/>
+      <c r="E38" s="124"/>
+      <c r="F38" s="124"/>
       <c r="G38" s="76"/>
       <c r="H38" s="83"/>
       <c r="I38" s="77"/>
@@ -3762,15 +3839,15 @@
       <c r="A39" s="78" t="s">
         <v>50</v>
       </c>
-      <c r="B39" s="94" t="s">
+      <c r="B39" s="93" t="s">
         <v>149</v>
       </c>
       <c r="C39" s="77" t="s">
         <v>150</v>
       </c>
-      <c r="D39" s="119"/>
-      <c r="E39" s="120"/>
-      <c r="F39" s="120"/>
+      <c r="D39" s="123"/>
+      <c r="E39" s="124"/>
+      <c r="F39" s="124"/>
       <c r="G39" s="76"/>
       <c r="H39" s="83"/>
       <c r="I39" s="77"/>
@@ -3780,47 +3857,47 @@
       <c r="A40" s="78" t="s">
         <v>53</v>
       </c>
-      <c r="B40" s="94" t="s">
+      <c r="B40" s="93" t="s">
         <v>151</v>
       </c>
       <c r="C40" s="77" t="s">
         <v>152</v>
       </c>
-      <c r="D40" s="119"/>
-      <c r="E40" s="120"/>
-      <c r="F40" s="120"/>
+      <c r="D40" s="123"/>
+      <c r="E40" s="124"/>
+      <c r="F40" s="124"/>
       <c r="G40" s="76"/>
       <c r="H40" s="83"/>
       <c r="I40" s="77"/>
       <c r="J40" s="75"/>
     </row>
     <row r="41" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A41" s="117" t="s">
+      <c r="A41" s="121" t="s">
         <v>120</v>
       </c>
-      <c r="B41" s="118"/>
-      <c r="C41" s="118"/>
-      <c r="D41" s="99"/>
-      <c r="E41" s="99"/>
-      <c r="F41" s="99"/>
-      <c r="G41" s="99"/>
-      <c r="H41" s="99"/>
-      <c r="I41" s="99"/>
-      <c r="J41" s="100"/>
+      <c r="B41" s="122"/>
+      <c r="C41" s="122"/>
+      <c r="D41" s="98"/>
+      <c r="E41" s="98"/>
+      <c r="F41" s="98"/>
+      <c r="G41" s="98"/>
+      <c r="H41" s="98"/>
+      <c r="I41" s="98"/>
+      <c r="J41" s="99"/>
     </row>
     <row r="42" spans="1:10" s="4" customFormat="1" ht="78.75" customHeight="1" outlineLevel="1">
       <c r="A42" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B42" s="94" t="s">
+      <c r="B42" s="93" t="s">
         <v>121</v>
       </c>
       <c r="C42" s="77" t="s">
         <v>127</v>
       </c>
-      <c r="D42" s="119"/>
-      <c r="E42" s="120"/>
-      <c r="F42" s="120"/>
+      <c r="D42" s="123"/>
+      <c r="E42" s="124"/>
+      <c r="F42" s="124"/>
       <c r="G42" s="76"/>
       <c r="H42" s="83"/>
       <c r="I42" s="77"/>
@@ -3830,15 +3907,15 @@
       <c r="A43" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="B43" s="94" t="s">
+      <c r="B43" s="93" t="s">
         <v>122</v>
       </c>
       <c r="C43" s="77" t="s">
         <v>128</v>
       </c>
-      <c r="D43" s="119"/>
-      <c r="E43" s="120"/>
-      <c r="F43" s="120"/>
+      <c r="D43" s="123"/>
+      <c r="E43" s="124"/>
+      <c r="F43" s="124"/>
       <c r="G43" s="76"/>
       <c r="H43" s="83"/>
       <c r="I43" s="77"/>
@@ -3848,15 +3925,15 @@
       <c r="A44" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="B44" s="94" t="s">
+      <c r="B44" s="93" t="s">
         <v>125</v>
       </c>
       <c r="C44" s="77" t="s">
         <v>129</v>
       </c>
-      <c r="D44" s="119"/>
-      <c r="E44" s="120"/>
-      <c r="F44" s="120"/>
+      <c r="D44" s="123"/>
+      <c r="E44" s="124"/>
+      <c r="F44" s="124"/>
       <c r="G44" s="76"/>
       <c r="H44" s="83"/>
       <c r="I44" s="77"/>
@@ -3866,15 +3943,15 @@
       <c r="A45" s="78" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="94" t="s">
+      <c r="B45" s="93" t="s">
         <v>126</v>
       </c>
       <c r="C45" s="77" t="s">
         <v>130</v>
       </c>
-      <c r="D45" s="119"/>
-      <c r="E45" s="120"/>
-      <c r="F45" s="120"/>
+      <c r="D45" s="123"/>
+      <c r="E45" s="124"/>
+      <c r="F45" s="124"/>
       <c r="G45" s="76"/>
       <c r="H45" s="83"/>
       <c r="I45" s="77"/>
@@ -3884,15 +3961,15 @@
       <c r="A46" s="78" t="s">
         <v>53</v>
       </c>
-      <c r="B46" s="94" t="s">
+      <c r="B46" s="93" t="s">
         <v>131</v>
       </c>
       <c r="C46" s="77" t="s">
         <v>132</v>
       </c>
-      <c r="D46" s="119"/>
-      <c r="E46" s="120"/>
-      <c r="F46" s="120"/>
+      <c r="D46" s="123"/>
+      <c r="E46" s="124"/>
+      <c r="F46" s="124"/>
       <c r="G46" s="76"/>
       <c r="H46" s="83"/>
       <c r="I46" s="77"/>
@@ -3902,215 +3979,215 @@
       <c r="A47" s="78" t="s">
         <v>55</v>
       </c>
-      <c r="B47" s="94" t="s">
+      <c r="B47" s="93" t="s">
         <v>123</v>
       </c>
       <c r="C47" s="77" t="s">
         <v>124</v>
       </c>
-      <c r="D47" s="119"/>
-      <c r="E47" s="120"/>
-      <c r="F47" s="120"/>
+      <c r="D47" s="123"/>
+      <c r="E47" s="124"/>
+      <c r="F47" s="124"/>
       <c r="G47" s="76"/>
       <c r="H47" s="83"/>
       <c r="I47" s="77"/>
       <c r="J47" s="75"/>
     </row>
     <row r="48" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A48" s="117" t="s">
+      <c r="A48" s="121" t="s">
         <v>133</v>
       </c>
-      <c r="B48" s="118"/>
-      <c r="C48" s="118"/>
-      <c r="D48" s="99"/>
-      <c r="E48" s="99"/>
-      <c r="F48" s="99"/>
-      <c r="G48" s="99"/>
-      <c r="H48" s="99"/>
-      <c r="I48" s="99"/>
-      <c r="J48" s="100"/>
+      <c r="B48" s="122"/>
+      <c r="C48" s="122"/>
+      <c r="D48" s="98"/>
+      <c r="E48" s="98"/>
+      <c r="F48" s="98"/>
+      <c r="G48" s="98"/>
+      <c r="H48" s="98"/>
+      <c r="I48" s="98"/>
+      <c r="J48" s="99"/>
     </row>
     <row r="49" spans="1:10" s="4" customFormat="1" ht="47.25" customHeight="1" outlineLevel="1">
       <c r="A49" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B49" s="94" t="s">
+      <c r="B49" s="93" t="s">
         <v>135</v>
       </c>
       <c r="C49" s="77" t="s">
         <v>134</v>
       </c>
-      <c r="D49" s="119"/>
-      <c r="E49" s="120"/>
-      <c r="F49" s="120"/>
+      <c r="D49" s="123"/>
+      <c r="E49" s="124"/>
+      <c r="F49" s="124"/>
       <c r="G49" s="76"/>
       <c r="H49" s="83"/>
       <c r="I49" s="77"/>
       <c r="J49" s="75"/>
     </row>
     <row r="50" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A50" s="117"/>
-      <c r="B50" s="118"/>
-      <c r="C50" s="118"/>
-      <c r="D50" s="99"/>
-      <c r="E50" s="99"/>
-      <c r="F50" s="99"/>
-      <c r="G50" s="99"/>
-      <c r="H50" s="99"/>
-      <c r="I50" s="99"/>
-      <c r="J50" s="100"/>
+      <c r="A50" s="121"/>
+      <c r="B50" s="122"/>
+      <c r="C50" s="122"/>
+      <c r="D50" s="98"/>
+      <c r="E50" s="98"/>
+      <c r="F50" s="98"/>
+      <c r="G50" s="98"/>
+      <c r="H50" s="98"/>
+      <c r="I50" s="98"/>
+      <c r="J50" s="99"/>
     </row>
     <row r="51" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A51" s="78"/>
-      <c r="B51" s="94"/>
+      <c r="B51" s="93"/>
       <c r="C51" s="77"/>
-      <c r="D51" s="119"/>
-      <c r="E51" s="120"/>
-      <c r="F51" s="120"/>
+      <c r="D51" s="123"/>
+      <c r="E51" s="124"/>
+      <c r="F51" s="124"/>
       <c r="G51" s="76"/>
       <c r="H51" s="83"/>
       <c r="I51" s="77"/>
       <c r="J51" s="75"/>
     </row>
     <row r="52" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A52" s="117"/>
-      <c r="B52" s="118"/>
-      <c r="C52" s="118"/>
-      <c r="D52" s="99"/>
-      <c r="E52" s="99"/>
-      <c r="F52" s="99"/>
-      <c r="G52" s="99"/>
-      <c r="H52" s="99"/>
-      <c r="I52" s="99"/>
-      <c r="J52" s="100"/>
+      <c r="A52" s="121"/>
+      <c r="B52" s="122"/>
+      <c r="C52" s="122"/>
+      <c r="D52" s="98"/>
+      <c r="E52" s="98"/>
+      <c r="F52" s="98"/>
+      <c r="G52" s="98"/>
+      <c r="H52" s="98"/>
+      <c r="I52" s="98"/>
+      <c r="J52" s="99"/>
     </row>
     <row r="53" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A53" s="78"/>
-      <c r="B53" s="94"/>
+      <c r="B53" s="93"/>
       <c r="C53" s="77"/>
-      <c r="D53" s="119"/>
-      <c r="E53" s="120"/>
-      <c r="F53" s="120"/>
+      <c r="D53" s="123"/>
+      <c r="E53" s="124"/>
+      <c r="F53" s="124"/>
       <c r="G53" s="76"/>
       <c r="H53" s="83"/>
       <c r="I53" s="77"/>
       <c r="J53" s="75"/>
     </row>
     <row r="54" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A54" s="117"/>
-      <c r="B54" s="118"/>
-      <c r="C54" s="118"/>
-      <c r="D54" s="99"/>
-      <c r="E54" s="99"/>
-      <c r="F54" s="99"/>
-      <c r="G54" s="99"/>
-      <c r="H54" s="99"/>
-      <c r="I54" s="99"/>
-      <c r="J54" s="100"/>
+      <c r="A54" s="121"/>
+      <c r="B54" s="122"/>
+      <c r="C54" s="122"/>
+      <c r="D54" s="98"/>
+      <c r="E54" s="98"/>
+      <c r="F54" s="98"/>
+      <c r="G54" s="98"/>
+      <c r="H54" s="98"/>
+      <c r="I54" s="98"/>
+      <c r="J54" s="99"/>
     </row>
     <row r="55" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A55" s="78"/>
-      <c r="B55" s="94"/>
+      <c r="B55" s="93"/>
       <c r="C55" s="77"/>
-      <c r="D55" s="119"/>
-      <c r="E55" s="120"/>
-      <c r="F55" s="120"/>
+      <c r="D55" s="123"/>
+      <c r="E55" s="124"/>
+      <c r="F55" s="124"/>
       <c r="G55" s="76"/>
       <c r="H55" s="83"/>
       <c r="I55" s="77"/>
       <c r="J55" s="75"/>
     </row>
     <row r="56" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A56" s="117"/>
-      <c r="B56" s="118"/>
-      <c r="C56" s="118"/>
-      <c r="D56" s="99"/>
-      <c r="E56" s="99"/>
-      <c r="F56" s="99"/>
-      <c r="G56" s="99"/>
-      <c r="H56" s="99"/>
-      <c r="I56" s="99"/>
-      <c r="J56" s="100"/>
+      <c r="A56" s="121"/>
+      <c r="B56" s="122"/>
+      <c r="C56" s="122"/>
+      <c r="D56" s="98"/>
+      <c r="E56" s="98"/>
+      <c r="F56" s="98"/>
+      <c r="G56" s="98"/>
+      <c r="H56" s="98"/>
+      <c r="I56" s="98"/>
+      <c r="J56" s="99"/>
     </row>
     <row r="57" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A57" s="78"/>
-      <c r="B57" s="94"/>
+      <c r="B57" s="93"/>
       <c r="C57" s="77"/>
-      <c r="D57" s="119"/>
-      <c r="E57" s="120"/>
-      <c r="F57" s="120"/>
+      <c r="D57" s="123"/>
+      <c r="E57" s="124"/>
+      <c r="F57" s="124"/>
       <c r="G57" s="76"/>
       <c r="H57" s="83"/>
       <c r="I57" s="77"/>
       <c r="J57" s="75"/>
     </row>
     <row r="58" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A58" s="117"/>
-      <c r="B58" s="118"/>
-      <c r="C58" s="118"/>
-      <c r="D58" s="99"/>
-      <c r="E58" s="99"/>
-      <c r="F58" s="99"/>
-      <c r="G58" s="99"/>
-      <c r="H58" s="99"/>
-      <c r="I58" s="99"/>
-      <c r="J58" s="100"/>
+      <c r="A58" s="121"/>
+      <c r="B58" s="122"/>
+      <c r="C58" s="122"/>
+      <c r="D58" s="98"/>
+      <c r="E58" s="98"/>
+      <c r="F58" s="98"/>
+      <c r="G58" s="98"/>
+      <c r="H58" s="98"/>
+      <c r="I58" s="98"/>
+      <c r="J58" s="99"/>
     </row>
     <row r="59" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A59" s="78"/>
-      <c r="B59" s="94"/>
+      <c r="B59" s="93"/>
       <c r="C59" s="77"/>
-      <c r="D59" s="119"/>
-      <c r="E59" s="120"/>
-      <c r="F59" s="120"/>
+      <c r="D59" s="123"/>
+      <c r="E59" s="124"/>
+      <c r="F59" s="124"/>
       <c r="G59" s="76"/>
       <c r="H59" s="83"/>
       <c r="I59" s="77"/>
       <c r="J59" s="75"/>
     </row>
     <row r="60" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A60" s="117"/>
-      <c r="B60" s="118"/>
-      <c r="C60" s="118"/>
-      <c r="D60" s="99"/>
-      <c r="E60" s="99"/>
-      <c r="F60" s="99"/>
-      <c r="G60" s="99"/>
-      <c r="H60" s="99"/>
-      <c r="I60" s="99"/>
-      <c r="J60" s="100"/>
+      <c r="A60" s="121"/>
+      <c r="B60" s="122"/>
+      <c r="C60" s="122"/>
+      <c r="D60" s="98"/>
+      <c r="E60" s="98"/>
+      <c r="F60" s="98"/>
+      <c r="G60" s="98"/>
+      <c r="H60" s="98"/>
+      <c r="I60" s="98"/>
+      <c r="J60" s="99"/>
     </row>
     <row r="61" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A61" s="78"/>
-      <c r="B61" s="94"/>
+      <c r="B61" s="93"/>
       <c r="C61" s="77"/>
-      <c r="D61" s="119"/>
-      <c r="E61" s="120"/>
-      <c r="F61" s="120"/>
+      <c r="D61" s="123"/>
+      <c r="E61" s="124"/>
+      <c r="F61" s="124"/>
       <c r="G61" s="76"/>
       <c r="H61" s="83"/>
       <c r="I61" s="77"/>
       <c r="J61" s="75"/>
     </row>
     <row r="62" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A62" s="117"/>
-      <c r="B62" s="118"/>
-      <c r="C62" s="118"/>
-      <c r="D62" s="99"/>
-      <c r="E62" s="99"/>
-      <c r="F62" s="99"/>
-      <c r="G62" s="99"/>
-      <c r="H62" s="99"/>
-      <c r="I62" s="99"/>
-      <c r="J62" s="100"/>
+      <c r="A62" s="121"/>
+      <c r="B62" s="122"/>
+      <c r="C62" s="122"/>
+      <c r="D62" s="98"/>
+      <c r="E62" s="98"/>
+      <c r="F62" s="98"/>
+      <c r="G62" s="98"/>
+      <c r="H62" s="98"/>
+      <c r="I62" s="98"/>
+      <c r="J62" s="99"/>
     </row>
     <row r="63" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A63" s="78"/>
-      <c r="B63" s="94"/>
+      <c r="B63" s="93"/>
       <c r="C63" s="77"/>
-      <c r="D63" s="119"/>
-      <c r="E63" s="120"/>
-      <c r="F63" s="120"/>
+      <c r="D63" s="123"/>
+      <c r="E63" s="124"/>
+      <c r="F63" s="124"/>
       <c r="G63" s="76"/>
       <c r="H63" s="83"/>
       <c r="I63" s="77"/>
@@ -4120,78 +4197,227 @@
       <c r="I64"/>
       <c r="J64"/>
     </row>
-    <row r="65" spans="9:10" ht="12" customHeight="1">
+    <row r="65" spans="8:12" ht="12" customHeight="1">
       <c r="I65"/>
       <c r="J65"/>
     </row>
-    <row r="66" spans="9:10" ht="12" customHeight="1">
+    <row r="66" spans="8:12" ht="12" customHeight="1">
       <c r="I66"/>
       <c r="J66"/>
     </row>
-    <row r="67" spans="9:10" ht="12" customHeight="1">
+    <row r="67" spans="8:12" ht="12" customHeight="1">
       <c r="I67"/>
       <c r="J67"/>
     </row>
-    <row r="68" spans="9:10" ht="12" customHeight="1">
+    <row r="68" spans="8:12" ht="12" customHeight="1">
       <c r="I68"/>
       <c r="J68"/>
     </row>
-    <row r="69" spans="9:10" ht="12" customHeight="1">
+    <row r="69" spans="8:12" ht="12" customHeight="1">
       <c r="I69"/>
       <c r="J69"/>
     </row>
-    <row r="70" spans="9:10" ht="12" customHeight="1">
+    <row r="70" spans="8:12" ht="12" customHeight="1">
       <c r="I70"/>
       <c r="J70"/>
     </row>
-    <row r="71" spans="9:10" ht="12" customHeight="1">
+    <row r="71" spans="8:12" ht="12" customHeight="1">
       <c r="I71"/>
       <c r="J71"/>
     </row>
-    <row r="72" spans="9:10" ht="12" customHeight="1">
+    <row r="72" spans="8:12" ht="12" customHeight="1">
       <c r="I72"/>
       <c r="J72"/>
     </row>
-    <row r="73" spans="9:10" ht="12" customHeight="1">
+    <row r="73" spans="8:12" ht="12" customHeight="1">
       <c r="I73"/>
       <c r="J73"/>
     </row>
-    <row r="74" spans="9:10" ht="12" customHeight="1">
+    <row r="74" spans="8:12" ht="12" customHeight="1">
       <c r="I74"/>
       <c r="J74"/>
     </row>
-    <row r="75" spans="9:10" ht="12" customHeight="1">
+    <row r="75" spans="8:12" ht="12" customHeight="1">
       <c r="I75"/>
       <c r="J75"/>
     </row>
-    <row r="76" spans="9:10" ht="12" customHeight="1">
+    <row r="76" spans="8:12" ht="12" customHeight="1">
       <c r="I76"/>
       <c r="J76"/>
     </row>
-    <row r="77" spans="9:10" ht="12" customHeight="1">
+    <row r="77" spans="8:12" ht="12" customHeight="1">
       <c r="I77"/>
       <c r="J77"/>
     </row>
-    <row r="78" spans="9:10" ht="12" customHeight="1">
+    <row r="78" spans="8:12" ht="12" customHeight="1">
       <c r="I78"/>
       <c r="J78"/>
     </row>
-    <row r="79" spans="9:10" ht="12" customHeight="1">
-      <c r="I79"/>
-      <c r="J79"/>
+    <row r="79" spans="8:12" ht="12" customHeight="1">
+      <c r="H79" s="154"/>
+      <c r="I79" s="154"/>
+      <c r="J79" s="154"/>
+      <c r="K79" s="154"/>
+      <c r="L79" s="154"/>
+    </row>
+    <row r="80" spans="8:12">
+      <c r="H80" s="154"/>
+      <c r="I80" s="155"/>
+      <c r="J80" s="154"/>
+      <c r="K80" s="154"/>
+      <c r="L80" s="154"/>
+    </row>
+    <row r="81" spans="8:12">
+      <c r="H81" s="154"/>
+      <c r="I81" s="155"/>
+      <c r="J81" s="154"/>
+      <c r="K81" s="154"/>
+      <c r="L81" s="154"/>
+    </row>
+    <row r="82" spans="8:12">
+      <c r="H82" s="154"/>
+      <c r="I82" s="155"/>
+      <c r="J82" s="154"/>
+      <c r="K82" s="154"/>
+      <c r="L82" s="154"/>
+    </row>
+    <row r="83" spans="8:12">
+      <c r="H83" s="154"/>
+      <c r="I83" s="155"/>
+      <c r="J83" s="154"/>
+      <c r="K83" s="154"/>
+      <c r="L83" s="154"/>
+    </row>
+    <row r="84" spans="8:12">
+      <c r="H84" s="154"/>
+      <c r="I84" s="155"/>
+      <c r="J84" s="154"/>
+      <c r="K84" s="154"/>
+      <c r="L84" s="154"/>
+    </row>
+    <row r="85" spans="8:12">
+      <c r="H85" s="154"/>
+      <c r="I85" s="155"/>
+      <c r="J85" s="154"/>
+      <c r="K85" s="154"/>
+      <c r="L85" s="154"/>
+    </row>
+    <row r="86" spans="8:12">
+      <c r="H86" s="154"/>
+      <c r="I86" s="155"/>
+      <c r="J86" s="154"/>
+      <c r="K86" s="154"/>
+      <c r="L86" s="154"/>
+    </row>
+    <row r="87" spans="8:12">
+      <c r="H87" s="154"/>
+      <c r="I87" s="155"/>
+      <c r="J87" s="154"/>
+      <c r="K87" s="154"/>
+      <c r="L87" s="154"/>
+    </row>
+    <row r="88" spans="8:12">
+      <c r="H88" s="154"/>
+      <c r="I88" s="155"/>
+      <c r="J88" s="154"/>
+      <c r="K88" s="154"/>
+      <c r="L88" s="154"/>
+    </row>
+    <row r="89" spans="8:12">
+      <c r="H89" s="154"/>
+      <c r="I89" s="155"/>
+      <c r="J89" s="154"/>
+      <c r="K89" s="154"/>
+      <c r="L89" s="154"/>
+    </row>
+    <row r="90" spans="8:12">
+      <c r="H90" s="154"/>
+      <c r="I90" s="155"/>
+      <c r="J90" s="154"/>
+      <c r="K90" s="154"/>
+      <c r="L90" s="154"/>
+    </row>
+    <row r="91" spans="8:12">
+      <c r="H91" s="154"/>
+      <c r="I91" s="155"/>
+      <c r="J91" s="154"/>
+      <c r="K91" s="154"/>
+      <c r="L91" s="154"/>
+    </row>
+    <row r="92" spans="8:12">
+      <c r="H92" s="154"/>
+      <c r="I92" s="155"/>
+      <c r="J92" s="154"/>
+      <c r="K92" s="154"/>
+      <c r="L92" s="154"/>
+    </row>
+    <row r="93" spans="8:12">
+      <c r="H93" s="154"/>
+      <c r="I93" s="155"/>
+      <c r="J93" s="154"/>
+      <c r="K93" s="154"/>
+      <c r="L93" s="154"/>
+    </row>
+    <row r="94" spans="8:12">
+      <c r="H94" s="154"/>
+      <c r="I94" s="155"/>
+      <c r="J94" s="154"/>
+      <c r="K94" s="154"/>
+      <c r="L94" s="154"/>
+    </row>
+    <row r="95" spans="8:12">
+      <c r="H95" s="154"/>
+      <c r="I95" s="155"/>
+      <c r="J95" s="154"/>
+      <c r="K95" s="154"/>
+      <c r="L95" s="154"/>
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="D63:F63"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D55:F55"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="D57:F57"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="D51:F51"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="D53:F53"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="B1:D2"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="D22:F22"/>
@@ -4208,50 +4434,16 @@
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="D25:F25"/>
     <mergeCell ref="D28:F28"/>
-    <mergeCell ref="B1:D2"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="D53:F53"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="A60:C60"/>
-    <mergeCell ref="D61:F61"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="D63:F63"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D55:F55"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="D57:F57"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="D59:F59"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="D51:F51"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D18:F18"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4261,11 +4453,800 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38A5C5E9-2A4C-42AB-BB4C-3FA17441B1A7}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:M69"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22:F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="15.625" customWidth="1"/>
+    <col min="2" max="2" width="18.125" customWidth="1"/>
+    <col min="3" max="3" width="42.125" customWidth="1"/>
+    <col min="6" max="6" width="23.625" customWidth="1"/>
+    <col min="7" max="7" width="18.5" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="17.125" customWidth="1"/>
+    <col min="9" max="9" width="8.875" style="85"/>
+    <col min="10" max="10" width="18" style="84" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A1" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="137"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="156"/>
+      <c r="M1" s="156"/>
+    </row>
+    <row r="2" spans="1:13" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
+      <c r="A2" s="7"/>
+      <c r="B2" s="138"/>
+      <c r="C2" s="138"/>
+      <c r="D2" s="138"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="156"/>
+      <c r="M2" s="156"/>
+    </row>
+    <row r="3" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="A3" s="58" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="114" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="114"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="145"/>
+      <c r="I3" s="145"/>
+      <c r="J3" s="145"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="157"/>
+      <c r="M3" s="157"/>
+    </row>
+    <row r="4" spans="1:13" s="3" customFormat="1" ht="12.75">
+      <c r="A4" s="63" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="146" t="s">
+        <v>160</v>
+      </c>
+      <c r="C4" s="147"/>
+      <c r="D4" s="148"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="145"/>
+      <c r="I4" s="145"/>
+      <c r="J4" s="145"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="157"/>
+      <c r="M4" s="157"/>
+    </row>
+    <row r="5" spans="1:13" s="71" customFormat="1" ht="25.5">
+      <c r="A5" s="63" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="140" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="141"/>
+      <c r="D5" s="142"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="144"/>
+      <c r="I5" s="144"/>
+      <c r="J5" s="144"/>
+      <c r="K5" s="70"/>
+      <c r="L5" s="158"/>
+      <c r="M5" s="158"/>
+    </row>
+    <row r="6" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="A6" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="80">
+        <f>COUNTIF(I12:I28,"Pass")</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="13">
+        <f>COUNTIF(I10:I734,"Pending")</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="145"/>
+      <c r="I6" s="145"/>
+      <c r="J6" s="145"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="157"/>
+      <c r="M6" s="157"/>
+    </row>
+    <row r="7" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
+      <c r="A7" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="81">
+        <f>COUNTIF(I12:I28,"Fail")</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="59">
+        <f>COUNTA(A12:A37) -2</f>
+        <v>2</v>
+      </c>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="145"/>
+      <c r="I7" s="145"/>
+      <c r="J7" s="145"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="157"/>
+      <c r="M7" s="157"/>
+    </row>
+    <row r="8" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="A8" s="139"/>
+      <c r="B8" s="139"/>
+      <c r="C8" s="139"/>
+      <c r="D8" s="139"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="92"/>
+      <c r="J8" s="92"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="157"/>
+      <c r="M8" s="157"/>
+    </row>
+    <row r="9" spans="1:13" s="73" customFormat="1" ht="12" customHeight="1">
+      <c r="A9" s="128" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="152" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="128" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="129" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="130"/>
+      <c r="F9" s="130"/>
+      <c r="G9" s="131"/>
+      <c r="H9" s="149" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="125" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" s="125" t="s">
+        <v>32</v>
+      </c>
+      <c r="K9" s="72"/>
+    </row>
+    <row r="10" spans="1:13" s="3" customFormat="1" ht="12" customHeight="1">
+      <c r="A10" s="125"/>
+      <c r="B10" s="153"/>
+      <c r="C10" s="125"/>
+      <c r="D10" s="132"/>
+      <c r="E10" s="133"/>
+      <c r="F10" s="133"/>
+      <c r="G10" s="134"/>
+      <c r="H10" s="132"/>
+      <c r="I10" s="125"/>
+      <c r="J10" s="125"/>
+      <c r="K10" s="9"/>
+    </row>
+    <row r="11" spans="1:13" s="74" customFormat="1" ht="15">
+      <c r="A11" s="150"/>
+      <c r="B11" s="150"/>
+      <c r="C11" s="150"/>
+      <c r="D11" s="150"/>
+      <c r="E11" s="150"/>
+      <c r="F11" s="150"/>
+      <c r="G11" s="150"/>
+      <c r="H11" s="150"/>
+      <c r="I11" s="150"/>
+      <c r="J11" s="151"/>
+    </row>
+    <row r="12" spans="1:13" s="4" customFormat="1" ht="12.75">
+      <c r="A12" s="135" t="s">
+        <v>161</v>
+      </c>
+      <c r="B12" s="136"/>
+      <c r="C12" s="136"/>
+      <c r="D12" s="136"/>
+      <c r="E12" s="136"/>
+      <c r="F12" s="136"/>
+      <c r="G12" s="136"/>
+      <c r="H12" s="136"/>
+      <c r="I12" s="136"/>
+      <c r="J12" s="143"/>
+    </row>
+    <row r="13" spans="1:13" s="4" customFormat="1" ht="102.75" customHeight="1" outlineLevel="1">
+      <c r="A13" s="78"/>
+      <c r="B13" s="82"/>
+      <c r="C13" s="77"/>
+      <c r="D13" s="116"/>
+      <c r="E13" s="117"/>
+      <c r="F13" s="117"/>
+      <c r="G13" s="76"/>
+      <c r="H13" s="90"/>
+      <c r="I13" s="77"/>
+      <c r="J13" s="75"/>
+    </row>
+    <row r="14" spans="1:13" s="4" customFormat="1" ht="57.75" customHeight="1" outlineLevel="1">
+      <c r="A14" s="78"/>
+      <c r="B14" s="82"/>
+      <c r="C14" s="77"/>
+      <c r="D14" s="116"/>
+      <c r="E14" s="117"/>
+      <c r="F14" s="117"/>
+      <c r="G14" s="76"/>
+      <c r="H14" s="90"/>
+      <c r="I14" s="77"/>
+      <c r="J14" s="75"/>
+    </row>
+    <row r="15" spans="1:13" s="4" customFormat="1" ht="66.75" customHeight="1" outlineLevel="1">
+      <c r="A15" s="78"/>
+      <c r="B15" s="82"/>
+      <c r="C15" s="77"/>
+      <c r="D15" s="116"/>
+      <c r="E15" s="117"/>
+      <c r="F15" s="117"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="90"/>
+      <c r="I15" s="77"/>
+      <c r="J15" s="75"/>
+    </row>
+    <row r="16" spans="1:13" s="4" customFormat="1" ht="66.75" customHeight="1" outlineLevel="1">
+      <c r="A16" s="78"/>
+      <c r="B16" s="82"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="116"/>
+      <c r="E16" s="117"/>
+      <c r="F16" s="117"/>
+      <c r="G16" s="76"/>
+      <c r="H16" s="90"/>
+      <c r="I16" s="77"/>
+      <c r="J16" s="75"/>
+    </row>
+    <row r="17" spans="1:10" s="4" customFormat="1" ht="93.75" customHeight="1" outlineLevel="1">
+      <c r="A17" s="78"/>
+      <c r="B17" s="82"/>
+      <c r="C17" s="77"/>
+      <c r="D17" s="116"/>
+      <c r="E17" s="117"/>
+      <c r="F17" s="117"/>
+      <c r="G17" s="76"/>
+      <c r="H17" s="90"/>
+      <c r="I17" s="77"/>
+      <c r="J17" s="75"/>
+    </row>
+    <row r="18" spans="1:10" s="4" customFormat="1" ht="93.75" customHeight="1" outlineLevel="1">
+      <c r="A18" s="78"/>
+      <c r="B18" s="82"/>
+      <c r="C18" s="77"/>
+      <c r="D18" s="116"/>
+      <c r="E18" s="117"/>
+      <c r="F18" s="117"/>
+      <c r="G18" s="76"/>
+      <c r="H18" s="90"/>
+      <c r="I18" s="77"/>
+      <c r="J18" s="75"/>
+    </row>
+    <row r="19" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
+      <c r="A19" s="135" t="s">
+        <v>162</v>
+      </c>
+      <c r="B19" s="136"/>
+      <c r="C19" s="136"/>
+      <c r="D19" s="88"/>
+      <c r="E19" s="88"/>
+      <c r="F19" s="88"/>
+      <c r="G19" s="88"/>
+      <c r="H19" s="88"/>
+      <c r="I19" s="88"/>
+      <c r="J19" s="89"/>
+    </row>
+    <row r="20" spans="1:10" s="4" customFormat="1" ht="90.75" customHeight="1" outlineLevel="1">
+      <c r="A20" s="94" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="86" t="s">
+        <v>163</v>
+      </c>
+      <c r="C20" s="87" t="s">
+        <v>165</v>
+      </c>
+      <c r="D20" s="126"/>
+      <c r="E20" s="127"/>
+      <c r="F20" s="127"/>
+      <c r="G20" s="95"/>
+      <c r="H20" s="96"/>
+      <c r="I20" s="87"/>
+      <c r="J20" s="97"/>
+    </row>
+    <row r="21" spans="1:10" s="4" customFormat="1" ht="91.5" customHeight="1" outlineLevel="1">
+      <c r="A21" s="94" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="86" t="s">
+        <v>164</v>
+      </c>
+      <c r="C21" s="87" t="s">
+        <v>166</v>
+      </c>
+      <c r="D21" s="126"/>
+      <c r="E21" s="127"/>
+      <c r="F21" s="127"/>
+      <c r="G21" s="95"/>
+      <c r="H21" s="96"/>
+      <c r="I21" s="87"/>
+      <c r="J21" s="97"/>
+    </row>
+    <row r="22" spans="1:10" s="4" customFormat="1" ht="68.25" customHeight="1" outlineLevel="1">
+      <c r="A22" s="94"/>
+      <c r="B22" s="86"/>
+      <c r="C22" s="87"/>
+      <c r="D22" s="126"/>
+      <c r="E22" s="127"/>
+      <c r="F22" s="127"/>
+      <c r="G22" s="95"/>
+      <c r="H22" s="96"/>
+      <c r="I22" s="87"/>
+      <c r="J22" s="97"/>
+    </row>
+    <row r="23" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
+      <c r="A23" s="135"/>
+      <c r="B23" s="136"/>
+      <c r="C23" s="136"/>
+      <c r="D23" s="88"/>
+      <c r="E23" s="88"/>
+      <c r="F23" s="88"/>
+      <c r="G23" s="88"/>
+      <c r="H23" s="88"/>
+      <c r="I23" s="88"/>
+      <c r="J23" s="89"/>
+    </row>
+    <row r="24" spans="1:10" s="4" customFormat="1" ht="116.25" customHeight="1" outlineLevel="1">
+      <c r="A24" s="78"/>
+      <c r="B24" s="93"/>
+      <c r="C24" s="77"/>
+      <c r="D24" s="123"/>
+      <c r="E24" s="124"/>
+      <c r="F24" s="124"/>
+      <c r="G24" s="76"/>
+      <c r="H24" s="83"/>
+      <c r="I24" s="77"/>
+      <c r="J24" s="75"/>
+    </row>
+    <row r="25" spans="1:10" s="4" customFormat="1" ht="67.5" customHeight="1" outlineLevel="1">
+      <c r="A25" s="78"/>
+      <c r="B25" s="82"/>
+      <c r="C25" s="77"/>
+      <c r="D25" s="123"/>
+      <c r="E25" s="124"/>
+      <c r="F25" s="124"/>
+      <c r="G25" s="76"/>
+      <c r="H25" s="83"/>
+      <c r="I25" s="77"/>
+      <c r="J25" s="75"/>
+    </row>
+    <row r="26" spans="1:10" s="4" customFormat="1" ht="81" customHeight="1" outlineLevel="1">
+      <c r="A26" s="78"/>
+      <c r="B26" s="93"/>
+      <c r="C26" s="77"/>
+      <c r="D26" s="123"/>
+      <c r="E26" s="124"/>
+      <c r="F26" s="124"/>
+      <c r="G26" s="76"/>
+      <c r="H26" s="83"/>
+      <c r="I26" s="77"/>
+      <c r="J26" s="75"/>
+    </row>
+    <row r="27" spans="1:10" s="4" customFormat="1" ht="93" customHeight="1" outlineLevel="1">
+      <c r="A27" s="78"/>
+      <c r="B27" s="93"/>
+      <c r="C27" s="77"/>
+      <c r="D27" s="123"/>
+      <c r="E27" s="124"/>
+      <c r="F27" s="124"/>
+      <c r="G27" s="76"/>
+      <c r="H27" s="83"/>
+      <c r="I27" s="77"/>
+      <c r="J27" s="75"/>
+    </row>
+    <row r="28" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A28" s="78"/>
+      <c r="B28" s="93"/>
+      <c r="C28" s="77"/>
+      <c r="D28" s="123"/>
+      <c r="E28" s="124"/>
+      <c r="F28" s="124"/>
+      <c r="G28" s="76"/>
+      <c r="H28" s="83"/>
+      <c r="I28" s="77"/>
+      <c r="J28" s="75"/>
+    </row>
+    <row r="29" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
+      <c r="A29" s="121"/>
+      <c r="B29" s="122"/>
+      <c r="C29" s="122"/>
+      <c r="D29" s="98"/>
+      <c r="E29" s="98"/>
+      <c r="F29" s="98"/>
+      <c r="G29" s="98"/>
+      <c r="H29" s="98"/>
+      <c r="I29" s="98"/>
+      <c r="J29" s="99"/>
+    </row>
+    <row r="30" spans="1:10" s="4" customFormat="1" ht="78.75" customHeight="1" outlineLevel="1">
+      <c r="A30" s="78"/>
+      <c r="B30" s="93"/>
+      <c r="C30" s="77"/>
+      <c r="D30" s="123"/>
+      <c r="E30" s="124"/>
+      <c r="F30" s="124"/>
+      <c r="G30" s="76"/>
+      <c r="H30" s="83"/>
+      <c r="I30" s="77"/>
+      <c r="J30" s="75"/>
+    </row>
+    <row r="31" spans="1:10" s="4" customFormat="1" ht="79.5" customHeight="1" outlineLevel="1">
+      <c r="A31" s="78"/>
+      <c r="B31" s="93"/>
+      <c r="C31" s="77"/>
+      <c r="D31" s="123"/>
+      <c r="E31" s="124"/>
+      <c r="F31" s="124"/>
+      <c r="G31" s="76"/>
+      <c r="H31" s="83"/>
+      <c r="I31" s="77"/>
+      <c r="J31" s="75"/>
+    </row>
+    <row r="32" spans="1:10" s="4" customFormat="1" ht="79.5" customHeight="1" outlineLevel="1">
+      <c r="A32" s="78"/>
+      <c r="B32" s="93"/>
+      <c r="C32" s="77"/>
+      <c r="D32" s="123"/>
+      <c r="E32" s="124"/>
+      <c r="F32" s="124"/>
+      <c r="G32" s="76"/>
+      <c r="H32" s="83"/>
+      <c r="I32" s="77"/>
+      <c r="J32" s="75"/>
+    </row>
+    <row r="33" spans="1:10" s="4" customFormat="1" ht="79.5" customHeight="1" outlineLevel="1">
+      <c r="A33" s="78"/>
+      <c r="B33" s="93"/>
+      <c r="C33" s="77"/>
+      <c r="D33" s="123"/>
+      <c r="E33" s="124"/>
+      <c r="F33" s="124"/>
+      <c r="G33" s="76"/>
+      <c r="H33" s="83"/>
+      <c r="I33" s="77"/>
+      <c r="J33" s="75"/>
+    </row>
+    <row r="34" spans="1:10" s="4" customFormat="1" ht="91.5" customHeight="1" outlineLevel="1">
+      <c r="A34" s="78"/>
+      <c r="B34" s="93"/>
+      <c r="C34" s="77"/>
+      <c r="D34" s="123"/>
+      <c r="E34" s="124"/>
+      <c r="F34" s="124"/>
+      <c r="G34" s="76"/>
+      <c r="H34" s="83"/>
+      <c r="I34" s="77"/>
+      <c r="J34" s="75"/>
+    </row>
+    <row r="35" spans="1:10" s="4" customFormat="1" ht="67.5" customHeight="1" outlineLevel="1">
+      <c r="A35" s="78"/>
+      <c r="B35" s="93"/>
+      <c r="C35" s="77"/>
+      <c r="D35" s="123"/>
+      <c r="E35" s="124"/>
+      <c r="F35" s="124"/>
+      <c r="G35" s="76"/>
+      <c r="H35" s="83"/>
+      <c r="I35" s="77"/>
+      <c r="J35" s="75"/>
+    </row>
+    <row r="36" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
+      <c r="A36" s="121"/>
+      <c r="B36" s="122"/>
+      <c r="C36" s="122"/>
+      <c r="D36" s="98"/>
+      <c r="E36" s="98"/>
+      <c r="F36" s="98"/>
+      <c r="G36" s="98"/>
+      <c r="H36" s="98"/>
+      <c r="I36" s="98"/>
+      <c r="J36" s="99"/>
+    </row>
+    <row r="37" spans="1:10" s="4" customFormat="1" ht="47.25" customHeight="1" outlineLevel="1">
+      <c r="A37" s="78"/>
+      <c r="B37" s="93"/>
+      <c r="C37" s="77"/>
+      <c r="D37" s="123"/>
+      <c r="E37" s="124"/>
+      <c r="F37" s="124"/>
+      <c r="G37" s="76"/>
+      <c r="H37" s="83"/>
+      <c r="I37" s="77"/>
+      <c r="J37" s="75"/>
+    </row>
+    <row r="38" spans="1:10" ht="12" customHeight="1">
+      <c r="I38"/>
+      <c r="J38"/>
+    </row>
+    <row r="39" spans="1:10" ht="12" customHeight="1">
+      <c r="I39"/>
+      <c r="J39"/>
+    </row>
+    <row r="40" spans="1:10" ht="12" customHeight="1">
+      <c r="I40"/>
+      <c r="J40"/>
+    </row>
+    <row r="41" spans="1:10" ht="12" customHeight="1">
+      <c r="I41"/>
+      <c r="J41"/>
+    </row>
+    <row r="42" spans="1:10" ht="12" customHeight="1">
+      <c r="I42"/>
+      <c r="J42"/>
+    </row>
+    <row r="43" spans="1:10" ht="12" customHeight="1">
+      <c r="I43"/>
+      <c r="J43"/>
+    </row>
+    <row r="44" spans="1:10" ht="12" customHeight="1">
+      <c r="I44"/>
+      <c r="J44"/>
+    </row>
+    <row r="45" spans="1:10" ht="12" customHeight="1">
+      <c r="I45"/>
+      <c r="J45"/>
+    </row>
+    <row r="46" spans="1:10" ht="12" customHeight="1">
+      <c r="I46"/>
+      <c r="J46"/>
+    </row>
+    <row r="47" spans="1:10" ht="12" customHeight="1">
+      <c r="I47"/>
+      <c r="J47"/>
+    </row>
+    <row r="48" spans="1:10" ht="12" customHeight="1">
+      <c r="I48"/>
+      <c r="J48"/>
+    </row>
+    <row r="49" spans="8:12" ht="12" customHeight="1">
+      <c r="I49"/>
+      <c r="J49"/>
+    </row>
+    <row r="50" spans="8:12" ht="12" customHeight="1">
+      <c r="I50"/>
+      <c r="J50"/>
+    </row>
+    <row r="51" spans="8:12" ht="12" customHeight="1">
+      <c r="I51"/>
+      <c r="J51"/>
+    </row>
+    <row r="52" spans="8:12" ht="12" customHeight="1">
+      <c r="I52"/>
+      <c r="J52"/>
+    </row>
+    <row r="53" spans="8:12" ht="12" customHeight="1">
+      <c r="H53" s="154"/>
+      <c r="I53" s="154"/>
+      <c r="J53" s="154"/>
+      <c r="K53" s="154"/>
+      <c r="L53" s="154"/>
+    </row>
+    <row r="54" spans="8:12">
+      <c r="H54" s="154"/>
+      <c r="I54" s="155"/>
+      <c r="J54" s="154"/>
+      <c r="K54" s="154"/>
+      <c r="L54" s="154"/>
+    </row>
+    <row r="55" spans="8:12">
+      <c r="H55" s="154"/>
+      <c r="I55" s="155"/>
+      <c r="J55" s="154"/>
+      <c r="K55" s="154"/>
+      <c r="L55" s="154"/>
+    </row>
+    <row r="56" spans="8:12">
+      <c r="H56" s="154"/>
+      <c r="I56" s="155"/>
+      <c r="J56" s="154"/>
+      <c r="K56" s="154"/>
+      <c r="L56" s="154"/>
+    </row>
+    <row r="57" spans="8:12">
+      <c r="H57" s="154"/>
+      <c r="I57" s="155"/>
+      <c r="J57" s="154"/>
+      <c r="K57" s="154"/>
+      <c r="L57" s="154"/>
+    </row>
+    <row r="58" spans="8:12">
+      <c r="H58" s="154"/>
+      <c r="I58" s="155"/>
+      <c r="J58" s="154"/>
+      <c r="K58" s="154"/>
+      <c r="L58" s="154"/>
+    </row>
+    <row r="59" spans="8:12">
+      <c r="H59" s="154"/>
+      <c r="I59" s="155"/>
+      <c r="J59" s="154"/>
+      <c r="K59" s="154"/>
+      <c r="L59" s="154"/>
+    </row>
+    <row r="60" spans="8:12">
+      <c r="H60" s="154"/>
+      <c r="I60" s="155"/>
+      <c r="J60" s="154"/>
+      <c r="K60" s="154"/>
+      <c r="L60" s="154"/>
+    </row>
+    <row r="61" spans="8:12">
+      <c r="H61" s="154"/>
+      <c r="I61" s="155"/>
+      <c r="J61" s="154"/>
+      <c r="K61" s="154"/>
+      <c r="L61" s="154"/>
+    </row>
+    <row r="62" spans="8:12">
+      <c r="H62" s="154"/>
+      <c r="I62" s="155"/>
+      <c r="J62" s="154"/>
+      <c r="K62" s="154"/>
+      <c r="L62" s="154"/>
+    </row>
+    <row r="63" spans="8:12">
+      <c r="H63" s="154"/>
+      <c r="I63" s="155"/>
+      <c r="J63" s="154"/>
+      <c r="K63" s="154"/>
+      <c r="L63" s="154"/>
+    </row>
+    <row r="64" spans="8:12">
+      <c r="H64" s="154"/>
+      <c r="I64" s="155"/>
+      <c r="J64" s="154"/>
+      <c r="K64" s="154"/>
+      <c r="L64" s="154"/>
+    </row>
+    <row r="65" spans="8:12">
+      <c r="H65" s="154"/>
+      <c r="I65" s="155"/>
+      <c r="J65" s="154"/>
+      <c r="K65" s="154"/>
+      <c r="L65" s="154"/>
+    </row>
+    <row r="66" spans="8:12">
+      <c r="H66" s="154"/>
+      <c r="I66" s="155"/>
+      <c r="J66" s="154"/>
+      <c r="K66" s="154"/>
+      <c r="L66" s="154"/>
+    </row>
+    <row r="67" spans="8:12">
+      <c r="H67" s="154"/>
+      <c r="I67" s="155"/>
+      <c r="J67" s="154"/>
+      <c r="K67" s="154"/>
+      <c r="L67" s="154"/>
+    </row>
+    <row r="68" spans="8:12">
+      <c r="H68" s="154"/>
+      <c r="I68" s="155"/>
+      <c r="J68" s="154"/>
+      <c r="K68" s="154"/>
+      <c r="L68" s="154"/>
+    </row>
+    <row r="69" spans="8:12">
+      <c r="H69" s="154"/>
+      <c r="I69" s="155"/>
+      <c r="J69" s="154"/>
+      <c r="K69" s="154"/>
+      <c r="L69" s="154"/>
+    </row>
+  </sheetData>
+  <mergeCells count="44">
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="B1:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="H5:J5"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
@@ -4308,7 +5289,9 @@
       <c r="B4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="91"/>
+      <c r="C4" s="161">
+        <v>45731</v>
+      </c>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
@@ -4379,78 +5362,104 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14.25">
-      <c r="A9" s="19"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="68"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="33"/>
+    <row r="9" spans="1:7" s="60" customFormat="1" ht="14.25">
+      <c r="A9" s="64"/>
+      <c r="B9" s="65">
+        <v>2</v>
+      </c>
+      <c r="C9" s="66" t="str">
+        <f>Samples2!B4</f>
+        <v>Đăng ký tham gia</v>
+      </c>
+      <c r="D9" s="159">
+        <f>Samples2!B6</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="160">
+        <f>Samples2!B7</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="160">
+        <f>Samples2!D6</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="67">
+        <f>Samples2!D7</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="14.25">
       <c r="A10" s="19"/>
-      <c r="B10" s="52"/>
-      <c r="C10" s="53" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="54">
-        <f>SUM(D6:D9)</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="54">
-        <f>SUM(E6:E9)</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="54">
-        <f>SUM(F6:F9)</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="55">
-        <f>SUM(G6:G9)</f>
-        <v>32</v>
-      </c>
+      <c r="B10" s="32"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="33"/>
     </row>
     <row r="11" spans="1:7" ht="14.25">
       <c r="A11" s="19"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="53" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="54">
+        <f>SUM(D6:D10)</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="54">
+        <f>SUM(E6:E10)</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="54">
+        <f>SUM(F6:F10)</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="55">
+        <f>SUM(G6:G10)</f>
+        <v>34</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="14.25">
       <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="23">
-        <f>(D10+E10)*100/G10</f>
-        <v>0</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="24"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
     </row>
     <row r="13" spans="1:7" ht="14.25">
       <c r="A13" s="19"/>
       <c r="B13" s="19"/>
       <c r="C13" s="19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="23">
-        <f>D10*100/G10</f>
+        <f>(D11+E11)*100/G11</f>
         <v>0</v>
       </c>
       <c r="F13" s="19" t="s">
         <v>22</v>
       </c>
       <c r="G13" s="24"/>
+    </row>
+    <row r="14" spans="1:7" ht="14.25">
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="19"/>
+      <c r="E14" s="23">
+        <f>D11*100/G11</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="24"/>
     </row>
   </sheetData>
   <phoneticPr fontId="13"/>

</xml_diff>

<commit_message>
up tc xem ds user
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University_IT\Tam\KiemThuPhanMem\event-manager-javafx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8A899B-20BA-492F-8BCA-5D07D47F73C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688289DC-7AE4-4DB3-9D41-8C2EF28DFCC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="183">
   <si>
     <t>TC1</t>
   </si>
@@ -570,9 +570,6 @@
 3: Chuyển hướng đến trang chi tiết sự kiện</t>
   </si>
   <si>
-    <t>Kiểm tra khả năng hiển thị đầy đủ thông tin sự kiện</t>
-  </si>
-  <si>
     <t>1.1</t>
   </si>
   <si>
@@ -665,9 +662,6 @@
     <t>Cập nhật TC Kiểm tra chức năng tạo sự kiện thành công</t>
   </si>
   <si>
-    <t>1.2</t>
-  </si>
-  <si>
     <t>Đăng ký tham gia</t>
   </si>
   <si>
@@ -699,7 +693,71 @@
 6: Hiển thị thông báo lỗi không thể hủy đăng ký sự kiện này</t>
   </si>
   <si>
-    <t>1.3</t>
+    <t>Viết TC Kiểm tra hủy đăng ký trong thời gian cho phép</t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra hủy đăng ký trong thời gian không cho phép</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>Kiểm tra khả năng hiển thị đầy đủ thông tin của một sự kiện</t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra khả năng hiển thị đầy đủ thông tin của một sự kiện</t>
+  </si>
+  <si>
+    <t>3. Xem danh sách người dùng</t>
+  </si>
+  <si>
+    <t>B1: Đăng nhập với tư cách là admin
+B2: Truy cập vào Trang Quản Trị
+B3: Chọn mục Quản lý người dùng
+B4: Hiển thị danh sách của người dùng</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng hiển thị danh sách người dùng với tài khoản admin</t>
+  </si>
+  <si>
+    <t>B1: Đăng nhập với tư cách là user
+B2: Truy cập vào Trang Quản Trị, mục Quản lý người dùng thông qua đường dẫn URL
+B4: Hiển thị thông báo lỗi hoặc không tìm thấy trang chủ</t>
+  </si>
+  <si>
+    <t>B1: Đăng nhập với tư cách là admin
+B2: Truy cập vào Trang Quản Trị
+B3: Chọn mục Quản lý người dùng
+B4: Chọn một user bất kỳ và nhấn vào nút Chi tiết hoặc icon thông tin
+B5: Hiển thị thông tin chi tiết của user đã chọn</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng hiển thị danh sách người dùng với tài khoản của</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng hiển thị thông tin chi tiết của một người dùng</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng tìm kiếm người dùng</t>
+  </si>
+  <si>
+    <t>B1: Đăng nhập với tư cách là admin
+B2: Truy cập vào Trang Quản Trị
+B3: Chọn mục Quản lý người dùng
+B4: Nhập từ khóa cần tìm vào ô tìm kiếm(tên đăng nhậo, email, tên)
+B5: Hiển thị các user phù hợp với kết quả tìm kiếm</t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra chức năng hiển thị danh sách người dùng với tài khoản admin</t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra chức năng hiển thị danh sách người dùng với tài khoản của</t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra chức năng hiển thị thông tin chi tiết của một người dùng</t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra chức năng tìm kiếm người dùng</t>
   </si>
 </sst>
 </file>
@@ -1405,7 +1463,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1700,6 +1758,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1819,22 +1886,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1843,7 +1894,18 @@
     <cellStyle name="Normal_Sheet1_Vanco_CR022a1_TestCase_v0.1" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="標準_結合試験(AllOvertheWorld)" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2158,8 +2220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H72"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+    <sheetView showGridLines="0" topLeftCell="A11" zoomScale="85" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -2226,11 +2288,11 @@
       <c r="B6" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="114" t="s">
+      <c r="C6" s="117" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="114"/>
-      <c r="E6" s="115"/>
+      <c r="D6" s="117"/>
+      <c r="E6" s="118"/>
       <c r="F6" s="110"/>
       <c r="G6" s="25"/>
     </row>
@@ -2239,11 +2301,11 @@
       <c r="B7" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="114" t="s">
+      <c r="C7" s="117" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="114"/>
-      <c r="E7" s="115"/>
+      <c r="D7" s="117"/>
+      <c r="E7" s="118"/>
       <c r="F7" s="110"/>
       <c r="G7" s="25"/>
     </row>
@@ -2336,7 +2398,7 @@
       </c>
       <c r="D14" s="40"/>
       <c r="E14" s="102" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F14" s="112" t="s">
         <v>44</v>
@@ -2395,7 +2457,7 @@
       <c r="G17" s="40"/>
       <c r="H17" s="41"/>
     </row>
-    <row r="18" spans="2:8" s="34" customFormat="1" ht="25.5">
+    <row r="18" spans="2:8" s="34" customFormat="1" ht="38.25">
       <c r="B18" s="36">
         <v>45738</v>
       </c>
@@ -2519,7 +2581,7 @@
         <v>45738</v>
       </c>
       <c r="C25" s="37" t="s">
-        <v>40</v>
+        <v>135</v>
       </c>
       <c r="D25" s="101"/>
       <c r="E25" s="102" t="s">
@@ -2536,7 +2598,7 @@
         <v>45738</v>
       </c>
       <c r="C26" s="37" t="s">
-        <v>40</v>
+        <v>135</v>
       </c>
       <c r="D26" s="101"/>
       <c r="E26" s="106" t="s">
@@ -2689,11 +2751,11 @@
         <v>45744</v>
       </c>
       <c r="C35" s="37" t="s">
-        <v>136</v>
+        <v>40</v>
       </c>
       <c r="D35" s="101"/>
       <c r="E35" s="106" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F35" s="112" t="s">
         <v>44</v>
@@ -2706,11 +2768,11 @@
         <v>45744</v>
       </c>
       <c r="C36" s="37" t="s">
-        <v>136</v>
+        <v>40</v>
       </c>
       <c r="D36" s="101"/>
       <c r="E36" s="106" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F36" s="112" t="s">
         <v>44</v>
@@ -2723,11 +2785,11 @@
         <v>45744</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>136</v>
+        <v>40</v>
       </c>
       <c r="D37" s="101"/>
       <c r="E37" s="106" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F37" s="112" t="s">
         <v>44</v>
@@ -2740,11 +2802,11 @@
         <v>45744</v>
       </c>
       <c r="C38" s="37" t="s">
-        <v>136</v>
+        <v>40</v>
       </c>
       <c r="D38" s="101"/>
       <c r="E38" s="106" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F38" s="112" t="s">
         <v>44</v>
@@ -2757,11 +2819,11 @@
         <v>45744</v>
       </c>
       <c r="C39" s="37" t="s">
-        <v>136</v>
+        <v>40</v>
       </c>
       <c r="D39" s="101"/>
       <c r="E39" s="106" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F39" s="112" t="s">
         <v>44</v>
@@ -2774,11 +2836,11 @@
         <v>45744</v>
       </c>
       <c r="C40" s="37" t="s">
-        <v>136</v>
+        <v>40</v>
       </c>
       <c r="D40" s="101"/>
       <c r="E40" s="106" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F40" s="112" t="s">
         <v>44</v>
@@ -2791,11 +2853,11 @@
         <v>45744</v>
       </c>
       <c r="C41" s="37" t="s">
-        <v>136</v>
+        <v>40</v>
       </c>
       <c r="D41" s="101"/>
       <c r="E41" s="106" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
       <c r="F41" s="112" t="s">
         <v>44</v>
@@ -2808,11 +2870,11 @@
         <v>45745</v>
       </c>
       <c r="C42" s="37" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="D42" s="101"/>
       <c r="E42" s="106" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F42" s="112" t="s">
         <v>44</v>
@@ -2825,11 +2887,11 @@
         <v>45745</v>
       </c>
       <c r="C43" s="37" t="s">
-        <v>159</v>
+        <v>40</v>
       </c>
       <c r="D43" s="101"/>
       <c r="E43" s="106" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F43" s="112" t="s">
         <v>44</v>
@@ -2842,11 +2904,11 @@
         <v>45745</v>
       </c>
       <c r="C44" s="37" t="s">
-        <v>159</v>
+        <v>40</v>
       </c>
       <c r="D44" s="101"/>
       <c r="E44" s="106" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F44" s="112" t="s">
         <v>44</v>
@@ -2859,11 +2921,11 @@
         <v>45745</v>
       </c>
       <c r="C45" s="37" t="s">
-        <v>159</v>
+        <v>40</v>
       </c>
       <c r="D45" s="101"/>
       <c r="E45" s="106" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F45" s="112" t="s">
         <v>44</v>
@@ -2876,11 +2938,11 @@
         <v>45745</v>
       </c>
       <c r="C46" s="37" t="s">
-        <v>159</v>
+        <v>40</v>
       </c>
       <c r="D46" s="101"/>
       <c r="E46" s="106" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F46" s="112" t="s">
         <v>44</v>
@@ -2893,11 +2955,11 @@
         <v>45746</v>
       </c>
       <c r="C47" s="37" t="s">
-        <v>167</v>
+        <v>40</v>
       </c>
       <c r="D47" s="101"/>
       <c r="E47" s="106" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="F47" s="112" t="s">
         <v>44</v>
@@ -2910,11 +2972,11 @@
         <v>45746</v>
       </c>
       <c r="C48" s="37" t="s">
-        <v>167</v>
+        <v>40</v>
       </c>
       <c r="D48" s="101"/>
       <c r="E48" s="106" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="F48" s="112" t="s">
         <v>44</v>
@@ -2922,39 +2984,71 @@
       <c r="G48" s="101"/>
       <c r="H48" s="107"/>
     </row>
-    <row r="49" spans="2:8" s="34" customFormat="1">
-      <c r="B49" s="36"/>
-      <c r="C49" s="37"/>
+    <row r="49" spans="2:8" s="34" customFormat="1" ht="25.5">
+      <c r="B49" s="36">
+        <v>45749</v>
+      </c>
+      <c r="C49" s="37" t="s">
+        <v>40</v>
+      </c>
       <c r="D49" s="101"/>
-      <c r="E49" s="106"/>
-      <c r="F49" s="112"/>
+      <c r="E49" s="106" t="s">
+        <v>179</v>
+      </c>
+      <c r="F49" s="112" t="s">
+        <v>44</v>
+      </c>
       <c r="G49" s="101"/>
       <c r="H49" s="107"/>
     </row>
-    <row r="50" spans="2:8" s="34" customFormat="1">
-      <c r="B50" s="36"/>
-      <c r="C50" s="37"/>
+    <row r="50" spans="2:8" s="34" customFormat="1" ht="25.5">
+      <c r="B50" s="36">
+        <v>45749</v>
+      </c>
+      <c r="C50" s="37" t="s">
+        <v>40</v>
+      </c>
       <c r="D50" s="101"/>
-      <c r="E50" s="106"/>
-      <c r="F50" s="112"/>
+      <c r="E50" s="106" t="s">
+        <v>180</v>
+      </c>
+      <c r="F50" s="112" t="s">
+        <v>44</v>
+      </c>
       <c r="G50" s="101"/>
       <c r="H50" s="107"/>
     </row>
-    <row r="51" spans="2:8" s="34" customFormat="1">
-      <c r="B51" s="36"/>
-      <c r="C51" s="37"/>
+    <row r="51" spans="2:8" s="34" customFormat="1" ht="25.5">
+      <c r="B51" s="36">
+        <v>45749</v>
+      </c>
+      <c r="C51" s="37" t="s">
+        <v>40</v>
+      </c>
       <c r="D51" s="101"/>
-      <c r="E51" s="106"/>
-      <c r="F51" s="112"/>
+      <c r="E51" s="106" t="s">
+        <v>181</v>
+      </c>
+      <c r="F51" s="112" t="s">
+        <v>44</v>
+      </c>
       <c r="G51" s="101"/>
       <c r="H51" s="107"/>
     </row>
-    <row r="52" spans="2:8" s="34" customFormat="1">
-      <c r="B52" s="36"/>
-      <c r="C52" s="37"/>
+    <row r="52" spans="2:8" s="34" customFormat="1" ht="25.5">
+      <c r="B52" s="36">
+        <v>45749</v>
+      </c>
+      <c r="C52" s="37" t="s">
+        <v>40</v>
+      </c>
       <c r="D52" s="101"/>
-      <c r="E52" s="106"/>
-      <c r="F52" s="112"/>
+      <c r="E52" s="106" t="s">
+        <v>182</v>
+      </c>
+      <c r="F52" s="112" t="s">
+        <v>44</v>
+      </c>
       <c r="G52" s="101"/>
       <c r="H52" s="107"/>
     </row>
@@ -3144,11 +3238,17 @@
     <mergeCell ref="C7:E7"/>
   </mergeCells>
   <phoneticPr fontId="0"/>
+  <conditionalFormatting sqref="C43:C52">
+    <cfRule type="uniqueValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.37" right="0.47" top="0.5" bottom="0.38" header="0.5" footer="0.17"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="96" verticalDpi="96" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;L&amp;"Tahoma,Regular"&amp;8 02ae-BM/PM/HDCV/FSOFT v1/0&amp;R&amp;"Tahoma,Regular"&amp;10&amp;P/&amp;N</oddFooter>
   </headerFooter>
+  <ignoredErrors>
+    <ignoredError sqref="C12:C34 C42 C35:C41 C43:C48 C49:C52" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -3157,10 +3257,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L95"/>
+  <dimension ref="A1:K95"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScale="85" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A45" zoomScale="85" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" outlineLevelRow="1"/>
@@ -3179,9 +3279,9 @@
       <c r="A1" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="137"/>
-      <c r="C1" s="137"/>
-      <c r="D1" s="137"/>
+      <c r="B1" s="140"/>
+      <c r="C1" s="140"/>
+      <c r="D1" s="140"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -3192,9 +3292,9 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="138"/>
-      <c r="C2" s="138"/>
-      <c r="D2" s="138"/>
+      <c r="B2" s="141"/>
+      <c r="C2" s="141"/>
+      <c r="D2" s="141"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -3207,51 +3307,51 @@
       <c r="A3" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="114" t="s">
+      <c r="B3" s="117" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="114"/>
-      <c r="D3" s="115"/>
+      <c r="C3" s="117"/>
+      <c r="D3" s="118"/>
       <c r="E3" s="61"/>
       <c r="F3" s="61"/>
       <c r="G3" s="61"/>
-      <c r="H3" s="145"/>
-      <c r="I3" s="145"/>
-      <c r="J3" s="145"/>
+      <c r="H3" s="148"/>
+      <c r="I3" s="148"/>
+      <c r="J3" s="148"/>
       <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="12.75">
       <c r="A4" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="146" t="s">
+      <c r="B4" s="149" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="147"/>
-      <c r="D4" s="148"/>
+      <c r="C4" s="150"/>
+      <c r="D4" s="151"/>
       <c r="E4" s="61"/>
       <c r="F4" s="61"/>
       <c r="G4" s="61"/>
-      <c r="H4" s="145"/>
-      <c r="I4" s="145"/>
-      <c r="J4" s="145"/>
+      <c r="H4" s="148"/>
+      <c r="I4" s="148"/>
+      <c r="J4" s="148"/>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" s="71" customFormat="1" ht="25.5">
       <c r="A5" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="140" t="s">
+      <c r="B5" s="143" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="141"/>
-      <c r="D5" s="142"/>
+      <c r="C5" s="144"/>
+      <c r="D5" s="145"/>
       <c r="E5" s="69"/>
       <c r="F5" s="69"/>
       <c r="G5" s="69"/>
-      <c r="H5" s="144"/>
-      <c r="I5" s="144"/>
-      <c r="J5" s="144"/>
+      <c r="H5" s="147"/>
+      <c r="I5" s="147"/>
+      <c r="J5" s="147"/>
       <c r="K5" s="70"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
@@ -3272,9 +3372,9 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="145"/>
-      <c r="I6" s="145"/>
-      <c r="J6" s="145"/>
+      <c r="H6" s="148"/>
+      <c r="I6" s="148"/>
+      <c r="J6" s="148"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -3295,16 +3395,16 @@
       <c r="E7" s="62"/>
       <c r="F7" s="62"/>
       <c r="G7" s="62"/>
-      <c r="H7" s="145"/>
-      <c r="I7" s="145"/>
-      <c r="J7" s="145"/>
+      <c r="H7" s="148"/>
+      <c r="I7" s="148"/>
+      <c r="J7" s="148"/>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="139"/>
-      <c r="B8" s="139"/>
-      <c r="C8" s="139"/>
-      <c r="D8" s="139"/>
+      <c r="A8" s="142"/>
+      <c r="B8" s="142"/>
+      <c r="C8" s="142"/>
+      <c r="D8" s="142"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -3314,72 +3414,72 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" s="73" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="128" t="s">
+      <c r="A9" s="131" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="152" t="s">
+      <c r="B9" s="155" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="128" t="s">
+      <c r="C9" s="131" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="129" t="s">
+      <c r="D9" s="132" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="130"/>
-      <c r="F9" s="130"/>
-      <c r="G9" s="131"/>
-      <c r="H9" s="149" t="s">
+      <c r="E9" s="133"/>
+      <c r="F9" s="133"/>
+      <c r="G9" s="134"/>
+      <c r="H9" s="152" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="125" t="s">
+      <c r="I9" s="128" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="125" t="s">
+      <c r="J9" s="128" t="s">
         <v>32</v>
       </c>
       <c r="K9" s="72"/>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="125"/>
-      <c r="B10" s="153"/>
-      <c r="C10" s="125"/>
-      <c r="D10" s="132"/>
-      <c r="E10" s="133"/>
-      <c r="F10" s="133"/>
-      <c r="G10" s="134"/>
-      <c r="H10" s="132"/>
-      <c r="I10" s="125"/>
-      <c r="J10" s="125"/>
+      <c r="A10" s="128"/>
+      <c r="B10" s="156"/>
+      <c r="C10" s="128"/>
+      <c r="D10" s="135"/>
+      <c r="E10" s="136"/>
+      <c r="F10" s="136"/>
+      <c r="G10" s="137"/>
+      <c r="H10" s="135"/>
+      <c r="I10" s="128"/>
+      <c r="J10" s="128"/>
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" s="74" customFormat="1" ht="15">
-      <c r="A11" s="150"/>
-      <c r="B11" s="150"/>
-      <c r="C11" s="150"/>
-      <c r="D11" s="150"/>
-      <c r="E11" s="150"/>
-      <c r="F11" s="150"/>
-      <c r="G11" s="150"/>
-      <c r="H11" s="150"/>
-      <c r="I11" s="150"/>
-      <c r="J11" s="151"/>
+      <c r="A11" s="153"/>
+      <c r="B11" s="153"/>
+      <c r="C11" s="153"/>
+      <c r="D11" s="153"/>
+      <c r="E11" s="153"/>
+      <c r="F11" s="153"/>
+      <c r="G11" s="153"/>
+      <c r="H11" s="153"/>
+      <c r="I11" s="153"/>
+      <c r="J11" s="154"/>
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A12" s="135" t="s">
+      <c r="A12" s="138" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="136"/>
-      <c r="C12" s="136"/>
-      <c r="D12" s="136"/>
-      <c r="E12" s="136"/>
-      <c r="F12" s="136"/>
-      <c r="G12" s="136"/>
-      <c r="H12" s="136"/>
-      <c r="I12" s="136"/>
-      <c r="J12" s="143"/>
-    </row>
-    <row r="13" spans="1:11" s="4" customFormat="1" ht="102.75" customHeight="1" outlineLevel="1">
+      <c r="B12" s="139"/>
+      <c r="C12" s="139"/>
+      <c r="D12" s="139"/>
+      <c r="E12" s="139"/>
+      <c r="F12" s="139"/>
+      <c r="G12" s="139"/>
+      <c r="H12" s="139"/>
+      <c r="I12" s="139"/>
+      <c r="J12" s="146"/>
+    </row>
+    <row r="13" spans="1:11" s="4" customFormat="1" ht="66.75" customHeight="1" outlineLevel="1">
       <c r="A13" s="78" t="s">
         <v>0</v>
       </c>
@@ -3389,9 +3489,9 @@
       <c r="C13" s="77" t="s">
         <v>85</v>
       </c>
-      <c r="D13" s="116"/>
-      <c r="E13" s="117"/>
-      <c r="F13" s="117"/>
+      <c r="D13" s="119"/>
+      <c r="E13" s="120"/>
+      <c r="F13" s="120"/>
       <c r="G13" s="76"/>
       <c r="H13" s="90"/>
       <c r="I13" s="77"/>
@@ -3407,9 +3507,9 @@
       <c r="C14" s="77" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="116"/>
-      <c r="E14" s="117"/>
-      <c r="F14" s="117"/>
+      <c r="D14" s="119"/>
+      <c r="E14" s="120"/>
+      <c r="F14" s="120"/>
       <c r="G14" s="76"/>
       <c r="H14" s="90"/>
       <c r="I14" s="77"/>
@@ -3425,9 +3525,9 @@
       <c r="C15" s="77" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="116"/>
-      <c r="E15" s="117"/>
-      <c r="F15" s="117"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="120"/>
+      <c r="F15" s="120"/>
       <c r="G15" s="76"/>
       <c r="H15" s="90"/>
       <c r="I15" s="77"/>
@@ -3443,9 +3543,9 @@
       <c r="C16" s="77" t="s">
         <v>95</v>
       </c>
-      <c r="D16" s="116"/>
-      <c r="E16" s="117"/>
-      <c r="F16" s="117"/>
+      <c r="D16" s="119"/>
+      <c r="E16" s="120"/>
+      <c r="F16" s="120"/>
       <c r="G16" s="76"/>
       <c r="H16" s="90"/>
       <c r="I16" s="77"/>
@@ -3461,9 +3561,9 @@
       <c r="C17" s="77" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="116"/>
-      <c r="E17" s="117"/>
-      <c r="F17" s="117"/>
+      <c r="D17" s="119"/>
+      <c r="E17" s="120"/>
+      <c r="F17" s="120"/>
       <c r="G17" s="76"/>
       <c r="H17" s="90"/>
       <c r="I17" s="77"/>
@@ -3479,9 +3579,9 @@
       <c r="C18" s="77" t="s">
         <v>93</v>
       </c>
-      <c r="D18" s="116"/>
-      <c r="E18" s="117"/>
-      <c r="F18" s="117"/>
+      <c r="D18" s="119"/>
+      <c r="E18" s="120"/>
+      <c r="F18" s="120"/>
       <c r="G18" s="76"/>
       <c r="H18" s="90"/>
       <c r="I18" s="77"/>
@@ -3497,9 +3597,9 @@
       <c r="C19" s="87" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="118"/>
-      <c r="E19" s="119"/>
-      <c r="F19" s="120"/>
+      <c r="D19" s="121"/>
+      <c r="E19" s="122"/>
+      <c r="F19" s="123"/>
       <c r="G19" s="77"/>
       <c r="H19" s="77"/>
       <c r="I19" s="77"/>
@@ -3515,20 +3615,20 @@
       <c r="C20" s="77" t="s">
         <v>102</v>
       </c>
-      <c r="D20" s="118"/>
-      <c r="E20" s="119"/>
-      <c r="F20" s="120"/>
+      <c r="D20" s="121"/>
+      <c r="E20" s="122"/>
+      <c r="F20" s="123"/>
       <c r="G20" s="77"/>
       <c r="H20" s="77"/>
       <c r="I20" s="77"/>
       <c r="J20" s="75"/>
     </row>
     <row r="21" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A21" s="135" t="s">
+      <c r="A21" s="138" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="136"/>
-      <c r="C21" s="136"/>
+      <c r="B21" s="139"/>
+      <c r="C21" s="139"/>
       <c r="D21" s="88"/>
       <c r="E21" s="88"/>
       <c r="F21" s="88"/>
@@ -3547,9 +3647,9 @@
       <c r="C22" s="87" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="126"/>
-      <c r="E22" s="127"/>
-      <c r="F22" s="127"/>
+      <c r="D22" s="129"/>
+      <c r="E22" s="130"/>
+      <c r="F22" s="130"/>
       <c r="G22" s="95"/>
       <c r="H22" s="96"/>
       <c r="I22" s="87"/>
@@ -3565,9 +3665,9 @@
       <c r="C23" s="87" t="s">
         <v>72</v>
       </c>
-      <c r="D23" s="126"/>
-      <c r="E23" s="127"/>
-      <c r="F23" s="127"/>
+      <c r="D23" s="129"/>
+      <c r="E23" s="130"/>
+      <c r="F23" s="130"/>
       <c r="G23" s="95"/>
       <c r="H23" s="96"/>
       <c r="I23" s="87"/>
@@ -3583,9 +3683,9 @@
       <c r="C24" s="87" t="s">
         <v>75</v>
       </c>
-      <c r="D24" s="126"/>
-      <c r="E24" s="127"/>
-      <c r="F24" s="127"/>
+      <c r="D24" s="129"/>
+      <c r="E24" s="130"/>
+      <c r="F24" s="130"/>
       <c r="G24" s="95"/>
       <c r="H24" s="96"/>
       <c r="I24" s="87"/>
@@ -3601,9 +3701,9 @@
       <c r="C25" s="87" t="s">
         <v>77</v>
       </c>
-      <c r="D25" s="118"/>
-      <c r="E25" s="119"/>
-      <c r="F25" s="120"/>
+      <c r="D25" s="121"/>
+      <c r="E25" s="122"/>
+      <c r="F25" s="123"/>
       <c r="G25" s="77"/>
       <c r="H25" s="77"/>
       <c r="I25" s="77"/>
@@ -3619,9 +3719,9 @@
       <c r="C26" s="87" t="s">
         <v>99</v>
       </c>
-      <c r="D26" s="118"/>
-      <c r="E26" s="119"/>
-      <c r="F26" s="120"/>
+      <c r="D26" s="121"/>
+      <c r="E26" s="122"/>
+      <c r="F26" s="123"/>
       <c r="G26" s="77"/>
       <c r="H26" s="77"/>
       <c r="I26" s="77"/>
@@ -3637,9 +3737,9 @@
       <c r="C27" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="118"/>
-      <c r="E27" s="119"/>
-      <c r="F27" s="120"/>
+      <c r="D27" s="121"/>
+      <c r="E27" s="122"/>
+      <c r="F27" s="123"/>
       <c r="G27" s="77"/>
       <c r="H27" s="77"/>
       <c r="I27" s="77"/>
@@ -3655,9 +3755,9 @@
       <c r="C28" s="77" t="s">
         <v>79</v>
       </c>
-      <c r="D28" s="118"/>
-      <c r="E28" s="119"/>
-      <c r="F28" s="120"/>
+      <c r="D28" s="121"/>
+      <c r="E28" s="122"/>
+      <c r="F28" s="123"/>
       <c r="G28" s="77"/>
       <c r="H28" s="77"/>
       <c r="I28" s="77"/>
@@ -3673,9 +3773,9 @@
       <c r="C29" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="118"/>
-      <c r="E29" s="119"/>
-      <c r="F29" s="120"/>
+      <c r="D29" s="121"/>
+      <c r="E29" s="122"/>
+      <c r="F29" s="123"/>
       <c r="G29" s="77"/>
       <c r="H29" s="77"/>
       <c r="I29" s="77"/>
@@ -3691,9 +3791,9 @@
       <c r="C30" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="D30" s="118"/>
-      <c r="E30" s="119"/>
-      <c r="F30" s="120"/>
+      <c r="D30" s="121"/>
+      <c r="E30" s="122"/>
+      <c r="F30" s="123"/>
       <c r="G30" s="77"/>
       <c r="H30" s="77"/>
       <c r="I30" s="77"/>
@@ -3709,9 +3809,9 @@
       <c r="C31" s="77" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="118"/>
-      <c r="E31" s="119"/>
-      <c r="F31" s="120"/>
+      <c r="D31" s="121"/>
+      <c r="E31" s="122"/>
+      <c r="F31" s="123"/>
       <c r="G31" s="77"/>
       <c r="H31" s="77"/>
       <c r="I31" s="77"/>
@@ -3727,20 +3827,20 @@
       <c r="C32" s="77" t="s">
         <v>101</v>
       </c>
-      <c r="D32" s="118"/>
-      <c r="E32" s="119"/>
-      <c r="F32" s="120"/>
+      <c r="D32" s="121"/>
+      <c r="E32" s="122"/>
+      <c r="F32" s="123"/>
       <c r="G32" s="77"/>
       <c r="H32" s="77"/>
       <c r="I32" s="77"/>
       <c r="J32" s="75"/>
     </row>
     <row r="33" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A33" s="121" t="s">
+      <c r="A33" s="124" t="s">
         <v>81</v>
       </c>
-      <c r="B33" s="122"/>
-      <c r="C33" s="122"/>
+      <c r="B33" s="125"/>
+      <c r="C33" s="125"/>
       <c r="D33" s="98"/>
       <c r="E33" s="98"/>
       <c r="F33" s="98"/>
@@ -3759,20 +3859,20 @@
       <c r="C34" s="77" t="s">
         <v>84</v>
       </c>
-      <c r="D34" s="123"/>
-      <c r="E34" s="124"/>
-      <c r="F34" s="124"/>
+      <c r="D34" s="126"/>
+      <c r="E34" s="127"/>
+      <c r="F34" s="127"/>
       <c r="G34" s="76"/>
       <c r="H34" s="83"/>
       <c r="I34" s="77"/>
       <c r="J34" s="75"/>
     </row>
     <row r="35" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A35" s="121" t="s">
+      <c r="A35" s="124" t="s">
         <v>82</v>
       </c>
-      <c r="B35" s="122"/>
-      <c r="C35" s="122"/>
+      <c r="B35" s="125"/>
+      <c r="C35" s="125"/>
       <c r="D35" s="98"/>
       <c r="E35" s="98"/>
       <c r="F35" s="98"/>
@@ -3786,14 +3886,14 @@
         <v>0</v>
       </c>
       <c r="B36" s="93" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C36" s="77" t="s">
-        <v>146</v>
-      </c>
-      <c r="D36" s="123"/>
-      <c r="E36" s="124"/>
-      <c r="F36" s="124"/>
+        <v>145</v>
+      </c>
+      <c r="D36" s="126"/>
+      <c r="E36" s="127"/>
+      <c r="F36" s="127"/>
       <c r="G36" s="76"/>
       <c r="H36" s="83"/>
       <c r="I36" s="77"/>
@@ -3804,14 +3904,14 @@
         <v>1</v>
       </c>
       <c r="B37" s="82" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C37" s="77" t="s">
-        <v>148</v>
-      </c>
-      <c r="D37" s="123"/>
-      <c r="E37" s="124"/>
-      <c r="F37" s="124"/>
+        <v>147</v>
+      </c>
+      <c r="D37" s="126"/>
+      <c r="E37" s="127"/>
+      <c r="F37" s="127"/>
       <c r="G37" s="76"/>
       <c r="H37" s="83"/>
       <c r="I37" s="77"/>
@@ -3822,14 +3922,14 @@
         <v>2</v>
       </c>
       <c r="B38" s="93" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C38" s="77" t="s">
-        <v>147</v>
-      </c>
-      <c r="D38" s="123"/>
-      <c r="E38" s="124"/>
-      <c r="F38" s="124"/>
+        <v>146</v>
+      </c>
+      <c r="D38" s="126"/>
+      <c r="E38" s="127"/>
+      <c r="F38" s="127"/>
       <c r="G38" s="76"/>
       <c r="H38" s="83"/>
       <c r="I38" s="77"/>
@@ -3840,14 +3940,14 @@
         <v>50</v>
       </c>
       <c r="B39" s="93" t="s">
+        <v>148</v>
+      </c>
+      <c r="C39" s="77" t="s">
         <v>149</v>
       </c>
-      <c r="C39" s="77" t="s">
-        <v>150</v>
-      </c>
-      <c r="D39" s="123"/>
-      <c r="E39" s="124"/>
-      <c r="F39" s="124"/>
+      <c r="D39" s="126"/>
+      <c r="E39" s="127"/>
+      <c r="F39" s="127"/>
       <c r="G39" s="76"/>
       <c r="H39" s="83"/>
       <c r="I39" s="77"/>
@@ -3858,25 +3958,25 @@
         <v>53</v>
       </c>
       <c r="B40" s="93" t="s">
+        <v>150</v>
+      </c>
+      <c r="C40" s="77" t="s">
         <v>151</v>
       </c>
-      <c r="C40" s="77" t="s">
-        <v>152</v>
-      </c>
-      <c r="D40" s="123"/>
-      <c r="E40" s="124"/>
-      <c r="F40" s="124"/>
+      <c r="D40" s="126"/>
+      <c r="E40" s="127"/>
+      <c r="F40" s="127"/>
       <c r="G40" s="76"/>
       <c r="H40" s="83"/>
       <c r="I40" s="77"/>
       <c r="J40" s="75"/>
     </row>
     <row r="41" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A41" s="121" t="s">
+      <c r="A41" s="124" t="s">
         <v>120</v>
       </c>
-      <c r="B41" s="122"/>
-      <c r="C41" s="122"/>
+      <c r="B41" s="125"/>
+      <c r="C41" s="125"/>
       <c r="D41" s="98"/>
       <c r="E41" s="98"/>
       <c r="F41" s="98"/>
@@ -3895,9 +3995,9 @@
       <c r="C42" s="77" t="s">
         <v>127</v>
       </c>
-      <c r="D42" s="123"/>
-      <c r="E42" s="124"/>
-      <c r="F42" s="124"/>
+      <c r="D42" s="126"/>
+      <c r="E42" s="127"/>
+      <c r="F42" s="127"/>
       <c r="G42" s="76"/>
       <c r="H42" s="83"/>
       <c r="I42" s="77"/>
@@ -3913,9 +4013,9 @@
       <c r="C43" s="77" t="s">
         <v>128</v>
       </c>
-      <c r="D43" s="123"/>
-      <c r="E43" s="124"/>
-      <c r="F43" s="124"/>
+      <c r="D43" s="126"/>
+      <c r="E43" s="127"/>
+      <c r="F43" s="127"/>
       <c r="G43" s="76"/>
       <c r="H43" s="83"/>
       <c r="I43" s="77"/>
@@ -3931,9 +4031,9 @@
       <c r="C44" s="77" t="s">
         <v>129</v>
       </c>
-      <c r="D44" s="123"/>
-      <c r="E44" s="124"/>
-      <c r="F44" s="124"/>
+      <c r="D44" s="126"/>
+      <c r="E44" s="127"/>
+      <c r="F44" s="127"/>
       <c r="G44" s="76"/>
       <c r="H44" s="83"/>
       <c r="I44" s="77"/>
@@ -3949,9 +4049,9 @@
       <c r="C45" s="77" t="s">
         <v>130</v>
       </c>
-      <c r="D45" s="123"/>
-      <c r="E45" s="124"/>
-      <c r="F45" s="124"/>
+      <c r="D45" s="126"/>
+      <c r="E45" s="127"/>
+      <c r="F45" s="127"/>
       <c r="G45" s="76"/>
       <c r="H45" s="83"/>
       <c r="I45" s="77"/>
@@ -3967,9 +4067,9 @@
       <c r="C46" s="77" t="s">
         <v>132</v>
       </c>
-      <c r="D46" s="123"/>
-      <c r="E46" s="124"/>
-      <c r="F46" s="124"/>
+      <c r="D46" s="126"/>
+      <c r="E46" s="127"/>
+      <c r="F46" s="127"/>
       <c r="G46" s="76"/>
       <c r="H46" s="83"/>
       <c r="I46" s="77"/>
@@ -3985,20 +4085,20 @@
       <c r="C47" s="77" t="s">
         <v>124</v>
       </c>
-      <c r="D47" s="123"/>
-      <c r="E47" s="124"/>
-      <c r="F47" s="124"/>
+      <c r="D47" s="126"/>
+      <c r="E47" s="127"/>
+      <c r="F47" s="127"/>
       <c r="G47" s="76"/>
       <c r="H47" s="83"/>
       <c r="I47" s="77"/>
       <c r="J47" s="75"/>
     </row>
     <row r="48" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A48" s="121" t="s">
+      <c r="A48" s="124" t="s">
         <v>133</v>
       </c>
-      <c r="B48" s="122"/>
-      <c r="C48" s="122"/>
+      <c r="B48" s="125"/>
+      <c r="C48" s="125"/>
       <c r="D48" s="98"/>
       <c r="E48" s="98"/>
       <c r="F48" s="98"/>
@@ -4012,23 +4112,23 @@
         <v>0</v>
       </c>
       <c r="B49" s="93" t="s">
-        <v>135</v>
+        <v>168</v>
       </c>
       <c r="C49" s="77" t="s">
         <v>134</v>
       </c>
-      <c r="D49" s="123"/>
-      <c r="E49" s="124"/>
-      <c r="F49" s="124"/>
+      <c r="D49" s="126"/>
+      <c r="E49" s="127"/>
+      <c r="F49" s="127"/>
       <c r="G49" s="76"/>
       <c r="H49" s="83"/>
       <c r="I49" s="77"/>
       <c r="J49" s="75"/>
     </row>
     <row r="50" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A50" s="121"/>
-      <c r="B50" s="122"/>
-      <c r="C50" s="122"/>
+      <c r="A50" s="124"/>
+      <c r="B50" s="125"/>
+      <c r="C50" s="125"/>
       <c r="D50" s="98"/>
       <c r="E50" s="98"/>
       <c r="F50" s="98"/>
@@ -4041,18 +4141,18 @@
       <c r="A51" s="78"/>
       <c r="B51" s="93"/>
       <c r="C51" s="77"/>
-      <c r="D51" s="123"/>
-      <c r="E51" s="124"/>
-      <c r="F51" s="124"/>
+      <c r="D51" s="126"/>
+      <c r="E51" s="127"/>
+      <c r="F51" s="127"/>
       <c r="G51" s="76"/>
       <c r="H51" s="83"/>
       <c r="I51" s="77"/>
       <c r="J51" s="75"/>
     </row>
     <row r="52" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A52" s="121"/>
-      <c r="B52" s="122"/>
-      <c r="C52" s="122"/>
+      <c r="A52" s="124"/>
+      <c r="B52" s="125"/>
+      <c r="C52" s="125"/>
       <c r="D52" s="98"/>
       <c r="E52" s="98"/>
       <c r="F52" s="98"/>
@@ -4065,18 +4165,18 @@
       <c r="A53" s="78"/>
       <c r="B53" s="93"/>
       <c r="C53" s="77"/>
-      <c r="D53" s="123"/>
-      <c r="E53" s="124"/>
-      <c r="F53" s="124"/>
+      <c r="D53" s="126"/>
+      <c r="E53" s="127"/>
+      <c r="F53" s="127"/>
       <c r="G53" s="76"/>
       <c r="H53" s="83"/>
       <c r="I53" s="77"/>
       <c r="J53" s="75"/>
     </row>
     <row r="54" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A54" s="121"/>
-      <c r="B54" s="122"/>
-      <c r="C54" s="122"/>
+      <c r="A54" s="124"/>
+      <c r="B54" s="125"/>
+      <c r="C54" s="125"/>
       <c r="D54" s="98"/>
       <c r="E54" s="98"/>
       <c r="F54" s="98"/>
@@ -4089,18 +4189,18 @@
       <c r="A55" s="78"/>
       <c r="B55" s="93"/>
       <c r="C55" s="77"/>
-      <c r="D55" s="123"/>
-      <c r="E55" s="124"/>
-      <c r="F55" s="124"/>
+      <c r="D55" s="126"/>
+      <c r="E55" s="127"/>
+      <c r="F55" s="127"/>
       <c r="G55" s="76"/>
       <c r="H55" s="83"/>
       <c r="I55" s="77"/>
       <c r="J55" s="75"/>
     </row>
     <row r="56" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A56" s="121"/>
-      <c r="B56" s="122"/>
-      <c r="C56" s="122"/>
+      <c r="A56" s="124"/>
+      <c r="B56" s="125"/>
+      <c r="C56" s="125"/>
       <c r="D56" s="98"/>
       <c r="E56" s="98"/>
       <c r="F56" s="98"/>
@@ -4113,18 +4213,18 @@
       <c r="A57" s="78"/>
       <c r="B57" s="93"/>
       <c r="C57" s="77"/>
-      <c r="D57" s="123"/>
-      <c r="E57" s="124"/>
-      <c r="F57" s="124"/>
+      <c r="D57" s="126"/>
+      <c r="E57" s="127"/>
+      <c r="F57" s="127"/>
       <c r="G57" s="76"/>
       <c r="H57" s="83"/>
       <c r="I57" s="77"/>
       <c r="J57" s="75"/>
     </row>
     <row r="58" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A58" s="121"/>
-      <c r="B58" s="122"/>
-      <c r="C58" s="122"/>
+      <c r="A58" s="124"/>
+      <c r="B58" s="125"/>
+      <c r="C58" s="125"/>
       <c r="D58" s="98"/>
       <c r="E58" s="98"/>
       <c r="F58" s="98"/>
@@ -4137,18 +4237,18 @@
       <c r="A59" s="78"/>
       <c r="B59" s="93"/>
       <c r="C59" s="77"/>
-      <c r="D59" s="123"/>
-      <c r="E59" s="124"/>
-      <c r="F59" s="124"/>
+      <c r="D59" s="126"/>
+      <c r="E59" s="127"/>
+      <c r="F59" s="127"/>
       <c r="G59" s="76"/>
       <c r="H59" s="83"/>
       <c r="I59" s="77"/>
       <c r="J59" s="75"/>
     </row>
     <row r="60" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A60" s="121"/>
-      <c r="B60" s="122"/>
-      <c r="C60" s="122"/>
+      <c r="A60" s="124"/>
+      <c r="B60" s="125"/>
+      <c r="C60" s="125"/>
       <c r="D60" s="98"/>
       <c r="E60" s="98"/>
       <c r="F60" s="98"/>
@@ -4161,18 +4261,18 @@
       <c r="A61" s="78"/>
       <c r="B61" s="93"/>
       <c r="C61" s="77"/>
-      <c r="D61" s="123"/>
-      <c r="E61" s="124"/>
-      <c r="F61" s="124"/>
+      <c r="D61" s="126"/>
+      <c r="E61" s="127"/>
+      <c r="F61" s="127"/>
       <c r="G61" s="76"/>
       <c r="H61" s="83"/>
       <c r="I61" s="77"/>
       <c r="J61" s="75"/>
     </row>
     <row r="62" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A62" s="121"/>
-      <c r="B62" s="122"/>
-      <c r="C62" s="122"/>
+      <c r="A62" s="124"/>
+      <c r="B62" s="125"/>
+      <c r="C62" s="125"/>
       <c r="D62" s="98"/>
       <c r="E62" s="98"/>
       <c r="F62" s="98"/>
@@ -4185,9 +4285,9 @@
       <c r="A63" s="78"/>
       <c r="B63" s="93"/>
       <c r="C63" s="77"/>
-      <c r="D63" s="123"/>
-      <c r="E63" s="124"/>
-      <c r="F63" s="124"/>
+      <c r="D63" s="126"/>
+      <c r="E63" s="127"/>
+      <c r="F63" s="127"/>
       <c r="G63" s="76"/>
       <c r="H63" s="83"/>
       <c r="I63" s="77"/>
@@ -4197,180 +4297,129 @@
       <c r="I64"/>
       <c r="J64"/>
     </row>
-    <row r="65" spans="8:12" ht="12" customHeight="1">
+    <row r="65" spans="9:10" ht="12" customHeight="1">
       <c r="I65"/>
       <c r="J65"/>
     </row>
-    <row r="66" spans="8:12" ht="12" customHeight="1">
+    <row r="66" spans="9:10" ht="12" customHeight="1">
       <c r="I66"/>
       <c r="J66"/>
     </row>
-    <row r="67" spans="8:12" ht="12" customHeight="1">
+    <row r="67" spans="9:10" ht="12" customHeight="1">
       <c r="I67"/>
       <c r="J67"/>
     </row>
-    <row r="68" spans="8:12" ht="12" customHeight="1">
+    <row r="68" spans="9:10" ht="12" customHeight="1">
       <c r="I68"/>
       <c r="J68"/>
     </row>
-    <row r="69" spans="8:12" ht="12" customHeight="1">
+    <row r="69" spans="9:10" ht="12" customHeight="1">
       <c r="I69"/>
       <c r="J69"/>
     </row>
-    <row r="70" spans="8:12" ht="12" customHeight="1">
+    <row r="70" spans="9:10" ht="12" customHeight="1">
       <c r="I70"/>
       <c r="J70"/>
     </row>
-    <row r="71" spans="8:12" ht="12" customHeight="1">
+    <row r="71" spans="9:10" ht="12" customHeight="1">
       <c r="I71"/>
       <c r="J71"/>
     </row>
-    <row r="72" spans="8:12" ht="12" customHeight="1">
+    <row r="72" spans="9:10" ht="12" customHeight="1">
       <c r="I72"/>
       <c r="J72"/>
     </row>
-    <row r="73" spans="8:12" ht="12" customHeight="1">
+    <row r="73" spans="9:10" ht="12" customHeight="1">
       <c r="I73"/>
       <c r="J73"/>
     </row>
-    <row r="74" spans="8:12" ht="12" customHeight="1">
+    <row r="74" spans="9:10" ht="12" customHeight="1">
       <c r="I74"/>
       <c r="J74"/>
     </row>
-    <row r="75" spans="8:12" ht="12" customHeight="1">
+    <row r="75" spans="9:10" ht="12" customHeight="1">
       <c r="I75"/>
       <c r="J75"/>
     </row>
-    <row r="76" spans="8:12" ht="12" customHeight="1">
+    <row r="76" spans="9:10" ht="12" customHeight="1">
       <c r="I76"/>
       <c r="J76"/>
     </row>
-    <row r="77" spans="8:12" ht="12" customHeight="1">
+    <row r="77" spans="9:10" ht="12" customHeight="1">
       <c r="I77"/>
       <c r="J77"/>
     </row>
-    <row r="78" spans="8:12" ht="12" customHeight="1">
+    <row r="78" spans="9:10" ht="12" customHeight="1">
       <c r="I78"/>
       <c r="J78"/>
     </row>
-    <row r="79" spans="8:12" ht="12" customHeight="1">
-      <c r="H79" s="154"/>
-      <c r="I79" s="154"/>
-      <c r="J79" s="154"/>
-      <c r="K79" s="154"/>
-      <c r="L79" s="154"/>
-    </row>
-    <row r="80" spans="8:12">
-      <c r="H80" s="154"/>
-      <c r="I80" s="155"/>
-      <c r="J80" s="154"/>
-      <c r="K80" s="154"/>
-      <c r="L80" s="154"/>
-    </row>
-    <row r="81" spans="8:12">
-      <c r="H81" s="154"/>
-      <c r="I81" s="155"/>
-      <c r="J81" s="154"/>
-      <c r="K81" s="154"/>
-      <c r="L81" s="154"/>
-    </row>
-    <row r="82" spans="8:12">
-      <c r="H82" s="154"/>
-      <c r="I82" s="155"/>
-      <c r="J82" s="154"/>
-      <c r="K82" s="154"/>
-      <c r="L82" s="154"/>
-    </row>
-    <row r="83" spans="8:12">
-      <c r="H83" s="154"/>
-      <c r="I83" s="155"/>
-      <c r="J83" s="154"/>
-      <c r="K83" s="154"/>
-      <c r="L83" s="154"/>
-    </row>
-    <row r="84" spans="8:12">
-      <c r="H84" s="154"/>
-      <c r="I84" s="155"/>
-      <c r="J84" s="154"/>
-      <c r="K84" s="154"/>
-      <c r="L84" s="154"/>
-    </row>
-    <row r="85" spans="8:12">
-      <c r="H85" s="154"/>
-      <c r="I85" s="155"/>
-      <c r="J85" s="154"/>
-      <c r="K85" s="154"/>
-      <c r="L85" s="154"/>
-    </row>
-    <row r="86" spans="8:12">
-      <c r="H86" s="154"/>
-      <c r="I86" s="155"/>
-      <c r="J86" s="154"/>
-      <c r="K86" s="154"/>
-      <c r="L86" s="154"/>
-    </row>
-    <row r="87" spans="8:12">
-      <c r="H87" s="154"/>
-      <c r="I87" s="155"/>
-      <c r="J87" s="154"/>
-      <c r="K87" s="154"/>
-      <c r="L87" s="154"/>
-    </row>
-    <row r="88" spans="8:12">
-      <c r="H88" s="154"/>
-      <c r="I88" s="155"/>
-      <c r="J88" s="154"/>
-      <c r="K88" s="154"/>
-      <c r="L88" s="154"/>
-    </row>
-    <row r="89" spans="8:12">
-      <c r="H89" s="154"/>
-      <c r="I89" s="155"/>
-      <c r="J89" s="154"/>
-      <c r="K89" s="154"/>
-      <c r="L89" s="154"/>
-    </row>
-    <row r="90" spans="8:12">
-      <c r="H90" s="154"/>
-      <c r="I90" s="155"/>
-      <c r="J90" s="154"/>
-      <c r="K90" s="154"/>
-      <c r="L90" s="154"/>
-    </row>
-    <row r="91" spans="8:12">
-      <c r="H91" s="154"/>
-      <c r="I91" s="155"/>
-      <c r="J91" s="154"/>
-      <c r="K91" s="154"/>
-      <c r="L91" s="154"/>
-    </row>
-    <row r="92" spans="8:12">
-      <c r="H92" s="154"/>
-      <c r="I92" s="155"/>
-      <c r="J92" s="154"/>
-      <c r="K92" s="154"/>
-      <c r="L92" s="154"/>
-    </row>
-    <row r="93" spans="8:12">
-      <c r="H93" s="154"/>
-      <c r="I93" s="155"/>
-      <c r="J93" s="154"/>
-      <c r="K93" s="154"/>
-      <c r="L93" s="154"/>
-    </row>
-    <row r="94" spans="8:12">
-      <c r="H94" s="154"/>
-      <c r="I94" s="155"/>
-      <c r="J94" s="154"/>
-      <c r="K94" s="154"/>
-      <c r="L94" s="154"/>
-    </row>
-    <row r="95" spans="8:12">
-      <c r="H95" s="154"/>
-      <c r="I95" s="155"/>
-      <c r="J95" s="154"/>
-      <c r="K95" s="154"/>
-      <c r="L95" s="154"/>
+    <row r="79" spans="9:10" ht="12" customHeight="1">
+      <c r="I79"/>
+      <c r="J79"/>
+    </row>
+    <row r="80" spans="9:10">
+      <c r="I80" s="19"/>
+      <c r="J80"/>
+    </row>
+    <row r="81" spans="9:10">
+      <c r="I81" s="19"/>
+      <c r="J81"/>
+    </row>
+    <row r="82" spans="9:10">
+      <c r="I82" s="19"/>
+      <c r="J82"/>
+    </row>
+    <row r="83" spans="9:10">
+      <c r="I83" s="19"/>
+      <c r="J83"/>
+    </row>
+    <row r="84" spans="9:10">
+      <c r="I84" s="19"/>
+      <c r="J84"/>
+    </row>
+    <row r="85" spans="9:10">
+      <c r="I85" s="19"/>
+      <c r="J85"/>
+    </row>
+    <row r="86" spans="9:10">
+      <c r="I86" s="19"/>
+      <c r="J86"/>
+    </row>
+    <row r="87" spans="9:10">
+      <c r="I87" s="19"/>
+      <c r="J87"/>
+    </row>
+    <row r="88" spans="9:10">
+      <c r="I88" s="19"/>
+      <c r="J88"/>
+    </row>
+    <row r="89" spans="9:10">
+      <c r="I89" s="19"/>
+      <c r="J89"/>
+    </row>
+    <row r="90" spans="9:10">
+      <c r="I90" s="19"/>
+      <c r="J90"/>
+    </row>
+    <row r="91" spans="9:10">
+      <c r="I91" s="19"/>
+      <c r="J91"/>
+    </row>
+    <row r="92" spans="9:10">
+      <c r="I92" s="19"/>
+      <c r="J92"/>
+    </row>
+    <row r="93" spans="9:10">
+      <c r="I93" s="19"/>
+      <c r="J93"/>
+    </row>
+    <row r="94" spans="9:10">
+      <c r="I94" s="19"/>
+      <c r="J94"/>
+    </row>
+    <row r="95" spans="9:10">
+      <c r="I95" s="19"/>
+      <c r="J95"/>
     </row>
   </sheetData>
   <mergeCells count="70">
@@ -4457,10 +4506,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:M69"/>
+  <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22:F22"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="85" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26:F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" outlineLevelRow="1"/>
@@ -4475,13 +4524,13 @@
     <col min="10" max="10" width="18" style="84" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" ht="12.75" customHeight="1">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A1" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="137"/>
-      <c r="C1" s="137"/>
-      <c r="D1" s="137"/>
+      <c r="B1" s="140"/>
+      <c r="C1" s="140"/>
+      <c r="D1" s="140"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -4489,14 +4538,12 @@
       <c r="I1" s="91"/>
       <c r="J1" s="6"/>
       <c r="K1" s="7"/>
-      <c r="L1" s="156"/>
-      <c r="M1" s="156"/>
-    </row>
-    <row r="2" spans="1:13" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
+    </row>
+    <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="138"/>
-      <c r="C2" s="138"/>
-      <c r="D2" s="138"/>
+      <c r="B2" s="141"/>
+      <c r="C2" s="141"/>
+      <c r="D2" s="141"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -4504,121 +4551,109 @@
       <c r="I2" s="91"/>
       <c r="J2" s="6"/>
       <c r="K2" s="7"/>
-      <c r="L2" s="156"/>
-      <c r="M2" s="156"/>
-    </row>
-    <row r="3" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="3" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="114" t="s">
+      <c r="B3" s="117" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="114"/>
-      <c r="D3" s="115"/>
+      <c r="C3" s="117"/>
+      <c r="D3" s="118"/>
       <c r="E3" s="61"/>
       <c r="F3" s="61"/>
       <c r="G3" s="61"/>
-      <c r="H3" s="145"/>
-      <c r="I3" s="145"/>
-      <c r="J3" s="145"/>
+      <c r="H3" s="148"/>
+      <c r="I3" s="148"/>
+      <c r="J3" s="148"/>
       <c r="K3" s="9"/>
-      <c r="L3" s="157"/>
-      <c r="M3" s="157"/>
-    </row>
-    <row r="4" spans="1:13" s="3" customFormat="1" ht="12.75">
+    </row>
+    <row r="4" spans="1:11" s="3" customFormat="1" ht="12.75">
       <c r="A4" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="146" t="s">
-        <v>160</v>
-      </c>
-      <c r="C4" s="147"/>
-      <c r="D4" s="148"/>
+      <c r="B4" s="149" t="s">
+        <v>158</v>
+      </c>
+      <c r="C4" s="150"/>
+      <c r="D4" s="151"/>
       <c r="E4" s="61"/>
       <c r="F4" s="61"/>
       <c r="G4" s="61"/>
-      <c r="H4" s="145"/>
-      <c r="I4" s="145"/>
-      <c r="J4" s="145"/>
+      <c r="H4" s="148"/>
+      <c r="I4" s="148"/>
+      <c r="J4" s="148"/>
       <c r="K4" s="9"/>
-      <c r="L4" s="157"/>
-      <c r="M4" s="157"/>
-    </row>
-    <row r="5" spans="1:13" s="71" customFormat="1" ht="25.5">
+    </row>
+    <row r="5" spans="1:11" s="71" customFormat="1" ht="25.5">
       <c r="A5" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="140" t="s">
+      <c r="B5" s="143" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="141"/>
-      <c r="D5" s="142"/>
+      <c r="C5" s="144"/>
+      <c r="D5" s="145"/>
       <c r="E5" s="69"/>
       <c r="F5" s="69"/>
       <c r="G5" s="69"/>
-      <c r="H5" s="144"/>
-      <c r="I5" s="144"/>
-      <c r="J5" s="144"/>
+      <c r="H5" s="147"/>
+      <c r="I5" s="147"/>
+      <c r="J5" s="147"/>
       <c r="K5" s="70"/>
-      <c r="L5" s="158"/>
-      <c r="M5" s="158"/>
-    </row>
-    <row r="6" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A6" s="12" t="s">
         <v>38</v>
       </c>
       <c r="B6" s="80">
-        <f>COUNTIF(I12:I28,"Pass")</f>
+        <f>COUNTIF(I12:I27,"Pass")</f>
         <v>0</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>39</v>
       </c>
       <c r="D6" s="13">
-        <f>COUNTIF(I10:I734,"Pending")</f>
+        <f>COUNTIF(I10:I733,"Pending")</f>
         <v>0</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="145"/>
-      <c r="I6" s="145"/>
-      <c r="J6" s="145"/>
+      <c r="H6" s="148"/>
+      <c r="I6" s="148"/>
+      <c r="J6" s="148"/>
       <c r="K6" s="9"/>
-      <c r="L6" s="157"/>
-      <c r="M6" s="157"/>
-    </row>
-    <row r="7" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
+    </row>
+    <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="A7" s="14" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="81">
-        <f>COUNTIF(I12:I28,"Fail")</f>
+        <f>COUNTIF(I12:I27,"Fail")</f>
         <v>0</v>
       </c>
       <c r="C7" s="29" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="59">
-        <f>COUNTA(A12:A37) -2</f>
-        <v>2</v>
+        <f>COUNTA(A12:A36) -3</f>
+        <v>6</v>
       </c>
       <c r="E7" s="62"/>
       <c r="F7" s="62"/>
       <c r="G7" s="62"/>
-      <c r="H7" s="145"/>
-      <c r="I7" s="145"/>
-      <c r="J7" s="145"/>
+      <c r="H7" s="148"/>
+      <c r="I7" s="148"/>
+      <c r="J7" s="148"/>
       <c r="K7" s="9"/>
-      <c r="L7" s="157"/>
-      <c r="M7" s="157"/>
-    </row>
-    <row r="8" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="139"/>
-      <c r="B8" s="139"/>
-      <c r="C8" s="139"/>
-      <c r="D8" s="139"/>
+    </row>
+    <row r="8" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="A8" s="142"/>
+      <c r="B8" s="142"/>
+      <c r="C8" s="142"/>
+      <c r="D8" s="142"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -4626,118 +4661,116 @@
       <c r="I8" s="92"/>
       <c r="J8" s="92"/>
       <c r="K8" s="9"/>
-      <c r="L8" s="157"/>
-      <c r="M8" s="157"/>
-    </row>
-    <row r="9" spans="1:13" s="73" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="128" t="s">
+    </row>
+    <row r="9" spans="1:11" s="73" customFormat="1" ht="12" customHeight="1">
+      <c r="A9" s="131" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="152" t="s">
+      <c r="B9" s="155" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="128" t="s">
+      <c r="C9" s="131" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="129" t="s">
+      <c r="D9" s="132" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="130"/>
-      <c r="F9" s="130"/>
-      <c r="G9" s="131"/>
-      <c r="H9" s="149" t="s">
+      <c r="E9" s="133"/>
+      <c r="F9" s="133"/>
+      <c r="G9" s="134"/>
+      <c r="H9" s="152" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="125" t="s">
+      <c r="I9" s="128" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="125" t="s">
+      <c r="J9" s="128" t="s">
         <v>32</v>
       </c>
       <c r="K9" s="72"/>
     </row>
-    <row r="10" spans="1:13" s="3" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="125"/>
-      <c r="B10" s="153"/>
-      <c r="C10" s="125"/>
-      <c r="D10" s="132"/>
-      <c r="E10" s="133"/>
-      <c r="F10" s="133"/>
-      <c r="G10" s="134"/>
-      <c r="H10" s="132"/>
-      <c r="I10" s="125"/>
-      <c r="J10" s="125"/>
+    <row r="10" spans="1:11" s="3" customFormat="1" ht="12" customHeight="1">
+      <c r="A10" s="128"/>
+      <c r="B10" s="156"/>
+      <c r="C10" s="128"/>
+      <c r="D10" s="135"/>
+      <c r="E10" s="136"/>
+      <c r="F10" s="136"/>
+      <c r="G10" s="137"/>
+      <c r="H10" s="135"/>
+      <c r="I10" s="128"/>
+      <c r="J10" s="128"/>
       <c r="K10" s="9"/>
     </row>
-    <row r="11" spans="1:13" s="74" customFormat="1" ht="15">
-      <c r="A11" s="150"/>
-      <c r="B11" s="150"/>
-      <c r="C11" s="150"/>
-      <c r="D11" s="150"/>
-      <c r="E11" s="150"/>
-      <c r="F11" s="150"/>
-      <c r="G11" s="150"/>
-      <c r="H11" s="150"/>
-      <c r="I11" s="150"/>
-      <c r="J11" s="151"/>
-    </row>
-    <row r="12" spans="1:13" s="4" customFormat="1" ht="12.75">
-      <c r="A12" s="135" t="s">
-        <v>161</v>
-      </c>
-      <c r="B12" s="136"/>
-      <c r="C12" s="136"/>
-      <c r="D12" s="136"/>
-      <c r="E12" s="136"/>
-      <c r="F12" s="136"/>
-      <c r="G12" s="136"/>
-      <c r="H12" s="136"/>
-      <c r="I12" s="136"/>
-      <c r="J12" s="143"/>
-    </row>
-    <row r="13" spans="1:13" s="4" customFormat="1" ht="102.75" customHeight="1" outlineLevel="1">
+    <row r="11" spans="1:11" s="74" customFormat="1" ht="15">
+      <c r="A11" s="153"/>
+      <c r="B11" s="153"/>
+      <c r="C11" s="153"/>
+      <c r="D11" s="153"/>
+      <c r="E11" s="153"/>
+      <c r="F11" s="153"/>
+      <c r="G11" s="153"/>
+      <c r="H11" s="153"/>
+      <c r="I11" s="153"/>
+      <c r="J11" s="154"/>
+    </row>
+    <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
+      <c r="A12" s="138" t="s">
+        <v>159</v>
+      </c>
+      <c r="B12" s="139"/>
+      <c r="C12" s="139"/>
+      <c r="D12" s="139"/>
+      <c r="E12" s="139"/>
+      <c r="F12" s="139"/>
+      <c r="G12" s="139"/>
+      <c r="H12" s="139"/>
+      <c r="I12" s="139"/>
+      <c r="J12" s="146"/>
+    </row>
+    <row r="13" spans="1:11" s="4" customFormat="1" ht="102.75" customHeight="1" outlineLevel="1">
       <c r="A13" s="78"/>
       <c r="B13" s="82"/>
       <c r="C13" s="77"/>
-      <c r="D13" s="116"/>
-      <c r="E13" s="117"/>
-      <c r="F13" s="117"/>
+      <c r="D13" s="119"/>
+      <c r="E13" s="120"/>
+      <c r="F13" s="120"/>
       <c r="G13" s="76"/>
       <c r="H13" s="90"/>
       <c r="I13" s="77"/>
       <c r="J13" s="75"/>
     </row>
-    <row r="14" spans="1:13" s="4" customFormat="1" ht="57.75" customHeight="1" outlineLevel="1">
+    <row r="14" spans="1:11" s="4" customFormat="1" ht="57.75" customHeight="1" outlineLevel="1">
       <c r="A14" s="78"/>
       <c r="B14" s="82"/>
       <c r="C14" s="77"/>
-      <c r="D14" s="116"/>
-      <c r="E14" s="117"/>
-      <c r="F14" s="117"/>
+      <c r="D14" s="119"/>
+      <c r="E14" s="120"/>
+      <c r="F14" s="120"/>
       <c r="G14" s="76"/>
       <c r="H14" s="90"/>
       <c r="I14" s="77"/>
       <c r="J14" s="75"/>
     </row>
-    <row r="15" spans="1:13" s="4" customFormat="1" ht="66.75" customHeight="1" outlineLevel="1">
+    <row r="15" spans="1:11" s="4" customFormat="1" ht="66.75" customHeight="1" outlineLevel="1">
       <c r="A15" s="78"/>
       <c r="B15" s="82"/>
       <c r="C15" s="77"/>
-      <c r="D15" s="116"/>
-      <c r="E15" s="117"/>
-      <c r="F15" s="117"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="120"/>
+      <c r="F15" s="120"/>
       <c r="G15" s="76"/>
       <c r="H15" s="90"/>
       <c r="I15" s="77"/>
       <c r="J15" s="75"/>
     </row>
-    <row r="16" spans="1:13" s="4" customFormat="1" ht="66.75" customHeight="1" outlineLevel="1">
+    <row r="16" spans="1:11" s="4" customFormat="1" ht="66.75" customHeight="1" outlineLevel="1">
       <c r="A16" s="78"/>
       <c r="B16" s="82"/>
       <c r="C16" s="77"/>
-      <c r="D16" s="116"/>
-      <c r="E16" s="117"/>
-      <c r="F16" s="117"/>
+      <c r="D16" s="119"/>
+      <c r="E16" s="120"/>
+      <c r="F16" s="120"/>
       <c r="G16" s="76"/>
       <c r="H16" s="90"/>
       <c r="I16" s="77"/>
@@ -4747,9 +4780,9 @@
       <c r="A17" s="78"/>
       <c r="B17" s="82"/>
       <c r="C17" s="77"/>
-      <c r="D17" s="116"/>
-      <c r="E17" s="117"/>
-      <c r="F17" s="117"/>
+      <c r="D17" s="119"/>
+      <c r="E17" s="120"/>
+      <c r="F17" s="120"/>
       <c r="G17" s="76"/>
       <c r="H17" s="90"/>
       <c r="I17" s="77"/>
@@ -4759,20 +4792,20 @@
       <c r="A18" s="78"/>
       <c r="B18" s="82"/>
       <c r="C18" s="77"/>
-      <c r="D18" s="116"/>
-      <c r="E18" s="117"/>
-      <c r="F18" s="117"/>
+      <c r="D18" s="119"/>
+      <c r="E18" s="120"/>
+      <c r="F18" s="120"/>
       <c r="G18" s="76"/>
       <c r="H18" s="90"/>
       <c r="I18" s="77"/>
       <c r="J18" s="75"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A19" s="135" t="s">
-        <v>162</v>
-      </c>
-      <c r="B19" s="136"/>
-      <c r="C19" s="136"/>
+      <c r="A19" s="138" t="s">
+        <v>160</v>
+      </c>
+      <c r="B19" s="139"/>
+      <c r="C19" s="139"/>
       <c r="D19" s="88"/>
       <c r="E19" s="88"/>
       <c r="F19" s="88"/>
@@ -4786,14 +4819,14 @@
         <v>0</v>
       </c>
       <c r="B20" s="86" t="s">
+        <v>161</v>
+      </c>
+      <c r="C20" s="87" t="s">
         <v>163</v>
       </c>
-      <c r="C20" s="87" t="s">
-        <v>165</v>
-      </c>
-      <c r="D20" s="126"/>
-      <c r="E20" s="127"/>
-      <c r="F20" s="127"/>
+      <c r="D20" s="129"/>
+      <c r="E20" s="130"/>
+      <c r="F20" s="130"/>
       <c r="G20" s="95"/>
       <c r="H20" s="96"/>
       <c r="I20" s="87"/>
@@ -4804,14 +4837,14 @@
         <v>1</v>
       </c>
       <c r="B21" s="86" t="s">
+        <v>162</v>
+      </c>
+      <c r="C21" s="87" t="s">
         <v>164</v>
       </c>
-      <c r="C21" s="87" t="s">
-        <v>166</v>
-      </c>
-      <c r="D21" s="126"/>
-      <c r="E21" s="127"/>
-      <c r="F21" s="127"/>
+      <c r="D21" s="129"/>
+      <c r="E21" s="130"/>
+      <c r="F21" s="130"/>
       <c r="G21" s="95"/>
       <c r="H21" s="96"/>
       <c r="I21" s="87"/>
@@ -4821,18 +4854,20 @@
       <c r="A22" s="94"/>
       <c r="B22" s="86"/>
       <c r="C22" s="87"/>
-      <c r="D22" s="126"/>
-      <c r="E22" s="127"/>
-      <c r="F22" s="127"/>
+      <c r="D22" s="129"/>
+      <c r="E22" s="130"/>
+      <c r="F22" s="130"/>
       <c r="G22" s="95"/>
       <c r="H22" s="96"/>
       <c r="I22" s="87"/>
       <c r="J22" s="97"/>
     </row>
     <row r="23" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A23" s="135"/>
-      <c r="B23" s="136"/>
-      <c r="C23" s="136"/>
+      <c r="A23" s="138" t="s">
+        <v>170</v>
+      </c>
+      <c r="B23" s="139"/>
+      <c r="C23" s="139"/>
       <c r="D23" s="88"/>
       <c r="E23" s="88"/>
       <c r="F23" s="88"/>
@@ -4842,84 +4877,108 @@
       <c r="J23" s="89"/>
     </row>
     <row r="24" spans="1:10" s="4" customFormat="1" ht="116.25" customHeight="1" outlineLevel="1">
-      <c r="A24" s="78"/>
-      <c r="B24" s="93"/>
-      <c r="C24" s="77"/>
-      <c r="D24" s="123"/>
-      <c r="E24" s="124"/>
-      <c r="F24" s="124"/>
+      <c r="A24" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="93" t="s">
+        <v>172</v>
+      </c>
+      <c r="C24" s="77" t="s">
+        <v>171</v>
+      </c>
+      <c r="D24" s="126"/>
+      <c r="E24" s="127"/>
+      <c r="F24" s="127"/>
       <c r="G24" s="76"/>
       <c r="H24" s="83"/>
       <c r="I24" s="77"/>
       <c r="J24" s="75"/>
     </row>
     <row r="25" spans="1:10" s="4" customFormat="1" ht="67.5" customHeight="1" outlineLevel="1">
-      <c r="A25" s="78"/>
-      <c r="B25" s="82"/>
-      <c r="C25" s="77"/>
-      <c r="D25" s="123"/>
-      <c r="E25" s="124"/>
-      <c r="F25" s="124"/>
+      <c r="A25" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="93" t="s">
+        <v>175</v>
+      </c>
+      <c r="C25" s="77" t="s">
+        <v>173</v>
+      </c>
+      <c r="D25" s="126"/>
+      <c r="E25" s="127"/>
+      <c r="F25" s="127"/>
       <c r="G25" s="76"/>
       <c r="H25" s="83"/>
       <c r="I25" s="77"/>
       <c r="J25" s="75"/>
     </row>
     <row r="26" spans="1:10" s="4" customFormat="1" ht="81" customHeight="1" outlineLevel="1">
-      <c r="A26" s="78"/>
-      <c r="B26" s="93"/>
-      <c r="C26" s="77"/>
-      <c r="D26" s="123"/>
-      <c r="E26" s="124"/>
-      <c r="F26" s="124"/>
+      <c r="A26" s="78" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="93" t="s">
+        <v>176</v>
+      </c>
+      <c r="C26" s="77" t="s">
+        <v>174</v>
+      </c>
+      <c r="D26" s="126"/>
+      <c r="E26" s="127"/>
+      <c r="F26" s="127"/>
       <c r="G26" s="76"/>
       <c r="H26" s="83"/>
       <c r="I26" s="77"/>
       <c r="J26" s="75"/>
     </row>
     <row r="27" spans="1:10" s="4" customFormat="1" ht="93" customHeight="1" outlineLevel="1">
-      <c r="A27" s="78"/>
-      <c r="B27" s="93"/>
-      <c r="C27" s="77"/>
-      <c r="D27" s="123"/>
-      <c r="E27" s="124"/>
-      <c r="F27" s="124"/>
+      <c r="A27" s="78" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="93" t="s">
+        <v>177</v>
+      </c>
+      <c r="C27" s="77" t="s">
+        <v>178</v>
+      </c>
+      <c r="D27" s="126"/>
+      <c r="E27" s="127"/>
+      <c r="F27" s="127"/>
       <c r="G27" s="76"/>
       <c r="H27" s="83"/>
       <c r="I27" s="77"/>
       <c r="J27" s="75"/>
     </row>
-    <row r="28" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
-      <c r="A28" s="78"/>
-      <c r="B28" s="93"/>
-      <c r="C28" s="77"/>
-      <c r="D28" s="123"/>
-      <c r="E28" s="124"/>
-      <c r="F28" s="124"/>
-      <c r="G28" s="76"/>
-      <c r="H28" s="83"/>
-      <c r="I28" s="77"/>
-      <c r="J28" s="75"/>
-    </row>
-    <row r="29" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A29" s="121"/>
-      <c r="B29" s="122"/>
-      <c r="C29" s="122"/>
-      <c r="D29" s="98"/>
-      <c r="E29" s="98"/>
-      <c r="F29" s="98"/>
-      <c r="G29" s="98"/>
-      <c r="H29" s="98"/>
-      <c r="I29" s="98"/>
-      <c r="J29" s="99"/>
-    </row>
-    <row r="30" spans="1:10" s="4" customFormat="1" ht="78.75" customHeight="1" outlineLevel="1">
+    <row r="28" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
+      <c r="A28" s="124"/>
+      <c r="B28" s="125"/>
+      <c r="C28" s="125"/>
+      <c r="D28" s="98"/>
+      <c r="E28" s="98"/>
+      <c r="F28" s="98"/>
+      <c r="G28" s="98"/>
+      <c r="H28" s="98"/>
+      <c r="I28" s="98"/>
+      <c r="J28" s="99"/>
+    </row>
+    <row r="29" spans="1:10" s="4" customFormat="1" ht="78.75" customHeight="1" outlineLevel="1">
+      <c r="A29" s="78"/>
+      <c r="B29" s="93"/>
+      <c r="C29" s="77"/>
+      <c r="D29" s="126"/>
+      <c r="E29" s="127"/>
+      <c r="F29" s="127"/>
+      <c r="G29" s="76"/>
+      <c r="H29" s="83"/>
+      <c r="I29" s="77"/>
+      <c r="J29" s="75"/>
+    </row>
+    <row r="30" spans="1:10" s="4" customFormat="1" ht="79.5" customHeight="1" outlineLevel="1">
       <c r="A30" s="78"/>
       <c r="B30" s="93"/>
       <c r="C30" s="77"/>
-      <c r="D30" s="123"/>
-      <c r="E30" s="124"/>
-      <c r="F30" s="124"/>
+      <c r="D30" s="126"/>
+      <c r="E30" s="127"/>
+      <c r="F30" s="127"/>
       <c r="G30" s="76"/>
       <c r="H30" s="83"/>
       <c r="I30" s="77"/>
@@ -4929,9 +4988,9 @@
       <c r="A31" s="78"/>
       <c r="B31" s="93"/>
       <c r="C31" s="77"/>
-      <c r="D31" s="123"/>
-      <c r="E31" s="124"/>
-      <c r="F31" s="124"/>
+      <c r="D31" s="126"/>
+      <c r="E31" s="127"/>
+      <c r="F31" s="127"/>
       <c r="G31" s="76"/>
       <c r="H31" s="83"/>
       <c r="I31" s="77"/>
@@ -4941,73 +5000,65 @@
       <c r="A32" s="78"/>
       <c r="B32" s="93"/>
       <c r="C32" s="77"/>
-      <c r="D32" s="123"/>
-      <c r="E32" s="124"/>
-      <c r="F32" s="124"/>
+      <c r="D32" s="126"/>
+      <c r="E32" s="127"/>
+      <c r="F32" s="127"/>
       <c r="G32" s="76"/>
       <c r="H32" s="83"/>
       <c r="I32" s="77"/>
       <c r="J32" s="75"/>
     </row>
-    <row r="33" spans="1:10" s="4" customFormat="1" ht="79.5" customHeight="1" outlineLevel="1">
+    <row r="33" spans="1:10" s="4" customFormat="1" ht="91.5" customHeight="1" outlineLevel="1">
       <c r="A33" s="78"/>
       <c r="B33" s="93"/>
       <c r="C33" s="77"/>
-      <c r="D33" s="123"/>
-      <c r="E33" s="124"/>
-      <c r="F33" s="124"/>
+      <c r="D33" s="126"/>
+      <c r="E33" s="127"/>
+      <c r="F33" s="127"/>
       <c r="G33" s="76"/>
       <c r="H33" s="83"/>
       <c r="I33" s="77"/>
       <c r="J33" s="75"/>
     </row>
-    <row r="34" spans="1:10" s="4" customFormat="1" ht="91.5" customHeight="1" outlineLevel="1">
+    <row r="34" spans="1:10" s="4" customFormat="1" ht="67.5" customHeight="1" outlineLevel="1">
       <c r="A34" s="78"/>
       <c r="B34" s="93"/>
       <c r="C34" s="77"/>
-      <c r="D34" s="123"/>
-      <c r="E34" s="124"/>
-      <c r="F34" s="124"/>
+      <c r="D34" s="126"/>
+      <c r="E34" s="127"/>
+      <c r="F34" s="127"/>
       <c r="G34" s="76"/>
       <c r="H34" s="83"/>
       <c r="I34" s="77"/>
       <c r="J34" s="75"/>
     </row>
-    <row r="35" spans="1:10" s="4" customFormat="1" ht="67.5" customHeight="1" outlineLevel="1">
-      <c r="A35" s="78"/>
-      <c r="B35" s="93"/>
-      <c r="C35" s="77"/>
-      <c r="D35" s="123"/>
-      <c r="E35" s="124"/>
-      <c r="F35" s="124"/>
-      <c r="G35" s="76"/>
-      <c r="H35" s="83"/>
-      <c r="I35" s="77"/>
-      <c r="J35" s="75"/>
-    </row>
-    <row r="36" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A36" s="121"/>
-      <c r="B36" s="122"/>
-      <c r="C36" s="122"/>
-      <c r="D36" s="98"/>
-      <c r="E36" s="98"/>
-      <c r="F36" s="98"/>
-      <c r="G36" s="98"/>
-      <c r="H36" s="98"/>
-      <c r="I36" s="98"/>
-      <c r="J36" s="99"/>
-    </row>
-    <row r="37" spans="1:10" s="4" customFormat="1" ht="47.25" customHeight="1" outlineLevel="1">
-      <c r="A37" s="78"/>
-      <c r="B37" s="93"/>
-      <c r="C37" s="77"/>
-      <c r="D37" s="123"/>
-      <c r="E37" s="124"/>
-      <c r="F37" s="124"/>
-      <c r="G37" s="76"/>
-      <c r="H37" s="83"/>
-      <c r="I37" s="77"/>
-      <c r="J37" s="75"/>
+    <row r="35" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
+      <c r="A35" s="124"/>
+      <c r="B35" s="125"/>
+      <c r="C35" s="125"/>
+      <c r="D35" s="98"/>
+      <c r="E35" s="98"/>
+      <c r="F35" s="98"/>
+      <c r="G35" s="98"/>
+      <c r="H35" s="98"/>
+      <c r="I35" s="98"/>
+      <c r="J35" s="99"/>
+    </row>
+    <row r="36" spans="1:10" s="4" customFormat="1" ht="47.25" customHeight="1" outlineLevel="1">
+      <c r="A36" s="78"/>
+      <c r="B36" s="93"/>
+      <c r="C36" s="77"/>
+      <c r="D36" s="126"/>
+      <c r="E36" s="127"/>
+      <c r="F36" s="127"/>
+      <c r="G36" s="76"/>
+      <c r="H36" s="83"/>
+      <c r="I36" s="77"/>
+      <c r="J36" s="75"/>
+    </row>
+    <row r="37" spans="1:10" ht="12" customHeight="1">
+      <c r="I37"/>
+      <c r="J37"/>
     </row>
     <row r="38" spans="1:10" ht="12" customHeight="1">
       <c r="I38"/>
@@ -5053,158 +5104,102 @@
       <c r="I48"/>
       <c r="J48"/>
     </row>
-    <row r="49" spans="8:12" ht="12" customHeight="1">
+    <row r="49" spans="9:10" ht="12" customHeight="1">
       <c r="I49"/>
       <c r="J49"/>
     </row>
-    <row r="50" spans="8:12" ht="12" customHeight="1">
+    <row r="50" spans="9:10" ht="12" customHeight="1">
       <c r="I50"/>
       <c r="J50"/>
     </row>
-    <row r="51" spans="8:12" ht="12" customHeight="1">
+    <row r="51" spans="9:10" ht="12" customHeight="1">
       <c r="I51"/>
       <c r="J51"/>
     </row>
-    <row r="52" spans="8:12" ht="12" customHeight="1">
+    <row r="52" spans="9:10" ht="12" customHeight="1">
       <c r="I52"/>
       <c r="J52"/>
     </row>
-    <row r="53" spans="8:12" ht="12" customHeight="1">
-      <c r="H53" s="154"/>
-      <c r="I53" s="154"/>
-      <c r="J53" s="154"/>
-      <c r="K53" s="154"/>
-      <c r="L53" s="154"/>
-    </row>
-    <row r="54" spans="8:12">
-      <c r="H54" s="154"/>
-      <c r="I54" s="155"/>
-      <c r="J54" s="154"/>
-      <c r="K54" s="154"/>
-      <c r="L54" s="154"/>
-    </row>
-    <row r="55" spans="8:12">
-      <c r="H55" s="154"/>
-      <c r="I55" s="155"/>
-      <c r="J55" s="154"/>
-      <c r="K55" s="154"/>
-      <c r="L55" s="154"/>
-    </row>
-    <row r="56" spans="8:12">
-      <c r="H56" s="154"/>
-      <c r="I56" s="155"/>
-      <c r="J56" s="154"/>
-      <c r="K56" s="154"/>
-      <c r="L56" s="154"/>
-    </row>
-    <row r="57" spans="8:12">
-      <c r="H57" s="154"/>
-      <c r="I57" s="155"/>
-      <c r="J57" s="154"/>
-      <c r="K57" s="154"/>
-      <c r="L57" s="154"/>
-    </row>
-    <row r="58" spans="8:12">
-      <c r="H58" s="154"/>
-      <c r="I58" s="155"/>
-      <c r="J58" s="154"/>
-      <c r="K58" s="154"/>
-      <c r="L58" s="154"/>
-    </row>
-    <row r="59" spans="8:12">
-      <c r="H59" s="154"/>
-      <c r="I59" s="155"/>
-      <c r="J59" s="154"/>
-      <c r="K59" s="154"/>
-      <c r="L59" s="154"/>
-    </row>
-    <row r="60" spans="8:12">
-      <c r="H60" s="154"/>
-      <c r="I60" s="155"/>
-      <c r="J60" s="154"/>
-      <c r="K60" s="154"/>
-      <c r="L60" s="154"/>
-    </row>
-    <row r="61" spans="8:12">
-      <c r="H61" s="154"/>
-      <c r="I61" s="155"/>
-      <c r="J61" s="154"/>
-      <c r="K61" s="154"/>
-      <c r="L61" s="154"/>
-    </row>
-    <row r="62" spans="8:12">
-      <c r="H62" s="154"/>
-      <c r="I62" s="155"/>
-      <c r="J62" s="154"/>
-      <c r="K62" s="154"/>
-      <c r="L62" s="154"/>
-    </row>
-    <row r="63" spans="8:12">
-      <c r="H63" s="154"/>
-      <c r="I63" s="155"/>
-      <c r="J63" s="154"/>
-      <c r="K63" s="154"/>
-      <c r="L63" s="154"/>
-    </row>
-    <row r="64" spans="8:12">
-      <c r="H64" s="154"/>
-      <c r="I64" s="155"/>
-      <c r="J64" s="154"/>
-      <c r="K64" s="154"/>
-      <c r="L64" s="154"/>
-    </row>
-    <row r="65" spans="8:12">
-      <c r="H65" s="154"/>
-      <c r="I65" s="155"/>
-      <c r="J65" s="154"/>
-      <c r="K65" s="154"/>
-      <c r="L65" s="154"/>
-    </row>
-    <row r="66" spans="8:12">
-      <c r="H66" s="154"/>
-      <c r="I66" s="155"/>
-      <c r="J66" s="154"/>
-      <c r="K66" s="154"/>
-      <c r="L66" s="154"/>
-    </row>
-    <row r="67" spans="8:12">
-      <c r="H67" s="154"/>
-      <c r="I67" s="155"/>
-      <c r="J67" s="154"/>
-      <c r="K67" s="154"/>
-      <c r="L67" s="154"/>
-    </row>
-    <row r="68" spans="8:12">
-      <c r="H68" s="154"/>
-      <c r="I68" s="155"/>
-      <c r="J68" s="154"/>
-      <c r="K68" s="154"/>
-      <c r="L68" s="154"/>
-    </row>
-    <row r="69" spans="8:12">
-      <c r="H69" s="154"/>
-      <c r="I69" s="155"/>
-      <c r="J69" s="154"/>
-      <c r="K69" s="154"/>
-      <c r="L69" s="154"/>
+    <row r="53" spans="9:10">
+      <c r="I53" s="19"/>
+      <c r="J53"/>
+    </row>
+    <row r="54" spans="9:10">
+      <c r="I54" s="19"/>
+      <c r="J54"/>
+    </row>
+    <row r="55" spans="9:10">
+      <c r="I55" s="19"/>
+      <c r="J55"/>
+    </row>
+    <row r="56" spans="9:10">
+      <c r="I56" s="19"/>
+      <c r="J56"/>
+    </row>
+    <row r="57" spans="9:10">
+      <c r="I57" s="19"/>
+      <c r="J57"/>
+    </row>
+    <row r="58" spans="9:10">
+      <c r="I58" s="19"/>
+      <c r="J58"/>
+    </row>
+    <row r="59" spans="9:10">
+      <c r="I59" s="19"/>
+      <c r="J59"/>
+    </row>
+    <row r="60" spans="9:10">
+      <c r="I60" s="19"/>
+      <c r="J60"/>
+    </row>
+    <row r="61" spans="9:10">
+      <c r="I61" s="19"/>
+      <c r="J61"/>
+    </row>
+    <row r="62" spans="9:10">
+      <c r="I62" s="19"/>
+      <c r="J62"/>
+    </row>
+    <row r="63" spans="9:10">
+      <c r="I63" s="19"/>
+      <c r="J63"/>
+    </row>
+    <row r="64" spans="9:10">
+      <c r="I64" s="19"/>
+      <c r="J64"/>
+    </row>
+    <row r="65" spans="9:10">
+      <c r="I65" s="19"/>
+      <c r="J65"/>
+    </row>
+    <row r="66" spans="9:10">
+      <c r="I66" s="19"/>
+      <c r="J66"/>
+    </row>
+    <row r="67" spans="9:10">
+      <c r="I67" s="19"/>
+      <c r="J67"/>
+    </row>
+    <row r="68" spans="9:10">
+      <c r="I68" s="19"/>
+      <c r="J68"/>
     </row>
   </sheetData>
-  <mergeCells count="44">
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="A29:C29"/>
+  <mergeCells count="43">
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="D29:F29"/>
     <mergeCell ref="D30:F30"/>
     <mergeCell ref="D31:F31"/>
     <mergeCell ref="D32:F32"/>
     <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="D25:F25"/>
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D28:F28"/>
     <mergeCell ref="D21:F21"/>
     <mergeCell ref="D22:F22"/>
     <mergeCell ref="D17:F17"/>
@@ -5227,13 +5222,13 @@
     <mergeCell ref="H9:H10"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="H5:J5"/>
     <mergeCell ref="B1:D2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="H4:J4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="H5:J5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5289,7 +5284,7 @@
       <c r="B4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="161">
+      <c r="C4" s="116">
         <v>45731</v>
       </c>
       <c r="D4" s="19"/>
@@ -5371,21 +5366,21 @@
         <f>Samples2!B4</f>
         <v>Đăng ký tham gia</v>
       </c>
-      <c r="D9" s="159">
+      <c r="D9" s="114">
         <f>Samples2!B6</f>
         <v>0</v>
       </c>
-      <c r="E9" s="160">
+      <c r="E9" s="115">
         <f>Samples2!B7</f>
         <v>0</v>
       </c>
-      <c r="F9" s="160">
+      <c r="F9" s="115">
         <f>Samples2!D6</f>
         <v>0</v>
       </c>
       <c r="G9" s="67">
         <f>Samples2!D7</f>
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.25">
@@ -5417,7 +5412,7 @@
       </c>
       <c r="G11" s="55">
         <f>SUM(G6:G10)</f>
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14.25">

</xml_diff>

<commit_message>
update tc user huy dang ky sk
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University_IT\Tam\KiemThuPhanMem\event-manager-javafx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688289DC-7AE4-4DB3-9D41-8C2EF28DFCC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB323376-314C-4F1F-92E8-44DD1A5317AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9810" yWindow="465" windowWidth="10365" windowHeight="10155" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="97" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="190">
   <si>
     <t>TC1</t>
   </si>
@@ -671,34 +671,6 @@
     <t>2. Hủy đăng ký</t>
   </si>
   <si>
-    <t>Kiểm tra hủy đăng ký trong thời gian cho phép</t>
-  </si>
-  <si>
-    <t>Kiểm tra hủy đăng ký trong thời gian không cho phép</t>
-  </si>
-  <si>
-    <t>1: User đăng nhập thành công vào hệ thống
-2: User đăng ký một sự kiện bất kỳ
-3: Sau đó truy cập vào trang Sự kiện đã đăng ký
-4: Chọn sự kiện và nhấn Hủy đăng ký(trong vòng 48h)
-5: Xác nhận hủy đăng ký
-6: Hiển thị thông báo hủy đăng ký sự kiện thành công(sự kiện đã được xóa khỏi danh sách sự kiện đã đăng ký)</t>
-  </si>
-  <si>
-    <t>1: User đăng nhập thành công vào hệ thống
-2: User đăng ký một sự kiện bất kỳ
-3: Sau đó truy cập vào trang Sự kiện đã đăng ký
-4: Chọn sự kiện và nhấn Hủy đăng ký(sau 48h)
-5: Xác nhận hủy đăng ký
-6: Hiển thị thông báo lỗi không thể hủy đăng ký sự kiện này</t>
-  </si>
-  <si>
-    <t>Viết TC Kiểm tra hủy đăng ký trong thời gian cho phép</t>
-  </si>
-  <si>
-    <t>Viết TC Kiểm tra hủy đăng ký trong thời gian không cho phép</t>
-  </si>
-  <si>
     <t>2.0</t>
   </si>
   <si>
@@ -759,12 +731,65 @@
   <si>
     <t>Viết TC Kiểm tra chức năng tìm kiếm người dùng</t>
   </si>
+  <si>
+    <t>Kiểm tra chức năng hủy đăng ký trong thời gian không cho phép</t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra chức năng hủy đăng ký trong thời gian cho phép</t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra chức năng hủy đăng ký trong thời gian không cho phép</t>
+  </si>
+  <si>
+    <t>Hiển thị thông báo hủy đăng ký thành công sự kiện
+Hoàn tiền đầy đủ cho user
+Sự kiện đã được xóa khỏi danh sách sự kiện đã đăng ký</t>
+  </si>
+  <si>
+    <t>1: User đăng nhập thành công vào hệ thống
+2: Truy cập vào trang Quản lý đăng ký sự kiện
+3: Chọn sự kiện cần hủy đăng ký(trước khi diễn ra sự kiện ít nhất 24h)
+4: Nhấn Hủy đăng ký
+5: Xác nhận hủy đăng ký</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng hủy đăng ký thành công trong thời gian cho phép</t>
+  </si>
+  <si>
+    <t>1: User đăng nhập thành công vào hệ thống
+2: Truy cập vào trang Quản lý đăng ký sự kiện
+3: Chọn sự kiện cần hủy đăng ký(trước khi diễn ra sự kiện dưới 24h)
+4: Nhấn Hủy đăng ký</t>
+  </si>
+  <si>
+    <t>Hiển thị thông báo lỗi không thể hủy đăng ký do đã quá thời hạn hủy
+Không hoàn tiền
+Sự kiện vẫn hiển thị trong danh sách sự kiện đã đăng ký</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng hủy đăng ký với sự kiện miễn phí</t>
+  </si>
+  <si>
+    <t>Hiển thị thông báo hủy đăng ký thành công sự kiện
+Không hoàn tiền vì sự kiện miễn phí
+Sự kiện đã được xóa khỏi danh sách sự kiện đã đăng ký</t>
+  </si>
+  <si>
+    <t>Cập nhật TC Kiểm tra chức năng hủy đăng ký thành công trong thời gian cho phép</t>
+  </si>
+  <si>
+    <t>Cập nhật TC Kiểm tra chức năng hủy đăng ký trong thời gian không cho phép</t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra chức năng hủy đăng ký với sự kiện miễn phí</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
@@ -1457,13 +1482,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1773,12 +1799,111 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1788,107 +1913,15 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="Comma" xfId="4" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Functional Test Case v1.0" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal_Sheet1_Vanco_CR022a1_TestCase_v0.1" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -2220,8 +2253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H72"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A11" zoomScale="85" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView showGridLines="0" topLeftCell="B44" zoomScale="85" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -2857,7 +2890,7 @@
       </c>
       <c r="D41" s="101"/>
       <c r="E41" s="106" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="F41" s="112" t="s">
         <v>44</v>
@@ -2870,7 +2903,7 @@
         <v>45745</v>
       </c>
       <c r="C42" s="37" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D42" s="101"/>
       <c r="E42" s="106" t="s">
@@ -2959,7 +2992,7 @@
       </c>
       <c r="D47" s="101"/>
       <c r="E47" s="106" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="F47" s="112" t="s">
         <v>44</v>
@@ -2976,7 +3009,7 @@
       </c>
       <c r="D48" s="101"/>
       <c r="E48" s="106" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="F48" s="112" t="s">
         <v>44</v>
@@ -2993,7 +3026,7 @@
       </c>
       <c r="D49" s="101"/>
       <c r="E49" s="106" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="F49" s="112" t="s">
         <v>44</v>
@@ -3010,7 +3043,7 @@
       </c>
       <c r="D50" s="101"/>
       <c r="E50" s="106" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="F50" s="112" t="s">
         <v>44</v>
@@ -3027,7 +3060,7 @@
       </c>
       <c r="D51" s="101"/>
       <c r="E51" s="106" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="F51" s="112" t="s">
         <v>44</v>
@@ -3044,7 +3077,7 @@
       </c>
       <c r="D52" s="101"/>
       <c r="E52" s="106" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="F52" s="112" t="s">
         <v>44</v>
@@ -3052,30 +3085,54 @@
       <c r="G52" s="101"/>
       <c r="H52" s="107"/>
     </row>
-    <row r="53" spans="2:8" s="34" customFormat="1">
-      <c r="B53" s="36"/>
-      <c r="C53" s="37"/>
+    <row r="53" spans="2:8" s="34" customFormat="1" ht="25.5">
+      <c r="B53" s="36">
+        <v>45750</v>
+      </c>
+      <c r="C53" s="37" t="s">
+        <v>161</v>
+      </c>
       <c r="D53" s="101"/>
-      <c r="E53" s="106"/>
-      <c r="F53" s="112"/>
+      <c r="E53" s="106" t="s">
+        <v>187</v>
+      </c>
+      <c r="F53" s="112" t="s">
+        <v>44</v>
+      </c>
       <c r="G53" s="101"/>
       <c r="H53" s="107"/>
     </row>
-    <row r="54" spans="2:8" s="34" customFormat="1">
-      <c r="B54" s="36"/>
-      <c r="C54" s="37"/>
+    <row r="54" spans="2:8" s="34" customFormat="1" ht="25.5">
+      <c r="B54" s="36">
+        <v>45750</v>
+      </c>
+      <c r="C54" s="37" t="s">
+        <v>161</v>
+      </c>
       <c r="D54" s="101"/>
-      <c r="E54" s="106"/>
-      <c r="F54" s="112"/>
+      <c r="E54" s="106" t="s">
+        <v>188</v>
+      </c>
+      <c r="F54" s="112" t="s">
+        <v>44</v>
+      </c>
       <c r="G54" s="101"/>
       <c r="H54" s="107"/>
     </row>
-    <row r="55" spans="2:8" s="34" customFormat="1">
-      <c r="B55" s="36"/>
-      <c r="C55" s="37"/>
+    <row r="55" spans="2:8" s="34" customFormat="1" ht="25.5">
+      <c r="B55" s="36">
+        <v>45750</v>
+      </c>
+      <c r="C55" s="37" t="s">
+        <v>40</v>
+      </c>
       <c r="D55" s="101"/>
-      <c r="E55" s="106"/>
-      <c r="F55" s="112"/>
+      <c r="E55" s="106" t="s">
+        <v>189</v>
+      </c>
+      <c r="F55" s="112" t="s">
+        <v>44</v>
+      </c>
       <c r="G55" s="101"/>
       <c r="H55" s="107"/>
     </row>
@@ -3247,7 +3304,7 @@
     <oddFooter>&amp;L&amp;"Tahoma,Regular"&amp;8 02ae-BM/PM/HDCV/FSOFT v1/0&amp;R&amp;"Tahoma,Regular"&amp;10&amp;P/&amp;N</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="C12:C34 C42 C35:C41 C43:C48 C49:C52" numberStoredAsText="1"/>
+    <ignoredError sqref="C12:C34 C42 C35:C41 C43:C48 C49:C52 C53:C55" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -3259,8 +3316,8 @@
   </sheetPr>
   <dimension ref="A1:K95"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" zoomScale="85" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView topLeftCell="A5" zoomScale="85" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" outlineLevelRow="1"/>
@@ -3279,9 +3336,9 @@
       <c r="A1" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="140"/>
-      <c r="C1" s="140"/>
-      <c r="D1" s="140"/>
+      <c r="B1" s="123"/>
+      <c r="C1" s="123"/>
+      <c r="D1" s="123"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -3292,9 +3349,9 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="141"/>
-      <c r="C2" s="141"/>
-      <c r="D2" s="141"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="124"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -3315,43 +3372,43 @@
       <c r="E3" s="61"/>
       <c r="F3" s="61"/>
       <c r="G3" s="61"/>
-      <c r="H3" s="148"/>
-      <c r="I3" s="148"/>
-      <c r="J3" s="148"/>
+      <c r="H3" s="133"/>
+      <c r="I3" s="133"/>
+      <c r="J3" s="133"/>
       <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="12.75">
       <c r="A4" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="149" t="s">
+      <c r="B4" s="135" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="150"/>
-      <c r="D4" s="151"/>
+      <c r="C4" s="136"/>
+      <c r="D4" s="137"/>
       <c r="E4" s="61"/>
       <c r="F4" s="61"/>
       <c r="G4" s="61"/>
-      <c r="H4" s="148"/>
-      <c r="I4" s="148"/>
-      <c r="J4" s="148"/>
+      <c r="H4" s="133"/>
+      <c r="I4" s="133"/>
+      <c r="J4" s="133"/>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" s="71" customFormat="1" ht="25.5">
       <c r="A5" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="143" t="s">
+      <c r="B5" s="126" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="144"/>
-      <c r="D5" s="145"/>
+      <c r="C5" s="127"/>
+      <c r="D5" s="128"/>
       <c r="E5" s="69"/>
       <c r="F5" s="69"/>
       <c r="G5" s="69"/>
-      <c r="H5" s="147"/>
-      <c r="I5" s="147"/>
-      <c r="J5" s="147"/>
+      <c r="H5" s="132"/>
+      <c r="I5" s="132"/>
+      <c r="J5" s="132"/>
       <c r="K5" s="70"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
@@ -3372,9 +3429,9 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="148"/>
-      <c r="I6" s="148"/>
-      <c r="J6" s="148"/>
+      <c r="H6" s="133"/>
+      <c r="I6" s="133"/>
+      <c r="J6" s="133"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -3395,16 +3452,16 @@
       <c r="E7" s="62"/>
       <c r="F7" s="62"/>
       <c r="G7" s="62"/>
-      <c r="H7" s="148"/>
-      <c r="I7" s="148"/>
-      <c r="J7" s="148"/>
+      <c r="H7" s="133"/>
+      <c r="I7" s="133"/>
+      <c r="J7" s="133"/>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="142"/>
-      <c r="B8" s="142"/>
-      <c r="C8" s="142"/>
-      <c r="D8" s="142"/>
+      <c r="A8" s="125"/>
+      <c r="B8" s="125"/>
+      <c r="C8" s="125"/>
+      <c r="D8" s="125"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -3414,70 +3471,70 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" s="73" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="131" t="s">
+      <c r="A9" s="142" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="155" t="s">
+      <c r="B9" s="143" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="131" t="s">
+      <c r="C9" s="142" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="132" t="s">
+      <c r="D9" s="149" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="133"/>
-      <c r="F9" s="133"/>
-      <c r="G9" s="134"/>
-      <c r="H9" s="152" t="s">
+      <c r="E9" s="150"/>
+      <c r="F9" s="150"/>
+      <c r="G9" s="151"/>
+      <c r="H9" s="138" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="128" t="s">
+      <c r="I9" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="128" t="s">
+      <c r="J9" s="134" t="s">
         <v>32</v>
       </c>
       <c r="K9" s="72"/>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="128"/>
-      <c r="B10" s="156"/>
-      <c r="C10" s="128"/>
-      <c r="D10" s="135"/>
-      <c r="E10" s="136"/>
-      <c r="F10" s="136"/>
-      <c r="G10" s="137"/>
-      <c r="H10" s="135"/>
-      <c r="I10" s="128"/>
-      <c r="J10" s="128"/>
+      <c r="A10" s="134"/>
+      <c r="B10" s="144"/>
+      <c r="C10" s="134"/>
+      <c r="D10" s="139"/>
+      <c r="E10" s="152"/>
+      <c r="F10" s="152"/>
+      <c r="G10" s="153"/>
+      <c r="H10" s="139"/>
+      <c r="I10" s="134"/>
+      <c r="J10" s="134"/>
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" s="74" customFormat="1" ht="15">
-      <c r="A11" s="153"/>
-      <c r="B11" s="153"/>
-      <c r="C11" s="153"/>
-      <c r="D11" s="153"/>
-      <c r="E11" s="153"/>
-      <c r="F11" s="153"/>
-      <c r="G11" s="153"/>
-      <c r="H11" s="153"/>
-      <c r="I11" s="153"/>
-      <c r="J11" s="154"/>
+      <c r="A11" s="140"/>
+      <c r="B11" s="140"/>
+      <c r="C11" s="140"/>
+      <c r="D11" s="140"/>
+      <c r="E11" s="140"/>
+      <c r="F11" s="140"/>
+      <c r="G11" s="140"/>
+      <c r="H11" s="140"/>
+      <c r="I11" s="140"/>
+      <c r="J11" s="141"/>
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A12" s="138" t="s">
+      <c r="A12" s="129" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="139"/>
-      <c r="C12" s="139"/>
-      <c r="D12" s="139"/>
-      <c r="E12" s="139"/>
-      <c r="F12" s="139"/>
-      <c r="G12" s="139"/>
-      <c r="H12" s="139"/>
-      <c r="I12" s="139"/>
-      <c r="J12" s="146"/>
+      <c r="B12" s="130"/>
+      <c r="C12" s="130"/>
+      <c r="D12" s="130"/>
+      <c r="E12" s="130"/>
+      <c r="F12" s="130"/>
+      <c r="G12" s="130"/>
+      <c r="H12" s="130"/>
+      <c r="I12" s="130"/>
+      <c r="J12" s="131"/>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" ht="66.75" customHeight="1" outlineLevel="1">
       <c r="A13" s="78" t="s">
@@ -3489,9 +3546,9 @@
       <c r="C13" s="77" t="s">
         <v>85</v>
       </c>
-      <c r="D13" s="119"/>
-      <c r="E13" s="120"/>
-      <c r="F13" s="120"/>
+      <c r="D13" s="147"/>
+      <c r="E13" s="148"/>
+      <c r="F13" s="148"/>
       <c r="G13" s="76"/>
       <c r="H13" s="90"/>
       <c r="I13" s="77"/>
@@ -3507,9 +3564,9 @@
       <c r="C14" s="77" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="119"/>
-      <c r="E14" s="120"/>
-      <c r="F14" s="120"/>
+      <c r="D14" s="147"/>
+      <c r="E14" s="148"/>
+      <c r="F14" s="148"/>
       <c r="G14" s="76"/>
       <c r="H14" s="90"/>
       <c r="I14" s="77"/>
@@ -3525,9 +3582,9 @@
       <c r="C15" s="77" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="119"/>
-      <c r="E15" s="120"/>
-      <c r="F15" s="120"/>
+      <c r="D15" s="147"/>
+      <c r="E15" s="148"/>
+      <c r="F15" s="148"/>
       <c r="G15" s="76"/>
       <c r="H15" s="90"/>
       <c r="I15" s="77"/>
@@ -3543,9 +3600,9 @@
       <c r="C16" s="77" t="s">
         <v>95</v>
       </c>
-      <c r="D16" s="119"/>
-      <c r="E16" s="120"/>
-      <c r="F16" s="120"/>
+      <c r="D16" s="147"/>
+      <c r="E16" s="148"/>
+      <c r="F16" s="148"/>
       <c r="G16" s="76"/>
       <c r="H16" s="90"/>
       <c r="I16" s="77"/>
@@ -3561,9 +3618,9 @@
       <c r="C17" s="77" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="119"/>
-      <c r="E17" s="120"/>
-      <c r="F17" s="120"/>
+      <c r="D17" s="147"/>
+      <c r="E17" s="148"/>
+      <c r="F17" s="148"/>
       <c r="G17" s="76"/>
       <c r="H17" s="90"/>
       <c r="I17" s="77"/>
@@ -3579,9 +3636,9 @@
       <c r="C18" s="77" t="s">
         <v>93</v>
       </c>
-      <c r="D18" s="119"/>
-      <c r="E18" s="120"/>
-      <c r="F18" s="120"/>
+      <c r="D18" s="147"/>
+      <c r="E18" s="148"/>
+      <c r="F18" s="148"/>
       <c r="G18" s="76"/>
       <c r="H18" s="90"/>
       <c r="I18" s="77"/>
@@ -3597,9 +3654,9 @@
       <c r="C19" s="87" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="121"/>
-      <c r="E19" s="122"/>
-      <c r="F19" s="123"/>
+      <c r="D19" s="154"/>
+      <c r="E19" s="155"/>
+      <c r="F19" s="156"/>
       <c r="G19" s="77"/>
       <c r="H19" s="77"/>
       <c r="I19" s="77"/>
@@ -3615,20 +3672,20 @@
       <c r="C20" s="77" t="s">
         <v>102</v>
       </c>
-      <c r="D20" s="121"/>
-      <c r="E20" s="122"/>
-      <c r="F20" s="123"/>
+      <c r="D20" s="154"/>
+      <c r="E20" s="155"/>
+      <c r="F20" s="156"/>
       <c r="G20" s="77"/>
       <c r="H20" s="77"/>
       <c r="I20" s="77"/>
       <c r="J20" s="75"/>
     </row>
     <row r="21" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A21" s="138" t="s">
+      <c r="A21" s="129" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="139"/>
-      <c r="C21" s="139"/>
+      <c r="B21" s="130"/>
+      <c r="C21" s="130"/>
       <c r="D21" s="88"/>
       <c r="E21" s="88"/>
       <c r="F21" s="88"/>
@@ -3647,9 +3704,9 @@
       <c r="C22" s="87" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="129"/>
-      <c r="E22" s="130"/>
-      <c r="F22" s="130"/>
+      <c r="D22" s="145"/>
+      <c r="E22" s="146"/>
+      <c r="F22" s="146"/>
       <c r="G22" s="95"/>
       <c r="H22" s="96"/>
       <c r="I22" s="87"/>
@@ -3665,9 +3722,9 @@
       <c r="C23" s="87" t="s">
         <v>72</v>
       </c>
-      <c r="D23" s="129"/>
-      <c r="E23" s="130"/>
-      <c r="F23" s="130"/>
+      <c r="D23" s="145"/>
+      <c r="E23" s="146"/>
+      <c r="F23" s="146"/>
       <c r="G23" s="95"/>
       <c r="H23" s="96"/>
       <c r="I23" s="87"/>
@@ -3683,9 +3740,9 @@
       <c r="C24" s="87" t="s">
         <v>75</v>
       </c>
-      <c r="D24" s="129"/>
-      <c r="E24" s="130"/>
-      <c r="F24" s="130"/>
+      <c r="D24" s="145"/>
+      <c r="E24" s="146"/>
+      <c r="F24" s="146"/>
       <c r="G24" s="95"/>
       <c r="H24" s="96"/>
       <c r="I24" s="87"/>
@@ -3701,9 +3758,9 @@
       <c r="C25" s="87" t="s">
         <v>77</v>
       </c>
-      <c r="D25" s="121"/>
-      <c r="E25" s="122"/>
-      <c r="F25" s="123"/>
+      <c r="D25" s="154"/>
+      <c r="E25" s="155"/>
+      <c r="F25" s="156"/>
       <c r="G25" s="77"/>
       <c r="H25" s="77"/>
       <c r="I25" s="77"/>
@@ -3719,9 +3776,9 @@
       <c r="C26" s="87" t="s">
         <v>99</v>
       </c>
-      <c r="D26" s="121"/>
-      <c r="E26" s="122"/>
-      <c r="F26" s="123"/>
+      <c r="D26" s="154"/>
+      <c r="E26" s="155"/>
+      <c r="F26" s="156"/>
       <c r="G26" s="77"/>
       <c r="H26" s="77"/>
       <c r="I26" s="77"/>
@@ -3737,9 +3794,9 @@
       <c r="C27" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="121"/>
-      <c r="E27" s="122"/>
-      <c r="F27" s="123"/>
+      <c r="D27" s="154"/>
+      <c r="E27" s="155"/>
+      <c r="F27" s="156"/>
       <c r="G27" s="77"/>
       <c r="H27" s="77"/>
       <c r="I27" s="77"/>
@@ -3755,9 +3812,9 @@
       <c r="C28" s="77" t="s">
         <v>79</v>
       </c>
-      <c r="D28" s="121"/>
-      <c r="E28" s="122"/>
-      <c r="F28" s="123"/>
+      <c r="D28" s="154"/>
+      <c r="E28" s="155"/>
+      <c r="F28" s="156"/>
       <c r="G28" s="77"/>
       <c r="H28" s="77"/>
       <c r="I28" s="77"/>
@@ -3773,9 +3830,9 @@
       <c r="C29" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="121"/>
-      <c r="E29" s="122"/>
-      <c r="F29" s="123"/>
+      <c r="D29" s="154"/>
+      <c r="E29" s="155"/>
+      <c r="F29" s="156"/>
       <c r="G29" s="77"/>
       <c r="H29" s="77"/>
       <c r="I29" s="77"/>
@@ -3791,9 +3848,9 @@
       <c r="C30" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="D30" s="121"/>
-      <c r="E30" s="122"/>
-      <c r="F30" s="123"/>
+      <c r="D30" s="154"/>
+      <c r="E30" s="155"/>
+      <c r="F30" s="156"/>
       <c r="G30" s="77"/>
       <c r="H30" s="77"/>
       <c r="I30" s="77"/>
@@ -3809,9 +3866,9 @@
       <c r="C31" s="77" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="121"/>
-      <c r="E31" s="122"/>
-      <c r="F31" s="123"/>
+      <c r="D31" s="154"/>
+      <c r="E31" s="155"/>
+      <c r="F31" s="156"/>
       <c r="G31" s="77"/>
       <c r="H31" s="77"/>
       <c r="I31" s="77"/>
@@ -3827,20 +3884,20 @@
       <c r="C32" s="77" t="s">
         <v>101</v>
       </c>
-      <c r="D32" s="121"/>
-      <c r="E32" s="122"/>
-      <c r="F32" s="123"/>
+      <c r="D32" s="154"/>
+      <c r="E32" s="155"/>
+      <c r="F32" s="156"/>
       <c r="G32" s="77"/>
       <c r="H32" s="77"/>
       <c r="I32" s="77"/>
       <c r="J32" s="75"/>
     </row>
     <row r="33" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A33" s="124" t="s">
+      <c r="A33" s="119" t="s">
         <v>81</v>
       </c>
-      <c r="B33" s="125"/>
-      <c r="C33" s="125"/>
+      <c r="B33" s="120"/>
+      <c r="C33" s="120"/>
       <c r="D33" s="98"/>
       <c r="E33" s="98"/>
       <c r="F33" s="98"/>
@@ -3859,20 +3916,20 @@
       <c r="C34" s="77" t="s">
         <v>84</v>
       </c>
-      <c r="D34" s="126"/>
-      <c r="E34" s="127"/>
-      <c r="F34" s="127"/>
+      <c r="D34" s="121"/>
+      <c r="E34" s="122"/>
+      <c r="F34" s="122"/>
       <c r="G34" s="76"/>
       <c r="H34" s="83"/>
       <c r="I34" s="77"/>
       <c r="J34" s="75"/>
     </row>
     <row r="35" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A35" s="124" t="s">
+      <c r="A35" s="119" t="s">
         <v>82</v>
       </c>
-      <c r="B35" s="125"/>
-      <c r="C35" s="125"/>
+      <c r="B35" s="120"/>
+      <c r="C35" s="120"/>
       <c r="D35" s="98"/>
       <c r="E35" s="98"/>
       <c r="F35" s="98"/>
@@ -3891,9 +3948,9 @@
       <c r="C36" s="77" t="s">
         <v>145</v>
       </c>
-      <c r="D36" s="126"/>
-      <c r="E36" s="127"/>
-      <c r="F36" s="127"/>
+      <c r="D36" s="121"/>
+      <c r="E36" s="122"/>
+      <c r="F36" s="122"/>
       <c r="G36" s="76"/>
       <c r="H36" s="83"/>
       <c r="I36" s="77"/>
@@ -3909,9 +3966,9 @@
       <c r="C37" s="77" t="s">
         <v>147</v>
       </c>
-      <c r="D37" s="126"/>
-      <c r="E37" s="127"/>
-      <c r="F37" s="127"/>
+      <c r="D37" s="121"/>
+      <c r="E37" s="122"/>
+      <c r="F37" s="122"/>
       <c r="G37" s="76"/>
       <c r="H37" s="83"/>
       <c r="I37" s="77"/>
@@ -3927,9 +3984,9 @@
       <c r="C38" s="77" t="s">
         <v>146</v>
       </c>
-      <c r="D38" s="126"/>
-      <c r="E38" s="127"/>
-      <c r="F38" s="127"/>
+      <c r="D38" s="121"/>
+      <c r="E38" s="122"/>
+      <c r="F38" s="122"/>
       <c r="G38" s="76"/>
       <c r="H38" s="83"/>
       <c r="I38" s="77"/>
@@ -3945,9 +4002,9 @@
       <c r="C39" s="77" t="s">
         <v>149</v>
       </c>
-      <c r="D39" s="126"/>
-      <c r="E39" s="127"/>
-      <c r="F39" s="127"/>
+      <c r="D39" s="121"/>
+      <c r="E39" s="122"/>
+      <c r="F39" s="122"/>
       <c r="G39" s="76"/>
       <c r="H39" s="83"/>
       <c r="I39" s="77"/>
@@ -3963,20 +4020,20 @@
       <c r="C40" s="77" t="s">
         <v>151</v>
       </c>
-      <c r="D40" s="126"/>
-      <c r="E40" s="127"/>
-      <c r="F40" s="127"/>
+      <c r="D40" s="121"/>
+      <c r="E40" s="122"/>
+      <c r="F40" s="122"/>
       <c r="G40" s="76"/>
       <c r="H40" s="83"/>
       <c r="I40" s="77"/>
       <c r="J40" s="75"/>
     </row>
     <row r="41" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A41" s="124" t="s">
+      <c r="A41" s="119" t="s">
         <v>120</v>
       </c>
-      <c r="B41" s="125"/>
-      <c r="C41" s="125"/>
+      <c r="B41" s="120"/>
+      <c r="C41" s="120"/>
       <c r="D41" s="98"/>
       <c r="E41" s="98"/>
       <c r="F41" s="98"/>
@@ -3995,9 +4052,9 @@
       <c r="C42" s="77" t="s">
         <v>127</v>
       </c>
-      <c r="D42" s="126"/>
-      <c r="E42" s="127"/>
-      <c r="F42" s="127"/>
+      <c r="D42" s="121"/>
+      <c r="E42" s="122"/>
+      <c r="F42" s="122"/>
       <c r="G42" s="76"/>
       <c r="H42" s="83"/>
       <c r="I42" s="77"/>
@@ -4013,9 +4070,9 @@
       <c r="C43" s="77" t="s">
         <v>128</v>
       </c>
-      <c r="D43" s="126"/>
-      <c r="E43" s="127"/>
-      <c r="F43" s="127"/>
+      <c r="D43" s="121"/>
+      <c r="E43" s="122"/>
+      <c r="F43" s="122"/>
       <c r="G43" s="76"/>
       <c r="H43" s="83"/>
       <c r="I43" s="77"/>
@@ -4031,9 +4088,9 @@
       <c r="C44" s="77" t="s">
         <v>129</v>
       </c>
-      <c r="D44" s="126"/>
-      <c r="E44" s="127"/>
-      <c r="F44" s="127"/>
+      <c r="D44" s="121"/>
+      <c r="E44" s="122"/>
+      <c r="F44" s="122"/>
       <c r="G44" s="76"/>
       <c r="H44" s="83"/>
       <c r="I44" s="77"/>
@@ -4049,9 +4106,9 @@
       <c r="C45" s="77" t="s">
         <v>130</v>
       </c>
-      <c r="D45" s="126"/>
-      <c r="E45" s="127"/>
-      <c r="F45" s="127"/>
+      <c r="D45" s="121"/>
+      <c r="E45" s="122"/>
+      <c r="F45" s="122"/>
       <c r="G45" s="76"/>
       <c r="H45" s="83"/>
       <c r="I45" s="77"/>
@@ -4067,9 +4124,9 @@
       <c r="C46" s="77" t="s">
         <v>132</v>
       </c>
-      <c r="D46" s="126"/>
-      <c r="E46" s="127"/>
-      <c r="F46" s="127"/>
+      <c r="D46" s="121"/>
+      <c r="E46" s="122"/>
+      <c r="F46" s="122"/>
       <c r="G46" s="76"/>
       <c r="H46" s="83"/>
       <c r="I46" s="77"/>
@@ -4085,20 +4142,20 @@
       <c r="C47" s="77" t="s">
         <v>124</v>
       </c>
-      <c r="D47" s="126"/>
-      <c r="E47" s="127"/>
-      <c r="F47" s="127"/>
+      <c r="D47" s="121"/>
+      <c r="E47" s="122"/>
+      <c r="F47" s="122"/>
       <c r="G47" s="76"/>
       <c r="H47" s="83"/>
       <c r="I47" s="77"/>
       <c r="J47" s="75"/>
     </row>
     <row r="48" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A48" s="124" t="s">
+      <c r="A48" s="119" t="s">
         <v>133</v>
       </c>
-      <c r="B48" s="125"/>
-      <c r="C48" s="125"/>
+      <c r="B48" s="120"/>
+      <c r="C48" s="120"/>
       <c r="D48" s="98"/>
       <c r="E48" s="98"/>
       <c r="F48" s="98"/>
@@ -4112,23 +4169,23 @@
         <v>0</v>
       </c>
       <c r="B49" s="93" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C49" s="77" t="s">
         <v>134</v>
       </c>
-      <c r="D49" s="126"/>
-      <c r="E49" s="127"/>
-      <c r="F49" s="127"/>
+      <c r="D49" s="121"/>
+      <c r="E49" s="122"/>
+      <c r="F49" s="122"/>
       <c r="G49" s="76"/>
       <c r="H49" s="83"/>
       <c r="I49" s="77"/>
       <c r="J49" s="75"/>
     </row>
     <row r="50" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A50" s="124"/>
-      <c r="B50" s="125"/>
-      <c r="C50" s="125"/>
+      <c r="A50" s="119"/>
+      <c r="B50" s="120"/>
+      <c r="C50" s="120"/>
       <c r="D50" s="98"/>
       <c r="E50" s="98"/>
       <c r="F50" s="98"/>
@@ -4141,18 +4198,18 @@
       <c r="A51" s="78"/>
       <c r="B51" s="93"/>
       <c r="C51" s="77"/>
-      <c r="D51" s="126"/>
-      <c r="E51" s="127"/>
-      <c r="F51" s="127"/>
+      <c r="D51" s="121"/>
+      <c r="E51" s="122"/>
+      <c r="F51" s="122"/>
       <c r="G51" s="76"/>
       <c r="H51" s="83"/>
       <c r="I51" s="77"/>
       <c r="J51" s="75"/>
     </row>
     <row r="52" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A52" s="124"/>
-      <c r="B52" s="125"/>
-      <c r="C52" s="125"/>
+      <c r="A52" s="119"/>
+      <c r="B52" s="120"/>
+      <c r="C52" s="120"/>
       <c r="D52" s="98"/>
       <c r="E52" s="98"/>
       <c r="F52" s="98"/>
@@ -4165,18 +4222,18 @@
       <c r="A53" s="78"/>
       <c r="B53" s="93"/>
       <c r="C53" s="77"/>
-      <c r="D53" s="126"/>
-      <c r="E53" s="127"/>
-      <c r="F53" s="127"/>
+      <c r="D53" s="121"/>
+      <c r="E53" s="122"/>
+      <c r="F53" s="122"/>
       <c r="G53" s="76"/>
       <c r="H53" s="83"/>
       <c r="I53" s="77"/>
       <c r="J53" s="75"/>
     </row>
     <row r="54" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A54" s="124"/>
-      <c r="B54" s="125"/>
-      <c r="C54" s="125"/>
+      <c r="A54" s="119"/>
+      <c r="B54" s="120"/>
+      <c r="C54" s="120"/>
       <c r="D54" s="98"/>
       <c r="E54" s="98"/>
       <c r="F54" s="98"/>
@@ -4189,18 +4246,18 @@
       <c r="A55" s="78"/>
       <c r="B55" s="93"/>
       <c r="C55" s="77"/>
-      <c r="D55" s="126"/>
-      <c r="E55" s="127"/>
-      <c r="F55" s="127"/>
+      <c r="D55" s="121"/>
+      <c r="E55" s="122"/>
+      <c r="F55" s="122"/>
       <c r="G55" s="76"/>
       <c r="H55" s="83"/>
       <c r="I55" s="77"/>
       <c r="J55" s="75"/>
     </row>
     <row r="56" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A56" s="124"/>
-      <c r="B56" s="125"/>
-      <c r="C56" s="125"/>
+      <c r="A56" s="119"/>
+      <c r="B56" s="120"/>
+      <c r="C56" s="120"/>
       <c r="D56" s="98"/>
       <c r="E56" s="98"/>
       <c r="F56" s="98"/>
@@ -4213,18 +4270,18 @@
       <c r="A57" s="78"/>
       <c r="B57" s="93"/>
       <c r="C57" s="77"/>
-      <c r="D57" s="126"/>
-      <c r="E57" s="127"/>
-      <c r="F57" s="127"/>
+      <c r="D57" s="121"/>
+      <c r="E57" s="122"/>
+      <c r="F57" s="122"/>
       <c r="G57" s="76"/>
       <c r="H57" s="83"/>
       <c r="I57" s="77"/>
       <c r="J57" s="75"/>
     </row>
     <row r="58" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A58" s="124"/>
-      <c r="B58" s="125"/>
-      <c r="C58" s="125"/>
+      <c r="A58" s="119"/>
+      <c r="B58" s="120"/>
+      <c r="C58" s="120"/>
       <c r="D58" s="98"/>
       <c r="E58" s="98"/>
       <c r="F58" s="98"/>
@@ -4237,18 +4294,18 @@
       <c r="A59" s="78"/>
       <c r="B59" s="93"/>
       <c r="C59" s="77"/>
-      <c r="D59" s="126"/>
-      <c r="E59" s="127"/>
-      <c r="F59" s="127"/>
+      <c r="D59" s="121"/>
+      <c r="E59" s="122"/>
+      <c r="F59" s="122"/>
       <c r="G59" s="76"/>
       <c r="H59" s="83"/>
       <c r="I59" s="77"/>
       <c r="J59" s="75"/>
     </row>
     <row r="60" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A60" s="124"/>
-      <c r="B60" s="125"/>
-      <c r="C60" s="125"/>
+      <c r="A60" s="119"/>
+      <c r="B60" s="120"/>
+      <c r="C60" s="120"/>
       <c r="D60" s="98"/>
       <c r="E60" s="98"/>
       <c r="F60" s="98"/>
@@ -4261,18 +4318,18 @@
       <c r="A61" s="78"/>
       <c r="B61" s="93"/>
       <c r="C61" s="77"/>
-      <c r="D61" s="126"/>
-      <c r="E61" s="127"/>
-      <c r="F61" s="127"/>
+      <c r="D61" s="121"/>
+      <c r="E61" s="122"/>
+      <c r="F61" s="122"/>
       <c r="G61" s="76"/>
       <c r="H61" s="83"/>
       <c r="I61" s="77"/>
       <c r="J61" s="75"/>
     </row>
     <row r="62" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A62" s="124"/>
-      <c r="B62" s="125"/>
-      <c r="C62" s="125"/>
+      <c r="A62" s="119"/>
+      <c r="B62" s="120"/>
+      <c r="C62" s="120"/>
       <c r="D62" s="98"/>
       <c r="E62" s="98"/>
       <c r="F62" s="98"/>
@@ -4285,9 +4342,9 @@
       <c r="A63" s="78"/>
       <c r="B63" s="93"/>
       <c r="C63" s="77"/>
-      <c r="D63" s="126"/>
-      <c r="E63" s="127"/>
-      <c r="F63" s="127"/>
+      <c r="D63" s="121"/>
+      <c r="E63" s="122"/>
+      <c r="F63" s="122"/>
       <c r="G63" s="76"/>
       <c r="H63" s="83"/>
       <c r="I63" s="77"/>
@@ -4423,6 +4480,60 @@
     </row>
   </sheetData>
   <mergeCells count="70">
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:G10"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="B1:D2"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="D53:F53"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="D47:F47"/>
     <mergeCell ref="A60:C60"/>
     <mergeCell ref="D61:F61"/>
     <mergeCell ref="A62:C62"/>
@@ -4439,60 +4550,6 @@
     <mergeCell ref="D59:F59"/>
     <mergeCell ref="A50:C50"/>
     <mergeCell ref="D51:F51"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="D53:F53"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="B1:D2"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:G10"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D18:F18"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4508,8 +4565,8 @@
   </sheetPr>
   <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="85" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26:F26"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="82" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" outlineLevelRow="1"/>
@@ -4528,9 +4585,9 @@
       <c r="A1" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="140"/>
-      <c r="C1" s="140"/>
-      <c r="D1" s="140"/>
+      <c r="B1" s="123"/>
+      <c r="C1" s="123"/>
+      <c r="D1" s="123"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -4541,9 +4598,9 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="141"/>
-      <c r="C2" s="141"/>
-      <c r="D2" s="141"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="124"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -4564,43 +4621,43 @@
       <c r="E3" s="61"/>
       <c r="F3" s="61"/>
       <c r="G3" s="61"/>
-      <c r="H3" s="148"/>
-      <c r="I3" s="148"/>
-      <c r="J3" s="148"/>
+      <c r="H3" s="133"/>
+      <c r="I3" s="133"/>
+      <c r="J3" s="133"/>
       <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="12.75">
       <c r="A4" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="149" t="s">
+      <c r="B4" s="135" t="s">
         <v>158</v>
       </c>
-      <c r="C4" s="150"/>
-      <c r="D4" s="151"/>
+      <c r="C4" s="136"/>
+      <c r="D4" s="137"/>
       <c r="E4" s="61"/>
       <c r="F4" s="61"/>
       <c r="G4" s="61"/>
-      <c r="H4" s="148"/>
-      <c r="I4" s="148"/>
-      <c r="J4" s="148"/>
+      <c r="H4" s="133"/>
+      <c r="I4" s="133"/>
+      <c r="J4" s="133"/>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" s="71" customFormat="1" ht="25.5">
       <c r="A5" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="143" t="s">
+      <c r="B5" s="126" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="144"/>
-      <c r="D5" s="145"/>
+      <c r="C5" s="127"/>
+      <c r="D5" s="128"/>
       <c r="E5" s="69"/>
       <c r="F5" s="69"/>
       <c r="G5" s="69"/>
-      <c r="H5" s="147"/>
-      <c r="I5" s="147"/>
-      <c r="J5" s="147"/>
+      <c r="H5" s="132"/>
+      <c r="I5" s="132"/>
+      <c r="J5" s="132"/>
       <c r="K5" s="70"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
@@ -4621,9 +4678,9 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="148"/>
-      <c r="I6" s="148"/>
-      <c r="J6" s="148"/>
+      <c r="H6" s="133"/>
+      <c r="I6" s="133"/>
+      <c r="J6" s="133"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -4639,21 +4696,21 @@
       </c>
       <c r="D7" s="59">
         <f>COUNTA(A12:A36) -3</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E7" s="62"/>
       <c r="F7" s="62"/>
       <c r="G7" s="62"/>
-      <c r="H7" s="148"/>
-      <c r="I7" s="148"/>
-      <c r="J7" s="148"/>
+      <c r="H7" s="133"/>
+      <c r="I7" s="133"/>
+      <c r="J7" s="133"/>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="142"/>
-      <c r="B8" s="142"/>
-      <c r="C8" s="142"/>
-      <c r="D8" s="142"/>
+      <c r="A8" s="125"/>
+      <c r="B8" s="125"/>
+      <c r="C8" s="125"/>
+      <c r="D8" s="125"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -4663,78 +4720,78 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" s="73" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="131" t="s">
+      <c r="A9" s="142" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="155" t="s">
+      <c r="B9" s="143" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="131" t="s">
+      <c r="C9" s="142" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="132" t="s">
+      <c r="D9" s="149" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="133"/>
-      <c r="F9" s="133"/>
-      <c r="G9" s="134"/>
-      <c r="H9" s="152" t="s">
+      <c r="E9" s="150"/>
+      <c r="F9" s="150"/>
+      <c r="G9" s="151"/>
+      <c r="H9" s="138" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="128" t="s">
+      <c r="I9" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="128" t="s">
+      <c r="J9" s="134" t="s">
         <v>32</v>
       </c>
       <c r="K9" s="72"/>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="128"/>
-      <c r="B10" s="156"/>
-      <c r="C10" s="128"/>
-      <c r="D10" s="135"/>
-      <c r="E10" s="136"/>
-      <c r="F10" s="136"/>
-      <c r="G10" s="137"/>
-      <c r="H10" s="135"/>
-      <c r="I10" s="128"/>
-      <c r="J10" s="128"/>
+      <c r="A10" s="134"/>
+      <c r="B10" s="144"/>
+      <c r="C10" s="134"/>
+      <c r="D10" s="139"/>
+      <c r="E10" s="152"/>
+      <c r="F10" s="152"/>
+      <c r="G10" s="153"/>
+      <c r="H10" s="139"/>
+      <c r="I10" s="134"/>
+      <c r="J10" s="134"/>
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" s="74" customFormat="1" ht="15">
-      <c r="A11" s="153"/>
-      <c r="B11" s="153"/>
-      <c r="C11" s="153"/>
-      <c r="D11" s="153"/>
-      <c r="E11" s="153"/>
-      <c r="F11" s="153"/>
-      <c r="G11" s="153"/>
-      <c r="H11" s="153"/>
-      <c r="I11" s="153"/>
-      <c r="J11" s="154"/>
+      <c r="A11" s="140"/>
+      <c r="B11" s="140"/>
+      <c r="C11" s="140"/>
+      <c r="D11" s="140"/>
+      <c r="E11" s="140"/>
+      <c r="F11" s="140"/>
+      <c r="G11" s="140"/>
+      <c r="H11" s="140"/>
+      <c r="I11" s="140"/>
+      <c r="J11" s="141"/>
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A12" s="138" t="s">
+      <c r="A12" s="129" t="s">
         <v>159</v>
       </c>
-      <c r="B12" s="139"/>
-      <c r="C12" s="139"/>
-      <c r="D12" s="139"/>
-      <c r="E12" s="139"/>
-      <c r="F12" s="139"/>
-      <c r="G12" s="139"/>
-      <c r="H12" s="139"/>
-      <c r="I12" s="139"/>
-      <c r="J12" s="146"/>
+      <c r="B12" s="130"/>
+      <c r="C12" s="130"/>
+      <c r="D12" s="130"/>
+      <c r="E12" s="130"/>
+      <c r="F12" s="130"/>
+      <c r="G12" s="130"/>
+      <c r="H12" s="130"/>
+      <c r="I12" s="130"/>
+      <c r="J12" s="131"/>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" ht="102.75" customHeight="1" outlineLevel="1">
       <c r="A13" s="78"/>
       <c r="B13" s="82"/>
       <c r="C13" s="77"/>
-      <c r="D13" s="119"/>
-      <c r="E13" s="120"/>
-      <c r="F13" s="120"/>
+      <c r="D13" s="147"/>
+      <c r="E13" s="148"/>
+      <c r="F13" s="148"/>
       <c r="G13" s="76"/>
       <c r="H13" s="90"/>
       <c r="I13" s="77"/>
@@ -4744,9 +4801,9 @@
       <c r="A14" s="78"/>
       <c r="B14" s="82"/>
       <c r="C14" s="77"/>
-      <c r="D14" s="119"/>
-      <c r="E14" s="120"/>
-      <c r="F14" s="120"/>
+      <c r="D14" s="147"/>
+      <c r="E14" s="148"/>
+      <c r="F14" s="148"/>
       <c r="G14" s="76"/>
       <c r="H14" s="90"/>
       <c r="I14" s="77"/>
@@ -4756,9 +4813,9 @@
       <c r="A15" s="78"/>
       <c r="B15" s="82"/>
       <c r="C15" s="77"/>
-      <c r="D15" s="119"/>
-      <c r="E15" s="120"/>
-      <c r="F15" s="120"/>
+      <c r="D15" s="147"/>
+      <c r="E15" s="148"/>
+      <c r="F15" s="148"/>
       <c r="G15" s="76"/>
       <c r="H15" s="90"/>
       <c r="I15" s="77"/>
@@ -4768,9 +4825,9 @@
       <c r="A16" s="78"/>
       <c r="B16" s="82"/>
       <c r="C16" s="77"/>
-      <c r="D16" s="119"/>
-      <c r="E16" s="120"/>
-      <c r="F16" s="120"/>
+      <c r="D16" s="147"/>
+      <c r="E16" s="148"/>
+      <c r="F16" s="148"/>
       <c r="G16" s="76"/>
       <c r="H16" s="90"/>
       <c r="I16" s="77"/>
@@ -4780,9 +4837,9 @@
       <c r="A17" s="78"/>
       <c r="B17" s="82"/>
       <c r="C17" s="77"/>
-      <c r="D17" s="119"/>
-      <c r="E17" s="120"/>
-      <c r="F17" s="120"/>
+      <c r="D17" s="147"/>
+      <c r="E17" s="148"/>
+      <c r="F17" s="148"/>
       <c r="G17" s="76"/>
       <c r="H17" s="90"/>
       <c r="I17" s="77"/>
@@ -4792,20 +4849,20 @@
       <c r="A18" s="78"/>
       <c r="B18" s="82"/>
       <c r="C18" s="77"/>
-      <c r="D18" s="119"/>
-      <c r="E18" s="120"/>
-      <c r="F18" s="120"/>
+      <c r="D18" s="147"/>
+      <c r="E18" s="148"/>
+      <c r="F18" s="148"/>
       <c r="G18" s="76"/>
       <c r="H18" s="90"/>
       <c r="I18" s="77"/>
       <c r="J18" s="75"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A19" s="138" t="s">
+      <c r="A19" s="129" t="s">
         <v>160</v>
       </c>
-      <c r="B19" s="139"/>
-      <c r="C19" s="139"/>
+      <c r="B19" s="130"/>
+      <c r="C19" s="130"/>
       <c r="D19" s="88"/>
       <c r="E19" s="88"/>
       <c r="F19" s="88"/>
@@ -4814,60 +4871,72 @@
       <c r="I19" s="88"/>
       <c r="J19" s="89"/>
     </row>
-    <row r="20" spans="1:10" s="4" customFormat="1" ht="90.75" customHeight="1" outlineLevel="1">
+    <row r="20" spans="1:10" s="4" customFormat="1" ht="79.5" customHeight="1" outlineLevel="1">
       <c r="A20" s="94" t="s">
         <v>0</v>
       </c>
       <c r="B20" s="86" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
       <c r="C20" s="87" t="s">
-        <v>163</v>
-      </c>
-      <c r="D20" s="129"/>
-      <c r="E20" s="130"/>
-      <c r="F20" s="130"/>
+        <v>181</v>
+      </c>
+      <c r="D20" s="157" t="s">
+        <v>180</v>
+      </c>
+      <c r="E20" s="158"/>
+      <c r="F20" s="158"/>
       <c r="G20" s="95"/>
       <c r="H20" s="96"/>
       <c r="I20" s="87"/>
       <c r="J20" s="97"/>
     </row>
-    <row r="21" spans="1:10" s="4" customFormat="1" ht="91.5" customHeight="1" outlineLevel="1">
+    <row r="21" spans="1:10" s="4" customFormat="1" ht="66.75" customHeight="1" outlineLevel="1">
       <c r="A21" s="94" t="s">
         <v>1</v>
       </c>
       <c r="B21" s="86" t="s">
-        <v>162</v>
+        <v>177</v>
       </c>
       <c r="C21" s="87" t="s">
-        <v>164</v>
-      </c>
-      <c r="D21" s="129"/>
-      <c r="E21" s="130"/>
-      <c r="F21" s="130"/>
+        <v>183</v>
+      </c>
+      <c r="D21" s="157" t="s">
+        <v>184</v>
+      </c>
+      <c r="E21" s="158"/>
+      <c r="F21" s="158"/>
       <c r="G21" s="95"/>
       <c r="H21" s="96"/>
       <c r="I21" s="87"/>
       <c r="J21" s="97"/>
     </row>
-    <row r="22" spans="1:10" s="4" customFormat="1" ht="68.25" customHeight="1" outlineLevel="1">
-      <c r="A22" s="94"/>
-      <c r="B22" s="86"/>
-      <c r="C22" s="87"/>
-      <c r="D22" s="129"/>
-      <c r="E22" s="130"/>
-      <c r="F22" s="130"/>
+    <row r="22" spans="1:10" s="4" customFormat="1" ht="79.5" customHeight="1" outlineLevel="1">
+      <c r="A22" s="94" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="86" t="s">
+        <v>185</v>
+      </c>
+      <c r="C22" s="87" t="s">
+        <v>181</v>
+      </c>
+      <c r="D22" s="157" t="s">
+        <v>186</v>
+      </c>
+      <c r="E22" s="158"/>
+      <c r="F22" s="158"/>
       <c r="G22" s="95"/>
       <c r="H22" s="96"/>
       <c r="I22" s="87"/>
       <c r="J22" s="97"/>
     </row>
     <row r="23" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A23" s="138" t="s">
-        <v>170</v>
-      </c>
-      <c r="B23" s="139"/>
-      <c r="C23" s="139"/>
+      <c r="A23" s="129" t="s">
+        <v>164</v>
+      </c>
+      <c r="B23" s="130"/>
+      <c r="C23" s="130"/>
       <c r="D23" s="88"/>
       <c r="E23" s="88"/>
       <c r="F23" s="88"/>
@@ -4881,14 +4950,14 @@
         <v>0</v>
       </c>
       <c r="B24" s="93" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C24" s="77" t="s">
-        <v>171</v>
-      </c>
-      <c r="D24" s="126"/>
-      <c r="E24" s="127"/>
-      <c r="F24" s="127"/>
+        <v>165</v>
+      </c>
+      <c r="D24" s="121"/>
+      <c r="E24" s="122"/>
+      <c r="F24" s="122"/>
       <c r="G24" s="76"/>
       <c r="H24" s="83"/>
       <c r="I24" s="77"/>
@@ -4899,14 +4968,14 @@
         <v>1</v>
       </c>
       <c r="B25" s="93" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C25" s="77" t="s">
-        <v>173</v>
-      </c>
-      <c r="D25" s="126"/>
-      <c r="E25" s="127"/>
-      <c r="F25" s="127"/>
+        <v>167</v>
+      </c>
+      <c r="D25" s="121"/>
+      <c r="E25" s="122"/>
+      <c r="F25" s="122"/>
       <c r="G25" s="76"/>
       <c r="H25" s="83"/>
       <c r="I25" s="77"/>
@@ -4917,14 +4986,14 @@
         <v>2</v>
       </c>
       <c r="B26" s="93" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C26" s="77" t="s">
-        <v>174</v>
-      </c>
-      <c r="D26" s="126"/>
-      <c r="E26" s="127"/>
-      <c r="F26" s="127"/>
+        <v>168</v>
+      </c>
+      <c r="D26" s="121"/>
+      <c r="E26" s="122"/>
+      <c r="F26" s="122"/>
       <c r="G26" s="76"/>
       <c r="H26" s="83"/>
       <c r="I26" s="77"/>
@@ -4935,23 +5004,23 @@
         <v>50</v>
       </c>
       <c r="B27" s="93" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="C27" s="77" t="s">
-        <v>178</v>
-      </c>
-      <c r="D27" s="126"/>
-      <c r="E27" s="127"/>
-      <c r="F27" s="127"/>
+        <v>172</v>
+      </c>
+      <c r="D27" s="121"/>
+      <c r="E27" s="122"/>
+      <c r="F27" s="122"/>
       <c r="G27" s="76"/>
       <c r="H27" s="83"/>
       <c r="I27" s="77"/>
       <c r="J27" s="75"/>
     </row>
     <row r="28" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A28" s="124"/>
-      <c r="B28" s="125"/>
-      <c r="C28" s="125"/>
+      <c r="A28" s="119"/>
+      <c r="B28" s="120"/>
+      <c r="C28" s="120"/>
       <c r="D28" s="98"/>
       <c r="E28" s="98"/>
       <c r="F28" s="98"/>
@@ -4964,9 +5033,9 @@
       <c r="A29" s="78"/>
       <c r="B29" s="93"/>
       <c r="C29" s="77"/>
-      <c r="D29" s="126"/>
-      <c r="E29" s="127"/>
-      <c r="F29" s="127"/>
+      <c r="D29" s="121"/>
+      <c r="E29" s="122"/>
+      <c r="F29" s="122"/>
       <c r="G29" s="76"/>
       <c r="H29" s="83"/>
       <c r="I29" s="77"/>
@@ -4976,9 +5045,9 @@
       <c r="A30" s="78"/>
       <c r="B30" s="93"/>
       <c r="C30" s="77"/>
-      <c r="D30" s="126"/>
-      <c r="E30" s="127"/>
-      <c r="F30" s="127"/>
+      <c r="D30" s="121"/>
+      <c r="E30" s="122"/>
+      <c r="F30" s="122"/>
       <c r="G30" s="76"/>
       <c r="H30" s="83"/>
       <c r="I30" s="77"/>
@@ -4988,9 +5057,9 @@
       <c r="A31" s="78"/>
       <c r="B31" s="93"/>
       <c r="C31" s="77"/>
-      <c r="D31" s="126"/>
-      <c r="E31" s="127"/>
-      <c r="F31" s="127"/>
+      <c r="D31" s="121"/>
+      <c r="E31" s="122"/>
+      <c r="F31" s="122"/>
       <c r="G31" s="76"/>
       <c r="H31" s="83"/>
       <c r="I31" s="77"/>
@@ -5000,9 +5069,9 @@
       <c r="A32" s="78"/>
       <c r="B32" s="93"/>
       <c r="C32" s="77"/>
-      <c r="D32" s="126"/>
-      <c r="E32" s="127"/>
-      <c r="F32" s="127"/>
+      <c r="D32" s="121"/>
+      <c r="E32" s="122"/>
+      <c r="F32" s="122"/>
       <c r="G32" s="76"/>
       <c r="H32" s="83"/>
       <c r="I32" s="77"/>
@@ -5012,9 +5081,9 @@
       <c r="A33" s="78"/>
       <c r="B33" s="93"/>
       <c r="C33" s="77"/>
-      <c r="D33" s="126"/>
-      <c r="E33" s="127"/>
-      <c r="F33" s="127"/>
+      <c r="D33" s="121"/>
+      <c r="E33" s="122"/>
+      <c r="F33" s="122"/>
       <c r="G33" s="76"/>
       <c r="H33" s="83"/>
       <c r="I33" s="77"/>
@@ -5024,18 +5093,18 @@
       <c r="A34" s="78"/>
       <c r="B34" s="93"/>
       <c r="C34" s="77"/>
-      <c r="D34" s="126"/>
-      <c r="E34" s="127"/>
-      <c r="F34" s="127"/>
+      <c r="D34" s="121"/>
+      <c r="E34" s="122"/>
+      <c r="F34" s="122"/>
       <c r="G34" s="76"/>
       <c r="H34" s="83"/>
       <c r="I34" s="77"/>
       <c r="J34" s="75"/>
     </row>
     <row r="35" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A35" s="124"/>
-      <c r="B35" s="125"/>
-      <c r="C35" s="125"/>
+      <c r="A35" s="119"/>
+      <c r="B35" s="120"/>
+      <c r="C35" s="120"/>
       <c r="D35" s="98"/>
       <c r="E35" s="98"/>
       <c r="F35" s="98"/>
@@ -5048,9 +5117,9 @@
       <c r="A36" s="78"/>
       <c r="B36" s="93"/>
       <c r="C36" s="77"/>
-      <c r="D36" s="126"/>
-      <c r="E36" s="127"/>
-      <c r="F36" s="127"/>
+      <c r="D36" s="121"/>
+      <c r="E36" s="122"/>
+      <c r="F36" s="122"/>
       <c r="G36" s="76"/>
       <c r="H36" s="83"/>
       <c r="I36" s="77"/>
@@ -5186,31 +5255,13 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="B1:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="H4:J4"/>
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="H6:J6"/>
     <mergeCell ref="H7:J7"/>
@@ -5222,13 +5273,31 @@
     <mergeCell ref="H9:H10"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="B1:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5380,7 +5449,7 @@
       </c>
       <c r="G9" s="67">
         <f>Samples2!D7</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.25">
@@ -5412,7 +5481,7 @@
       </c>
       <c r="G11" s="55">
         <f>SUM(G6:G10)</f>
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14.25">

</xml_diff>

<commit_message>
update xem ds user dk sk
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University_IT\Tam\KiemThuPhanMem\event-manager-javafx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB323376-314C-4F1F-92E8-44DD1A5317AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E517A05C-C2C9-424C-A1D9-C7C66F60CB4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9810" yWindow="465" windowWidth="10365" windowHeight="10155" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="197">
   <si>
     <t>TC1</t>
   </si>
@@ -680,58 +680,6 @@
     <t>Viết TC Kiểm tra khả năng hiển thị đầy đủ thông tin của một sự kiện</t>
   </si>
   <si>
-    <t>3. Xem danh sách người dùng</t>
-  </si>
-  <si>
-    <t>B1: Đăng nhập với tư cách là admin
-B2: Truy cập vào Trang Quản Trị
-B3: Chọn mục Quản lý người dùng
-B4: Hiển thị danh sách của người dùng</t>
-  </si>
-  <si>
-    <t>Kiểm tra chức năng hiển thị danh sách người dùng với tài khoản admin</t>
-  </si>
-  <si>
-    <t>B1: Đăng nhập với tư cách là user
-B2: Truy cập vào Trang Quản Trị, mục Quản lý người dùng thông qua đường dẫn URL
-B4: Hiển thị thông báo lỗi hoặc không tìm thấy trang chủ</t>
-  </si>
-  <si>
-    <t>B1: Đăng nhập với tư cách là admin
-B2: Truy cập vào Trang Quản Trị
-B3: Chọn mục Quản lý người dùng
-B4: Chọn một user bất kỳ và nhấn vào nút Chi tiết hoặc icon thông tin
-B5: Hiển thị thông tin chi tiết của user đã chọn</t>
-  </si>
-  <si>
-    <t>Kiểm tra chức năng hiển thị danh sách người dùng với tài khoản của</t>
-  </si>
-  <si>
-    <t>Kiểm tra chức năng hiển thị thông tin chi tiết của một người dùng</t>
-  </si>
-  <si>
-    <t>Kiểm tra chức năng tìm kiếm người dùng</t>
-  </si>
-  <si>
-    <t>B1: Đăng nhập với tư cách là admin
-B2: Truy cập vào Trang Quản Trị
-B3: Chọn mục Quản lý người dùng
-B4: Nhập từ khóa cần tìm vào ô tìm kiếm(tên đăng nhậo, email, tên)
-B5: Hiển thị các user phù hợp với kết quả tìm kiếm</t>
-  </si>
-  <si>
-    <t>Viết TC Kiểm tra chức năng hiển thị danh sách người dùng với tài khoản admin</t>
-  </si>
-  <si>
-    <t>Viết TC Kiểm tra chức năng hiển thị danh sách người dùng với tài khoản của</t>
-  </si>
-  <si>
-    <t>Viết TC Kiểm tra chức năng hiển thị thông tin chi tiết của một người dùng</t>
-  </si>
-  <si>
-    <t>Viết TC Kiểm tra chức năng tìm kiếm người dùng</t>
-  </si>
-  <si>
     <t>Kiểm tra chức năng hủy đăng ký trong thời gian không cho phép</t>
   </si>
   <si>
@@ -782,6 +730,80 @@
   </si>
   <si>
     <t>Viết TC Kiểm tra chức năng hủy đăng ký với sự kiện miễn phí</t>
+  </si>
+  <si>
+    <t>3. Xem danh sách user tham gia sự kiện</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng hiển thị danh sách user tham gia sự kiện với tài khoản admin</t>
+  </si>
+  <si>
+    <t>Hiển thị danh sách user đăng ký tham gia sự kiện</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kiểm tra chức năng hiển thị danh sách user tham gia sự kiện với tài khoản user </t>
+  </si>
+  <si>
+    <t>B1: Đăng nhập với tư cách là admin
+B2: Truy cập vào trang Quản lý sự kiện
+B3: Chọn một sự kiện đã có user đăng ký
+B4: Nhấn Xem danh sách người tham gia sự kiện</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B1: Đăng nhập với tư cách là user
+B2: Truy cập URL trực tiếp đến trang xem danh sách người tham gia sự kiện
+</t>
+  </si>
+  <si>
+    <t>Hiển thị thông báo lỗi không thể truy cập chức năng này</t>
+  </si>
+  <si>
+    <t>Kiểm tra giao diện hiển thị khi sự kiện chưa có người đăng ký tham gia</t>
+  </si>
+  <si>
+    <t>B1: Đăng nhập với tư cách là admin
+B2: Truy cập vào trang Quản lý sự kiện
+B3: Chọn một sự kiện chưa có người đăng ký tham gia
+B4: Nhấn Xem danh sách người tham gia sự kiện</t>
+  </si>
+  <si>
+    <t>Hiển thị thông báo chưa có người tham gia sự kiện</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng tìm kiếm user đăng ký tham gia sự kiện</t>
+  </si>
+  <si>
+    <t>B1: Đăng nhập với tư cách là admin
+B2: Truy cập vào trang Quản lý sự kiện
+B3: Chọn sự kiện cần xem danh sách người tham gia
+B4: Nhấn Xem danh sách người tham gia sự kiện
+B5: Nhấn chọn thanh tìm kiếm
+B6: Nhập tên hoặc email của người tham gia vào thanh tìm kiếm
+B7: Nhấn Tìm</t>
+  </si>
+  <si>
+    <t>Hiển thị danh sách user phù hợp với từ khóa đã nhập</t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra chức năng hiển thị danh sách user tham gia sự kiện với tài khoản admin</t>
+  </si>
+  <si>
+    <t>Cập nhật TC Kiểm tra chức năng hiển thị danh sách user tham gia sự kiện với tài khoản admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viết TC Kiểm tra chức năng hiển thị danh sách user tham gia sự kiện với tài khoản user </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cập nhật TC Kiểm tra chức năng hiển thị danh sách user tham gia sự kiện với tài khoản user </t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra giao diện hiển thị khi sự kiện chưa có người đăng ký tham gia</t>
+  </si>
+  <si>
+    <t>Cập nhật TC Kiểm tra chức năng tìm kiếm user đăng ký tham gia sự kiện</t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra chức năng tìm kiếm user đăng ký tham gia sự kiện</t>
   </si>
 </sst>
 </file>
@@ -1799,6 +1821,21 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1811,6 +1848,42 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1829,12 +1902,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1844,9 +1911,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1859,9 +1923,6 @@
     <xf numFmtId="0" fontId="15" fillId="5" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1869,49 +1930,10 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2251,10 +2273,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H72"/>
+  <dimension ref="A2:H71"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B44" zoomScale="85" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView showGridLines="0" topLeftCell="D50" zoomScale="85" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -2992,7 +3014,7 @@
       </c>
       <c r="D47" s="101"/>
       <c r="E47" s="106" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="F47" s="112" t="s">
         <v>44</v>
@@ -3009,7 +3031,7 @@
       </c>
       <c r="D48" s="101"/>
       <c r="E48" s="106" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="F48" s="112" t="s">
         <v>44</v>
@@ -3017,7 +3039,7 @@
       <c r="G48" s="101"/>
       <c r="H48" s="107"/>
     </row>
-    <row r="49" spans="2:8" s="34" customFormat="1" ht="25.5">
+    <row r="49" spans="2:8" s="34" customFormat="1" ht="38.25">
       <c r="B49" s="36">
         <v>45749</v>
       </c>
@@ -3026,7 +3048,7 @@
       </c>
       <c r="D49" s="101"/>
       <c r="E49" s="106" t="s">
-        <v>173</v>
+        <v>190</v>
       </c>
       <c r="F49" s="112" t="s">
         <v>44</v>
@@ -3034,7 +3056,7 @@
       <c r="G49" s="101"/>
       <c r="H49" s="107"/>
     </row>
-    <row r="50" spans="2:8" s="34" customFormat="1" ht="25.5">
+    <row r="50" spans="2:8" s="34" customFormat="1" ht="38.25">
       <c r="B50" s="36">
         <v>45749</v>
       </c>
@@ -3043,7 +3065,7 @@
       </c>
       <c r="D50" s="101"/>
       <c r="E50" s="106" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="F50" s="112" t="s">
         <v>44</v>
@@ -3060,7 +3082,7 @@
       </c>
       <c r="D51" s="101"/>
       <c r="E51" s="106" t="s">
-        <v>175</v>
+        <v>196</v>
       </c>
       <c r="F51" s="112" t="s">
         <v>44</v>
@@ -3070,14 +3092,14 @@
     </row>
     <row r="52" spans="2:8" s="34" customFormat="1" ht="25.5">
       <c r="B52" s="36">
-        <v>45749</v>
+        <v>45750</v>
       </c>
       <c r="C52" s="37" t="s">
-        <v>40</v>
+        <v>161</v>
       </c>
       <c r="D52" s="101"/>
       <c r="E52" s="106" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F52" s="112" t="s">
         <v>44</v>
@@ -3094,7 +3116,7 @@
       </c>
       <c r="D53" s="101"/>
       <c r="E53" s="106" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="F53" s="112" t="s">
         <v>44</v>
@@ -3107,11 +3129,11 @@
         <v>45750</v>
       </c>
       <c r="C54" s="37" t="s">
-        <v>161</v>
+        <v>40</v>
       </c>
       <c r="D54" s="101"/>
       <c r="E54" s="106" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="F54" s="112" t="s">
         <v>44</v>
@@ -3119,16 +3141,16 @@
       <c r="G54" s="101"/>
       <c r="H54" s="107"/>
     </row>
-    <row r="55" spans="2:8" s="34" customFormat="1" ht="25.5">
+    <row r="55" spans="2:8" s="34" customFormat="1" ht="38.25">
       <c r="B55" s="36">
         <v>45750</v>
       </c>
       <c r="C55" s="37" t="s">
-        <v>40</v>
+        <v>161</v>
       </c>
       <c r="D55" s="101"/>
       <c r="E55" s="106" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F55" s="112" t="s">
         <v>44</v>
@@ -3136,30 +3158,54 @@
       <c r="G55" s="101"/>
       <c r="H55" s="107"/>
     </row>
-    <row r="56" spans="2:8" s="34" customFormat="1">
-      <c r="B56" s="36"/>
-      <c r="C56" s="37"/>
+    <row r="56" spans="2:8" s="34" customFormat="1" ht="38.25">
+      <c r="B56" s="36">
+        <v>45750</v>
+      </c>
+      <c r="C56" s="37" t="s">
+        <v>161</v>
+      </c>
       <c r="D56" s="101"/>
-      <c r="E56" s="106"/>
-      <c r="F56" s="112"/>
+      <c r="E56" s="106" t="s">
+        <v>193</v>
+      </c>
+      <c r="F56" s="112" t="s">
+        <v>44</v>
+      </c>
       <c r="G56" s="101"/>
       <c r="H56" s="107"/>
     </row>
-    <row r="57" spans="2:8" s="34" customFormat="1">
-      <c r="B57" s="36"/>
-      <c r="C57" s="37"/>
+    <row r="57" spans="2:8" s="34" customFormat="1" ht="25.5">
+      <c r="B57" s="36">
+        <v>45750</v>
+      </c>
+      <c r="C57" s="37" t="s">
+        <v>40</v>
+      </c>
       <c r="D57" s="101"/>
-      <c r="E57" s="106"/>
-      <c r="F57" s="112"/>
+      <c r="E57" s="106" t="s">
+        <v>194</v>
+      </c>
+      <c r="F57" s="112" t="s">
+        <v>44</v>
+      </c>
       <c r="G57" s="101"/>
       <c r="H57" s="107"/>
     </row>
-    <row r="58" spans="2:8" s="34" customFormat="1">
-      <c r="B58" s="36"/>
-      <c r="C58" s="37"/>
+    <row r="58" spans="2:8" s="34" customFormat="1" ht="25.5">
+      <c r="B58" s="36">
+        <v>45750</v>
+      </c>
+      <c r="C58" s="37" t="s">
+        <v>161</v>
+      </c>
       <c r="D58" s="101"/>
-      <c r="E58" s="106"/>
-      <c r="F58" s="112"/>
+      <c r="E58" s="106" t="s">
+        <v>195</v>
+      </c>
+      <c r="F58" s="112" t="s">
+        <v>44</v>
+      </c>
       <c r="G58" s="101"/>
       <c r="H58" s="107"/>
     </row>
@@ -3272,22 +3318,13 @@
       <c r="H70" s="107"/>
     </row>
     <row r="71" spans="2:8" s="34" customFormat="1">
-      <c r="B71" s="36"/>
-      <c r="C71" s="37"/>
-      <c r="D71" s="101"/>
-      <c r="E71" s="106"/>
-      <c r="F71" s="112"/>
-      <c r="G71" s="101"/>
-      <c r="H71" s="107"/>
-    </row>
-    <row r="72" spans="2:8" s="34" customFormat="1">
-      <c r="B72" s="109"/>
-      <c r="C72" s="108"/>
-      <c r="D72" s="43"/>
-      <c r="E72" s="105"/>
-      <c r="F72" s="113"/>
-      <c r="G72" s="43"/>
-      <c r="H72" s="44"/>
+      <c r="B71" s="109"/>
+      <c r="C71" s="108"/>
+      <c r="D71" s="43"/>
+      <c r="E71" s="105"/>
+      <c r="F71" s="113"/>
+      <c r="G71" s="43"/>
+      <c r="H71" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3295,8 +3332,8 @@
     <mergeCell ref="C7:E7"/>
   </mergeCells>
   <phoneticPr fontId="0"/>
-  <conditionalFormatting sqref="C43:C52">
-    <cfRule type="uniqueValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="C43:C51">
+    <cfRule type="uniqueValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.37" right="0.47" top="0.5" bottom="0.38" header="0.5" footer="0.17"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="96" verticalDpi="96" r:id="rId1"/>
@@ -3304,7 +3341,7 @@
     <oddFooter>&amp;L&amp;"Tahoma,Regular"&amp;8 02ae-BM/PM/HDCV/FSOFT v1/0&amp;R&amp;"Tahoma,Regular"&amp;10&amp;P/&amp;N</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="C12:C34 C42 C35:C41 C43:C48 C49:C52 C53:C55" numberStoredAsText="1"/>
+    <ignoredError sqref="C12:C34 C42 C35:C41 C43:C48 C49:C50 C52:C54 C51 C55:C58" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -3316,7 +3353,7 @@
   </sheetPr>
   <dimension ref="A1:K95"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="85" workbookViewId="0">
+    <sheetView topLeftCell="A39" zoomScale="85" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -3336,9 +3373,9 @@
       <c r="A1" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
+      <c r="B1" s="140"/>
+      <c r="C1" s="140"/>
+      <c r="D1" s="140"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -3349,9 +3386,9 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="124"/>
-      <c r="C2" s="124"/>
-      <c r="D2" s="124"/>
+      <c r="B2" s="141"/>
+      <c r="C2" s="141"/>
+      <c r="D2" s="141"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -3372,43 +3409,43 @@
       <c r="E3" s="61"/>
       <c r="F3" s="61"/>
       <c r="G3" s="61"/>
-      <c r="H3" s="133"/>
-      <c r="I3" s="133"/>
-      <c r="J3" s="133"/>
+      <c r="H3" s="148"/>
+      <c r="I3" s="148"/>
+      <c r="J3" s="148"/>
       <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="12.75">
       <c r="A4" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="135" t="s">
+      <c r="B4" s="149" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="136"/>
-      <c r="D4" s="137"/>
+      <c r="C4" s="150"/>
+      <c r="D4" s="151"/>
       <c r="E4" s="61"/>
       <c r="F4" s="61"/>
       <c r="G4" s="61"/>
-      <c r="H4" s="133"/>
-      <c r="I4" s="133"/>
-      <c r="J4" s="133"/>
+      <c r="H4" s="148"/>
+      <c r="I4" s="148"/>
+      <c r="J4" s="148"/>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" s="71" customFormat="1" ht="25.5">
       <c r="A5" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="126" t="s">
+      <c r="B5" s="143" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="127"/>
-      <c r="D5" s="128"/>
+      <c r="C5" s="144"/>
+      <c r="D5" s="145"/>
       <c r="E5" s="69"/>
       <c r="F5" s="69"/>
       <c r="G5" s="69"/>
-      <c r="H5" s="132"/>
-      <c r="I5" s="132"/>
-      <c r="J5" s="132"/>
+      <c r="H5" s="147"/>
+      <c r="I5" s="147"/>
+      <c r="J5" s="147"/>
       <c r="K5" s="70"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
@@ -3429,9 +3466,9 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="133"/>
-      <c r="I6" s="133"/>
-      <c r="J6" s="133"/>
+      <c r="H6" s="148"/>
+      <c r="I6" s="148"/>
+      <c r="J6" s="148"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -3452,16 +3489,16 @@
       <c r="E7" s="62"/>
       <c r="F7" s="62"/>
       <c r="G7" s="62"/>
-      <c r="H7" s="133"/>
-      <c r="I7" s="133"/>
-      <c r="J7" s="133"/>
+      <c r="H7" s="148"/>
+      <c r="I7" s="148"/>
+      <c r="J7" s="148"/>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="125"/>
-      <c r="B8" s="125"/>
-      <c r="C8" s="125"/>
-      <c r="D8" s="125"/>
+      <c r="A8" s="142"/>
+      <c r="B8" s="142"/>
+      <c r="C8" s="142"/>
+      <c r="D8" s="142"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -3471,70 +3508,70 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" s="73" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="142" t="s">
+      <c r="A9" s="131" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="143" t="s">
+      <c r="B9" s="155" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="142" t="s">
+      <c r="C9" s="131" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="149" t="s">
+      <c r="D9" s="132" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="150"/>
-      <c r="F9" s="150"/>
-      <c r="G9" s="151"/>
-      <c r="H9" s="138" t="s">
+      <c r="E9" s="133"/>
+      <c r="F9" s="133"/>
+      <c r="G9" s="134"/>
+      <c r="H9" s="152" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="134" t="s">
+      <c r="I9" s="128" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="134" t="s">
+      <c r="J9" s="128" t="s">
         <v>32</v>
       </c>
       <c r="K9" s="72"/>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="134"/>
-      <c r="B10" s="144"/>
-      <c r="C10" s="134"/>
-      <c r="D10" s="139"/>
-      <c r="E10" s="152"/>
-      <c r="F10" s="152"/>
-      <c r="G10" s="153"/>
-      <c r="H10" s="139"/>
-      <c r="I10" s="134"/>
-      <c r="J10" s="134"/>
+      <c r="A10" s="128"/>
+      <c r="B10" s="156"/>
+      <c r="C10" s="128"/>
+      <c r="D10" s="135"/>
+      <c r="E10" s="136"/>
+      <c r="F10" s="136"/>
+      <c r="G10" s="137"/>
+      <c r="H10" s="135"/>
+      <c r="I10" s="128"/>
+      <c r="J10" s="128"/>
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" s="74" customFormat="1" ht="15">
-      <c r="A11" s="140"/>
-      <c r="B11" s="140"/>
-      <c r="C11" s="140"/>
-      <c r="D11" s="140"/>
-      <c r="E11" s="140"/>
-      <c r="F11" s="140"/>
-      <c r="G11" s="140"/>
-      <c r="H11" s="140"/>
-      <c r="I11" s="140"/>
-      <c r="J11" s="141"/>
+      <c r="A11" s="153"/>
+      <c r="B11" s="153"/>
+      <c r="C11" s="153"/>
+      <c r="D11" s="153"/>
+      <c r="E11" s="153"/>
+      <c r="F11" s="153"/>
+      <c r="G11" s="153"/>
+      <c r="H11" s="153"/>
+      <c r="I11" s="153"/>
+      <c r="J11" s="154"/>
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A12" s="129" t="s">
+      <c r="A12" s="138" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="130"/>
-      <c r="C12" s="130"/>
-      <c r="D12" s="130"/>
-      <c r="E12" s="130"/>
-      <c r="F12" s="130"/>
-      <c r="G12" s="130"/>
-      <c r="H12" s="130"/>
-      <c r="I12" s="130"/>
-      <c r="J12" s="131"/>
+      <c r="B12" s="139"/>
+      <c r="C12" s="139"/>
+      <c r="D12" s="139"/>
+      <c r="E12" s="139"/>
+      <c r="F12" s="139"/>
+      <c r="G12" s="139"/>
+      <c r="H12" s="139"/>
+      <c r="I12" s="139"/>
+      <c r="J12" s="146"/>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" ht="66.75" customHeight="1" outlineLevel="1">
       <c r="A13" s="78" t="s">
@@ -3546,9 +3583,9 @@
       <c r="C13" s="77" t="s">
         <v>85</v>
       </c>
-      <c r="D13" s="147"/>
-      <c r="E13" s="148"/>
-      <c r="F13" s="148"/>
+      <c r="D13" s="119"/>
+      <c r="E13" s="120"/>
+      <c r="F13" s="120"/>
       <c r="G13" s="76"/>
       <c r="H13" s="90"/>
       <c r="I13" s="77"/>
@@ -3564,9 +3601,9 @@
       <c r="C14" s="77" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="147"/>
-      <c r="E14" s="148"/>
-      <c r="F14" s="148"/>
+      <c r="D14" s="119"/>
+      <c r="E14" s="120"/>
+      <c r="F14" s="120"/>
       <c r="G14" s="76"/>
       <c r="H14" s="90"/>
       <c r="I14" s="77"/>
@@ -3582,9 +3619,9 @@
       <c r="C15" s="77" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="147"/>
-      <c r="E15" s="148"/>
-      <c r="F15" s="148"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="120"/>
+      <c r="F15" s="120"/>
       <c r="G15" s="76"/>
       <c r="H15" s="90"/>
       <c r="I15" s="77"/>
@@ -3600,9 +3637,9 @@
       <c r="C16" s="77" t="s">
         <v>95</v>
       </c>
-      <c r="D16" s="147"/>
-      <c r="E16" s="148"/>
-      <c r="F16" s="148"/>
+      <c r="D16" s="119"/>
+      <c r="E16" s="120"/>
+      <c r="F16" s="120"/>
       <c r="G16" s="76"/>
       <c r="H16" s="90"/>
       <c r="I16" s="77"/>
@@ -3618,9 +3655,9 @@
       <c r="C17" s="77" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="147"/>
-      <c r="E17" s="148"/>
-      <c r="F17" s="148"/>
+      <c r="D17" s="119"/>
+      <c r="E17" s="120"/>
+      <c r="F17" s="120"/>
       <c r="G17" s="76"/>
       <c r="H17" s="90"/>
       <c r="I17" s="77"/>
@@ -3636,9 +3673,9 @@
       <c r="C18" s="77" t="s">
         <v>93</v>
       </c>
-      <c r="D18" s="147"/>
-      <c r="E18" s="148"/>
-      <c r="F18" s="148"/>
+      <c r="D18" s="119"/>
+      <c r="E18" s="120"/>
+      <c r="F18" s="120"/>
       <c r="G18" s="76"/>
       <c r="H18" s="90"/>
       <c r="I18" s="77"/>
@@ -3654,9 +3691,9 @@
       <c r="C19" s="87" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="154"/>
-      <c r="E19" s="155"/>
-      <c r="F19" s="156"/>
+      <c r="D19" s="121"/>
+      <c r="E19" s="122"/>
+      <c r="F19" s="123"/>
       <c r="G19" s="77"/>
       <c r="H19" s="77"/>
       <c r="I19" s="77"/>
@@ -3672,20 +3709,20 @@
       <c r="C20" s="77" t="s">
         <v>102</v>
       </c>
-      <c r="D20" s="154"/>
-      <c r="E20" s="155"/>
-      <c r="F20" s="156"/>
+      <c r="D20" s="121"/>
+      <c r="E20" s="122"/>
+      <c r="F20" s="123"/>
       <c r="G20" s="77"/>
       <c r="H20" s="77"/>
       <c r="I20" s="77"/>
       <c r="J20" s="75"/>
     </row>
     <row r="21" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A21" s="129" t="s">
+      <c r="A21" s="138" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="130"/>
-      <c r="C21" s="130"/>
+      <c r="B21" s="139"/>
+      <c r="C21" s="139"/>
       <c r="D21" s="88"/>
       <c r="E21" s="88"/>
       <c r="F21" s="88"/>
@@ -3704,9 +3741,9 @@
       <c r="C22" s="87" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="145"/>
-      <c r="E22" s="146"/>
-      <c r="F22" s="146"/>
+      <c r="D22" s="129"/>
+      <c r="E22" s="130"/>
+      <c r="F22" s="130"/>
       <c r="G22" s="95"/>
       <c r="H22" s="96"/>
       <c r="I22" s="87"/>
@@ -3722,9 +3759,9 @@
       <c r="C23" s="87" t="s">
         <v>72</v>
       </c>
-      <c r="D23" s="145"/>
-      <c r="E23" s="146"/>
-      <c r="F23" s="146"/>
+      <c r="D23" s="129"/>
+      <c r="E23" s="130"/>
+      <c r="F23" s="130"/>
       <c r="G23" s="95"/>
       <c r="H23" s="96"/>
       <c r="I23" s="87"/>
@@ -3740,9 +3777,9 @@
       <c r="C24" s="87" t="s">
         <v>75</v>
       </c>
-      <c r="D24" s="145"/>
-      <c r="E24" s="146"/>
-      <c r="F24" s="146"/>
+      <c r="D24" s="129"/>
+      <c r="E24" s="130"/>
+      <c r="F24" s="130"/>
       <c r="G24" s="95"/>
       <c r="H24" s="96"/>
       <c r="I24" s="87"/>
@@ -3758,9 +3795,9 @@
       <c r="C25" s="87" t="s">
         <v>77</v>
       </c>
-      <c r="D25" s="154"/>
-      <c r="E25" s="155"/>
-      <c r="F25" s="156"/>
+      <c r="D25" s="121"/>
+      <c r="E25" s="122"/>
+      <c r="F25" s="123"/>
       <c r="G25" s="77"/>
       <c r="H25" s="77"/>
       <c r="I25" s="77"/>
@@ -3776,9 +3813,9 @@
       <c r="C26" s="87" t="s">
         <v>99</v>
       </c>
-      <c r="D26" s="154"/>
-      <c r="E26" s="155"/>
-      <c r="F26" s="156"/>
+      <c r="D26" s="121"/>
+      <c r="E26" s="122"/>
+      <c r="F26" s="123"/>
       <c r="G26" s="77"/>
       <c r="H26" s="77"/>
       <c r="I26" s="77"/>
@@ -3794,9 +3831,9 @@
       <c r="C27" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="154"/>
-      <c r="E27" s="155"/>
-      <c r="F27" s="156"/>
+      <c r="D27" s="121"/>
+      <c r="E27" s="122"/>
+      <c r="F27" s="123"/>
       <c r="G27" s="77"/>
       <c r="H27" s="77"/>
       <c r="I27" s="77"/>
@@ -3812,9 +3849,9 @@
       <c r="C28" s="77" t="s">
         <v>79</v>
       </c>
-      <c r="D28" s="154"/>
-      <c r="E28" s="155"/>
-      <c r="F28" s="156"/>
+      <c r="D28" s="121"/>
+      <c r="E28" s="122"/>
+      <c r="F28" s="123"/>
       <c r="G28" s="77"/>
       <c r="H28" s="77"/>
       <c r="I28" s="77"/>
@@ -3830,9 +3867,9 @@
       <c r="C29" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="154"/>
-      <c r="E29" s="155"/>
-      <c r="F29" s="156"/>
+      <c r="D29" s="121"/>
+      <c r="E29" s="122"/>
+      <c r="F29" s="123"/>
       <c r="G29" s="77"/>
       <c r="H29" s="77"/>
       <c r="I29" s="77"/>
@@ -3848,9 +3885,9 @@
       <c r="C30" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="D30" s="154"/>
-      <c r="E30" s="155"/>
-      <c r="F30" s="156"/>
+      <c r="D30" s="121"/>
+      <c r="E30" s="122"/>
+      <c r="F30" s="123"/>
       <c r="G30" s="77"/>
       <c r="H30" s="77"/>
       <c r="I30" s="77"/>
@@ -3866,9 +3903,9 @@
       <c r="C31" s="77" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="154"/>
-      <c r="E31" s="155"/>
-      <c r="F31" s="156"/>
+      <c r="D31" s="121"/>
+      <c r="E31" s="122"/>
+      <c r="F31" s="123"/>
       <c r="G31" s="77"/>
       <c r="H31" s="77"/>
       <c r="I31" s="77"/>
@@ -3884,20 +3921,20 @@
       <c r="C32" s="77" t="s">
         <v>101</v>
       </c>
-      <c r="D32" s="154"/>
-      <c r="E32" s="155"/>
-      <c r="F32" s="156"/>
+      <c r="D32" s="121"/>
+      <c r="E32" s="122"/>
+      <c r="F32" s="123"/>
       <c r="G32" s="77"/>
       <c r="H32" s="77"/>
       <c r="I32" s="77"/>
       <c r="J32" s="75"/>
     </row>
     <row r="33" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A33" s="119" t="s">
+      <c r="A33" s="124" t="s">
         <v>81</v>
       </c>
-      <c r="B33" s="120"/>
-      <c r="C33" s="120"/>
+      <c r="B33" s="125"/>
+      <c r="C33" s="125"/>
       <c r="D33" s="98"/>
       <c r="E33" s="98"/>
       <c r="F33" s="98"/>
@@ -3916,20 +3953,20 @@
       <c r="C34" s="77" t="s">
         <v>84</v>
       </c>
-      <c r="D34" s="121"/>
-      <c r="E34" s="122"/>
-      <c r="F34" s="122"/>
+      <c r="D34" s="126"/>
+      <c r="E34" s="127"/>
+      <c r="F34" s="127"/>
       <c r="G34" s="76"/>
       <c r="H34" s="83"/>
       <c r="I34" s="77"/>
       <c r="J34" s="75"/>
     </row>
     <row r="35" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A35" s="119" t="s">
+      <c r="A35" s="124" t="s">
         <v>82</v>
       </c>
-      <c r="B35" s="120"/>
-      <c r="C35" s="120"/>
+      <c r="B35" s="125"/>
+      <c r="C35" s="125"/>
       <c r="D35" s="98"/>
       <c r="E35" s="98"/>
       <c r="F35" s="98"/>
@@ -3948,9 +3985,9 @@
       <c r="C36" s="77" t="s">
         <v>145</v>
       </c>
-      <c r="D36" s="121"/>
-      <c r="E36" s="122"/>
-      <c r="F36" s="122"/>
+      <c r="D36" s="126"/>
+      <c r="E36" s="127"/>
+      <c r="F36" s="127"/>
       <c r="G36" s="76"/>
       <c r="H36" s="83"/>
       <c r="I36" s="77"/>
@@ -3966,9 +4003,9 @@
       <c r="C37" s="77" t="s">
         <v>147</v>
       </c>
-      <c r="D37" s="121"/>
-      <c r="E37" s="122"/>
-      <c r="F37" s="122"/>
+      <c r="D37" s="126"/>
+      <c r="E37" s="127"/>
+      <c r="F37" s="127"/>
       <c r="G37" s="76"/>
       <c r="H37" s="83"/>
       <c r="I37" s="77"/>
@@ -3984,9 +4021,9 @@
       <c r="C38" s="77" t="s">
         <v>146</v>
       </c>
-      <c r="D38" s="121"/>
-      <c r="E38" s="122"/>
-      <c r="F38" s="122"/>
+      <c r="D38" s="126"/>
+      <c r="E38" s="127"/>
+      <c r="F38" s="127"/>
       <c r="G38" s="76"/>
       <c r="H38" s="83"/>
       <c r="I38" s="77"/>
@@ -4002,9 +4039,9 @@
       <c r="C39" s="77" t="s">
         <v>149</v>
       </c>
-      <c r="D39" s="121"/>
-      <c r="E39" s="122"/>
-      <c r="F39" s="122"/>
+      <c r="D39" s="126"/>
+      <c r="E39" s="127"/>
+      <c r="F39" s="127"/>
       <c r="G39" s="76"/>
       <c r="H39" s="83"/>
       <c r="I39" s="77"/>
@@ -4020,20 +4057,20 @@
       <c r="C40" s="77" t="s">
         <v>151</v>
       </c>
-      <c r="D40" s="121"/>
-      <c r="E40" s="122"/>
-      <c r="F40" s="122"/>
+      <c r="D40" s="126"/>
+      <c r="E40" s="127"/>
+      <c r="F40" s="127"/>
       <c r="G40" s="76"/>
       <c r="H40" s="83"/>
       <c r="I40" s="77"/>
       <c r="J40" s="75"/>
     </row>
     <row r="41" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A41" s="119" t="s">
+      <c r="A41" s="124" t="s">
         <v>120</v>
       </c>
-      <c r="B41" s="120"/>
-      <c r="C41" s="120"/>
+      <c r="B41" s="125"/>
+      <c r="C41" s="125"/>
       <c r="D41" s="98"/>
       <c r="E41" s="98"/>
       <c r="F41" s="98"/>
@@ -4052,9 +4089,9 @@
       <c r="C42" s="77" t="s">
         <v>127</v>
       </c>
-      <c r="D42" s="121"/>
-      <c r="E42" s="122"/>
-      <c r="F42" s="122"/>
+      <c r="D42" s="126"/>
+      <c r="E42" s="127"/>
+      <c r="F42" s="127"/>
       <c r="G42" s="76"/>
       <c r="H42" s="83"/>
       <c r="I42" s="77"/>
@@ -4070,9 +4107,9 @@
       <c r="C43" s="77" t="s">
         <v>128</v>
       </c>
-      <c r="D43" s="121"/>
-      <c r="E43" s="122"/>
-      <c r="F43" s="122"/>
+      <c r="D43" s="126"/>
+      <c r="E43" s="127"/>
+      <c r="F43" s="127"/>
       <c r="G43" s="76"/>
       <c r="H43" s="83"/>
       <c r="I43" s="77"/>
@@ -4088,9 +4125,9 @@
       <c r="C44" s="77" t="s">
         <v>129</v>
       </c>
-      <c r="D44" s="121"/>
-      <c r="E44" s="122"/>
-      <c r="F44" s="122"/>
+      <c r="D44" s="126"/>
+      <c r="E44" s="127"/>
+      <c r="F44" s="127"/>
       <c r="G44" s="76"/>
       <c r="H44" s="83"/>
       <c r="I44" s="77"/>
@@ -4106,9 +4143,9 @@
       <c r="C45" s="77" t="s">
         <v>130</v>
       </c>
-      <c r="D45" s="121"/>
-      <c r="E45" s="122"/>
-      <c r="F45" s="122"/>
+      <c r="D45" s="126"/>
+      <c r="E45" s="127"/>
+      <c r="F45" s="127"/>
       <c r="G45" s="76"/>
       <c r="H45" s="83"/>
       <c r="I45" s="77"/>
@@ -4124,9 +4161,9 @@
       <c r="C46" s="77" t="s">
         <v>132</v>
       </c>
-      <c r="D46" s="121"/>
-      <c r="E46" s="122"/>
-      <c r="F46" s="122"/>
+      <c r="D46" s="126"/>
+      <c r="E46" s="127"/>
+      <c r="F46" s="127"/>
       <c r="G46" s="76"/>
       <c r="H46" s="83"/>
       <c r="I46" s="77"/>
@@ -4142,20 +4179,20 @@
       <c r="C47" s="77" t="s">
         <v>124</v>
       </c>
-      <c r="D47" s="121"/>
-      <c r="E47" s="122"/>
-      <c r="F47" s="122"/>
+      <c r="D47" s="126"/>
+      <c r="E47" s="127"/>
+      <c r="F47" s="127"/>
       <c r="G47" s="76"/>
       <c r="H47" s="83"/>
       <c r="I47" s="77"/>
       <c r="J47" s="75"/>
     </row>
     <row r="48" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A48" s="119" t="s">
+      <c r="A48" s="124" t="s">
         <v>133</v>
       </c>
-      <c r="B48" s="120"/>
-      <c r="C48" s="120"/>
+      <c r="B48" s="125"/>
+      <c r="C48" s="125"/>
       <c r="D48" s="98"/>
       <c r="E48" s="98"/>
       <c r="F48" s="98"/>
@@ -4174,18 +4211,18 @@
       <c r="C49" s="77" t="s">
         <v>134</v>
       </c>
-      <c r="D49" s="121"/>
-      <c r="E49" s="122"/>
-      <c r="F49" s="122"/>
+      <c r="D49" s="126"/>
+      <c r="E49" s="127"/>
+      <c r="F49" s="127"/>
       <c r="G49" s="76"/>
       <c r="H49" s="83"/>
       <c r="I49" s="77"/>
       <c r="J49" s="75"/>
     </row>
     <row r="50" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A50" s="119"/>
-      <c r="B50" s="120"/>
-      <c r="C50" s="120"/>
+      <c r="A50" s="124"/>
+      <c r="B50" s="125"/>
+      <c r="C50" s="125"/>
       <c r="D50" s="98"/>
       <c r="E50" s="98"/>
       <c r="F50" s="98"/>
@@ -4198,18 +4235,18 @@
       <c r="A51" s="78"/>
       <c r="B51" s="93"/>
       <c r="C51" s="77"/>
-      <c r="D51" s="121"/>
-      <c r="E51" s="122"/>
-      <c r="F51" s="122"/>
+      <c r="D51" s="126"/>
+      <c r="E51" s="127"/>
+      <c r="F51" s="127"/>
       <c r="G51" s="76"/>
       <c r="H51" s="83"/>
       <c r="I51" s="77"/>
       <c r="J51" s="75"/>
     </row>
     <row r="52" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A52" s="119"/>
-      <c r="B52" s="120"/>
-      <c r="C52" s="120"/>
+      <c r="A52" s="124"/>
+      <c r="B52" s="125"/>
+      <c r="C52" s="125"/>
       <c r="D52" s="98"/>
       <c r="E52" s="98"/>
       <c r="F52" s="98"/>
@@ -4222,18 +4259,18 @@
       <c r="A53" s="78"/>
       <c r="B53" s="93"/>
       <c r="C53" s="77"/>
-      <c r="D53" s="121"/>
-      <c r="E53" s="122"/>
-      <c r="F53" s="122"/>
+      <c r="D53" s="126"/>
+      <c r="E53" s="127"/>
+      <c r="F53" s="127"/>
       <c r="G53" s="76"/>
       <c r="H53" s="83"/>
       <c r="I53" s="77"/>
       <c r="J53" s="75"/>
     </row>
     <row r="54" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A54" s="119"/>
-      <c r="B54" s="120"/>
-      <c r="C54" s="120"/>
+      <c r="A54" s="124"/>
+      <c r="B54" s="125"/>
+      <c r="C54" s="125"/>
       <c r="D54" s="98"/>
       <c r="E54" s="98"/>
       <c r="F54" s="98"/>
@@ -4246,18 +4283,18 @@
       <c r="A55" s="78"/>
       <c r="B55" s="93"/>
       <c r="C55" s="77"/>
-      <c r="D55" s="121"/>
-      <c r="E55" s="122"/>
-      <c r="F55" s="122"/>
+      <c r="D55" s="126"/>
+      <c r="E55" s="127"/>
+      <c r="F55" s="127"/>
       <c r="G55" s="76"/>
       <c r="H55" s="83"/>
       <c r="I55" s="77"/>
       <c r="J55" s="75"/>
     </row>
     <row r="56" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A56" s="119"/>
-      <c r="B56" s="120"/>
-      <c r="C56" s="120"/>
+      <c r="A56" s="124"/>
+      <c r="B56" s="125"/>
+      <c r="C56" s="125"/>
       <c r="D56" s="98"/>
       <c r="E56" s="98"/>
       <c r="F56" s="98"/>
@@ -4270,18 +4307,18 @@
       <c r="A57" s="78"/>
       <c r="B57" s="93"/>
       <c r="C57" s="77"/>
-      <c r="D57" s="121"/>
-      <c r="E57" s="122"/>
-      <c r="F57" s="122"/>
+      <c r="D57" s="126"/>
+      <c r="E57" s="127"/>
+      <c r="F57" s="127"/>
       <c r="G57" s="76"/>
       <c r="H57" s="83"/>
       <c r="I57" s="77"/>
       <c r="J57" s="75"/>
     </row>
     <row r="58" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A58" s="119"/>
-      <c r="B58" s="120"/>
-      <c r="C58" s="120"/>
+      <c r="A58" s="124"/>
+      <c r="B58" s="125"/>
+      <c r="C58" s="125"/>
       <c r="D58" s="98"/>
       <c r="E58" s="98"/>
       <c r="F58" s="98"/>
@@ -4294,18 +4331,18 @@
       <c r="A59" s="78"/>
       <c r="B59" s="93"/>
       <c r="C59" s="77"/>
-      <c r="D59" s="121"/>
-      <c r="E59" s="122"/>
-      <c r="F59" s="122"/>
+      <c r="D59" s="126"/>
+      <c r="E59" s="127"/>
+      <c r="F59" s="127"/>
       <c r="G59" s="76"/>
       <c r="H59" s="83"/>
       <c r="I59" s="77"/>
       <c r="J59" s="75"/>
     </row>
     <row r="60" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A60" s="119"/>
-      <c r="B60" s="120"/>
-      <c r="C60" s="120"/>
+      <c r="A60" s="124"/>
+      <c r="B60" s="125"/>
+      <c r="C60" s="125"/>
       <c r="D60" s="98"/>
       <c r="E60" s="98"/>
       <c r="F60" s="98"/>
@@ -4318,18 +4355,18 @@
       <c r="A61" s="78"/>
       <c r="B61" s="93"/>
       <c r="C61" s="77"/>
-      <c r="D61" s="121"/>
-      <c r="E61" s="122"/>
-      <c r="F61" s="122"/>
+      <c r="D61" s="126"/>
+      <c r="E61" s="127"/>
+      <c r="F61" s="127"/>
       <c r="G61" s="76"/>
       <c r="H61" s="83"/>
       <c r="I61" s="77"/>
       <c r="J61" s="75"/>
     </row>
     <row r="62" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A62" s="119"/>
-      <c r="B62" s="120"/>
-      <c r="C62" s="120"/>
+      <c r="A62" s="124"/>
+      <c r="B62" s="125"/>
+      <c r="C62" s="125"/>
       <c r="D62" s="98"/>
       <c r="E62" s="98"/>
       <c r="F62" s="98"/>
@@ -4342,9 +4379,9 @@
       <c r="A63" s="78"/>
       <c r="B63" s="93"/>
       <c r="C63" s="77"/>
-      <c r="D63" s="121"/>
-      <c r="E63" s="122"/>
-      <c r="F63" s="122"/>
+      <c r="D63" s="126"/>
+      <c r="E63" s="127"/>
+      <c r="F63" s="127"/>
       <c r="G63" s="76"/>
       <c r="H63" s="83"/>
       <c r="I63" s="77"/>
@@ -4480,16 +4517,50 @@
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="D63:F63"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D55:F55"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="D57:F57"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="D51:F51"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="D53:F53"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="B1:D2"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="D22:F22"/>
@@ -4506,50 +4577,16 @@
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="D25:F25"/>
     <mergeCell ref="D28:F28"/>
-    <mergeCell ref="B1:D2"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="D53:F53"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="A60:C60"/>
-    <mergeCell ref="D61:F61"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="D63:F63"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D55:F55"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="D57:F57"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="D59:F59"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="D51:F51"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D18:F18"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4565,8 +4602,8 @@
   </sheetPr>
   <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="82" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="82" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" outlineLevelRow="1"/>
@@ -4585,9 +4622,9 @@
       <c r="A1" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
+      <c r="B1" s="140"/>
+      <c r="C1" s="140"/>
+      <c r="D1" s="140"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -4598,9 +4635,9 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="124"/>
-      <c r="C2" s="124"/>
-      <c r="D2" s="124"/>
+      <c r="B2" s="141"/>
+      <c r="C2" s="141"/>
+      <c r="D2" s="141"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -4621,43 +4658,43 @@
       <c r="E3" s="61"/>
       <c r="F3" s="61"/>
       <c r="G3" s="61"/>
-      <c r="H3" s="133"/>
-      <c r="I3" s="133"/>
-      <c r="J3" s="133"/>
+      <c r="H3" s="148"/>
+      <c r="I3" s="148"/>
+      <c r="J3" s="148"/>
       <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="12.75">
       <c r="A4" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="135" t="s">
+      <c r="B4" s="149" t="s">
         <v>158</v>
       </c>
-      <c r="C4" s="136"/>
-      <c r="D4" s="137"/>
+      <c r="C4" s="150"/>
+      <c r="D4" s="151"/>
       <c r="E4" s="61"/>
       <c r="F4" s="61"/>
       <c r="G4" s="61"/>
-      <c r="H4" s="133"/>
-      <c r="I4" s="133"/>
-      <c r="J4" s="133"/>
+      <c r="H4" s="148"/>
+      <c r="I4" s="148"/>
+      <c r="J4" s="148"/>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" s="71" customFormat="1" ht="25.5">
       <c r="A5" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="126" t="s">
+      <c r="B5" s="143" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="127"/>
-      <c r="D5" s="128"/>
+      <c r="C5" s="144"/>
+      <c r="D5" s="145"/>
       <c r="E5" s="69"/>
       <c r="F5" s="69"/>
       <c r="G5" s="69"/>
-      <c r="H5" s="132"/>
-      <c r="I5" s="132"/>
-      <c r="J5" s="132"/>
+      <c r="H5" s="147"/>
+      <c r="I5" s="147"/>
+      <c r="J5" s="147"/>
       <c r="K5" s="70"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
@@ -4678,9 +4715,9 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="133"/>
-      <c r="I6" s="133"/>
-      <c r="J6" s="133"/>
+      <c r="H6" s="148"/>
+      <c r="I6" s="148"/>
+      <c r="J6" s="148"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -4701,16 +4738,16 @@
       <c r="E7" s="62"/>
       <c r="F7" s="62"/>
       <c r="G7" s="62"/>
-      <c r="H7" s="133"/>
-      <c r="I7" s="133"/>
-      <c r="J7" s="133"/>
+      <c r="H7" s="148"/>
+      <c r="I7" s="148"/>
+      <c r="J7" s="148"/>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="125"/>
-      <c r="B8" s="125"/>
-      <c r="C8" s="125"/>
-      <c r="D8" s="125"/>
+      <c r="A8" s="142"/>
+      <c r="B8" s="142"/>
+      <c r="C8" s="142"/>
+      <c r="D8" s="142"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -4720,78 +4757,78 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" s="73" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="142" t="s">
+      <c r="A9" s="131" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="143" t="s">
+      <c r="B9" s="155" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="142" t="s">
+      <c r="C9" s="131" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="149" t="s">
+      <c r="D9" s="132" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="150"/>
-      <c r="F9" s="150"/>
-      <c r="G9" s="151"/>
-      <c r="H9" s="138" t="s">
+      <c r="E9" s="133"/>
+      <c r="F9" s="133"/>
+      <c r="G9" s="134"/>
+      <c r="H9" s="152" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="134" t="s">
+      <c r="I9" s="128" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="134" t="s">
+      <c r="J9" s="128" t="s">
         <v>32</v>
       </c>
       <c r="K9" s="72"/>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="134"/>
-      <c r="B10" s="144"/>
-      <c r="C10" s="134"/>
-      <c r="D10" s="139"/>
-      <c r="E10" s="152"/>
-      <c r="F10" s="152"/>
-      <c r="G10" s="153"/>
-      <c r="H10" s="139"/>
-      <c r="I10" s="134"/>
-      <c r="J10" s="134"/>
+      <c r="A10" s="128"/>
+      <c r="B10" s="156"/>
+      <c r="C10" s="128"/>
+      <c r="D10" s="135"/>
+      <c r="E10" s="136"/>
+      <c r="F10" s="136"/>
+      <c r="G10" s="137"/>
+      <c r="H10" s="135"/>
+      <c r="I10" s="128"/>
+      <c r="J10" s="128"/>
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" s="74" customFormat="1" ht="15">
-      <c r="A11" s="140"/>
-      <c r="B11" s="140"/>
-      <c r="C11" s="140"/>
-      <c r="D11" s="140"/>
-      <c r="E11" s="140"/>
-      <c r="F11" s="140"/>
-      <c r="G11" s="140"/>
-      <c r="H11" s="140"/>
-      <c r="I11" s="140"/>
-      <c r="J11" s="141"/>
+      <c r="A11" s="153"/>
+      <c r="B11" s="153"/>
+      <c r="C11" s="153"/>
+      <c r="D11" s="153"/>
+      <c r="E11" s="153"/>
+      <c r="F11" s="153"/>
+      <c r="G11" s="153"/>
+      <c r="H11" s="153"/>
+      <c r="I11" s="153"/>
+      <c r="J11" s="154"/>
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A12" s="129" t="s">
+      <c r="A12" s="138" t="s">
         <v>159</v>
       </c>
-      <c r="B12" s="130"/>
-      <c r="C12" s="130"/>
-      <c r="D12" s="130"/>
-      <c r="E12" s="130"/>
-      <c r="F12" s="130"/>
-      <c r="G12" s="130"/>
-      <c r="H12" s="130"/>
-      <c r="I12" s="130"/>
-      <c r="J12" s="131"/>
+      <c r="B12" s="139"/>
+      <c r="C12" s="139"/>
+      <c r="D12" s="139"/>
+      <c r="E12" s="139"/>
+      <c r="F12" s="139"/>
+      <c r="G12" s="139"/>
+      <c r="H12" s="139"/>
+      <c r="I12" s="139"/>
+      <c r="J12" s="146"/>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" ht="102.75" customHeight="1" outlineLevel="1">
       <c r="A13" s="78"/>
       <c r="B13" s="82"/>
       <c r="C13" s="77"/>
-      <c r="D13" s="147"/>
-      <c r="E13" s="148"/>
-      <c r="F13" s="148"/>
+      <c r="D13" s="119"/>
+      <c r="E13" s="120"/>
+      <c r="F13" s="120"/>
       <c r="G13" s="76"/>
       <c r="H13" s="90"/>
       <c r="I13" s="77"/>
@@ -4801,9 +4838,9 @@
       <c r="A14" s="78"/>
       <c r="B14" s="82"/>
       <c r="C14" s="77"/>
-      <c r="D14" s="147"/>
-      <c r="E14" s="148"/>
-      <c r="F14" s="148"/>
+      <c r="D14" s="119"/>
+      <c r="E14" s="120"/>
+      <c r="F14" s="120"/>
       <c r="G14" s="76"/>
       <c r="H14" s="90"/>
       <c r="I14" s="77"/>
@@ -4813,9 +4850,9 @@
       <c r="A15" s="78"/>
       <c r="B15" s="82"/>
       <c r="C15" s="77"/>
-      <c r="D15" s="147"/>
-      <c r="E15" s="148"/>
-      <c r="F15" s="148"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="120"/>
+      <c r="F15" s="120"/>
       <c r="G15" s="76"/>
       <c r="H15" s="90"/>
       <c r="I15" s="77"/>
@@ -4825,9 +4862,9 @@
       <c r="A16" s="78"/>
       <c r="B16" s="82"/>
       <c r="C16" s="77"/>
-      <c r="D16" s="147"/>
-      <c r="E16" s="148"/>
-      <c r="F16" s="148"/>
+      <c r="D16" s="119"/>
+      <c r="E16" s="120"/>
+      <c r="F16" s="120"/>
       <c r="G16" s="76"/>
       <c r="H16" s="90"/>
       <c r="I16" s="77"/>
@@ -4837,9 +4874,9 @@
       <c r="A17" s="78"/>
       <c r="B17" s="82"/>
       <c r="C17" s="77"/>
-      <c r="D17" s="147"/>
-      <c r="E17" s="148"/>
-      <c r="F17" s="148"/>
+      <c r="D17" s="119"/>
+      <c r="E17" s="120"/>
+      <c r="F17" s="120"/>
       <c r="G17" s="76"/>
       <c r="H17" s="90"/>
       <c r="I17" s="77"/>
@@ -4849,20 +4886,20 @@
       <c r="A18" s="78"/>
       <c r="B18" s="82"/>
       <c r="C18" s="77"/>
-      <c r="D18" s="147"/>
-      <c r="E18" s="148"/>
-      <c r="F18" s="148"/>
+      <c r="D18" s="119"/>
+      <c r="E18" s="120"/>
+      <c r="F18" s="120"/>
       <c r="G18" s="76"/>
       <c r="H18" s="90"/>
       <c r="I18" s="77"/>
       <c r="J18" s="75"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A19" s="129" t="s">
+      <c r="A19" s="138" t="s">
         <v>160</v>
       </c>
-      <c r="B19" s="130"/>
-      <c r="C19" s="130"/>
+      <c r="B19" s="139"/>
+      <c r="C19" s="139"/>
       <c r="D19" s="88"/>
       <c r="E19" s="88"/>
       <c r="F19" s="88"/>
@@ -4876,13 +4913,13 @@
         <v>0</v>
       </c>
       <c r="B20" s="86" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="C20" s="87" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="D20" s="157" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="E20" s="158"/>
       <c r="F20" s="158"/>
@@ -4896,13 +4933,13 @@
         <v>1</v>
       </c>
       <c r="B21" s="86" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="C21" s="87" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="D21" s="157" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="E21" s="158"/>
       <c r="F21" s="158"/>
@@ -4916,13 +4953,13 @@
         <v>2</v>
       </c>
       <c r="B22" s="86" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C22" s="87" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="D22" s="157" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="E22" s="158"/>
       <c r="F22" s="158"/>
@@ -4932,11 +4969,11 @@
       <c r="J22" s="97"/>
     </row>
     <row r="23" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A23" s="129" t="s">
-        <v>164</v>
-      </c>
-      <c r="B23" s="130"/>
-      <c r="C23" s="130"/>
+      <c r="A23" s="138" t="s">
+        <v>177</v>
+      </c>
+      <c r="B23" s="139"/>
+      <c r="C23" s="139"/>
       <c r="D23" s="88"/>
       <c r="E23" s="88"/>
       <c r="F23" s="88"/>
@@ -4950,14 +4987,16 @@
         <v>0</v>
       </c>
       <c r="B24" s="93" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="C24" s="77" t="s">
-        <v>165</v>
-      </c>
-      <c r="D24" s="121"/>
-      <c r="E24" s="122"/>
-      <c r="F24" s="122"/>
+        <v>181</v>
+      </c>
+      <c r="D24" s="119" t="s">
+        <v>179</v>
+      </c>
+      <c r="E24" s="120"/>
+      <c r="F24" s="120"/>
       <c r="G24" s="76"/>
       <c r="H24" s="83"/>
       <c r="I24" s="77"/>
@@ -4968,14 +5007,16 @@
         <v>1</v>
       </c>
       <c r="B25" s="93" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="C25" s="77" t="s">
-        <v>167</v>
-      </c>
-      <c r="D25" s="121"/>
-      <c r="E25" s="122"/>
-      <c r="F25" s="122"/>
+        <v>182</v>
+      </c>
+      <c r="D25" s="119" t="s">
+        <v>183</v>
+      </c>
+      <c r="E25" s="120"/>
+      <c r="F25" s="120"/>
       <c r="G25" s="76"/>
       <c r="H25" s="83"/>
       <c r="I25" s="77"/>
@@ -4986,41 +5027,45 @@
         <v>2</v>
       </c>
       <c r="B26" s="93" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="C26" s="77" t="s">
-        <v>168</v>
-      </c>
-      <c r="D26" s="121"/>
-      <c r="E26" s="122"/>
-      <c r="F26" s="122"/>
+        <v>185</v>
+      </c>
+      <c r="D26" s="119" t="s">
+        <v>186</v>
+      </c>
+      <c r="E26" s="120"/>
+      <c r="F26" s="120"/>
       <c r="G26" s="76"/>
       <c r="H26" s="83"/>
       <c r="I26" s="77"/>
       <c r="J26" s="75"/>
     </row>
-    <row r="27" spans="1:10" s="4" customFormat="1" ht="93" customHeight="1" outlineLevel="1">
+    <row r="27" spans="1:10" s="4" customFormat="1" ht="113.25" customHeight="1" outlineLevel="1">
       <c r="A27" s="78" t="s">
         <v>50</v>
       </c>
       <c r="B27" s="93" t="s">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="C27" s="77" t="s">
-        <v>172</v>
-      </c>
-      <c r="D27" s="121"/>
-      <c r="E27" s="122"/>
-      <c r="F27" s="122"/>
+        <v>188</v>
+      </c>
+      <c r="D27" s="119" t="s">
+        <v>189</v>
+      </c>
+      <c r="E27" s="120"/>
+      <c r="F27" s="120"/>
       <c r="G27" s="76"/>
       <c r="H27" s="83"/>
       <c r="I27" s="77"/>
       <c r="J27" s="75"/>
     </row>
     <row r="28" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A28" s="119"/>
-      <c r="B28" s="120"/>
-      <c r="C28" s="120"/>
+      <c r="A28" s="124"/>
+      <c r="B28" s="125"/>
+      <c r="C28" s="125"/>
       <c r="D28" s="98"/>
       <c r="E28" s="98"/>
       <c r="F28" s="98"/>
@@ -5033,9 +5078,9 @@
       <c r="A29" s="78"/>
       <c r="B29" s="93"/>
       <c r="C29" s="77"/>
-      <c r="D29" s="121"/>
-      <c r="E29" s="122"/>
-      <c r="F29" s="122"/>
+      <c r="D29" s="126"/>
+      <c r="E29" s="127"/>
+      <c r="F29" s="127"/>
       <c r="G29" s="76"/>
       <c r="H29" s="83"/>
       <c r="I29" s="77"/>
@@ -5045,9 +5090,9 @@
       <c r="A30" s="78"/>
       <c r="B30" s="93"/>
       <c r="C30" s="77"/>
-      <c r="D30" s="121"/>
-      <c r="E30" s="122"/>
-      <c r="F30" s="122"/>
+      <c r="D30" s="126"/>
+      <c r="E30" s="127"/>
+      <c r="F30" s="127"/>
       <c r="G30" s="76"/>
       <c r="H30" s="83"/>
       <c r="I30" s="77"/>
@@ -5057,9 +5102,9 @@
       <c r="A31" s="78"/>
       <c r="B31" s="93"/>
       <c r="C31" s="77"/>
-      <c r="D31" s="121"/>
-      <c r="E31" s="122"/>
-      <c r="F31" s="122"/>
+      <c r="D31" s="126"/>
+      <c r="E31" s="127"/>
+      <c r="F31" s="127"/>
       <c r="G31" s="76"/>
       <c r="H31" s="83"/>
       <c r="I31" s="77"/>
@@ -5069,9 +5114,9 @@
       <c r="A32" s="78"/>
       <c r="B32" s="93"/>
       <c r="C32" s="77"/>
-      <c r="D32" s="121"/>
-      <c r="E32" s="122"/>
-      <c r="F32" s="122"/>
+      <c r="D32" s="126"/>
+      <c r="E32" s="127"/>
+      <c r="F32" s="127"/>
       <c r="G32" s="76"/>
       <c r="H32" s="83"/>
       <c r="I32" s="77"/>
@@ -5081,9 +5126,9 @@
       <c r="A33" s="78"/>
       <c r="B33" s="93"/>
       <c r="C33" s="77"/>
-      <c r="D33" s="121"/>
-      <c r="E33" s="122"/>
-      <c r="F33" s="122"/>
+      <c r="D33" s="126"/>
+      <c r="E33" s="127"/>
+      <c r="F33" s="127"/>
       <c r="G33" s="76"/>
       <c r="H33" s="83"/>
       <c r="I33" s="77"/>
@@ -5093,18 +5138,18 @@
       <c r="A34" s="78"/>
       <c r="B34" s="93"/>
       <c r="C34" s="77"/>
-      <c r="D34" s="121"/>
-      <c r="E34" s="122"/>
-      <c r="F34" s="122"/>
+      <c r="D34" s="126"/>
+      <c r="E34" s="127"/>
+      <c r="F34" s="127"/>
       <c r="G34" s="76"/>
       <c r="H34" s="83"/>
       <c r="I34" s="77"/>
       <c r="J34" s="75"/>
     </row>
     <row r="35" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A35" s="119"/>
-      <c r="B35" s="120"/>
-      <c r="C35" s="120"/>
+      <c r="A35" s="124"/>
+      <c r="B35" s="125"/>
+      <c r="C35" s="125"/>
       <c r="D35" s="98"/>
       <c r="E35" s="98"/>
       <c r="F35" s="98"/>
@@ -5117,9 +5162,9 @@
       <c r="A36" s="78"/>
       <c r="B36" s="93"/>
       <c r="C36" s="77"/>
-      <c r="D36" s="121"/>
-      <c r="E36" s="122"/>
-      <c r="F36" s="122"/>
+      <c r="D36" s="126"/>
+      <c r="E36" s="127"/>
+      <c r="F36" s="127"/>
       <c r="G36" s="76"/>
       <c r="H36" s="83"/>
       <c r="I36" s="77"/>
@@ -5255,13 +5300,26 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="B1:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="D20:F20"/>
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="H6:J6"/>
     <mergeCell ref="H7:J7"/>
@@ -5278,26 +5336,13 @@
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="D14:F14"/>
     <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="B1:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="H4:J4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
up tc dk sk
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University_IT\Tam\KiemThuPhanMem\event-manager-javafx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E517A05C-C2C9-424C-A1D9-C7C66F60CB4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EB88BF-55DF-4E75-A9FC-4082554362AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9810" yWindow="465" windowWidth="10365" windowHeight="10155" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9810" yWindow="465" windowWidth="10365" windowHeight="10155" tabRatio="821" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="97" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="209">
   <si>
     <t>TC1</t>
   </si>
@@ -804,6 +804,57 @@
   </si>
   <si>
     <t>Viết TC Kiểm tra chức năng tìm kiếm user đăng ký tham gia sự kiện</t>
+  </si>
+  <si>
+    <t>B1: Đăng nhập với tư cách là user
+B2: Truy cập vào trang Sự kiện
+B3: Chọn sự kiện còn vé
+B4: Nhập đầy đủ thông tin hợp lệ
+B5: Nhấn nút Đăng ký tham gia
+B6: Xác nhận đăng ký</t>
+  </si>
+  <si>
+    <t>Hiển thị thông báo đăng ký tham gia sự kiện thành công</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng đăng ký tham gia sự kiện thành công với tư cách là user</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng không cho phép đăng ký tham gia sự kiện trùng giờ</t>
+  </si>
+  <si>
+    <t>B1: Đăng nhập với tư cách là user và user đã đăng ký một sự kiện trước đó 
+B2: Truy cập vào trang Sự kiện
+B3: Chọn sự kiện còn vé và diễn ra cùng thời gian với sự kiện đã đăng ký trước đó
+B4: Nhập đầy đủ thông tin hợp lệ
+B5: Nhấn nút Đăng ký tham gia
+B6: Xác nhận đăng ký</t>
+  </si>
+  <si>
+    <t>Hiển thị thông báo lỗi không thể đăng ký do trùng thời gian với sự kiện khác</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng không cho phép đăng ký khi sự kiện đã hết vé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B1: Đăng nhập với tư cách là user
+B2: Truy cập vào trang Sự kiện
+B3: Chọn một sự kiện đã hết vé(Số lượng vé: 0)
+B4: Nhập đầy đủ thông tin hợp lệ
+B5: Nhấn nút đăng ký
+B6: Xác nhận đăng ký </t>
+  </si>
+  <si>
+    <t>Hiển thị thông báo sự kiện đã hết vé</t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra chức năng đăng ký tham gia sự kiện thành công với tư cách là user</t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra chức năng không cho phép đăng ký tham gia sự kiện trùng giờ</t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra chức năng không cho phép đăng ký khi sự kiện đã hết vé</t>
   </si>
 </sst>
 </file>
@@ -1821,12 +1872,111 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1835,105 +1985,6 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2275,8 +2326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H71"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D50" zoomScale="85" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A53" zoomScale="85" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -3209,30 +3260,54 @@
       <c r="G58" s="101"/>
       <c r="H58" s="107"/>
     </row>
-    <row r="59" spans="2:8" s="34" customFormat="1">
-      <c r="B59" s="36"/>
-      <c r="C59" s="37"/>
+    <row r="59" spans="2:8" s="34" customFormat="1" ht="25.5">
+      <c r="B59" s="36">
+        <v>45751</v>
+      </c>
+      <c r="C59" s="37" t="s">
+        <v>40</v>
+      </c>
       <c r="D59" s="101"/>
-      <c r="E59" s="106"/>
-      <c r="F59" s="112"/>
+      <c r="E59" s="106" t="s">
+        <v>206</v>
+      </c>
+      <c r="F59" s="112" t="s">
+        <v>44</v>
+      </c>
       <c r="G59" s="101"/>
       <c r="H59" s="107"/>
     </row>
-    <row r="60" spans="2:8" s="34" customFormat="1">
-      <c r="B60" s="36"/>
-      <c r="C60" s="37"/>
+    <row r="60" spans="2:8" s="34" customFormat="1" ht="25.5">
+      <c r="B60" s="36">
+        <v>45751</v>
+      </c>
+      <c r="C60" s="37" t="s">
+        <v>40</v>
+      </c>
       <c r="D60" s="101"/>
-      <c r="E60" s="106"/>
-      <c r="F60" s="112"/>
+      <c r="E60" s="106" t="s">
+        <v>207</v>
+      </c>
+      <c r="F60" s="112" t="s">
+        <v>44</v>
+      </c>
       <c r="G60" s="101"/>
       <c r="H60" s="107"/>
     </row>
-    <row r="61" spans="2:8" s="34" customFormat="1">
-      <c r="B61" s="36"/>
-      <c r="C61" s="37"/>
+    <row r="61" spans="2:8" s="34" customFormat="1" ht="25.5">
+      <c r="B61" s="36">
+        <v>45751</v>
+      </c>
+      <c r="C61" s="37" t="s">
+        <v>40</v>
+      </c>
       <c r="D61" s="101"/>
-      <c r="E61" s="106"/>
-      <c r="F61" s="112"/>
+      <c r="E61" s="106" t="s">
+        <v>208</v>
+      </c>
+      <c r="F61" s="112" t="s">
+        <v>44</v>
+      </c>
       <c r="G61" s="101"/>
       <c r="H61" s="107"/>
     </row>
@@ -3341,7 +3416,7 @@
     <oddFooter>&amp;L&amp;"Tahoma,Regular"&amp;8 02ae-BM/PM/HDCV/FSOFT v1/0&amp;R&amp;"Tahoma,Regular"&amp;10&amp;P/&amp;N</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="C12:C34 C42 C35:C41 C43:C48 C49:C50 C52:C54 C51 C55:C58" numberStoredAsText="1"/>
+    <ignoredError sqref="C12:C34 C42 C35:C41 C43:C48 C49:C50 C52:C54 C51 C55:C58 C59:C61" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -3373,9 +3448,9 @@
       <c r="A1" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="140"/>
-      <c r="C1" s="140"/>
-      <c r="D1" s="140"/>
+      <c r="B1" s="123"/>
+      <c r="C1" s="123"/>
+      <c r="D1" s="123"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -3386,9 +3461,9 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="141"/>
-      <c r="C2" s="141"/>
-      <c r="D2" s="141"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="124"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -3409,43 +3484,43 @@
       <c r="E3" s="61"/>
       <c r="F3" s="61"/>
       <c r="G3" s="61"/>
-      <c r="H3" s="148"/>
-      <c r="I3" s="148"/>
-      <c r="J3" s="148"/>
+      <c r="H3" s="133"/>
+      <c r="I3" s="133"/>
+      <c r="J3" s="133"/>
       <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="12.75">
       <c r="A4" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="149" t="s">
+      <c r="B4" s="135" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="150"/>
-      <c r="D4" s="151"/>
+      <c r="C4" s="136"/>
+      <c r="D4" s="137"/>
       <c r="E4" s="61"/>
       <c r="F4" s="61"/>
       <c r="G4" s="61"/>
-      <c r="H4" s="148"/>
-      <c r="I4" s="148"/>
-      <c r="J4" s="148"/>
+      <c r="H4" s="133"/>
+      <c r="I4" s="133"/>
+      <c r="J4" s="133"/>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" s="71" customFormat="1" ht="25.5">
       <c r="A5" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="143" t="s">
+      <c r="B5" s="126" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="144"/>
-      <c r="D5" s="145"/>
+      <c r="C5" s="127"/>
+      <c r="D5" s="128"/>
       <c r="E5" s="69"/>
       <c r="F5" s="69"/>
       <c r="G5" s="69"/>
-      <c r="H5" s="147"/>
-      <c r="I5" s="147"/>
-      <c r="J5" s="147"/>
+      <c r="H5" s="132"/>
+      <c r="I5" s="132"/>
+      <c r="J5" s="132"/>
       <c r="K5" s="70"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
@@ -3466,9 +3541,9 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="148"/>
-      <c r="I6" s="148"/>
-      <c r="J6" s="148"/>
+      <c r="H6" s="133"/>
+      <c r="I6" s="133"/>
+      <c r="J6" s="133"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -3489,16 +3564,16 @@
       <c r="E7" s="62"/>
       <c r="F7" s="62"/>
       <c r="G7" s="62"/>
-      <c r="H7" s="148"/>
-      <c r="I7" s="148"/>
-      <c r="J7" s="148"/>
+      <c r="H7" s="133"/>
+      <c r="I7" s="133"/>
+      <c r="J7" s="133"/>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="142"/>
-      <c r="B8" s="142"/>
-      <c r="C8" s="142"/>
-      <c r="D8" s="142"/>
+      <c r="A8" s="125"/>
+      <c r="B8" s="125"/>
+      <c r="C8" s="125"/>
+      <c r="D8" s="125"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -3508,70 +3583,70 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" s="73" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="131" t="s">
+      <c r="A9" s="142" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="155" t="s">
+      <c r="B9" s="143" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="131" t="s">
+      <c r="C9" s="142" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="132" t="s">
+      <c r="D9" s="149" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="133"/>
-      <c r="F9" s="133"/>
-      <c r="G9" s="134"/>
-      <c r="H9" s="152" t="s">
+      <c r="E9" s="150"/>
+      <c r="F9" s="150"/>
+      <c r="G9" s="151"/>
+      <c r="H9" s="138" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="128" t="s">
+      <c r="I9" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="128" t="s">
+      <c r="J9" s="134" t="s">
         <v>32</v>
       </c>
       <c r="K9" s="72"/>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="128"/>
-      <c r="B10" s="156"/>
-      <c r="C10" s="128"/>
-      <c r="D10" s="135"/>
-      <c r="E10" s="136"/>
-      <c r="F10" s="136"/>
-      <c r="G10" s="137"/>
-      <c r="H10" s="135"/>
-      <c r="I10" s="128"/>
-      <c r="J10" s="128"/>
+      <c r="A10" s="134"/>
+      <c r="B10" s="144"/>
+      <c r="C10" s="134"/>
+      <c r="D10" s="139"/>
+      <c r="E10" s="152"/>
+      <c r="F10" s="152"/>
+      <c r="G10" s="153"/>
+      <c r="H10" s="139"/>
+      <c r="I10" s="134"/>
+      <c r="J10" s="134"/>
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" s="74" customFormat="1" ht="15">
-      <c r="A11" s="153"/>
-      <c r="B11" s="153"/>
-      <c r="C11" s="153"/>
-      <c r="D11" s="153"/>
-      <c r="E11" s="153"/>
-      <c r="F11" s="153"/>
-      <c r="G11" s="153"/>
-      <c r="H11" s="153"/>
-      <c r="I11" s="153"/>
-      <c r="J11" s="154"/>
+      <c r="A11" s="140"/>
+      <c r="B11" s="140"/>
+      <c r="C11" s="140"/>
+      <c r="D11" s="140"/>
+      <c r="E11" s="140"/>
+      <c r="F11" s="140"/>
+      <c r="G11" s="140"/>
+      <c r="H11" s="140"/>
+      <c r="I11" s="140"/>
+      <c r="J11" s="141"/>
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A12" s="138" t="s">
+      <c r="A12" s="129" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="139"/>
-      <c r="C12" s="139"/>
-      <c r="D12" s="139"/>
-      <c r="E12" s="139"/>
-      <c r="F12" s="139"/>
-      <c r="G12" s="139"/>
-      <c r="H12" s="139"/>
-      <c r="I12" s="139"/>
-      <c r="J12" s="146"/>
+      <c r="B12" s="130"/>
+      <c r="C12" s="130"/>
+      <c r="D12" s="130"/>
+      <c r="E12" s="130"/>
+      <c r="F12" s="130"/>
+      <c r="G12" s="130"/>
+      <c r="H12" s="130"/>
+      <c r="I12" s="130"/>
+      <c r="J12" s="131"/>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" ht="66.75" customHeight="1" outlineLevel="1">
       <c r="A13" s="78" t="s">
@@ -3583,9 +3658,9 @@
       <c r="C13" s="77" t="s">
         <v>85</v>
       </c>
-      <c r="D13" s="119"/>
-      <c r="E13" s="120"/>
-      <c r="F13" s="120"/>
+      <c r="D13" s="147"/>
+      <c r="E13" s="148"/>
+      <c r="F13" s="148"/>
       <c r="G13" s="76"/>
       <c r="H13" s="90"/>
       <c r="I13" s="77"/>
@@ -3601,9 +3676,9 @@
       <c r="C14" s="77" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="119"/>
-      <c r="E14" s="120"/>
-      <c r="F14" s="120"/>
+      <c r="D14" s="147"/>
+      <c r="E14" s="148"/>
+      <c r="F14" s="148"/>
       <c r="G14" s="76"/>
       <c r="H14" s="90"/>
       <c r="I14" s="77"/>
@@ -3619,9 +3694,9 @@
       <c r="C15" s="77" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="119"/>
-      <c r="E15" s="120"/>
-      <c r="F15" s="120"/>
+      <c r="D15" s="147"/>
+      <c r="E15" s="148"/>
+      <c r="F15" s="148"/>
       <c r="G15" s="76"/>
       <c r="H15" s="90"/>
       <c r="I15" s="77"/>
@@ -3637,9 +3712,9 @@
       <c r="C16" s="77" t="s">
         <v>95</v>
       </c>
-      <c r="D16" s="119"/>
-      <c r="E16" s="120"/>
-      <c r="F16" s="120"/>
+      <c r="D16" s="147"/>
+      <c r="E16" s="148"/>
+      <c r="F16" s="148"/>
       <c r="G16" s="76"/>
       <c r="H16" s="90"/>
       <c r="I16" s="77"/>
@@ -3655,9 +3730,9 @@
       <c r="C17" s="77" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="119"/>
-      <c r="E17" s="120"/>
-      <c r="F17" s="120"/>
+      <c r="D17" s="147"/>
+      <c r="E17" s="148"/>
+      <c r="F17" s="148"/>
       <c r="G17" s="76"/>
       <c r="H17" s="90"/>
       <c r="I17" s="77"/>
@@ -3673,9 +3748,9 @@
       <c r="C18" s="77" t="s">
         <v>93</v>
       </c>
-      <c r="D18" s="119"/>
-      <c r="E18" s="120"/>
-      <c r="F18" s="120"/>
+      <c r="D18" s="147"/>
+      <c r="E18" s="148"/>
+      <c r="F18" s="148"/>
       <c r="G18" s="76"/>
       <c r="H18" s="90"/>
       <c r="I18" s="77"/>
@@ -3691,9 +3766,9 @@
       <c r="C19" s="87" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="121"/>
-      <c r="E19" s="122"/>
-      <c r="F19" s="123"/>
+      <c r="D19" s="154"/>
+      <c r="E19" s="155"/>
+      <c r="F19" s="156"/>
       <c r="G19" s="77"/>
       <c r="H19" s="77"/>
       <c r="I19" s="77"/>
@@ -3709,20 +3784,20 @@
       <c r="C20" s="77" t="s">
         <v>102</v>
       </c>
-      <c r="D20" s="121"/>
-      <c r="E20" s="122"/>
-      <c r="F20" s="123"/>
+      <c r="D20" s="154"/>
+      <c r="E20" s="155"/>
+      <c r="F20" s="156"/>
       <c r="G20" s="77"/>
       <c r="H20" s="77"/>
       <c r="I20" s="77"/>
       <c r="J20" s="75"/>
     </row>
     <row r="21" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A21" s="138" t="s">
+      <c r="A21" s="129" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="139"/>
-      <c r="C21" s="139"/>
+      <c r="B21" s="130"/>
+      <c r="C21" s="130"/>
       <c r="D21" s="88"/>
       <c r="E21" s="88"/>
       <c r="F21" s="88"/>
@@ -3741,9 +3816,9 @@
       <c r="C22" s="87" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="129"/>
-      <c r="E22" s="130"/>
-      <c r="F22" s="130"/>
+      <c r="D22" s="145"/>
+      <c r="E22" s="146"/>
+      <c r="F22" s="146"/>
       <c r="G22" s="95"/>
       <c r="H22" s="96"/>
       <c r="I22" s="87"/>
@@ -3759,9 +3834,9 @@
       <c r="C23" s="87" t="s">
         <v>72</v>
       </c>
-      <c r="D23" s="129"/>
-      <c r="E23" s="130"/>
-      <c r="F23" s="130"/>
+      <c r="D23" s="145"/>
+      <c r="E23" s="146"/>
+      <c r="F23" s="146"/>
       <c r="G23" s="95"/>
       <c r="H23" s="96"/>
       <c r="I23" s="87"/>
@@ -3777,9 +3852,9 @@
       <c r="C24" s="87" t="s">
         <v>75</v>
       </c>
-      <c r="D24" s="129"/>
-      <c r="E24" s="130"/>
-      <c r="F24" s="130"/>
+      <c r="D24" s="145"/>
+      <c r="E24" s="146"/>
+      <c r="F24" s="146"/>
       <c r="G24" s="95"/>
       <c r="H24" s="96"/>
       <c r="I24" s="87"/>
@@ -3795,9 +3870,9 @@
       <c r="C25" s="87" t="s">
         <v>77</v>
       </c>
-      <c r="D25" s="121"/>
-      <c r="E25" s="122"/>
-      <c r="F25" s="123"/>
+      <c r="D25" s="154"/>
+      <c r="E25" s="155"/>
+      <c r="F25" s="156"/>
       <c r="G25" s="77"/>
       <c r="H25" s="77"/>
       <c r="I25" s="77"/>
@@ -3813,9 +3888,9 @@
       <c r="C26" s="87" t="s">
         <v>99</v>
       </c>
-      <c r="D26" s="121"/>
-      <c r="E26" s="122"/>
-      <c r="F26" s="123"/>
+      <c r="D26" s="154"/>
+      <c r="E26" s="155"/>
+      <c r="F26" s="156"/>
       <c r="G26" s="77"/>
       <c r="H26" s="77"/>
       <c r="I26" s="77"/>
@@ -3831,9 +3906,9 @@
       <c r="C27" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="121"/>
-      <c r="E27" s="122"/>
-      <c r="F27" s="123"/>
+      <c r="D27" s="154"/>
+      <c r="E27" s="155"/>
+      <c r="F27" s="156"/>
       <c r="G27" s="77"/>
       <c r="H27" s="77"/>
       <c r="I27" s="77"/>
@@ -3849,9 +3924,9 @@
       <c r="C28" s="77" t="s">
         <v>79</v>
       </c>
-      <c r="D28" s="121"/>
-      <c r="E28" s="122"/>
-      <c r="F28" s="123"/>
+      <c r="D28" s="154"/>
+      <c r="E28" s="155"/>
+      <c r="F28" s="156"/>
       <c r="G28" s="77"/>
       <c r="H28" s="77"/>
       <c r="I28" s="77"/>
@@ -3867,9 +3942,9 @@
       <c r="C29" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="121"/>
-      <c r="E29" s="122"/>
-      <c r="F29" s="123"/>
+      <c r="D29" s="154"/>
+      <c r="E29" s="155"/>
+      <c r="F29" s="156"/>
       <c r="G29" s="77"/>
       <c r="H29" s="77"/>
       <c r="I29" s="77"/>
@@ -3885,9 +3960,9 @@
       <c r="C30" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="D30" s="121"/>
-      <c r="E30" s="122"/>
-      <c r="F30" s="123"/>
+      <c r="D30" s="154"/>
+      <c r="E30" s="155"/>
+      <c r="F30" s="156"/>
       <c r="G30" s="77"/>
       <c r="H30" s="77"/>
       <c r="I30" s="77"/>
@@ -3903,9 +3978,9 @@
       <c r="C31" s="77" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="121"/>
-      <c r="E31" s="122"/>
-      <c r="F31" s="123"/>
+      <c r="D31" s="154"/>
+      <c r="E31" s="155"/>
+      <c r="F31" s="156"/>
       <c r="G31" s="77"/>
       <c r="H31" s="77"/>
       <c r="I31" s="77"/>
@@ -3921,20 +3996,20 @@
       <c r="C32" s="77" t="s">
         <v>101</v>
       </c>
-      <c r="D32" s="121"/>
-      <c r="E32" s="122"/>
-      <c r="F32" s="123"/>
+      <c r="D32" s="154"/>
+      <c r="E32" s="155"/>
+      <c r="F32" s="156"/>
       <c r="G32" s="77"/>
       <c r="H32" s="77"/>
       <c r="I32" s="77"/>
       <c r="J32" s="75"/>
     </row>
     <row r="33" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A33" s="124" t="s">
+      <c r="A33" s="119" t="s">
         <v>81</v>
       </c>
-      <c r="B33" s="125"/>
-      <c r="C33" s="125"/>
+      <c r="B33" s="120"/>
+      <c r="C33" s="120"/>
       <c r="D33" s="98"/>
       <c r="E33" s="98"/>
       <c r="F33" s="98"/>
@@ -3953,20 +4028,20 @@
       <c r="C34" s="77" t="s">
         <v>84</v>
       </c>
-      <c r="D34" s="126"/>
-      <c r="E34" s="127"/>
-      <c r="F34" s="127"/>
+      <c r="D34" s="121"/>
+      <c r="E34" s="122"/>
+      <c r="F34" s="122"/>
       <c r="G34" s="76"/>
       <c r="H34" s="83"/>
       <c r="I34" s="77"/>
       <c r="J34" s="75"/>
     </row>
     <row r="35" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A35" s="124" t="s">
+      <c r="A35" s="119" t="s">
         <v>82</v>
       </c>
-      <c r="B35" s="125"/>
-      <c r="C35" s="125"/>
+      <c r="B35" s="120"/>
+      <c r="C35" s="120"/>
       <c r="D35" s="98"/>
       <c r="E35" s="98"/>
       <c r="F35" s="98"/>
@@ -3985,9 +4060,9 @@
       <c r="C36" s="77" t="s">
         <v>145</v>
       </c>
-      <c r="D36" s="126"/>
-      <c r="E36" s="127"/>
-      <c r="F36" s="127"/>
+      <c r="D36" s="121"/>
+      <c r="E36" s="122"/>
+      <c r="F36" s="122"/>
       <c r="G36" s="76"/>
       <c r="H36" s="83"/>
       <c r="I36" s="77"/>
@@ -4003,9 +4078,9 @@
       <c r="C37" s="77" t="s">
         <v>147</v>
       </c>
-      <c r="D37" s="126"/>
-      <c r="E37" s="127"/>
-      <c r="F37" s="127"/>
+      <c r="D37" s="121"/>
+      <c r="E37" s="122"/>
+      <c r="F37" s="122"/>
       <c r="G37" s="76"/>
       <c r="H37" s="83"/>
       <c r="I37" s="77"/>
@@ -4021,9 +4096,9 @@
       <c r="C38" s="77" t="s">
         <v>146</v>
       </c>
-      <c r="D38" s="126"/>
-      <c r="E38" s="127"/>
-      <c r="F38" s="127"/>
+      <c r="D38" s="121"/>
+      <c r="E38" s="122"/>
+      <c r="F38" s="122"/>
       <c r="G38" s="76"/>
       <c r="H38" s="83"/>
       <c r="I38" s="77"/>
@@ -4039,9 +4114,9 @@
       <c r="C39" s="77" t="s">
         <v>149</v>
       </c>
-      <c r="D39" s="126"/>
-      <c r="E39" s="127"/>
-      <c r="F39" s="127"/>
+      <c r="D39" s="121"/>
+      <c r="E39" s="122"/>
+      <c r="F39" s="122"/>
       <c r="G39" s="76"/>
       <c r="H39" s="83"/>
       <c r="I39" s="77"/>
@@ -4057,20 +4132,20 @@
       <c r="C40" s="77" t="s">
         <v>151</v>
       </c>
-      <c r="D40" s="126"/>
-      <c r="E40" s="127"/>
-      <c r="F40" s="127"/>
+      <c r="D40" s="121"/>
+      <c r="E40" s="122"/>
+      <c r="F40" s="122"/>
       <c r="G40" s="76"/>
       <c r="H40" s="83"/>
       <c r="I40" s="77"/>
       <c r="J40" s="75"/>
     </row>
     <row r="41" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A41" s="124" t="s">
+      <c r="A41" s="119" t="s">
         <v>120</v>
       </c>
-      <c r="B41" s="125"/>
-      <c r="C41" s="125"/>
+      <c r="B41" s="120"/>
+      <c r="C41" s="120"/>
       <c r="D41" s="98"/>
       <c r="E41" s="98"/>
       <c r="F41" s="98"/>
@@ -4089,9 +4164,9 @@
       <c r="C42" s="77" t="s">
         <v>127</v>
       </c>
-      <c r="D42" s="126"/>
-      <c r="E42" s="127"/>
-      <c r="F42" s="127"/>
+      <c r="D42" s="121"/>
+      <c r="E42" s="122"/>
+      <c r="F42" s="122"/>
       <c r="G42" s="76"/>
       <c r="H42" s="83"/>
       <c r="I42" s="77"/>
@@ -4107,9 +4182,9 @@
       <c r="C43" s="77" t="s">
         <v>128</v>
       </c>
-      <c r="D43" s="126"/>
-      <c r="E43" s="127"/>
-      <c r="F43" s="127"/>
+      <c r="D43" s="121"/>
+      <c r="E43" s="122"/>
+      <c r="F43" s="122"/>
       <c r="G43" s="76"/>
       <c r="H43" s="83"/>
       <c r="I43" s="77"/>
@@ -4125,9 +4200,9 @@
       <c r="C44" s="77" t="s">
         <v>129</v>
       </c>
-      <c r="D44" s="126"/>
-      <c r="E44" s="127"/>
-      <c r="F44" s="127"/>
+      <c r="D44" s="121"/>
+      <c r="E44" s="122"/>
+      <c r="F44" s="122"/>
       <c r="G44" s="76"/>
       <c r="H44" s="83"/>
       <c r="I44" s="77"/>
@@ -4143,9 +4218,9 @@
       <c r="C45" s="77" t="s">
         <v>130</v>
       </c>
-      <c r="D45" s="126"/>
-      <c r="E45" s="127"/>
-      <c r="F45" s="127"/>
+      <c r="D45" s="121"/>
+      <c r="E45" s="122"/>
+      <c r="F45" s="122"/>
       <c r="G45" s="76"/>
       <c r="H45" s="83"/>
       <c r="I45" s="77"/>
@@ -4161,9 +4236,9 @@
       <c r="C46" s="77" t="s">
         <v>132</v>
       </c>
-      <c r="D46" s="126"/>
-      <c r="E46" s="127"/>
-      <c r="F46" s="127"/>
+      <c r="D46" s="121"/>
+      <c r="E46" s="122"/>
+      <c r="F46" s="122"/>
       <c r="G46" s="76"/>
       <c r="H46" s="83"/>
       <c r="I46" s="77"/>
@@ -4179,20 +4254,20 @@
       <c r="C47" s="77" t="s">
         <v>124</v>
       </c>
-      <c r="D47" s="126"/>
-      <c r="E47" s="127"/>
-      <c r="F47" s="127"/>
+      <c r="D47" s="121"/>
+      <c r="E47" s="122"/>
+      <c r="F47" s="122"/>
       <c r="G47" s="76"/>
       <c r="H47" s="83"/>
       <c r="I47" s="77"/>
       <c r="J47" s="75"/>
     </row>
     <row r="48" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A48" s="124" t="s">
+      <c r="A48" s="119" t="s">
         <v>133</v>
       </c>
-      <c r="B48" s="125"/>
-      <c r="C48" s="125"/>
+      <c r="B48" s="120"/>
+      <c r="C48" s="120"/>
       <c r="D48" s="98"/>
       <c r="E48" s="98"/>
       <c r="F48" s="98"/>
@@ -4211,18 +4286,18 @@
       <c r="C49" s="77" t="s">
         <v>134</v>
       </c>
-      <c r="D49" s="126"/>
-      <c r="E49" s="127"/>
-      <c r="F49" s="127"/>
+      <c r="D49" s="121"/>
+      <c r="E49" s="122"/>
+      <c r="F49" s="122"/>
       <c r="G49" s="76"/>
       <c r="H49" s="83"/>
       <c r="I49" s="77"/>
       <c r="J49" s="75"/>
     </row>
     <row r="50" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A50" s="124"/>
-      <c r="B50" s="125"/>
-      <c r="C50" s="125"/>
+      <c r="A50" s="119"/>
+      <c r="B50" s="120"/>
+      <c r="C50" s="120"/>
       <c r="D50" s="98"/>
       <c r="E50" s="98"/>
       <c r="F50" s="98"/>
@@ -4235,18 +4310,18 @@
       <c r="A51" s="78"/>
       <c r="B51" s="93"/>
       <c r="C51" s="77"/>
-      <c r="D51" s="126"/>
-      <c r="E51" s="127"/>
-      <c r="F51" s="127"/>
+      <c r="D51" s="121"/>
+      <c r="E51" s="122"/>
+      <c r="F51" s="122"/>
       <c r="G51" s="76"/>
       <c r="H51" s="83"/>
       <c r="I51" s="77"/>
       <c r="J51" s="75"/>
     </row>
     <row r="52" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A52" s="124"/>
-      <c r="B52" s="125"/>
-      <c r="C52" s="125"/>
+      <c r="A52" s="119"/>
+      <c r="B52" s="120"/>
+      <c r="C52" s="120"/>
       <c r="D52" s="98"/>
       <c r="E52" s="98"/>
       <c r="F52" s="98"/>
@@ -4259,18 +4334,18 @@
       <c r="A53" s="78"/>
       <c r="B53" s="93"/>
       <c r="C53" s="77"/>
-      <c r="D53" s="126"/>
-      <c r="E53" s="127"/>
-      <c r="F53" s="127"/>
+      <c r="D53" s="121"/>
+      <c r="E53" s="122"/>
+      <c r="F53" s="122"/>
       <c r="G53" s="76"/>
       <c r="H53" s="83"/>
       <c r="I53" s="77"/>
       <c r="J53" s="75"/>
     </row>
     <row r="54" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A54" s="124"/>
-      <c r="B54" s="125"/>
-      <c r="C54" s="125"/>
+      <c r="A54" s="119"/>
+      <c r="B54" s="120"/>
+      <c r="C54" s="120"/>
       <c r="D54" s="98"/>
       <c r="E54" s="98"/>
       <c r="F54" s="98"/>
@@ -4283,18 +4358,18 @@
       <c r="A55" s="78"/>
       <c r="B55" s="93"/>
       <c r="C55" s="77"/>
-      <c r="D55" s="126"/>
-      <c r="E55" s="127"/>
-      <c r="F55" s="127"/>
+      <c r="D55" s="121"/>
+      <c r="E55" s="122"/>
+      <c r="F55" s="122"/>
       <c r="G55" s="76"/>
       <c r="H55" s="83"/>
       <c r="I55" s="77"/>
       <c r="J55" s="75"/>
     </row>
     <row r="56" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A56" s="124"/>
-      <c r="B56" s="125"/>
-      <c r="C56" s="125"/>
+      <c r="A56" s="119"/>
+      <c r="B56" s="120"/>
+      <c r="C56" s="120"/>
       <c r="D56" s="98"/>
       <c r="E56" s="98"/>
       <c r="F56" s="98"/>
@@ -4307,18 +4382,18 @@
       <c r="A57" s="78"/>
       <c r="B57" s="93"/>
       <c r="C57" s="77"/>
-      <c r="D57" s="126"/>
-      <c r="E57" s="127"/>
-      <c r="F57" s="127"/>
+      <c r="D57" s="121"/>
+      <c r="E57" s="122"/>
+      <c r="F57" s="122"/>
       <c r="G57" s="76"/>
       <c r="H57" s="83"/>
       <c r="I57" s="77"/>
       <c r="J57" s="75"/>
     </row>
     <row r="58" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A58" s="124"/>
-      <c r="B58" s="125"/>
-      <c r="C58" s="125"/>
+      <c r="A58" s="119"/>
+      <c r="B58" s="120"/>
+      <c r="C58" s="120"/>
       <c r="D58" s="98"/>
       <c r="E58" s="98"/>
       <c r="F58" s="98"/>
@@ -4331,18 +4406,18 @@
       <c r="A59" s="78"/>
       <c r="B59" s="93"/>
       <c r="C59" s="77"/>
-      <c r="D59" s="126"/>
-      <c r="E59" s="127"/>
-      <c r="F59" s="127"/>
+      <c r="D59" s="121"/>
+      <c r="E59" s="122"/>
+      <c r="F59" s="122"/>
       <c r="G59" s="76"/>
       <c r="H59" s="83"/>
       <c r="I59" s="77"/>
       <c r="J59" s="75"/>
     </row>
     <row r="60" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A60" s="124"/>
-      <c r="B60" s="125"/>
-      <c r="C60" s="125"/>
+      <c r="A60" s="119"/>
+      <c r="B60" s="120"/>
+      <c r="C60" s="120"/>
       <c r="D60" s="98"/>
       <c r="E60" s="98"/>
       <c r="F60" s="98"/>
@@ -4355,18 +4430,18 @@
       <c r="A61" s="78"/>
       <c r="B61" s="93"/>
       <c r="C61" s="77"/>
-      <c r="D61" s="126"/>
-      <c r="E61" s="127"/>
-      <c r="F61" s="127"/>
+      <c r="D61" s="121"/>
+      <c r="E61" s="122"/>
+      <c r="F61" s="122"/>
       <c r="G61" s="76"/>
       <c r="H61" s="83"/>
       <c r="I61" s="77"/>
       <c r="J61" s="75"/>
     </row>
     <row r="62" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A62" s="124"/>
-      <c r="B62" s="125"/>
-      <c r="C62" s="125"/>
+      <c r="A62" s="119"/>
+      <c r="B62" s="120"/>
+      <c r="C62" s="120"/>
       <c r="D62" s="98"/>
       <c r="E62" s="98"/>
       <c r="F62" s="98"/>
@@ -4379,9 +4454,9 @@
       <c r="A63" s="78"/>
       <c r="B63" s="93"/>
       <c r="C63" s="77"/>
-      <c r="D63" s="126"/>
-      <c r="E63" s="127"/>
-      <c r="F63" s="127"/>
+      <c r="D63" s="121"/>
+      <c r="E63" s="122"/>
+      <c r="F63" s="122"/>
       <c r="G63" s="76"/>
       <c r="H63" s="83"/>
       <c r="I63" s="77"/>
@@ -4517,6 +4592,60 @@
     </row>
   </sheetData>
   <mergeCells count="70">
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:G10"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="B1:D2"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="D53:F53"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="D47:F47"/>
     <mergeCell ref="A60:C60"/>
     <mergeCell ref="D61:F61"/>
     <mergeCell ref="A62:C62"/>
@@ -4533,60 +4662,6 @@
     <mergeCell ref="D59:F59"/>
     <mergeCell ref="A50:C50"/>
     <mergeCell ref="D51:F51"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="D53:F53"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="B1:D2"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:G10"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D18:F18"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4602,8 +4677,8 @@
   </sheetPr>
   <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="82" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="A13" zoomScale="82" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" outlineLevelRow="1"/>
@@ -4622,9 +4697,9 @@
       <c r="A1" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="140"/>
-      <c r="C1" s="140"/>
-      <c r="D1" s="140"/>
+      <c r="B1" s="123"/>
+      <c r="C1" s="123"/>
+      <c r="D1" s="123"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -4635,9 +4710,9 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="141"/>
-      <c r="C2" s="141"/>
-      <c r="D2" s="141"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="124"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -4658,43 +4733,43 @@
       <c r="E3" s="61"/>
       <c r="F3" s="61"/>
       <c r="G3" s="61"/>
-      <c r="H3" s="148"/>
-      <c r="I3" s="148"/>
-      <c r="J3" s="148"/>
+      <c r="H3" s="133"/>
+      <c r="I3" s="133"/>
+      <c r="J3" s="133"/>
       <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="12.75">
       <c r="A4" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="149" t="s">
+      <c r="B4" s="135" t="s">
         <v>158</v>
       </c>
-      <c r="C4" s="150"/>
-      <c r="D4" s="151"/>
+      <c r="C4" s="136"/>
+      <c r="D4" s="137"/>
       <c r="E4" s="61"/>
       <c r="F4" s="61"/>
       <c r="G4" s="61"/>
-      <c r="H4" s="148"/>
-      <c r="I4" s="148"/>
-      <c r="J4" s="148"/>
+      <c r="H4" s="133"/>
+      <c r="I4" s="133"/>
+      <c r="J4" s="133"/>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" s="71" customFormat="1" ht="25.5">
       <c r="A5" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="143" t="s">
+      <c r="B5" s="126" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="144"/>
-      <c r="D5" s="145"/>
+      <c r="C5" s="127"/>
+      <c r="D5" s="128"/>
       <c r="E5" s="69"/>
       <c r="F5" s="69"/>
       <c r="G5" s="69"/>
-      <c r="H5" s="147"/>
-      <c r="I5" s="147"/>
-      <c r="J5" s="147"/>
+      <c r="H5" s="132"/>
+      <c r="I5" s="132"/>
+      <c r="J5" s="132"/>
       <c r="K5" s="70"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
@@ -4715,9 +4790,9 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="148"/>
-      <c r="I6" s="148"/>
-      <c r="J6" s="148"/>
+      <c r="H6" s="133"/>
+      <c r="I6" s="133"/>
+      <c r="J6" s="133"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -4733,21 +4808,21 @@
       </c>
       <c r="D7" s="59">
         <f>COUNTA(A12:A36) -3</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E7" s="62"/>
       <c r="F7" s="62"/>
       <c r="G7" s="62"/>
-      <c r="H7" s="148"/>
-      <c r="I7" s="148"/>
-      <c r="J7" s="148"/>
+      <c r="H7" s="133"/>
+      <c r="I7" s="133"/>
+      <c r="J7" s="133"/>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="142"/>
-      <c r="B8" s="142"/>
-      <c r="C8" s="142"/>
-      <c r="D8" s="142"/>
+      <c r="A8" s="125"/>
+      <c r="B8" s="125"/>
+      <c r="C8" s="125"/>
+      <c r="D8" s="125"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -4757,102 +4832,126 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" s="73" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="131" t="s">
+      <c r="A9" s="142" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="155" t="s">
+      <c r="B9" s="143" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="131" t="s">
+      <c r="C9" s="142" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="132" t="s">
+      <c r="D9" s="149" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="133"/>
-      <c r="F9" s="133"/>
-      <c r="G9" s="134"/>
-      <c r="H9" s="152" t="s">
+      <c r="E9" s="150"/>
+      <c r="F9" s="150"/>
+      <c r="G9" s="151"/>
+      <c r="H9" s="138" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="128" t="s">
+      <c r="I9" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="128" t="s">
+      <c r="J9" s="134" t="s">
         <v>32</v>
       </c>
       <c r="K9" s="72"/>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="128"/>
-      <c r="B10" s="156"/>
-      <c r="C10" s="128"/>
-      <c r="D10" s="135"/>
-      <c r="E10" s="136"/>
-      <c r="F10" s="136"/>
-      <c r="G10" s="137"/>
-      <c r="H10" s="135"/>
-      <c r="I10" s="128"/>
-      <c r="J10" s="128"/>
+      <c r="A10" s="134"/>
+      <c r="B10" s="144"/>
+      <c r="C10" s="134"/>
+      <c r="D10" s="139"/>
+      <c r="E10" s="152"/>
+      <c r="F10" s="152"/>
+      <c r="G10" s="153"/>
+      <c r="H10" s="139"/>
+      <c r="I10" s="134"/>
+      <c r="J10" s="134"/>
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" s="74" customFormat="1" ht="15">
-      <c r="A11" s="153"/>
-      <c r="B11" s="153"/>
-      <c r="C11" s="153"/>
-      <c r="D11" s="153"/>
-      <c r="E11" s="153"/>
-      <c r="F11" s="153"/>
-      <c r="G11" s="153"/>
-      <c r="H11" s="153"/>
-      <c r="I11" s="153"/>
-      <c r="J11" s="154"/>
+      <c r="A11" s="140"/>
+      <c r="B11" s="140"/>
+      <c r="C11" s="140"/>
+      <c r="D11" s="140"/>
+      <c r="E11" s="140"/>
+      <c r="F11" s="140"/>
+      <c r="G11" s="140"/>
+      <c r="H11" s="140"/>
+      <c r="I11" s="140"/>
+      <c r="J11" s="141"/>
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A12" s="138" t="s">
+      <c r="A12" s="129" t="s">
         <v>159</v>
       </c>
-      <c r="B12" s="139"/>
-      <c r="C12" s="139"/>
-      <c r="D12" s="139"/>
-      <c r="E12" s="139"/>
-      <c r="F12" s="139"/>
-      <c r="G12" s="139"/>
-      <c r="H12" s="139"/>
-      <c r="I12" s="139"/>
-      <c r="J12" s="146"/>
+      <c r="B12" s="130"/>
+      <c r="C12" s="130"/>
+      <c r="D12" s="130"/>
+      <c r="E12" s="130"/>
+      <c r="F12" s="130"/>
+      <c r="G12" s="130"/>
+      <c r="H12" s="130"/>
+      <c r="I12" s="130"/>
+      <c r="J12" s="131"/>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" ht="102.75" customHeight="1" outlineLevel="1">
-      <c r="A13" s="78"/>
-      <c r="B13" s="82"/>
-      <c r="C13" s="77"/>
-      <c r="D13" s="119"/>
-      <c r="E13" s="120"/>
-      <c r="F13" s="120"/>
+      <c r="A13" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="82" t="s">
+        <v>199</v>
+      </c>
+      <c r="C13" s="77" t="s">
+        <v>197</v>
+      </c>
+      <c r="D13" s="147" t="s">
+        <v>198</v>
+      </c>
+      <c r="E13" s="148"/>
+      <c r="F13" s="148"/>
       <c r="G13" s="76"/>
       <c r="H13" s="90"/>
       <c r="I13" s="77"/>
       <c r="J13" s="75"/>
     </row>
-    <row r="14" spans="1:11" s="4" customFormat="1" ht="57.75" customHeight="1" outlineLevel="1">
-      <c r="A14" s="78"/>
-      <c r="B14" s="82"/>
-      <c r="C14" s="77"/>
-      <c r="D14" s="119"/>
-      <c r="E14" s="120"/>
-      <c r="F14" s="120"/>
+    <row r="14" spans="1:11" s="4" customFormat="1" ht="107.25" customHeight="1" outlineLevel="1">
+      <c r="A14" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="82" t="s">
+        <v>200</v>
+      </c>
+      <c r="C14" s="77" t="s">
+        <v>201</v>
+      </c>
+      <c r="D14" s="147" t="s">
+        <v>202</v>
+      </c>
+      <c r="E14" s="148"/>
+      <c r="F14" s="148"/>
       <c r="G14" s="76"/>
       <c r="H14" s="90"/>
       <c r="I14" s="77"/>
       <c r="J14" s="75"/>
     </row>
-    <row r="15" spans="1:11" s="4" customFormat="1" ht="66.75" customHeight="1" outlineLevel="1">
-      <c r="A15" s="78"/>
-      <c r="B15" s="82"/>
-      <c r="C15" s="77"/>
-      <c r="D15" s="119"/>
-      <c r="E15" s="120"/>
-      <c r="F15" s="120"/>
+    <row r="15" spans="1:11" s="4" customFormat="1" ht="82.5" customHeight="1" outlineLevel="1">
+      <c r="A15" s="78" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="82" t="s">
+        <v>203</v>
+      </c>
+      <c r="C15" s="77" t="s">
+        <v>204</v>
+      </c>
+      <c r="D15" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="E15" s="148"/>
+      <c r="F15" s="148"/>
       <c r="G15" s="76"/>
       <c r="H15" s="90"/>
       <c r="I15" s="77"/>
@@ -4862,9 +4961,9 @@
       <c r="A16" s="78"/>
       <c r="B16" s="82"/>
       <c r="C16" s="77"/>
-      <c r="D16" s="119"/>
-      <c r="E16" s="120"/>
-      <c r="F16" s="120"/>
+      <c r="D16" s="147"/>
+      <c r="E16" s="148"/>
+      <c r="F16" s="148"/>
       <c r="G16" s="76"/>
       <c r="H16" s="90"/>
       <c r="I16" s="77"/>
@@ -4874,9 +4973,9 @@
       <c r="A17" s="78"/>
       <c r="B17" s="82"/>
       <c r="C17" s="77"/>
-      <c r="D17" s="119"/>
-      <c r="E17" s="120"/>
-      <c r="F17" s="120"/>
+      <c r="D17" s="147"/>
+      <c r="E17" s="148"/>
+      <c r="F17" s="148"/>
       <c r="G17" s="76"/>
       <c r="H17" s="90"/>
       <c r="I17" s="77"/>
@@ -4886,20 +4985,20 @@
       <c r="A18" s="78"/>
       <c r="B18" s="82"/>
       <c r="C18" s="77"/>
-      <c r="D18" s="119"/>
-      <c r="E18" s="120"/>
-      <c r="F18" s="120"/>
+      <c r="D18" s="147"/>
+      <c r="E18" s="148"/>
+      <c r="F18" s="148"/>
       <c r="G18" s="76"/>
       <c r="H18" s="90"/>
       <c r="I18" s="77"/>
       <c r="J18" s="75"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A19" s="138" t="s">
+      <c r="A19" s="129" t="s">
         <v>160</v>
       </c>
-      <c r="B19" s="139"/>
-      <c r="C19" s="139"/>
+      <c r="B19" s="130"/>
+      <c r="C19" s="130"/>
       <c r="D19" s="88"/>
       <c r="E19" s="88"/>
       <c r="F19" s="88"/>
@@ -4969,11 +5068,11 @@
       <c r="J22" s="97"/>
     </row>
     <row r="23" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A23" s="138" t="s">
+      <c r="A23" s="129" t="s">
         <v>177</v>
       </c>
-      <c r="B23" s="139"/>
-      <c r="C23" s="139"/>
+      <c r="B23" s="130"/>
+      <c r="C23" s="130"/>
       <c r="D23" s="88"/>
       <c r="E23" s="88"/>
       <c r="F23" s="88"/>
@@ -4992,11 +5091,11 @@
       <c r="C24" s="77" t="s">
         <v>181</v>
       </c>
-      <c r="D24" s="119" t="s">
+      <c r="D24" s="147" t="s">
         <v>179</v>
       </c>
-      <c r="E24" s="120"/>
-      <c r="F24" s="120"/>
+      <c r="E24" s="148"/>
+      <c r="F24" s="148"/>
       <c r="G24" s="76"/>
       <c r="H24" s="83"/>
       <c r="I24" s="77"/>
@@ -5012,11 +5111,11 @@
       <c r="C25" s="77" t="s">
         <v>182</v>
       </c>
-      <c r="D25" s="119" t="s">
+      <c r="D25" s="147" t="s">
         <v>183</v>
       </c>
-      <c r="E25" s="120"/>
-      <c r="F25" s="120"/>
+      <c r="E25" s="148"/>
+      <c r="F25" s="148"/>
       <c r="G25" s="76"/>
       <c r="H25" s="83"/>
       <c r="I25" s="77"/>
@@ -5032,11 +5131,11 @@
       <c r="C26" s="77" t="s">
         <v>185</v>
       </c>
-      <c r="D26" s="119" t="s">
+      <c r="D26" s="147" t="s">
         <v>186</v>
       </c>
-      <c r="E26" s="120"/>
-      <c r="F26" s="120"/>
+      <c r="E26" s="148"/>
+      <c r="F26" s="148"/>
       <c r="G26" s="76"/>
       <c r="H26" s="83"/>
       <c r="I26" s="77"/>
@@ -5052,20 +5151,20 @@
       <c r="C27" s="77" t="s">
         <v>188</v>
       </c>
-      <c r="D27" s="119" t="s">
+      <c r="D27" s="147" t="s">
         <v>189</v>
       </c>
-      <c r="E27" s="120"/>
-      <c r="F27" s="120"/>
+      <c r="E27" s="148"/>
+      <c r="F27" s="148"/>
       <c r="G27" s="76"/>
       <c r="H27" s="83"/>
       <c r="I27" s="77"/>
       <c r="J27" s="75"/>
     </row>
     <row r="28" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A28" s="124"/>
-      <c r="B28" s="125"/>
-      <c r="C28" s="125"/>
+      <c r="A28" s="119"/>
+      <c r="B28" s="120"/>
+      <c r="C28" s="120"/>
       <c r="D28" s="98"/>
       <c r="E28" s="98"/>
       <c r="F28" s="98"/>
@@ -5078,9 +5177,9 @@
       <c r="A29" s="78"/>
       <c r="B29" s="93"/>
       <c r="C29" s="77"/>
-      <c r="D29" s="126"/>
-      <c r="E29" s="127"/>
-      <c r="F29" s="127"/>
+      <c r="D29" s="121"/>
+      <c r="E29" s="122"/>
+      <c r="F29" s="122"/>
       <c r="G29" s="76"/>
       <c r="H29" s="83"/>
       <c r="I29" s="77"/>
@@ -5090,9 +5189,9 @@
       <c r="A30" s="78"/>
       <c r="B30" s="93"/>
       <c r="C30" s="77"/>
-      <c r="D30" s="126"/>
-      <c r="E30" s="127"/>
-      <c r="F30" s="127"/>
+      <c r="D30" s="121"/>
+      <c r="E30" s="122"/>
+      <c r="F30" s="122"/>
       <c r="G30" s="76"/>
       <c r="H30" s="83"/>
       <c r="I30" s="77"/>
@@ -5102,9 +5201,9 @@
       <c r="A31" s="78"/>
       <c r="B31" s="93"/>
       <c r="C31" s="77"/>
-      <c r="D31" s="126"/>
-      <c r="E31" s="127"/>
-      <c r="F31" s="127"/>
+      <c r="D31" s="121"/>
+      <c r="E31" s="122"/>
+      <c r="F31" s="122"/>
       <c r="G31" s="76"/>
       <c r="H31" s="83"/>
       <c r="I31" s="77"/>
@@ -5114,9 +5213,9 @@
       <c r="A32" s="78"/>
       <c r="B32" s="93"/>
       <c r="C32" s="77"/>
-      <c r="D32" s="126"/>
-      <c r="E32" s="127"/>
-      <c r="F32" s="127"/>
+      <c r="D32" s="121"/>
+      <c r="E32" s="122"/>
+      <c r="F32" s="122"/>
       <c r="G32" s="76"/>
       <c r="H32" s="83"/>
       <c r="I32" s="77"/>
@@ -5126,9 +5225,9 @@
       <c r="A33" s="78"/>
       <c r="B33" s="93"/>
       <c r="C33" s="77"/>
-      <c r="D33" s="126"/>
-      <c r="E33" s="127"/>
-      <c r="F33" s="127"/>
+      <c r="D33" s="121"/>
+      <c r="E33" s="122"/>
+      <c r="F33" s="122"/>
       <c r="G33" s="76"/>
       <c r="H33" s="83"/>
       <c r="I33" s="77"/>
@@ -5138,18 +5237,18 @@
       <c r="A34" s="78"/>
       <c r="B34" s="93"/>
       <c r="C34" s="77"/>
-      <c r="D34" s="126"/>
-      <c r="E34" s="127"/>
-      <c r="F34" s="127"/>
+      <c r="D34" s="121"/>
+      <c r="E34" s="122"/>
+      <c r="F34" s="122"/>
       <c r="G34" s="76"/>
       <c r="H34" s="83"/>
       <c r="I34" s="77"/>
       <c r="J34" s="75"/>
     </row>
     <row r="35" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A35" s="124"/>
-      <c r="B35" s="125"/>
-      <c r="C35" s="125"/>
+      <c r="A35" s="119"/>
+      <c r="B35" s="120"/>
+      <c r="C35" s="120"/>
       <c r="D35" s="98"/>
       <c r="E35" s="98"/>
       <c r="F35" s="98"/>
@@ -5162,9 +5261,9 @@
       <c r="A36" s="78"/>
       <c r="B36" s="93"/>
       <c r="C36" s="77"/>
-      <c r="D36" s="126"/>
-      <c r="E36" s="127"/>
-      <c r="F36" s="127"/>
+      <c r="D36" s="121"/>
+      <c r="E36" s="122"/>
+      <c r="F36" s="122"/>
       <c r="G36" s="76"/>
       <c r="H36" s="83"/>
       <c r="I36" s="77"/>
@@ -5300,26 +5399,13 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="B1:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="H4:J4"/>
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="H6:J6"/>
     <mergeCell ref="H7:J7"/>
@@ -5336,13 +5422,26 @@
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="D14:F14"/>
     <mergeCell ref="D15:F15"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="B1:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5494,7 +5593,7 @@
       </c>
       <c r="G9" s="67">
         <f>Samples2!D7</f>
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.25">
@@ -5526,7 +5625,7 @@
       </c>
       <c r="G11" s="55">
         <f>SUM(G6:G10)</f>
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14.25">

</xml_diff>

<commit_message>
up tc nhac nho tu dong
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University_IT\Tam\KiemThuPhanMem\event-manager-javafx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3316CDB-F35D-4F62-A5BC-04DA0FA7B104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703563E2-1A91-4B2D-914E-1548C2C14D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9810" yWindow="465" windowWidth="10365" windowHeight="10155" tabRatio="821" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="821" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="97" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="281">
   <si>
     <t>TC1</t>
   </si>
@@ -1021,6 +1021,117 @@
   </si>
   <si>
     <t>Viết TC Kiểm tra chức năng gửi thông báo thay đổi thời gian sự kiện cho người tham gia trong thời gian không cho phép</t>
+  </si>
+  <si>
+    <t>2. Thông báo sự kiện hủy, hoàn tiền cho người tham gia</t>
+  </si>
+  <si>
+    <t>3. Nhắc nhở tự động trước ngày diễn ra sự kiện</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng nhắc nhở tự động mới điều chỉnh theo thời gian khi sự kiện bị thay đổi thời gian sau khi đã gửi nhắc nhở</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng tự động gửi nhắc nhở đến người tham gia trước 1 ngày sự kiện diễn ra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Đăng nhập với tư cách là admin
+2: Chọn sự kiện đã có sẵn với thời gian diễn ra là 8h ngày 10/5
+3: Chạy tự động gửi nhắc nhở vào 8h ngày 9/5
+4: Kiểm tra kênh thông báo của người tham gia
+5: Hệ thống tự động gửi nhắc nhở đúng thời gian và đầy đủ thông tin đến tất cả người tham gia
+</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng gửi thông báo thay đổi thời gian sự kiện và gửi nhắc nhở mới</t>
+  </si>
+  <si>
+    <t>1: Đăng nhập với tư cách là admin
+2: Chọn sự kiện đã có sẵn với thời gian diễn ra là 8h ngày 15/5
+3: Chạy tự động gửi nhắc nhở vào 8h ngày 14/5
+4: Hệ thống tự động gửi thông báo nhắc nhở
+5: Thay đổi thời gian sự kiện thành 9h ngày 17/5
+6: Chạy tự động gửi nhắc nhở vào 9h ngày 16/5
+7: Hệ thống gửi thông báo thay đổi thời gian cho tất cả người tham gia ngay lập tức
+8:  Hệ thống tự động gửi nhắc nhở mới đúng thời gian và đầy đủ thông tin đến tất cả người tham gia</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng nhắc nhở tự động không gửi nếu hủy sự kiện trước khi gửi nhắc nhở</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng gửi thông báo nếu hủy sự kiện trước khi gửi nhắc nhở</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng nhắc nhở tự động nếu hủy sự kiện sau khi đã gửi nhắc nhở</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Đăng nhập với tư cách là admin
+2: Chọn sự kiện đã có sẵn với thời gian diễn ra là 8h ngày 10/5
+3: Chạy tự động gửi nhắc nhở vào 8h ngày 9/5
+4: Hệ thống tự động gửi nhắc nhở đúng thời gian(8h ngày 9/5) và đầy đủ thông tin đến tất cả người tham gia 
+5: Hủy sự kiện lúc 10h ngày 9/5
+6:Hệ thống từ chối hủy, hiển thị thông báo lỗi không thể hủy đăng ký do đã quá thời hạn hủy và không gửi thêm nhắc nhở nào
+</t>
+  </si>
+  <si>
+    <t>7. Hủy sự kiện</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Đăng nhập với tư cách là admin
+2: Chọn sự kiện đã có sẵn với thời gian diễn ra là 8h ngày 10/5
+3: Chạy tự động gửi nhắc nhở vào 8h ngày 9/5
+4: Hệ thống tự động gửi nhắc nhở đúng thời gian(8h ngày 9/5) và đầy đủ thông tin đến tất cả người tham gia 
+5: Hủy sự kiện lúc 10h ngày 9/5
+6: Hệ thống từ chối hủy, hiển thị thông báo lỗi không thể hủy đăng ký do đã quá thời hạn hủy và không gửi thêm nhắc nhở nào
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kiểm tra chức năng hủy sự kiện sau khi đã gửi nhắc nhở </t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng hủy sự kiện trước khi gửi nhắc nhở và hệ thống không gửi nhắc nhở tự động</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Đăng nhập với tư cách là admin
+2: Chọn sự kiện đã có sẵn với thời gian diễn ra là 8h ngày 10/5
+3: Chạy tự động gửi nhắc nhở vào 8h ngày 9/5
+4: Hủy sự kiện thành công lúc 7h ngày 9/5
+5: Hệ thống Gửi thông báo hủy ngay lập tức đến tất cả người tham gia
+6: Hệ thống không gửi nhắc nhở đến tất cả người tham gia vào 8h ngày 9/5
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Đăng nhập với tư cách là admin
+2: Chọn sự kiện đã có sẵn với thời gian diễn ra là 8h ngày 10/5
+3: Chạy tự động gửi nhắc nhở vào 8h ngày 9/5
+4: Hủy sự kiện thành công lúc 7h ngày 9/5
+5: Hệ thống Gửi thông báo hủy ngay lập tức đến tất cả người tham gia
+5: Hệ thống không gửi nhắc nhở đến tất cả người tham gia vào 8h ngày 9/5
+</t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra chức năng tự động gửi nhắc nhở đến người tham gia trước 1 ngày sự kiện diễn ra</t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra chức năng nhắc nhở tự động mới điều chỉnh theo thời gian khi sự kiện bị thay đổi thời gian sau khi đã gửi nhắc nhở</t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra chức năng nhắc nhở tự động không gửi nếu hủy sự kiện trước khi gửi nhắc nhở</t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra chức năng nhắc nhở tự động nếu hủy sự kiện sau khi đã gửi nhắc nhở</t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra chức năng gửi thông báo thay đổi thời gian sự kiện và gửi nhắc nhở mới</t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra chức năng gửi thông báo nếu hủy sự kiện trước khi gửi nhắc nhở</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viết TC Kiểm tra chức năng hủy sự kiện sau khi đã gửi nhắc nhở </t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra chức năng hủy sự kiện trước khi gửi nhắc nhở và hệ thống không gửi nhắc nhở tự động</t>
   </si>
 </sst>
 </file>
@@ -2063,26 +2174,122 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2090,9 +2297,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2102,109 +2306,16 @@
     <xf numFmtId="0" fontId="15" fillId="5" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3921,10 +4032,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H120"/>
+  <dimension ref="A2:H119"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A87" zoomScale="85" workbookViewId="0">
-      <selection activeCell="E99" sqref="E99"/>
+    <sheetView showGridLines="0" topLeftCell="A94" zoomScale="85" workbookViewId="0">
+      <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -3991,11 +4102,11 @@
       <c r="B6" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="121" t="s">
+      <c r="C6" s="123" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="121"/>
-      <c r="E6" s="122"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="124"/>
       <c r="F6" s="108"/>
       <c r="G6" s="25"/>
     </row>
@@ -4004,11 +4115,11 @@
       <c r="B7" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="121" t="s">
+      <c r="C7" s="123" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="121"/>
-      <c r="E7" s="122"/>
+      <c r="D7" s="123"/>
+      <c r="E7" s="124"/>
       <c r="F7" s="108"/>
       <c r="G7" s="25"/>
     </row>
@@ -5469,75 +5580,139 @@
       <c r="G94" s="99"/>
       <c r="H94" s="105"/>
     </row>
-    <row r="95" spans="2:8" s="33" customFormat="1">
-      <c r="B95" s="118"/>
-      <c r="C95" s="119"/>
+    <row r="95" spans="2:8" s="33" customFormat="1" ht="38.25">
+      <c r="B95" s="118">
+        <v>45761</v>
+      </c>
+      <c r="C95" s="119" t="s">
+        <v>40</v>
+      </c>
       <c r="D95" s="99"/>
-      <c r="E95" s="104"/>
-      <c r="F95" s="120"/>
+      <c r="E95" s="104" t="s">
+        <v>273</v>
+      </c>
+      <c r="F95" s="110" t="s">
+        <v>44</v>
+      </c>
       <c r="G95" s="99"/>
       <c r="H95" s="105"/>
     </row>
-    <row r="96" spans="2:8" s="33" customFormat="1">
-      <c r="B96" s="118"/>
-      <c r="C96" s="119"/>
+    <row r="96" spans="2:8" s="33" customFormat="1" ht="51">
+      <c r="B96" s="118">
+        <v>45761</v>
+      </c>
+      <c r="C96" s="119" t="s">
+        <v>40</v>
+      </c>
       <c r="D96" s="99"/>
-      <c r="E96" s="104"/>
-      <c r="F96" s="120"/>
+      <c r="E96" s="104" t="s">
+        <v>274</v>
+      </c>
+      <c r="F96" s="110" t="s">
+        <v>44</v>
+      </c>
       <c r="G96" s="99"/>
       <c r="H96" s="105"/>
     </row>
-    <row r="97" spans="2:8" s="33" customFormat="1">
-      <c r="B97" s="118"/>
-      <c r="C97" s="119"/>
+    <row r="97" spans="2:8" s="33" customFormat="1" ht="38.25">
+      <c r="B97" s="118">
+        <v>45761</v>
+      </c>
+      <c r="C97" s="119" t="s">
+        <v>40</v>
+      </c>
       <c r="D97" s="99"/>
-      <c r="E97" s="104"/>
-      <c r="F97" s="120"/>
+      <c r="E97" s="104" t="s">
+        <v>275</v>
+      </c>
+      <c r="F97" s="110" t="s">
+        <v>44</v>
+      </c>
       <c r="G97" s="99"/>
       <c r="H97" s="105"/>
     </row>
-    <row r="98" spans="2:8" s="33" customFormat="1">
-      <c r="B98" s="118"/>
-      <c r="C98" s="119"/>
+    <row r="98" spans="2:8" s="33" customFormat="1" ht="38.25">
+      <c r="B98" s="118">
+        <v>45761</v>
+      </c>
+      <c r="C98" s="119" t="s">
+        <v>40</v>
+      </c>
       <c r="D98" s="99"/>
-      <c r="E98" s="104"/>
-      <c r="F98" s="120"/>
+      <c r="E98" s="104" t="s">
+        <v>276</v>
+      </c>
+      <c r="F98" s="110" t="s">
+        <v>44</v>
+      </c>
       <c r="G98" s="99"/>
       <c r="H98" s="105"/>
     </row>
-    <row r="99" spans="2:8" s="33" customFormat="1">
-      <c r="B99" s="118"/>
-      <c r="C99" s="119"/>
+    <row r="99" spans="2:8" s="33" customFormat="1" ht="38.25">
+      <c r="B99" s="118">
+        <v>45762</v>
+      </c>
+      <c r="C99" s="119" t="s">
+        <v>40</v>
+      </c>
       <c r="D99" s="99"/>
-      <c r="E99" s="104"/>
-      <c r="F99" s="120"/>
+      <c r="E99" s="104" t="s">
+        <v>277</v>
+      </c>
+      <c r="F99" s="110" t="s">
+        <v>44</v>
+      </c>
       <c r="G99" s="99"/>
       <c r="H99" s="105"/>
     </row>
-    <row r="100" spans="2:8" s="33" customFormat="1">
-      <c r="B100" s="118"/>
-      <c r="C100" s="119"/>
+    <row r="100" spans="2:8" s="33" customFormat="1" ht="25.5">
+      <c r="B100" s="118">
+        <v>45762</v>
+      </c>
+      <c r="C100" s="119" t="s">
+        <v>40</v>
+      </c>
       <c r="D100" s="99"/>
-      <c r="E100" s="104"/>
-      <c r="F100" s="120"/>
+      <c r="E100" s="104" t="s">
+        <v>278</v>
+      </c>
+      <c r="F100" s="110" t="s">
+        <v>44</v>
+      </c>
       <c r="G100" s="99"/>
       <c r="H100" s="105"/>
     </row>
-    <row r="101" spans="2:8" s="33" customFormat="1">
-      <c r="B101" s="118"/>
-      <c r="C101" s="119"/>
+    <row r="101" spans="2:8" s="33" customFormat="1" ht="25.5">
+      <c r="B101" s="118">
+        <v>45762</v>
+      </c>
+      <c r="C101" s="119" t="s">
+        <v>40</v>
+      </c>
       <c r="D101" s="99"/>
-      <c r="E101" s="104"/>
-      <c r="F101" s="120"/>
+      <c r="E101" s="104" t="s">
+        <v>279</v>
+      </c>
+      <c r="F101" s="110" t="s">
+        <v>44</v>
+      </c>
       <c r="G101" s="99"/>
       <c r="H101" s="105"/>
     </row>
-    <row r="102" spans="2:8" s="33" customFormat="1">
-      <c r="B102" s="118"/>
-      <c r="C102" s="119"/>
+    <row r="102" spans="2:8" s="33" customFormat="1" ht="38.25">
+      <c r="B102" s="118">
+        <v>45762</v>
+      </c>
+      <c r="C102" s="119" t="s">
+        <v>40</v>
+      </c>
       <c r="D102" s="99"/>
-      <c r="E102" s="104"/>
-      <c r="F102" s="120"/>
+      <c r="E102" s="104" t="s">
+        <v>280</v>
+      </c>
+      <c r="F102" s="110" t="s">
+        <v>44</v>
+      </c>
       <c r="G102" s="99"/>
       <c r="H102" s="105"/>
     </row>
@@ -5686,22 +5861,13 @@
       <c r="H118" s="105"/>
     </row>
     <row r="119" spans="2:8" s="33" customFormat="1">
-      <c r="B119" s="118"/>
-      <c r="C119" s="119"/>
-      <c r="D119" s="99"/>
-      <c r="E119" s="104"/>
-      <c r="F119" s="120"/>
-      <c r="G119" s="99"/>
-      <c r="H119" s="105"/>
-    </row>
-    <row r="120" spans="2:8" s="33" customFormat="1">
-      <c r="B120" s="107"/>
-      <c r="C120" s="106"/>
-      <c r="D120" s="42"/>
-      <c r="E120" s="103"/>
-      <c r="F120" s="111"/>
-      <c r="G120" s="42"/>
-      <c r="H120" s="43"/>
+      <c r="B119" s="107"/>
+      <c r="C119" s="106"/>
+      <c r="D119" s="42"/>
+      <c r="E119" s="103"/>
+      <c r="F119" s="111"/>
+      <c r="G119" s="42"/>
+      <c r="H119" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5718,7 +5884,7 @@
     <oddFooter>&amp;L&amp;"Tahoma,Regular"&amp;8 02ae-BM/PM/HDCV/FSOFT v1/0&amp;R&amp;"Tahoma,Regular"&amp;10&amp;P/&amp;N</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="C12:C28 C41 C34:C40 C42:C47 C48:C49 C51:C53 C50 C54:C57 C58:C60 C29:C33 C61:C83 C84:C92 C93:C94" numberStoredAsText="1"/>
+    <ignoredError sqref="C12:C28 C41 C34:C40 C42:C47 C48:C49 C51:C53 C50 C54:C57 C58:C60 C29:C33 C61:C83 C84:C92 C93:C94 C95:C102" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -5728,10 +5894,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K87"/>
+  <dimension ref="A1:K88"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="65" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView showGridLines="0" zoomScale="69" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" outlineLevelRow="1"/>
@@ -5750,9 +5916,9 @@
       <c r="A1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="144"/>
-      <c r="C1" s="144"/>
-      <c r="D1" s="144"/>
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -5763,9 +5929,9 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="145"/>
-      <c r="C2" s="145"/>
-      <c r="D2" s="145"/>
+      <c r="B2" s="139"/>
+      <c r="C2" s="139"/>
+      <c r="D2" s="139"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -5778,51 +5944,51 @@
       <c r="A3" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="121" t="s">
+      <c r="B3" s="123" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="121"/>
-      <c r="D3" s="122"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="124"/>
       <c r="E3" s="60"/>
       <c r="F3" s="60"/>
       <c r="G3" s="60"/>
-      <c r="H3" s="152"/>
-      <c r="I3" s="152"/>
-      <c r="J3" s="152"/>
+      <c r="H3" s="148"/>
+      <c r="I3" s="148"/>
+      <c r="J3" s="148"/>
       <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="12.75">
       <c r="A4" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="153" t="s">
+      <c r="B4" s="150" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="154"/>
-      <c r="D4" s="155"/>
+      <c r="C4" s="151"/>
+      <c r="D4" s="152"/>
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
       <c r="G4" s="60"/>
-      <c r="H4" s="152"/>
-      <c r="I4" s="152"/>
-      <c r="J4" s="152"/>
+      <c r="H4" s="148"/>
+      <c r="I4" s="148"/>
+      <c r="J4" s="148"/>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" s="70" customFormat="1" ht="25.5">
       <c r="A5" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="147" t="s">
+      <c r="B5" s="141" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="148"/>
-      <c r="D5" s="149"/>
+      <c r="C5" s="142"/>
+      <c r="D5" s="143"/>
       <c r="E5" s="68"/>
       <c r="F5" s="68"/>
       <c r="G5" s="68"/>
-      <c r="H5" s="151"/>
-      <c r="I5" s="151"/>
-      <c r="J5" s="151"/>
+      <c r="H5" s="147"/>
+      <c r="I5" s="147"/>
+      <c r="J5" s="147"/>
       <c r="K5" s="69"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
@@ -5837,15 +6003,15 @@
         <v>39</v>
       </c>
       <c r="D6" s="13">
-        <f>COUNTIF(I10:I752,"Pending")</f>
+        <f>COUNTIF(I10:I753,"Pending")</f>
         <v>0</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="152"/>
-      <c r="I6" s="152"/>
-      <c r="J6" s="152"/>
+      <c r="H6" s="148"/>
+      <c r="I6" s="148"/>
+      <c r="J6" s="148"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -5860,22 +6026,22 @@
         <v>28</v>
       </c>
       <c r="D7" s="58">
-        <f>COUNTA(A12:A51) -6</f>
-        <v>34</v>
+        <f>COUNTA(A12:A54) -7</f>
+        <v>36</v>
       </c>
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
       <c r="G7" s="61"/>
-      <c r="H7" s="152"/>
-      <c r="I7" s="152"/>
-      <c r="J7" s="152"/>
+      <c r="H7" s="148"/>
+      <c r="I7" s="148"/>
+      <c r="J7" s="148"/>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="146"/>
-      <c r="B8" s="146"/>
-      <c r="C8" s="146"/>
-      <c r="D8" s="146"/>
+      <c r="A8" s="140"/>
+      <c r="B8" s="140"/>
+      <c r="C8" s="140"/>
+      <c r="D8" s="140"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -5885,70 +6051,70 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" s="72" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="130" t="s">
+      <c r="A9" s="157" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="159" t="s">
+      <c r="B9" s="158" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="130" t="s">
+      <c r="C9" s="157" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="131" t="s">
+      <c r="D9" s="162" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="132"/>
-      <c r="F9" s="132"/>
-      <c r="G9" s="133"/>
-      <c r="H9" s="156" t="s">
+      <c r="E9" s="163"/>
+      <c r="F9" s="163"/>
+      <c r="G9" s="164"/>
+      <c r="H9" s="153" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="125" t="s">
+      <c r="I9" s="149" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="125" t="s">
+      <c r="J9" s="149" t="s">
         <v>32</v>
       </c>
       <c r="K9" s="71"/>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="125"/>
-      <c r="B10" s="160"/>
-      <c r="C10" s="125"/>
-      <c r="D10" s="134"/>
-      <c r="E10" s="135"/>
-      <c r="F10" s="135"/>
-      <c r="G10" s="136"/>
-      <c r="H10" s="134"/>
-      <c r="I10" s="125"/>
-      <c r="J10" s="125"/>
+      <c r="A10" s="149"/>
+      <c r="B10" s="159"/>
+      <c r="C10" s="149"/>
+      <c r="D10" s="154"/>
+      <c r="E10" s="165"/>
+      <c r="F10" s="165"/>
+      <c r="G10" s="166"/>
+      <c r="H10" s="154"/>
+      <c r="I10" s="149"/>
+      <c r="J10" s="149"/>
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" s="73" customFormat="1" ht="15">
-      <c r="A11" s="157"/>
-      <c r="B11" s="157"/>
-      <c r="C11" s="157"/>
-      <c r="D11" s="157"/>
-      <c r="E11" s="157"/>
-      <c r="F11" s="157"/>
-      <c r="G11" s="157"/>
-      <c r="H11" s="157"/>
-      <c r="I11" s="157"/>
-      <c r="J11" s="158"/>
+      <c r="A11" s="155"/>
+      <c r="B11" s="155"/>
+      <c r="C11" s="155"/>
+      <c r="D11" s="155"/>
+      <c r="E11" s="155"/>
+      <c r="F11" s="155"/>
+      <c r="G11" s="155"/>
+      <c r="H11" s="155"/>
+      <c r="I11" s="155"/>
+      <c r="J11" s="156"/>
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A12" s="137" t="s">
+      <c r="A12" s="144" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="138"/>
-      <c r="C12" s="138"/>
-      <c r="D12" s="138"/>
-      <c r="E12" s="138"/>
-      <c r="F12" s="138"/>
-      <c r="G12" s="138"/>
-      <c r="H12" s="138"/>
-      <c r="I12" s="138"/>
-      <c r="J12" s="150"/>
+      <c r="B12" s="145"/>
+      <c r="C12" s="145"/>
+      <c r="D12" s="145"/>
+      <c r="E12" s="145"/>
+      <c r="F12" s="145"/>
+      <c r="G12" s="145"/>
+      <c r="H12" s="145"/>
+      <c r="I12" s="145"/>
+      <c r="J12" s="146"/>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" ht="350.1" customHeight="1" outlineLevel="1">
       <c r="A13" s="77" t="s">
@@ -5960,9 +6126,9 @@
       <c r="C13" s="76" t="s">
         <v>200</v>
       </c>
-      <c r="D13" s="123"/>
-      <c r="E13" s="124"/>
-      <c r="F13" s="124"/>
+      <c r="D13" s="128"/>
+      <c r="E13" s="129"/>
+      <c r="F13" s="129"/>
       <c r="G13" s="75"/>
       <c r="H13" s="116">
         <v>45755</v>
@@ -5982,9 +6148,9 @@
       <c r="C14" s="76" t="s">
         <v>199</v>
       </c>
-      <c r="D14" s="123"/>
-      <c r="E14" s="124"/>
-      <c r="F14" s="124"/>
+      <c r="D14" s="128"/>
+      <c r="E14" s="129"/>
+      <c r="F14" s="129"/>
       <c r="G14" s="75"/>
       <c r="H14" s="116">
         <v>45755</v>
@@ -6004,9 +6170,9 @@
       <c r="C15" s="76" t="s">
         <v>198</v>
       </c>
-      <c r="D15" s="123"/>
-      <c r="E15" s="124"/>
-      <c r="F15" s="124"/>
+      <c r="D15" s="128"/>
+      <c r="E15" s="129"/>
+      <c r="F15" s="129"/>
       <c r="G15" s="75"/>
       <c r="H15" s="116">
         <v>45755</v>
@@ -6028,9 +6194,9 @@
       <c r="C16" s="76" t="s">
         <v>197</v>
       </c>
-      <c r="D16" s="123"/>
-      <c r="E16" s="124"/>
-      <c r="F16" s="124"/>
+      <c r="D16" s="128"/>
+      <c r="E16" s="129"/>
+      <c r="F16" s="129"/>
       <c r="G16" s="75"/>
       <c r="H16" s="116">
         <v>45755</v>
@@ -6050,9 +6216,9 @@
       <c r="C17" s="76" t="s">
         <v>196</v>
       </c>
-      <c r="D17" s="123"/>
-      <c r="E17" s="124"/>
-      <c r="F17" s="124"/>
+      <c r="D17" s="128"/>
+      <c r="E17" s="129"/>
+      <c r="F17" s="129"/>
       <c r="G17" s="75"/>
       <c r="H17" s="116">
         <v>45755</v>
@@ -6072,9 +6238,9 @@
       <c r="C18" s="86" t="s">
         <v>195</v>
       </c>
-      <c r="D18" s="123"/>
-      <c r="E18" s="124"/>
-      <c r="F18" s="124"/>
+      <c r="D18" s="128"/>
+      <c r="E18" s="129"/>
+      <c r="F18" s="129"/>
       <c r="G18" s="75"/>
       <c r="H18" s="116">
         <v>45755</v>
@@ -6096,9 +6262,9 @@
       <c r="C19" s="86" t="s">
         <v>194</v>
       </c>
-      <c r="D19" s="123"/>
-      <c r="E19" s="124"/>
-      <c r="F19" s="124"/>
+      <c r="D19" s="128"/>
+      <c r="E19" s="129"/>
+      <c r="F19" s="129"/>
       <c r="G19" s="75"/>
       <c r="H19" s="116">
         <v>45755</v>
@@ -6120,9 +6286,9 @@
       <c r="C20" s="76" t="s">
         <v>192</v>
       </c>
-      <c r="D20" s="123"/>
-      <c r="E20" s="124"/>
-      <c r="F20" s="124"/>
+      <c r="D20" s="128"/>
+      <c r="E20" s="129"/>
+      <c r="F20" s="129"/>
       <c r="G20" s="75"/>
       <c r="H20" s="116">
         <v>45755</v>
@@ -6144,9 +6310,9 @@
       <c r="C21" s="76" t="s">
         <v>191</v>
       </c>
-      <c r="D21" s="123"/>
-      <c r="E21" s="124"/>
-      <c r="F21" s="124"/>
+      <c r="D21" s="128"/>
+      <c r="E21" s="129"/>
+      <c r="F21" s="129"/>
       <c r="G21" s="75"/>
       <c r="H21" s="116">
         <v>45755</v>
@@ -6168,9 +6334,9 @@
       <c r="C22" s="86" t="s">
         <v>193</v>
       </c>
-      <c r="D22" s="123"/>
-      <c r="E22" s="124"/>
-      <c r="F22" s="124"/>
+      <c r="D22" s="128"/>
+      <c r="E22" s="129"/>
+      <c r="F22" s="129"/>
       <c r="G22" s="75"/>
       <c r="H22" s="116">
         <v>45755</v>
@@ -6183,11 +6349,11 @@
       </c>
     </row>
     <row r="23" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A23" s="137" t="s">
+      <c r="A23" s="144" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="138"/>
-      <c r="C23" s="138"/>
+      <c r="B23" s="145"/>
+      <c r="C23" s="145"/>
       <c r="D23" s="87"/>
       <c r="E23" s="87"/>
       <c r="F23" s="87"/>
@@ -6206,9 +6372,9 @@
       <c r="C24" s="86" t="s">
         <v>228</v>
       </c>
-      <c r="D24" s="128"/>
-      <c r="E24" s="129"/>
-      <c r="F24" s="129"/>
+      <c r="D24" s="160"/>
+      <c r="E24" s="161"/>
+      <c r="F24" s="161"/>
       <c r="G24" s="94"/>
       <c r="H24" s="115">
         <v>45756</v>
@@ -6228,9 +6394,9 @@
       <c r="C25" s="86" t="s">
         <v>227</v>
       </c>
-      <c r="D25" s="128"/>
-      <c r="E25" s="129"/>
-      <c r="F25" s="129"/>
+      <c r="D25" s="160"/>
+      <c r="E25" s="161"/>
+      <c r="F25" s="161"/>
       <c r="G25" s="94"/>
       <c r="H25" s="115">
         <v>45755</v>
@@ -6252,9 +6418,9 @@
       <c r="C26" s="86" t="s">
         <v>232</v>
       </c>
-      <c r="D26" s="139"/>
-      <c r="E26" s="140"/>
-      <c r="F26" s="140"/>
+      <c r="D26" s="134"/>
+      <c r="E26" s="135"/>
+      <c r="F26" s="135"/>
       <c r="G26" s="94"/>
       <c r="H26" s="115">
         <v>45756</v>
@@ -6274,9 +6440,9 @@
       <c r="C27" s="86" t="s">
         <v>233</v>
       </c>
-      <c r="D27" s="141"/>
-      <c r="E27" s="142"/>
-      <c r="F27" s="143"/>
+      <c r="D27" s="125"/>
+      <c r="E27" s="126"/>
+      <c r="F27" s="127"/>
       <c r="G27" s="94"/>
       <c r="H27" s="115">
         <v>45755</v>
@@ -6296,9 +6462,9 @@
       <c r="C28" s="86" t="s">
         <v>237</v>
       </c>
-      <c r="D28" s="141"/>
-      <c r="E28" s="142"/>
-      <c r="F28" s="143"/>
+      <c r="D28" s="125"/>
+      <c r="E28" s="126"/>
+      <c r="F28" s="127"/>
       <c r="G28" s="94"/>
       <c r="H28" s="115">
         <v>45756</v>
@@ -6320,9 +6486,9 @@
       <c r="C29" s="86" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="141"/>
-      <c r="E29" s="142"/>
-      <c r="F29" s="143"/>
+      <c r="D29" s="125"/>
+      <c r="E29" s="126"/>
+      <c r="F29" s="127"/>
       <c r="G29" s="94"/>
       <c r="H29" s="115">
         <v>45756</v>
@@ -6344,9 +6510,9 @@
       <c r="C30" s="86" t="s">
         <v>234</v>
       </c>
-      <c r="D30" s="141"/>
-      <c r="E30" s="142"/>
-      <c r="F30" s="143"/>
+      <c r="D30" s="125"/>
+      <c r="E30" s="126"/>
+      <c r="F30" s="127"/>
       <c r="G30" s="94"/>
       <c r="H30" s="115">
         <v>45755</v>
@@ -6366,9 +6532,9 @@
       <c r="C31" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="141"/>
-      <c r="E31" s="142"/>
-      <c r="F31" s="143"/>
+      <c r="D31" s="125"/>
+      <c r="E31" s="126"/>
+      <c r="F31" s="127"/>
       <c r="G31" s="94"/>
       <c r="H31" s="115">
         <v>45756</v>
@@ -6390,9 +6556,9 @@
       <c r="C32" s="86" t="s">
         <v>70</v>
       </c>
-      <c r="D32" s="141"/>
-      <c r="E32" s="142"/>
-      <c r="F32" s="143"/>
+      <c r="D32" s="125"/>
+      <c r="E32" s="126"/>
+      <c r="F32" s="127"/>
       <c r="G32" s="94"/>
       <c r="H32" s="115">
         <v>45756</v>
@@ -6414,9 +6580,9 @@
       <c r="C33" s="86" t="s">
         <v>241</v>
       </c>
-      <c r="D33" s="123"/>
-      <c r="E33" s="124"/>
-      <c r="F33" s="161"/>
+      <c r="D33" s="128"/>
+      <c r="E33" s="129"/>
+      <c r="F33" s="130"/>
       <c r="G33" s="94"/>
       <c r="H33" s="115">
         <v>45755</v>
@@ -6436,9 +6602,9 @@
       <c r="C34" s="86" t="s">
         <v>201</v>
       </c>
-      <c r="D34" s="162"/>
-      <c r="E34" s="163"/>
-      <c r="F34" s="164"/>
+      <c r="D34" s="131"/>
+      <c r="E34" s="132"/>
+      <c r="F34" s="133"/>
       <c r="G34" s="94"/>
       <c r="H34" s="115">
         <v>45755</v>
@@ -6449,11 +6615,11 @@
       <c r="J34" s="96"/>
     </row>
     <row r="35" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A35" s="137" t="s">
+      <c r="A35" s="144" t="s">
         <v>71</v>
       </c>
-      <c r="B35" s="138"/>
-      <c r="C35" s="138"/>
+      <c r="B35" s="145"/>
+      <c r="C35" s="145"/>
       <c r="D35" s="87"/>
       <c r="E35" s="87"/>
       <c r="F35" s="87"/>
@@ -6472,20 +6638,20 @@
       <c r="C36" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="D36" s="139"/>
-      <c r="E36" s="140"/>
-      <c r="F36" s="140"/>
+      <c r="D36" s="134"/>
+      <c r="E36" s="135"/>
+      <c r="F36" s="135"/>
       <c r="G36" s="75"/>
       <c r="H36" s="82"/>
       <c r="I36" s="76"/>
       <c r="J36" s="74"/>
     </row>
     <row r="37" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A37" s="126" t="s">
+      <c r="A37" s="136" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="127"/>
-      <c r="C37" s="127"/>
+      <c r="B37" s="137"/>
+      <c r="C37" s="137"/>
       <c r="D37" s="97"/>
       <c r="E37" s="97"/>
       <c r="F37" s="97"/>
@@ -6504,9 +6670,9 @@
       <c r="C38" s="76" t="s">
         <v>113</v>
       </c>
-      <c r="D38" s="139"/>
-      <c r="E38" s="140"/>
-      <c r="F38" s="140"/>
+      <c r="D38" s="134"/>
+      <c r="E38" s="135"/>
+      <c r="F38" s="135"/>
       <c r="G38" s="75"/>
       <c r="H38" s="82"/>
       <c r="I38" s="76"/>
@@ -6522,9 +6688,9 @@
       <c r="C39" s="76" t="s">
         <v>115</v>
       </c>
-      <c r="D39" s="139"/>
-      <c r="E39" s="140"/>
-      <c r="F39" s="140"/>
+      <c r="D39" s="134"/>
+      <c r="E39" s="135"/>
+      <c r="F39" s="135"/>
       <c r="G39" s="75"/>
       <c r="H39" s="82"/>
       <c r="I39" s="76"/>
@@ -6540,9 +6706,9 @@
       <c r="C40" s="76" t="s">
         <v>114</v>
       </c>
-      <c r="D40" s="139"/>
-      <c r="E40" s="140"/>
-      <c r="F40" s="140"/>
+      <c r="D40" s="134"/>
+      <c r="E40" s="135"/>
+      <c r="F40" s="135"/>
       <c r="G40" s="75"/>
       <c r="H40" s="82"/>
       <c r="I40" s="76"/>
@@ -6558,9 +6724,9 @@
       <c r="C41" s="76" t="s">
         <v>117</v>
       </c>
-      <c r="D41" s="139"/>
-      <c r="E41" s="140"/>
-      <c r="F41" s="140"/>
+      <c r="D41" s="134"/>
+      <c r="E41" s="135"/>
+      <c r="F41" s="135"/>
       <c r="G41" s="75"/>
       <c r="H41" s="82"/>
       <c r="I41" s="76"/>
@@ -6576,20 +6742,20 @@
       <c r="C42" s="76" t="s">
         <v>119</v>
       </c>
-      <c r="D42" s="139"/>
-      <c r="E42" s="140"/>
-      <c r="F42" s="140"/>
+      <c r="D42" s="134"/>
+      <c r="E42" s="135"/>
+      <c r="F42" s="135"/>
       <c r="G42" s="75"/>
       <c r="H42" s="82"/>
       <c r="I42" s="76"/>
       <c r="J42" s="74"/>
     </row>
     <row r="43" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A43" s="126" t="s">
+      <c r="A43" s="136" t="s">
         <v>88</v>
       </c>
-      <c r="B43" s="127"/>
-      <c r="C43" s="127"/>
+      <c r="B43" s="137"/>
+      <c r="C43" s="137"/>
       <c r="D43" s="97"/>
       <c r="E43" s="97"/>
       <c r="F43" s="97"/>
@@ -6608,9 +6774,9 @@
       <c r="C44" s="76" t="s">
         <v>95</v>
       </c>
-      <c r="D44" s="139"/>
-      <c r="E44" s="140"/>
-      <c r="F44" s="140"/>
+      <c r="D44" s="134"/>
+      <c r="E44" s="135"/>
+      <c r="F44" s="135"/>
       <c r="G44" s="75"/>
       <c r="H44" s="82"/>
       <c r="I44" s="76"/>
@@ -6626,9 +6792,9 @@
       <c r="C45" s="76" t="s">
         <v>96</v>
       </c>
-      <c r="D45" s="139"/>
-      <c r="E45" s="140"/>
-      <c r="F45" s="140"/>
+      <c r="D45" s="134"/>
+      <c r="E45" s="135"/>
+      <c r="F45" s="135"/>
       <c r="G45" s="75"/>
       <c r="H45" s="82"/>
       <c r="I45" s="76"/>
@@ -6644,9 +6810,9 @@
       <c r="C46" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="D46" s="139"/>
-      <c r="E46" s="140"/>
-      <c r="F46" s="140"/>
+      <c r="D46" s="134"/>
+      <c r="E46" s="135"/>
+      <c r="F46" s="135"/>
       <c r="G46" s="75"/>
       <c r="H46" s="82"/>
       <c r="I46" s="76"/>
@@ -6662,9 +6828,9 @@
       <c r="C47" s="76" t="s">
         <v>98</v>
       </c>
-      <c r="D47" s="139"/>
-      <c r="E47" s="140"/>
-      <c r="F47" s="140"/>
+      <c r="D47" s="134"/>
+      <c r="E47" s="135"/>
+      <c r="F47" s="135"/>
       <c r="G47" s="75"/>
       <c r="H47" s="82"/>
       <c r="I47" s="76"/>
@@ -6680,9 +6846,9 @@
       <c r="C48" s="76" t="s">
         <v>100</v>
       </c>
-      <c r="D48" s="139"/>
-      <c r="E48" s="140"/>
-      <c r="F48" s="140"/>
+      <c r="D48" s="134"/>
+      <c r="E48" s="135"/>
+      <c r="F48" s="135"/>
       <c r="G48" s="75"/>
       <c r="H48" s="82"/>
       <c r="I48" s="76"/>
@@ -6698,20 +6864,20 @@
       <c r="C49" s="76" t="s">
         <v>92</v>
       </c>
-      <c r="D49" s="139"/>
-      <c r="E49" s="140"/>
-      <c r="F49" s="140"/>
+      <c r="D49" s="134"/>
+      <c r="E49" s="135"/>
+      <c r="F49" s="135"/>
       <c r="G49" s="75"/>
       <c r="H49" s="82"/>
       <c r="I49" s="76"/>
       <c r="J49" s="74"/>
     </row>
     <row r="50" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A50" s="126" t="s">
+      <c r="A50" s="136" t="s">
         <v>101</v>
       </c>
-      <c r="B50" s="127"/>
-      <c r="C50" s="127"/>
+      <c r="B50" s="137"/>
+      <c r="C50" s="137"/>
       <c r="D50" s="97"/>
       <c r="E50" s="97"/>
       <c r="F50" s="97"/>
@@ -6730,18 +6896,20 @@
       <c r="C51" s="76" t="s">
         <v>102</v>
       </c>
-      <c r="D51" s="139"/>
-      <c r="E51" s="140"/>
-      <c r="F51" s="140"/>
+      <c r="D51" s="134"/>
+      <c r="E51" s="135"/>
+      <c r="F51" s="135"/>
       <c r="G51" s="75"/>
       <c r="H51" s="82"/>
       <c r="I51" s="76"/>
       <c r="J51" s="74"/>
     </row>
     <row r="52" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A52" s="126"/>
-      <c r="B52" s="127"/>
-      <c r="C52" s="127"/>
+      <c r="A52" s="136" t="s">
+        <v>267</v>
+      </c>
+      <c r="B52" s="137"/>
+      <c r="C52" s="137"/>
       <c r="D52" s="97"/>
       <c r="E52" s="97"/>
       <c r="F52" s="97"/>
@@ -6750,45 +6918,65 @@
       <c r="I52" s="97"/>
       <c r="J52" s="98"/>
     </row>
-    <row r="53" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
-      <c r="A53" s="77"/>
-      <c r="B53" s="92"/>
-      <c r="C53" s="76"/>
-      <c r="D53" s="139"/>
-      <c r="E53" s="140"/>
-      <c r="F53" s="140"/>
+    <row r="53" spans="1:10" s="4" customFormat="1" ht="144" customHeight="1" outlineLevel="1">
+      <c r="A53" s="77" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="92" t="s">
+        <v>269</v>
+      </c>
+      <c r="C53" s="76" t="s">
+        <v>266</v>
+      </c>
+      <c r="D53" s="134"/>
+      <c r="E53" s="135"/>
+      <c r="F53" s="135"/>
       <c r="G53" s="75"/>
       <c r="H53" s="82"/>
       <c r="I53" s="76"/>
       <c r="J53" s="74"/>
     </row>
-    <row r="54" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A54" s="126"/>
-      <c r="B54" s="127"/>
-      <c r="C54" s="127"/>
-      <c r="D54" s="97"/>
-      <c r="E54" s="97"/>
-      <c r="F54" s="97"/>
-      <c r="G54" s="97"/>
-      <c r="H54" s="97"/>
-      <c r="I54" s="97"/>
-      <c r="J54" s="98"/>
-    </row>
-    <row r="55" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
-      <c r="A55" s="77"/>
-      <c r="B55" s="92"/>
-      <c r="C55" s="76"/>
-      <c r="D55" s="139"/>
-      <c r="E55" s="140"/>
-      <c r="F55" s="140"/>
-      <c r="G55" s="75"/>
-      <c r="H55" s="82"/>
-      <c r="I55" s="76"/>
-      <c r="J55" s="74"/>
-    </row>
-    <row r="56" spans="1:10" ht="12" customHeight="1">
-      <c r="I56"/>
-      <c r="J56"/>
+    <row r="54" spans="1:10" s="4" customFormat="1" ht="123" customHeight="1" outlineLevel="1">
+      <c r="A54" s="77" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54" s="92" t="s">
+        <v>270</v>
+      </c>
+      <c r="C54" s="76" t="s">
+        <v>271</v>
+      </c>
+      <c r="D54" s="134"/>
+      <c r="E54" s="135"/>
+      <c r="F54" s="135"/>
+      <c r="G54" s="75"/>
+      <c r="H54" s="82"/>
+      <c r="I54" s="76"/>
+      <c r="J54" s="74"/>
+    </row>
+    <row r="55" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
+      <c r="A55" s="136"/>
+      <c r="B55" s="137"/>
+      <c r="C55" s="137"/>
+      <c r="D55" s="97"/>
+      <c r="E55" s="97"/>
+      <c r="F55" s="97"/>
+      <c r="G55" s="97"/>
+      <c r="H55" s="97"/>
+      <c r="I55" s="97"/>
+      <c r="J55" s="98"/>
+    </row>
+    <row r="56" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A56" s="77"/>
+      <c r="B56" s="92"/>
+      <c r="C56" s="76"/>
+      <c r="D56" s="134"/>
+      <c r="E56" s="135"/>
+      <c r="F56" s="135"/>
+      <c r="G56" s="75"/>
+      <c r="H56" s="82"/>
+      <c r="I56" s="76"/>
+      <c r="J56" s="74"/>
     </row>
     <row r="57" spans="1:10" ht="12" customHeight="1">
       <c r="I57"/>
@@ -6850,8 +7038,8 @@
       <c r="I71"/>
       <c r="J71"/>
     </row>
-    <row r="72" spans="9:10">
-      <c r="I72" s="19"/>
+    <row r="72" spans="9:10" ht="12" customHeight="1">
+      <c r="I72"/>
       <c r="J72"/>
     </row>
     <row r="73" spans="9:10">
@@ -6914,33 +7102,33 @@
       <c r="I87" s="19"/>
       <c r="J87"/>
     </row>
+    <row r="88" spans="9:10">
+      <c r="I88" s="19"/>
+      <c r="J88"/>
+    </row>
   </sheetData>
-  <mergeCells count="62">
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="D53:F53"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="D55:F55"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="D51:F51"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="D48:F48"/>
+  <mergeCells count="63">
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:G10"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D22:F22"/>
     <mergeCell ref="B1:D2"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="B5:D5"/>
@@ -6957,27 +7145,32 @@
     <mergeCell ref="A11:J11"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:G10"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D56:F56"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="D51:F51"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="D53:F53"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="D54:F54"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6994,8 +7187,8 @@
   </sheetPr>
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="82" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="A18" zoomScale="82" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" outlineLevelRow="1"/>
@@ -7014,9 +7207,9 @@
       <c r="A1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="144"/>
-      <c r="C1" s="144"/>
-      <c r="D1" s="144"/>
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -7027,9 +7220,9 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="145"/>
-      <c r="C2" s="145"/>
-      <c r="D2" s="145"/>
+      <c r="B2" s="139"/>
+      <c r="C2" s="139"/>
+      <c r="D2" s="139"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -7042,51 +7235,51 @@
       <c r="A3" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="121" t="s">
+      <c r="B3" s="123" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="121"/>
-      <c r="D3" s="122"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="124"/>
       <c r="E3" s="60"/>
       <c r="F3" s="60"/>
       <c r="G3" s="60"/>
-      <c r="H3" s="152"/>
-      <c r="I3" s="152"/>
-      <c r="J3" s="152"/>
+      <c r="H3" s="148"/>
+      <c r="I3" s="148"/>
+      <c r="J3" s="148"/>
       <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="12.75">
       <c r="A4" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="153" t="s">
+      <c r="B4" s="150" t="s">
         <v>126</v>
       </c>
-      <c r="C4" s="154"/>
-      <c r="D4" s="155"/>
+      <c r="C4" s="151"/>
+      <c r="D4" s="152"/>
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
       <c r="G4" s="60"/>
-      <c r="H4" s="152"/>
-      <c r="I4" s="152"/>
-      <c r="J4" s="152"/>
+      <c r="H4" s="148"/>
+      <c r="I4" s="148"/>
+      <c r="J4" s="148"/>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" s="70" customFormat="1" ht="25.5">
       <c r="A5" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="147" t="s">
+      <c r="B5" s="141" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="148"/>
-      <c r="D5" s="149"/>
+      <c r="C5" s="142"/>
+      <c r="D5" s="143"/>
       <c r="E5" s="68"/>
       <c r="F5" s="68"/>
       <c r="G5" s="68"/>
-      <c r="H5" s="151"/>
-      <c r="I5" s="151"/>
-      <c r="J5" s="151"/>
+      <c r="H5" s="147"/>
+      <c r="I5" s="147"/>
+      <c r="J5" s="147"/>
       <c r="K5" s="69"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
@@ -7107,9 +7300,9 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="152"/>
-      <c r="I6" s="152"/>
-      <c r="J6" s="152"/>
+      <c r="H6" s="148"/>
+      <c r="I6" s="148"/>
+      <c r="J6" s="148"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -7130,16 +7323,16 @@
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
       <c r="G7" s="61"/>
-      <c r="H7" s="152"/>
-      <c r="I7" s="152"/>
-      <c r="J7" s="152"/>
+      <c r="H7" s="148"/>
+      <c r="I7" s="148"/>
+      <c r="J7" s="148"/>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="146"/>
-      <c r="B8" s="146"/>
-      <c r="C8" s="146"/>
-      <c r="D8" s="146"/>
+      <c r="A8" s="140"/>
+      <c r="B8" s="140"/>
+      <c r="C8" s="140"/>
+      <c r="D8" s="140"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -7149,70 +7342,70 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" s="72" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="130" t="s">
+      <c r="A9" s="157" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="159" t="s">
+      <c r="B9" s="158" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="130" t="s">
+      <c r="C9" s="157" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="131" t="s">
+      <c r="D9" s="162" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="132"/>
-      <c r="F9" s="132"/>
-      <c r="G9" s="133"/>
-      <c r="H9" s="156" t="s">
+      <c r="E9" s="163"/>
+      <c r="F9" s="163"/>
+      <c r="G9" s="164"/>
+      <c r="H9" s="153" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="125" t="s">
+      <c r="I9" s="149" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="125" t="s">
+      <c r="J9" s="149" t="s">
         <v>32</v>
       </c>
       <c r="K9" s="71"/>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="125"/>
-      <c r="B10" s="160"/>
-      <c r="C10" s="125"/>
-      <c r="D10" s="134"/>
-      <c r="E10" s="135"/>
-      <c r="F10" s="135"/>
-      <c r="G10" s="136"/>
-      <c r="H10" s="134"/>
-      <c r="I10" s="125"/>
-      <c r="J10" s="125"/>
+      <c r="A10" s="149"/>
+      <c r="B10" s="159"/>
+      <c r="C10" s="149"/>
+      <c r="D10" s="154"/>
+      <c r="E10" s="165"/>
+      <c r="F10" s="165"/>
+      <c r="G10" s="166"/>
+      <c r="H10" s="154"/>
+      <c r="I10" s="149"/>
+      <c r="J10" s="149"/>
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" s="73" customFormat="1" ht="15">
-      <c r="A11" s="157"/>
-      <c r="B11" s="157"/>
-      <c r="C11" s="157"/>
-      <c r="D11" s="157"/>
-      <c r="E11" s="157"/>
-      <c r="F11" s="157"/>
-      <c r="G11" s="157"/>
-      <c r="H11" s="157"/>
-      <c r="I11" s="157"/>
-      <c r="J11" s="158"/>
+      <c r="A11" s="155"/>
+      <c r="B11" s="155"/>
+      <c r="C11" s="155"/>
+      <c r="D11" s="155"/>
+      <c r="E11" s="155"/>
+      <c r="F11" s="155"/>
+      <c r="G11" s="155"/>
+      <c r="H11" s="155"/>
+      <c r="I11" s="155"/>
+      <c r="J11" s="156"/>
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A12" s="137" t="s">
+      <c r="A12" s="144" t="s">
         <v>127</v>
       </c>
-      <c r="B12" s="138"/>
-      <c r="C12" s="138"/>
-      <c r="D12" s="138"/>
-      <c r="E12" s="138"/>
-      <c r="F12" s="138"/>
-      <c r="G12" s="138"/>
-      <c r="H12" s="138"/>
-      <c r="I12" s="138"/>
-      <c r="J12" s="150"/>
+      <c r="B12" s="145"/>
+      <c r="C12" s="145"/>
+      <c r="D12" s="145"/>
+      <c r="E12" s="145"/>
+      <c r="F12" s="145"/>
+      <c r="G12" s="145"/>
+      <c r="H12" s="145"/>
+      <c r="I12" s="145"/>
+      <c r="J12" s="146"/>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" ht="102.75" customHeight="1" outlineLevel="1">
       <c r="A13" s="77" t="s">
@@ -7224,11 +7417,11 @@
       <c r="C13" s="76" t="s">
         <v>165</v>
       </c>
-      <c r="D13" s="123" t="s">
+      <c r="D13" s="128" t="s">
         <v>166</v>
       </c>
-      <c r="E13" s="124"/>
-      <c r="F13" s="124"/>
+      <c r="E13" s="129"/>
+      <c r="F13" s="129"/>
       <c r="G13" s="75"/>
       <c r="H13" s="89"/>
       <c r="I13" s="76"/>
@@ -7244,11 +7437,11 @@
       <c r="C14" s="76" t="s">
         <v>169</v>
       </c>
-      <c r="D14" s="123" t="s">
+      <c r="D14" s="128" t="s">
         <v>170</v>
       </c>
-      <c r="E14" s="124"/>
-      <c r="F14" s="124"/>
+      <c r="E14" s="129"/>
+      <c r="F14" s="129"/>
       <c r="G14" s="75"/>
       <c r="H14" s="89"/>
       <c r="I14" s="76"/>
@@ -7264,22 +7457,22 @@
       <c r="C15" s="76" t="s">
         <v>172</v>
       </c>
-      <c r="D15" s="123" t="s">
+      <c r="D15" s="128" t="s">
         <v>173</v>
       </c>
-      <c r="E15" s="124"/>
-      <c r="F15" s="124"/>
+      <c r="E15" s="129"/>
+      <c r="F15" s="129"/>
       <c r="G15" s="75"/>
       <c r="H15" s="89"/>
       <c r="I15" s="76"/>
       <c r="J15" s="74"/>
     </row>
     <row r="16" spans="1:11" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A16" s="137" t="s">
+      <c r="A16" s="144" t="s">
         <v>128</v>
       </c>
-      <c r="B16" s="138"/>
-      <c r="C16" s="138"/>
+      <c r="B16" s="145"/>
+      <c r="C16" s="145"/>
       <c r="D16" s="87"/>
       <c r="E16" s="87"/>
       <c r="F16" s="87"/>
@@ -7298,11 +7491,11 @@
       <c r="C17" s="86" t="s">
         <v>136</v>
       </c>
-      <c r="D17" s="165" t="s">
+      <c r="D17" s="167" t="s">
         <v>135</v>
       </c>
-      <c r="E17" s="166"/>
-      <c r="F17" s="166"/>
+      <c r="E17" s="168"/>
+      <c r="F17" s="168"/>
       <c r="G17" s="94"/>
       <c r="H17" s="95"/>
       <c r="I17" s="86"/>
@@ -7318,11 +7511,11 @@
       <c r="C18" s="86" t="s">
         <v>138</v>
       </c>
-      <c r="D18" s="165" t="s">
+      <c r="D18" s="167" t="s">
         <v>139</v>
       </c>
-      <c r="E18" s="166"/>
-      <c r="F18" s="166"/>
+      <c r="E18" s="168"/>
+      <c r="F18" s="168"/>
       <c r="G18" s="94"/>
       <c r="H18" s="95"/>
       <c r="I18" s="86"/>
@@ -7338,22 +7531,22 @@
       <c r="C19" s="86" t="s">
         <v>136</v>
       </c>
-      <c r="D19" s="165" t="s">
+      <c r="D19" s="167" t="s">
         <v>141</v>
       </c>
-      <c r="E19" s="166"/>
-      <c r="F19" s="166"/>
+      <c r="E19" s="168"/>
+      <c r="F19" s="168"/>
       <c r="G19" s="94"/>
       <c r="H19" s="95"/>
       <c r="I19" s="86"/>
       <c r="J19" s="96"/>
     </row>
     <row r="20" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A20" s="137" t="s">
+      <c r="A20" s="144" t="s">
         <v>145</v>
       </c>
-      <c r="B20" s="138"/>
-      <c r="C20" s="138"/>
+      <c r="B20" s="145"/>
+      <c r="C20" s="145"/>
       <c r="D20" s="87"/>
       <c r="E20" s="87"/>
       <c r="F20" s="87"/>
@@ -7372,11 +7565,11 @@
       <c r="C21" s="76" t="s">
         <v>149</v>
       </c>
-      <c r="D21" s="123" t="s">
+      <c r="D21" s="128" t="s">
         <v>147</v>
       </c>
-      <c r="E21" s="124"/>
-      <c r="F21" s="124"/>
+      <c r="E21" s="129"/>
+      <c r="F21" s="129"/>
       <c r="G21" s="75"/>
       <c r="H21" s="82"/>
       <c r="I21" s="76"/>
@@ -7392,11 +7585,11 @@
       <c r="C22" s="76" t="s">
         <v>150</v>
       </c>
-      <c r="D22" s="123" t="s">
+      <c r="D22" s="128" t="s">
         <v>151</v>
       </c>
-      <c r="E22" s="124"/>
-      <c r="F22" s="124"/>
+      <c r="E22" s="129"/>
+      <c r="F22" s="129"/>
       <c r="G22" s="75"/>
       <c r="H22" s="82"/>
       <c r="I22" s="76"/>
@@ -7412,11 +7605,11 @@
       <c r="C23" s="76" t="s">
         <v>153</v>
       </c>
-      <c r="D23" s="123" t="s">
+      <c r="D23" s="128" t="s">
         <v>154</v>
       </c>
-      <c r="E23" s="124"/>
-      <c r="F23" s="124"/>
+      <c r="E23" s="129"/>
+      <c r="F23" s="129"/>
       <c r="G23" s="75"/>
       <c r="H23" s="82"/>
       <c r="I23" s="76"/>
@@ -7432,20 +7625,20 @@
       <c r="C24" s="76" t="s">
         <v>156</v>
       </c>
-      <c r="D24" s="123" t="s">
+      <c r="D24" s="128" t="s">
         <v>157</v>
       </c>
-      <c r="E24" s="124"/>
-      <c r="F24" s="124"/>
+      <c r="E24" s="129"/>
+      <c r="F24" s="129"/>
       <c r="G24" s="75"/>
       <c r="H24" s="82"/>
       <c r="I24" s="76"/>
       <c r="J24" s="74"/>
     </row>
     <row r="25" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A25" s="126"/>
-      <c r="B25" s="127"/>
-      <c r="C25" s="127"/>
+      <c r="A25" s="136"/>
+      <c r="B25" s="137"/>
+      <c r="C25" s="137"/>
       <c r="D25" s="97"/>
       <c r="E25" s="97"/>
       <c r="F25" s="97"/>
@@ -7458,9 +7651,9 @@
       <c r="A26" s="77"/>
       <c r="B26" s="92"/>
       <c r="C26" s="76"/>
-      <c r="D26" s="139"/>
-      <c r="E26" s="140"/>
-      <c r="F26" s="140"/>
+      <c r="D26" s="134"/>
+      <c r="E26" s="135"/>
+      <c r="F26" s="135"/>
       <c r="G26" s="75"/>
       <c r="H26" s="82"/>
       <c r="I26" s="76"/>
@@ -7470,9 +7663,9 @@
       <c r="A27" s="77"/>
       <c r="B27" s="92"/>
       <c r="C27" s="76"/>
-      <c r="D27" s="139"/>
-      <c r="E27" s="140"/>
-      <c r="F27" s="140"/>
+      <c r="D27" s="134"/>
+      <c r="E27" s="135"/>
+      <c r="F27" s="135"/>
       <c r="G27" s="75"/>
       <c r="H27" s="82"/>
       <c r="I27" s="76"/>
@@ -7482,9 +7675,9 @@
       <c r="A28" s="77"/>
       <c r="B28" s="92"/>
       <c r="C28" s="76"/>
-      <c r="D28" s="139"/>
-      <c r="E28" s="140"/>
-      <c r="F28" s="140"/>
+      <c r="D28" s="134"/>
+      <c r="E28" s="135"/>
+      <c r="F28" s="135"/>
       <c r="G28" s="75"/>
       <c r="H28" s="82"/>
       <c r="I28" s="76"/>
@@ -7494,9 +7687,9 @@
       <c r="A29" s="77"/>
       <c r="B29" s="92"/>
       <c r="C29" s="76"/>
-      <c r="D29" s="139"/>
-      <c r="E29" s="140"/>
-      <c r="F29" s="140"/>
+      <c r="D29" s="134"/>
+      <c r="E29" s="135"/>
+      <c r="F29" s="135"/>
       <c r="G29" s="75"/>
       <c r="H29" s="82"/>
       <c r="I29" s="76"/>
@@ -7506,9 +7699,9 @@
       <c r="A30" s="77"/>
       <c r="B30" s="92"/>
       <c r="C30" s="76"/>
-      <c r="D30" s="139"/>
-      <c r="E30" s="140"/>
-      <c r="F30" s="140"/>
+      <c r="D30" s="134"/>
+      <c r="E30" s="135"/>
+      <c r="F30" s="135"/>
       <c r="G30" s="75"/>
       <c r="H30" s="82"/>
       <c r="I30" s="76"/>
@@ -7518,18 +7711,18 @@
       <c r="A31" s="77"/>
       <c r="B31" s="92"/>
       <c r="C31" s="76"/>
-      <c r="D31" s="139"/>
-      <c r="E31" s="140"/>
-      <c r="F31" s="140"/>
+      <c r="D31" s="134"/>
+      <c r="E31" s="135"/>
+      <c r="F31" s="135"/>
       <c r="G31" s="75"/>
       <c r="H31" s="82"/>
       <c r="I31" s="76"/>
       <c r="J31" s="74"/>
     </row>
     <row r="32" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A32" s="126"/>
-      <c r="B32" s="127"/>
-      <c r="C32" s="127"/>
+      <c r="A32" s="136"/>
+      <c r="B32" s="137"/>
+      <c r="C32" s="137"/>
       <c r="D32" s="97"/>
       <c r="E32" s="97"/>
       <c r="F32" s="97"/>
@@ -7542,9 +7735,9 @@
       <c r="A33" s="77"/>
       <c r="B33" s="92"/>
       <c r="C33" s="76"/>
-      <c r="D33" s="139"/>
-      <c r="E33" s="140"/>
-      <c r="F33" s="140"/>
+      <c r="D33" s="134"/>
+      <c r="E33" s="135"/>
+      <c r="F33" s="135"/>
       <c r="G33" s="75"/>
       <c r="H33" s="82"/>
       <c r="I33" s="76"/>
@@ -7680,22 +7873,18 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="B1:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="H5:J5"/>
     <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="H6:J6"/>
@@ -7710,16 +7899,20 @@
     <mergeCell ref="J9:J10"/>
     <mergeCell ref="A11:J11"/>
     <mergeCell ref="A12:J12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="B1:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -7732,10 +7925,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K64"/>
+  <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="82" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:B14"/>
+    <sheetView topLeftCell="A22" zoomScale="80" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" outlineLevelRow="1"/>
@@ -7754,9 +7947,9 @@
       <c r="A1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="144"/>
-      <c r="C1" s="144"/>
-      <c r="D1" s="144"/>
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -7767,9 +7960,9 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="145"/>
-      <c r="C2" s="145"/>
-      <c r="D2" s="145"/>
+      <c r="B2" s="139"/>
+      <c r="C2" s="139"/>
+      <c r="D2" s="139"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -7782,51 +7975,51 @@
       <c r="A3" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="121" t="s">
+      <c r="B3" s="123" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="121"/>
-      <c r="D3" s="122"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="124"/>
       <c r="E3" s="60"/>
       <c r="F3" s="60"/>
       <c r="G3" s="60"/>
-      <c r="H3" s="152"/>
-      <c r="I3" s="152"/>
-      <c r="J3" s="152"/>
+      <c r="H3" s="148"/>
+      <c r="I3" s="148"/>
+      <c r="J3" s="148"/>
       <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="12.75">
       <c r="A4" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="153" t="s">
+      <c r="B4" s="150" t="s">
         <v>248</v>
       </c>
-      <c r="C4" s="154"/>
-      <c r="D4" s="155"/>
+      <c r="C4" s="151"/>
+      <c r="D4" s="152"/>
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
       <c r="G4" s="60"/>
-      <c r="H4" s="152"/>
-      <c r="I4" s="152"/>
-      <c r="J4" s="152"/>
+      <c r="H4" s="148"/>
+      <c r="I4" s="148"/>
+      <c r="J4" s="148"/>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" s="70" customFormat="1" ht="25.5">
       <c r="A5" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="147" t="s">
+      <c r="B5" s="141" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="148"/>
-      <c r="D5" s="149"/>
+      <c r="C5" s="142"/>
+      <c r="D5" s="143"/>
       <c r="E5" s="68"/>
       <c r="F5" s="68"/>
       <c r="G5" s="68"/>
-      <c r="H5" s="151"/>
-      <c r="I5" s="151"/>
-      <c r="J5" s="151"/>
+      <c r="H5" s="147"/>
+      <c r="I5" s="147"/>
+      <c r="J5" s="147"/>
       <c r="K5" s="69"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
@@ -7834,22 +8027,22 @@
         <v>38</v>
       </c>
       <c r="B6" s="79">
-        <f>COUNTIF(I12:I23,"Pass")</f>
+        <f>COUNTIF(I12:I24,"Pass")</f>
         <v>0</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>39</v>
       </c>
       <c r="D6" s="13">
-        <f>COUNTIF(I10:I729,"Pending")</f>
+        <f>COUNTIF(I10:I730,"Pending")</f>
         <v>0</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="152"/>
-      <c r="I6" s="152"/>
-      <c r="J6" s="152"/>
+      <c r="H6" s="148"/>
+      <c r="I6" s="148"/>
+      <c r="J6" s="148"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -7857,29 +8050,29 @@
         <v>3</v>
       </c>
       <c r="B7" s="80">
-        <f>COUNTIF(I12:I23,"Fail")</f>
+        <f>COUNTIF(I12:I24,"Fail")</f>
         <v>0</v>
       </c>
       <c r="C7" s="29" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="58">
-        <f>COUNTA(A12:A32) -1</f>
-        <v>2</v>
+        <f>COUNTA(A12:A33) -3</f>
+        <v>8</v>
       </c>
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
       <c r="G7" s="61"/>
-      <c r="H7" s="152"/>
-      <c r="I7" s="152"/>
-      <c r="J7" s="152"/>
+      <c r="H7" s="148"/>
+      <c r="I7" s="148"/>
+      <c r="J7" s="148"/>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="146"/>
-      <c r="B8" s="146"/>
-      <c r="C8" s="146"/>
-      <c r="D8" s="146"/>
+      <c r="A8" s="140"/>
+      <c r="B8" s="140"/>
+      <c r="C8" s="140"/>
+      <c r="D8" s="140"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -7889,70 +8082,70 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" s="72" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="130" t="s">
+      <c r="A9" s="157" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="159" t="s">
+      <c r="B9" s="158" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="130" t="s">
+      <c r="C9" s="157" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="131" t="s">
+      <c r="D9" s="162" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="132"/>
-      <c r="F9" s="132"/>
-      <c r="G9" s="133"/>
-      <c r="H9" s="156" t="s">
+      <c r="E9" s="163"/>
+      <c r="F9" s="163"/>
+      <c r="G9" s="164"/>
+      <c r="H9" s="153" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="125" t="s">
+      <c r="I9" s="149" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="125" t="s">
+      <c r="J9" s="149" t="s">
         <v>32</v>
       </c>
       <c r="K9" s="71"/>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="125"/>
-      <c r="B10" s="160"/>
-      <c r="C10" s="125"/>
-      <c r="D10" s="134"/>
-      <c r="E10" s="135"/>
-      <c r="F10" s="135"/>
-      <c r="G10" s="136"/>
-      <c r="H10" s="134"/>
-      <c r="I10" s="125"/>
-      <c r="J10" s="125"/>
+      <c r="A10" s="149"/>
+      <c r="B10" s="159"/>
+      <c r="C10" s="149"/>
+      <c r="D10" s="154"/>
+      <c r="E10" s="165"/>
+      <c r="F10" s="165"/>
+      <c r="G10" s="166"/>
+      <c r="H10" s="154"/>
+      <c r="I10" s="149"/>
+      <c r="J10" s="149"/>
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" s="73" customFormat="1" ht="15">
-      <c r="A11" s="157"/>
-      <c r="B11" s="157"/>
-      <c r="C11" s="157"/>
-      <c r="D11" s="157"/>
-      <c r="E11" s="157"/>
-      <c r="F11" s="157"/>
-      <c r="G11" s="157"/>
-      <c r="H11" s="157"/>
-      <c r="I11" s="157"/>
-      <c r="J11" s="158"/>
+      <c r="A11" s="155"/>
+      <c r="B11" s="155"/>
+      <c r="C11" s="155"/>
+      <c r="D11" s="155"/>
+      <c r="E11" s="155"/>
+      <c r="F11" s="155"/>
+      <c r="G11" s="155"/>
+      <c r="H11" s="155"/>
+      <c r="I11" s="155"/>
+      <c r="J11" s="156"/>
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A12" s="137" t="s">
+      <c r="A12" s="144" t="s">
         <v>249</v>
       </c>
-      <c r="B12" s="138"/>
-      <c r="C12" s="138"/>
-      <c r="D12" s="138"/>
-      <c r="E12" s="138"/>
-      <c r="F12" s="138"/>
-      <c r="G12" s="138"/>
-      <c r="H12" s="138"/>
-      <c r="I12" s="138"/>
-      <c r="J12" s="150"/>
+      <c r="B12" s="145"/>
+      <c r="C12" s="145"/>
+      <c r="D12" s="145"/>
+      <c r="E12" s="145"/>
+      <c r="F12" s="145"/>
+      <c r="G12" s="145"/>
+      <c r="H12" s="145"/>
+      <c r="I12" s="145"/>
+      <c r="J12" s="146"/>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" ht="132.75" customHeight="1" outlineLevel="1">
       <c r="A13" s="77" t="s">
@@ -7961,12 +8154,12 @@
       <c r="B13" s="81" t="s">
         <v>250</v>
       </c>
-      <c r="C13" s="168" t="s">
+      <c r="C13" s="122" t="s">
         <v>252</v>
       </c>
-      <c r="D13" s="123"/>
-      <c r="E13" s="124"/>
-      <c r="F13" s="124"/>
+      <c r="D13" s="128"/>
+      <c r="E13" s="129"/>
+      <c r="F13" s="129"/>
       <c r="G13" s="75"/>
       <c r="H13" s="89"/>
       <c r="I13" s="76"/>
@@ -7979,156 +8172,196 @@
       <c r="B14" s="81" t="s">
         <v>251</v>
       </c>
-      <c r="C14" s="168" t="s">
+      <c r="C14" s="122" t="s">
         <v>253</v>
       </c>
-      <c r="D14" s="123"/>
-      <c r="E14" s="124"/>
-      <c r="F14" s="124"/>
+      <c r="D14" s="128"/>
+      <c r="E14" s="129"/>
+      <c r="F14" s="129"/>
       <c r="G14" s="75"/>
       <c r="H14" s="89"/>
       <c r="I14" s="76"/>
       <c r="J14" s="74"/>
     </row>
-    <row r="15" spans="1:11" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A15" s="137"/>
-      <c r="B15" s="138"/>
-      <c r="C15" s="138"/>
-      <c r="D15" s="87"/>
-      <c r="E15" s="87"/>
-      <c r="F15" s="87"/>
-      <c r="G15" s="87"/>
-      <c r="H15" s="87"/>
-      <c r="I15" s="87"/>
-      <c r="J15" s="88"/>
-    </row>
-    <row r="16" spans="1:11" s="4" customFormat="1" ht="79.5" customHeight="1" outlineLevel="1">
-      <c r="A16" s="93"/>
-      <c r="B16" s="85"/>
-      <c r="C16" s="86"/>
-      <c r="D16" s="165"/>
-      <c r="E16" s="166"/>
-      <c r="F16" s="166"/>
-      <c r="G16" s="94"/>
-      <c r="H16" s="95"/>
-      <c r="I16" s="86"/>
-      <c r="J16" s="96"/>
-    </row>
-    <row r="17" spans="1:10" s="4" customFormat="1" ht="66.75" customHeight="1" outlineLevel="1">
+    <row r="15" spans="1:11" s="4" customFormat="1" ht="144.75" customHeight="1" outlineLevel="1">
+      <c r="A15" s="77" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="81" t="s">
+        <v>261</v>
+      </c>
+      <c r="C15" s="76" t="s">
+        <v>262</v>
+      </c>
+      <c r="D15" s="128"/>
+      <c r="E15" s="129"/>
+      <c r="F15" s="129"/>
+      <c r="G15" s="75"/>
+      <c r="H15" s="89"/>
+      <c r="I15" s="76"/>
+      <c r="J15" s="74"/>
+    </row>
+    <row r="16" spans="1:11" s="4" customFormat="1" ht="12.75" outlineLevel="1">
+      <c r="A16" s="144" t="s">
+        <v>256</v>
+      </c>
+      <c r="B16" s="145"/>
+      <c r="C16" s="145"/>
+      <c r="D16" s="87"/>
+      <c r="E16" s="87"/>
+      <c r="F16" s="87"/>
+      <c r="G16" s="87"/>
+      <c r="H16" s="87"/>
+      <c r="I16" s="87"/>
+      <c r="J16" s="88"/>
+    </row>
+    <row r="17" spans="1:10" s="4" customFormat="1" ht="79.5" customHeight="1" outlineLevel="1">
       <c r="A17" s="93"/>
       <c r="B17" s="85"/>
       <c r="C17" s="86"/>
-      <c r="D17" s="165"/>
-      <c r="E17" s="166"/>
-      <c r="F17" s="166"/>
+      <c r="D17" s="167"/>
+      <c r="E17" s="168"/>
+      <c r="F17" s="168"/>
       <c r="G17" s="94"/>
       <c r="H17" s="95"/>
       <c r="I17" s="86"/>
       <c r="J17" s="96"/>
     </row>
-    <row r="18" spans="1:10" s="4" customFormat="1" ht="79.5" customHeight="1" outlineLevel="1">
-      <c r="A18" s="93"/>
-      <c r="B18" s="85"/>
-      <c r="C18" s="86"/>
-      <c r="D18" s="165"/>
-      <c r="E18" s="166"/>
-      <c r="F18" s="166"/>
+    <row r="18" spans="1:10" s="4" customFormat="1" ht="124.5" customHeight="1" outlineLevel="1">
+      <c r="A18" s="93" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="92" t="s">
+        <v>264</v>
+      </c>
+      <c r="C18" s="76" t="s">
+        <v>272</v>
+      </c>
+      <c r="D18" s="167"/>
+      <c r="E18" s="168"/>
+      <c r="F18" s="168"/>
       <c r="G18" s="94"/>
       <c r="H18" s="95"/>
       <c r="I18" s="86"/>
       <c r="J18" s="96"/>
     </row>
-    <row r="19" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A19" s="137"/>
-      <c r="B19" s="138"/>
-      <c r="C19" s="138"/>
-      <c r="D19" s="87"/>
-      <c r="E19" s="87"/>
-      <c r="F19" s="87"/>
-      <c r="G19" s="87"/>
-      <c r="H19" s="87"/>
-      <c r="I19" s="87"/>
-      <c r="J19" s="88"/>
-    </row>
-    <row r="20" spans="1:10" s="4" customFormat="1" ht="116.25" customHeight="1" outlineLevel="1">
-      <c r="A20" s="77"/>
-      <c r="B20" s="92"/>
-      <c r="C20" s="76"/>
-      <c r="D20" s="123"/>
-      <c r="E20" s="124"/>
-      <c r="F20" s="124"/>
-      <c r="G20" s="75"/>
-      <c r="H20" s="82"/>
-      <c r="I20" s="76"/>
-      <c r="J20" s="74"/>
-    </row>
-    <row r="21" spans="1:10" s="4" customFormat="1" ht="67.5" customHeight="1" outlineLevel="1">
-      <c r="A21" s="77"/>
-      <c r="B21" s="92"/>
-      <c r="C21" s="76"/>
-      <c r="D21" s="123"/>
-      <c r="E21" s="124"/>
-      <c r="F21" s="124"/>
+    <row r="19" spans="1:10" s="4" customFormat="1" ht="79.5" customHeight="1" outlineLevel="1">
+      <c r="A19" s="93"/>
+      <c r="B19" s="85"/>
+      <c r="C19" s="86"/>
+      <c r="D19" s="167"/>
+      <c r="E19" s="168"/>
+      <c r="F19" s="168"/>
+      <c r="G19" s="94"/>
+      <c r="H19" s="95"/>
+      <c r="I19" s="86"/>
+      <c r="J19" s="96"/>
+    </row>
+    <row r="20" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
+      <c r="A20" s="144" t="s">
+        <v>257</v>
+      </c>
+      <c r="B20" s="145"/>
+      <c r="C20" s="145"/>
+      <c r="D20" s="87"/>
+      <c r="E20" s="87"/>
+      <c r="F20" s="87"/>
+      <c r="G20" s="87"/>
+      <c r="H20" s="87"/>
+      <c r="I20" s="87"/>
+      <c r="J20" s="88"/>
+    </row>
+    <row r="21" spans="1:10" s="4" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A21" s="77" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="92" t="s">
+        <v>259</v>
+      </c>
+      <c r="C21" s="76" t="s">
+        <v>260</v>
+      </c>
+      <c r="D21" s="128"/>
+      <c r="E21" s="129"/>
+      <c r="F21" s="129"/>
       <c r="G21" s="75"/>
       <c r="H21" s="82"/>
       <c r="I21" s="76"/>
       <c r="J21" s="74"/>
     </row>
-    <row r="22" spans="1:10" s="4" customFormat="1" ht="81" customHeight="1" outlineLevel="1">
-      <c r="A22" s="77"/>
-      <c r="B22" s="92"/>
-      <c r="C22" s="76"/>
-      <c r="D22" s="123"/>
-      <c r="E22" s="124"/>
-      <c r="F22" s="124"/>
+    <row r="22" spans="1:10" s="4" customFormat="1" ht="148.5" customHeight="1" outlineLevel="1">
+      <c r="A22" s="77" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="92" t="s">
+        <v>258</v>
+      </c>
+      <c r="C22" s="76" t="s">
+        <v>262</v>
+      </c>
+      <c r="D22" s="128"/>
+      <c r="E22" s="129"/>
+      <c r="F22" s="129"/>
       <c r="G22" s="75"/>
       <c r="H22" s="82"/>
       <c r="I22" s="76"/>
       <c r="J22" s="74"/>
     </row>
-    <row r="23" spans="1:10" s="4" customFormat="1" ht="113.25" customHeight="1" outlineLevel="1">
-      <c r="A23" s="77"/>
-      <c r="B23" s="92"/>
-      <c r="C23" s="76"/>
-      <c r="D23" s="123"/>
-      <c r="E23" s="124"/>
-      <c r="F23" s="124"/>
+    <row r="23" spans="1:10" s="4" customFormat="1" ht="123.75" customHeight="1" outlineLevel="1">
+      <c r="A23" s="77" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="92" t="s">
+        <v>263</v>
+      </c>
+      <c r="C23" s="76" t="s">
+        <v>271</v>
+      </c>
+      <c r="D23" s="128"/>
+      <c r="E23" s="129"/>
+      <c r="F23" s="129"/>
       <c r="G23" s="75"/>
       <c r="H23" s="82"/>
       <c r="I23" s="76"/>
       <c r="J23" s="74"/>
     </row>
-    <row r="24" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A24" s="126"/>
-      <c r="B24" s="127"/>
-      <c r="C24" s="127"/>
-      <c r="D24" s="97"/>
-      <c r="E24" s="97"/>
-      <c r="F24" s="97"/>
-      <c r="G24" s="97"/>
-      <c r="H24" s="97"/>
-      <c r="I24" s="97"/>
-      <c r="J24" s="98"/>
-    </row>
-    <row r="25" spans="1:10" s="4" customFormat="1" ht="78.75" customHeight="1" outlineLevel="1">
-      <c r="A25" s="77"/>
-      <c r="B25" s="92"/>
-      <c r="C25" s="76"/>
-      <c r="D25" s="139"/>
-      <c r="E25" s="140"/>
-      <c r="F25" s="140"/>
-      <c r="G25" s="75"/>
-      <c r="H25" s="82"/>
-      <c r="I25" s="76"/>
-      <c r="J25" s="74"/>
-    </row>
-    <row r="26" spans="1:10" s="4" customFormat="1" ht="79.5" customHeight="1" outlineLevel="1">
+    <row r="24" spans="1:10" s="4" customFormat="1" ht="148.5" customHeight="1" outlineLevel="1">
+      <c r="A24" s="77" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="92" t="s">
+        <v>265</v>
+      </c>
+      <c r="C24" s="76" t="s">
+        <v>268</v>
+      </c>
+      <c r="D24" s="128"/>
+      <c r="E24" s="129"/>
+      <c r="F24" s="129"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="82"/>
+      <c r="I24" s="76"/>
+      <c r="J24" s="74"/>
+    </row>
+    <row r="25" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
+      <c r="A25" s="136"/>
+      <c r="B25" s="137"/>
+      <c r="C25" s="137"/>
+      <c r="D25" s="97"/>
+      <c r="E25" s="97"/>
+      <c r="F25" s="97"/>
+      <c r="G25" s="97"/>
+      <c r="H25" s="97"/>
+      <c r="I25" s="97"/>
+      <c r="J25" s="98"/>
+    </row>
+    <row r="26" spans="1:10" s="4" customFormat="1" ht="78.75" customHeight="1" outlineLevel="1">
       <c r="A26" s="77"/>
       <c r="B26" s="92"/>
       <c r="C26" s="76"/>
-      <c r="D26" s="139"/>
-      <c r="E26" s="140"/>
-      <c r="F26" s="140"/>
+      <c r="D26" s="134"/>
+      <c r="E26" s="135"/>
+      <c r="F26" s="135"/>
       <c r="G26" s="75"/>
       <c r="H26" s="82"/>
       <c r="I26" s="76"/>
@@ -8138,9 +8371,9 @@
       <c r="A27" s="77"/>
       <c r="B27" s="92"/>
       <c r="C27" s="76"/>
-      <c r="D27" s="139"/>
-      <c r="E27" s="140"/>
-      <c r="F27" s="140"/>
+      <c r="D27" s="134"/>
+      <c r="E27" s="135"/>
+      <c r="F27" s="135"/>
       <c r="G27" s="75"/>
       <c r="H27" s="82"/>
       <c r="I27" s="76"/>
@@ -8150,128 +8383,136 @@
       <c r="A28" s="77"/>
       <c r="B28" s="92"/>
       <c r="C28" s="76"/>
-      <c r="D28" s="139"/>
-      <c r="E28" s="140"/>
-      <c r="F28" s="140"/>
+      <c r="D28" s="134"/>
+      <c r="E28" s="135"/>
+      <c r="F28" s="135"/>
       <c r="G28" s="75"/>
       <c r="H28" s="82"/>
       <c r="I28" s="76"/>
       <c r="J28" s="74"/>
     </row>
-    <row r="29" spans="1:10" s="4" customFormat="1" ht="91.5" customHeight="1" outlineLevel="1">
+    <row r="29" spans="1:10" s="4" customFormat="1" ht="79.5" customHeight="1" outlineLevel="1">
       <c r="A29" s="77"/>
       <c r="B29" s="92"/>
       <c r="C29" s="76"/>
-      <c r="D29" s="139"/>
-      <c r="E29" s="140"/>
-      <c r="F29" s="140"/>
+      <c r="D29" s="134"/>
+      <c r="E29" s="135"/>
+      <c r="F29" s="135"/>
       <c r="G29" s="75"/>
       <c r="H29" s="82"/>
       <c r="I29" s="76"/>
       <c r="J29" s="74"/>
     </row>
-    <row r="30" spans="1:10" s="4" customFormat="1" ht="67.5" customHeight="1" outlineLevel="1">
+    <row r="30" spans="1:10" s="4" customFormat="1" ht="91.5" customHeight="1" outlineLevel="1">
       <c r="A30" s="77"/>
       <c r="B30" s="92"/>
       <c r="C30" s="76"/>
-      <c r="D30" s="139"/>
-      <c r="E30" s="140"/>
-      <c r="F30" s="140"/>
+      <c r="D30" s="134"/>
+      <c r="E30" s="135"/>
+      <c r="F30" s="135"/>
       <c r="G30" s="75"/>
       <c r="H30" s="82"/>
       <c r="I30" s="76"/>
       <c r="J30" s="74"/>
     </row>
-    <row r="31" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A31" s="126"/>
-      <c r="B31" s="127"/>
-      <c r="C31" s="127"/>
-      <c r="D31" s="97"/>
-      <c r="E31" s="97"/>
-      <c r="F31" s="97"/>
-      <c r="G31" s="97"/>
-      <c r="H31" s="97"/>
-      <c r="I31" s="97"/>
-      <c r="J31" s="98"/>
-    </row>
-    <row r="32" spans="1:10" s="4" customFormat="1" ht="47.25" customHeight="1" outlineLevel="1">
-      <c r="A32" s="77"/>
-      <c r="B32" s="92"/>
-      <c r="C32" s="76"/>
-      <c r="D32" s="139"/>
-      <c r="E32" s="140"/>
-      <c r="F32" s="140"/>
-      <c r="G32" s="75"/>
-      <c r="H32" s="82"/>
-      <c r="I32" s="76"/>
-      <c r="J32" s="74"/>
-    </row>
-    <row r="33" spans="9:10" ht="12" customHeight="1">
-      <c r="I33"/>
-      <c r="J33"/>
-    </row>
-    <row r="34" spans="9:10" ht="12" customHeight="1">
+    <row r="31" spans="1:10" s="4" customFormat="1" ht="67.5" customHeight="1" outlineLevel="1">
+      <c r="A31" s="77"/>
+      <c r="B31" s="92"/>
+      <c r="C31" s="76"/>
+      <c r="D31" s="134"/>
+      <c r="E31" s="135"/>
+      <c r="F31" s="135"/>
+      <c r="G31" s="75"/>
+      <c r="H31" s="82"/>
+      <c r="I31" s="76"/>
+      <c r="J31" s="74"/>
+    </row>
+    <row r="32" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
+      <c r="A32" s="136"/>
+      <c r="B32" s="137"/>
+      <c r="C32" s="137"/>
+      <c r="D32" s="97"/>
+      <c r="E32" s="97"/>
+      <c r="F32" s="97"/>
+      <c r="G32" s="97"/>
+      <c r="H32" s="97"/>
+      <c r="I32" s="97"/>
+      <c r="J32" s="98"/>
+    </row>
+    <row r="33" spans="1:10" s="4" customFormat="1" ht="47.25" customHeight="1" outlineLevel="1">
+      <c r="A33" s="77"/>
+      <c r="B33" s="92"/>
+      <c r="C33" s="76"/>
+      <c r="D33" s="134"/>
+      <c r="E33" s="135"/>
+      <c r="F33" s="135"/>
+      <c r="G33" s="75"/>
+      <c r="H33" s="82"/>
+      <c r="I33" s="76"/>
+      <c r="J33" s="74"/>
+    </row>
+    <row r="34" spans="1:10" ht="12" customHeight="1">
       <c r="I34"/>
       <c r="J34"/>
     </row>
-    <row r="35" spans="9:10" ht="12" customHeight="1">
+    <row r="35" spans="1:10" ht="12" customHeight="1">
       <c r="I35"/>
       <c r="J35"/>
     </row>
-    <row r="36" spans="9:10" ht="12" customHeight="1">
+    <row r="36" spans="1:10" ht="12" customHeight="1">
       <c r="I36"/>
       <c r="J36"/>
     </row>
-    <row r="37" spans="9:10" ht="12" customHeight="1">
+    <row r="37" spans="1:10" ht="12" customHeight="1">
       <c r="I37"/>
       <c r="J37"/>
     </row>
-    <row r="38" spans="9:10" ht="12" customHeight="1">
+    <row r="38" spans="1:10" ht="12" customHeight="1">
       <c r="I38"/>
       <c r="J38"/>
     </row>
-    <row r="39" spans="9:10" ht="12" customHeight="1">
+    <row r="39" spans="1:10" ht="12" customHeight="1">
       <c r="I39"/>
       <c r="J39"/>
     </row>
-    <row r="40" spans="9:10" ht="12" customHeight="1">
+    <row r="40" spans="1:10" ht="12" customHeight="1">
       <c r="I40"/>
       <c r="J40"/>
     </row>
-    <row r="41" spans="9:10" ht="12" customHeight="1">
+    <row r="41" spans="1:10" ht="12" customHeight="1">
       <c r="I41"/>
       <c r="J41"/>
     </row>
-    <row r="42" spans="9:10" ht="12" customHeight="1">
+    <row r="42" spans="1:10" ht="12" customHeight="1">
       <c r="I42"/>
       <c r="J42"/>
     </row>
-    <row r="43" spans="9:10" ht="12" customHeight="1">
+    <row r="43" spans="1:10" ht="12" customHeight="1">
       <c r="I43"/>
       <c r="J43"/>
     </row>
-    <row r="44" spans="9:10" ht="12" customHeight="1">
+    <row r="44" spans="1:10" ht="12" customHeight="1">
       <c r="I44"/>
       <c r="J44"/>
     </row>
-    <row r="45" spans="9:10" ht="12" customHeight="1">
+    <row r="45" spans="1:10" ht="12" customHeight="1">
       <c r="I45"/>
       <c r="J45"/>
     </row>
-    <row r="46" spans="9:10" ht="12" customHeight="1">
+    <row r="46" spans="1:10" ht="12" customHeight="1">
       <c r="I46"/>
       <c r="J46"/>
     </row>
-    <row r="47" spans="9:10" ht="12" customHeight="1">
+    <row r="47" spans="1:10" ht="12" customHeight="1">
       <c r="I47"/>
       <c r="J47"/>
     </row>
-    <row r="48" spans="9:10" ht="12" customHeight="1">
+    <row r="48" spans="1:10" ht="12" customHeight="1">
       <c r="I48"/>
       <c r="J48"/>
     </row>
-    <row r="49" spans="9:10">
-      <c r="I49" s="19"/>
+    <row r="49" spans="9:10" ht="12" customHeight="1">
+      <c r="I49"/>
       <c r="J49"/>
     </row>
     <row r="50" spans="9:10">
@@ -8334,30 +8575,20 @@
       <c r="I64" s="19"/>
       <c r="J64"/>
     </row>
+    <row r="65" spans="9:10">
+      <c r="I65" s="19"/>
+      <c r="J65"/>
+    </row>
   </sheetData>
-  <mergeCells count="39">
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="D13:F13"/>
+  <mergeCells count="40">
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="H5:J5"/>
     <mergeCell ref="D14:F14"/>
-    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="B1:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="H4:J4"/>
     <mergeCell ref="H6:J6"/>
     <mergeCell ref="H7:J7"/>
     <mergeCell ref="A8:D8"/>
@@ -8368,13 +8599,28 @@
     <mergeCell ref="H9:H10"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
-    <mergeCell ref="B1:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="D33:F33"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -8386,7 +8632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -8500,7 +8746,7 @@
       </c>
       <c r="G8" s="66">
         <f>Samples!D7</f>
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="59" customFormat="1" ht="14.25">
@@ -8550,9 +8796,9 @@
         <f>Samples3!D6</f>
         <v>0</v>
       </c>
-      <c r="G10" s="167">
+      <c r="G10" s="121">
         <f>Samples3!D7</f>
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14.25">
@@ -8575,7 +8821,7 @@
       </c>
       <c r="G11" s="54">
         <f>SUM(G6:G10)</f>
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14.25">
@@ -8596,7 +8842,7 @@
       <c r="D13" s="19"/>
       <c r="E13" s="23">
         <f>(D11+E11)*100/G11</f>
-        <v>45.652173913043477</v>
+        <v>38.888888888888886</v>
       </c>
       <c r="F13" s="19" t="s">
         <v>22</v>
@@ -8612,7 +8858,7 @@
       <c r="D14" s="19"/>
       <c r="E14" s="23">
         <f>D11*100/G11</f>
-        <v>28.260869565217391</v>
+        <v>24.074074074074073</v>
       </c>
       <c r="F14" s="19" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
up gui tb huy
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University_IT\Tam\KiemThuPhanMem\event-manager-javafx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703563E2-1A91-4B2D-914E-1548C2C14D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799C555B-6FC1-47F0-95C0-2CCDD4BE8CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="821" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="821" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="97" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="288">
   <si>
     <t>TC1</t>
   </si>
@@ -990,9 +990,6 @@
     <t>Gửi thông báo và nhắc nhở</t>
   </si>
   <si>
-    <t>1. Thông báo thay đổi thời gian sự kiện</t>
-  </si>
-  <si>
     <t>Kiểm tra chức năng gửi thông báo thay đổi thời gian sự kiện cho người tham gia trong thời gian cho phép</t>
   </si>
   <si>
@@ -1021,9 +1018,6 @@
   </si>
   <si>
     <t>Viết TC Kiểm tra chức năng gửi thông báo thay đổi thời gian sự kiện cho người tham gia trong thời gian không cho phép</t>
-  </si>
-  <si>
-    <t>2. Thông báo sự kiện hủy, hoàn tiền cho người tham gia</t>
   </si>
   <si>
     <t>3. Nhắc nhở tự động trước ngày diễn ra sự kiện</t>
@@ -1101,15 +1095,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">1: Đăng nhập với tư cách là admin
-2: Chọn sự kiện đã có sẵn với thời gian diễn ra là 8h ngày 10/5
-3: Chạy tự động gửi nhắc nhở vào 8h ngày 9/5
-4: Hủy sự kiện thành công lúc 7h ngày 9/5
-5: Hệ thống Gửi thông báo hủy ngay lập tức đến tất cả người tham gia
-5: Hệ thống không gửi nhắc nhở đến tất cả người tham gia vào 8h ngày 9/5
-</t>
-  </si>
-  <si>
     <t>Viết TC Kiểm tra chức năng tự động gửi nhắc nhở đến người tham gia trước 1 ngày sự kiện diễn ra</t>
   </si>
   <si>
@@ -1132,6 +1117,59 @@
   </si>
   <si>
     <t>Viết TC Kiểm tra chức năng hủy sự kiện trước khi gửi nhắc nhở và hệ thống không gửi nhắc nhở tự động</t>
+  </si>
+  <si>
+    <t>1. Gửi thông báo thay đổi thời gian sự kiện</t>
+  </si>
+  <si>
+    <t>2. Gửi thông báo hủy sự kiện</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng xử lý lỗi khi gửi thông báo hủy sự kiện</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng gửi thông báo khi hủy sự kiện không có người đăng ký tham gia</t>
+  </si>
+  <si>
+    <t>1: Đăng nhập với tư cách là admin
+2: Truy cập vào trang Quản lý sự kiện
+3: Chọn sự kiện không có người đăng ký tham gia để hủy 
+4: Chọn Hủy sự kiện và nhập lý do hủy
+5: Xác nhận hủy sự kiện 
+6: Hệ thống không gửi thông báo nào và thông báo việc Không có người đăng ký tham gia để gửi thông báo</t>
+  </si>
+  <si>
+    <t>1: Đăng nhập với tư cách là admin
+2: Truy cập vào trang Quản lý sự kiện
+3: Chọn sự kiện cần hủy
+4: Giả lập lỗi gửi thông báo(Vd: ngắt kết nối mạng, máy chủ không phản hồi, ngắt kết nối database..)
+5: Chọn Hủy, nhập lý do và xác nhận hủy sự kiện 
+6: Gửi thông báo hủy sự kiện
+7: Hệ thống hiển thị lỗi không thể gửi thông báo vì một số lý do 
+8: Sửa lỗi(Vd: kết nối lại mạng, kết nối lại database..), và thực hiện việc gửi lại thông báo
+9: Hệ thống thành công việc gửi thông báo hủy sự kiện đến tất cả người tham gia</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng gửi thông báo khi hủy sự kiện trong thời gian cho phép hủy</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng gửi thông báo khi hủy sự kiện trong thời gian không cho phép hủy</t>
+  </si>
+  <si>
+    <t>1: Đăng nhập với tư cách là admin
+2: Truy cập vào trang Quản lý sự kiện
+3: Chọn sự kiện cần hủy(trước ngày diễn ra sự kiện 24h) 
+4: Chọn Hủy sự kiện và nhập lý do hủy(bao gồm việc thông báo sẽ hoàn tiền cho tất cả người tham gia đối với sự kiện có phí)
+5: Xác nhận hủy sự kiện 
+6: Hệ thống gửi thông báo hủy sự kiện đến tất cả người tham gia</t>
+  </si>
+  <si>
+    <t>1: Đăng nhập với tư cách là admin
+2: Truy cập vào trang Quản lý sự kiện
+3: Chọn sự kiện đã quá thời gian cho phép hủy 
+4: Chọn Hủy sự kiện và nhập lý do hủy(bao gồm việc sẽ hoàn tiền cho tất cả người tham gia đối với sự kiện có phí)
+5: Xác nhận hủy sự kiện 
+6: Hệ thống hiển thị thông báo lỗi về giới hạn thời gian</t>
   </si>
 </sst>
 </file>
@@ -1858,7 +1896,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2186,6 +2224,60 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2195,11 +2287,56 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2213,109 +2350,19 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="6" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4032,10 +4079,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H119"/>
+  <dimension ref="A2:H118"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A94" zoomScale="85" workbookViewId="0">
-      <selection activeCell="D97" sqref="D97"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A98" zoomScale="85" workbookViewId="0">
+      <selection activeCell="G104" sqref="G104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -5555,7 +5602,7 @@
       </c>
       <c r="D93" s="99"/>
       <c r="E93" s="104" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F93" s="110" t="s">
         <v>44</v>
@@ -5572,7 +5619,7 @@
       </c>
       <c r="D94" s="99"/>
       <c r="E94" s="104" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F94" s="110" t="s">
         <v>44</v>
@@ -5589,7 +5636,7 @@
       </c>
       <c r="D95" s="99"/>
       <c r="E95" s="104" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="F95" s="110" t="s">
         <v>44</v>
@@ -5606,7 +5653,7 @@
       </c>
       <c r="D96" s="99"/>
       <c r="E96" s="104" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F96" s="110" t="s">
         <v>44</v>
@@ -5623,7 +5670,7 @@
       </c>
       <c r="D97" s="99"/>
       <c r="E97" s="104" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F97" s="110" t="s">
         <v>44</v>
@@ -5640,7 +5687,7 @@
       </c>
       <c r="D98" s="99"/>
       <c r="E98" s="104" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F98" s="110" t="s">
         <v>44</v>
@@ -5657,7 +5704,7 @@
       </c>
       <c r="D99" s="99"/>
       <c r="E99" s="104" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="F99" s="110" t="s">
         <v>44</v>
@@ -5674,7 +5721,7 @@
       </c>
       <c r="D100" s="99"/>
       <c r="E100" s="104" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="F100" s="110" t="s">
         <v>44</v>
@@ -5691,7 +5738,7 @@
       </c>
       <c r="D101" s="99"/>
       <c r="E101" s="104" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F101" s="110" t="s">
         <v>44</v>
@@ -5708,7 +5755,7 @@
       </c>
       <c r="D102" s="99"/>
       <c r="E102" s="104" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F102" s="110" t="s">
         <v>44</v>
@@ -5716,48 +5763,88 @@
       <c r="G102" s="99"/>
       <c r="H102" s="105"/>
     </row>
-    <row r="103" spans="2:8" s="33" customFormat="1">
-      <c r="B103" s="118"/>
-      <c r="C103" s="119"/>
+    <row r="103" spans="2:8" s="33" customFormat="1" ht="25.5">
+      <c r="B103" s="118">
+        <v>45763</v>
+      </c>
+      <c r="C103" s="119" t="s">
+        <v>40</v>
+      </c>
       <c r="D103" s="99"/>
-      <c r="E103" s="104"/>
-      <c r="F103" s="120"/>
+      <c r="E103" s="104" t="s">
+        <v>284</v>
+      </c>
+      <c r="F103" s="110" t="s">
+        <v>44</v>
+      </c>
       <c r="G103" s="99"/>
       <c r="H103" s="105"/>
     </row>
-    <row r="104" spans="2:8" s="33" customFormat="1">
-      <c r="B104" s="118"/>
-      <c r="C104" s="119"/>
+    <row r="104" spans="2:8" s="33" customFormat="1" ht="38.25">
+      <c r="B104" s="118">
+        <v>45763</v>
+      </c>
+      <c r="C104" s="119" t="s">
+        <v>40</v>
+      </c>
       <c r="D104" s="99"/>
-      <c r="E104" s="104"/>
-      <c r="F104" s="120"/>
+      <c r="E104" s="104" t="s">
+        <v>285</v>
+      </c>
+      <c r="F104" s="110" t="s">
+        <v>44</v>
+      </c>
       <c r="G104" s="99"/>
       <c r="H104" s="105"/>
     </row>
-    <row r="105" spans="2:8" s="33" customFormat="1">
-      <c r="B105" s="118"/>
-      <c r="C105" s="119"/>
+    <row r="105" spans="2:8" s="33" customFormat="1" ht="25.5">
+      <c r="B105" s="118">
+        <v>45763</v>
+      </c>
+      <c r="C105" s="119" t="s">
+        <v>40</v>
+      </c>
       <c r="D105" s="99"/>
-      <c r="E105" s="104"/>
-      <c r="F105" s="120"/>
+      <c r="E105" s="104" t="s">
+        <v>281</v>
+      </c>
+      <c r="F105" s="110" t="s">
+        <v>44</v>
+      </c>
       <c r="G105" s="99"/>
       <c r="H105" s="105"/>
     </row>
-    <row r="106" spans="2:8" s="33" customFormat="1">
-      <c r="B106" s="118"/>
-      <c r="C106" s="119"/>
+    <row r="106" spans="2:8" s="33" customFormat="1" ht="25.5">
+      <c r="B106" s="118">
+        <v>45763</v>
+      </c>
+      <c r="C106" s="119" t="s">
+        <v>40</v>
+      </c>
       <c r="D106" s="99"/>
-      <c r="E106" s="104"/>
-      <c r="F106" s="120"/>
+      <c r="E106" s="104" t="s">
+        <v>280</v>
+      </c>
+      <c r="F106" s="110" t="s">
+        <v>44</v>
+      </c>
       <c r="G106" s="99"/>
       <c r="H106" s="105"/>
     </row>
-    <row r="107" spans="2:8" s="33" customFormat="1">
-      <c r="B107" s="118"/>
-      <c r="C107" s="119"/>
+    <row r="107" spans="2:8" s="33" customFormat="1" ht="25.5">
+      <c r="B107" s="118">
+        <v>45763</v>
+      </c>
+      <c r="C107" s="119" t="s">
+        <v>40</v>
+      </c>
       <c r="D107" s="99"/>
-      <c r="E107" s="104"/>
-      <c r="F107" s="120"/>
+      <c r="E107" s="104" t="s">
+        <v>280</v>
+      </c>
+      <c r="F107" s="110" t="s">
+        <v>44</v>
+      </c>
       <c r="G107" s="99"/>
       <c r="H107" s="105"/>
     </row>
@@ -5852,22 +5939,13 @@
       <c r="H117" s="105"/>
     </row>
     <row r="118" spans="2:8" s="33" customFormat="1">
-      <c r="B118" s="118"/>
-      <c r="C118" s="119"/>
-      <c r="D118" s="99"/>
-      <c r="E118" s="104"/>
-      <c r="F118" s="120"/>
-      <c r="G118" s="99"/>
-      <c r="H118" s="105"/>
-    </row>
-    <row r="119" spans="2:8" s="33" customFormat="1">
-      <c r="B119" s="107"/>
-      <c r="C119" s="106"/>
-      <c r="D119" s="42"/>
-      <c r="E119" s="103"/>
-      <c r="F119" s="111"/>
-      <c r="G119" s="42"/>
-      <c r="H119" s="43"/>
+      <c r="B118" s="107"/>
+      <c r="C118" s="106"/>
+      <c r="D118" s="42"/>
+      <c r="E118" s="103"/>
+      <c r="F118" s="111"/>
+      <c r="G118" s="42"/>
+      <c r="H118" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5896,7 +5974,7 @@
   </sheetPr>
   <dimension ref="A1:K88"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="69" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A48" zoomScale="69" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
@@ -5916,9 +5994,9 @@
       <c r="A1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="138"/>
-      <c r="C1" s="138"/>
-      <c r="D1" s="138"/>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -5929,9 +6007,9 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="139"/>
-      <c r="C2" s="139"/>
-      <c r="D2" s="139"/>
+      <c r="B2" s="147"/>
+      <c r="C2" s="147"/>
+      <c r="D2" s="147"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -5952,43 +6030,43 @@
       <c r="E3" s="60"/>
       <c r="F3" s="60"/>
       <c r="G3" s="60"/>
-      <c r="H3" s="148"/>
-      <c r="I3" s="148"/>
-      <c r="J3" s="148"/>
+      <c r="H3" s="154"/>
+      <c r="I3" s="154"/>
+      <c r="J3" s="154"/>
       <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="12.75">
       <c r="A4" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="150" t="s">
+      <c r="B4" s="155" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="151"/>
-      <c r="D4" s="152"/>
+      <c r="C4" s="156"/>
+      <c r="D4" s="157"/>
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
       <c r="G4" s="60"/>
-      <c r="H4" s="148"/>
-      <c r="I4" s="148"/>
-      <c r="J4" s="148"/>
+      <c r="H4" s="154"/>
+      <c r="I4" s="154"/>
+      <c r="J4" s="154"/>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" s="70" customFormat="1" ht="25.5">
       <c r="A5" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="141" t="s">
+      <c r="B5" s="149" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="142"/>
-      <c r="D5" s="143"/>
+      <c r="C5" s="150"/>
+      <c r="D5" s="151"/>
       <c r="E5" s="68"/>
       <c r="F5" s="68"/>
       <c r="G5" s="68"/>
-      <c r="H5" s="147"/>
-      <c r="I5" s="147"/>
-      <c r="J5" s="147"/>
+      <c r="H5" s="153"/>
+      <c r="I5" s="153"/>
+      <c r="J5" s="153"/>
       <c r="K5" s="69"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
@@ -6009,9 +6087,9 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="148"/>
-      <c r="I6" s="148"/>
-      <c r="J6" s="148"/>
+      <c r="H6" s="154"/>
+      <c r="I6" s="154"/>
+      <c r="J6" s="154"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -6032,16 +6110,16 @@
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
       <c r="G7" s="61"/>
-      <c r="H7" s="148"/>
-      <c r="I7" s="148"/>
-      <c r="J7" s="148"/>
+      <c r="H7" s="154"/>
+      <c r="I7" s="154"/>
+      <c r="J7" s="154"/>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="140"/>
-      <c r="B8" s="140"/>
-      <c r="C8" s="140"/>
-      <c r="D8" s="140"/>
+      <c r="A8" s="148"/>
+      <c r="B8" s="148"/>
+      <c r="C8" s="148"/>
+      <c r="D8" s="148"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -6051,70 +6129,70 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" s="72" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="157" t="s">
+      <c r="A9" s="132" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="158" t="s">
+      <c r="B9" s="161" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="157" t="s">
+      <c r="C9" s="132" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="162" t="s">
+      <c r="D9" s="133" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="163"/>
-      <c r="F9" s="163"/>
-      <c r="G9" s="164"/>
-      <c r="H9" s="153" t="s">
+      <c r="E9" s="134"/>
+      <c r="F9" s="134"/>
+      <c r="G9" s="135"/>
+      <c r="H9" s="158" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="149" t="s">
+      <c r="I9" s="127" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="149" t="s">
+      <c r="J9" s="127" t="s">
         <v>32</v>
       </c>
       <c r="K9" s="71"/>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="149"/>
-      <c r="B10" s="159"/>
-      <c r="C10" s="149"/>
-      <c r="D10" s="154"/>
-      <c r="E10" s="165"/>
-      <c r="F10" s="165"/>
-      <c r="G10" s="166"/>
-      <c r="H10" s="154"/>
-      <c r="I10" s="149"/>
-      <c r="J10" s="149"/>
+      <c r="A10" s="127"/>
+      <c r="B10" s="162"/>
+      <c r="C10" s="127"/>
+      <c r="D10" s="136"/>
+      <c r="E10" s="137"/>
+      <c r="F10" s="137"/>
+      <c r="G10" s="138"/>
+      <c r="H10" s="136"/>
+      <c r="I10" s="127"/>
+      <c r="J10" s="127"/>
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" s="73" customFormat="1" ht="15">
-      <c r="A11" s="155"/>
-      <c r="B11" s="155"/>
-      <c r="C11" s="155"/>
-      <c r="D11" s="155"/>
-      <c r="E11" s="155"/>
-      <c r="F11" s="155"/>
-      <c r="G11" s="155"/>
-      <c r="H11" s="155"/>
-      <c r="I11" s="155"/>
-      <c r="J11" s="156"/>
+      <c r="A11" s="159"/>
+      <c r="B11" s="159"/>
+      <c r="C11" s="159"/>
+      <c r="D11" s="159"/>
+      <c r="E11" s="159"/>
+      <c r="F11" s="159"/>
+      <c r="G11" s="159"/>
+      <c r="H11" s="159"/>
+      <c r="I11" s="159"/>
+      <c r="J11" s="160"/>
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A12" s="144" t="s">
+      <c r="A12" s="139" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="145"/>
-      <c r="C12" s="145"/>
-      <c r="D12" s="145"/>
-      <c r="E12" s="145"/>
-      <c r="F12" s="145"/>
-      <c r="G12" s="145"/>
-      <c r="H12" s="145"/>
-      <c r="I12" s="145"/>
-      <c r="J12" s="146"/>
+      <c r="B12" s="140"/>
+      <c r="C12" s="140"/>
+      <c r="D12" s="140"/>
+      <c r="E12" s="140"/>
+      <c r="F12" s="140"/>
+      <c r="G12" s="140"/>
+      <c r="H12" s="140"/>
+      <c r="I12" s="140"/>
+      <c r="J12" s="152"/>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" ht="350.1" customHeight="1" outlineLevel="1">
       <c r="A13" s="77" t="s">
@@ -6126,9 +6204,9 @@
       <c r="C13" s="76" t="s">
         <v>200</v>
       </c>
-      <c r="D13" s="128"/>
-      <c r="E13" s="129"/>
-      <c r="F13" s="129"/>
+      <c r="D13" s="125"/>
+      <c r="E13" s="126"/>
+      <c r="F13" s="126"/>
       <c r="G13" s="75"/>
       <c r="H13" s="116">
         <v>45755</v>
@@ -6148,9 +6226,9 @@
       <c r="C14" s="76" t="s">
         <v>199</v>
       </c>
-      <c r="D14" s="128"/>
-      <c r="E14" s="129"/>
-      <c r="F14" s="129"/>
+      <c r="D14" s="125"/>
+      <c r="E14" s="126"/>
+      <c r="F14" s="126"/>
       <c r="G14" s="75"/>
       <c r="H14" s="116">
         <v>45755</v>
@@ -6170,9 +6248,9 @@
       <c r="C15" s="76" t="s">
         <v>198</v>
       </c>
-      <c r="D15" s="128"/>
-      <c r="E15" s="129"/>
-      <c r="F15" s="129"/>
+      <c r="D15" s="125"/>
+      <c r="E15" s="126"/>
+      <c r="F15" s="126"/>
       <c r="G15" s="75"/>
       <c r="H15" s="116">
         <v>45755</v>
@@ -6194,9 +6272,9 @@
       <c r="C16" s="76" t="s">
         <v>197</v>
       </c>
-      <c r="D16" s="128"/>
-      <c r="E16" s="129"/>
-      <c r="F16" s="129"/>
+      <c r="D16" s="125"/>
+      <c r="E16" s="126"/>
+      <c r="F16" s="126"/>
       <c r="G16" s="75"/>
       <c r="H16" s="116">
         <v>45755</v>
@@ -6216,9 +6294,9 @@
       <c r="C17" s="76" t="s">
         <v>196</v>
       </c>
-      <c r="D17" s="128"/>
-      <c r="E17" s="129"/>
-      <c r="F17" s="129"/>
+      <c r="D17" s="125"/>
+      <c r="E17" s="126"/>
+      <c r="F17" s="126"/>
       <c r="G17" s="75"/>
       <c r="H17" s="116">
         <v>45755</v>
@@ -6238,9 +6316,9 @@
       <c r="C18" s="86" t="s">
         <v>195</v>
       </c>
-      <c r="D18" s="128"/>
-      <c r="E18" s="129"/>
-      <c r="F18" s="129"/>
+      <c r="D18" s="125"/>
+      <c r="E18" s="126"/>
+      <c r="F18" s="126"/>
       <c r="G18" s="75"/>
       <c r="H18" s="116">
         <v>45755</v>
@@ -6262,9 +6340,9 @@
       <c r="C19" s="86" t="s">
         <v>194</v>
       </c>
-      <c r="D19" s="128"/>
-      <c r="E19" s="129"/>
-      <c r="F19" s="129"/>
+      <c r="D19" s="125"/>
+      <c r="E19" s="126"/>
+      <c r="F19" s="126"/>
       <c r="G19" s="75"/>
       <c r="H19" s="116">
         <v>45755</v>
@@ -6286,9 +6364,9 @@
       <c r="C20" s="76" t="s">
         <v>192</v>
       </c>
-      <c r="D20" s="128"/>
-      <c r="E20" s="129"/>
-      <c r="F20" s="129"/>
+      <c r="D20" s="125"/>
+      <c r="E20" s="126"/>
+      <c r="F20" s="126"/>
       <c r="G20" s="75"/>
       <c r="H20" s="116">
         <v>45755</v>
@@ -6310,9 +6388,9 @@
       <c r="C21" s="76" t="s">
         <v>191</v>
       </c>
-      <c r="D21" s="128"/>
-      <c r="E21" s="129"/>
-      <c r="F21" s="129"/>
+      <c r="D21" s="125"/>
+      <c r="E21" s="126"/>
+      <c r="F21" s="126"/>
       <c r="G21" s="75"/>
       <c r="H21" s="116">
         <v>45755</v>
@@ -6334,9 +6412,9 @@
       <c r="C22" s="86" t="s">
         <v>193</v>
       </c>
-      <c r="D22" s="128"/>
-      <c r="E22" s="129"/>
-      <c r="F22" s="129"/>
+      <c r="D22" s="125"/>
+      <c r="E22" s="126"/>
+      <c r="F22" s="126"/>
       <c r="G22" s="75"/>
       <c r="H22" s="116">
         <v>45755</v>
@@ -6349,11 +6427,11 @@
       </c>
     </row>
     <row r="23" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A23" s="144" t="s">
+      <c r="A23" s="139" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="145"/>
-      <c r="C23" s="145"/>
+      <c r="B23" s="140"/>
+      <c r="C23" s="140"/>
       <c r="D23" s="87"/>
       <c r="E23" s="87"/>
       <c r="F23" s="87"/>
@@ -6372,9 +6450,9 @@
       <c r="C24" s="86" t="s">
         <v>228</v>
       </c>
-      <c r="D24" s="160"/>
-      <c r="E24" s="161"/>
-      <c r="F24" s="161"/>
+      <c r="D24" s="130"/>
+      <c r="E24" s="131"/>
+      <c r="F24" s="131"/>
       <c r="G24" s="94"/>
       <c r="H24" s="115">
         <v>45756</v>
@@ -6394,9 +6472,9 @@
       <c r="C25" s="86" t="s">
         <v>227</v>
       </c>
-      <c r="D25" s="160"/>
-      <c r="E25" s="161"/>
-      <c r="F25" s="161"/>
+      <c r="D25" s="130"/>
+      <c r="E25" s="131"/>
+      <c r="F25" s="131"/>
       <c r="G25" s="94"/>
       <c r="H25" s="115">
         <v>45755</v>
@@ -6418,9 +6496,9 @@
       <c r="C26" s="86" t="s">
         <v>232</v>
       </c>
-      <c r="D26" s="134"/>
-      <c r="E26" s="135"/>
-      <c r="F26" s="135"/>
+      <c r="D26" s="141"/>
+      <c r="E26" s="142"/>
+      <c r="F26" s="142"/>
       <c r="G26" s="94"/>
       <c r="H26" s="115">
         <v>45756</v>
@@ -6440,9 +6518,9 @@
       <c r="C27" s="86" t="s">
         <v>233</v>
       </c>
-      <c r="D27" s="125"/>
-      <c r="E27" s="126"/>
-      <c r="F27" s="127"/>
+      <c r="D27" s="143"/>
+      <c r="E27" s="144"/>
+      <c r="F27" s="145"/>
       <c r="G27" s="94"/>
       <c r="H27" s="115">
         <v>45755</v>
@@ -6462,9 +6540,9 @@
       <c r="C28" s="86" t="s">
         <v>237</v>
       </c>
-      <c r="D28" s="125"/>
-      <c r="E28" s="126"/>
-      <c r="F28" s="127"/>
+      <c r="D28" s="143"/>
+      <c r="E28" s="144"/>
+      <c r="F28" s="145"/>
       <c r="G28" s="94"/>
       <c r="H28" s="115">
         <v>45756</v>
@@ -6486,9 +6564,9 @@
       <c r="C29" s="86" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="125"/>
-      <c r="E29" s="126"/>
-      <c r="F29" s="127"/>
+      <c r="D29" s="143"/>
+      <c r="E29" s="144"/>
+      <c r="F29" s="145"/>
       <c r="G29" s="94"/>
       <c r="H29" s="115">
         <v>45756</v>
@@ -6510,9 +6588,9 @@
       <c r="C30" s="86" t="s">
         <v>234</v>
       </c>
-      <c r="D30" s="125"/>
-      <c r="E30" s="126"/>
-      <c r="F30" s="127"/>
+      <c r="D30" s="143"/>
+      <c r="E30" s="144"/>
+      <c r="F30" s="145"/>
       <c r="G30" s="94"/>
       <c r="H30" s="115">
         <v>45755</v>
@@ -6532,9 +6610,9 @@
       <c r="C31" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="125"/>
-      <c r="E31" s="126"/>
-      <c r="F31" s="127"/>
+      <c r="D31" s="143"/>
+      <c r="E31" s="144"/>
+      <c r="F31" s="145"/>
       <c r="G31" s="94"/>
       <c r="H31" s="115">
         <v>45756</v>
@@ -6556,9 +6634,9 @@
       <c r="C32" s="86" t="s">
         <v>70</v>
       </c>
-      <c r="D32" s="125"/>
-      <c r="E32" s="126"/>
-      <c r="F32" s="127"/>
+      <c r="D32" s="143"/>
+      <c r="E32" s="144"/>
+      <c r="F32" s="145"/>
       <c r="G32" s="94"/>
       <c r="H32" s="115">
         <v>45756</v>
@@ -6580,9 +6658,9 @@
       <c r="C33" s="86" t="s">
         <v>241</v>
       </c>
-      <c r="D33" s="128"/>
-      <c r="E33" s="129"/>
-      <c r="F33" s="130"/>
+      <c r="D33" s="125"/>
+      <c r="E33" s="126"/>
+      <c r="F33" s="163"/>
       <c r="G33" s="94"/>
       <c r="H33" s="115">
         <v>45755</v>
@@ -6602,9 +6680,9 @@
       <c r="C34" s="86" t="s">
         <v>201</v>
       </c>
-      <c r="D34" s="131"/>
-      <c r="E34" s="132"/>
-      <c r="F34" s="133"/>
+      <c r="D34" s="164"/>
+      <c r="E34" s="165"/>
+      <c r="F34" s="166"/>
       <c r="G34" s="94"/>
       <c r="H34" s="115">
         <v>45755</v>
@@ -6615,11 +6693,11 @@
       <c r="J34" s="96"/>
     </row>
     <row r="35" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A35" s="144" t="s">
+      <c r="A35" s="139" t="s">
         <v>71</v>
       </c>
-      <c r="B35" s="145"/>
-      <c r="C35" s="145"/>
+      <c r="B35" s="140"/>
+      <c r="C35" s="140"/>
       <c r="D35" s="87"/>
       <c r="E35" s="87"/>
       <c r="F35" s="87"/>
@@ -6638,20 +6716,20 @@
       <c r="C36" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="D36" s="134"/>
-      <c r="E36" s="135"/>
-      <c r="F36" s="135"/>
+      <c r="D36" s="141"/>
+      <c r="E36" s="142"/>
+      <c r="F36" s="142"/>
       <c r="G36" s="75"/>
       <c r="H36" s="82"/>
       <c r="I36" s="76"/>
       <c r="J36" s="74"/>
     </row>
     <row r="37" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A37" s="136" t="s">
+      <c r="A37" s="128" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="137"/>
-      <c r="C37" s="137"/>
+      <c r="B37" s="129"/>
+      <c r="C37" s="129"/>
       <c r="D37" s="97"/>
       <c r="E37" s="97"/>
       <c r="F37" s="97"/>
@@ -6670,9 +6748,9 @@
       <c r="C38" s="76" t="s">
         <v>113</v>
       </c>
-      <c r="D38" s="134"/>
-      <c r="E38" s="135"/>
-      <c r="F38" s="135"/>
+      <c r="D38" s="141"/>
+      <c r="E38" s="142"/>
+      <c r="F38" s="142"/>
       <c r="G38" s="75"/>
       <c r="H38" s="82"/>
       <c r="I38" s="76"/>
@@ -6688,9 +6766,9 @@
       <c r="C39" s="76" t="s">
         <v>115</v>
       </c>
-      <c r="D39" s="134"/>
-      <c r="E39" s="135"/>
-      <c r="F39" s="135"/>
+      <c r="D39" s="141"/>
+      <c r="E39" s="142"/>
+      <c r="F39" s="142"/>
       <c r="G39" s="75"/>
       <c r="H39" s="82"/>
       <c r="I39" s="76"/>
@@ -6706,9 +6784,9 @@
       <c r="C40" s="76" t="s">
         <v>114</v>
       </c>
-      <c r="D40" s="134"/>
-      <c r="E40" s="135"/>
-      <c r="F40" s="135"/>
+      <c r="D40" s="141"/>
+      <c r="E40" s="142"/>
+      <c r="F40" s="142"/>
       <c r="G40" s="75"/>
       <c r="H40" s="82"/>
       <c r="I40" s="76"/>
@@ -6724,9 +6802,9 @@
       <c r="C41" s="76" t="s">
         <v>117</v>
       </c>
-      <c r="D41" s="134"/>
-      <c r="E41" s="135"/>
-      <c r="F41" s="135"/>
+      <c r="D41" s="141"/>
+      <c r="E41" s="142"/>
+      <c r="F41" s="142"/>
       <c r="G41" s="75"/>
       <c r="H41" s="82"/>
       <c r="I41" s="76"/>
@@ -6742,20 +6820,20 @@
       <c r="C42" s="76" t="s">
         <v>119</v>
       </c>
-      <c r="D42" s="134"/>
-      <c r="E42" s="135"/>
-      <c r="F42" s="135"/>
+      <c r="D42" s="141"/>
+      <c r="E42" s="142"/>
+      <c r="F42" s="142"/>
       <c r="G42" s="75"/>
       <c r="H42" s="82"/>
       <c r="I42" s="76"/>
       <c r="J42" s="74"/>
     </row>
     <row r="43" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A43" s="136" t="s">
+      <c r="A43" s="128" t="s">
         <v>88</v>
       </c>
-      <c r="B43" s="137"/>
-      <c r="C43" s="137"/>
+      <c r="B43" s="129"/>
+      <c r="C43" s="129"/>
       <c r="D43" s="97"/>
       <c r="E43" s="97"/>
       <c r="F43" s="97"/>
@@ -6774,9 +6852,9 @@
       <c r="C44" s="76" t="s">
         <v>95</v>
       </c>
-      <c r="D44" s="134"/>
-      <c r="E44" s="135"/>
-      <c r="F44" s="135"/>
+      <c r="D44" s="141"/>
+      <c r="E44" s="142"/>
+      <c r="F44" s="142"/>
       <c r="G44" s="75"/>
       <c r="H44" s="82"/>
       <c r="I44" s="76"/>
@@ -6792,9 +6870,9 @@
       <c r="C45" s="76" t="s">
         <v>96</v>
       </c>
-      <c r="D45" s="134"/>
-      <c r="E45" s="135"/>
-      <c r="F45" s="135"/>
+      <c r="D45" s="141"/>
+      <c r="E45" s="142"/>
+      <c r="F45" s="142"/>
       <c r="G45" s="75"/>
       <c r="H45" s="82"/>
       <c r="I45" s="76"/>
@@ -6810,9 +6888,9 @@
       <c r="C46" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="D46" s="134"/>
-      <c r="E46" s="135"/>
-      <c r="F46" s="135"/>
+      <c r="D46" s="141"/>
+      <c r="E46" s="142"/>
+      <c r="F46" s="142"/>
       <c r="G46" s="75"/>
       <c r="H46" s="82"/>
       <c r="I46" s="76"/>
@@ -6828,9 +6906,9 @@
       <c r="C47" s="76" t="s">
         <v>98</v>
       </c>
-      <c r="D47" s="134"/>
-      <c r="E47" s="135"/>
-      <c r="F47" s="135"/>
+      <c r="D47" s="141"/>
+      <c r="E47" s="142"/>
+      <c r="F47" s="142"/>
       <c r="G47" s="75"/>
       <c r="H47" s="82"/>
       <c r="I47" s="76"/>
@@ -6846,9 +6924,9 @@
       <c r="C48" s="76" t="s">
         <v>100</v>
       </c>
-      <c r="D48" s="134"/>
-      <c r="E48" s="135"/>
-      <c r="F48" s="135"/>
+      <c r="D48" s="141"/>
+      <c r="E48" s="142"/>
+      <c r="F48" s="142"/>
       <c r="G48" s="75"/>
       <c r="H48" s="82"/>
       <c r="I48" s="76"/>
@@ -6864,20 +6942,20 @@
       <c r="C49" s="76" t="s">
         <v>92</v>
       </c>
-      <c r="D49" s="134"/>
-      <c r="E49" s="135"/>
-      <c r="F49" s="135"/>
+      <c r="D49" s="141"/>
+      <c r="E49" s="142"/>
+      <c r="F49" s="142"/>
       <c r="G49" s="75"/>
       <c r="H49" s="82"/>
       <c r="I49" s="76"/>
       <c r="J49" s="74"/>
     </row>
     <row r="50" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A50" s="136" t="s">
+      <c r="A50" s="128" t="s">
         <v>101</v>
       </c>
-      <c r="B50" s="137"/>
-      <c r="C50" s="137"/>
+      <c r="B50" s="129"/>
+      <c r="C50" s="129"/>
       <c r="D50" s="97"/>
       <c r="E50" s="97"/>
       <c r="F50" s="97"/>
@@ -6896,20 +6974,20 @@
       <c r="C51" s="76" t="s">
         <v>102</v>
       </c>
-      <c r="D51" s="134"/>
-      <c r="E51" s="135"/>
-      <c r="F51" s="135"/>
+      <c r="D51" s="141"/>
+      <c r="E51" s="142"/>
+      <c r="F51" s="142"/>
       <c r="G51" s="75"/>
       <c r="H51" s="82"/>
       <c r="I51" s="76"/>
       <c r="J51" s="74"/>
     </row>
     <row r="52" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A52" s="136" t="s">
-        <v>267</v>
-      </c>
-      <c r="B52" s="137"/>
-      <c r="C52" s="137"/>
+      <c r="A52" s="128" t="s">
+        <v>265</v>
+      </c>
+      <c r="B52" s="129"/>
+      <c r="C52" s="129"/>
       <c r="D52" s="97"/>
       <c r="E52" s="97"/>
       <c r="F52" s="97"/>
@@ -6923,14 +7001,14 @@
         <v>0</v>
       </c>
       <c r="B53" s="92" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C53" s="76" t="s">
-        <v>266</v>
-      </c>
-      <c r="D53" s="134"/>
-      <c r="E53" s="135"/>
-      <c r="F53" s="135"/>
+        <v>264</v>
+      </c>
+      <c r="D53" s="141"/>
+      <c r="E53" s="142"/>
+      <c r="F53" s="142"/>
       <c r="G53" s="75"/>
       <c r="H53" s="82"/>
       <c r="I53" s="76"/>
@@ -6941,23 +7019,23 @@
         <v>1</v>
       </c>
       <c r="B54" s="92" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C54" s="76" t="s">
-        <v>271</v>
-      </c>
-      <c r="D54" s="134"/>
-      <c r="E54" s="135"/>
-      <c r="F54" s="135"/>
+        <v>269</v>
+      </c>
+      <c r="D54" s="141"/>
+      <c r="E54" s="142"/>
+      <c r="F54" s="142"/>
       <c r="G54" s="75"/>
       <c r="H54" s="82"/>
       <c r="I54" s="76"/>
       <c r="J54" s="74"/>
     </row>
     <row r="55" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A55" s="136"/>
-      <c r="B55" s="137"/>
-      <c r="C55" s="137"/>
+      <c r="A55" s="128"/>
+      <c r="B55" s="129"/>
+      <c r="C55" s="129"/>
       <c r="D55" s="97"/>
       <c r="E55" s="97"/>
       <c r="F55" s="97"/>
@@ -6970,9 +7048,9 @@
       <c r="A56" s="77"/>
       <c r="B56" s="92"/>
       <c r="C56" s="76"/>
-      <c r="D56" s="134"/>
-      <c r="E56" s="135"/>
-      <c r="F56" s="135"/>
+      <c r="D56" s="141"/>
+      <c r="E56" s="142"/>
+      <c r="F56" s="142"/>
       <c r="G56" s="75"/>
       <c r="H56" s="82"/>
       <c r="I56" s="76"/>
@@ -7108,11 +7186,48 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="D54:F54"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="D56:F56"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="D51:F51"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="D53:F53"/>
+    <mergeCell ref="B1:D2"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="A37:C37"/>
     <mergeCell ref="D24:F24"/>
@@ -7129,48 +7244,11 @@
     <mergeCell ref="D20:F20"/>
     <mergeCell ref="D18:F18"/>
     <mergeCell ref="D22:F22"/>
-    <mergeCell ref="B1:D2"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="D56:F56"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="D51:F51"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="D48:F48"/>
-    <mergeCell ref="D53:F53"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="D54:F54"/>
-    <mergeCell ref="A55:C55"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D17:F17"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7187,7 +7265,7 @@
   </sheetPr>
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="82" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="82" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -7207,9 +7285,9 @@
       <c r="A1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="138"/>
-      <c r="C1" s="138"/>
-      <c r="D1" s="138"/>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -7220,9 +7298,9 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="139"/>
-      <c r="C2" s="139"/>
-      <c r="D2" s="139"/>
+      <c r="B2" s="147"/>
+      <c r="C2" s="147"/>
+      <c r="D2" s="147"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -7243,43 +7321,43 @@
       <c r="E3" s="60"/>
       <c r="F3" s="60"/>
       <c r="G3" s="60"/>
-      <c r="H3" s="148"/>
-      <c r="I3" s="148"/>
-      <c r="J3" s="148"/>
+      <c r="H3" s="154"/>
+      <c r="I3" s="154"/>
+      <c r="J3" s="154"/>
       <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="12.75">
       <c r="A4" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="150" t="s">
+      <c r="B4" s="155" t="s">
         <v>126</v>
       </c>
-      <c r="C4" s="151"/>
-      <c r="D4" s="152"/>
+      <c r="C4" s="156"/>
+      <c r="D4" s="157"/>
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
       <c r="G4" s="60"/>
-      <c r="H4" s="148"/>
-      <c r="I4" s="148"/>
-      <c r="J4" s="148"/>
+      <c r="H4" s="154"/>
+      <c r="I4" s="154"/>
+      <c r="J4" s="154"/>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" s="70" customFormat="1" ht="25.5">
       <c r="A5" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="141" t="s">
+      <c r="B5" s="149" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="142"/>
-      <c r="D5" s="143"/>
+      <c r="C5" s="150"/>
+      <c r="D5" s="151"/>
       <c r="E5" s="68"/>
       <c r="F5" s="68"/>
       <c r="G5" s="68"/>
-      <c r="H5" s="147"/>
-      <c r="I5" s="147"/>
-      <c r="J5" s="147"/>
+      <c r="H5" s="153"/>
+      <c r="I5" s="153"/>
+      <c r="J5" s="153"/>
       <c r="K5" s="69"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
@@ -7300,9 +7378,9 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="148"/>
-      <c r="I6" s="148"/>
-      <c r="J6" s="148"/>
+      <c r="H6" s="154"/>
+      <c r="I6" s="154"/>
+      <c r="J6" s="154"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -7323,16 +7401,16 @@
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
       <c r="G7" s="61"/>
-      <c r="H7" s="148"/>
-      <c r="I7" s="148"/>
-      <c r="J7" s="148"/>
+      <c r="H7" s="154"/>
+      <c r="I7" s="154"/>
+      <c r="J7" s="154"/>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="140"/>
-      <c r="B8" s="140"/>
-      <c r="C8" s="140"/>
-      <c r="D8" s="140"/>
+      <c r="A8" s="148"/>
+      <c r="B8" s="148"/>
+      <c r="C8" s="148"/>
+      <c r="D8" s="148"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -7342,70 +7420,70 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" s="72" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="157" t="s">
+      <c r="A9" s="132" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="158" t="s">
+      <c r="B9" s="161" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="157" t="s">
+      <c r="C9" s="132" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="162" t="s">
+      <c r="D9" s="133" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="163"/>
-      <c r="F9" s="163"/>
-      <c r="G9" s="164"/>
-      <c r="H9" s="153" t="s">
+      <c r="E9" s="134"/>
+      <c r="F9" s="134"/>
+      <c r="G9" s="135"/>
+      <c r="H9" s="158" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="149" t="s">
+      <c r="I9" s="127" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="149" t="s">
+      <c r="J9" s="127" t="s">
         <v>32</v>
       </c>
       <c r="K9" s="71"/>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="149"/>
-      <c r="B10" s="159"/>
-      <c r="C10" s="149"/>
-      <c r="D10" s="154"/>
-      <c r="E10" s="165"/>
-      <c r="F10" s="165"/>
-      <c r="G10" s="166"/>
-      <c r="H10" s="154"/>
-      <c r="I10" s="149"/>
-      <c r="J10" s="149"/>
+      <c r="A10" s="127"/>
+      <c r="B10" s="162"/>
+      <c r="C10" s="127"/>
+      <c r="D10" s="136"/>
+      <c r="E10" s="137"/>
+      <c r="F10" s="137"/>
+      <c r="G10" s="138"/>
+      <c r="H10" s="136"/>
+      <c r="I10" s="127"/>
+      <c r="J10" s="127"/>
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" s="73" customFormat="1" ht="15">
-      <c r="A11" s="155"/>
-      <c r="B11" s="155"/>
-      <c r="C11" s="155"/>
-      <c r="D11" s="155"/>
-      <c r="E11" s="155"/>
-      <c r="F11" s="155"/>
-      <c r="G11" s="155"/>
-      <c r="H11" s="155"/>
-      <c r="I11" s="155"/>
-      <c r="J11" s="156"/>
+      <c r="A11" s="159"/>
+      <c r="B11" s="159"/>
+      <c r="C11" s="159"/>
+      <c r="D11" s="159"/>
+      <c r="E11" s="159"/>
+      <c r="F11" s="159"/>
+      <c r="G11" s="159"/>
+      <c r="H11" s="159"/>
+      <c r="I11" s="159"/>
+      <c r="J11" s="160"/>
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A12" s="144" t="s">
+      <c r="A12" s="139" t="s">
         <v>127</v>
       </c>
-      <c r="B12" s="145"/>
-      <c r="C12" s="145"/>
-      <c r="D12" s="145"/>
-      <c r="E12" s="145"/>
-      <c r="F12" s="145"/>
-      <c r="G12" s="145"/>
-      <c r="H12" s="145"/>
-      <c r="I12" s="145"/>
-      <c r="J12" s="146"/>
+      <c r="B12" s="140"/>
+      <c r="C12" s="140"/>
+      <c r="D12" s="140"/>
+      <c r="E12" s="140"/>
+      <c r="F12" s="140"/>
+      <c r="G12" s="140"/>
+      <c r="H12" s="140"/>
+      <c r="I12" s="140"/>
+      <c r="J12" s="152"/>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" ht="102.75" customHeight="1" outlineLevel="1">
       <c r="A13" s="77" t="s">
@@ -7417,11 +7495,11 @@
       <c r="C13" s="76" t="s">
         <v>165</v>
       </c>
-      <c r="D13" s="128" t="s">
+      <c r="D13" s="125" t="s">
         <v>166</v>
       </c>
-      <c r="E13" s="129"/>
-      <c r="F13" s="129"/>
+      <c r="E13" s="126"/>
+      <c r="F13" s="126"/>
       <c r="G13" s="75"/>
       <c r="H13" s="89"/>
       <c r="I13" s="76"/>
@@ -7437,11 +7515,11 @@
       <c r="C14" s="76" t="s">
         <v>169</v>
       </c>
-      <c r="D14" s="128" t="s">
+      <c r="D14" s="125" t="s">
         <v>170</v>
       </c>
-      <c r="E14" s="129"/>
-      <c r="F14" s="129"/>
+      <c r="E14" s="126"/>
+      <c r="F14" s="126"/>
       <c r="G14" s="75"/>
       <c r="H14" s="89"/>
       <c r="I14" s="76"/>
@@ -7457,22 +7535,22 @@
       <c r="C15" s="76" t="s">
         <v>172</v>
       </c>
-      <c r="D15" s="128" t="s">
+      <c r="D15" s="125" t="s">
         <v>173</v>
       </c>
-      <c r="E15" s="129"/>
-      <c r="F15" s="129"/>
+      <c r="E15" s="126"/>
+      <c r="F15" s="126"/>
       <c r="G15" s="75"/>
       <c r="H15" s="89"/>
       <c r="I15" s="76"/>
       <c r="J15" s="74"/>
     </row>
     <row r="16" spans="1:11" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A16" s="144" t="s">
+      <c r="A16" s="139" t="s">
         <v>128</v>
       </c>
-      <c r="B16" s="145"/>
-      <c r="C16" s="145"/>
+      <c r="B16" s="140"/>
+      <c r="C16" s="140"/>
       <c r="D16" s="87"/>
       <c r="E16" s="87"/>
       <c r="F16" s="87"/>
@@ -7542,11 +7620,11 @@
       <c r="J19" s="96"/>
     </row>
     <row r="20" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A20" s="144" t="s">
+      <c r="A20" s="139" t="s">
         <v>145</v>
       </c>
-      <c r="B20" s="145"/>
-      <c r="C20" s="145"/>
+      <c r="B20" s="140"/>
+      <c r="C20" s="140"/>
       <c r="D20" s="87"/>
       <c r="E20" s="87"/>
       <c r="F20" s="87"/>
@@ -7565,11 +7643,11 @@
       <c r="C21" s="76" t="s">
         <v>149</v>
       </c>
-      <c r="D21" s="128" t="s">
+      <c r="D21" s="125" t="s">
         <v>147</v>
       </c>
-      <c r="E21" s="129"/>
-      <c r="F21" s="129"/>
+      <c r="E21" s="126"/>
+      <c r="F21" s="126"/>
       <c r="G21" s="75"/>
       <c r="H21" s="82"/>
       <c r="I21" s="76"/>
@@ -7585,11 +7663,11 @@
       <c r="C22" s="76" t="s">
         <v>150</v>
       </c>
-      <c r="D22" s="128" t="s">
+      <c r="D22" s="125" t="s">
         <v>151</v>
       </c>
-      <c r="E22" s="129"/>
-      <c r="F22" s="129"/>
+      <c r="E22" s="126"/>
+      <c r="F22" s="126"/>
       <c r="G22" s="75"/>
       <c r="H22" s="82"/>
       <c r="I22" s="76"/>
@@ -7605,11 +7683,11 @@
       <c r="C23" s="76" t="s">
         <v>153</v>
       </c>
-      <c r="D23" s="128" t="s">
+      <c r="D23" s="125" t="s">
         <v>154</v>
       </c>
-      <c r="E23" s="129"/>
-      <c r="F23" s="129"/>
+      <c r="E23" s="126"/>
+      <c r="F23" s="126"/>
       <c r="G23" s="75"/>
       <c r="H23" s="82"/>
       <c r="I23" s="76"/>
@@ -7625,20 +7703,20 @@
       <c r="C24" s="76" t="s">
         <v>156</v>
       </c>
-      <c r="D24" s="128" t="s">
+      <c r="D24" s="125" t="s">
         <v>157</v>
       </c>
-      <c r="E24" s="129"/>
-      <c r="F24" s="129"/>
+      <c r="E24" s="126"/>
+      <c r="F24" s="126"/>
       <c r="G24" s="75"/>
       <c r="H24" s="82"/>
       <c r="I24" s="76"/>
       <c r="J24" s="74"/>
     </row>
     <row r="25" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A25" s="136"/>
-      <c r="B25" s="137"/>
-      <c r="C25" s="137"/>
+      <c r="A25" s="128"/>
+      <c r="B25" s="129"/>
+      <c r="C25" s="129"/>
       <c r="D25" s="97"/>
       <c r="E25" s="97"/>
       <c r="F25" s="97"/>
@@ -7651,9 +7729,9 @@
       <c r="A26" s="77"/>
       <c r="B26" s="92"/>
       <c r="C26" s="76"/>
-      <c r="D26" s="134"/>
-      <c r="E26" s="135"/>
-      <c r="F26" s="135"/>
+      <c r="D26" s="141"/>
+      <c r="E26" s="142"/>
+      <c r="F26" s="142"/>
       <c r="G26" s="75"/>
       <c r="H26" s="82"/>
       <c r="I26" s="76"/>
@@ -7663,9 +7741,9 @@
       <c r="A27" s="77"/>
       <c r="B27" s="92"/>
       <c r="C27" s="76"/>
-      <c r="D27" s="134"/>
-      <c r="E27" s="135"/>
-      <c r="F27" s="135"/>
+      <c r="D27" s="141"/>
+      <c r="E27" s="142"/>
+      <c r="F27" s="142"/>
       <c r="G27" s="75"/>
       <c r="H27" s="82"/>
       <c r="I27" s="76"/>
@@ -7675,9 +7753,9 @@
       <c r="A28" s="77"/>
       <c r="B28" s="92"/>
       <c r="C28" s="76"/>
-      <c r="D28" s="134"/>
-      <c r="E28" s="135"/>
-      <c r="F28" s="135"/>
+      <c r="D28" s="141"/>
+      <c r="E28" s="142"/>
+      <c r="F28" s="142"/>
       <c r="G28" s="75"/>
       <c r="H28" s="82"/>
       <c r="I28" s="76"/>
@@ -7687,9 +7765,9 @@
       <c r="A29" s="77"/>
       <c r="B29" s="92"/>
       <c r="C29" s="76"/>
-      <c r="D29" s="134"/>
-      <c r="E29" s="135"/>
-      <c r="F29" s="135"/>
+      <c r="D29" s="141"/>
+      <c r="E29" s="142"/>
+      <c r="F29" s="142"/>
       <c r="G29" s="75"/>
       <c r="H29" s="82"/>
       <c r="I29" s="76"/>
@@ -7699,9 +7777,9 @@
       <c r="A30" s="77"/>
       <c r="B30" s="92"/>
       <c r="C30" s="76"/>
-      <c r="D30" s="134"/>
-      <c r="E30" s="135"/>
-      <c r="F30" s="135"/>
+      <c r="D30" s="141"/>
+      <c r="E30" s="142"/>
+      <c r="F30" s="142"/>
       <c r="G30" s="75"/>
       <c r="H30" s="82"/>
       <c r="I30" s="76"/>
@@ -7711,18 +7789,18 @@
       <c r="A31" s="77"/>
       <c r="B31" s="92"/>
       <c r="C31" s="76"/>
-      <c r="D31" s="134"/>
-      <c r="E31" s="135"/>
-      <c r="F31" s="135"/>
+      <c r="D31" s="141"/>
+      <c r="E31" s="142"/>
+      <c r="F31" s="142"/>
       <c r="G31" s="75"/>
       <c r="H31" s="82"/>
       <c r="I31" s="76"/>
       <c r="J31" s="74"/>
     </row>
     <row r="32" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A32" s="136"/>
-      <c r="B32" s="137"/>
-      <c r="C32" s="137"/>
+      <c r="A32" s="128"/>
+      <c r="B32" s="129"/>
+      <c r="C32" s="129"/>
       <c r="D32" s="97"/>
       <c r="E32" s="97"/>
       <c r="F32" s="97"/>
@@ -7735,9 +7813,9 @@
       <c r="A33" s="77"/>
       <c r="B33" s="92"/>
       <c r="C33" s="76"/>
-      <c r="D33" s="134"/>
-      <c r="E33" s="135"/>
-      <c r="F33" s="135"/>
+      <c r="D33" s="141"/>
+      <c r="E33" s="142"/>
+      <c r="F33" s="142"/>
       <c r="G33" s="75"/>
       <c r="H33" s="82"/>
       <c r="I33" s="76"/>
@@ -7873,6 +7951,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:G10"/>
     <mergeCell ref="D19:F19"/>
     <mergeCell ref="B1:D2"/>
     <mergeCell ref="B3:D3"/>
@@ -7889,30 +7991,6 @@
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="H6:J6"/>
     <mergeCell ref="H7:J7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -7925,10 +8003,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K65"/>
+  <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="80" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A21" zoomScale="80" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" outlineLevelRow="1"/>
@@ -7947,9 +8025,9 @@
       <c r="A1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="138"/>
-      <c r="C1" s="138"/>
-      <c r="D1" s="138"/>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -7960,9 +8038,9 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="139"/>
-      <c r="C2" s="139"/>
-      <c r="D2" s="139"/>
+      <c r="B2" s="147"/>
+      <c r="C2" s="147"/>
+      <c r="D2" s="147"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -7983,43 +8061,43 @@
       <c r="E3" s="60"/>
       <c r="F3" s="60"/>
       <c r="G3" s="60"/>
-      <c r="H3" s="148"/>
-      <c r="I3" s="148"/>
-      <c r="J3" s="148"/>
+      <c r="H3" s="154"/>
+      <c r="I3" s="154"/>
+      <c r="J3" s="154"/>
       <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="12.75">
       <c r="A4" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="150" t="s">
+      <c r="B4" s="155" t="s">
         <v>248</v>
       </c>
-      <c r="C4" s="151"/>
-      <c r="D4" s="152"/>
+      <c r="C4" s="156"/>
+      <c r="D4" s="157"/>
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
       <c r="G4" s="60"/>
-      <c r="H4" s="148"/>
-      <c r="I4" s="148"/>
-      <c r="J4" s="148"/>
+      <c r="H4" s="154"/>
+      <c r="I4" s="154"/>
+      <c r="J4" s="154"/>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" s="70" customFormat="1" ht="25.5">
       <c r="A5" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="141" t="s">
+      <c r="B5" s="149" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="142"/>
-      <c r="D5" s="143"/>
+      <c r="C5" s="150"/>
+      <c r="D5" s="151"/>
       <c r="E5" s="68"/>
       <c r="F5" s="68"/>
       <c r="G5" s="68"/>
-      <c r="H5" s="147"/>
-      <c r="I5" s="147"/>
-      <c r="J5" s="147"/>
+      <c r="H5" s="153"/>
+      <c r="I5" s="153"/>
+      <c r="J5" s="153"/>
       <c r="K5" s="69"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
@@ -8027,22 +8105,22 @@
         <v>38</v>
       </c>
       <c r="B6" s="79">
-        <f>COUNTIF(I12:I24,"Pass")</f>
+        <f>COUNTIF(I12:I27,"Pass")</f>
         <v>0</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>39</v>
       </c>
       <c r="D6" s="13">
-        <f>COUNTIF(I10:I730,"Pending")</f>
+        <f>COUNTIF(I10:I733,"Pending")</f>
         <v>0</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="148"/>
-      <c r="I6" s="148"/>
-      <c r="J6" s="148"/>
+      <c r="H6" s="154"/>
+      <c r="I6" s="154"/>
+      <c r="J6" s="154"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -8050,29 +8128,29 @@
         <v>3</v>
       </c>
       <c r="B7" s="80">
-        <f>COUNTIF(I12:I24,"Fail")</f>
+        <f>COUNTIF(I12:I27,"Fail")</f>
         <v>0</v>
       </c>
       <c r="C7" s="29" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="58">
-        <f>COUNTA(A12:A33) -3</f>
-        <v>8</v>
+        <f>COUNTA(A12:A36) -3</f>
+        <v>13</v>
       </c>
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
       <c r="G7" s="61"/>
-      <c r="H7" s="148"/>
-      <c r="I7" s="148"/>
-      <c r="J7" s="148"/>
+      <c r="H7" s="154"/>
+      <c r="I7" s="154"/>
+      <c r="J7" s="154"/>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="140"/>
-      <c r="B8" s="140"/>
-      <c r="C8" s="140"/>
-      <c r="D8" s="140"/>
+      <c r="A8" s="148"/>
+      <c r="B8" s="148"/>
+      <c r="C8" s="148"/>
+      <c r="D8" s="148"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -8082,84 +8160,84 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" s="72" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="157" t="s">
+      <c r="A9" s="132" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="158" t="s">
+      <c r="B9" s="161" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="157" t="s">
+      <c r="C9" s="132" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="162" t="s">
+      <c r="D9" s="133" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="163"/>
-      <c r="F9" s="163"/>
-      <c r="G9" s="164"/>
-      <c r="H9" s="153" t="s">
+      <c r="E9" s="134"/>
+      <c r="F9" s="134"/>
+      <c r="G9" s="135"/>
+      <c r="H9" s="158" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="149" t="s">
+      <c r="I9" s="127" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="149" t="s">
+      <c r="J9" s="127" t="s">
         <v>32</v>
       </c>
       <c r="K9" s="71"/>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="149"/>
-      <c r="B10" s="159"/>
-      <c r="C10" s="149"/>
-      <c r="D10" s="154"/>
-      <c r="E10" s="165"/>
-      <c r="F10" s="165"/>
-      <c r="G10" s="166"/>
-      <c r="H10" s="154"/>
-      <c r="I10" s="149"/>
-      <c r="J10" s="149"/>
+      <c r="A10" s="127"/>
+      <c r="B10" s="162"/>
+      <c r="C10" s="127"/>
+      <c r="D10" s="136"/>
+      <c r="E10" s="137"/>
+      <c r="F10" s="137"/>
+      <c r="G10" s="138"/>
+      <c r="H10" s="136"/>
+      <c r="I10" s="127"/>
+      <c r="J10" s="127"/>
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" s="73" customFormat="1" ht="15">
-      <c r="A11" s="155"/>
-      <c r="B11" s="155"/>
-      <c r="C11" s="155"/>
-      <c r="D11" s="155"/>
-      <c r="E11" s="155"/>
-      <c r="F11" s="155"/>
-      <c r="G11" s="155"/>
-      <c r="H11" s="155"/>
-      <c r="I11" s="155"/>
-      <c r="J11" s="156"/>
+      <c r="A11" s="159"/>
+      <c r="B11" s="159"/>
+      <c r="C11" s="159"/>
+      <c r="D11" s="159"/>
+      <c r="E11" s="159"/>
+      <c r="F11" s="159"/>
+      <c r="G11" s="159"/>
+      <c r="H11" s="159"/>
+      <c r="I11" s="159"/>
+      <c r="J11" s="160"/>
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A12" s="144" t="s">
-        <v>249</v>
-      </c>
-      <c r="B12" s="145"/>
-      <c r="C12" s="145"/>
-      <c r="D12" s="145"/>
-      <c r="E12" s="145"/>
-      <c r="F12" s="145"/>
-      <c r="G12" s="145"/>
-      <c r="H12" s="145"/>
-      <c r="I12" s="145"/>
-      <c r="J12" s="146"/>
+      <c r="A12" s="139" t="s">
+        <v>278</v>
+      </c>
+      <c r="B12" s="140"/>
+      <c r="C12" s="140"/>
+      <c r="D12" s="140"/>
+      <c r="E12" s="140"/>
+      <c r="F12" s="140"/>
+      <c r="G12" s="140"/>
+      <c r="H12" s="140"/>
+      <c r="I12" s="140"/>
+      <c r="J12" s="152"/>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" ht="132.75" customHeight="1" outlineLevel="1">
       <c r="A13" s="77" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="81" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C13" s="122" t="s">
-        <v>252</v>
-      </c>
-      <c r="D13" s="128"/>
-      <c r="E13" s="129"/>
-      <c r="F13" s="129"/>
+        <v>251</v>
+      </c>
+      <c r="D13" s="125"/>
+      <c r="E13" s="126"/>
+      <c r="F13" s="126"/>
       <c r="G13" s="75"/>
       <c r="H13" s="89"/>
       <c r="I13" s="76"/>
@@ -8170,14 +8248,14 @@
         <v>1</v>
       </c>
       <c r="B14" s="81" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C14" s="122" t="s">
-        <v>253</v>
-      </c>
-      <c r="D14" s="128"/>
-      <c r="E14" s="129"/>
-      <c r="F14" s="129"/>
+        <v>252</v>
+      </c>
+      <c r="D14" s="125"/>
+      <c r="E14" s="126"/>
+      <c r="F14" s="126"/>
       <c r="G14" s="75"/>
       <c r="H14" s="89"/>
       <c r="I14" s="76"/>
@@ -8188,25 +8266,25 @@
         <v>2</v>
       </c>
       <c r="B15" s="81" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C15" s="76" t="s">
-        <v>262</v>
-      </c>
-      <c r="D15" s="128"/>
-      <c r="E15" s="129"/>
-      <c r="F15" s="129"/>
+        <v>260</v>
+      </c>
+      <c r="D15" s="125"/>
+      <c r="E15" s="126"/>
+      <c r="F15" s="126"/>
       <c r="G15" s="75"/>
       <c r="H15" s="89"/>
       <c r="I15" s="76"/>
       <c r="J15" s="74"/>
     </row>
     <row r="16" spans="1:11" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A16" s="144" t="s">
-        <v>256</v>
-      </c>
-      <c r="B16" s="145"/>
-      <c r="C16" s="145"/>
+      <c r="A16" s="139" t="s">
+        <v>279</v>
+      </c>
+      <c r="B16" s="140"/>
+      <c r="C16" s="140"/>
       <c r="D16" s="87"/>
       <c r="E16" s="87"/>
       <c r="F16" s="87"/>
@@ -8215,10 +8293,16 @@
       <c r="I16" s="87"/>
       <c r="J16" s="88"/>
     </row>
-    <row r="17" spans="1:10" s="4" customFormat="1" ht="79.5" customHeight="1" outlineLevel="1">
-      <c r="A17" s="93"/>
-      <c r="B17" s="85"/>
-      <c r="C17" s="86"/>
+    <row r="17" spans="1:10" s="4" customFormat="1" ht="138" customHeight="1" outlineLevel="1">
+      <c r="A17" s="93" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="85" t="s">
+        <v>284</v>
+      </c>
+      <c r="C17" s="86" t="s">
+        <v>286</v>
+      </c>
       <c r="D17" s="167"/>
       <c r="E17" s="168"/>
       <c r="F17" s="168"/>
@@ -8227,15 +8311,15 @@
       <c r="I17" s="86"/>
       <c r="J17" s="96"/>
     </row>
-    <row r="18" spans="1:10" s="4" customFormat="1" ht="124.5" customHeight="1" outlineLevel="1">
+    <row r="18" spans="1:10" s="4" customFormat="1" ht="138" customHeight="1" outlineLevel="1">
       <c r="A18" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="92" t="s">
-        <v>264</v>
-      </c>
-      <c r="C18" s="76" t="s">
-        <v>272</v>
+      <c r="B18" s="85" t="s">
+        <v>285</v>
+      </c>
+      <c r="C18" s="86" t="s">
+        <v>287</v>
       </c>
       <c r="D18" s="167"/>
       <c r="E18" s="168"/>
@@ -8245,10 +8329,16 @@
       <c r="I18" s="86"/>
       <c r="J18" s="96"/>
     </row>
-    <row r="19" spans="1:10" s="4" customFormat="1" ht="79.5" customHeight="1" outlineLevel="1">
-      <c r="A19" s="93"/>
-      <c r="B19" s="85"/>
-      <c r="C19" s="86"/>
+    <row r="19" spans="1:10" s="4" customFormat="1" ht="124.5" customHeight="1" outlineLevel="1">
+      <c r="A19" s="93" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="92" t="s">
+        <v>262</v>
+      </c>
+      <c r="C19" s="76" t="s">
+        <v>269</v>
+      </c>
       <c r="D19" s="167"/>
       <c r="E19" s="168"/>
       <c r="F19" s="168"/>
@@ -8257,211 +8347,253 @@
       <c r="I19" s="86"/>
       <c r="J19" s="96"/>
     </row>
-    <row r="20" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A20" s="144" t="s">
+    <row r="20" spans="1:10" s="4" customFormat="1" ht="123.75" customHeight="1" outlineLevel="1">
+      <c r="A20" s="93" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="85" t="s">
+        <v>281</v>
+      </c>
+      <c r="C20" s="86" t="s">
+        <v>282</v>
+      </c>
+      <c r="D20" s="167"/>
+      <c r="E20" s="168"/>
+      <c r="F20" s="168"/>
+      <c r="G20" s="94"/>
+      <c r="H20" s="95"/>
+      <c r="I20" s="86"/>
+      <c r="J20" s="96"/>
+    </row>
+    <row r="21" spans="1:10" s="4" customFormat="1" ht="179.25" customHeight="1" outlineLevel="1">
+      <c r="A21" s="93" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="85" t="s">
+        <v>280</v>
+      </c>
+      <c r="C21" s="169" t="s">
+        <v>283</v>
+      </c>
+      <c r="D21" s="167"/>
+      <c r="E21" s="168"/>
+      <c r="F21" s="168"/>
+      <c r="G21" s="94"/>
+      <c r="H21" s="95"/>
+      <c r="I21" s="86"/>
+      <c r="J21" s="96"/>
+    </row>
+    <row r="22" spans="1:10" s="4" customFormat="1" ht="179.25" customHeight="1" outlineLevel="1">
+      <c r="A22" s="93" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="85" t="s">
+        <v>280</v>
+      </c>
+      <c r="C22" s="169" t="s">
+        <v>283</v>
+      </c>
+      <c r="D22" s="170"/>
+      <c r="E22" s="171"/>
+      <c r="F22" s="171"/>
+      <c r="G22" s="94"/>
+      <c r="H22" s="95"/>
+      <c r="I22" s="86"/>
+      <c r="J22" s="96"/>
+    </row>
+    <row r="23" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
+      <c r="A23" s="139" t="s">
+        <v>255</v>
+      </c>
+      <c r="B23" s="140"/>
+      <c r="C23" s="140"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="87"/>
+      <c r="F23" s="87"/>
+      <c r="G23" s="87"/>
+      <c r="H23" s="87"/>
+      <c r="I23" s="87"/>
+      <c r="J23" s="88"/>
+    </row>
+    <row r="24" spans="1:10" s="4" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A24" s="77" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="92" t="s">
         <v>257</v>
       </c>
-      <c r="B20" s="145"/>
-      <c r="C20" s="145"/>
-      <c r="D20" s="87"/>
-      <c r="E20" s="87"/>
-      <c r="F20" s="87"/>
-      <c r="G20" s="87"/>
-      <c r="H20" s="87"/>
-      <c r="I20" s="87"/>
-      <c r="J20" s="88"/>
-    </row>
-    <row r="21" spans="1:10" s="4" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A21" s="77" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="92" t="s">
-        <v>259</v>
-      </c>
-      <c r="C21" s="76" t="s">
-        <v>260</v>
-      </c>
-      <c r="D21" s="128"/>
-      <c r="E21" s="129"/>
-      <c r="F21" s="129"/>
-      <c r="G21" s="75"/>
-      <c r="H21" s="82"/>
-      <c r="I21" s="76"/>
-      <c r="J21" s="74"/>
-    </row>
-    <row r="22" spans="1:10" s="4" customFormat="1" ht="148.5" customHeight="1" outlineLevel="1">
-      <c r="A22" s="77" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="92" t="s">
+      <c r="C24" s="76" t="s">
         <v>258</v>
       </c>
-      <c r="C22" s="76" t="s">
-        <v>262</v>
-      </c>
-      <c r="D22" s="128"/>
-      <c r="E22" s="129"/>
-      <c r="F22" s="129"/>
-      <c r="G22" s="75"/>
-      <c r="H22" s="82"/>
-      <c r="I22" s="76"/>
-      <c r="J22" s="74"/>
-    </row>
-    <row r="23" spans="1:10" s="4" customFormat="1" ht="123.75" customHeight="1" outlineLevel="1">
-      <c r="A23" s="77" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" s="92" t="s">
-        <v>263</v>
-      </c>
-      <c r="C23" s="76" t="s">
-        <v>271</v>
-      </c>
-      <c r="D23" s="128"/>
-      <c r="E23" s="129"/>
-      <c r="F23" s="129"/>
-      <c r="G23" s="75"/>
-      <c r="H23" s="82"/>
-      <c r="I23" s="76"/>
-      <c r="J23" s="74"/>
-    </row>
-    <row r="24" spans="1:10" s="4" customFormat="1" ht="148.5" customHeight="1" outlineLevel="1">
-      <c r="A24" s="77" t="s">
-        <v>49</v>
-      </c>
-      <c r="B24" s="92" t="s">
-        <v>265</v>
-      </c>
-      <c r="C24" s="76" t="s">
-        <v>268</v>
-      </c>
-      <c r="D24" s="128"/>
-      <c r="E24" s="129"/>
-      <c r="F24" s="129"/>
+      <c r="D24" s="125"/>
+      <c r="E24" s="126"/>
+      <c r="F24" s="126"/>
       <c r="G24" s="75"/>
       <c r="H24" s="82"/>
       <c r="I24" s="76"/>
       <c r="J24" s="74"/>
     </row>
-    <row r="25" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A25" s="136"/>
-      <c r="B25" s="137"/>
-      <c r="C25" s="137"/>
-      <c r="D25" s="97"/>
-      <c r="E25" s="97"/>
-      <c r="F25" s="97"/>
-      <c r="G25" s="97"/>
-      <c r="H25" s="97"/>
-      <c r="I25" s="97"/>
-      <c r="J25" s="98"/>
-    </row>
-    <row r="26" spans="1:10" s="4" customFormat="1" ht="78.75" customHeight="1" outlineLevel="1">
-      <c r="A26" s="77"/>
-      <c r="B26" s="92"/>
-      <c r="C26" s="76"/>
-      <c r="D26" s="134"/>
-      <c r="E26" s="135"/>
-      <c r="F26" s="135"/>
+    <row r="25" spans="1:10" s="4" customFormat="1" ht="148.5" customHeight="1" outlineLevel="1">
+      <c r="A25" s="77" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="92" t="s">
+        <v>256</v>
+      </c>
+      <c r="C25" s="76" t="s">
+        <v>260</v>
+      </c>
+      <c r="D25" s="125"/>
+      <c r="E25" s="126"/>
+      <c r="F25" s="126"/>
+      <c r="G25" s="75"/>
+      <c r="H25" s="82"/>
+      <c r="I25" s="76"/>
+      <c r="J25" s="74"/>
+    </row>
+    <row r="26" spans="1:10" s="4" customFormat="1" ht="123.75" customHeight="1" outlineLevel="1">
+      <c r="A26" s="77" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="92" t="s">
+        <v>261</v>
+      </c>
+      <c r="C26" s="76" t="s">
+        <v>269</v>
+      </c>
+      <c r="D26" s="125"/>
+      <c r="E26" s="126"/>
+      <c r="F26" s="126"/>
       <c r="G26" s="75"/>
       <c r="H26" s="82"/>
       <c r="I26" s="76"/>
       <c r="J26" s="74"/>
     </row>
-    <row r="27" spans="1:10" s="4" customFormat="1" ht="79.5" customHeight="1" outlineLevel="1">
-      <c r="A27" s="77"/>
-      <c r="B27" s="92"/>
-      <c r="C27" s="76"/>
-      <c r="D27" s="134"/>
-      <c r="E27" s="135"/>
-      <c r="F27" s="135"/>
+    <row r="27" spans="1:10" s="4" customFormat="1" ht="148.5" customHeight="1" outlineLevel="1">
+      <c r="A27" s="77" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="92" t="s">
+        <v>263</v>
+      </c>
+      <c r="C27" s="76" t="s">
+        <v>266</v>
+      </c>
+      <c r="D27" s="125"/>
+      <c r="E27" s="126"/>
+      <c r="F27" s="126"/>
       <c r="G27" s="75"/>
       <c r="H27" s="82"/>
       <c r="I27" s="76"/>
       <c r="J27" s="74"/>
     </row>
-    <row r="28" spans="1:10" s="4" customFormat="1" ht="79.5" customHeight="1" outlineLevel="1">
-      <c r="A28" s="77"/>
-      <c r="B28" s="92"/>
-      <c r="C28" s="76"/>
-      <c r="D28" s="134"/>
-      <c r="E28" s="135"/>
-      <c r="F28" s="135"/>
-      <c r="G28" s="75"/>
-      <c r="H28" s="82"/>
-      <c r="I28" s="76"/>
-      <c r="J28" s="74"/>
-    </row>
-    <row r="29" spans="1:10" s="4" customFormat="1" ht="79.5" customHeight="1" outlineLevel="1">
+    <row r="28" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
+      <c r="A28" s="128"/>
+      <c r="B28" s="129"/>
+      <c r="C28" s="129"/>
+      <c r="D28" s="97"/>
+      <c r="E28" s="97"/>
+      <c r="F28" s="97"/>
+      <c r="G28" s="97"/>
+      <c r="H28" s="97"/>
+      <c r="I28" s="97"/>
+      <c r="J28" s="98"/>
+    </row>
+    <row r="29" spans="1:10" s="4" customFormat="1" ht="78.75" customHeight="1" outlineLevel="1">
       <c r="A29" s="77"/>
       <c r="B29" s="92"/>
       <c r="C29" s="76"/>
-      <c r="D29" s="134"/>
-      <c r="E29" s="135"/>
-      <c r="F29" s="135"/>
+      <c r="D29" s="141"/>
+      <c r="E29" s="142"/>
+      <c r="F29" s="142"/>
       <c r="G29" s="75"/>
       <c r="H29" s="82"/>
       <c r="I29" s="76"/>
       <c r="J29" s="74"/>
     </row>
-    <row r="30" spans="1:10" s="4" customFormat="1" ht="91.5" customHeight="1" outlineLevel="1">
+    <row r="30" spans="1:10" s="4" customFormat="1" ht="79.5" customHeight="1" outlineLevel="1">
       <c r="A30" s="77"/>
       <c r="B30" s="92"/>
       <c r="C30" s="76"/>
-      <c r="D30" s="134"/>
-      <c r="E30" s="135"/>
-      <c r="F30" s="135"/>
+      <c r="D30" s="141"/>
+      <c r="E30" s="142"/>
+      <c r="F30" s="142"/>
       <c r="G30" s="75"/>
       <c r="H30" s="82"/>
       <c r="I30" s="76"/>
       <c r="J30" s="74"/>
     </row>
-    <row r="31" spans="1:10" s="4" customFormat="1" ht="67.5" customHeight="1" outlineLevel="1">
+    <row r="31" spans="1:10" s="4" customFormat="1" ht="79.5" customHeight="1" outlineLevel="1">
       <c r="A31" s="77"/>
       <c r="B31" s="92"/>
       <c r="C31" s="76"/>
-      <c r="D31" s="134"/>
-      <c r="E31" s="135"/>
-      <c r="F31" s="135"/>
+      <c r="D31" s="141"/>
+      <c r="E31" s="142"/>
+      <c r="F31" s="142"/>
       <c r="G31" s="75"/>
       <c r="H31" s="82"/>
       <c r="I31" s="76"/>
       <c r="J31" s="74"/>
     </row>
-    <row r="32" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A32" s="136"/>
-      <c r="B32" s="137"/>
-      <c r="C32" s="137"/>
-      <c r="D32" s="97"/>
-      <c r="E32" s="97"/>
-      <c r="F32" s="97"/>
-      <c r="G32" s="97"/>
-      <c r="H32" s="97"/>
-      <c r="I32" s="97"/>
-      <c r="J32" s="98"/>
-    </row>
-    <row r="33" spans="1:10" s="4" customFormat="1" ht="47.25" customHeight="1" outlineLevel="1">
+    <row r="32" spans="1:10" s="4" customFormat="1" ht="79.5" customHeight="1" outlineLevel="1">
+      <c r="A32" s="77"/>
+      <c r="B32" s="92"/>
+      <c r="C32" s="76"/>
+      <c r="D32" s="141"/>
+      <c r="E32" s="142"/>
+      <c r="F32" s="142"/>
+      <c r="G32" s="75"/>
+      <c r="H32" s="82"/>
+      <c r="I32" s="76"/>
+      <c r="J32" s="74"/>
+    </row>
+    <row r="33" spans="1:10" s="4" customFormat="1" ht="91.5" customHeight="1" outlineLevel="1">
       <c r="A33" s="77"/>
       <c r="B33" s="92"/>
       <c r="C33" s="76"/>
-      <c r="D33" s="134"/>
-      <c r="E33" s="135"/>
-      <c r="F33" s="135"/>
+      <c r="D33" s="141"/>
+      <c r="E33" s="142"/>
+      <c r="F33" s="142"/>
       <c r="G33" s="75"/>
       <c r="H33" s="82"/>
       <c r="I33" s="76"/>
       <c r="J33" s="74"/>
     </row>
-    <row r="34" spans="1:10" ht="12" customHeight="1">
-      <c r="I34"/>
-      <c r="J34"/>
-    </row>
-    <row r="35" spans="1:10" ht="12" customHeight="1">
-      <c r="I35"/>
-      <c r="J35"/>
-    </row>
-    <row r="36" spans="1:10" ht="12" customHeight="1">
-      <c r="I36"/>
-      <c r="J36"/>
+    <row r="34" spans="1:10" s="4" customFormat="1" ht="67.5" customHeight="1" outlineLevel="1">
+      <c r="A34" s="77"/>
+      <c r="B34" s="92"/>
+      <c r="C34" s="76"/>
+      <c r="D34" s="141"/>
+      <c r="E34" s="142"/>
+      <c r="F34" s="142"/>
+      <c r="G34" s="75"/>
+      <c r="H34" s="82"/>
+      <c r="I34" s="76"/>
+      <c r="J34" s="74"/>
+    </row>
+    <row r="35" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
+      <c r="A35" s="128"/>
+      <c r="B35" s="129"/>
+      <c r="C35" s="129"/>
+      <c r="D35" s="97"/>
+      <c r="E35" s="97"/>
+      <c r="F35" s="97"/>
+      <c r="G35" s="97"/>
+      <c r="H35" s="97"/>
+      <c r="I35" s="97"/>
+      <c r="J35" s="98"/>
+    </row>
+    <row r="36" spans="1:10" s="4" customFormat="1" ht="47.25" customHeight="1" outlineLevel="1">
+      <c r="A36" s="77"/>
+      <c r="B36" s="92"/>
+      <c r="C36" s="76"/>
+      <c r="D36" s="141"/>
+      <c r="E36" s="142"/>
+      <c r="F36" s="142"/>
+      <c r="G36" s="75"/>
+      <c r="H36" s="82"/>
+      <c r="I36" s="76"/>
+      <c r="J36" s="74"/>
     </row>
     <row r="37" spans="1:10" ht="12" customHeight="1">
       <c r="I37"/>
@@ -8515,16 +8647,16 @@
       <c r="I49"/>
       <c r="J49"/>
     </row>
-    <row r="50" spans="9:10">
-      <c r="I50" s="19"/>
+    <row r="50" spans="9:10" ht="12" customHeight="1">
+      <c r="I50"/>
       <c r="J50"/>
     </row>
-    <row r="51" spans="9:10">
-      <c r="I51" s="19"/>
+    <row r="51" spans="9:10" ht="12" customHeight="1">
+      <c r="I51"/>
       <c r="J51"/>
     </row>
-    <row r="52" spans="9:10">
-      <c r="I52" s="19"/>
+    <row r="52" spans="9:10" ht="12" customHeight="1">
+      <c r="I52"/>
       <c r="J52"/>
     </row>
     <row r="53" spans="9:10">
@@ -8579,8 +8711,47 @@
       <c r="I65" s="19"/>
       <c r="J65"/>
     </row>
+    <row r="66" spans="9:10">
+      <c r="I66" s="19"/>
+      <c r="J66"/>
+    </row>
+    <row r="67" spans="9:10">
+      <c r="I67" s="19"/>
+      <c r="J67"/>
+    </row>
+    <row r="68" spans="9:10">
+      <c r="I68" s="19"/>
+      <c r="J68"/>
+    </row>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="43">
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="D13:F13"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="D14:F14"/>
@@ -8597,30 +8768,6 @@
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:G10"/>
     <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="D33:F33"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -8632,7 +8779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -8798,7 +8945,7 @@
       </c>
       <c r="G10" s="121">
         <f>Samples3!D7</f>
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14.25">
@@ -8821,7 +8968,7 @@
       </c>
       <c r="G11" s="54">
         <f>SUM(G6:G10)</f>
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14.25">
@@ -8842,7 +8989,7 @@
       <c r="D13" s="19"/>
       <c r="E13" s="23">
         <f>(D11+E11)*100/G11</f>
-        <v>38.888888888888886</v>
+        <v>35.593220338983052</v>
       </c>
       <c r="F13" s="19" t="s">
         <v>22</v>
@@ -8858,7 +9005,7 @@
       <c r="D14" s="19"/>
       <c r="E14" s="23">
         <f>D11*100/G11</f>
-        <v>24.074074074074073</v>
+        <v>22.033898305084747</v>
       </c>
       <c r="F14" s="19" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
up tc huy sk va hoan tien
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University_IT\Tam\KiemThuPhanMem\event-manager-javafx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799C555B-6FC1-47F0-95C0-2CCDD4BE8CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB550F96-B6F7-4BC1-8DCF-2E60EC380933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="821" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="304">
   <si>
     <t>TC1</t>
   </si>
@@ -1170,6 +1170,80 @@
 4: Chọn Hủy sự kiện và nhập lý do hủy(bao gồm việc sẽ hoàn tiền cho tất cả người tham gia đối với sự kiện có phí)
 5: Xác nhận hủy sự kiện 
 6: Hệ thống hiển thị thông báo lỗi về giới hạn thời gian</t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra chức năng gửi thông báo khi hủy sự kiện trong thời gian cho phép hủy</t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra chức năng gửi thông báo khi hủy sự kiện trong thời gian không cho phép hủy</t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra chức năng gửi thông báo khi hủy sự kiện không có người đăng ký tham gia</t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra chức năng xử lý lỗi khi gửi thông báo hủy sự kiện</t>
+  </si>
+  <si>
+    <t>8. Hoàn tiền</t>
+  </si>
+  <si>
+    <t>9. Hủy sự kiện và hoàn tiền cho người tham gia</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng hủy sự kiện thành công và hoàn tiền đầy đủ đối với sự kiện có phí</t>
+  </si>
+  <si>
+    <t>1: Đăng nhập với tư cách là admin
+2: Truy cập vào trang Quản lý sự kiện
+3: Chọn sự kiện cần hủy(có người tham gia)
+4: Nhấn nút Hủy sự kiện 
+5: Nhập lý do hủy sự kiện
+6: Xác nhận hủy sự kiện
+7: Hệ thống xử lý và chuyển qua trang hoàn tiền
+8: Xác nhận hoàn tiền đầy đủ cho tất cả người tham gia
+9: Hệ thống thông báo hủy sự kiện và hoàn tiền thành công và gửi thông báo hủy sự kiện đến người tham gia</t>
+  </si>
+  <si>
+    <t>1: Đăng nhập với tư cách là admin
+2: Truy cập vào trang Quản lý sự kiện
+3: Chọn sự kiện cần hủy(có người tham gia)
+4: Nhấn nút Hủy sự kiện 
+5: Nhập lý do hủy sự kiện
+6: Xác nhận hủy sự kiện
+7: Hệ thống xử lý và không chuyển trang hoàn tiền vì đây là sự kiện miễn phí
+9: Hệ thống thông báo hủy sự kiện thành công và gửi thông báo hủy sự kiện đến người tham gia</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng xử lý lỗi trong quá trình hủy sự kiện và hoàn tiền</t>
+  </si>
+  <si>
+    <t>1: Đăng nhập với tư cách là admin
+2: Truy cập trang Quản lý sự kiện
+3: Chọn sự kiện cần hủy
+4: Giả lập lỗi trong quá trình hủy và hoàn(Vd: ngắt kết nối mạng, database hay thông tin thanh toán không hợp lệ)
+5: Nhấn nút Hủy và xác nhận hủy sự kiện
+6: Hệ thống thông báo lỗi không thể hủy hay hoàn tiền
+7: Sửa lỗi và thử lại quá trình hủy và hoàn
+8: Hệ thống thông báo hủy sự kiện thành công và gửi thông báo hủy sự kiện đến người tham gia</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng xử lý lỗi khi hủy sự kiện thành công nhưng hoàn tiền thất bại</t>
+  </si>
+  <si>
+    <t>1: Đăng nhập với tư cách là admin
+2: Giả lập lỗi hoàn tiền(Vd: tài khoản hết tiền, hết hạn hay bị đóng băng..)
+3: Hủy sự kiện theo các quy trình đã nêu 
+4: Hệ thống thông báo lỗi đến admin và ghi nhận lỗi
+5: Hệ thống gửi thông báo đến người tham gia về việc quá trình hoàn tiền bị trì hoãn và đang được xử lý</t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra chức năng hủy sự kiện thành công và hoàn tiền đầy đủ đối với sự kiện có phí</t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra chức năng xử lý lỗi trong quá trình hủy sự kiện và hoàn tiền</t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra chức năng xử lý lỗi khi hủy sự kiện thành công nhưng hoàn tiền thất bại</t>
   </si>
 </sst>
 </file>
@@ -1896,7 +1970,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="172">
+  <cellXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2218,6 +2292,9 @@
     <xf numFmtId="20" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="6" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -2356,13 +2433,19 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="6" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4081,8 +4164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H118"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A98" zoomScale="85" workbookViewId="0">
-      <selection activeCell="G104" sqref="G104"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A102" zoomScale="85" workbookViewId="0">
+      <selection activeCell="D107" sqref="D107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -4149,11 +4232,11 @@
       <c r="B6" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="123" t="s">
+      <c r="C6" s="124" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="123"/>
-      <c r="E6" s="124"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="125"/>
       <c r="F6" s="108"/>
       <c r="G6" s="25"/>
     </row>
@@ -4162,11 +4245,11 @@
       <c r="B7" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="123" t="s">
+      <c r="C7" s="124" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="123"/>
-      <c r="E7" s="124"/>
+      <c r="D7" s="124"/>
+      <c r="E7" s="125"/>
       <c r="F7" s="108"/>
       <c r="G7" s="25"/>
     </row>
@@ -5763,7 +5846,7 @@
       <c r="G102" s="99"/>
       <c r="H102" s="105"/>
     </row>
-    <row r="103" spans="2:8" s="33" customFormat="1" ht="25.5">
+    <row r="103" spans="2:8" s="33" customFormat="1" ht="38.25">
       <c r="B103" s="118">
         <v>45763</v>
       </c>
@@ -5772,7 +5855,7 @@
       </c>
       <c r="D103" s="99"/>
       <c r="E103" s="104" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="F103" s="110" t="s">
         <v>44</v>
@@ -5789,7 +5872,7 @@
       </c>
       <c r="D104" s="99"/>
       <c r="E104" s="104" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="F104" s="110" t="s">
         <v>44</v>
@@ -5797,7 +5880,7 @@
       <c r="G104" s="99"/>
       <c r="H104" s="105"/>
     </row>
-    <row r="105" spans="2:8" s="33" customFormat="1" ht="25.5">
+    <row r="105" spans="2:8" s="33" customFormat="1" ht="38.25">
       <c r="B105" s="118">
         <v>45763</v>
       </c>
@@ -5806,7 +5889,7 @@
       </c>
       <c r="D105" s="99"/>
       <c r="E105" s="104" t="s">
-        <v>281</v>
+        <v>290</v>
       </c>
       <c r="F105" s="110" t="s">
         <v>44</v>
@@ -5823,7 +5906,7 @@
       </c>
       <c r="D106" s="99"/>
       <c r="E106" s="104" t="s">
-        <v>280</v>
+        <v>291</v>
       </c>
       <c r="F106" s="110" t="s">
         <v>44</v>
@@ -5831,16 +5914,16 @@
       <c r="G106" s="99"/>
       <c r="H106" s="105"/>
     </row>
-    <row r="107" spans="2:8" s="33" customFormat="1" ht="25.5">
+    <row r="107" spans="2:8" s="33" customFormat="1" ht="38.25">
       <c r="B107" s="118">
-        <v>45763</v>
+        <v>45764</v>
       </c>
       <c r="C107" s="119" t="s">
         <v>40</v>
       </c>
       <c r="D107" s="99"/>
       <c r="E107" s="104" t="s">
-        <v>280</v>
+        <v>301</v>
       </c>
       <c r="F107" s="110" t="s">
         <v>44</v>
@@ -5848,30 +5931,54 @@
       <c r="G107" s="99"/>
       <c r="H107" s="105"/>
     </row>
-    <row r="108" spans="2:8" s="33" customFormat="1">
-      <c r="B108" s="118"/>
-      <c r="C108" s="119"/>
+    <row r="108" spans="2:8" s="33" customFormat="1" ht="38.25">
+      <c r="B108" s="118">
+        <v>45764</v>
+      </c>
+      <c r="C108" s="119" t="s">
+        <v>40</v>
+      </c>
       <c r="D108" s="99"/>
-      <c r="E108" s="104"/>
-      <c r="F108" s="120"/>
+      <c r="E108" s="104" t="s">
+        <v>301</v>
+      </c>
+      <c r="F108" s="110" t="s">
+        <v>44</v>
+      </c>
       <c r="G108" s="99"/>
       <c r="H108" s="105"/>
     </row>
-    <row r="109" spans="2:8" s="33" customFormat="1">
-      <c r="B109" s="118"/>
-      <c r="C109" s="119"/>
+    <row r="109" spans="2:8" s="33" customFormat="1" ht="25.5">
+      <c r="B109" s="118">
+        <v>45764</v>
+      </c>
+      <c r="C109" s="119" t="s">
+        <v>40</v>
+      </c>
       <c r="D109" s="99"/>
-      <c r="E109" s="104"/>
-      <c r="F109" s="120"/>
+      <c r="E109" s="104" t="s">
+        <v>302</v>
+      </c>
+      <c r="F109" s="110" t="s">
+        <v>44</v>
+      </c>
       <c r="G109" s="99"/>
       <c r="H109" s="105"/>
     </row>
-    <row r="110" spans="2:8" s="33" customFormat="1">
-      <c r="B110" s="118"/>
-      <c r="C110" s="119"/>
+    <row r="110" spans="2:8" s="33" customFormat="1" ht="38.25">
+      <c r="B110" s="118">
+        <v>45764</v>
+      </c>
+      <c r="C110" s="119" t="s">
+        <v>40</v>
+      </c>
       <c r="D110" s="99"/>
-      <c r="E110" s="104"/>
-      <c r="F110" s="120"/>
+      <c r="E110" s="104" t="s">
+        <v>303</v>
+      </c>
+      <c r="F110" s="110" t="s">
+        <v>44</v>
+      </c>
       <c r="G110" s="99"/>
       <c r="H110" s="105"/>
     </row>
@@ -5962,7 +6069,7 @@
     <oddFooter>&amp;L&amp;"Tahoma,Regular"&amp;8 02ae-BM/PM/HDCV/FSOFT v1/0&amp;R&amp;"Tahoma,Regular"&amp;10&amp;P/&amp;N</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="C12:C28 C41 C34:C40 C42:C47 C48:C49 C51:C53 C50 C54:C57 C58:C60 C29:C33 C61:C83 C84:C92 C93:C94 C95:C102" numberStoredAsText="1"/>
+    <ignoredError sqref="C12:C28 C41 C34:C40 C42:C47 C48:C49 C51:C53 C50 C54:C57 C58:C60 C29:C33 C61:C83 C84:C92 C93:C94 C95:C102 C103:C105 C106:C110" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -5972,10 +6079,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K88"/>
+  <dimension ref="A1:K99"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A48" zoomScale="69" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView showGridLines="0" topLeftCell="A61" zoomScale="69" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59:B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" outlineLevelRow="1"/>
@@ -5994,9 +6101,9 @@
       <c r="A1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="146"/>
-      <c r="D1" s="146"/>
+      <c r="B1" s="147"/>
+      <c r="C1" s="147"/>
+      <c r="D1" s="147"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -6007,9 +6114,9 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="147"/>
-      <c r="C2" s="147"/>
-      <c r="D2" s="147"/>
+      <c r="B2" s="148"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -6022,51 +6129,51 @@
       <c r="A3" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="123" t="s">
+      <c r="B3" s="124" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="123"/>
-      <c r="D3" s="124"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="125"/>
       <c r="E3" s="60"/>
       <c r="F3" s="60"/>
       <c r="G3" s="60"/>
-      <c r="H3" s="154"/>
-      <c r="I3" s="154"/>
-      <c r="J3" s="154"/>
+      <c r="H3" s="155"/>
+      <c r="I3" s="155"/>
+      <c r="J3" s="155"/>
       <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="12.75">
       <c r="A4" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="155" t="s">
+      <c r="B4" s="156" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="156"/>
-      <c r="D4" s="157"/>
+      <c r="C4" s="157"/>
+      <c r="D4" s="158"/>
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
       <c r="G4" s="60"/>
-      <c r="H4" s="154"/>
-      <c r="I4" s="154"/>
-      <c r="J4" s="154"/>
+      <c r="H4" s="155"/>
+      <c r="I4" s="155"/>
+      <c r="J4" s="155"/>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" s="70" customFormat="1" ht="25.5">
       <c r="A5" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="149" t="s">
+      <c r="B5" s="150" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="150"/>
-      <c r="D5" s="151"/>
+      <c r="C5" s="151"/>
+      <c r="D5" s="152"/>
       <c r="E5" s="68"/>
       <c r="F5" s="68"/>
       <c r="G5" s="68"/>
-      <c r="H5" s="153"/>
-      <c r="I5" s="153"/>
-      <c r="J5" s="153"/>
+      <c r="H5" s="154"/>
+      <c r="I5" s="154"/>
+      <c r="J5" s="154"/>
       <c r="K5" s="69"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
@@ -6081,15 +6188,15 @@
         <v>39</v>
       </c>
       <c r="D6" s="13">
-        <f>COUNTIF(I10:I753,"Pending")</f>
+        <f>COUNTIF(I10:I764,"Pending")</f>
         <v>0</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="154"/>
-      <c r="I6" s="154"/>
-      <c r="J6" s="154"/>
+      <c r="H6" s="155"/>
+      <c r="I6" s="155"/>
+      <c r="J6" s="155"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -6104,22 +6211,22 @@
         <v>28</v>
       </c>
       <c r="D7" s="58">
-        <f>COUNTA(A12:A54) -7</f>
-        <v>36</v>
+        <f>COUNTA(A12:A62) -9</f>
+        <v>40</v>
       </c>
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
       <c r="G7" s="61"/>
-      <c r="H7" s="154"/>
-      <c r="I7" s="154"/>
-      <c r="J7" s="154"/>
+      <c r="H7" s="155"/>
+      <c r="I7" s="155"/>
+      <c r="J7" s="155"/>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="148"/>
-      <c r="B8" s="148"/>
-      <c r="C8" s="148"/>
-      <c r="D8" s="148"/>
+      <c r="A8" s="149"/>
+      <c r="B8" s="149"/>
+      <c r="C8" s="149"/>
+      <c r="D8" s="149"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -6129,70 +6236,70 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" s="72" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="132" t="s">
+      <c r="A9" s="133" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="161" t="s">
+      <c r="B9" s="162" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="132" t="s">
+      <c r="C9" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="133" t="s">
+      <c r="D9" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="134"/>
-      <c r="F9" s="134"/>
-      <c r="G9" s="135"/>
-      <c r="H9" s="158" t="s">
+      <c r="E9" s="135"/>
+      <c r="F9" s="135"/>
+      <c r="G9" s="136"/>
+      <c r="H9" s="159" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="127" t="s">
+      <c r="I9" s="128" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="127" t="s">
+      <c r="J9" s="128" t="s">
         <v>32</v>
       </c>
       <c r="K9" s="71"/>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="127"/>
-      <c r="B10" s="162"/>
-      <c r="C10" s="127"/>
-      <c r="D10" s="136"/>
-      <c r="E10" s="137"/>
-      <c r="F10" s="137"/>
-      <c r="G10" s="138"/>
-      <c r="H10" s="136"/>
-      <c r="I10" s="127"/>
-      <c r="J10" s="127"/>
+      <c r="A10" s="128"/>
+      <c r="B10" s="163"/>
+      <c r="C10" s="128"/>
+      <c r="D10" s="137"/>
+      <c r="E10" s="138"/>
+      <c r="F10" s="138"/>
+      <c r="G10" s="139"/>
+      <c r="H10" s="137"/>
+      <c r="I10" s="128"/>
+      <c r="J10" s="128"/>
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" s="73" customFormat="1" ht="15">
-      <c r="A11" s="159"/>
-      <c r="B11" s="159"/>
-      <c r="C11" s="159"/>
-      <c r="D11" s="159"/>
-      <c r="E11" s="159"/>
-      <c r="F11" s="159"/>
-      <c r="G11" s="159"/>
-      <c r="H11" s="159"/>
-      <c r="I11" s="159"/>
-      <c r="J11" s="160"/>
+      <c r="A11" s="160"/>
+      <c r="B11" s="160"/>
+      <c r="C11" s="160"/>
+      <c r="D11" s="160"/>
+      <c r="E11" s="160"/>
+      <c r="F11" s="160"/>
+      <c r="G11" s="160"/>
+      <c r="H11" s="160"/>
+      <c r="I11" s="160"/>
+      <c r="J11" s="161"/>
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A12" s="139" t="s">
+      <c r="A12" s="140" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="140"/>
-      <c r="C12" s="140"/>
-      <c r="D12" s="140"/>
-      <c r="E12" s="140"/>
-      <c r="F12" s="140"/>
-      <c r="G12" s="140"/>
-      <c r="H12" s="140"/>
-      <c r="I12" s="140"/>
-      <c r="J12" s="152"/>
+      <c r="B12" s="141"/>
+      <c r="C12" s="141"/>
+      <c r="D12" s="141"/>
+      <c r="E12" s="141"/>
+      <c r="F12" s="141"/>
+      <c r="G12" s="141"/>
+      <c r="H12" s="141"/>
+      <c r="I12" s="141"/>
+      <c r="J12" s="153"/>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" ht="350.1" customHeight="1" outlineLevel="1">
       <c r="A13" s="77" t="s">
@@ -6204,9 +6311,9 @@
       <c r="C13" s="76" t="s">
         <v>200</v>
       </c>
-      <c r="D13" s="125"/>
-      <c r="E13" s="126"/>
-      <c r="F13" s="126"/>
+      <c r="D13" s="126"/>
+      <c r="E13" s="127"/>
+      <c r="F13" s="127"/>
       <c r="G13" s="75"/>
       <c r="H13" s="116">
         <v>45755</v>
@@ -6226,9 +6333,9 @@
       <c r="C14" s="76" t="s">
         <v>199</v>
       </c>
-      <c r="D14" s="125"/>
-      <c r="E14" s="126"/>
-      <c r="F14" s="126"/>
+      <c r="D14" s="126"/>
+      <c r="E14" s="127"/>
+      <c r="F14" s="127"/>
       <c r="G14" s="75"/>
       <c r="H14" s="116">
         <v>45755</v>
@@ -6248,9 +6355,9 @@
       <c r="C15" s="76" t="s">
         <v>198</v>
       </c>
-      <c r="D15" s="125"/>
-      <c r="E15" s="126"/>
-      <c r="F15" s="126"/>
+      <c r="D15" s="126"/>
+      <c r="E15" s="127"/>
+      <c r="F15" s="127"/>
       <c r="G15" s="75"/>
       <c r="H15" s="116">
         <v>45755</v>
@@ -6272,9 +6379,9 @@
       <c r="C16" s="76" t="s">
         <v>197</v>
       </c>
-      <c r="D16" s="125"/>
-      <c r="E16" s="126"/>
-      <c r="F16" s="126"/>
+      <c r="D16" s="126"/>
+      <c r="E16" s="127"/>
+      <c r="F16" s="127"/>
       <c r="G16" s="75"/>
       <c r="H16" s="116">
         <v>45755</v>
@@ -6294,9 +6401,9 @@
       <c r="C17" s="76" t="s">
         <v>196</v>
       </c>
-      <c r="D17" s="125"/>
-      <c r="E17" s="126"/>
-      <c r="F17" s="126"/>
+      <c r="D17" s="126"/>
+      <c r="E17" s="127"/>
+      <c r="F17" s="127"/>
       <c r="G17" s="75"/>
       <c r="H17" s="116">
         <v>45755</v>
@@ -6316,9 +6423,9 @@
       <c r="C18" s="86" t="s">
         <v>195</v>
       </c>
-      <c r="D18" s="125"/>
-      <c r="E18" s="126"/>
-      <c r="F18" s="126"/>
+      <c r="D18" s="126"/>
+      <c r="E18" s="127"/>
+      <c r="F18" s="127"/>
       <c r="G18" s="75"/>
       <c r="H18" s="116">
         <v>45755</v>
@@ -6340,9 +6447,9 @@
       <c r="C19" s="86" t="s">
         <v>194</v>
       </c>
-      <c r="D19" s="125"/>
-      <c r="E19" s="126"/>
-      <c r="F19" s="126"/>
+      <c r="D19" s="126"/>
+      <c r="E19" s="127"/>
+      <c r="F19" s="127"/>
       <c r="G19" s="75"/>
       <c r="H19" s="116">
         <v>45755</v>
@@ -6364,9 +6471,9 @@
       <c r="C20" s="76" t="s">
         <v>192</v>
       </c>
-      <c r="D20" s="125"/>
-      <c r="E20" s="126"/>
-      <c r="F20" s="126"/>
+      <c r="D20" s="126"/>
+      <c r="E20" s="127"/>
+      <c r="F20" s="127"/>
       <c r="G20" s="75"/>
       <c r="H20" s="116">
         <v>45755</v>
@@ -6388,9 +6495,9 @@
       <c r="C21" s="76" t="s">
         <v>191</v>
       </c>
-      <c r="D21" s="125"/>
-      <c r="E21" s="126"/>
-      <c r="F21" s="126"/>
+      <c r="D21" s="126"/>
+      <c r="E21" s="127"/>
+      <c r="F21" s="127"/>
       <c r="G21" s="75"/>
       <c r="H21" s="116">
         <v>45755</v>
@@ -6412,9 +6519,9 @@
       <c r="C22" s="86" t="s">
         <v>193</v>
       </c>
-      <c r="D22" s="125"/>
-      <c r="E22" s="126"/>
-      <c r="F22" s="126"/>
+      <c r="D22" s="126"/>
+      <c r="E22" s="127"/>
+      <c r="F22" s="127"/>
       <c r="G22" s="75"/>
       <c r="H22" s="116">
         <v>45755</v>
@@ -6427,11 +6534,11 @@
       </c>
     </row>
     <row r="23" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A23" s="139" t="s">
+      <c r="A23" s="140" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="140"/>
-      <c r="C23" s="140"/>
+      <c r="B23" s="141"/>
+      <c r="C23" s="141"/>
       <c r="D23" s="87"/>
       <c r="E23" s="87"/>
       <c r="F23" s="87"/>
@@ -6450,9 +6557,9 @@
       <c r="C24" s="86" t="s">
         <v>228</v>
       </c>
-      <c r="D24" s="130"/>
-      <c r="E24" s="131"/>
-      <c r="F24" s="131"/>
+      <c r="D24" s="131"/>
+      <c r="E24" s="132"/>
+      <c r="F24" s="132"/>
       <c r="G24" s="94"/>
       <c r="H24" s="115">
         <v>45756</v>
@@ -6472,9 +6579,9 @@
       <c r="C25" s="86" t="s">
         <v>227</v>
       </c>
-      <c r="D25" s="130"/>
-      <c r="E25" s="131"/>
-      <c r="F25" s="131"/>
+      <c r="D25" s="131"/>
+      <c r="E25" s="132"/>
+      <c r="F25" s="132"/>
       <c r="G25" s="94"/>
       <c r="H25" s="115">
         <v>45755</v>
@@ -6496,9 +6603,9 @@
       <c r="C26" s="86" t="s">
         <v>232</v>
       </c>
-      <c r="D26" s="141"/>
-      <c r="E26" s="142"/>
-      <c r="F26" s="142"/>
+      <c r="D26" s="142"/>
+      <c r="E26" s="143"/>
+      <c r="F26" s="143"/>
       <c r="G26" s="94"/>
       <c r="H26" s="115">
         <v>45756</v>
@@ -6518,9 +6625,9 @@
       <c r="C27" s="86" t="s">
         <v>233</v>
       </c>
-      <c r="D27" s="143"/>
-      <c r="E27" s="144"/>
-      <c r="F27" s="145"/>
+      <c r="D27" s="144"/>
+      <c r="E27" s="145"/>
+      <c r="F27" s="146"/>
       <c r="G27" s="94"/>
       <c r="H27" s="115">
         <v>45755</v>
@@ -6540,9 +6647,9 @@
       <c r="C28" s="86" t="s">
         <v>237</v>
       </c>
-      <c r="D28" s="143"/>
-      <c r="E28" s="144"/>
-      <c r="F28" s="145"/>
+      <c r="D28" s="144"/>
+      <c r="E28" s="145"/>
+      <c r="F28" s="146"/>
       <c r="G28" s="94"/>
       <c r="H28" s="115">
         <v>45756</v>
@@ -6564,9 +6671,9 @@
       <c r="C29" s="86" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="143"/>
-      <c r="E29" s="144"/>
-      <c r="F29" s="145"/>
+      <c r="D29" s="144"/>
+      <c r="E29" s="145"/>
+      <c r="F29" s="146"/>
       <c r="G29" s="94"/>
       <c r="H29" s="115">
         <v>45756</v>
@@ -6588,9 +6695,9 @@
       <c r="C30" s="86" t="s">
         <v>234</v>
       </c>
-      <c r="D30" s="143"/>
-      <c r="E30" s="144"/>
-      <c r="F30" s="145"/>
+      <c r="D30" s="144"/>
+      <c r="E30" s="145"/>
+      <c r="F30" s="146"/>
       <c r="G30" s="94"/>
       <c r="H30" s="115">
         <v>45755</v>
@@ -6610,9 +6717,9 @@
       <c r="C31" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="143"/>
-      <c r="E31" s="144"/>
-      <c r="F31" s="145"/>
+      <c r="D31" s="144"/>
+      <c r="E31" s="145"/>
+      <c r="F31" s="146"/>
       <c r="G31" s="94"/>
       <c r="H31" s="115">
         <v>45756</v>
@@ -6634,9 +6741,9 @@
       <c r="C32" s="86" t="s">
         <v>70</v>
       </c>
-      <c r="D32" s="143"/>
-      <c r="E32" s="144"/>
-      <c r="F32" s="145"/>
+      <c r="D32" s="144"/>
+      <c r="E32" s="145"/>
+      <c r="F32" s="146"/>
       <c r="G32" s="94"/>
       <c r="H32" s="115">
         <v>45756</v>
@@ -6658,9 +6765,9 @@
       <c r="C33" s="86" t="s">
         <v>241</v>
       </c>
-      <c r="D33" s="125"/>
-      <c r="E33" s="126"/>
-      <c r="F33" s="163"/>
+      <c r="D33" s="126"/>
+      <c r="E33" s="127"/>
+      <c r="F33" s="164"/>
       <c r="G33" s="94"/>
       <c r="H33" s="115">
         <v>45755</v>
@@ -6680,9 +6787,9 @@
       <c r="C34" s="86" t="s">
         <v>201</v>
       </c>
-      <c r="D34" s="164"/>
-      <c r="E34" s="165"/>
-      <c r="F34" s="166"/>
+      <c r="D34" s="165"/>
+      <c r="E34" s="166"/>
+      <c r="F34" s="167"/>
       <c r="G34" s="94"/>
       <c r="H34" s="115">
         <v>45755</v>
@@ -6693,11 +6800,11 @@
       <c r="J34" s="96"/>
     </row>
     <row r="35" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A35" s="139" t="s">
+      <c r="A35" s="140" t="s">
         <v>71</v>
       </c>
-      <c r="B35" s="140"/>
-      <c r="C35" s="140"/>
+      <c r="B35" s="141"/>
+      <c r="C35" s="141"/>
       <c r="D35" s="87"/>
       <c r="E35" s="87"/>
       <c r="F35" s="87"/>
@@ -6716,20 +6823,20 @@
       <c r="C36" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="D36" s="141"/>
-      <c r="E36" s="142"/>
-      <c r="F36" s="142"/>
+      <c r="D36" s="142"/>
+      <c r="E36" s="143"/>
+      <c r="F36" s="143"/>
       <c r="G36" s="75"/>
       <c r="H36" s="82"/>
       <c r="I36" s="76"/>
       <c r="J36" s="74"/>
     </row>
     <row r="37" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A37" s="128" t="s">
+      <c r="A37" s="129" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="129"/>
-      <c r="C37" s="129"/>
+      <c r="B37" s="130"/>
+      <c r="C37" s="130"/>
       <c r="D37" s="97"/>
       <c r="E37" s="97"/>
       <c r="F37" s="97"/>
@@ -6748,9 +6855,9 @@
       <c r="C38" s="76" t="s">
         <v>113</v>
       </c>
-      <c r="D38" s="141"/>
-      <c r="E38" s="142"/>
-      <c r="F38" s="142"/>
+      <c r="D38" s="142"/>
+      <c r="E38" s="143"/>
+      <c r="F38" s="143"/>
       <c r="G38" s="75"/>
       <c r="H38" s="82"/>
       <c r="I38" s="76"/>
@@ -6766,9 +6873,9 @@
       <c r="C39" s="76" t="s">
         <v>115</v>
       </c>
-      <c r="D39" s="141"/>
-      <c r="E39" s="142"/>
-      <c r="F39" s="142"/>
+      <c r="D39" s="142"/>
+      <c r="E39" s="143"/>
+      <c r="F39" s="143"/>
       <c r="G39" s="75"/>
       <c r="H39" s="82"/>
       <c r="I39" s="76"/>
@@ -6784,9 +6891,9 @@
       <c r="C40" s="76" t="s">
         <v>114</v>
       </c>
-      <c r="D40" s="141"/>
-      <c r="E40" s="142"/>
-      <c r="F40" s="142"/>
+      <c r="D40" s="142"/>
+      <c r="E40" s="143"/>
+      <c r="F40" s="143"/>
       <c r="G40" s="75"/>
       <c r="H40" s="82"/>
       <c r="I40" s="76"/>
@@ -6802,9 +6909,9 @@
       <c r="C41" s="76" t="s">
         <v>117</v>
       </c>
-      <c r="D41" s="141"/>
-      <c r="E41" s="142"/>
-      <c r="F41" s="142"/>
+      <c r="D41" s="142"/>
+      <c r="E41" s="143"/>
+      <c r="F41" s="143"/>
       <c r="G41" s="75"/>
       <c r="H41" s="82"/>
       <c r="I41" s="76"/>
@@ -6820,20 +6927,20 @@
       <c r="C42" s="76" t="s">
         <v>119</v>
       </c>
-      <c r="D42" s="141"/>
-      <c r="E42" s="142"/>
-      <c r="F42" s="142"/>
+      <c r="D42" s="142"/>
+      <c r="E42" s="143"/>
+      <c r="F42" s="143"/>
       <c r="G42" s="75"/>
       <c r="H42" s="82"/>
       <c r="I42" s="76"/>
       <c r="J42" s="74"/>
     </row>
     <row r="43" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A43" s="128" t="s">
+      <c r="A43" s="129" t="s">
         <v>88</v>
       </c>
-      <c r="B43" s="129"/>
-      <c r="C43" s="129"/>
+      <c r="B43" s="130"/>
+      <c r="C43" s="130"/>
       <c r="D43" s="97"/>
       <c r="E43" s="97"/>
       <c r="F43" s="97"/>
@@ -6852,9 +6959,9 @@
       <c r="C44" s="76" t="s">
         <v>95</v>
       </c>
-      <c r="D44" s="141"/>
-      <c r="E44" s="142"/>
-      <c r="F44" s="142"/>
+      <c r="D44" s="142"/>
+      <c r="E44" s="143"/>
+      <c r="F44" s="143"/>
       <c r="G44" s="75"/>
       <c r="H44" s="82"/>
       <c r="I44" s="76"/>
@@ -6870,9 +6977,9 @@
       <c r="C45" s="76" t="s">
         <v>96</v>
       </c>
-      <c r="D45" s="141"/>
-      <c r="E45" s="142"/>
-      <c r="F45" s="142"/>
+      <c r="D45" s="142"/>
+      <c r="E45" s="143"/>
+      <c r="F45" s="143"/>
       <c r="G45" s="75"/>
       <c r="H45" s="82"/>
       <c r="I45" s="76"/>
@@ -6888,9 +6995,9 @@
       <c r="C46" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="D46" s="141"/>
-      <c r="E46" s="142"/>
-      <c r="F46" s="142"/>
+      <c r="D46" s="142"/>
+      <c r="E46" s="143"/>
+      <c r="F46" s="143"/>
       <c r="G46" s="75"/>
       <c r="H46" s="82"/>
       <c r="I46" s="76"/>
@@ -6906,9 +7013,9 @@
       <c r="C47" s="76" t="s">
         <v>98</v>
       </c>
-      <c r="D47" s="141"/>
-      <c r="E47" s="142"/>
-      <c r="F47" s="142"/>
+      <c r="D47" s="142"/>
+      <c r="E47" s="143"/>
+      <c r="F47" s="143"/>
       <c r="G47" s="75"/>
       <c r="H47" s="82"/>
       <c r="I47" s="76"/>
@@ -6924,9 +7031,9 @@
       <c r="C48" s="76" t="s">
         <v>100</v>
       </c>
-      <c r="D48" s="141"/>
-      <c r="E48" s="142"/>
-      <c r="F48" s="142"/>
+      <c r="D48" s="142"/>
+      <c r="E48" s="143"/>
+      <c r="F48" s="143"/>
       <c r="G48" s="75"/>
       <c r="H48" s="82"/>
       <c r="I48" s="76"/>
@@ -6942,20 +7049,20 @@
       <c r="C49" s="76" t="s">
         <v>92</v>
       </c>
-      <c r="D49" s="141"/>
-      <c r="E49" s="142"/>
-      <c r="F49" s="142"/>
+      <c r="D49" s="142"/>
+      <c r="E49" s="143"/>
+      <c r="F49" s="143"/>
       <c r="G49" s="75"/>
       <c r="H49" s="82"/>
       <c r="I49" s="76"/>
       <c r="J49" s="74"/>
     </row>
     <row r="50" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A50" s="128" t="s">
+      <c r="A50" s="129" t="s">
         <v>101</v>
       </c>
-      <c r="B50" s="129"/>
-      <c r="C50" s="129"/>
+      <c r="B50" s="130"/>
+      <c r="C50" s="130"/>
       <c r="D50" s="97"/>
       <c r="E50" s="97"/>
       <c r="F50" s="97"/>
@@ -6974,20 +7081,20 @@
       <c r="C51" s="76" t="s">
         <v>102</v>
       </c>
-      <c r="D51" s="141"/>
-      <c r="E51" s="142"/>
-      <c r="F51" s="142"/>
+      <c r="D51" s="142"/>
+      <c r="E51" s="143"/>
+      <c r="F51" s="143"/>
       <c r="G51" s="75"/>
       <c r="H51" s="82"/>
       <c r="I51" s="76"/>
       <c r="J51" s="74"/>
     </row>
     <row r="52" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A52" s="128" t="s">
+      <c r="A52" s="129" t="s">
         <v>265</v>
       </c>
-      <c r="B52" s="129"/>
-      <c r="C52" s="129"/>
+      <c r="B52" s="130"/>
+      <c r="C52" s="130"/>
       <c r="D52" s="97"/>
       <c r="E52" s="97"/>
       <c r="F52" s="97"/>
@@ -7006,9 +7113,9 @@
       <c r="C53" s="76" t="s">
         <v>264</v>
       </c>
-      <c r="D53" s="141"/>
-      <c r="E53" s="142"/>
-      <c r="F53" s="142"/>
+      <c r="D53" s="142"/>
+      <c r="E53" s="143"/>
+      <c r="F53" s="143"/>
       <c r="G53" s="75"/>
       <c r="H53" s="82"/>
       <c r="I53" s="76"/>
@@ -7024,18 +7131,20 @@
       <c r="C54" s="76" t="s">
         <v>269</v>
       </c>
-      <c r="D54" s="141"/>
-      <c r="E54" s="142"/>
-      <c r="F54" s="142"/>
+      <c r="D54" s="142"/>
+      <c r="E54" s="143"/>
+      <c r="F54" s="143"/>
       <c r="G54" s="75"/>
       <c r="H54" s="82"/>
       <c r="I54" s="76"/>
       <c r="J54" s="74"/>
     </row>
     <row r="55" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A55" s="128"/>
-      <c r="B55" s="129"/>
-      <c r="C55" s="129"/>
+      <c r="A55" s="129" t="s">
+        <v>292</v>
+      </c>
+      <c r="B55" s="130"/>
+      <c r="C55" s="130"/>
       <c r="D55" s="97"/>
       <c r="E55" s="97"/>
       <c r="F55" s="97"/>
@@ -7048,120 +7157,234 @@
       <c r="A56" s="77"/>
       <c r="B56" s="92"/>
       <c r="C56" s="76"/>
-      <c r="D56" s="141"/>
-      <c r="E56" s="142"/>
-      <c r="F56" s="142"/>
+      <c r="D56" s="142"/>
+      <c r="E56" s="143"/>
+      <c r="F56" s="143"/>
       <c r="G56" s="75"/>
       <c r="H56" s="82"/>
       <c r="I56" s="76"/>
       <c r="J56" s="74"/>
     </row>
-    <row r="57" spans="1:10" ht="12" customHeight="1">
-      <c r="I57"/>
-      <c r="J57"/>
-    </row>
-    <row r="58" spans="1:10" ht="12" customHeight="1">
-      <c r="I58"/>
-      <c r="J58"/>
-    </row>
-    <row r="59" spans="1:10" ht="12" customHeight="1">
-      <c r="I59"/>
-      <c r="J59"/>
-    </row>
-    <row r="60" spans="1:10" ht="12" customHeight="1">
-      <c r="I60"/>
-      <c r="J60"/>
-    </row>
-    <row r="61" spans="1:10" ht="12" customHeight="1">
-      <c r="I61"/>
-      <c r="J61"/>
-    </row>
-    <row r="62" spans="1:10" ht="12" customHeight="1">
-      <c r="I62"/>
-      <c r="J62"/>
-    </row>
-    <row r="63" spans="1:10" ht="12" customHeight="1">
-      <c r="I63"/>
-      <c r="J63"/>
-    </row>
-    <row r="64" spans="1:10" ht="12" customHeight="1">
-      <c r="I64"/>
-      <c r="J64"/>
-    </row>
-    <row r="65" spans="9:10" ht="12" customHeight="1">
-      <c r="I65"/>
-      <c r="J65"/>
-    </row>
-    <row r="66" spans="9:10" ht="12" customHeight="1">
-      <c r="I66"/>
-      <c r="J66"/>
-    </row>
-    <row r="67" spans="9:10" ht="12" customHeight="1">
-      <c r="I67"/>
-      <c r="J67"/>
-    </row>
-    <row r="68" spans="9:10" ht="12" customHeight="1">
+    <row r="57" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A57" s="77"/>
+      <c r="B57" s="92"/>
+      <c r="C57" s="76"/>
+      <c r="D57" s="142"/>
+      <c r="E57" s="143"/>
+      <c r="F57" s="143"/>
+      <c r="G57" s="75"/>
+      <c r="H57" s="82"/>
+      <c r="I57" s="76"/>
+      <c r="J57" s="74"/>
+    </row>
+    <row r="58" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
+      <c r="A58" s="129" t="s">
+        <v>293</v>
+      </c>
+      <c r="B58" s="130"/>
+      <c r="C58" s="130"/>
+      <c r="D58" s="97"/>
+      <c r="E58" s="97"/>
+      <c r="F58" s="97"/>
+      <c r="G58" s="97"/>
+      <c r="H58" s="97"/>
+      <c r="I58" s="97"/>
+      <c r="J58" s="98"/>
+    </row>
+    <row r="59" spans="1:10" s="4" customFormat="1" ht="136.5" customHeight="1" outlineLevel="1">
+      <c r="A59" s="77" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="92" t="s">
+        <v>294</v>
+      </c>
+      <c r="C59" s="76" t="s">
+        <v>295</v>
+      </c>
+      <c r="D59" s="142"/>
+      <c r="E59" s="143"/>
+      <c r="F59" s="143"/>
+      <c r="G59" s="75"/>
+      <c r="H59" s="82"/>
+      <c r="I59" s="76"/>
+      <c r="J59" s="74"/>
+    </row>
+    <row r="60" spans="1:10" s="4" customFormat="1" ht="136.5" customHeight="1" outlineLevel="1">
+      <c r="A60" s="77" t="s">
+        <v>1</v>
+      </c>
+      <c r="B60" s="92" t="s">
+        <v>294</v>
+      </c>
+      <c r="C60" s="76" t="s">
+        <v>296</v>
+      </c>
+      <c r="D60" s="142"/>
+      <c r="E60" s="143"/>
+      <c r="F60" s="143"/>
+      <c r="G60" s="75"/>
+      <c r="H60" s="82"/>
+      <c r="I60" s="76"/>
+      <c r="J60" s="74"/>
+    </row>
+    <row r="61" spans="1:10" s="4" customFormat="1" ht="148.5" customHeight="1" outlineLevel="1">
+      <c r="A61" s="77" t="s">
+        <v>2</v>
+      </c>
+      <c r="B61" s="92" t="s">
+        <v>297</v>
+      </c>
+      <c r="C61" s="76" t="s">
+        <v>298</v>
+      </c>
+      <c r="D61" s="142"/>
+      <c r="E61" s="143"/>
+      <c r="F61" s="143"/>
+      <c r="G61" s="75"/>
+      <c r="H61" s="82"/>
+      <c r="I61" s="76"/>
+      <c r="J61" s="74"/>
+    </row>
+    <row r="62" spans="1:10" s="4" customFormat="1" ht="101.25" customHeight="1" outlineLevel="1">
+      <c r="A62" s="77" t="s">
+        <v>49</v>
+      </c>
+      <c r="B62" s="92" t="s">
+        <v>299</v>
+      </c>
+      <c r="C62" s="76" t="s">
+        <v>300</v>
+      </c>
+      <c r="D62" s="142"/>
+      <c r="E62" s="143"/>
+      <c r="F62" s="143"/>
+      <c r="G62" s="75"/>
+      <c r="H62" s="82"/>
+      <c r="I62" s="76"/>
+      <c r="J62" s="74"/>
+    </row>
+    <row r="63" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
+      <c r="A63" s="129"/>
+      <c r="B63" s="130"/>
+      <c r="C63" s="130"/>
+      <c r="D63" s="97"/>
+      <c r="E63" s="97"/>
+      <c r="F63" s="97"/>
+      <c r="G63" s="97"/>
+      <c r="H63" s="97"/>
+      <c r="I63" s="97"/>
+      <c r="J63" s="98"/>
+    </row>
+    <row r="64" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A64" s="77"/>
+      <c r="B64" s="92"/>
+      <c r="C64" s="76"/>
+      <c r="D64" s="142"/>
+      <c r="E64" s="143"/>
+      <c r="F64" s="143"/>
+      <c r="G64" s="75"/>
+      <c r="H64" s="82"/>
+      <c r="I64" s="76"/>
+      <c r="J64" s="74"/>
+    </row>
+    <row r="65" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
+      <c r="A65" s="129"/>
+      <c r="B65" s="130"/>
+      <c r="C65" s="130"/>
+      <c r="D65" s="97"/>
+      <c r="E65" s="97"/>
+      <c r="F65" s="97"/>
+      <c r="G65" s="97"/>
+      <c r="H65" s="97"/>
+      <c r="I65" s="97"/>
+      <c r="J65" s="98"/>
+    </row>
+    <row r="66" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A66" s="77"/>
+      <c r="B66" s="92"/>
+      <c r="C66" s="76"/>
+      <c r="D66" s="142"/>
+      <c r="E66" s="143"/>
+      <c r="F66" s="143"/>
+      <c r="G66" s="75"/>
+      <c r="H66" s="82"/>
+      <c r="I66" s="76"/>
+      <c r="J66" s="74"/>
+    </row>
+    <row r="67" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A67" s="170"/>
+      <c r="B67" s="171"/>
+      <c r="C67" s="172"/>
+      <c r="D67" s="173"/>
+      <c r="E67" s="173"/>
+      <c r="F67" s="173"/>
+      <c r="G67" s="172"/>
+      <c r="H67" s="172"/>
+      <c r="I67" s="172"/>
+      <c r="J67" s="174"/>
+    </row>
+    <row r="68" spans="1:10" ht="12" customHeight="1">
       <c r="I68"/>
       <c r="J68"/>
     </row>
-    <row r="69" spans="9:10" ht="12" customHeight="1">
+    <row r="69" spans="1:10" ht="12" customHeight="1">
       <c r="I69"/>
       <c r="J69"/>
     </row>
-    <row r="70" spans="9:10" ht="12" customHeight="1">
+    <row r="70" spans="1:10" ht="12" customHeight="1">
       <c r="I70"/>
       <c r="J70"/>
     </row>
-    <row r="71" spans="9:10" ht="12" customHeight="1">
+    <row r="71" spans="1:10" ht="12" customHeight="1">
       <c r="I71"/>
       <c r="J71"/>
     </row>
-    <row r="72" spans="9:10" ht="12" customHeight="1">
+    <row r="72" spans="1:10" ht="12" customHeight="1">
       <c r="I72"/>
       <c r="J72"/>
     </row>
-    <row r="73" spans="9:10">
-      <c r="I73" s="19"/>
+    <row r="73" spans="1:10" ht="12" customHeight="1">
+      <c r="I73"/>
       <c r="J73"/>
     </row>
-    <row r="74" spans="9:10">
-      <c r="I74" s="19"/>
+    <row r="74" spans="1:10" ht="12" customHeight="1">
+      <c r="I74"/>
       <c r="J74"/>
     </row>
-    <row r="75" spans="9:10">
-      <c r="I75" s="19"/>
+    <row r="75" spans="1:10" ht="12" customHeight="1">
+      <c r="I75"/>
       <c r="J75"/>
     </row>
-    <row r="76" spans="9:10">
-      <c r="I76" s="19"/>
+    <row r="76" spans="1:10" ht="12" customHeight="1">
+      <c r="I76"/>
       <c r="J76"/>
     </row>
-    <row r="77" spans="9:10">
-      <c r="I77" s="19"/>
+    <row r="77" spans="1:10" ht="12" customHeight="1">
+      <c r="I77"/>
       <c r="J77"/>
     </row>
-    <row r="78" spans="9:10">
-      <c r="I78" s="19"/>
+    <row r="78" spans="1:10" ht="12" customHeight="1">
+      <c r="I78"/>
       <c r="J78"/>
     </row>
-    <row r="79" spans="9:10">
-      <c r="I79" s="19"/>
+    <row r="79" spans="1:10" ht="12" customHeight="1">
+      <c r="I79"/>
       <c r="J79"/>
     </row>
-    <row r="80" spans="9:10">
-      <c r="I80" s="19"/>
+    <row r="80" spans="1:10" ht="12" customHeight="1">
+      <c r="I80"/>
       <c r="J80"/>
     </row>
-    <row r="81" spans="9:10">
-      <c r="I81" s="19"/>
+    <row r="81" spans="9:10" ht="12" customHeight="1">
+      <c r="I81"/>
       <c r="J81"/>
     </row>
-    <row r="82" spans="9:10">
-      <c r="I82" s="19"/>
+    <row r="82" spans="9:10" ht="12" customHeight="1">
+      <c r="I82"/>
       <c r="J82"/>
     </row>
-    <row r="83" spans="9:10">
-      <c r="I83" s="19"/>
+    <row r="83" spans="9:10" ht="12" customHeight="1">
+      <c r="I83"/>
       <c r="J83"/>
     </row>
     <row r="84" spans="9:10">
@@ -7184,8 +7407,62 @@
       <c r="I88" s="19"/>
       <c r="J88"/>
     </row>
+    <row r="89" spans="9:10">
+      <c r="I89" s="19"/>
+      <c r="J89"/>
+    </row>
+    <row r="90" spans="9:10">
+      <c r="I90" s="19"/>
+      <c r="J90"/>
+    </row>
+    <row r="91" spans="9:10">
+      <c r="I91" s="19"/>
+      <c r="J91"/>
+    </row>
+    <row r="92" spans="9:10">
+      <c r="I92" s="19"/>
+      <c r="J92"/>
+    </row>
+    <row r="93" spans="9:10">
+      <c r="I93" s="19"/>
+      <c r="J93"/>
+    </row>
+    <row r="94" spans="9:10">
+      <c r="I94" s="19"/>
+      <c r="J94"/>
+    </row>
+    <row r="95" spans="9:10">
+      <c r="I95" s="19"/>
+      <c r="J95"/>
+    </row>
+    <row r="96" spans="9:10">
+      <c r="I96" s="19"/>
+      <c r="J96"/>
+    </row>
+    <row r="97" spans="9:10">
+      <c r="I97" s="19"/>
+      <c r="J97"/>
+    </row>
+    <row r="98" spans="9:10">
+      <c r="I98" s="19"/>
+      <c r="J98"/>
+    </row>
+    <row r="99" spans="9:10">
+      <c r="I99" s="19"/>
+      <c r="J99"/>
+    </row>
   </sheetData>
-  <mergeCells count="63">
+  <mergeCells count="73">
+    <mergeCell ref="D66:F66"/>
+    <mergeCell ref="D56:F56"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="D60:F60"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="D62:F62"/>
+    <mergeCell ref="A63:C63"/>
+    <mergeCell ref="D64:F64"/>
+    <mergeCell ref="A65:C65"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="D29:F29"/>
     <mergeCell ref="D30:F30"/>
@@ -7202,7 +7479,7 @@
     <mergeCell ref="D54:F54"/>
     <mergeCell ref="A55:C55"/>
     <mergeCell ref="A43:C43"/>
-    <mergeCell ref="D56:F56"/>
+    <mergeCell ref="D57:F57"/>
     <mergeCell ref="D44:F44"/>
     <mergeCell ref="A50:C50"/>
     <mergeCell ref="D51:F51"/>
@@ -7265,7 +7542,7 @@
   </sheetPr>
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="82" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="82" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -7285,9 +7562,9 @@
       <c r="A1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="146"/>
-      <c r="D1" s="146"/>
+      <c r="B1" s="147"/>
+      <c r="C1" s="147"/>
+      <c r="D1" s="147"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -7298,9 +7575,9 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="147"/>
-      <c r="C2" s="147"/>
-      <c r="D2" s="147"/>
+      <c r="B2" s="148"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -7313,51 +7590,51 @@
       <c r="A3" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="123" t="s">
+      <c r="B3" s="124" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="123"/>
-      <c r="D3" s="124"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="125"/>
       <c r="E3" s="60"/>
       <c r="F3" s="60"/>
       <c r="G3" s="60"/>
-      <c r="H3" s="154"/>
-      <c r="I3" s="154"/>
-      <c r="J3" s="154"/>
+      <c r="H3" s="155"/>
+      <c r="I3" s="155"/>
+      <c r="J3" s="155"/>
       <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="12.75">
       <c r="A4" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="155" t="s">
+      <c r="B4" s="156" t="s">
         <v>126</v>
       </c>
-      <c r="C4" s="156"/>
-      <c r="D4" s="157"/>
+      <c r="C4" s="157"/>
+      <c r="D4" s="158"/>
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
       <c r="G4" s="60"/>
-      <c r="H4" s="154"/>
-      <c r="I4" s="154"/>
-      <c r="J4" s="154"/>
+      <c r="H4" s="155"/>
+      <c r="I4" s="155"/>
+      <c r="J4" s="155"/>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" s="70" customFormat="1" ht="25.5">
       <c r="A5" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="149" t="s">
+      <c r="B5" s="150" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="150"/>
-      <c r="D5" s="151"/>
+      <c r="C5" s="151"/>
+      <c r="D5" s="152"/>
       <c r="E5" s="68"/>
       <c r="F5" s="68"/>
       <c r="G5" s="68"/>
-      <c r="H5" s="153"/>
-      <c r="I5" s="153"/>
-      <c r="J5" s="153"/>
+      <c r="H5" s="154"/>
+      <c r="I5" s="154"/>
+      <c r="J5" s="154"/>
       <c r="K5" s="69"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
@@ -7378,9 +7655,9 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="154"/>
-      <c r="I6" s="154"/>
-      <c r="J6" s="154"/>
+      <c r="H6" s="155"/>
+      <c r="I6" s="155"/>
+      <c r="J6" s="155"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -7401,16 +7678,16 @@
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
       <c r="G7" s="61"/>
-      <c r="H7" s="154"/>
-      <c r="I7" s="154"/>
-      <c r="J7" s="154"/>
+      <c r="H7" s="155"/>
+      <c r="I7" s="155"/>
+      <c r="J7" s="155"/>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="148"/>
-      <c r="B8" s="148"/>
-      <c r="C8" s="148"/>
-      <c r="D8" s="148"/>
+      <c r="A8" s="149"/>
+      <c r="B8" s="149"/>
+      <c r="C8" s="149"/>
+      <c r="D8" s="149"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -7420,70 +7697,70 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" s="72" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="132" t="s">
+      <c r="A9" s="133" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="161" t="s">
+      <c r="B9" s="162" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="132" t="s">
+      <c r="C9" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="133" t="s">
+      <c r="D9" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="134"/>
-      <c r="F9" s="134"/>
-      <c r="G9" s="135"/>
-      <c r="H9" s="158" t="s">
+      <c r="E9" s="135"/>
+      <c r="F9" s="135"/>
+      <c r="G9" s="136"/>
+      <c r="H9" s="159" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="127" t="s">
+      <c r="I9" s="128" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="127" t="s">
+      <c r="J9" s="128" t="s">
         <v>32</v>
       </c>
       <c r="K9" s="71"/>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="127"/>
-      <c r="B10" s="162"/>
-      <c r="C10" s="127"/>
-      <c r="D10" s="136"/>
-      <c r="E10" s="137"/>
-      <c r="F10" s="137"/>
-      <c r="G10" s="138"/>
-      <c r="H10" s="136"/>
-      <c r="I10" s="127"/>
-      <c r="J10" s="127"/>
+      <c r="A10" s="128"/>
+      <c r="B10" s="163"/>
+      <c r="C10" s="128"/>
+      <c r="D10" s="137"/>
+      <c r="E10" s="138"/>
+      <c r="F10" s="138"/>
+      <c r="G10" s="139"/>
+      <c r="H10" s="137"/>
+      <c r="I10" s="128"/>
+      <c r="J10" s="128"/>
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" s="73" customFormat="1" ht="15">
-      <c r="A11" s="159"/>
-      <c r="B11" s="159"/>
-      <c r="C11" s="159"/>
-      <c r="D11" s="159"/>
-      <c r="E11" s="159"/>
-      <c r="F11" s="159"/>
-      <c r="G11" s="159"/>
-      <c r="H11" s="159"/>
-      <c r="I11" s="159"/>
-      <c r="J11" s="160"/>
+      <c r="A11" s="160"/>
+      <c r="B11" s="160"/>
+      <c r="C11" s="160"/>
+      <c r="D11" s="160"/>
+      <c r="E11" s="160"/>
+      <c r="F11" s="160"/>
+      <c r="G11" s="160"/>
+      <c r="H11" s="160"/>
+      <c r="I11" s="160"/>
+      <c r="J11" s="161"/>
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A12" s="139" t="s">
+      <c r="A12" s="140" t="s">
         <v>127</v>
       </c>
-      <c r="B12" s="140"/>
-      <c r="C12" s="140"/>
-      <c r="D12" s="140"/>
-      <c r="E12" s="140"/>
-      <c r="F12" s="140"/>
-      <c r="G12" s="140"/>
-      <c r="H12" s="140"/>
-      <c r="I12" s="140"/>
-      <c r="J12" s="152"/>
+      <c r="B12" s="141"/>
+      <c r="C12" s="141"/>
+      <c r="D12" s="141"/>
+      <c r="E12" s="141"/>
+      <c r="F12" s="141"/>
+      <c r="G12" s="141"/>
+      <c r="H12" s="141"/>
+      <c r="I12" s="141"/>
+      <c r="J12" s="153"/>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" ht="102.75" customHeight="1" outlineLevel="1">
       <c r="A13" s="77" t="s">
@@ -7495,11 +7772,11 @@
       <c r="C13" s="76" t="s">
         <v>165</v>
       </c>
-      <c r="D13" s="125" t="s">
+      <c r="D13" s="126" t="s">
         <v>166</v>
       </c>
-      <c r="E13" s="126"/>
-      <c r="F13" s="126"/>
+      <c r="E13" s="127"/>
+      <c r="F13" s="127"/>
       <c r="G13" s="75"/>
       <c r="H13" s="89"/>
       <c r="I13" s="76"/>
@@ -7515,11 +7792,11 @@
       <c r="C14" s="76" t="s">
         <v>169</v>
       </c>
-      <c r="D14" s="125" t="s">
+      <c r="D14" s="126" t="s">
         <v>170</v>
       </c>
-      <c r="E14" s="126"/>
-      <c r="F14" s="126"/>
+      <c r="E14" s="127"/>
+      <c r="F14" s="127"/>
       <c r="G14" s="75"/>
       <c r="H14" s="89"/>
       <c r="I14" s="76"/>
@@ -7535,22 +7812,22 @@
       <c r="C15" s="76" t="s">
         <v>172</v>
       </c>
-      <c r="D15" s="125" t="s">
+      <c r="D15" s="126" t="s">
         <v>173</v>
       </c>
-      <c r="E15" s="126"/>
-      <c r="F15" s="126"/>
+      <c r="E15" s="127"/>
+      <c r="F15" s="127"/>
       <c r="G15" s="75"/>
       <c r="H15" s="89"/>
       <c r="I15" s="76"/>
       <c r="J15" s="74"/>
     </row>
     <row r="16" spans="1:11" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A16" s="139" t="s">
+      <c r="A16" s="140" t="s">
         <v>128</v>
       </c>
-      <c r="B16" s="140"/>
-      <c r="C16" s="140"/>
+      <c r="B16" s="141"/>
+      <c r="C16" s="141"/>
       <c r="D16" s="87"/>
       <c r="E16" s="87"/>
       <c r="F16" s="87"/>
@@ -7569,11 +7846,11 @@
       <c r="C17" s="86" t="s">
         <v>136</v>
       </c>
-      <c r="D17" s="167" t="s">
+      <c r="D17" s="168" t="s">
         <v>135</v>
       </c>
-      <c r="E17" s="168"/>
-      <c r="F17" s="168"/>
+      <c r="E17" s="169"/>
+      <c r="F17" s="169"/>
       <c r="G17" s="94"/>
       <c r="H17" s="95"/>
       <c r="I17" s="86"/>
@@ -7589,11 +7866,11 @@
       <c r="C18" s="86" t="s">
         <v>138</v>
       </c>
-      <c r="D18" s="167" t="s">
+      <c r="D18" s="168" t="s">
         <v>139</v>
       </c>
-      <c r="E18" s="168"/>
-      <c r="F18" s="168"/>
+      <c r="E18" s="169"/>
+      <c r="F18" s="169"/>
       <c r="G18" s="94"/>
       <c r="H18" s="95"/>
       <c r="I18" s="86"/>
@@ -7609,22 +7886,22 @@
       <c r="C19" s="86" t="s">
         <v>136</v>
       </c>
-      <c r="D19" s="167" t="s">
+      <c r="D19" s="168" t="s">
         <v>141</v>
       </c>
-      <c r="E19" s="168"/>
-      <c r="F19" s="168"/>
+      <c r="E19" s="169"/>
+      <c r="F19" s="169"/>
       <c r="G19" s="94"/>
       <c r="H19" s="95"/>
       <c r="I19" s="86"/>
       <c r="J19" s="96"/>
     </row>
     <row r="20" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A20" s="139" t="s">
+      <c r="A20" s="140" t="s">
         <v>145</v>
       </c>
-      <c r="B20" s="140"/>
-      <c r="C20" s="140"/>
+      <c r="B20" s="141"/>
+      <c r="C20" s="141"/>
       <c r="D20" s="87"/>
       <c r="E20" s="87"/>
       <c r="F20" s="87"/>
@@ -7643,11 +7920,11 @@
       <c r="C21" s="76" t="s">
         <v>149</v>
       </c>
-      <c r="D21" s="125" t="s">
+      <c r="D21" s="126" t="s">
         <v>147</v>
       </c>
-      <c r="E21" s="126"/>
-      <c r="F21" s="126"/>
+      <c r="E21" s="127"/>
+      <c r="F21" s="127"/>
       <c r="G21" s="75"/>
       <c r="H21" s="82"/>
       <c r="I21" s="76"/>
@@ -7663,11 +7940,11 @@
       <c r="C22" s="76" t="s">
         <v>150</v>
       </c>
-      <c r="D22" s="125" t="s">
+      <c r="D22" s="126" t="s">
         <v>151</v>
       </c>
-      <c r="E22" s="126"/>
-      <c r="F22" s="126"/>
+      <c r="E22" s="127"/>
+      <c r="F22" s="127"/>
       <c r="G22" s="75"/>
       <c r="H22" s="82"/>
       <c r="I22" s="76"/>
@@ -7683,11 +7960,11 @@
       <c r="C23" s="76" t="s">
         <v>153</v>
       </c>
-      <c r="D23" s="125" t="s">
+      <c r="D23" s="126" t="s">
         <v>154</v>
       </c>
-      <c r="E23" s="126"/>
-      <c r="F23" s="126"/>
+      <c r="E23" s="127"/>
+      <c r="F23" s="127"/>
       <c r="G23" s="75"/>
       <c r="H23" s="82"/>
       <c r="I23" s="76"/>
@@ -7703,20 +7980,20 @@
       <c r="C24" s="76" t="s">
         <v>156</v>
       </c>
-      <c r="D24" s="125" t="s">
+      <c r="D24" s="126" t="s">
         <v>157</v>
       </c>
-      <c r="E24" s="126"/>
-      <c r="F24" s="126"/>
+      <c r="E24" s="127"/>
+      <c r="F24" s="127"/>
       <c r="G24" s="75"/>
       <c r="H24" s="82"/>
       <c r="I24" s="76"/>
       <c r="J24" s="74"/>
     </row>
     <row r="25" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A25" s="128"/>
-      <c r="B25" s="129"/>
-      <c r="C25" s="129"/>
+      <c r="A25" s="129"/>
+      <c r="B25" s="130"/>
+      <c r="C25" s="130"/>
       <c r="D25" s="97"/>
       <c r="E25" s="97"/>
       <c r="F25" s="97"/>
@@ -7729,9 +8006,9 @@
       <c r="A26" s="77"/>
       <c r="B26" s="92"/>
       <c r="C26" s="76"/>
-      <c r="D26" s="141"/>
-      <c r="E26" s="142"/>
-      <c r="F26" s="142"/>
+      <c r="D26" s="142"/>
+      <c r="E26" s="143"/>
+      <c r="F26" s="143"/>
       <c r="G26" s="75"/>
       <c r="H26" s="82"/>
       <c r="I26" s="76"/>
@@ -7741,9 +8018,9 @@
       <c r="A27" s="77"/>
       <c r="B27" s="92"/>
       <c r="C27" s="76"/>
-      <c r="D27" s="141"/>
-      <c r="E27" s="142"/>
-      <c r="F27" s="142"/>
+      <c r="D27" s="142"/>
+      <c r="E27" s="143"/>
+      <c r="F27" s="143"/>
       <c r="G27" s="75"/>
       <c r="H27" s="82"/>
       <c r="I27" s="76"/>
@@ -7753,9 +8030,9 @@
       <c r="A28" s="77"/>
       <c r="B28" s="92"/>
       <c r="C28" s="76"/>
-      <c r="D28" s="141"/>
-      <c r="E28" s="142"/>
-      <c r="F28" s="142"/>
+      <c r="D28" s="142"/>
+      <c r="E28" s="143"/>
+      <c r="F28" s="143"/>
       <c r="G28" s="75"/>
       <c r="H28" s="82"/>
       <c r="I28" s="76"/>
@@ -7765,9 +8042,9 @@
       <c r="A29" s="77"/>
       <c r="B29" s="92"/>
       <c r="C29" s="76"/>
-      <c r="D29" s="141"/>
-      <c r="E29" s="142"/>
-      <c r="F29" s="142"/>
+      <c r="D29" s="142"/>
+      <c r="E29" s="143"/>
+      <c r="F29" s="143"/>
       <c r="G29" s="75"/>
       <c r="H29" s="82"/>
       <c r="I29" s="76"/>
@@ -7777,9 +8054,9 @@
       <c r="A30" s="77"/>
       <c r="B30" s="92"/>
       <c r="C30" s="76"/>
-      <c r="D30" s="141"/>
-      <c r="E30" s="142"/>
-      <c r="F30" s="142"/>
+      <c r="D30" s="142"/>
+      <c r="E30" s="143"/>
+      <c r="F30" s="143"/>
       <c r="G30" s="75"/>
       <c r="H30" s="82"/>
       <c r="I30" s="76"/>
@@ -7789,18 +8066,18 @@
       <c r="A31" s="77"/>
       <c r="B31" s="92"/>
       <c r="C31" s="76"/>
-      <c r="D31" s="141"/>
-      <c r="E31" s="142"/>
-      <c r="F31" s="142"/>
+      <c r="D31" s="142"/>
+      <c r="E31" s="143"/>
+      <c r="F31" s="143"/>
       <c r="G31" s="75"/>
       <c r="H31" s="82"/>
       <c r="I31" s="76"/>
       <c r="J31" s="74"/>
     </row>
     <row r="32" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A32" s="128"/>
-      <c r="B32" s="129"/>
-      <c r="C32" s="129"/>
+      <c r="A32" s="129"/>
+      <c r="B32" s="130"/>
+      <c r="C32" s="130"/>
       <c r="D32" s="97"/>
       <c r="E32" s="97"/>
       <c r="F32" s="97"/>
@@ -7813,9 +8090,9 @@
       <c r="A33" s="77"/>
       <c r="B33" s="92"/>
       <c r="C33" s="76"/>
-      <c r="D33" s="141"/>
-      <c r="E33" s="142"/>
-      <c r="F33" s="142"/>
+      <c r="D33" s="142"/>
+      <c r="E33" s="143"/>
+      <c r="F33" s="143"/>
       <c r="G33" s="75"/>
       <c r="H33" s="82"/>
       <c r="I33" s="76"/>
@@ -8003,10 +8280,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K68"/>
+  <dimension ref="A1:K67"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="80" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:B22"/>
+    <sheetView topLeftCell="A20" zoomScale="80" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" outlineLevelRow="1"/>
@@ -8025,9 +8302,9 @@
       <c r="A1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="146"/>
-      <c r="D1" s="146"/>
+      <c r="B1" s="147"/>
+      <c r="C1" s="147"/>
+      <c r="D1" s="147"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -8038,9 +8315,9 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="147"/>
-      <c r="C2" s="147"/>
-      <c r="D2" s="147"/>
+      <c r="B2" s="148"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -8053,51 +8330,51 @@
       <c r="A3" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="123" t="s">
+      <c r="B3" s="124" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="123"/>
-      <c r="D3" s="124"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="125"/>
       <c r="E3" s="60"/>
       <c r="F3" s="60"/>
       <c r="G3" s="60"/>
-      <c r="H3" s="154"/>
-      <c r="I3" s="154"/>
-      <c r="J3" s="154"/>
+      <c r="H3" s="155"/>
+      <c r="I3" s="155"/>
+      <c r="J3" s="155"/>
       <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="12.75">
       <c r="A4" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="155" t="s">
+      <c r="B4" s="156" t="s">
         <v>248</v>
       </c>
-      <c r="C4" s="156"/>
-      <c r="D4" s="157"/>
+      <c r="C4" s="157"/>
+      <c r="D4" s="158"/>
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
       <c r="G4" s="60"/>
-      <c r="H4" s="154"/>
-      <c r="I4" s="154"/>
-      <c r="J4" s="154"/>
+      <c r="H4" s="155"/>
+      <c r="I4" s="155"/>
+      <c r="J4" s="155"/>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" s="70" customFormat="1" ht="25.5">
       <c r="A5" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="149" t="s">
+      <c r="B5" s="150" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="150"/>
-      <c r="D5" s="151"/>
+      <c r="C5" s="151"/>
+      <c r="D5" s="152"/>
       <c r="E5" s="68"/>
       <c r="F5" s="68"/>
       <c r="G5" s="68"/>
-      <c r="H5" s="153"/>
-      <c r="I5" s="153"/>
-      <c r="J5" s="153"/>
+      <c r="H5" s="154"/>
+      <c r="I5" s="154"/>
+      <c r="J5" s="154"/>
       <c r="K5" s="69"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
@@ -8105,22 +8382,22 @@
         <v>38</v>
       </c>
       <c r="B6" s="79">
-        <f>COUNTIF(I12:I27,"Pass")</f>
+        <f>COUNTIF(I12:I26,"Pass")</f>
         <v>0</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>39</v>
       </c>
       <c r="D6" s="13">
-        <f>COUNTIF(I10:I733,"Pending")</f>
+        <f>COUNTIF(I10:I732,"Pending")</f>
         <v>0</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="154"/>
-      <c r="I6" s="154"/>
-      <c r="J6" s="154"/>
+      <c r="H6" s="155"/>
+      <c r="I6" s="155"/>
+      <c r="J6" s="155"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -8128,29 +8405,29 @@
         <v>3</v>
       </c>
       <c r="B7" s="80">
-        <f>COUNTIF(I12:I27,"Fail")</f>
+        <f>COUNTIF(I12:I26,"Fail")</f>
         <v>0</v>
       </c>
       <c r="C7" s="29" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="58">
-        <f>COUNTA(A12:A36) -3</f>
-        <v>13</v>
+        <f>COUNTA(A12:A35) -3</f>
+        <v>12</v>
       </c>
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
       <c r="G7" s="61"/>
-      <c r="H7" s="154"/>
-      <c r="I7" s="154"/>
-      <c r="J7" s="154"/>
+      <c r="H7" s="155"/>
+      <c r="I7" s="155"/>
+      <c r="J7" s="155"/>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="148"/>
-      <c r="B8" s="148"/>
-      <c r="C8" s="148"/>
-      <c r="D8" s="148"/>
+      <c r="A8" s="149"/>
+      <c r="B8" s="149"/>
+      <c r="C8" s="149"/>
+      <c r="D8" s="149"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -8160,70 +8437,70 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" s="72" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="132" t="s">
+      <c r="A9" s="133" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="161" t="s">
+      <c r="B9" s="162" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="132" t="s">
+      <c r="C9" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="133" t="s">
+      <c r="D9" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="134"/>
-      <c r="F9" s="134"/>
-      <c r="G9" s="135"/>
-      <c r="H9" s="158" t="s">
+      <c r="E9" s="135"/>
+      <c r="F9" s="135"/>
+      <c r="G9" s="136"/>
+      <c r="H9" s="159" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="127" t="s">
+      <c r="I9" s="128" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="127" t="s">
+      <c r="J9" s="128" t="s">
         <v>32</v>
       </c>
       <c r="K9" s="71"/>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="127"/>
-      <c r="B10" s="162"/>
-      <c r="C10" s="127"/>
-      <c r="D10" s="136"/>
-      <c r="E10" s="137"/>
-      <c r="F10" s="137"/>
-      <c r="G10" s="138"/>
-      <c r="H10" s="136"/>
-      <c r="I10" s="127"/>
-      <c r="J10" s="127"/>
+      <c r="A10" s="128"/>
+      <c r="B10" s="163"/>
+      <c r="C10" s="128"/>
+      <c r="D10" s="137"/>
+      <c r="E10" s="138"/>
+      <c r="F10" s="138"/>
+      <c r="G10" s="139"/>
+      <c r="H10" s="137"/>
+      <c r="I10" s="128"/>
+      <c r="J10" s="128"/>
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" s="73" customFormat="1" ht="15">
-      <c r="A11" s="159"/>
-      <c r="B11" s="159"/>
-      <c r="C11" s="159"/>
-      <c r="D11" s="159"/>
-      <c r="E11" s="159"/>
-      <c r="F11" s="159"/>
-      <c r="G11" s="159"/>
-      <c r="H11" s="159"/>
-      <c r="I11" s="159"/>
-      <c r="J11" s="160"/>
+      <c r="A11" s="160"/>
+      <c r="B11" s="160"/>
+      <c r="C11" s="160"/>
+      <c r="D11" s="160"/>
+      <c r="E11" s="160"/>
+      <c r="F11" s="160"/>
+      <c r="G11" s="160"/>
+      <c r="H11" s="160"/>
+      <c r="I11" s="160"/>
+      <c r="J11" s="161"/>
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A12" s="139" t="s">
+      <c r="A12" s="140" t="s">
         <v>278</v>
       </c>
-      <c r="B12" s="140"/>
-      <c r="C12" s="140"/>
-      <c r="D12" s="140"/>
-      <c r="E12" s="140"/>
-      <c r="F12" s="140"/>
-      <c r="G12" s="140"/>
-      <c r="H12" s="140"/>
-      <c r="I12" s="140"/>
-      <c r="J12" s="152"/>
+      <c r="B12" s="141"/>
+      <c r="C12" s="141"/>
+      <c r="D12" s="141"/>
+      <c r="E12" s="141"/>
+      <c r="F12" s="141"/>
+      <c r="G12" s="141"/>
+      <c r="H12" s="141"/>
+      <c r="I12" s="141"/>
+      <c r="J12" s="153"/>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" ht="132.75" customHeight="1" outlineLevel="1">
       <c r="A13" s="77" t="s">
@@ -8235,9 +8512,9 @@
       <c r="C13" s="122" t="s">
         <v>251</v>
       </c>
-      <c r="D13" s="125"/>
-      <c r="E13" s="126"/>
-      <c r="F13" s="126"/>
+      <c r="D13" s="126"/>
+      <c r="E13" s="127"/>
+      <c r="F13" s="127"/>
       <c r="G13" s="75"/>
       <c r="H13" s="89"/>
       <c r="I13" s="76"/>
@@ -8253,9 +8530,9 @@
       <c r="C14" s="122" t="s">
         <v>252</v>
       </c>
-      <c r="D14" s="125"/>
-      <c r="E14" s="126"/>
-      <c r="F14" s="126"/>
+      <c r="D14" s="126"/>
+      <c r="E14" s="127"/>
+      <c r="F14" s="127"/>
       <c r="G14" s="75"/>
       <c r="H14" s="89"/>
       <c r="I14" s="76"/>
@@ -8271,20 +8548,20 @@
       <c r="C15" s="76" t="s">
         <v>260</v>
       </c>
-      <c r="D15" s="125"/>
-      <c r="E15" s="126"/>
-      <c r="F15" s="126"/>
+      <c r="D15" s="126"/>
+      <c r="E15" s="127"/>
+      <c r="F15" s="127"/>
       <c r="G15" s="75"/>
       <c r="H15" s="89"/>
       <c r="I15" s="76"/>
       <c r="J15" s="74"/>
     </row>
     <row r="16" spans="1:11" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A16" s="139" t="s">
+      <c r="A16" s="140" t="s">
         <v>279</v>
       </c>
-      <c r="B16" s="140"/>
-      <c r="C16" s="140"/>
+      <c r="B16" s="141"/>
+      <c r="C16" s="141"/>
       <c r="D16" s="87"/>
       <c r="E16" s="87"/>
       <c r="F16" s="87"/>
@@ -8303,9 +8580,9 @@
       <c r="C17" s="86" t="s">
         <v>286</v>
       </c>
-      <c r="D17" s="167"/>
-      <c r="E17" s="168"/>
-      <c r="F17" s="168"/>
+      <c r="D17" s="168"/>
+      <c r="E17" s="169"/>
+      <c r="F17" s="169"/>
       <c r="G17" s="94"/>
       <c r="H17" s="95"/>
       <c r="I17" s="86"/>
@@ -8321,9 +8598,9 @@
       <c r="C18" s="86" t="s">
         <v>287</v>
       </c>
-      <c r="D18" s="167"/>
-      <c r="E18" s="168"/>
-      <c r="F18" s="168"/>
+      <c r="D18" s="168"/>
+      <c r="E18" s="169"/>
+      <c r="F18" s="169"/>
       <c r="G18" s="94"/>
       <c r="H18" s="95"/>
       <c r="I18" s="86"/>
@@ -8339,9 +8616,9 @@
       <c r="C19" s="76" t="s">
         <v>269</v>
       </c>
-      <c r="D19" s="167"/>
-      <c r="E19" s="168"/>
-      <c r="F19" s="168"/>
+      <c r="D19" s="168"/>
+      <c r="E19" s="169"/>
+      <c r="F19" s="169"/>
       <c r="G19" s="94"/>
       <c r="H19" s="95"/>
       <c r="I19" s="86"/>
@@ -8357,9 +8634,9 @@
       <c r="C20" s="86" t="s">
         <v>282</v>
       </c>
-      <c r="D20" s="167"/>
-      <c r="E20" s="168"/>
-      <c r="F20" s="168"/>
+      <c r="D20" s="168"/>
+      <c r="E20" s="169"/>
+      <c r="F20" s="169"/>
       <c r="G20" s="94"/>
       <c r="H20" s="95"/>
       <c r="I20" s="86"/>
@@ -8372,140 +8649,134 @@
       <c r="B21" s="85" t="s">
         <v>280</v>
       </c>
-      <c r="C21" s="169" t="s">
+      <c r="C21" s="123" t="s">
         <v>283</v>
       </c>
-      <c r="D21" s="167"/>
-      <c r="E21" s="168"/>
-      <c r="F21" s="168"/>
+      <c r="D21" s="168"/>
+      <c r="E21" s="169"/>
+      <c r="F21" s="169"/>
       <c r="G21" s="94"/>
       <c r="H21" s="95"/>
       <c r="I21" s="86"/>
       <c r="J21" s="96"/>
     </row>
-    <row r="22" spans="1:10" s="4" customFormat="1" ht="179.25" customHeight="1" outlineLevel="1">
-      <c r="A22" s="93" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="85" t="s">
-        <v>280</v>
-      </c>
-      <c r="C22" s="169" t="s">
-        <v>283</v>
-      </c>
-      <c r="D22" s="170"/>
-      <c r="E22" s="171"/>
-      <c r="F22" s="171"/>
-      <c r="G22" s="94"/>
-      <c r="H22" s="95"/>
-      <c r="I22" s="86"/>
-      <c r="J22" s="96"/>
-    </row>
-    <row r="23" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A23" s="139" t="s">
+    <row r="22" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
+      <c r="A22" s="140" t="s">
         <v>255</v>
       </c>
-      <c r="B23" s="140"/>
-      <c r="C23" s="140"/>
-      <c r="D23" s="87"/>
-      <c r="E23" s="87"/>
-      <c r="F23" s="87"/>
-      <c r="G23" s="87"/>
-      <c r="H23" s="87"/>
-      <c r="I23" s="87"/>
-      <c r="J23" s="88"/>
-    </row>
-    <row r="24" spans="1:10" s="4" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="B22" s="141"/>
+      <c r="C22" s="141"/>
+      <c r="D22" s="87"/>
+      <c r="E22" s="87"/>
+      <c r="F22" s="87"/>
+      <c r="G22" s="87"/>
+      <c r="H22" s="87"/>
+      <c r="I22" s="87"/>
+      <c r="J22" s="88"/>
+    </row>
+    <row r="23" spans="1:10" s="4" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A23" s="77" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="92" t="s">
+        <v>257</v>
+      </c>
+      <c r="C23" s="76" t="s">
+        <v>258</v>
+      </c>
+      <c r="D23" s="126"/>
+      <c r="E23" s="127"/>
+      <c r="F23" s="127"/>
+      <c r="G23" s="75"/>
+      <c r="H23" s="82"/>
+      <c r="I23" s="76"/>
+      <c r="J23" s="74"/>
+    </row>
+    <row r="24" spans="1:10" s="4" customFormat="1" ht="148.5" customHeight="1" outlineLevel="1">
       <c r="A24" s="77" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B24" s="92" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C24" s="76" t="s">
-        <v>258</v>
-      </c>
-      <c r="D24" s="125"/>
-      <c r="E24" s="126"/>
-      <c r="F24" s="126"/>
+        <v>260</v>
+      </c>
+      <c r="D24" s="126"/>
+      <c r="E24" s="127"/>
+      <c r="F24" s="127"/>
       <c r="G24" s="75"/>
       <c r="H24" s="82"/>
       <c r="I24" s="76"/>
       <c r="J24" s="74"/>
     </row>
-    <row r="25" spans="1:10" s="4" customFormat="1" ht="148.5" customHeight="1" outlineLevel="1">
+    <row r="25" spans="1:10" s="4" customFormat="1" ht="123.75" customHeight="1" outlineLevel="1">
       <c r="A25" s="77" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B25" s="92" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="C25" s="76" t="s">
-        <v>260</v>
-      </c>
-      <c r="D25" s="125"/>
-      <c r="E25" s="126"/>
-      <c r="F25" s="126"/>
+        <v>269</v>
+      </c>
+      <c r="D25" s="126"/>
+      <c r="E25" s="127"/>
+      <c r="F25" s="127"/>
       <c r="G25" s="75"/>
       <c r="H25" s="82"/>
       <c r="I25" s="76"/>
       <c r="J25" s="74"/>
     </row>
-    <row r="26" spans="1:10" s="4" customFormat="1" ht="123.75" customHeight="1" outlineLevel="1">
+    <row r="26" spans="1:10" s="4" customFormat="1" ht="148.5" customHeight="1" outlineLevel="1">
       <c r="A26" s="77" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="B26" s="92" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C26" s="76" t="s">
-        <v>269</v>
-      </c>
-      <c r="D26" s="125"/>
-      <c r="E26" s="126"/>
-      <c r="F26" s="126"/>
+        <v>266</v>
+      </c>
+      <c r="D26" s="126"/>
+      <c r="E26" s="127"/>
+      <c r="F26" s="127"/>
       <c r="G26" s="75"/>
       <c r="H26" s="82"/>
       <c r="I26" s="76"/>
       <c r="J26" s="74"/>
     </row>
-    <row r="27" spans="1:10" s="4" customFormat="1" ht="148.5" customHeight="1" outlineLevel="1">
-      <c r="A27" s="77" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" s="92" t="s">
-        <v>263</v>
-      </c>
-      <c r="C27" s="76" t="s">
-        <v>266</v>
-      </c>
-      <c r="D27" s="125"/>
-      <c r="E27" s="126"/>
-      <c r="F27" s="126"/>
-      <c r="G27" s="75"/>
-      <c r="H27" s="82"/>
-      <c r="I27" s="76"/>
-      <c r="J27" s="74"/>
-    </row>
-    <row r="28" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A28" s="128"/>
-      <c r="B28" s="129"/>
-      <c r="C28" s="129"/>
-      <c r="D28" s="97"/>
-      <c r="E28" s="97"/>
-      <c r="F28" s="97"/>
-      <c r="G28" s="97"/>
-      <c r="H28" s="97"/>
-      <c r="I28" s="97"/>
-      <c r="J28" s="98"/>
-    </row>
-    <row r="29" spans="1:10" s="4" customFormat="1" ht="78.75" customHeight="1" outlineLevel="1">
+    <row r="27" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
+      <c r="A27" s="129"/>
+      <c r="B27" s="130"/>
+      <c r="C27" s="130"/>
+      <c r="D27" s="97"/>
+      <c r="E27" s="97"/>
+      <c r="F27" s="97"/>
+      <c r="G27" s="97"/>
+      <c r="H27" s="97"/>
+      <c r="I27" s="97"/>
+      <c r="J27" s="98"/>
+    </row>
+    <row r="28" spans="1:10" s="4" customFormat="1" ht="78.75" customHeight="1" outlineLevel="1">
+      <c r="A28" s="77"/>
+      <c r="B28" s="92"/>
+      <c r="C28" s="76"/>
+      <c r="D28" s="142"/>
+      <c r="E28" s="143"/>
+      <c r="F28" s="143"/>
+      <c r="G28" s="75"/>
+      <c r="H28" s="82"/>
+      <c r="I28" s="76"/>
+      <c r="J28" s="74"/>
+    </row>
+    <row r="29" spans="1:10" s="4" customFormat="1" ht="79.5" customHeight="1" outlineLevel="1">
       <c r="A29" s="77"/>
       <c r="B29" s="92"/>
       <c r="C29" s="76"/>
-      <c r="D29" s="141"/>
-      <c r="E29" s="142"/>
-      <c r="F29" s="142"/>
+      <c r="D29" s="142"/>
+      <c r="E29" s="143"/>
+      <c r="F29" s="143"/>
       <c r="G29" s="75"/>
       <c r="H29" s="82"/>
       <c r="I29" s="76"/>
@@ -8515,9 +8786,9 @@
       <c r="A30" s="77"/>
       <c r="B30" s="92"/>
       <c r="C30" s="76"/>
-      <c r="D30" s="141"/>
-      <c r="E30" s="142"/>
-      <c r="F30" s="142"/>
+      <c r="D30" s="142"/>
+      <c r="E30" s="143"/>
+      <c r="F30" s="143"/>
       <c r="G30" s="75"/>
       <c r="H30" s="82"/>
       <c r="I30" s="76"/>
@@ -8527,73 +8798,65 @@
       <c r="A31" s="77"/>
       <c r="B31" s="92"/>
       <c r="C31" s="76"/>
-      <c r="D31" s="141"/>
-      <c r="E31" s="142"/>
-      <c r="F31" s="142"/>
+      <c r="D31" s="142"/>
+      <c r="E31" s="143"/>
+      <c r="F31" s="143"/>
       <c r="G31" s="75"/>
       <c r="H31" s="82"/>
       <c r="I31" s="76"/>
       <c r="J31" s="74"/>
     </row>
-    <row r="32" spans="1:10" s="4" customFormat="1" ht="79.5" customHeight="1" outlineLevel="1">
+    <row r="32" spans="1:10" s="4" customFormat="1" ht="91.5" customHeight="1" outlineLevel="1">
       <c r="A32" s="77"/>
       <c r="B32" s="92"/>
       <c r="C32" s="76"/>
-      <c r="D32" s="141"/>
-      <c r="E32" s="142"/>
-      <c r="F32" s="142"/>
+      <c r="D32" s="142"/>
+      <c r="E32" s="143"/>
+      <c r="F32" s="143"/>
       <c r="G32" s="75"/>
       <c r="H32" s="82"/>
       <c r="I32" s="76"/>
       <c r="J32" s="74"/>
     </row>
-    <row r="33" spans="1:10" s="4" customFormat="1" ht="91.5" customHeight="1" outlineLevel="1">
+    <row r="33" spans="1:10" s="4" customFormat="1" ht="67.5" customHeight="1" outlineLevel="1">
       <c r="A33" s="77"/>
       <c r="B33" s="92"/>
       <c r="C33" s="76"/>
-      <c r="D33" s="141"/>
-      <c r="E33" s="142"/>
-      <c r="F33" s="142"/>
+      <c r="D33" s="142"/>
+      <c r="E33" s="143"/>
+      <c r="F33" s="143"/>
       <c r="G33" s="75"/>
       <c r="H33" s="82"/>
       <c r="I33" s="76"/>
       <c r="J33" s="74"/>
     </row>
-    <row r="34" spans="1:10" s="4" customFormat="1" ht="67.5" customHeight="1" outlineLevel="1">
-      <c r="A34" s="77"/>
-      <c r="B34" s="92"/>
-      <c r="C34" s="76"/>
-      <c r="D34" s="141"/>
-      <c r="E34" s="142"/>
-      <c r="F34" s="142"/>
-      <c r="G34" s="75"/>
-      <c r="H34" s="82"/>
-      <c r="I34" s="76"/>
-      <c r="J34" s="74"/>
-    </row>
-    <row r="35" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A35" s="128"/>
-      <c r="B35" s="129"/>
-      <c r="C35" s="129"/>
-      <c r="D35" s="97"/>
-      <c r="E35" s="97"/>
-      <c r="F35" s="97"/>
-      <c r="G35" s="97"/>
-      <c r="H35" s="97"/>
-      <c r="I35" s="97"/>
-      <c r="J35" s="98"/>
-    </row>
-    <row r="36" spans="1:10" s="4" customFormat="1" ht="47.25" customHeight="1" outlineLevel="1">
-      <c r="A36" s="77"/>
-      <c r="B36" s="92"/>
-      <c r="C36" s="76"/>
-      <c r="D36" s="141"/>
-      <c r="E36" s="142"/>
-      <c r="F36" s="142"/>
-      <c r="G36" s="75"/>
-      <c r="H36" s="82"/>
-      <c r="I36" s="76"/>
-      <c r="J36" s="74"/>
+    <row r="34" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
+      <c r="A34" s="129"/>
+      <c r="B34" s="130"/>
+      <c r="C34" s="130"/>
+      <c r="D34" s="97"/>
+      <c r="E34" s="97"/>
+      <c r="F34" s="97"/>
+      <c r="G34" s="97"/>
+      <c r="H34" s="97"/>
+      <c r="I34" s="97"/>
+      <c r="J34" s="98"/>
+    </row>
+    <row r="35" spans="1:10" s="4" customFormat="1" ht="47.25" customHeight="1" outlineLevel="1">
+      <c r="A35" s="77"/>
+      <c r="B35" s="92"/>
+      <c r="C35" s="76"/>
+      <c r="D35" s="142"/>
+      <c r="E35" s="143"/>
+      <c r="F35" s="143"/>
+      <c r="G35" s="75"/>
+      <c r="H35" s="82"/>
+      <c r="I35" s="76"/>
+      <c r="J35" s="74"/>
+    </row>
+    <row r="36" spans="1:10" ht="12" customHeight="1">
+      <c r="I36"/>
+      <c r="J36"/>
     </row>
     <row r="37" spans="1:10" ht="12" customHeight="1">
       <c r="I37"/>
@@ -8655,8 +8918,8 @@
       <c r="I51"/>
       <c r="J51"/>
     </row>
-    <row r="52" spans="9:10" ht="12" customHeight="1">
-      <c r="I52"/>
+    <row r="52" spans="9:10">
+      <c r="I52" s="19"/>
       <c r="J52"/>
     </row>
     <row r="53" spans="9:10">
@@ -8719,34 +8982,29 @@
       <c r="I67" s="19"/>
       <c r="J67"/>
     </row>
-    <row r="68" spans="9:10">
-      <c r="I68" s="19"/>
-      <c r="J68"/>
-    </row>
   </sheetData>
-  <mergeCells count="43">
-    <mergeCell ref="D18:F18"/>
+  <mergeCells count="42">
+    <mergeCell ref="D31:F31"/>
     <mergeCell ref="D32:F32"/>
     <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D35:F35"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D30:F30"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="D23:F23"/>
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="D25:F25"/>
     <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="D28:F28"/>
     <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
     <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D18:F18"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
     <mergeCell ref="A11:J11"/>
@@ -8893,7 +9151,7 @@
       </c>
       <c r="G8" s="66">
         <f>Samples!D7</f>
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="59" customFormat="1" ht="14.25">
@@ -8945,7 +9203,7 @@
       </c>
       <c r="G10" s="121">
         <f>Samples3!D7</f>
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14.25">
@@ -8968,7 +9226,7 @@
       </c>
       <c r="G11" s="54">
         <f>SUM(G6:G10)</f>
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14.25">
@@ -8989,7 +9247,7 @@
       <c r="D13" s="19"/>
       <c r="E13" s="23">
         <f>(D11+E11)*100/G11</f>
-        <v>35.593220338983052</v>
+        <v>33.87096774193548</v>
       </c>
       <c r="F13" s="19" t="s">
         <v>22</v>
@@ -9005,7 +9263,7 @@
       <c r="D14" s="19"/>
       <c r="E14" s="23">
         <f>D11*100/G11</f>
-        <v>22.033898305084747</v>
+        <v>20.967741935483872</v>
       </c>
       <c r="F14" s="19" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
up tc hoan tien sk
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University_IT\Tam\KiemThuPhanMem\event-manager-javafx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB550F96-B6F7-4BC1-8DCF-2E60EC380933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C9159E-EE17-4B22-BA2A-9B53560D4358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="821" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11790" yWindow="930" windowWidth="10365" windowHeight="10155" tabRatio="821" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="97" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="309">
   <si>
     <t>TC1</t>
   </si>
@@ -1230,20 +1230,49 @@
     <t>Kiểm tra chức năng xử lý lỗi khi hủy sự kiện thành công nhưng hoàn tiền thất bại</t>
   </si>
   <si>
+    <t>Viết TC Kiểm tra chức năng hủy sự kiện thành công và hoàn tiền đầy đủ đối với sự kiện có phí</t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra chức năng xử lý lỗi trong quá trình hủy sự kiện và hoàn tiền</t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra chức năng xử lý lỗi khi hủy sự kiện thành công nhưng hoàn tiền thất bại</t>
+  </si>
+  <si>
+    <t>1: Đăng nhập với tư cách là admin
+2: Truy cập vào trang Quản lý sự kiện
+3: Chọn sự kiện đã hủy
+4: Kiểm tra danh sách người tham gia cần hoàn tiền
+5: Xác nhận hoàn tiền đầy đủ cho tất cả người tham gia
+6: Hệ thống gửi thông báo hoàn tiền thành công và thông báo được gửi đến tất cả người tham gia</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng xử lý lỗi khi hoàn tiền sự kiện</t>
+  </si>
+  <si>
     <t>1: Đăng nhập với tư cách là admin
 2: Giả lập lỗi hoàn tiền(Vd: tài khoản hết tiền, hết hạn hay bị đóng băng..)
 3: Hủy sự kiện theo các quy trình đã nêu 
-4: Hệ thống thông báo lỗi đến admin và ghi nhận lỗi
-5: Hệ thống gửi thông báo đến người tham gia về việc quá trình hoàn tiền bị trì hoãn và đang được xử lý</t>
-  </si>
-  <si>
-    <t>Viết TC Kiểm tra chức năng hủy sự kiện thành công và hoàn tiền đầy đủ đối với sự kiện có phí</t>
-  </si>
-  <si>
-    <t>Viết TC Kiểm tra chức năng xử lý lỗi trong quá trình hủy sự kiện và hoàn tiền</t>
-  </si>
-  <si>
-    <t>Viết TC Kiểm tra chức năng xử lý lỗi khi hủy sự kiện thành công nhưng hoàn tiền thất bại</t>
+4: Hệ thống thông báo lỗi đến admin về việc hủy sự kiện thành công nhưng hoàn tiền thất bại
+5: Hệ thống gửi thông báo đến người tham gia về việc quá trình hoàn tiền bị trì hoãn và đang được xử lý
+6: Sửa lỗi và thử lại quá trình hoàn tiền 
+7: Hệ thống thông báo hoàn tiền thành công đến người tham gia</t>
+  </si>
+  <si>
+    <t>Cập nhật TC Kiểm tra chức năng xử lý lỗi khi hủy sự kiện thành công nhưng hoàn tiền thất bại</t>
+  </si>
+  <si>
+    <t>1: Đăng nhập với tư cách là admin
+2: Truy cập vào trang Quản lý sự kiện
+3: Chọn sự kiện đã hủy
+4: Giả lập lỗi trong quá trình hoàn tiền(tài khoản hết tiền, tài khoản không hợp lệ, lỗi kết nối với cổng thanh toán..)
+5: Xác nhận hoàn tiền trong các tình huống trên
+6: Hệ thống thông báo lỗi khi hoàn tiền và yêu cầu thử lại
+7: Sửa lỗi và thử lại quá trình hoàn tiền 
+7: Hệ thống thông báo hoàn tiền thành công đến người tham gia</t>
+  </si>
+  <si>
+    <t>Kiểm tra quá trình hoàn tiền đầy đủ cho người tham gia sau khi sự kiện bị hủy</t>
   </si>
 </sst>
 </file>
@@ -2295,26 +2324,131 @@
     <xf numFmtId="20" fontId="6" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2322,9 +2456,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2334,118 +2465,16 @@
     <xf numFmtId="0" fontId="15" fillId="5" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4162,10 +4191,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H118"/>
+  <dimension ref="A2:H146"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A102" zoomScale="85" workbookViewId="0">
-      <selection activeCell="D107" sqref="D107"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A116" zoomScale="85" workbookViewId="0">
+      <selection activeCell="B133" sqref="B133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -4232,11 +4261,11 @@
       <c r="B6" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="124" t="s">
+      <c r="C6" s="129" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="124"/>
-      <c r="E6" s="125"/>
+      <c r="D6" s="129"/>
+      <c r="E6" s="130"/>
       <c r="F6" s="108"/>
       <c r="G6" s="25"/>
     </row>
@@ -4245,11 +4274,11 @@
       <c r="B7" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="124" t="s">
+      <c r="C7" s="129" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="124"/>
-      <c r="E7" s="125"/>
+      <c r="D7" s="129"/>
+      <c r="E7" s="130"/>
       <c r="F7" s="108"/>
       <c r="G7" s="25"/>
     </row>
@@ -5923,7 +5952,7 @@
       </c>
       <c r="D107" s="99"/>
       <c r="E107" s="104" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F107" s="110" t="s">
         <v>44</v>
@@ -5940,7 +5969,7 @@
       </c>
       <c r="D108" s="99"/>
       <c r="E108" s="104" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F108" s="110" t="s">
         <v>44</v>
@@ -5957,7 +5986,7 @@
       </c>
       <c r="D109" s="99"/>
       <c r="E109" s="104" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F109" s="110" t="s">
         <v>44</v>
@@ -5974,7 +6003,7 @@
       </c>
       <c r="D110" s="99"/>
       <c r="E110" s="104" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F110" s="110" t="s">
         <v>44</v>
@@ -5982,30 +6011,54 @@
       <c r="G110" s="99"/>
       <c r="H110" s="105"/>
     </row>
-    <row r="111" spans="2:8" s="33" customFormat="1">
-      <c r="B111" s="118"/>
-      <c r="C111" s="119"/>
+    <row r="111" spans="2:8" s="33" customFormat="1" ht="38.25">
+      <c r="B111" s="118">
+        <v>45767</v>
+      </c>
+      <c r="C111" s="119" t="s">
+        <v>40</v>
+      </c>
       <c r="D111" s="99"/>
-      <c r="E111" s="104"/>
-      <c r="F111" s="120"/>
+      <c r="E111" s="104" t="s">
+        <v>306</v>
+      </c>
+      <c r="F111" s="110" t="s">
+        <v>44</v>
+      </c>
       <c r="G111" s="99"/>
       <c r="H111" s="105"/>
     </row>
-    <row r="112" spans="2:8" s="33" customFormat="1">
-      <c r="B112" s="118"/>
-      <c r="C112" s="119"/>
+    <row r="112" spans="2:8" s="33" customFormat="1" ht="25.5">
+      <c r="B112" s="118">
+        <v>45767</v>
+      </c>
+      <c r="C112" s="119" t="s">
+        <v>40</v>
+      </c>
       <c r="D112" s="99"/>
-      <c r="E112" s="104"/>
-      <c r="F112" s="120"/>
+      <c r="E112" s="104" t="s">
+        <v>308</v>
+      </c>
+      <c r="F112" s="110" t="s">
+        <v>44</v>
+      </c>
       <c r="G112" s="99"/>
       <c r="H112" s="105"/>
     </row>
-    <row r="113" spans="2:8" s="33" customFormat="1">
-      <c r="B113" s="118"/>
-      <c r="C113" s="119"/>
+    <row r="113" spans="2:8" s="33" customFormat="1" ht="25.5">
+      <c r="B113" s="118">
+        <v>45767</v>
+      </c>
+      <c r="C113" s="119" t="s">
+        <v>40</v>
+      </c>
       <c r="D113" s="99"/>
-      <c r="E113" s="104"/>
-      <c r="F113" s="120"/>
+      <c r="E113" s="104" t="s">
+        <v>304</v>
+      </c>
+      <c r="F113" s="110" t="s">
+        <v>44</v>
+      </c>
       <c r="G113" s="99"/>
       <c r="H113" s="105"/>
     </row>
@@ -6046,13 +6099,265 @@
       <c r="H117" s="105"/>
     </row>
     <row r="118" spans="2:8" s="33" customFormat="1">
-      <c r="B118" s="107"/>
-      <c r="C118" s="106"/>
-      <c r="D118" s="42"/>
-      <c r="E118" s="103"/>
-      <c r="F118" s="111"/>
-      <c r="G118" s="42"/>
-      <c r="H118" s="43"/>
+      <c r="B118" s="118"/>
+      <c r="C118" s="119"/>
+      <c r="D118" s="99"/>
+      <c r="E118" s="104"/>
+      <c r="F118" s="120"/>
+      <c r="G118" s="99"/>
+      <c r="H118" s="105"/>
+    </row>
+    <row r="119" spans="2:8" s="33" customFormat="1">
+      <c r="B119" s="118"/>
+      <c r="C119" s="119"/>
+      <c r="D119" s="99"/>
+      <c r="E119" s="104"/>
+      <c r="F119" s="120"/>
+      <c r="G119" s="99"/>
+      <c r="H119" s="105"/>
+    </row>
+    <row r="120" spans="2:8" s="33" customFormat="1">
+      <c r="B120" s="118"/>
+      <c r="C120" s="119"/>
+      <c r="D120" s="99"/>
+      <c r="E120" s="104"/>
+      <c r="F120" s="120"/>
+      <c r="G120" s="99"/>
+      <c r="H120" s="105"/>
+    </row>
+    <row r="121" spans="2:8" s="33" customFormat="1">
+      <c r="B121" s="118"/>
+      <c r="C121" s="119"/>
+      <c r="D121" s="99"/>
+      <c r="E121" s="104"/>
+      <c r="F121" s="120"/>
+      <c r="G121" s="99"/>
+      <c r="H121" s="105"/>
+    </row>
+    <row r="122" spans="2:8" s="33" customFormat="1">
+      <c r="B122" s="118"/>
+      <c r="C122" s="119"/>
+      <c r="D122" s="99"/>
+      <c r="E122" s="104"/>
+      <c r="F122" s="120"/>
+      <c r="G122" s="99"/>
+      <c r="H122" s="105"/>
+    </row>
+    <row r="123" spans="2:8" s="33" customFormat="1">
+      <c r="B123" s="118"/>
+      <c r="C123" s="119"/>
+      <c r="D123" s="99"/>
+      <c r="E123" s="104"/>
+      <c r="F123" s="120"/>
+      <c r="G123" s="99"/>
+      <c r="H123" s="105"/>
+    </row>
+    <row r="124" spans="2:8" s="33" customFormat="1">
+      <c r="B124" s="118"/>
+      <c r="C124" s="119"/>
+      <c r="D124" s="99"/>
+      <c r="E124" s="104"/>
+      <c r="F124" s="120"/>
+      <c r="G124" s="99"/>
+      <c r="H124" s="105"/>
+    </row>
+    <row r="125" spans="2:8" s="33" customFormat="1">
+      <c r="B125" s="118"/>
+      <c r="C125" s="119"/>
+      <c r="D125" s="99"/>
+      <c r="E125" s="104"/>
+      <c r="F125" s="120"/>
+      <c r="G125" s="99"/>
+      <c r="H125" s="105"/>
+    </row>
+    <row r="126" spans="2:8" s="33" customFormat="1">
+      <c r="B126" s="118"/>
+      <c r="C126" s="119"/>
+      <c r="D126" s="99"/>
+      <c r="E126" s="104"/>
+      <c r="F126" s="120"/>
+      <c r="G126" s="99"/>
+      <c r="H126" s="105"/>
+    </row>
+    <row r="127" spans="2:8" s="33" customFormat="1">
+      <c r="B127" s="118"/>
+      <c r="C127" s="119"/>
+      <c r="D127" s="99"/>
+      <c r="E127" s="104"/>
+      <c r="F127" s="120"/>
+      <c r="G127" s="99"/>
+      <c r="H127" s="105"/>
+    </row>
+    <row r="128" spans="2:8" s="33" customFormat="1">
+      <c r="B128" s="118"/>
+      <c r="C128" s="119"/>
+      <c r="D128" s="99"/>
+      <c r="E128" s="104"/>
+      <c r="F128" s="120"/>
+      <c r="G128" s="99"/>
+      <c r="H128" s="105"/>
+    </row>
+    <row r="129" spans="2:8" s="33" customFormat="1">
+      <c r="B129" s="118"/>
+      <c r="C129" s="119"/>
+      <c r="D129" s="99"/>
+      <c r="E129" s="104"/>
+      <c r="F129" s="120"/>
+      <c r="G129" s="99"/>
+      <c r="H129" s="105"/>
+    </row>
+    <row r="130" spans="2:8" s="33" customFormat="1">
+      <c r="B130" s="118"/>
+      <c r="C130" s="119"/>
+      <c r="D130" s="99"/>
+      <c r="E130" s="104"/>
+      <c r="F130" s="120"/>
+      <c r="G130" s="99"/>
+      <c r="H130" s="105"/>
+    </row>
+    <row r="131" spans="2:8" s="33" customFormat="1">
+      <c r="B131" s="118"/>
+      <c r="C131" s="119"/>
+      <c r="D131" s="99"/>
+      <c r="E131" s="104"/>
+      <c r="F131" s="120"/>
+      <c r="G131" s="99"/>
+      <c r="H131" s="105"/>
+    </row>
+    <row r="132" spans="2:8" s="33" customFormat="1">
+      <c r="B132" s="118"/>
+      <c r="C132" s="119"/>
+      <c r="D132" s="99"/>
+      <c r="E132" s="104"/>
+      <c r="F132" s="120"/>
+      <c r="G132" s="99"/>
+      <c r="H132" s="105"/>
+    </row>
+    <row r="133" spans="2:8" s="33" customFormat="1">
+      <c r="B133" s="118"/>
+      <c r="C133" s="119"/>
+      <c r="D133" s="99"/>
+      <c r="E133" s="104"/>
+      <c r="F133" s="120"/>
+      <c r="G133" s="99"/>
+      <c r="H133" s="105"/>
+    </row>
+    <row r="134" spans="2:8" s="33" customFormat="1">
+      <c r="B134" s="118"/>
+      <c r="C134" s="119"/>
+      <c r="D134" s="99"/>
+      <c r="E134" s="104"/>
+      <c r="F134" s="120"/>
+      <c r="G134" s="99"/>
+      <c r="H134" s="105"/>
+    </row>
+    <row r="135" spans="2:8" s="33" customFormat="1">
+      <c r="B135" s="118"/>
+      <c r="C135" s="119"/>
+      <c r="D135" s="99"/>
+      <c r="E135" s="104"/>
+      <c r="F135" s="120"/>
+      <c r="G135" s="99"/>
+      <c r="H135" s="105"/>
+    </row>
+    <row r="136" spans="2:8" s="33" customFormat="1">
+      <c r="B136" s="118"/>
+      <c r="C136" s="119"/>
+      <c r="D136" s="99"/>
+      <c r="E136" s="104"/>
+      <c r="F136" s="120"/>
+      <c r="G136" s="99"/>
+      <c r="H136" s="105"/>
+    </row>
+    <row r="137" spans="2:8" s="33" customFormat="1">
+      <c r="B137" s="118"/>
+      <c r="C137" s="119"/>
+      <c r="D137" s="99"/>
+      <c r="E137" s="104"/>
+      <c r="F137" s="120"/>
+      <c r="G137" s="99"/>
+      <c r="H137" s="105"/>
+    </row>
+    <row r="138" spans="2:8" s="33" customFormat="1">
+      <c r="B138" s="118"/>
+      <c r="C138" s="119"/>
+      <c r="D138" s="99"/>
+      <c r="E138" s="104"/>
+      <c r="F138" s="120"/>
+      <c r="G138" s="99"/>
+      <c r="H138" s="105"/>
+    </row>
+    <row r="139" spans="2:8" s="33" customFormat="1">
+      <c r="B139" s="118"/>
+      <c r="C139" s="119"/>
+      <c r="D139" s="99"/>
+      <c r="E139" s="104"/>
+      <c r="F139" s="120"/>
+      <c r="G139" s="99"/>
+      <c r="H139" s="105"/>
+    </row>
+    <row r="140" spans="2:8" s="33" customFormat="1">
+      <c r="B140" s="118"/>
+      <c r="C140" s="119"/>
+      <c r="D140" s="99"/>
+      <c r="E140" s="104"/>
+      <c r="F140" s="120"/>
+      <c r="G140" s="99"/>
+      <c r="H140" s="105"/>
+    </row>
+    <row r="141" spans="2:8" s="33" customFormat="1">
+      <c r="B141" s="118"/>
+      <c r="C141" s="119"/>
+      <c r="D141" s="99"/>
+      <c r="E141" s="104"/>
+      <c r="F141" s="120"/>
+      <c r="G141" s="99"/>
+      <c r="H141" s="105"/>
+    </row>
+    <row r="142" spans="2:8" s="33" customFormat="1">
+      <c r="B142" s="118"/>
+      <c r="C142" s="119"/>
+      <c r="D142" s="99"/>
+      <c r="E142" s="104"/>
+      <c r="F142" s="120"/>
+      <c r="G142" s="99"/>
+      <c r="H142" s="105"/>
+    </row>
+    <row r="143" spans="2:8" s="33" customFormat="1">
+      <c r="B143" s="118"/>
+      <c r="C143" s="119"/>
+      <c r="D143" s="99"/>
+      <c r="E143" s="104"/>
+      <c r="F143" s="120"/>
+      <c r="G143" s="99"/>
+      <c r="H143" s="105"/>
+    </row>
+    <row r="144" spans="2:8" s="33" customFormat="1">
+      <c r="B144" s="118"/>
+      <c r="C144" s="119"/>
+      <c r="D144" s="99"/>
+      <c r="E144" s="104"/>
+      <c r="F144" s="120"/>
+      <c r="G144" s="99"/>
+      <c r="H144" s="105"/>
+    </row>
+    <row r="145" spans="2:8" s="33" customFormat="1">
+      <c r="B145" s="118"/>
+      <c r="C145" s="119"/>
+      <c r="D145" s="99"/>
+      <c r="E145" s="104"/>
+      <c r="F145" s="120"/>
+      <c r="G145" s="99"/>
+      <c r="H145" s="105"/>
+    </row>
+    <row r="146" spans="2:8" s="33" customFormat="1">
+      <c r="B146" s="107"/>
+      <c r="C146" s="106"/>
+      <c r="D146" s="42"/>
+      <c r="E146" s="103"/>
+      <c r="F146" s="111"/>
+      <c r="G146" s="42"/>
+      <c r="H146" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -6069,7 +6374,7 @@
     <oddFooter>&amp;L&amp;"Tahoma,Regular"&amp;8 02ae-BM/PM/HDCV/FSOFT v1/0&amp;R&amp;"Tahoma,Regular"&amp;10&amp;P/&amp;N</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="C12:C28 C41 C34:C40 C42:C47 C48:C49 C51:C53 C50 C54:C57 C58:C60 C29:C33 C61:C83 C84:C92 C93:C94 C95:C102 C103:C105 C106:C110" numberStoredAsText="1"/>
+    <ignoredError sqref="C12:C28 C41 C34:C40 C42:C47 C48:C49 C51:C53 C50 C54:C57 C58:C60 C29:C33 C61:C83 C84:C92 C93:C94 C95:C102 C103:C105 C106:C110 C111:C113" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -6081,8 +6386,8 @@
   </sheetPr>
   <dimension ref="A1:K99"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A61" zoomScale="69" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59:B62"/>
+    <sheetView showGridLines="0" topLeftCell="A54" zoomScale="69" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56:B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" outlineLevelRow="1"/>
@@ -6101,9 +6406,9 @@
       <c r="A1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="147"/>
-      <c r="C1" s="147"/>
-      <c r="D1" s="147"/>
+      <c r="B1" s="144"/>
+      <c r="C1" s="144"/>
+      <c r="D1" s="144"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -6114,9 +6419,9 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="148"/>
-      <c r="C2" s="148"/>
-      <c r="D2" s="148"/>
+      <c r="B2" s="145"/>
+      <c r="C2" s="145"/>
+      <c r="D2" s="145"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -6129,17 +6434,17 @@
       <c r="A3" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="124" t="s">
+      <c r="B3" s="129" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="124"/>
-      <c r="D3" s="125"/>
+      <c r="C3" s="129"/>
+      <c r="D3" s="130"/>
       <c r="E3" s="60"/>
       <c r="F3" s="60"/>
       <c r="G3" s="60"/>
-      <c r="H3" s="155"/>
-      <c r="I3" s="155"/>
-      <c r="J3" s="155"/>
+      <c r="H3" s="154"/>
+      <c r="I3" s="154"/>
+      <c r="J3" s="154"/>
       <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="12.75">
@@ -6154,26 +6459,26 @@
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
       <c r="G4" s="60"/>
-      <c r="H4" s="155"/>
-      <c r="I4" s="155"/>
-      <c r="J4" s="155"/>
+      <c r="H4" s="154"/>
+      <c r="I4" s="154"/>
+      <c r="J4" s="154"/>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" s="70" customFormat="1" ht="25.5">
       <c r="A5" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="150" t="s">
+      <c r="B5" s="147" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="151"/>
-      <c r="D5" s="152"/>
+      <c r="C5" s="148"/>
+      <c r="D5" s="149"/>
       <c r="E5" s="68"/>
       <c r="F5" s="68"/>
       <c r="G5" s="68"/>
-      <c r="H5" s="154"/>
-      <c r="I5" s="154"/>
-      <c r="J5" s="154"/>
+      <c r="H5" s="153"/>
+      <c r="I5" s="153"/>
+      <c r="J5" s="153"/>
       <c r="K5" s="69"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
@@ -6194,9 +6499,9 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="155"/>
-      <c r="I6" s="155"/>
-      <c r="J6" s="155"/>
+      <c r="H6" s="154"/>
+      <c r="I6" s="154"/>
+      <c r="J6" s="154"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -6212,21 +6517,21 @@
       </c>
       <c r="D7" s="58">
         <f>COUNTA(A12:A62) -9</f>
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
       <c r="G7" s="61"/>
-      <c r="H7" s="155"/>
-      <c r="I7" s="155"/>
-      <c r="J7" s="155"/>
+      <c r="H7" s="154"/>
+      <c r="I7" s="154"/>
+      <c r="J7" s="154"/>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="149"/>
-      <c r="B8" s="149"/>
-      <c r="C8" s="149"/>
-      <c r="D8" s="149"/>
+      <c r="A8" s="146"/>
+      <c r="B8" s="146"/>
+      <c r="C8" s="146"/>
+      <c r="D8" s="146"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -6236,70 +6541,70 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" s="72" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="133" t="s">
+      <c r="A9" s="163" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="162" t="s">
+      <c r="B9" s="164" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="133" t="s">
+      <c r="C9" s="163" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="134" t="s">
+      <c r="D9" s="168" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="135"/>
-      <c r="F9" s="135"/>
-      <c r="G9" s="136"/>
+      <c r="E9" s="169"/>
+      <c r="F9" s="169"/>
+      <c r="G9" s="170"/>
       <c r="H9" s="159" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="128" t="s">
+      <c r="I9" s="155" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="128" t="s">
+      <c r="J9" s="155" t="s">
         <v>32</v>
       </c>
       <c r="K9" s="71"/>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="128"/>
-      <c r="B10" s="163"/>
-      <c r="C10" s="128"/>
-      <c r="D10" s="137"/>
-      <c r="E10" s="138"/>
-      <c r="F10" s="138"/>
-      <c r="G10" s="139"/>
-      <c r="H10" s="137"/>
-      <c r="I10" s="128"/>
-      <c r="J10" s="128"/>
+      <c r="A10" s="155"/>
+      <c r="B10" s="165"/>
+      <c r="C10" s="155"/>
+      <c r="D10" s="160"/>
+      <c r="E10" s="171"/>
+      <c r="F10" s="171"/>
+      <c r="G10" s="172"/>
+      <c r="H10" s="160"/>
+      <c r="I10" s="155"/>
+      <c r="J10" s="155"/>
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" s="73" customFormat="1" ht="15">
-      <c r="A11" s="160"/>
-      <c r="B11" s="160"/>
-      <c r="C11" s="160"/>
-      <c r="D11" s="160"/>
-      <c r="E11" s="160"/>
-      <c r="F11" s="160"/>
-      <c r="G11" s="160"/>
-      <c r="H11" s="160"/>
-      <c r="I11" s="160"/>
-      <c r="J11" s="161"/>
+      <c r="A11" s="161"/>
+      <c r="B11" s="161"/>
+      <c r="C11" s="161"/>
+      <c r="D11" s="161"/>
+      <c r="E11" s="161"/>
+      <c r="F11" s="161"/>
+      <c r="G11" s="161"/>
+      <c r="H11" s="161"/>
+      <c r="I11" s="161"/>
+      <c r="J11" s="162"/>
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A12" s="140" t="s">
+      <c r="A12" s="150" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="141"/>
-      <c r="C12" s="141"/>
-      <c r="D12" s="141"/>
-      <c r="E12" s="141"/>
-      <c r="F12" s="141"/>
-      <c r="G12" s="141"/>
-      <c r="H12" s="141"/>
-      <c r="I12" s="141"/>
-      <c r="J12" s="153"/>
+      <c r="B12" s="151"/>
+      <c r="C12" s="151"/>
+      <c r="D12" s="151"/>
+      <c r="E12" s="151"/>
+      <c r="F12" s="151"/>
+      <c r="G12" s="151"/>
+      <c r="H12" s="151"/>
+      <c r="I12" s="151"/>
+      <c r="J12" s="152"/>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" ht="350.1" customHeight="1" outlineLevel="1">
       <c r="A13" s="77" t="s">
@@ -6311,9 +6616,9 @@
       <c r="C13" s="76" t="s">
         <v>200</v>
       </c>
-      <c r="D13" s="126"/>
-      <c r="E13" s="127"/>
-      <c r="F13" s="127"/>
+      <c r="D13" s="138"/>
+      <c r="E13" s="139"/>
+      <c r="F13" s="139"/>
       <c r="G13" s="75"/>
       <c r="H13" s="116">
         <v>45755</v>
@@ -6333,9 +6638,9 @@
       <c r="C14" s="76" t="s">
         <v>199</v>
       </c>
-      <c r="D14" s="126"/>
-      <c r="E14" s="127"/>
-      <c r="F14" s="127"/>
+      <c r="D14" s="138"/>
+      <c r="E14" s="139"/>
+      <c r="F14" s="139"/>
       <c r="G14" s="75"/>
       <c r="H14" s="116">
         <v>45755</v>
@@ -6355,9 +6660,9 @@
       <c r="C15" s="76" t="s">
         <v>198</v>
       </c>
-      <c r="D15" s="126"/>
-      <c r="E15" s="127"/>
-      <c r="F15" s="127"/>
+      <c r="D15" s="138"/>
+      <c r="E15" s="139"/>
+      <c r="F15" s="139"/>
       <c r="G15" s="75"/>
       <c r="H15" s="116">
         <v>45755</v>
@@ -6379,9 +6684,9 @@
       <c r="C16" s="76" t="s">
         <v>197</v>
       </c>
-      <c r="D16" s="126"/>
-      <c r="E16" s="127"/>
-      <c r="F16" s="127"/>
+      <c r="D16" s="138"/>
+      <c r="E16" s="139"/>
+      <c r="F16" s="139"/>
       <c r="G16" s="75"/>
       <c r="H16" s="116">
         <v>45755</v>
@@ -6401,9 +6706,9 @@
       <c r="C17" s="76" t="s">
         <v>196</v>
       </c>
-      <c r="D17" s="126"/>
-      <c r="E17" s="127"/>
-      <c r="F17" s="127"/>
+      <c r="D17" s="138"/>
+      <c r="E17" s="139"/>
+      <c r="F17" s="139"/>
       <c r="G17" s="75"/>
       <c r="H17" s="116">
         <v>45755</v>
@@ -6423,9 +6728,9 @@
       <c r="C18" s="86" t="s">
         <v>195</v>
       </c>
-      <c r="D18" s="126"/>
-      <c r="E18" s="127"/>
-      <c r="F18" s="127"/>
+      <c r="D18" s="138"/>
+      <c r="E18" s="139"/>
+      <c r="F18" s="139"/>
       <c r="G18" s="75"/>
       <c r="H18" s="116">
         <v>45755</v>
@@ -6447,9 +6752,9 @@
       <c r="C19" s="86" t="s">
         <v>194</v>
       </c>
-      <c r="D19" s="126"/>
-      <c r="E19" s="127"/>
-      <c r="F19" s="127"/>
+      <c r="D19" s="138"/>
+      <c r="E19" s="139"/>
+      <c r="F19" s="139"/>
       <c r="G19" s="75"/>
       <c r="H19" s="116">
         <v>45755</v>
@@ -6471,9 +6776,9 @@
       <c r="C20" s="76" t="s">
         <v>192</v>
       </c>
-      <c r="D20" s="126"/>
-      <c r="E20" s="127"/>
-      <c r="F20" s="127"/>
+      <c r="D20" s="138"/>
+      <c r="E20" s="139"/>
+      <c r="F20" s="139"/>
       <c r="G20" s="75"/>
       <c r="H20" s="116">
         <v>45755</v>
@@ -6495,9 +6800,9 @@
       <c r="C21" s="76" t="s">
         <v>191</v>
       </c>
-      <c r="D21" s="126"/>
-      <c r="E21" s="127"/>
-      <c r="F21" s="127"/>
+      <c r="D21" s="138"/>
+      <c r="E21" s="139"/>
+      <c r="F21" s="139"/>
       <c r="G21" s="75"/>
       <c r="H21" s="116">
         <v>45755</v>
@@ -6519,9 +6824,9 @@
       <c r="C22" s="86" t="s">
         <v>193</v>
       </c>
-      <c r="D22" s="126"/>
-      <c r="E22" s="127"/>
-      <c r="F22" s="127"/>
+      <c r="D22" s="138"/>
+      <c r="E22" s="139"/>
+      <c r="F22" s="139"/>
       <c r="G22" s="75"/>
       <c r="H22" s="116">
         <v>45755</v>
@@ -6534,11 +6839,11 @@
       </c>
     </row>
     <row r="23" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A23" s="140" t="s">
+      <c r="A23" s="150" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="141"/>
-      <c r="C23" s="141"/>
+      <c r="B23" s="151"/>
+      <c r="C23" s="151"/>
       <c r="D23" s="87"/>
       <c r="E23" s="87"/>
       <c r="F23" s="87"/>
@@ -6557,9 +6862,9 @@
       <c r="C24" s="86" t="s">
         <v>228</v>
       </c>
-      <c r="D24" s="131"/>
-      <c r="E24" s="132"/>
-      <c r="F24" s="132"/>
+      <c r="D24" s="166"/>
+      <c r="E24" s="167"/>
+      <c r="F24" s="167"/>
       <c r="G24" s="94"/>
       <c r="H24" s="115">
         <v>45756</v>
@@ -6579,9 +6884,9 @@
       <c r="C25" s="86" t="s">
         <v>227</v>
       </c>
-      <c r="D25" s="131"/>
-      <c r="E25" s="132"/>
-      <c r="F25" s="132"/>
+      <c r="D25" s="166"/>
+      <c r="E25" s="167"/>
+      <c r="F25" s="167"/>
       <c r="G25" s="94"/>
       <c r="H25" s="115">
         <v>45755</v>
@@ -6603,9 +6908,9 @@
       <c r="C26" s="86" t="s">
         <v>232</v>
       </c>
-      <c r="D26" s="142"/>
-      <c r="E26" s="143"/>
-      <c r="F26" s="143"/>
+      <c r="D26" s="131"/>
+      <c r="E26" s="132"/>
+      <c r="F26" s="132"/>
       <c r="G26" s="94"/>
       <c r="H26" s="115">
         <v>45756</v>
@@ -6625,9 +6930,9 @@
       <c r="C27" s="86" t="s">
         <v>233</v>
       </c>
-      <c r="D27" s="144"/>
-      <c r="E27" s="145"/>
-      <c r="F27" s="146"/>
+      <c r="D27" s="135"/>
+      <c r="E27" s="136"/>
+      <c r="F27" s="137"/>
       <c r="G27" s="94"/>
       <c r="H27" s="115">
         <v>45755</v>
@@ -6647,9 +6952,9 @@
       <c r="C28" s="86" t="s">
         <v>237</v>
       </c>
-      <c r="D28" s="144"/>
-      <c r="E28" s="145"/>
-      <c r="F28" s="146"/>
+      <c r="D28" s="135"/>
+      <c r="E28" s="136"/>
+      <c r="F28" s="137"/>
       <c r="G28" s="94"/>
       <c r="H28" s="115">
         <v>45756</v>
@@ -6671,9 +6976,9 @@
       <c r="C29" s="86" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="144"/>
-      <c r="E29" s="145"/>
-      <c r="F29" s="146"/>
+      <c r="D29" s="135"/>
+      <c r="E29" s="136"/>
+      <c r="F29" s="137"/>
       <c r="G29" s="94"/>
       <c r="H29" s="115">
         <v>45756</v>
@@ -6695,9 +7000,9 @@
       <c r="C30" s="86" t="s">
         <v>234</v>
       </c>
-      <c r="D30" s="144"/>
-      <c r="E30" s="145"/>
-      <c r="F30" s="146"/>
+      <c r="D30" s="135"/>
+      <c r="E30" s="136"/>
+      <c r="F30" s="137"/>
       <c r="G30" s="94"/>
       <c r="H30" s="115">
         <v>45755</v>
@@ -6717,9 +7022,9 @@
       <c r="C31" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="144"/>
-      <c r="E31" s="145"/>
-      <c r="F31" s="146"/>
+      <c r="D31" s="135"/>
+      <c r="E31" s="136"/>
+      <c r="F31" s="137"/>
       <c r="G31" s="94"/>
       <c r="H31" s="115">
         <v>45756</v>
@@ -6741,9 +7046,9 @@
       <c r="C32" s="86" t="s">
         <v>70</v>
       </c>
-      <c r="D32" s="144"/>
-      <c r="E32" s="145"/>
-      <c r="F32" s="146"/>
+      <c r="D32" s="135"/>
+      <c r="E32" s="136"/>
+      <c r="F32" s="137"/>
       <c r="G32" s="94"/>
       <c r="H32" s="115">
         <v>45756</v>
@@ -6765,9 +7070,9 @@
       <c r="C33" s="86" t="s">
         <v>241</v>
       </c>
-      <c r="D33" s="126"/>
-      <c r="E33" s="127"/>
-      <c r="F33" s="164"/>
+      <c r="D33" s="138"/>
+      <c r="E33" s="139"/>
+      <c r="F33" s="140"/>
       <c r="G33" s="94"/>
       <c r="H33" s="115">
         <v>45755</v>
@@ -6787,9 +7092,9 @@
       <c r="C34" s="86" t="s">
         <v>201</v>
       </c>
-      <c r="D34" s="165"/>
-      <c r="E34" s="166"/>
-      <c r="F34" s="167"/>
+      <c r="D34" s="141"/>
+      <c r="E34" s="142"/>
+      <c r="F34" s="143"/>
       <c r="G34" s="94"/>
       <c r="H34" s="115">
         <v>45755</v>
@@ -6800,11 +7105,11 @@
       <c r="J34" s="96"/>
     </row>
     <row r="35" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A35" s="140" t="s">
+      <c r="A35" s="150" t="s">
         <v>71</v>
       </c>
-      <c r="B35" s="141"/>
-      <c r="C35" s="141"/>
+      <c r="B35" s="151"/>
+      <c r="C35" s="151"/>
       <c r="D35" s="87"/>
       <c r="E35" s="87"/>
       <c r="F35" s="87"/>
@@ -6823,20 +7128,20 @@
       <c r="C36" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="D36" s="142"/>
-      <c r="E36" s="143"/>
-      <c r="F36" s="143"/>
+      <c r="D36" s="131"/>
+      <c r="E36" s="132"/>
+      <c r="F36" s="132"/>
       <c r="G36" s="75"/>
       <c r="H36" s="82"/>
       <c r="I36" s="76"/>
       <c r="J36" s="74"/>
     </row>
     <row r="37" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A37" s="129" t="s">
+      <c r="A37" s="133" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="130"/>
-      <c r="C37" s="130"/>
+      <c r="B37" s="134"/>
+      <c r="C37" s="134"/>
       <c r="D37" s="97"/>
       <c r="E37" s="97"/>
       <c r="F37" s="97"/>
@@ -6855,9 +7160,9 @@
       <c r="C38" s="76" t="s">
         <v>113</v>
       </c>
-      <c r="D38" s="142"/>
-      <c r="E38" s="143"/>
-      <c r="F38" s="143"/>
+      <c r="D38" s="131"/>
+      <c r="E38" s="132"/>
+      <c r="F38" s="132"/>
       <c r="G38" s="75"/>
       <c r="H38" s="82"/>
       <c r="I38" s="76"/>
@@ -6873,9 +7178,9 @@
       <c r="C39" s="76" t="s">
         <v>115</v>
       </c>
-      <c r="D39" s="142"/>
-      <c r="E39" s="143"/>
-      <c r="F39" s="143"/>
+      <c r="D39" s="131"/>
+      <c r="E39" s="132"/>
+      <c r="F39" s="132"/>
       <c r="G39" s="75"/>
       <c r="H39" s="82"/>
       <c r="I39" s="76"/>
@@ -6891,9 +7196,9 @@
       <c r="C40" s="76" t="s">
         <v>114</v>
       </c>
-      <c r="D40" s="142"/>
-      <c r="E40" s="143"/>
-      <c r="F40" s="143"/>
+      <c r="D40" s="131"/>
+      <c r="E40" s="132"/>
+      <c r="F40" s="132"/>
       <c r="G40" s="75"/>
       <c r="H40" s="82"/>
       <c r="I40" s="76"/>
@@ -6909,9 +7214,9 @@
       <c r="C41" s="76" t="s">
         <v>117</v>
       </c>
-      <c r="D41" s="142"/>
-      <c r="E41" s="143"/>
-      <c r="F41" s="143"/>
+      <c r="D41" s="131"/>
+      <c r="E41" s="132"/>
+      <c r="F41" s="132"/>
       <c r="G41" s="75"/>
       <c r="H41" s="82"/>
       <c r="I41" s="76"/>
@@ -6927,20 +7232,20 @@
       <c r="C42" s="76" t="s">
         <v>119</v>
       </c>
-      <c r="D42" s="142"/>
-      <c r="E42" s="143"/>
-      <c r="F42" s="143"/>
+      <c r="D42" s="131"/>
+      <c r="E42" s="132"/>
+      <c r="F42" s="132"/>
       <c r="G42" s="75"/>
       <c r="H42" s="82"/>
       <c r="I42" s="76"/>
       <c r="J42" s="74"/>
     </row>
     <row r="43" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A43" s="129" t="s">
+      <c r="A43" s="133" t="s">
         <v>88</v>
       </c>
-      <c r="B43" s="130"/>
-      <c r="C43" s="130"/>
+      <c r="B43" s="134"/>
+      <c r="C43" s="134"/>
       <c r="D43" s="97"/>
       <c r="E43" s="97"/>
       <c r="F43" s="97"/>
@@ -6959,9 +7264,9 @@
       <c r="C44" s="76" t="s">
         <v>95</v>
       </c>
-      <c r="D44" s="142"/>
-      <c r="E44" s="143"/>
-      <c r="F44" s="143"/>
+      <c r="D44" s="131"/>
+      <c r="E44" s="132"/>
+      <c r="F44" s="132"/>
       <c r="G44" s="75"/>
       <c r="H44" s="82"/>
       <c r="I44" s="76"/>
@@ -6977,9 +7282,9 @@
       <c r="C45" s="76" t="s">
         <v>96</v>
       </c>
-      <c r="D45" s="142"/>
-      <c r="E45" s="143"/>
-      <c r="F45" s="143"/>
+      <c r="D45" s="131"/>
+      <c r="E45" s="132"/>
+      <c r="F45" s="132"/>
       <c r="G45" s="75"/>
       <c r="H45" s="82"/>
       <c r="I45" s="76"/>
@@ -6995,9 +7300,9 @@
       <c r="C46" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="D46" s="142"/>
-      <c r="E46" s="143"/>
-      <c r="F46" s="143"/>
+      <c r="D46" s="131"/>
+      <c r="E46" s="132"/>
+      <c r="F46" s="132"/>
       <c r="G46" s="75"/>
       <c r="H46" s="82"/>
       <c r="I46" s="76"/>
@@ -7013,9 +7318,9 @@
       <c r="C47" s="76" t="s">
         <v>98</v>
       </c>
-      <c r="D47" s="142"/>
-      <c r="E47" s="143"/>
-      <c r="F47" s="143"/>
+      <c r="D47" s="131"/>
+      <c r="E47" s="132"/>
+      <c r="F47" s="132"/>
       <c r="G47" s="75"/>
       <c r="H47" s="82"/>
       <c r="I47" s="76"/>
@@ -7031,9 +7336,9 @@
       <c r="C48" s="76" t="s">
         <v>100</v>
       </c>
-      <c r="D48" s="142"/>
-      <c r="E48" s="143"/>
-      <c r="F48" s="143"/>
+      <c r="D48" s="131"/>
+      <c r="E48" s="132"/>
+      <c r="F48" s="132"/>
       <c r="G48" s="75"/>
       <c r="H48" s="82"/>
       <c r="I48" s="76"/>
@@ -7049,20 +7354,20 @@
       <c r="C49" s="76" t="s">
         <v>92</v>
       </c>
-      <c r="D49" s="142"/>
-      <c r="E49" s="143"/>
-      <c r="F49" s="143"/>
+      <c r="D49" s="131"/>
+      <c r="E49" s="132"/>
+      <c r="F49" s="132"/>
       <c r="G49" s="75"/>
       <c r="H49" s="82"/>
       <c r="I49" s="76"/>
       <c r="J49" s="74"/>
     </row>
     <row r="50" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A50" s="129" t="s">
+      <c r="A50" s="133" t="s">
         <v>101</v>
       </c>
-      <c r="B50" s="130"/>
-      <c r="C50" s="130"/>
+      <c r="B50" s="134"/>
+      <c r="C50" s="134"/>
       <c r="D50" s="97"/>
       <c r="E50" s="97"/>
       <c r="F50" s="97"/>
@@ -7081,20 +7386,20 @@
       <c r="C51" s="76" t="s">
         <v>102</v>
       </c>
-      <c r="D51" s="142"/>
-      <c r="E51" s="143"/>
-      <c r="F51" s="143"/>
+      <c r="D51" s="131"/>
+      <c r="E51" s="132"/>
+      <c r="F51" s="132"/>
       <c r="G51" s="75"/>
       <c r="H51" s="82"/>
       <c r="I51" s="76"/>
       <c r="J51" s="74"/>
     </row>
     <row r="52" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A52" s="129" t="s">
+      <c r="A52" s="133" t="s">
         <v>265</v>
       </c>
-      <c r="B52" s="130"/>
-      <c r="C52" s="130"/>
+      <c r="B52" s="134"/>
+      <c r="C52" s="134"/>
       <c r="D52" s="97"/>
       <c r="E52" s="97"/>
       <c r="F52" s="97"/>
@@ -7113,9 +7418,9 @@
       <c r="C53" s="76" t="s">
         <v>264</v>
       </c>
-      <c r="D53" s="142"/>
-      <c r="E53" s="143"/>
-      <c r="F53" s="143"/>
+      <c r="D53" s="131"/>
+      <c r="E53" s="132"/>
+      <c r="F53" s="132"/>
       <c r="G53" s="75"/>
       <c r="H53" s="82"/>
       <c r="I53" s="76"/>
@@ -7131,20 +7436,20 @@
       <c r="C54" s="76" t="s">
         <v>269</v>
       </c>
-      <c r="D54" s="142"/>
-      <c r="E54" s="143"/>
-      <c r="F54" s="143"/>
+      <c r="D54" s="131"/>
+      <c r="E54" s="132"/>
+      <c r="F54" s="132"/>
       <c r="G54" s="75"/>
       <c r="H54" s="82"/>
       <c r="I54" s="76"/>
       <c r="J54" s="74"/>
     </row>
     <row r="55" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A55" s="129" t="s">
+      <c r="A55" s="133" t="s">
         <v>292</v>
       </c>
-      <c r="B55" s="130"/>
-      <c r="C55" s="130"/>
+      <c r="B55" s="134"/>
+      <c r="C55" s="134"/>
       <c r="D55" s="97"/>
       <c r="E55" s="97"/>
       <c r="F55" s="97"/>
@@ -7153,36 +7458,48 @@
       <c r="I55" s="97"/>
       <c r="J55" s="98"/>
     </row>
-    <row r="56" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
-      <c r="A56" s="77"/>
-      <c r="B56" s="92"/>
-      <c r="C56" s="76"/>
-      <c r="D56" s="142"/>
-      <c r="E56" s="143"/>
-      <c r="F56" s="143"/>
+    <row r="56" spans="1:10" s="4" customFormat="1" ht="98.25" customHeight="1" outlineLevel="1">
+      <c r="A56" s="77" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" s="92" t="s">
+        <v>308</v>
+      </c>
+      <c r="C56" s="76" t="s">
+        <v>303</v>
+      </c>
+      <c r="D56" s="131"/>
+      <c r="E56" s="132"/>
+      <c r="F56" s="132"/>
       <c r="G56" s="75"/>
       <c r="H56" s="82"/>
       <c r="I56" s="76"/>
       <c r="J56" s="74"/>
     </row>
-    <row r="57" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
-      <c r="A57" s="77"/>
-      <c r="B57" s="92"/>
-      <c r="C57" s="76"/>
-      <c r="D57" s="142"/>
-      <c r="E57" s="143"/>
-      <c r="F57" s="143"/>
+    <row r="57" spans="1:10" s="4" customFormat="1" ht="160.5" customHeight="1" outlineLevel="1">
+      <c r="A57" s="77" t="s">
+        <v>1</v>
+      </c>
+      <c r="B57" s="92" t="s">
+        <v>304</v>
+      </c>
+      <c r="C57" s="76" t="s">
+        <v>307</v>
+      </c>
+      <c r="D57" s="131"/>
+      <c r="E57" s="132"/>
+      <c r="F57" s="132"/>
       <c r="G57" s="75"/>
       <c r="H57" s="82"/>
       <c r="I57" s="76"/>
       <c r="J57" s="74"/>
     </row>
     <row r="58" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A58" s="129" t="s">
+      <c r="A58" s="133" t="s">
         <v>293</v>
       </c>
-      <c r="B58" s="130"/>
-      <c r="C58" s="130"/>
+      <c r="B58" s="134"/>
+      <c r="C58" s="134"/>
       <c r="D58" s="97"/>
       <c r="E58" s="97"/>
       <c r="F58" s="97"/>
@@ -7201,9 +7518,9 @@
       <c r="C59" s="76" t="s">
         <v>295</v>
       </c>
-      <c r="D59" s="142"/>
-      <c r="E59" s="143"/>
-      <c r="F59" s="143"/>
+      <c r="D59" s="131"/>
+      <c r="E59" s="132"/>
+      <c r="F59" s="132"/>
       <c r="G59" s="75"/>
       <c r="H59" s="82"/>
       <c r="I59" s="76"/>
@@ -7219,9 +7536,9 @@
       <c r="C60" s="76" t="s">
         <v>296</v>
       </c>
-      <c r="D60" s="142"/>
-      <c r="E60" s="143"/>
-      <c r="F60" s="143"/>
+      <c r="D60" s="131"/>
+      <c r="E60" s="132"/>
+      <c r="F60" s="132"/>
       <c r="G60" s="75"/>
       <c r="H60" s="82"/>
       <c r="I60" s="76"/>
@@ -7237,15 +7554,15 @@
       <c r="C61" s="76" t="s">
         <v>298</v>
       </c>
-      <c r="D61" s="142"/>
-      <c r="E61" s="143"/>
-      <c r="F61" s="143"/>
+      <c r="D61" s="131"/>
+      <c r="E61" s="132"/>
+      <c r="F61" s="132"/>
       <c r="G61" s="75"/>
       <c r="H61" s="82"/>
       <c r="I61" s="76"/>
       <c r="J61" s="74"/>
     </row>
-    <row r="62" spans="1:10" s="4" customFormat="1" ht="101.25" customHeight="1" outlineLevel="1">
+    <row r="62" spans="1:10" s="4" customFormat="1" ht="146.25" customHeight="1" outlineLevel="1">
       <c r="A62" s="77" t="s">
         <v>49</v>
       </c>
@@ -7253,20 +7570,20 @@
         <v>299</v>
       </c>
       <c r="C62" s="76" t="s">
-        <v>300</v>
-      </c>
-      <c r="D62" s="142"/>
-      <c r="E62" s="143"/>
-      <c r="F62" s="143"/>
+        <v>305</v>
+      </c>
+      <c r="D62" s="131"/>
+      <c r="E62" s="132"/>
+      <c r="F62" s="132"/>
       <c r="G62" s="75"/>
       <c r="H62" s="82"/>
       <c r="I62" s="76"/>
       <c r="J62" s="74"/>
     </row>
     <row r="63" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A63" s="129"/>
-      <c r="B63" s="130"/>
-      <c r="C63" s="130"/>
+      <c r="A63" s="133"/>
+      <c r="B63" s="134"/>
+      <c r="C63" s="134"/>
       <c r="D63" s="97"/>
       <c r="E63" s="97"/>
       <c r="F63" s="97"/>
@@ -7279,18 +7596,18 @@
       <c r="A64" s="77"/>
       <c r="B64" s="92"/>
       <c r="C64" s="76"/>
-      <c r="D64" s="142"/>
-      <c r="E64" s="143"/>
-      <c r="F64" s="143"/>
+      <c r="D64" s="131"/>
+      <c r="E64" s="132"/>
+      <c r="F64" s="132"/>
       <c r="G64" s="75"/>
       <c r="H64" s="82"/>
       <c r="I64" s="76"/>
       <c r="J64" s="74"/>
     </row>
     <row r="65" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A65" s="129"/>
-      <c r="B65" s="130"/>
-      <c r="C65" s="130"/>
+      <c r="A65" s="133"/>
+      <c r="B65" s="134"/>
+      <c r="C65" s="134"/>
       <c r="D65" s="97"/>
       <c r="E65" s="97"/>
       <c r="F65" s="97"/>
@@ -7303,25 +7620,25 @@
       <c r="A66" s="77"/>
       <c r="B66" s="92"/>
       <c r="C66" s="76"/>
-      <c r="D66" s="142"/>
-      <c r="E66" s="143"/>
-      <c r="F66" s="143"/>
+      <c r="D66" s="131"/>
+      <c r="E66" s="132"/>
+      <c r="F66" s="132"/>
       <c r="G66" s="75"/>
       <c r="H66" s="82"/>
       <c r="I66" s="76"/>
       <c r="J66" s="74"/>
     </row>
     <row r="67" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
-      <c r="A67" s="170"/>
-      <c r="B67" s="171"/>
-      <c r="C67" s="172"/>
-      <c r="D67" s="173"/>
-      <c r="E67" s="173"/>
-      <c r="F67" s="173"/>
-      <c r="G67" s="172"/>
-      <c r="H67" s="172"/>
-      <c r="I67" s="172"/>
-      <c r="J67" s="174"/>
+      <c r="A67" s="124"/>
+      <c r="B67" s="125"/>
+      <c r="C67" s="126"/>
+      <c r="D67" s="127"/>
+      <c r="E67" s="127"/>
+      <c r="F67" s="127"/>
+      <c r="G67" s="126"/>
+      <c r="H67" s="126"/>
+      <c r="I67" s="126"/>
+      <c r="J67" s="128"/>
     </row>
     <row r="68" spans="1:10" ht="12" customHeight="1">
       <c r="I68"/>
@@ -7453,42 +7770,27 @@
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="D66:F66"/>
-    <mergeCell ref="D56:F56"/>
-    <mergeCell ref="D61:F61"/>
-    <mergeCell ref="D59:F59"/>
-    <mergeCell ref="D60:F60"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="D62:F62"/>
-    <mergeCell ref="A63:C63"/>
-    <mergeCell ref="D64:F64"/>
-    <mergeCell ref="A65:C65"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="D54:F54"/>
-    <mergeCell ref="A55:C55"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="D57:F57"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="D51:F51"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="D48:F48"/>
-    <mergeCell ref="D53:F53"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:G10"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D22:F22"/>
     <mergeCell ref="B1:D2"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="B5:D5"/>
@@ -7505,27 +7807,42 @@
     <mergeCell ref="A11:J11"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:G10"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="D54:F54"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="D51:F51"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="D53:F53"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="D62:F62"/>
+    <mergeCell ref="A63:C63"/>
+    <mergeCell ref="D64:F64"/>
+    <mergeCell ref="A65:C65"/>
+    <mergeCell ref="D66:F66"/>
+    <mergeCell ref="D56:F56"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="D60:F60"/>
+    <mergeCell ref="D57:F57"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7542,7 +7859,7 @@
   </sheetPr>
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="82" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScale="82" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -7562,9 +7879,9 @@
       <c r="A1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="147"/>
-      <c r="C1" s="147"/>
-      <c r="D1" s="147"/>
+      <c r="B1" s="144"/>
+      <c r="C1" s="144"/>
+      <c r="D1" s="144"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -7575,9 +7892,9 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="148"/>
-      <c r="C2" s="148"/>
-      <c r="D2" s="148"/>
+      <c r="B2" s="145"/>
+      <c r="C2" s="145"/>
+      <c r="D2" s="145"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -7590,17 +7907,17 @@
       <c r="A3" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="124" t="s">
+      <c r="B3" s="129" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="124"/>
-      <c r="D3" s="125"/>
+      <c r="C3" s="129"/>
+      <c r="D3" s="130"/>
       <c r="E3" s="60"/>
       <c r="F3" s="60"/>
       <c r="G3" s="60"/>
-      <c r="H3" s="155"/>
-      <c r="I3" s="155"/>
-      <c r="J3" s="155"/>
+      <c r="H3" s="154"/>
+      <c r="I3" s="154"/>
+      <c r="J3" s="154"/>
       <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="12.75">
@@ -7615,26 +7932,26 @@
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
       <c r="G4" s="60"/>
-      <c r="H4" s="155"/>
-      <c r="I4" s="155"/>
-      <c r="J4" s="155"/>
+      <c r="H4" s="154"/>
+      <c r="I4" s="154"/>
+      <c r="J4" s="154"/>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" s="70" customFormat="1" ht="25.5">
       <c r="A5" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="150" t="s">
+      <c r="B5" s="147" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="151"/>
-      <c r="D5" s="152"/>
+      <c r="C5" s="148"/>
+      <c r="D5" s="149"/>
       <c r="E5" s="68"/>
       <c r="F5" s="68"/>
       <c r="G5" s="68"/>
-      <c r="H5" s="154"/>
-      <c r="I5" s="154"/>
-      <c r="J5" s="154"/>
+      <c r="H5" s="153"/>
+      <c r="I5" s="153"/>
+      <c r="J5" s="153"/>
       <c r="K5" s="69"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
@@ -7655,9 +7972,9 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="155"/>
-      <c r="I6" s="155"/>
-      <c r="J6" s="155"/>
+      <c r="H6" s="154"/>
+      <c r="I6" s="154"/>
+      <c r="J6" s="154"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -7678,16 +7995,16 @@
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
       <c r="G7" s="61"/>
-      <c r="H7" s="155"/>
-      <c r="I7" s="155"/>
-      <c r="J7" s="155"/>
+      <c r="H7" s="154"/>
+      <c r="I7" s="154"/>
+      <c r="J7" s="154"/>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="149"/>
-      <c r="B8" s="149"/>
-      <c r="C8" s="149"/>
-      <c r="D8" s="149"/>
+      <c r="A8" s="146"/>
+      <c r="B8" s="146"/>
+      <c r="C8" s="146"/>
+      <c r="D8" s="146"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -7697,70 +8014,70 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" s="72" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="133" t="s">
+      <c r="A9" s="163" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="162" t="s">
+      <c r="B9" s="164" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="133" t="s">
+      <c r="C9" s="163" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="134" t="s">
+      <c r="D9" s="168" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="135"/>
-      <c r="F9" s="135"/>
-      <c r="G9" s="136"/>
+      <c r="E9" s="169"/>
+      <c r="F9" s="169"/>
+      <c r="G9" s="170"/>
       <c r="H9" s="159" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="128" t="s">
+      <c r="I9" s="155" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="128" t="s">
+      <c r="J9" s="155" t="s">
         <v>32</v>
       </c>
       <c r="K9" s="71"/>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="128"/>
-      <c r="B10" s="163"/>
-      <c r="C10" s="128"/>
-      <c r="D10" s="137"/>
-      <c r="E10" s="138"/>
-      <c r="F10" s="138"/>
-      <c r="G10" s="139"/>
-      <c r="H10" s="137"/>
-      <c r="I10" s="128"/>
-      <c r="J10" s="128"/>
+      <c r="A10" s="155"/>
+      <c r="B10" s="165"/>
+      <c r="C10" s="155"/>
+      <c r="D10" s="160"/>
+      <c r="E10" s="171"/>
+      <c r="F10" s="171"/>
+      <c r="G10" s="172"/>
+      <c r="H10" s="160"/>
+      <c r="I10" s="155"/>
+      <c r="J10" s="155"/>
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" s="73" customFormat="1" ht="15">
-      <c r="A11" s="160"/>
-      <c r="B11" s="160"/>
-      <c r="C11" s="160"/>
-      <c r="D11" s="160"/>
-      <c r="E11" s="160"/>
-      <c r="F11" s="160"/>
-      <c r="G11" s="160"/>
-      <c r="H11" s="160"/>
-      <c r="I11" s="160"/>
-      <c r="J11" s="161"/>
+      <c r="A11" s="161"/>
+      <c r="B11" s="161"/>
+      <c r="C11" s="161"/>
+      <c r="D11" s="161"/>
+      <c r="E11" s="161"/>
+      <c r="F11" s="161"/>
+      <c r="G11" s="161"/>
+      <c r="H11" s="161"/>
+      <c r="I11" s="161"/>
+      <c r="J11" s="162"/>
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A12" s="140" t="s">
+      <c r="A12" s="150" t="s">
         <v>127</v>
       </c>
-      <c r="B12" s="141"/>
-      <c r="C12" s="141"/>
-      <c r="D12" s="141"/>
-      <c r="E12" s="141"/>
-      <c r="F12" s="141"/>
-      <c r="G12" s="141"/>
-      <c r="H12" s="141"/>
-      <c r="I12" s="141"/>
-      <c r="J12" s="153"/>
+      <c r="B12" s="151"/>
+      <c r="C12" s="151"/>
+      <c r="D12" s="151"/>
+      <c r="E12" s="151"/>
+      <c r="F12" s="151"/>
+      <c r="G12" s="151"/>
+      <c r="H12" s="151"/>
+      <c r="I12" s="151"/>
+      <c r="J12" s="152"/>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" ht="102.75" customHeight="1" outlineLevel="1">
       <c r="A13" s="77" t="s">
@@ -7772,11 +8089,11 @@
       <c r="C13" s="76" t="s">
         <v>165</v>
       </c>
-      <c r="D13" s="126" t="s">
+      <c r="D13" s="138" t="s">
         <v>166</v>
       </c>
-      <c r="E13" s="127"/>
-      <c r="F13" s="127"/>
+      <c r="E13" s="139"/>
+      <c r="F13" s="139"/>
       <c r="G13" s="75"/>
       <c r="H13" s="89"/>
       <c r="I13" s="76"/>
@@ -7792,11 +8109,11 @@
       <c r="C14" s="76" t="s">
         <v>169</v>
       </c>
-      <c r="D14" s="126" t="s">
+      <c r="D14" s="138" t="s">
         <v>170</v>
       </c>
-      <c r="E14" s="127"/>
-      <c r="F14" s="127"/>
+      <c r="E14" s="139"/>
+      <c r="F14" s="139"/>
       <c r="G14" s="75"/>
       <c r="H14" s="89"/>
       <c r="I14" s="76"/>
@@ -7812,22 +8129,22 @@
       <c r="C15" s="76" t="s">
         <v>172</v>
       </c>
-      <c r="D15" s="126" t="s">
+      <c r="D15" s="138" t="s">
         <v>173</v>
       </c>
-      <c r="E15" s="127"/>
-      <c r="F15" s="127"/>
+      <c r="E15" s="139"/>
+      <c r="F15" s="139"/>
       <c r="G15" s="75"/>
       <c r="H15" s="89"/>
       <c r="I15" s="76"/>
       <c r="J15" s="74"/>
     </row>
     <row r="16" spans="1:11" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A16" s="140" t="s">
+      <c r="A16" s="150" t="s">
         <v>128</v>
       </c>
-      <c r="B16" s="141"/>
-      <c r="C16" s="141"/>
+      <c r="B16" s="151"/>
+      <c r="C16" s="151"/>
       <c r="D16" s="87"/>
       <c r="E16" s="87"/>
       <c r="F16" s="87"/>
@@ -7846,11 +8163,11 @@
       <c r="C17" s="86" t="s">
         <v>136</v>
       </c>
-      <c r="D17" s="168" t="s">
+      <c r="D17" s="173" t="s">
         <v>135</v>
       </c>
-      <c r="E17" s="169"/>
-      <c r="F17" s="169"/>
+      <c r="E17" s="174"/>
+      <c r="F17" s="174"/>
       <c r="G17" s="94"/>
       <c r="H17" s="95"/>
       <c r="I17" s="86"/>
@@ -7866,11 +8183,11 @@
       <c r="C18" s="86" t="s">
         <v>138</v>
       </c>
-      <c r="D18" s="168" t="s">
+      <c r="D18" s="173" t="s">
         <v>139</v>
       </c>
-      <c r="E18" s="169"/>
-      <c r="F18" s="169"/>
+      <c r="E18" s="174"/>
+      <c r="F18" s="174"/>
       <c r="G18" s="94"/>
       <c r="H18" s="95"/>
       <c r="I18" s="86"/>
@@ -7886,22 +8203,22 @@
       <c r="C19" s="86" t="s">
         <v>136</v>
       </c>
-      <c r="D19" s="168" t="s">
+      <c r="D19" s="173" t="s">
         <v>141</v>
       </c>
-      <c r="E19" s="169"/>
-      <c r="F19" s="169"/>
+      <c r="E19" s="174"/>
+      <c r="F19" s="174"/>
       <c r="G19" s="94"/>
       <c r="H19" s="95"/>
       <c r="I19" s="86"/>
       <c r="J19" s="96"/>
     </row>
     <row r="20" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A20" s="140" t="s">
+      <c r="A20" s="150" t="s">
         <v>145</v>
       </c>
-      <c r="B20" s="141"/>
-      <c r="C20" s="141"/>
+      <c r="B20" s="151"/>
+      <c r="C20" s="151"/>
       <c r="D20" s="87"/>
       <c r="E20" s="87"/>
       <c r="F20" s="87"/>
@@ -7920,11 +8237,11 @@
       <c r="C21" s="76" t="s">
         <v>149</v>
       </c>
-      <c r="D21" s="126" t="s">
+      <c r="D21" s="138" t="s">
         <v>147</v>
       </c>
-      <c r="E21" s="127"/>
-      <c r="F21" s="127"/>
+      <c r="E21" s="139"/>
+      <c r="F21" s="139"/>
       <c r="G21" s="75"/>
       <c r="H21" s="82"/>
       <c r="I21" s="76"/>
@@ -7940,11 +8257,11 @@
       <c r="C22" s="76" t="s">
         <v>150</v>
       </c>
-      <c r="D22" s="126" t="s">
+      <c r="D22" s="138" t="s">
         <v>151</v>
       </c>
-      <c r="E22" s="127"/>
-      <c r="F22" s="127"/>
+      <c r="E22" s="139"/>
+      <c r="F22" s="139"/>
       <c r="G22" s="75"/>
       <c r="H22" s="82"/>
       <c r="I22" s="76"/>
@@ -7960,11 +8277,11 @@
       <c r="C23" s="76" t="s">
         <v>153</v>
       </c>
-      <c r="D23" s="126" t="s">
+      <c r="D23" s="138" t="s">
         <v>154</v>
       </c>
-      <c r="E23" s="127"/>
-      <c r="F23" s="127"/>
+      <c r="E23" s="139"/>
+      <c r="F23" s="139"/>
       <c r="G23" s="75"/>
       <c r="H23" s="82"/>
       <c r="I23" s="76"/>
@@ -7980,20 +8297,20 @@
       <c r="C24" s="76" t="s">
         <v>156</v>
       </c>
-      <c r="D24" s="126" t="s">
+      <c r="D24" s="138" t="s">
         <v>157</v>
       </c>
-      <c r="E24" s="127"/>
-      <c r="F24" s="127"/>
+      <c r="E24" s="139"/>
+      <c r="F24" s="139"/>
       <c r="G24" s="75"/>
       <c r="H24" s="82"/>
       <c r="I24" s="76"/>
       <c r="J24" s="74"/>
     </row>
     <row r="25" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A25" s="129"/>
-      <c r="B25" s="130"/>
-      <c r="C25" s="130"/>
+      <c r="A25" s="133"/>
+      <c r="B25" s="134"/>
+      <c r="C25" s="134"/>
       <c r="D25" s="97"/>
       <c r="E25" s="97"/>
       <c r="F25" s="97"/>
@@ -8006,9 +8323,9 @@
       <c r="A26" s="77"/>
       <c r="B26" s="92"/>
       <c r="C26" s="76"/>
-      <c r="D26" s="142"/>
-      <c r="E26" s="143"/>
-      <c r="F26" s="143"/>
+      <c r="D26" s="131"/>
+      <c r="E26" s="132"/>
+      <c r="F26" s="132"/>
       <c r="G26" s="75"/>
       <c r="H26" s="82"/>
       <c r="I26" s="76"/>
@@ -8018,9 +8335,9 @@
       <c r="A27" s="77"/>
       <c r="B27" s="92"/>
       <c r="C27" s="76"/>
-      <c r="D27" s="142"/>
-      <c r="E27" s="143"/>
-      <c r="F27" s="143"/>
+      <c r="D27" s="131"/>
+      <c r="E27" s="132"/>
+      <c r="F27" s="132"/>
       <c r="G27" s="75"/>
       <c r="H27" s="82"/>
       <c r="I27" s="76"/>
@@ -8030,9 +8347,9 @@
       <c r="A28" s="77"/>
       <c r="B28" s="92"/>
       <c r="C28" s="76"/>
-      <c r="D28" s="142"/>
-      <c r="E28" s="143"/>
-      <c r="F28" s="143"/>
+      <c r="D28" s="131"/>
+      <c r="E28" s="132"/>
+      <c r="F28" s="132"/>
       <c r="G28" s="75"/>
       <c r="H28" s="82"/>
       <c r="I28" s="76"/>
@@ -8042,9 +8359,9 @@
       <c r="A29" s="77"/>
       <c r="B29" s="92"/>
       <c r="C29" s="76"/>
-      <c r="D29" s="142"/>
-      <c r="E29" s="143"/>
-      <c r="F29" s="143"/>
+      <c r="D29" s="131"/>
+      <c r="E29" s="132"/>
+      <c r="F29" s="132"/>
       <c r="G29" s="75"/>
       <c r="H29" s="82"/>
       <c r="I29" s="76"/>
@@ -8054,9 +8371,9 @@
       <c r="A30" s="77"/>
       <c r="B30" s="92"/>
       <c r="C30" s="76"/>
-      <c r="D30" s="142"/>
-      <c r="E30" s="143"/>
-      <c r="F30" s="143"/>
+      <c r="D30" s="131"/>
+      <c r="E30" s="132"/>
+      <c r="F30" s="132"/>
       <c r="G30" s="75"/>
       <c r="H30" s="82"/>
       <c r="I30" s="76"/>
@@ -8066,18 +8383,18 @@
       <c r="A31" s="77"/>
       <c r="B31" s="92"/>
       <c r="C31" s="76"/>
-      <c r="D31" s="142"/>
-      <c r="E31" s="143"/>
-      <c r="F31" s="143"/>
+      <c r="D31" s="131"/>
+      <c r="E31" s="132"/>
+      <c r="F31" s="132"/>
       <c r="G31" s="75"/>
       <c r="H31" s="82"/>
       <c r="I31" s="76"/>
       <c r="J31" s="74"/>
     </row>
     <row r="32" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A32" s="129"/>
-      <c r="B32" s="130"/>
-      <c r="C32" s="130"/>
+      <c r="A32" s="133"/>
+      <c r="B32" s="134"/>
+      <c r="C32" s="134"/>
       <c r="D32" s="97"/>
       <c r="E32" s="97"/>
       <c r="F32" s="97"/>
@@ -8090,9 +8407,9 @@
       <c r="A33" s="77"/>
       <c r="B33" s="92"/>
       <c r="C33" s="76"/>
-      <c r="D33" s="142"/>
-      <c r="E33" s="143"/>
-      <c r="F33" s="143"/>
+      <c r="D33" s="131"/>
+      <c r="E33" s="132"/>
+      <c r="F33" s="132"/>
       <c r="G33" s="75"/>
       <c r="H33" s="82"/>
       <c r="I33" s="76"/>
@@ -8228,30 +8545,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:G10"/>
     <mergeCell ref="D19:F19"/>
     <mergeCell ref="B1:D2"/>
     <mergeCell ref="B3:D3"/>
@@ -8268,6 +8561,30 @@
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="H6:J6"/>
     <mergeCell ref="H7:J7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -8282,7 +8599,7 @@
   </sheetPr>
   <dimension ref="A1:K67"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="80" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="80" workbookViewId="0">
       <selection activeCell="D21" sqref="D21:F21"/>
     </sheetView>
   </sheetViews>
@@ -8302,9 +8619,9 @@
       <c r="A1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="147"/>
-      <c r="C1" s="147"/>
-      <c r="D1" s="147"/>
+      <c r="B1" s="144"/>
+      <c r="C1" s="144"/>
+      <c r="D1" s="144"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -8315,9 +8632,9 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="148"/>
-      <c r="C2" s="148"/>
-      <c r="D2" s="148"/>
+      <c r="B2" s="145"/>
+      <c r="C2" s="145"/>
+      <c r="D2" s="145"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -8330,17 +8647,17 @@
       <c r="A3" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="124" t="s">
+      <c r="B3" s="129" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="124"/>
-      <c r="D3" s="125"/>
+      <c r="C3" s="129"/>
+      <c r="D3" s="130"/>
       <c r="E3" s="60"/>
       <c r="F3" s="60"/>
       <c r="G3" s="60"/>
-      <c r="H3" s="155"/>
-      <c r="I3" s="155"/>
-      <c r="J3" s="155"/>
+      <c r="H3" s="154"/>
+      <c r="I3" s="154"/>
+      <c r="J3" s="154"/>
       <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="12.75">
@@ -8355,26 +8672,26 @@
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
       <c r="G4" s="60"/>
-      <c r="H4" s="155"/>
-      <c r="I4" s="155"/>
-      <c r="J4" s="155"/>
+      <c r="H4" s="154"/>
+      <c r="I4" s="154"/>
+      <c r="J4" s="154"/>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" s="70" customFormat="1" ht="25.5">
       <c r="A5" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="150" t="s">
+      <c r="B5" s="147" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="151"/>
-      <c r="D5" s="152"/>
+      <c r="C5" s="148"/>
+      <c r="D5" s="149"/>
       <c r="E5" s="68"/>
       <c r="F5" s="68"/>
       <c r="G5" s="68"/>
-      <c r="H5" s="154"/>
-      <c r="I5" s="154"/>
-      <c r="J5" s="154"/>
+      <c r="H5" s="153"/>
+      <c r="I5" s="153"/>
+      <c r="J5" s="153"/>
       <c r="K5" s="69"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
@@ -8395,9 +8712,9 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="155"/>
-      <c r="I6" s="155"/>
-      <c r="J6" s="155"/>
+      <c r="H6" s="154"/>
+      <c r="I6" s="154"/>
+      <c r="J6" s="154"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -8418,16 +8735,16 @@
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
       <c r="G7" s="61"/>
-      <c r="H7" s="155"/>
-      <c r="I7" s="155"/>
-      <c r="J7" s="155"/>
+      <c r="H7" s="154"/>
+      <c r="I7" s="154"/>
+      <c r="J7" s="154"/>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="149"/>
-      <c r="B8" s="149"/>
-      <c r="C8" s="149"/>
-      <c r="D8" s="149"/>
+      <c r="A8" s="146"/>
+      <c r="B8" s="146"/>
+      <c r="C8" s="146"/>
+      <c r="D8" s="146"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -8437,70 +8754,70 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" s="72" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="133" t="s">
+      <c r="A9" s="163" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="162" t="s">
+      <c r="B9" s="164" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="133" t="s">
+      <c r="C9" s="163" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="134" t="s">
+      <c r="D9" s="168" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="135"/>
-      <c r="F9" s="135"/>
-      <c r="G9" s="136"/>
+      <c r="E9" s="169"/>
+      <c r="F9" s="169"/>
+      <c r="G9" s="170"/>
       <c r="H9" s="159" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="128" t="s">
+      <c r="I9" s="155" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="128" t="s">
+      <c r="J9" s="155" t="s">
         <v>32</v>
       </c>
       <c r="K9" s="71"/>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="128"/>
-      <c r="B10" s="163"/>
-      <c r="C10" s="128"/>
-      <c r="D10" s="137"/>
-      <c r="E10" s="138"/>
-      <c r="F10" s="138"/>
-      <c r="G10" s="139"/>
-      <c r="H10" s="137"/>
-      <c r="I10" s="128"/>
-      <c r="J10" s="128"/>
+      <c r="A10" s="155"/>
+      <c r="B10" s="165"/>
+      <c r="C10" s="155"/>
+      <c r="D10" s="160"/>
+      <c r="E10" s="171"/>
+      <c r="F10" s="171"/>
+      <c r="G10" s="172"/>
+      <c r="H10" s="160"/>
+      <c r="I10" s="155"/>
+      <c r="J10" s="155"/>
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" s="73" customFormat="1" ht="15">
-      <c r="A11" s="160"/>
-      <c r="B11" s="160"/>
-      <c r="C11" s="160"/>
-      <c r="D11" s="160"/>
-      <c r="E11" s="160"/>
-      <c r="F11" s="160"/>
-      <c r="G11" s="160"/>
-      <c r="H11" s="160"/>
-      <c r="I11" s="160"/>
-      <c r="J11" s="161"/>
+      <c r="A11" s="161"/>
+      <c r="B11" s="161"/>
+      <c r="C11" s="161"/>
+      <c r="D11" s="161"/>
+      <c r="E11" s="161"/>
+      <c r="F11" s="161"/>
+      <c r="G11" s="161"/>
+      <c r="H11" s="161"/>
+      <c r="I11" s="161"/>
+      <c r="J11" s="162"/>
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A12" s="140" t="s">
+      <c r="A12" s="150" t="s">
         <v>278</v>
       </c>
-      <c r="B12" s="141"/>
-      <c r="C12" s="141"/>
-      <c r="D12" s="141"/>
-      <c r="E12" s="141"/>
-      <c r="F12" s="141"/>
-      <c r="G12" s="141"/>
-      <c r="H12" s="141"/>
-      <c r="I12" s="141"/>
-      <c r="J12" s="153"/>
+      <c r="B12" s="151"/>
+      <c r="C12" s="151"/>
+      <c r="D12" s="151"/>
+      <c r="E12" s="151"/>
+      <c r="F12" s="151"/>
+      <c r="G12" s="151"/>
+      <c r="H12" s="151"/>
+      <c r="I12" s="151"/>
+      <c r="J12" s="152"/>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" ht="132.75" customHeight="1" outlineLevel="1">
       <c r="A13" s="77" t="s">
@@ -8512,9 +8829,9 @@
       <c r="C13" s="122" t="s">
         <v>251</v>
       </c>
-      <c r="D13" s="126"/>
-      <c r="E13" s="127"/>
-      <c r="F13" s="127"/>
+      <c r="D13" s="138"/>
+      <c r="E13" s="139"/>
+      <c r="F13" s="139"/>
       <c r="G13" s="75"/>
       <c r="H13" s="89"/>
       <c r="I13" s="76"/>
@@ -8530,9 +8847,9 @@
       <c r="C14" s="122" t="s">
         <v>252</v>
       </c>
-      <c r="D14" s="126"/>
-      <c r="E14" s="127"/>
-      <c r="F14" s="127"/>
+      <c r="D14" s="138"/>
+      <c r="E14" s="139"/>
+      <c r="F14" s="139"/>
       <c r="G14" s="75"/>
       <c r="H14" s="89"/>
       <c r="I14" s="76"/>
@@ -8548,20 +8865,20 @@
       <c r="C15" s="76" t="s">
         <v>260</v>
       </c>
-      <c r="D15" s="126"/>
-      <c r="E15" s="127"/>
-      <c r="F15" s="127"/>
+      <c r="D15" s="138"/>
+      <c r="E15" s="139"/>
+      <c r="F15" s="139"/>
       <c r="G15" s="75"/>
       <c r="H15" s="89"/>
       <c r="I15" s="76"/>
       <c r="J15" s="74"/>
     </row>
     <row r="16" spans="1:11" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A16" s="140" t="s">
+      <c r="A16" s="150" t="s">
         <v>279</v>
       </c>
-      <c r="B16" s="141"/>
-      <c r="C16" s="141"/>
+      <c r="B16" s="151"/>
+      <c r="C16" s="151"/>
       <c r="D16" s="87"/>
       <c r="E16" s="87"/>
       <c r="F16" s="87"/>
@@ -8580,9 +8897,9 @@
       <c r="C17" s="86" t="s">
         <v>286</v>
       </c>
-      <c r="D17" s="168"/>
-      <c r="E17" s="169"/>
-      <c r="F17" s="169"/>
+      <c r="D17" s="173"/>
+      <c r="E17" s="174"/>
+      <c r="F17" s="174"/>
       <c r="G17" s="94"/>
       <c r="H17" s="95"/>
       <c r="I17" s="86"/>
@@ -8598,9 +8915,9 @@
       <c r="C18" s="86" t="s">
         <v>287</v>
       </c>
-      <c r="D18" s="168"/>
-      <c r="E18" s="169"/>
-      <c r="F18" s="169"/>
+      <c r="D18" s="173"/>
+      <c r="E18" s="174"/>
+      <c r="F18" s="174"/>
       <c r="G18" s="94"/>
       <c r="H18" s="95"/>
       <c r="I18" s="86"/>
@@ -8616,9 +8933,9 @@
       <c r="C19" s="76" t="s">
         <v>269</v>
       </c>
-      <c r="D19" s="168"/>
-      <c r="E19" s="169"/>
-      <c r="F19" s="169"/>
+      <c r="D19" s="173"/>
+      <c r="E19" s="174"/>
+      <c r="F19" s="174"/>
       <c r="G19" s="94"/>
       <c r="H19" s="95"/>
       <c r="I19" s="86"/>
@@ -8634,9 +8951,9 @@
       <c r="C20" s="86" t="s">
         <v>282</v>
       </c>
-      <c r="D20" s="168"/>
-      <c r="E20" s="169"/>
-      <c r="F20" s="169"/>
+      <c r="D20" s="173"/>
+      <c r="E20" s="174"/>
+      <c r="F20" s="174"/>
       <c r="G20" s="94"/>
       <c r="H20" s="95"/>
       <c r="I20" s="86"/>
@@ -8652,20 +8969,20 @@
       <c r="C21" s="123" t="s">
         <v>283</v>
       </c>
-      <c r="D21" s="168"/>
-      <c r="E21" s="169"/>
-      <c r="F21" s="169"/>
+      <c r="D21" s="173"/>
+      <c r="E21" s="174"/>
+      <c r="F21" s="174"/>
       <c r="G21" s="94"/>
       <c r="H21" s="95"/>
       <c r="I21" s="86"/>
       <c r="J21" s="96"/>
     </row>
     <row r="22" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A22" s="140" t="s">
+      <c r="A22" s="150" t="s">
         <v>255</v>
       </c>
-      <c r="B22" s="141"/>
-      <c r="C22" s="141"/>
+      <c r="B22" s="151"/>
+      <c r="C22" s="151"/>
       <c r="D22" s="87"/>
       <c r="E22" s="87"/>
       <c r="F22" s="87"/>
@@ -8684,9 +9001,9 @@
       <c r="C23" s="76" t="s">
         <v>258</v>
       </c>
-      <c r="D23" s="126"/>
-      <c r="E23" s="127"/>
-      <c r="F23" s="127"/>
+      <c r="D23" s="138"/>
+      <c r="E23" s="139"/>
+      <c r="F23" s="139"/>
       <c r="G23" s="75"/>
       <c r="H23" s="82"/>
       <c r="I23" s="76"/>
@@ -8702,9 +9019,9 @@
       <c r="C24" s="76" t="s">
         <v>260</v>
       </c>
-      <c r="D24" s="126"/>
-      <c r="E24" s="127"/>
-      <c r="F24" s="127"/>
+      <c r="D24" s="138"/>
+      <c r="E24" s="139"/>
+      <c r="F24" s="139"/>
       <c r="G24" s="75"/>
       <c r="H24" s="82"/>
       <c r="I24" s="76"/>
@@ -8720,9 +9037,9 @@
       <c r="C25" s="76" t="s">
         <v>269</v>
       </c>
-      <c r="D25" s="126"/>
-      <c r="E25" s="127"/>
-      <c r="F25" s="127"/>
+      <c r="D25" s="138"/>
+      <c r="E25" s="139"/>
+      <c r="F25" s="139"/>
       <c r="G25" s="75"/>
       <c r="H25" s="82"/>
       <c r="I25" s="76"/>
@@ -8738,18 +9055,18 @@
       <c r="C26" s="76" t="s">
         <v>266</v>
       </c>
-      <c r="D26" s="126"/>
-      <c r="E26" s="127"/>
-      <c r="F26" s="127"/>
+      <c r="D26" s="138"/>
+      <c r="E26" s="139"/>
+      <c r="F26" s="139"/>
       <c r="G26" s="75"/>
       <c r="H26" s="82"/>
       <c r="I26" s="76"/>
       <c r="J26" s="74"/>
     </row>
     <row r="27" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A27" s="129"/>
-      <c r="B27" s="130"/>
-      <c r="C27" s="130"/>
+      <c r="A27" s="133"/>
+      <c r="B27" s="134"/>
+      <c r="C27" s="134"/>
       <c r="D27" s="97"/>
       <c r="E27" s="97"/>
       <c r="F27" s="97"/>
@@ -8762,9 +9079,9 @@
       <c r="A28" s="77"/>
       <c r="B28" s="92"/>
       <c r="C28" s="76"/>
-      <c r="D28" s="142"/>
-      <c r="E28" s="143"/>
-      <c r="F28" s="143"/>
+      <c r="D28" s="131"/>
+      <c r="E28" s="132"/>
+      <c r="F28" s="132"/>
       <c r="G28" s="75"/>
       <c r="H28" s="82"/>
       <c r="I28" s="76"/>
@@ -8774,9 +9091,9 @@
       <c r="A29" s="77"/>
       <c r="B29" s="92"/>
       <c r="C29" s="76"/>
-      <c r="D29" s="142"/>
-      <c r="E29" s="143"/>
-      <c r="F29" s="143"/>
+      <c r="D29" s="131"/>
+      <c r="E29" s="132"/>
+      <c r="F29" s="132"/>
       <c r="G29" s="75"/>
       <c r="H29" s="82"/>
       <c r="I29" s="76"/>
@@ -8786,9 +9103,9 @@
       <c r="A30" s="77"/>
       <c r="B30" s="92"/>
       <c r="C30" s="76"/>
-      <c r="D30" s="142"/>
-      <c r="E30" s="143"/>
-      <c r="F30" s="143"/>
+      <c r="D30" s="131"/>
+      <c r="E30" s="132"/>
+      <c r="F30" s="132"/>
       <c r="G30" s="75"/>
       <c r="H30" s="82"/>
       <c r="I30" s="76"/>
@@ -8798,9 +9115,9 @@
       <c r="A31" s="77"/>
       <c r="B31" s="92"/>
       <c r="C31" s="76"/>
-      <c r="D31" s="142"/>
-      <c r="E31" s="143"/>
-      <c r="F31" s="143"/>
+      <c r="D31" s="131"/>
+      <c r="E31" s="132"/>
+      <c r="F31" s="132"/>
       <c r="G31" s="75"/>
       <c r="H31" s="82"/>
       <c r="I31" s="76"/>
@@ -8810,9 +9127,9 @@
       <c r="A32" s="77"/>
       <c r="B32" s="92"/>
       <c r="C32" s="76"/>
-      <c r="D32" s="142"/>
-      <c r="E32" s="143"/>
-      <c r="F32" s="143"/>
+      <c r="D32" s="131"/>
+      <c r="E32" s="132"/>
+      <c r="F32" s="132"/>
       <c r="G32" s="75"/>
       <c r="H32" s="82"/>
       <c r="I32" s="76"/>
@@ -8822,18 +9139,18 @@
       <c r="A33" s="77"/>
       <c r="B33" s="92"/>
       <c r="C33" s="76"/>
-      <c r="D33" s="142"/>
-      <c r="E33" s="143"/>
-      <c r="F33" s="143"/>
+      <c r="D33" s="131"/>
+      <c r="E33" s="132"/>
+      <c r="F33" s="132"/>
       <c r="G33" s="75"/>
       <c r="H33" s="82"/>
       <c r="I33" s="76"/>
       <c r="J33" s="74"/>
     </row>
     <row r="34" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A34" s="129"/>
-      <c r="B34" s="130"/>
-      <c r="C34" s="130"/>
+      <c r="A34" s="133"/>
+      <c r="B34" s="134"/>
+      <c r="C34" s="134"/>
       <c r="D34" s="97"/>
       <c r="E34" s="97"/>
       <c r="F34" s="97"/>
@@ -8846,9 +9163,9 @@
       <c r="A35" s="77"/>
       <c r="B35" s="92"/>
       <c r="C35" s="76"/>
-      <c r="D35" s="142"/>
-      <c r="E35" s="143"/>
-      <c r="F35" s="143"/>
+      <c r="D35" s="131"/>
+      <c r="E35" s="132"/>
+      <c r="F35" s="132"/>
       <c r="G35" s="75"/>
       <c r="H35" s="82"/>
       <c r="I35" s="76"/>
@@ -8984,11 +9301,27 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="B1:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="D13:F13"/>
     <mergeCell ref="D35:F35"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="A16:C16"/>
@@ -9005,27 +9338,11 @@
     <mergeCell ref="D29:F29"/>
     <mergeCell ref="D20:F20"/>
     <mergeCell ref="D18:F18"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="B1:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:G10"/>
-    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="D21:F21"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -9151,7 +9468,7 @@
       </c>
       <c r="G8" s="66">
         <f>Samples!D7</f>
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="59" customFormat="1" ht="14.25">
@@ -9226,7 +9543,7 @@
       </c>
       <c r="G11" s="54">
         <f>SUM(G6:G10)</f>
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14.25">
@@ -9247,7 +9564,7 @@
       <c r="D13" s="19"/>
       <c r="E13" s="23">
         <f>(D11+E11)*100/G11</f>
-        <v>33.87096774193548</v>
+        <v>32.8125</v>
       </c>
       <c r="F13" s="19" t="s">
         <v>22</v>
@@ -9263,7 +9580,7 @@
       <c r="D14" s="19"/>
       <c r="E14" s="23">
         <f>D11*100/G11</f>
-        <v>20.967741935483872</v>
+        <v>20.3125</v>
       </c>
       <c r="F14" s="19" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
up test tc tao sk
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University_IT\Tam\KiemThuPhanMem\event-manager-javafx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C9159E-EE17-4B22-BA2A-9B53560D4358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F961AA-4C2D-437E-99CA-40F43B705F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11790" yWindow="930" windowWidth="10365" windowHeight="10155" tabRatio="821" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="821" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="97" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="315">
   <si>
     <t>TC1</t>
   </si>
@@ -457,48 +457,10 @@
     <t>Kiểm tra ngày tổ chức sự kiện</t>
   </si>
   <si>
-    <t>1: Truy cập vào trang quản trị
-2: Chọn "Thêm sự kiện" để tạo sự kiện mới
-3: Nhập thông tin sự kiện hợp lệ(tên sự kiện, ngày tổ chức, địa điểm, thời gian, sức chứa, số lượng khách, tên người tạo sự kiện). Trong đó:
-   + Ngày tổ chức phải lớn hơn ngày hiện tại
-   + Không trùng địa điểm và giờ với sự kiện khác
-   + Số lượng khách không vượt quá sức chứa địa điểm
-4: Nhấn nút Lưu sự kiện</t>
-  </si>
-  <si>
-    <t>1: Truy cập vào trang quản trị
-2: Chọn "Thêm sự kiện" để tạo sự kiện mới
-3: Nhập đầy đủ thông tin các trường bắt buộc. Riêng ngày tạo chọn ngày trong quá khứ
-4: Nhấn nút Lưu sự kiện
-5: Hiển thị thông báo lỗi thời gian không hợp lệ</t>
-  </si>
-  <si>
-    <t>1: Truy cập vào trang quản trị
-2: Chọn "Thêm sự kiện" để tạo sự kiện mới
-3: Để trống một hoặc nhiều ô thông tin bắt buộc
-4: Nhấn nút Lưu sự kiện
-5: Hiển thị thông báo lỗi cho từng ô thông tin bị bỏ trống</t>
-  </si>
-  <si>
     <t>Kiểm tra sự trùng lắp sự kiện</t>
   </si>
   <si>
-    <t>1: Truy cập vào trang quản trị
-2: Chọn "Thêm sự kiện" để tạo sự kiện mới
-3: Nhập đầy đủ thông tin các trường bắt buộc
-4: Nhấn nút Lưu sự kiện
-5: Sau đó tạo một sự kiện mới trùng địa điểm và thời gian với sự kiện mới tạo hồi nãy 
-6: Hiển thị thông báo cảnh báo trùng lắp sự kiện</t>
-  </si>
-  <si>
     <t>Kiểm tra sức chứa địa điểm</t>
-  </si>
-  <si>
-    <t>1: Truy cập vào trang quản trị
-2: Chọn "Thêm sự kiện" để tạo sự kiện mới
-3: Nhập đầy đủ thông tin các trường bắt buộc. Riêng số lượng khách thì nhập số lượng vượt quá sức chứa
-4: Nhấn nút Lưu sự kiện 
-6: Hiển thị thông báo lỗi vượt quá sức chứa địa điểm</t>
   </si>
   <si>
     <t>Viết TC Kiểm tra chức năng tạo sự kiện thành công</t>
@@ -1273,6 +1235,63 @@
   </si>
   <si>
     <t>Kiểm tra quá trình hoàn tiền đầy đủ cho người tham gia sau khi sự kiện bị hủy</t>
+  </si>
+  <si>
+    <t>1: Đăng nhập với tư cách là admin
+2: Truy cập vào trang quản trị, chọn mục Sự kiện
+3: Nhập, chọn đầy đủ thông tin sự kiện hợp lệ(tên sự kiện, thể loại, địa điểm, thời gian bắt đầu, thời gian kết thúc, số lượng vé còn, giá vé, ảnh sự kiện, mô tả về sự kiện). Trong đó:
+   + Ngày tổ chức phải lớn hơn ngày hiện tại
+   + Không trùng địa điểm và giờ với sự kiện khác
+   + Số lượng khách không vượt quá sức chứa địa điểm
+4: Nhấn nút Thêm sự kiện
+5: Hiển thị thông báo thêm sự kiện thành công, sự kiện được lưu vào hệ thống và database</t>
+  </si>
+  <si>
+    <t>Test TC Kiểm tra chức năng tạo sự kiện thành công</t>
+  </si>
+  <si>
+    <t>Test TC Kiểm tra tạo sự kiện với các trường nhập liệu cho ô thông tin bắt buộc</t>
+  </si>
+  <si>
+    <t>Cập nhật TC Kiểm tra tạo sự kiện với các trường nhập liệu cho ô thông tin bắt buộc</t>
+  </si>
+  <si>
+    <t>1: Đăng nhập với tư cách là admin
+2: Truy cập vào trang quản trị, chọn mục sự kiện
+3: Để trống một hoặc nhiều ô thông tin bắt buộc
+4: Nhấn nút Thêm sự kiện
+5: Hiển thị thông báo lỗi "Vui lòng điền đầy đủ thông tin"</t>
+  </si>
+  <si>
+    <t>Sự kiện sẽ không được tạo nếu để trống các ô thông tin</t>
+  </si>
+  <si>
+    <t>1: Đăng nhập với tư cách là admin
+2: Truy cập vào trang quản trị, chọn mục sự kiện
+3: Nhập đầy đủ thông tin các trường bắt buộc. Riêng ngày tạo chọn ngày trong quá khứ
+4: Nhấn nút Thêm sự kiện
+5: Hiển thị thông báo lỗi "Ngày tổ chức phải lớn hơn ngày hiện tại</t>
+  </si>
+  <si>
+    <t>Test TC Kiểm tra ngày tổ chức sự kiện</t>
+  </si>
+  <si>
+    <t>Cập nhật TC Kiểm tra ngày tổ chức sự kiện</t>
+  </si>
+  <si>
+    <t>1: Đăng nhập với tư cách là admin
+2: Truy cập vào trang quản trị, chọn mục sự kiện
+3: Nhập đầy đủ thông tin các trường bắt buộc
+4: Nhấn nút Lưu sự kiện
+5: Sau đó tạo một sự kiện mới trùng địa điểm và thời gian với sự kiện mới tạo hồi nãy 
+6: Hiển thị thông báo cảnh báo trùng lắp sự kiện</t>
+  </si>
+  <si>
+    <t>1: Đăng nhập với tư cách là admin
+2: Truy cập vào trang quản trị, chọn mục sự kiện
+3: Nhập đầy đủ thông tin các trường bắt buộc. Riêng số lượng vé còn thì nhập số lượng vượt quá sức chứa của địa điểm
+4: Nhấn nút Thêm sự kiện 
+6: Hiển thị thông báo lỗi "Số lượng khách không được vượt quá sức chứa địa điểm!"</t>
   </si>
 </sst>
 </file>
@@ -1999,7 +2018,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="176">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2345,18 +2364,60 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2366,11 +2427,56 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2384,97 +2490,13 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3888,6 +3910,306 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>1628913</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF0F6C10-C62B-7831-534E-39EA572ACBF6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5784022" y="49157284"/>
+          <a:ext cx="3147391" cy="1628912"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>1616365</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>3138007</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{895BE922-9DF2-FD53-AAC8-015CC44A8B1E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5784022" y="50773648"/>
+          <a:ext cx="3147391" cy="1521642"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>3161195</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C40825D-0689-E692-BE6B-8F052119309F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5784022" y="52318478"/>
+          <a:ext cx="3147391" cy="648805"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{056F7DE1-8512-6BBE-49B4-9336C6D106DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5784022" y="52967283"/>
+          <a:ext cx="3147391" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>-1</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F473A43-1CD3-BD94-8F7B-83961E0B5F92}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5784022" y="55507283"/>
+          <a:ext cx="3147391" cy="2539999"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{336B5F8C-B96F-575C-2054-A520A149CB37}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5784022" y="59234457"/>
+          <a:ext cx="3147391" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4193,8 +4515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H146"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A116" zoomScale="85" workbookViewId="0">
-      <selection activeCell="B133" sqref="B133"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A111" zoomScale="85" workbookViewId="0">
+      <selection activeCell="D116" sqref="D116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -4371,7 +4693,7 @@
       </c>
       <c r="D14" s="39"/>
       <c r="E14" s="100" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="F14" s="110" t="s">
         <v>44</v>
@@ -4439,7 +4761,7 @@
       </c>
       <c r="D18" s="39"/>
       <c r="E18" s="100" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="F18" s="110" t="s">
         <v>44</v>
@@ -4456,7 +4778,7 @@
       </c>
       <c r="D19" s="39"/>
       <c r="E19" s="100" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="F19" s="110" t="s">
         <v>44</v>
@@ -4592,7 +4914,7 @@
       </c>
       <c r="D27" s="99"/>
       <c r="E27" s="104" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F27" s="110" t="s">
         <v>44</v>
@@ -4609,7 +4931,7 @@
       </c>
       <c r="D28" s="99"/>
       <c r="E28" s="104" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="F28" s="110" t="s">
         <v>44</v>
@@ -4660,7 +4982,7 @@
       </c>
       <c r="D31" s="99"/>
       <c r="E31" s="104" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="F31" s="110" t="s">
         <v>44</v>
@@ -4677,7 +4999,7 @@
       </c>
       <c r="D32" s="99"/>
       <c r="E32" s="104" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="F32" s="110" t="s">
         <v>44</v>
@@ -4813,7 +5135,7 @@
       </c>
       <c r="D40" s="99"/>
       <c r="E40" s="104" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F40" s="110" t="s">
         <v>44</v>
@@ -4826,11 +5148,11 @@
         <v>45745</v>
       </c>
       <c r="C41" s="36" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D41" s="99"/>
       <c r="E41" s="104" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F41" s="110" t="s">
         <v>44</v>
@@ -4847,7 +5169,7 @@
       </c>
       <c r="D42" s="99"/>
       <c r="E42" s="104" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F42" s="110" t="s">
         <v>44</v>
@@ -4864,7 +5186,7 @@
       </c>
       <c r="D43" s="99"/>
       <c r="E43" s="104" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F43" s="110" t="s">
         <v>44</v>
@@ -4881,7 +5203,7 @@
       </c>
       <c r="D44" s="99"/>
       <c r="E44" s="104" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F44" s="110" t="s">
         <v>44</v>
@@ -4898,7 +5220,7 @@
       </c>
       <c r="D45" s="99"/>
       <c r="E45" s="104" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="F45" s="110" t="s">
         <v>44</v>
@@ -4915,7 +5237,7 @@
       </c>
       <c r="D46" s="99"/>
       <c r="E46" s="104" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F46" s="110" t="s">
         <v>44</v>
@@ -4932,7 +5254,7 @@
       </c>
       <c r="D47" s="99"/>
       <c r="E47" s="104" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F47" s="110" t="s">
         <v>44</v>
@@ -4949,7 +5271,7 @@
       </c>
       <c r="D48" s="99"/>
       <c r="E48" s="104" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="F48" s="110" t="s">
         <v>44</v>
@@ -4966,7 +5288,7 @@
       </c>
       <c r="D49" s="99"/>
       <c r="E49" s="104" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="F49" s="110" t="s">
         <v>44</v>
@@ -4983,7 +5305,7 @@
       </c>
       <c r="D50" s="99"/>
       <c r="E50" s="104" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F50" s="110" t="s">
         <v>44</v>
@@ -4996,11 +5318,11 @@
         <v>45750</v>
       </c>
       <c r="C51" s="36" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D51" s="99"/>
       <c r="E51" s="104" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F51" s="110" t="s">
         <v>44</v>
@@ -5013,11 +5335,11 @@
         <v>45750</v>
       </c>
       <c r="C52" s="36" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D52" s="99"/>
       <c r="E52" s="104" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F52" s="110" t="s">
         <v>44</v>
@@ -5034,7 +5356,7 @@
       </c>
       <c r="D53" s="99"/>
       <c r="E53" s="104" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F53" s="110" t="s">
         <v>44</v>
@@ -5047,11 +5369,11 @@
         <v>45750</v>
       </c>
       <c r="C54" s="36" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D54" s="99"/>
       <c r="E54" s="104" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="F54" s="110" t="s">
         <v>44</v>
@@ -5064,11 +5386,11 @@
         <v>45750</v>
       </c>
       <c r="C55" s="36" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D55" s="99"/>
       <c r="E55" s="104" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F55" s="110" t="s">
         <v>44</v>
@@ -5085,7 +5407,7 @@
       </c>
       <c r="D56" s="99"/>
       <c r="E56" s="104" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="F56" s="110" t="s">
         <v>44</v>
@@ -5098,11 +5420,11 @@
         <v>45750</v>
       </c>
       <c r="C57" s="36" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D57" s="99"/>
       <c r="E57" s="104" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="F57" s="110" t="s">
         <v>44</v>
@@ -5119,7 +5441,7 @@
       </c>
       <c r="D58" s="99"/>
       <c r="E58" s="104" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="F58" s="110" t="s">
         <v>44</v>
@@ -5136,7 +5458,7 @@
       </c>
       <c r="D59" s="99"/>
       <c r="E59" s="104" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F59" s="110" t="s">
         <v>44</v>
@@ -5153,7 +5475,7 @@
       </c>
       <c r="D60" s="99"/>
       <c r="E60" s="104" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="F60" s="110" t="s">
         <v>44</v>
@@ -5170,7 +5492,7 @@
       </c>
       <c r="D61" s="99"/>
       <c r="E61" s="104" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="F61" s="110" t="s">
         <v>44</v>
@@ -5187,7 +5509,7 @@
       </c>
       <c r="D62" s="99"/>
       <c r="E62" s="104" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="F62" s="110" t="s">
         <v>44</v>
@@ -5204,7 +5526,7 @@
       </c>
       <c r="D63" s="99"/>
       <c r="E63" s="104" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F63" s="110" t="s">
         <v>44</v>
@@ -5221,7 +5543,7 @@
       </c>
       <c r="D64" s="99"/>
       <c r="E64" s="104" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F64" s="110" t="s">
         <v>44</v>
@@ -5238,7 +5560,7 @@
       </c>
       <c r="D65" s="99"/>
       <c r="E65" s="104" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="F65" s="110" t="s">
         <v>44</v>
@@ -5255,7 +5577,7 @@
       </c>
       <c r="D66" s="99"/>
       <c r="E66" s="104" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="F66" s="110" t="s">
         <v>44</v>
@@ -5272,7 +5594,7 @@
       </c>
       <c r="D67" s="99"/>
       <c r="E67" s="104" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="F67" s="110" t="s">
         <v>44</v>
@@ -5289,7 +5611,7 @@
       </c>
       <c r="D68" s="99"/>
       <c r="E68" s="104" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="F68" s="110" t="s">
         <v>44</v>
@@ -5306,7 +5628,7 @@
       </c>
       <c r="D69" s="99"/>
       <c r="E69" s="104" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="F69" s="110" t="s">
         <v>44</v>
@@ -5323,7 +5645,7 @@
       </c>
       <c r="D70" s="99"/>
       <c r="E70" s="104" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="F70" s="110" t="s">
         <v>44</v>
@@ -5340,7 +5662,7 @@
       </c>
       <c r="D71" s="99"/>
       <c r="E71" s="104" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="F71" s="110" t="s">
         <v>44</v>
@@ -5357,7 +5679,7 @@
       </c>
       <c r="D72" s="99"/>
       <c r="E72" s="104" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="F72" s="110" t="s">
         <v>44</v>
@@ -5374,7 +5696,7 @@
       </c>
       <c r="D73" s="99"/>
       <c r="E73" s="104" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="F73" s="110" t="s">
         <v>44</v>
@@ -5387,7 +5709,7 @@
         <v>45755</v>
       </c>
       <c r="C74" s="36" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D74" s="99"/>
       <c r="E74" s="100" t="s">
@@ -5404,11 +5726,11 @@
         <v>45755</v>
       </c>
       <c r="C75" s="36" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D75" s="99"/>
       <c r="E75" s="104" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="F75" s="110" t="s">
         <v>44</v>
@@ -5425,7 +5747,7 @@
       </c>
       <c r="D76" s="99"/>
       <c r="E76" s="104" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="F76" s="110" t="s">
         <v>44</v>
@@ -5442,7 +5764,7 @@
       </c>
       <c r="D77" s="99"/>
       <c r="E77" s="104" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="F77" s="110" t="s">
         <v>44</v>
@@ -5459,7 +5781,7 @@
       </c>
       <c r="D78" s="99"/>
       <c r="E78" s="104" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="F78" s="110" t="s">
         <v>44</v>
@@ -5476,7 +5798,7 @@
       </c>
       <c r="D79" s="99"/>
       <c r="E79" s="104" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="F79" s="110" t="s">
         <v>44</v>
@@ -5493,7 +5815,7 @@
       </c>
       <c r="D80" s="99"/>
       <c r="E80" s="104" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="F80" s="110" t="s">
         <v>44</v>
@@ -5510,7 +5832,7 @@
       </c>
       <c r="D81" s="99"/>
       <c r="E81" s="104" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F81" s="110" t="s">
         <v>44</v>
@@ -5527,7 +5849,7 @@
       </c>
       <c r="D82" s="99"/>
       <c r="E82" s="104" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="F82" s="110" t="s">
         <v>44</v>
@@ -5544,7 +5866,7 @@
       </c>
       <c r="D83" s="99"/>
       <c r="E83" s="104" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="F83" s="110" t="s">
         <v>44</v>
@@ -5578,7 +5900,7 @@
       </c>
       <c r="D85" s="99"/>
       <c r="E85" s="104" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="F85" s="110" t="s">
         <v>44</v>
@@ -5595,7 +5917,7 @@
       </c>
       <c r="D86" s="99"/>
       <c r="E86" s="104" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="F86" s="110" t="s">
         <v>44</v>
@@ -5612,7 +5934,7 @@
       </c>
       <c r="D87" s="99"/>
       <c r="E87" s="104" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="F87" s="110" t="s">
         <v>44</v>
@@ -5629,7 +5951,7 @@
       </c>
       <c r="D88" s="99"/>
       <c r="E88" s="104" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="F88" s="110" t="s">
         <v>44</v>
@@ -5646,7 +5968,7 @@
       </c>
       <c r="D89" s="99"/>
       <c r="E89" s="104" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="F89" s="110" t="s">
         <v>44</v>
@@ -5663,7 +5985,7 @@
       </c>
       <c r="D90" s="99"/>
       <c r="E90" s="104" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="F90" s="110" t="s">
         <v>44</v>
@@ -5680,7 +6002,7 @@
       </c>
       <c r="D91" s="99"/>
       <c r="E91" s="104" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F91" s="110" t="s">
         <v>44</v>
@@ -5697,7 +6019,7 @@
       </c>
       <c r="D92" s="99"/>
       <c r="E92" s="104" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="F92" s="110" t="s">
         <v>44</v>
@@ -5714,7 +6036,7 @@
       </c>
       <c r="D93" s="99"/>
       <c r="E93" s="104" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="F93" s="110" t="s">
         <v>44</v>
@@ -5731,7 +6053,7 @@
       </c>
       <c r="D94" s="99"/>
       <c r="E94" s="104" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="F94" s="110" t="s">
         <v>44</v>
@@ -5748,7 +6070,7 @@
       </c>
       <c r="D95" s="99"/>
       <c r="E95" s="104" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="F95" s="110" t="s">
         <v>44</v>
@@ -5765,7 +6087,7 @@
       </c>
       <c r="D96" s="99"/>
       <c r="E96" s="104" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="F96" s="110" t="s">
         <v>44</v>
@@ -5782,7 +6104,7 @@
       </c>
       <c r="D97" s="99"/>
       <c r="E97" s="104" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="F97" s="110" t="s">
         <v>44</v>
@@ -5799,7 +6121,7 @@
       </c>
       <c r="D98" s="99"/>
       <c r="E98" s="104" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="F98" s="110" t="s">
         <v>44</v>
@@ -5816,7 +6138,7 @@
       </c>
       <c r="D99" s="99"/>
       <c r="E99" s="104" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="F99" s="110" t="s">
         <v>44</v>
@@ -5833,7 +6155,7 @@
       </c>
       <c r="D100" s="99"/>
       <c r="E100" s="104" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="F100" s="110" t="s">
         <v>44</v>
@@ -5850,7 +6172,7 @@
       </c>
       <c r="D101" s="99"/>
       <c r="E101" s="104" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="F101" s="110" t="s">
         <v>44</v>
@@ -5867,7 +6189,7 @@
       </c>
       <c r="D102" s="99"/>
       <c r="E102" s="104" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="F102" s="110" t="s">
         <v>44</v>
@@ -5884,7 +6206,7 @@
       </c>
       <c r="D103" s="99"/>
       <c r="E103" s="104" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="F103" s="110" t="s">
         <v>44</v>
@@ -5901,7 +6223,7 @@
       </c>
       <c r="D104" s="99"/>
       <c r="E104" s="104" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="F104" s="110" t="s">
         <v>44</v>
@@ -5918,7 +6240,7 @@
       </c>
       <c r="D105" s="99"/>
       <c r="E105" s="104" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="F105" s="110" t="s">
         <v>44</v>
@@ -5935,7 +6257,7 @@
       </c>
       <c r="D106" s="99"/>
       <c r="E106" s="104" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="F106" s="110" t="s">
         <v>44</v>
@@ -5952,7 +6274,7 @@
       </c>
       <c r="D107" s="99"/>
       <c r="E107" s="104" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="F107" s="110" t="s">
         <v>44</v>
@@ -5969,7 +6291,7 @@
       </c>
       <c r="D108" s="99"/>
       <c r="E108" s="104" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="F108" s="110" t="s">
         <v>44</v>
@@ -5986,7 +6308,7 @@
       </c>
       <c r="D109" s="99"/>
       <c r="E109" s="104" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="F109" s="110" t="s">
         <v>44</v>
@@ -6003,7 +6325,7 @@
       </c>
       <c r="D110" s="99"/>
       <c r="E110" s="104" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="F110" s="110" t="s">
         <v>44</v>
@@ -6020,7 +6342,7 @@
       </c>
       <c r="D111" s="99"/>
       <c r="E111" s="104" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="F111" s="110" t="s">
         <v>44</v>
@@ -6037,7 +6359,7 @@
       </c>
       <c r="D112" s="99"/>
       <c r="E112" s="104" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="F112" s="110" t="s">
         <v>44</v>
@@ -6054,7 +6376,7 @@
       </c>
       <c r="D113" s="99"/>
       <c r="E113" s="104" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="F113" s="110" t="s">
         <v>44</v>
@@ -6062,57 +6384,105 @@
       <c r="G113" s="99"/>
       <c r="H113" s="105"/>
     </row>
-    <row r="114" spans="2:8" s="33" customFormat="1">
-      <c r="B114" s="118"/>
-      <c r="C114" s="119"/>
+    <row r="114" spans="2:8" s="33" customFormat="1" ht="25.5">
+      <c r="B114" s="118">
+        <v>45768</v>
+      </c>
+      <c r="C114" s="119" t="s">
+        <v>103</v>
+      </c>
       <c r="D114" s="99"/>
-      <c r="E114" s="104"/>
-      <c r="F114" s="120"/>
+      <c r="E114" s="104" t="s">
+        <v>120</v>
+      </c>
+      <c r="F114" s="110" t="s">
+        <v>44</v>
+      </c>
       <c r="G114" s="99"/>
       <c r="H114" s="105"/>
     </row>
-    <row r="115" spans="2:8" s="33" customFormat="1">
-      <c r="B115" s="118"/>
-      <c r="C115" s="119"/>
+    <row r="115" spans="2:8" s="33" customFormat="1" ht="25.5">
+      <c r="B115" s="118">
+        <v>45768</v>
+      </c>
+      <c r="C115" s="119" t="s">
+        <v>40</v>
+      </c>
       <c r="D115" s="99"/>
-      <c r="E115" s="104"/>
-      <c r="F115" s="120"/>
+      <c r="E115" s="104" t="s">
+        <v>305</v>
+      </c>
+      <c r="F115" s="110" t="s">
+        <v>44</v>
+      </c>
       <c r="G115" s="99"/>
       <c r="H115" s="105"/>
     </row>
-    <row r="116" spans="2:8" s="33" customFormat="1">
-      <c r="B116" s="118"/>
-      <c r="C116" s="119"/>
+    <row r="116" spans="2:8" s="33" customFormat="1" ht="25.5">
+      <c r="B116" s="118">
+        <v>45768</v>
+      </c>
+      <c r="C116" s="119" t="s">
+        <v>40</v>
+      </c>
       <c r="D116" s="99"/>
-      <c r="E116" s="104"/>
-      <c r="F116" s="120"/>
+      <c r="E116" s="104" t="s">
+        <v>306</v>
+      </c>
+      <c r="F116" s="110" t="s">
+        <v>44</v>
+      </c>
       <c r="G116" s="99"/>
       <c r="H116" s="105"/>
     </row>
-    <row r="117" spans="2:8" s="33" customFormat="1">
-      <c r="B117" s="118"/>
-      <c r="C117" s="119"/>
+    <row r="117" spans="2:8" s="33" customFormat="1" ht="25.5">
+      <c r="B117" s="118">
+        <v>45768</v>
+      </c>
+      <c r="C117" s="119" t="s">
+        <v>103</v>
+      </c>
       <c r="D117" s="99"/>
-      <c r="E117" s="104"/>
-      <c r="F117" s="120"/>
+      <c r="E117" s="104" t="s">
+        <v>307</v>
+      </c>
+      <c r="F117" s="110" t="s">
+        <v>44</v>
+      </c>
       <c r="G117" s="99"/>
       <c r="H117" s="105"/>
     </row>
     <row r="118" spans="2:8" s="33" customFormat="1">
-      <c r="B118" s="118"/>
-      <c r="C118" s="119"/>
+      <c r="B118" s="118">
+        <v>45768</v>
+      </c>
+      <c r="C118" s="119" t="s">
+        <v>40</v>
+      </c>
       <c r="D118" s="99"/>
-      <c r="E118" s="104"/>
-      <c r="F118" s="120"/>
+      <c r="E118" s="104" t="s">
+        <v>311</v>
+      </c>
+      <c r="F118" s="110" t="s">
+        <v>44</v>
+      </c>
       <c r="G118" s="99"/>
       <c r="H118" s="105"/>
     </row>
     <row r="119" spans="2:8" s="33" customFormat="1">
-      <c r="B119" s="118"/>
-      <c r="C119" s="119"/>
+      <c r="B119" s="118">
+        <v>45768</v>
+      </c>
+      <c r="C119" s="119" t="s">
+        <v>103</v>
+      </c>
       <c r="D119" s="99"/>
-      <c r="E119" s="104"/>
-      <c r="F119" s="120"/>
+      <c r="E119" s="104" t="s">
+        <v>312</v>
+      </c>
+      <c r="F119" s="110" t="s">
+        <v>44</v>
+      </c>
       <c r="G119" s="99"/>
       <c r="H119" s="105"/>
     </row>
@@ -6374,7 +6744,7 @@
     <oddFooter>&amp;L&amp;"Tahoma,Regular"&amp;8 02ae-BM/PM/HDCV/FSOFT v1/0&amp;R&amp;"Tahoma,Regular"&amp;10&amp;P/&amp;N</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="C12:C28 C41 C34:C40 C42:C47 C48:C49 C51:C53 C50 C54:C57 C58:C60 C29:C33 C61:C83 C84:C92 C93:C94 C95:C102 C103:C105 C106:C110 C111:C113" numberStoredAsText="1"/>
+    <ignoredError sqref="C12:C28 C41 C34:C40 C42:C47 C48:C49 C51:C53 C50 C54:C57 C58:C60 C29:C33 C61:C83 C84:C92 C93:C94 C95:C102 C103:C105 C106:C110 C111:C113 C118 C115:C116 C114 C117 C119" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -6386,8 +6756,8 @@
   </sheetPr>
   <dimension ref="A1:K99"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A54" zoomScale="69" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56:B57"/>
+    <sheetView showGridLines="0" topLeftCell="A40" zoomScale="69" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" outlineLevelRow="1"/>
@@ -6406,9 +6776,9 @@
       <c r="A1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="144"/>
-      <c r="C1" s="144"/>
-      <c r="D1" s="144"/>
+      <c r="B1" s="152"/>
+      <c r="C1" s="152"/>
+      <c r="D1" s="152"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -6419,9 +6789,9 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="145"/>
-      <c r="C2" s="145"/>
-      <c r="D2" s="145"/>
+      <c r="B2" s="153"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -6442,43 +6812,43 @@
       <c r="E3" s="60"/>
       <c r="F3" s="60"/>
       <c r="G3" s="60"/>
-      <c r="H3" s="154"/>
-      <c r="I3" s="154"/>
-      <c r="J3" s="154"/>
+      <c r="H3" s="160"/>
+      <c r="I3" s="160"/>
+      <c r="J3" s="160"/>
       <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="12.75">
       <c r="A4" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="156" t="s">
+      <c r="B4" s="161" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="157"/>
-      <c r="D4" s="158"/>
+      <c r="C4" s="162"/>
+      <c r="D4" s="163"/>
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
       <c r="G4" s="60"/>
-      <c r="H4" s="154"/>
-      <c r="I4" s="154"/>
-      <c r="J4" s="154"/>
+      <c r="H4" s="160"/>
+      <c r="I4" s="160"/>
+      <c r="J4" s="160"/>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" s="70" customFormat="1" ht="25.5">
       <c r="A5" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="147" t="s">
+      <c r="B5" s="155" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="148"/>
-      <c r="D5" s="149"/>
+      <c r="C5" s="156"/>
+      <c r="D5" s="157"/>
       <c r="E5" s="68"/>
       <c r="F5" s="68"/>
       <c r="G5" s="68"/>
-      <c r="H5" s="153"/>
-      <c r="I5" s="153"/>
-      <c r="J5" s="153"/>
+      <c r="H5" s="159"/>
+      <c r="I5" s="159"/>
+      <c r="J5" s="159"/>
       <c r="K5" s="69"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
@@ -6487,7 +6857,7 @@
       </c>
       <c r="B6" s="79">
         <f>COUNTIF(I12:I42,"Pass")</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>39</v>
@@ -6499,9 +6869,9 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="154"/>
-      <c r="I6" s="154"/>
-      <c r="J6" s="154"/>
+      <c r="H6" s="160"/>
+      <c r="I6" s="160"/>
+      <c r="J6" s="160"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -6522,16 +6892,16 @@
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
       <c r="G7" s="61"/>
-      <c r="H7" s="154"/>
-      <c r="I7" s="154"/>
-      <c r="J7" s="154"/>
+      <c r="H7" s="160"/>
+      <c r="I7" s="160"/>
+      <c r="J7" s="160"/>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="146"/>
-      <c r="B8" s="146"/>
-      <c r="C8" s="146"/>
-      <c r="D8" s="146"/>
+      <c r="A8" s="154"/>
+      <c r="B8" s="154"/>
+      <c r="C8" s="154"/>
+      <c r="D8" s="154"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -6541,70 +6911,70 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" s="72" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="163" t="s">
+      <c r="A9" s="138" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="164" t="s">
+      <c r="B9" s="167" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="163" t="s">
+      <c r="C9" s="138" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="168" t="s">
+      <c r="D9" s="139" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="169"/>
-      <c r="F9" s="169"/>
-      <c r="G9" s="170"/>
-      <c r="H9" s="159" t="s">
+      <c r="E9" s="140"/>
+      <c r="F9" s="140"/>
+      <c r="G9" s="141"/>
+      <c r="H9" s="164" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="155" t="s">
+      <c r="I9" s="133" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="155" t="s">
+      <c r="J9" s="133" t="s">
         <v>32</v>
       </c>
       <c r="K9" s="71"/>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="155"/>
-      <c r="B10" s="165"/>
-      <c r="C10" s="155"/>
-      <c r="D10" s="160"/>
-      <c r="E10" s="171"/>
-      <c r="F10" s="171"/>
-      <c r="G10" s="172"/>
-      <c r="H10" s="160"/>
-      <c r="I10" s="155"/>
-      <c r="J10" s="155"/>
+      <c r="A10" s="133"/>
+      <c r="B10" s="168"/>
+      <c r="C10" s="133"/>
+      <c r="D10" s="142"/>
+      <c r="E10" s="143"/>
+      <c r="F10" s="143"/>
+      <c r="G10" s="144"/>
+      <c r="H10" s="142"/>
+      <c r="I10" s="133"/>
+      <c r="J10" s="133"/>
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" s="73" customFormat="1" ht="15">
-      <c r="A11" s="161"/>
-      <c r="B11" s="161"/>
-      <c r="C11" s="161"/>
-      <c r="D11" s="161"/>
-      <c r="E11" s="161"/>
-      <c r="F11" s="161"/>
-      <c r="G11" s="161"/>
-      <c r="H11" s="161"/>
-      <c r="I11" s="161"/>
-      <c r="J11" s="162"/>
+      <c r="A11" s="165"/>
+      <c r="B11" s="165"/>
+      <c r="C11" s="165"/>
+      <c r="D11" s="165"/>
+      <c r="E11" s="165"/>
+      <c r="F11" s="165"/>
+      <c r="G11" s="165"/>
+      <c r="H11" s="165"/>
+      <c r="I11" s="165"/>
+      <c r="J11" s="166"/>
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A12" s="150" t="s">
+      <c r="A12" s="145" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="151"/>
-      <c r="C12" s="151"/>
-      <c r="D12" s="151"/>
-      <c r="E12" s="151"/>
-      <c r="F12" s="151"/>
-      <c r="G12" s="151"/>
-      <c r="H12" s="151"/>
-      <c r="I12" s="151"/>
-      <c r="J12" s="152"/>
+      <c r="B12" s="146"/>
+      <c r="C12" s="146"/>
+      <c r="D12" s="146"/>
+      <c r="E12" s="146"/>
+      <c r="F12" s="146"/>
+      <c r="G12" s="146"/>
+      <c r="H12" s="146"/>
+      <c r="I12" s="146"/>
+      <c r="J12" s="158"/>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" ht="350.1" customHeight="1" outlineLevel="1">
       <c r="A13" s="77" t="s">
@@ -6614,11 +6984,11 @@
         <v>47</v>
       </c>
       <c r="C13" s="76" t="s">
-        <v>200</v>
-      </c>
-      <c r="D13" s="138"/>
-      <c r="E13" s="139"/>
-      <c r="F13" s="139"/>
+        <v>195</v>
+      </c>
+      <c r="D13" s="131"/>
+      <c r="E13" s="132"/>
+      <c r="F13" s="132"/>
       <c r="G13" s="75"/>
       <c r="H13" s="116">
         <v>45755</v>
@@ -6633,14 +7003,14 @@
         <v>1</v>
       </c>
       <c r="B14" s="81" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C14" s="76" t="s">
-        <v>199</v>
-      </c>
-      <c r="D14" s="138"/>
-      <c r="E14" s="139"/>
-      <c r="F14" s="139"/>
+        <v>194</v>
+      </c>
+      <c r="D14" s="131"/>
+      <c r="E14" s="132"/>
+      <c r="F14" s="132"/>
       <c r="G14" s="75"/>
       <c r="H14" s="116">
         <v>45755</v>
@@ -6655,14 +7025,14 @@
         <v>2</v>
       </c>
       <c r="B15" s="81" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C15" s="76" t="s">
-        <v>198</v>
-      </c>
-      <c r="D15" s="138"/>
-      <c r="E15" s="139"/>
-      <c r="F15" s="139"/>
+        <v>193</v>
+      </c>
+      <c r="D15" s="131"/>
+      <c r="E15" s="132"/>
+      <c r="F15" s="132"/>
       <c r="G15" s="75"/>
       <c r="H15" s="116">
         <v>45755</v>
@@ -6671,7 +7041,7 @@
         <v>3</v>
       </c>
       <c r="J15" s="74" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="4" customFormat="1" ht="150" customHeight="1" outlineLevel="1">
@@ -6682,11 +7052,11 @@
         <v>75</v>
       </c>
       <c r="C16" s="76" t="s">
-        <v>197</v>
-      </c>
-      <c r="D16" s="138"/>
-      <c r="E16" s="139"/>
-      <c r="F16" s="139"/>
+        <v>192</v>
+      </c>
+      <c r="D16" s="131"/>
+      <c r="E16" s="132"/>
+      <c r="F16" s="132"/>
       <c r="G16" s="75"/>
       <c r="H16" s="116">
         <v>45755</v>
@@ -6704,11 +7074,11 @@
         <v>76</v>
       </c>
       <c r="C17" s="76" t="s">
-        <v>196</v>
-      </c>
-      <c r="D17" s="138"/>
-      <c r="E17" s="139"/>
-      <c r="F17" s="139"/>
+        <v>191</v>
+      </c>
+      <c r="D17" s="131"/>
+      <c r="E17" s="132"/>
+      <c r="F17" s="132"/>
       <c r="G17" s="75"/>
       <c r="H17" s="116">
         <v>45755</v>
@@ -6723,14 +7093,14 @@
         <v>53</v>
       </c>
       <c r="B18" s="92" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C18" s="86" t="s">
-        <v>195</v>
-      </c>
-      <c r="D18" s="138"/>
-      <c r="E18" s="139"/>
-      <c r="F18" s="139"/>
+        <v>190</v>
+      </c>
+      <c r="D18" s="131"/>
+      <c r="E18" s="132"/>
+      <c r="F18" s="132"/>
       <c r="G18" s="75"/>
       <c r="H18" s="116">
         <v>45755</v>
@@ -6739,7 +7109,7 @@
         <v>3</v>
       </c>
       <c r="J18" s="74" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="150" customHeight="1" outlineLevel="1">
@@ -6747,14 +7117,14 @@
         <v>55</v>
       </c>
       <c r="B19" s="85" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C19" s="86" t="s">
-        <v>194</v>
-      </c>
-      <c r="D19" s="138"/>
-      <c r="E19" s="139"/>
-      <c r="F19" s="139"/>
+        <v>189</v>
+      </c>
+      <c r="D19" s="131"/>
+      <c r="E19" s="132"/>
+      <c r="F19" s="132"/>
       <c r="G19" s="75"/>
       <c r="H19" s="116">
         <v>45755</v>
@@ -6763,7 +7133,7 @@
         <v>38</v>
       </c>
       <c r="J19" s="74" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="4" customFormat="1" ht="200.1" customHeight="1" outlineLevel="1">
@@ -6771,14 +7141,14 @@
         <v>67</v>
       </c>
       <c r="B20" s="85" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C20" s="76" t="s">
-        <v>192</v>
-      </c>
-      <c r="D20" s="138"/>
-      <c r="E20" s="139"/>
-      <c r="F20" s="139"/>
+        <v>187</v>
+      </c>
+      <c r="D20" s="131"/>
+      <c r="E20" s="132"/>
+      <c r="F20" s="132"/>
       <c r="G20" s="75"/>
       <c r="H20" s="116">
         <v>45755</v>
@@ -6787,7 +7157,7 @@
         <v>3</v>
       </c>
       <c r="J20" s="74" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="4" customFormat="1" ht="200.1" customHeight="1" outlineLevel="1">
@@ -6795,14 +7165,14 @@
         <v>78</v>
       </c>
       <c r="B21" s="85" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C21" s="76" t="s">
-        <v>191</v>
-      </c>
-      <c r="D21" s="138"/>
-      <c r="E21" s="139"/>
-      <c r="F21" s="139"/>
+        <v>186</v>
+      </c>
+      <c r="D21" s="131"/>
+      <c r="E21" s="132"/>
+      <c r="F21" s="132"/>
       <c r="G21" s="75"/>
       <c r="H21" s="116">
         <v>45755</v>
@@ -6811,7 +7181,7 @@
         <v>3</v>
       </c>
       <c r="J21" s="74" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="4" customFormat="1" ht="150" customHeight="1" outlineLevel="1">
@@ -6819,14 +7189,14 @@
         <v>79</v>
       </c>
       <c r="B22" s="85" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C22" s="86" t="s">
-        <v>193</v>
-      </c>
-      <c r="D22" s="138"/>
-      <c r="E22" s="139"/>
-      <c r="F22" s="139"/>
+        <v>188</v>
+      </c>
+      <c r="D22" s="131"/>
+      <c r="E22" s="132"/>
+      <c r="F22" s="132"/>
       <c r="G22" s="75"/>
       <c r="H22" s="116">
         <v>45755</v>
@@ -6835,15 +7205,15 @@
         <v>38</v>
       </c>
       <c r="J22" s="74" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A23" s="150" t="s">
+      <c r="A23" s="145" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="151"/>
-      <c r="C23" s="151"/>
+      <c r="B23" s="146"/>
+      <c r="C23" s="146"/>
       <c r="D23" s="87"/>
       <c r="E23" s="87"/>
       <c r="F23" s="87"/>
@@ -6860,11 +7230,11 @@
         <v>59</v>
       </c>
       <c r="C24" s="86" t="s">
-        <v>228</v>
-      </c>
-      <c r="D24" s="166"/>
-      <c r="E24" s="167"/>
-      <c r="F24" s="167"/>
+        <v>223</v>
+      </c>
+      <c r="D24" s="136"/>
+      <c r="E24" s="137"/>
+      <c r="F24" s="137"/>
       <c r="G24" s="94"/>
       <c r="H24" s="115">
         <v>45756</v>
@@ -6879,14 +7249,14 @@
         <v>1</v>
       </c>
       <c r="B25" s="85" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C25" s="86" t="s">
-        <v>227</v>
-      </c>
-      <c r="D25" s="166"/>
-      <c r="E25" s="167"/>
-      <c r="F25" s="167"/>
+        <v>222</v>
+      </c>
+      <c r="D25" s="136"/>
+      <c r="E25" s="137"/>
+      <c r="F25" s="137"/>
       <c r="G25" s="94"/>
       <c r="H25" s="115">
         <v>45755</v>
@@ -6895,7 +7265,7 @@
         <v>38</v>
       </c>
       <c r="J25" s="96" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="4" customFormat="1" ht="150" customHeight="1" outlineLevel="1">
@@ -6906,11 +7276,11 @@
         <v>68</v>
       </c>
       <c r="C26" s="86" t="s">
-        <v>232</v>
-      </c>
-      <c r="D26" s="131"/>
-      <c r="E26" s="132"/>
-      <c r="F26" s="132"/>
+        <v>227</v>
+      </c>
+      <c r="D26" s="147"/>
+      <c r="E26" s="148"/>
+      <c r="F26" s="148"/>
       <c r="G26" s="94"/>
       <c r="H26" s="115">
         <v>45756</v>
@@ -6925,14 +7295,14 @@
         <v>49</v>
       </c>
       <c r="B27" s="85" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C27" s="86" t="s">
-        <v>233</v>
-      </c>
-      <c r="D27" s="135"/>
-      <c r="E27" s="136"/>
-      <c r="F27" s="137"/>
+        <v>228</v>
+      </c>
+      <c r="D27" s="149"/>
+      <c r="E27" s="150"/>
+      <c r="F27" s="151"/>
       <c r="G27" s="94"/>
       <c r="H27" s="115">
         <v>45755</v>
@@ -6947,14 +7317,14 @@
         <v>52</v>
       </c>
       <c r="B28" s="85" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C28" s="86" t="s">
-        <v>237</v>
-      </c>
-      <c r="D28" s="135"/>
-      <c r="E28" s="136"/>
-      <c r="F28" s="137"/>
+        <v>232</v>
+      </c>
+      <c r="D28" s="149"/>
+      <c r="E28" s="150"/>
+      <c r="F28" s="151"/>
       <c r="G28" s="94"/>
       <c r="H28" s="115">
         <v>45756</v>
@@ -6963,7 +7333,7 @@
         <v>3</v>
       </c>
       <c r="J28" s="96" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="4" customFormat="1" ht="150" customHeight="1" outlineLevel="1">
@@ -6971,14 +7341,14 @@
         <v>53</v>
       </c>
       <c r="B29" s="85" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C29" s="86" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="135"/>
-      <c r="E29" s="136"/>
-      <c r="F29" s="137"/>
+      <c r="D29" s="149"/>
+      <c r="E29" s="150"/>
+      <c r="F29" s="151"/>
       <c r="G29" s="94"/>
       <c r="H29" s="115">
         <v>45756</v>
@@ -6987,7 +7357,7 @@
         <v>3</v>
       </c>
       <c r="J29" s="96" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="4" customFormat="1" ht="150" customHeight="1" outlineLevel="1">
@@ -6998,11 +7368,11 @@
         <v>69</v>
       </c>
       <c r="C30" s="86" t="s">
-        <v>234</v>
-      </c>
-      <c r="D30" s="135"/>
-      <c r="E30" s="136"/>
-      <c r="F30" s="137"/>
+        <v>229</v>
+      </c>
+      <c r="D30" s="149"/>
+      <c r="E30" s="150"/>
+      <c r="F30" s="151"/>
       <c r="G30" s="94"/>
       <c r="H30" s="115">
         <v>45755</v>
@@ -7022,9 +7392,9 @@
       <c r="C31" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="135"/>
-      <c r="E31" s="136"/>
-      <c r="F31" s="137"/>
+      <c r="D31" s="149"/>
+      <c r="E31" s="150"/>
+      <c r="F31" s="151"/>
       <c r="G31" s="94"/>
       <c r="H31" s="115">
         <v>45756</v>
@@ -7033,7 +7403,7 @@
         <v>3</v>
       </c>
       <c r="J31" s="96" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="4" customFormat="1" ht="150" customHeight="1" outlineLevel="1">
@@ -7046,9 +7416,9 @@
       <c r="C32" s="86" t="s">
         <v>70</v>
       </c>
-      <c r="D32" s="135"/>
-      <c r="E32" s="136"/>
-      <c r="F32" s="137"/>
+      <c r="D32" s="149"/>
+      <c r="E32" s="150"/>
+      <c r="F32" s="151"/>
       <c r="G32" s="94"/>
       <c r="H32" s="115">
         <v>45756</v>
@@ -7057,7 +7427,7 @@
         <v>3</v>
       </c>
       <c r="J32" s="96" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="33" spans="1:10" s="4" customFormat="1" ht="150" customHeight="1" outlineLevel="1">
@@ -7068,11 +7438,11 @@
         <v>57</v>
       </c>
       <c r="C33" s="86" t="s">
-        <v>241</v>
-      </c>
-      <c r="D33" s="138"/>
-      <c r="E33" s="139"/>
-      <c r="F33" s="140"/>
+        <v>236</v>
+      </c>
+      <c r="D33" s="131"/>
+      <c r="E33" s="132"/>
+      <c r="F33" s="169"/>
       <c r="G33" s="94"/>
       <c r="H33" s="115">
         <v>45755</v>
@@ -7090,11 +7460,11 @@
         <v>56</v>
       </c>
       <c r="C34" s="86" t="s">
-        <v>201</v>
-      </c>
-      <c r="D34" s="141"/>
-      <c r="E34" s="142"/>
-      <c r="F34" s="143"/>
+        <v>196</v>
+      </c>
+      <c r="D34" s="170"/>
+      <c r="E34" s="171"/>
+      <c r="F34" s="172"/>
       <c r="G34" s="94"/>
       <c r="H34" s="115">
         <v>45755</v>
@@ -7105,11 +7475,11 @@
       <c r="J34" s="96"/>
     </row>
     <row r="35" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A35" s="150" t="s">
+      <c r="A35" s="145" t="s">
         <v>71</v>
       </c>
-      <c r="B35" s="151"/>
-      <c r="C35" s="151"/>
+      <c r="B35" s="146"/>
+      <c r="C35" s="146"/>
       <c r="D35" s="87"/>
       <c r="E35" s="87"/>
       <c r="F35" s="87"/>
@@ -7128,20 +7498,20 @@
       <c r="C36" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="D36" s="131"/>
-      <c r="E36" s="132"/>
-      <c r="F36" s="132"/>
+      <c r="D36" s="147"/>
+      <c r="E36" s="148"/>
+      <c r="F36" s="148"/>
       <c r="G36" s="75"/>
       <c r="H36" s="82"/>
       <c r="I36" s="76"/>
       <c r="J36" s="74"/>
     </row>
     <row r="37" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A37" s="133" t="s">
+      <c r="A37" s="134" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="134"/>
-      <c r="C37" s="134"/>
+      <c r="B37" s="135"/>
+      <c r="C37" s="135"/>
       <c r="D37" s="97"/>
       <c r="E37" s="97"/>
       <c r="F37" s="97"/>
@@ -7150,7 +7520,7 @@
       <c r="I37" s="97"/>
       <c r="J37" s="98"/>
     </row>
-    <row r="38" spans="1:10" s="4" customFormat="1" ht="116.25" customHeight="1" outlineLevel="1">
+    <row r="38" spans="1:10" s="4" customFormat="1" ht="300" customHeight="1" outlineLevel="1">
       <c r="A38" s="77" t="s">
         <v>0</v>
       </c>
@@ -7158,17 +7528,21 @@
         <v>110</v>
       </c>
       <c r="C38" s="76" t="s">
-        <v>113</v>
-      </c>
-      <c r="D38" s="131"/>
-      <c r="E38" s="132"/>
-      <c r="F38" s="132"/>
+        <v>304</v>
+      </c>
+      <c r="D38" s="147"/>
+      <c r="E38" s="148"/>
+      <c r="F38" s="148"/>
       <c r="G38" s="75"/>
-      <c r="H38" s="82"/>
-      <c r="I38" s="76"/>
+      <c r="H38" s="175">
+        <v>45768</v>
+      </c>
+      <c r="I38" s="76" t="s">
+        <v>38</v>
+      </c>
       <c r="J38" s="74"/>
     </row>
-    <row r="39" spans="1:10" s="4" customFormat="1" ht="67.5" customHeight="1" outlineLevel="1">
+    <row r="39" spans="1:10" s="4" customFormat="1" ht="200.1" customHeight="1" outlineLevel="1">
       <c r="A39" s="77" t="s">
         <v>1</v>
       </c>
@@ -7176,17 +7550,23 @@
         <v>111</v>
       </c>
       <c r="C39" s="76" t="s">
-        <v>115</v>
-      </c>
-      <c r="D39" s="131"/>
-      <c r="E39" s="132"/>
-      <c r="F39" s="132"/>
+        <v>308</v>
+      </c>
+      <c r="D39" s="147"/>
+      <c r="E39" s="148"/>
+      <c r="F39" s="148"/>
       <c r="G39" s="75"/>
-      <c r="H39" s="82"/>
-      <c r="I39" s="76"/>
-      <c r="J39" s="74"/>
-    </row>
-    <row r="40" spans="1:10" s="4" customFormat="1" ht="81" customHeight="1" outlineLevel="1">
+      <c r="H39" s="175">
+        <v>45768</v>
+      </c>
+      <c r="I39" s="76" t="s">
+        <v>38</v>
+      </c>
+      <c r="J39" s="74" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" s="4" customFormat="1" ht="200.1" customHeight="1" outlineLevel="1">
       <c r="A40" s="77" t="s">
         <v>2</v>
       </c>
@@ -7194,14 +7574,18 @@
         <v>112</v>
       </c>
       <c r="C40" s="76" t="s">
-        <v>114</v>
-      </c>
-      <c r="D40" s="131"/>
-      <c r="E40" s="132"/>
-      <c r="F40" s="132"/>
+        <v>310</v>
+      </c>
+      <c r="D40" s="147"/>
+      <c r="E40" s="148"/>
+      <c r="F40" s="148"/>
       <c r="G40" s="75"/>
-      <c r="H40" s="82"/>
-      <c r="I40" s="76"/>
+      <c r="H40" s="175">
+        <v>45768</v>
+      </c>
+      <c r="I40" s="76" t="s">
+        <v>38</v>
+      </c>
       <c r="J40" s="74"/>
     </row>
     <row r="41" spans="1:10" s="4" customFormat="1" ht="93" customHeight="1" outlineLevel="1">
@@ -7209,43 +7593,47 @@
         <v>49</v>
       </c>
       <c r="B41" s="92" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C41" s="76" t="s">
-        <v>117</v>
-      </c>
-      <c r="D41" s="131"/>
-      <c r="E41" s="132"/>
-      <c r="F41" s="132"/>
+        <v>313</v>
+      </c>
+      <c r="D41" s="147"/>
+      <c r="E41" s="148"/>
+      <c r="F41" s="148"/>
       <c r="G41" s="75"/>
       <c r="H41" s="82"/>
       <c r="I41" s="76"/>
       <c r="J41" s="74"/>
     </row>
-    <row r="42" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+    <row r="42" spans="1:10" s="4" customFormat="1" ht="200.1" customHeight="1" outlineLevel="1">
       <c r="A42" s="77" t="s">
         <v>52</v>
       </c>
       <c r="B42" s="92" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C42" s="76" t="s">
-        <v>119</v>
-      </c>
-      <c r="D42" s="131"/>
-      <c r="E42" s="132"/>
-      <c r="F42" s="132"/>
+        <v>314</v>
+      </c>
+      <c r="D42" s="147"/>
+      <c r="E42" s="148"/>
+      <c r="F42" s="148"/>
       <c r="G42" s="75"/>
-      <c r="H42" s="82"/>
-      <c r="I42" s="76"/>
+      <c r="H42" s="175">
+        <v>45768</v>
+      </c>
+      <c r="I42" s="76" t="s">
+        <v>38</v>
+      </c>
       <c r="J42" s="74"/>
     </row>
     <row r="43" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A43" s="133" t="s">
+      <c r="A43" s="134" t="s">
         <v>88</v>
       </c>
-      <c r="B43" s="134"/>
-      <c r="C43" s="134"/>
+      <c r="B43" s="135"/>
+      <c r="C43" s="135"/>
       <c r="D43" s="97"/>
       <c r="E43" s="97"/>
       <c r="F43" s="97"/>
@@ -7264,9 +7652,9 @@
       <c r="C44" s="76" t="s">
         <v>95</v>
       </c>
-      <c r="D44" s="131"/>
-      <c r="E44" s="132"/>
-      <c r="F44" s="132"/>
+      <c r="D44" s="147"/>
+      <c r="E44" s="148"/>
+      <c r="F44" s="148"/>
       <c r="G44" s="75"/>
       <c r="H44" s="82"/>
       <c r="I44" s="76"/>
@@ -7282,9 +7670,9 @@
       <c r="C45" s="76" t="s">
         <v>96</v>
       </c>
-      <c r="D45" s="131"/>
-      <c r="E45" s="132"/>
-      <c r="F45" s="132"/>
+      <c r="D45" s="147"/>
+      <c r="E45" s="148"/>
+      <c r="F45" s="148"/>
       <c r="G45" s="75"/>
       <c r="H45" s="82"/>
       <c r="I45" s="76"/>
@@ -7300,9 +7688,9 @@
       <c r="C46" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="D46" s="131"/>
-      <c r="E46" s="132"/>
-      <c r="F46" s="132"/>
+      <c r="D46" s="147"/>
+      <c r="E46" s="148"/>
+      <c r="F46" s="148"/>
       <c r="G46" s="75"/>
       <c r="H46" s="82"/>
       <c r="I46" s="76"/>
@@ -7318,9 +7706,9 @@
       <c r="C47" s="76" t="s">
         <v>98</v>
       </c>
-      <c r="D47" s="131"/>
-      <c r="E47" s="132"/>
-      <c r="F47" s="132"/>
+      <c r="D47" s="147"/>
+      <c r="E47" s="148"/>
+      <c r="F47" s="148"/>
       <c r="G47" s="75"/>
       <c r="H47" s="82"/>
       <c r="I47" s="76"/>
@@ -7336,9 +7724,9 @@
       <c r="C48" s="76" t="s">
         <v>100</v>
       </c>
-      <c r="D48" s="131"/>
-      <c r="E48" s="132"/>
-      <c r="F48" s="132"/>
+      <c r="D48" s="147"/>
+      <c r="E48" s="148"/>
+      <c r="F48" s="148"/>
       <c r="G48" s="75"/>
       <c r="H48" s="82"/>
       <c r="I48" s="76"/>
@@ -7354,20 +7742,20 @@
       <c r="C49" s="76" t="s">
         <v>92</v>
       </c>
-      <c r="D49" s="131"/>
-      <c r="E49" s="132"/>
-      <c r="F49" s="132"/>
+      <c r="D49" s="147"/>
+      <c r="E49" s="148"/>
+      <c r="F49" s="148"/>
       <c r="G49" s="75"/>
       <c r="H49" s="82"/>
       <c r="I49" s="76"/>
       <c r="J49" s="74"/>
     </row>
     <row r="50" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A50" s="133" t="s">
+      <c r="A50" s="134" t="s">
         <v>101</v>
       </c>
-      <c r="B50" s="134"/>
-      <c r="C50" s="134"/>
+      <c r="B50" s="135"/>
+      <c r="C50" s="135"/>
       <c r="D50" s="97"/>
       <c r="E50" s="97"/>
       <c r="F50" s="97"/>
@@ -7381,25 +7769,25 @@
         <v>0</v>
       </c>
       <c r="B51" s="92" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C51" s="76" t="s">
         <v>102</v>
       </c>
-      <c r="D51" s="131"/>
-      <c r="E51" s="132"/>
-      <c r="F51" s="132"/>
+      <c r="D51" s="147"/>
+      <c r="E51" s="148"/>
+      <c r="F51" s="148"/>
       <c r="G51" s="75"/>
       <c r="H51" s="82"/>
       <c r="I51" s="76"/>
       <c r="J51" s="74"/>
     </row>
     <row r="52" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A52" s="133" t="s">
-        <v>265</v>
-      </c>
-      <c r="B52" s="134"/>
-      <c r="C52" s="134"/>
+      <c r="A52" s="134" t="s">
+        <v>260</v>
+      </c>
+      <c r="B52" s="135"/>
+      <c r="C52" s="135"/>
       <c r="D52" s="97"/>
       <c r="E52" s="97"/>
       <c r="F52" s="97"/>
@@ -7413,14 +7801,14 @@
         <v>0</v>
       </c>
       <c r="B53" s="92" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="C53" s="76" t="s">
-        <v>264</v>
-      </c>
-      <c r="D53" s="131"/>
-      <c r="E53" s="132"/>
-      <c r="F53" s="132"/>
+        <v>259</v>
+      </c>
+      <c r="D53" s="147"/>
+      <c r="E53" s="148"/>
+      <c r="F53" s="148"/>
       <c r="G53" s="75"/>
       <c r="H53" s="82"/>
       <c r="I53" s="76"/>
@@ -7431,25 +7819,25 @@
         <v>1</v>
       </c>
       <c r="B54" s="92" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C54" s="76" t="s">
-        <v>269</v>
-      </c>
-      <c r="D54" s="131"/>
-      <c r="E54" s="132"/>
-      <c r="F54" s="132"/>
+        <v>264</v>
+      </c>
+      <c r="D54" s="147"/>
+      <c r="E54" s="148"/>
+      <c r="F54" s="148"/>
       <c r="G54" s="75"/>
       <c r="H54" s="82"/>
       <c r="I54" s="76"/>
       <c r="J54" s="74"/>
     </row>
     <row r="55" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A55" s="133" t="s">
-        <v>292</v>
-      </c>
-      <c r="B55" s="134"/>
-      <c r="C55" s="134"/>
+      <c r="A55" s="134" t="s">
+        <v>287</v>
+      </c>
+      <c r="B55" s="135"/>
+      <c r="C55" s="135"/>
       <c r="D55" s="97"/>
       <c r="E55" s="97"/>
       <c r="F55" s="97"/>
@@ -7463,14 +7851,14 @@
         <v>0</v>
       </c>
       <c r="B56" s="92" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="C56" s="76" t="s">
-        <v>303</v>
-      </c>
-      <c r="D56" s="131"/>
-      <c r="E56" s="132"/>
-      <c r="F56" s="132"/>
+        <v>298</v>
+      </c>
+      <c r="D56" s="147"/>
+      <c r="E56" s="148"/>
+      <c r="F56" s="148"/>
       <c r="G56" s="75"/>
       <c r="H56" s="82"/>
       <c r="I56" s="76"/>
@@ -7481,25 +7869,25 @@
         <v>1</v>
       </c>
       <c r="B57" s="92" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="C57" s="76" t="s">
-        <v>307</v>
-      </c>
-      <c r="D57" s="131"/>
-      <c r="E57" s="132"/>
-      <c r="F57" s="132"/>
+        <v>302</v>
+      </c>
+      <c r="D57" s="147"/>
+      <c r="E57" s="148"/>
+      <c r="F57" s="148"/>
       <c r="G57" s="75"/>
       <c r="H57" s="82"/>
       <c r="I57" s="76"/>
       <c r="J57" s="74"/>
     </row>
     <row r="58" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A58" s="133" t="s">
-        <v>293</v>
-      </c>
-      <c r="B58" s="134"/>
-      <c r="C58" s="134"/>
+      <c r="A58" s="134" t="s">
+        <v>288</v>
+      </c>
+      <c r="B58" s="135"/>
+      <c r="C58" s="135"/>
       <c r="D58" s="97"/>
       <c r="E58" s="97"/>
       <c r="F58" s="97"/>
@@ -7513,14 +7901,14 @@
         <v>0</v>
       </c>
       <c r="B59" s="92" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="C59" s="76" t="s">
-        <v>295</v>
-      </c>
-      <c r="D59" s="131"/>
-      <c r="E59" s="132"/>
-      <c r="F59" s="132"/>
+        <v>290</v>
+      </c>
+      <c r="D59" s="147"/>
+      <c r="E59" s="148"/>
+      <c r="F59" s="148"/>
       <c r="G59" s="75"/>
       <c r="H59" s="82"/>
       <c r="I59" s="76"/>
@@ -7531,14 +7919,14 @@
         <v>1</v>
       </c>
       <c r="B60" s="92" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="C60" s="76" t="s">
-        <v>296</v>
-      </c>
-      <c r="D60" s="131"/>
-      <c r="E60" s="132"/>
-      <c r="F60" s="132"/>
+        <v>291</v>
+      </c>
+      <c r="D60" s="147"/>
+      <c r="E60" s="148"/>
+      <c r="F60" s="148"/>
       <c r="G60" s="75"/>
       <c r="H60" s="82"/>
       <c r="I60" s="76"/>
@@ -7549,14 +7937,14 @@
         <v>2</v>
       </c>
       <c r="B61" s="92" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="C61" s="76" t="s">
-        <v>298</v>
-      </c>
-      <c r="D61" s="131"/>
-      <c r="E61" s="132"/>
-      <c r="F61" s="132"/>
+        <v>293</v>
+      </c>
+      <c r="D61" s="147"/>
+      <c r="E61" s="148"/>
+      <c r="F61" s="148"/>
       <c r="G61" s="75"/>
       <c r="H61" s="82"/>
       <c r="I61" s="76"/>
@@ -7567,23 +7955,23 @@
         <v>49</v>
       </c>
       <c r="B62" s="92" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="C62" s="76" t="s">
-        <v>305</v>
-      </c>
-      <c r="D62" s="131"/>
-      <c r="E62" s="132"/>
-      <c r="F62" s="132"/>
+        <v>300</v>
+      </c>
+      <c r="D62" s="147"/>
+      <c r="E62" s="148"/>
+      <c r="F62" s="148"/>
       <c r="G62" s="75"/>
       <c r="H62" s="82"/>
       <c r="I62" s="76"/>
       <c r="J62" s="74"/>
     </row>
     <row r="63" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A63" s="133"/>
-      <c r="B63" s="134"/>
-      <c r="C63" s="134"/>
+      <c r="A63" s="134"/>
+      <c r="B63" s="135"/>
+      <c r="C63" s="135"/>
       <c r="D63" s="97"/>
       <c r="E63" s="97"/>
       <c r="F63" s="97"/>
@@ -7596,18 +7984,18 @@
       <c r="A64" s="77"/>
       <c r="B64" s="92"/>
       <c r="C64" s="76"/>
-      <c r="D64" s="131"/>
-      <c r="E64" s="132"/>
-      <c r="F64" s="132"/>
+      <c r="D64" s="147"/>
+      <c r="E64" s="148"/>
+      <c r="F64" s="148"/>
       <c r="G64" s="75"/>
       <c r="H64" s="82"/>
       <c r="I64" s="76"/>
       <c r="J64" s="74"/>
     </row>
     <row r="65" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A65" s="133"/>
-      <c r="B65" s="134"/>
-      <c r="C65" s="134"/>
+      <c r="A65" s="134"/>
+      <c r="B65" s="135"/>
+      <c r="C65" s="135"/>
       <c r="D65" s="97"/>
       <c r="E65" s="97"/>
       <c r="F65" s="97"/>
@@ -7620,9 +8008,9 @@
       <c r="A66" s="77"/>
       <c r="B66" s="92"/>
       <c r="C66" s="76"/>
-      <c r="D66" s="131"/>
-      <c r="E66" s="132"/>
-      <c r="F66" s="132"/>
+      <c r="D66" s="147"/>
+      <c r="E66" s="148"/>
+      <c r="F66" s="148"/>
       <c r="G66" s="75"/>
       <c r="H66" s="82"/>
       <c r="I66" s="76"/>
@@ -7770,11 +8158,58 @@
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D66:F66"/>
+    <mergeCell ref="D56:F56"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="D60:F60"/>
+    <mergeCell ref="D57:F57"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="D62:F62"/>
+    <mergeCell ref="A63:C63"/>
+    <mergeCell ref="D64:F64"/>
+    <mergeCell ref="A65:C65"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="D54:F54"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="D51:F51"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="D53:F53"/>
+    <mergeCell ref="B1:D2"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="A37:C37"/>
     <mergeCell ref="D24:F24"/>
@@ -7791,58 +8226,11 @@
     <mergeCell ref="D20:F20"/>
     <mergeCell ref="D18:F18"/>
     <mergeCell ref="D22:F22"/>
-    <mergeCell ref="B1:D2"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="D54:F54"/>
-    <mergeCell ref="A55:C55"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="D51:F51"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="D48:F48"/>
-    <mergeCell ref="D53:F53"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="D62:F62"/>
-    <mergeCell ref="A63:C63"/>
-    <mergeCell ref="D64:F64"/>
-    <mergeCell ref="A65:C65"/>
-    <mergeCell ref="D66:F66"/>
-    <mergeCell ref="D56:F56"/>
-    <mergeCell ref="D61:F61"/>
-    <mergeCell ref="D59:F59"/>
-    <mergeCell ref="D60:F60"/>
-    <mergeCell ref="D57:F57"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D17:F17"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7879,9 +8267,9 @@
       <c r="A1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="144"/>
-      <c r="C1" s="144"/>
-      <c r="D1" s="144"/>
+      <c r="B1" s="152"/>
+      <c r="C1" s="152"/>
+      <c r="D1" s="152"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -7892,9 +8280,9 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="145"/>
-      <c r="C2" s="145"/>
-      <c r="D2" s="145"/>
+      <c r="B2" s="153"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -7915,43 +8303,43 @@
       <c r="E3" s="60"/>
       <c r="F3" s="60"/>
       <c r="G3" s="60"/>
-      <c r="H3" s="154"/>
-      <c r="I3" s="154"/>
-      <c r="J3" s="154"/>
+      <c r="H3" s="160"/>
+      <c r="I3" s="160"/>
+      <c r="J3" s="160"/>
       <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="12.75">
       <c r="A4" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="156" t="s">
-        <v>126</v>
-      </c>
-      <c r="C4" s="157"/>
-      <c r="D4" s="158"/>
+      <c r="B4" s="161" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" s="162"/>
+      <c r="D4" s="163"/>
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
       <c r="G4" s="60"/>
-      <c r="H4" s="154"/>
-      <c r="I4" s="154"/>
-      <c r="J4" s="154"/>
+      <c r="H4" s="160"/>
+      <c r="I4" s="160"/>
+      <c r="J4" s="160"/>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" s="70" customFormat="1" ht="25.5">
       <c r="A5" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="147" t="s">
+      <c r="B5" s="155" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="148"/>
-      <c r="D5" s="149"/>
+      <c r="C5" s="156"/>
+      <c r="D5" s="157"/>
       <c r="E5" s="68"/>
       <c r="F5" s="68"/>
       <c r="G5" s="68"/>
-      <c r="H5" s="153"/>
-      <c r="I5" s="153"/>
-      <c r="J5" s="153"/>
+      <c r="H5" s="159"/>
+      <c r="I5" s="159"/>
+      <c r="J5" s="159"/>
       <c r="K5" s="69"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
@@ -7972,9 +8360,9 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="154"/>
-      <c r="I6" s="154"/>
-      <c r="J6" s="154"/>
+      <c r="H6" s="160"/>
+      <c r="I6" s="160"/>
+      <c r="J6" s="160"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -7995,16 +8383,16 @@
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
       <c r="G7" s="61"/>
-      <c r="H7" s="154"/>
-      <c r="I7" s="154"/>
-      <c r="J7" s="154"/>
+      <c r="H7" s="160"/>
+      <c r="I7" s="160"/>
+      <c r="J7" s="160"/>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="146"/>
-      <c r="B8" s="146"/>
-      <c r="C8" s="146"/>
-      <c r="D8" s="146"/>
+      <c r="A8" s="154"/>
+      <c r="B8" s="154"/>
+      <c r="C8" s="154"/>
+      <c r="D8" s="154"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -8014,86 +8402,86 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" s="72" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="163" t="s">
+      <c r="A9" s="138" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="164" t="s">
+      <c r="B9" s="167" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="163" t="s">
+      <c r="C9" s="138" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="168" t="s">
+      <c r="D9" s="139" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="169"/>
-      <c r="F9" s="169"/>
-      <c r="G9" s="170"/>
-      <c r="H9" s="159" t="s">
+      <c r="E9" s="140"/>
+      <c r="F9" s="140"/>
+      <c r="G9" s="141"/>
+      <c r="H9" s="164" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="155" t="s">
+      <c r="I9" s="133" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="155" t="s">
+      <c r="J9" s="133" t="s">
         <v>32</v>
       </c>
       <c r="K9" s="71"/>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="155"/>
-      <c r="B10" s="165"/>
-      <c r="C10" s="155"/>
-      <c r="D10" s="160"/>
-      <c r="E10" s="171"/>
-      <c r="F10" s="171"/>
-      <c r="G10" s="172"/>
-      <c r="H10" s="160"/>
-      <c r="I10" s="155"/>
-      <c r="J10" s="155"/>
+      <c r="A10" s="133"/>
+      <c r="B10" s="168"/>
+      <c r="C10" s="133"/>
+      <c r="D10" s="142"/>
+      <c r="E10" s="143"/>
+      <c r="F10" s="143"/>
+      <c r="G10" s="144"/>
+      <c r="H10" s="142"/>
+      <c r="I10" s="133"/>
+      <c r="J10" s="133"/>
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" s="73" customFormat="1" ht="15">
-      <c r="A11" s="161"/>
-      <c r="B11" s="161"/>
-      <c r="C11" s="161"/>
-      <c r="D11" s="161"/>
-      <c r="E11" s="161"/>
-      <c r="F11" s="161"/>
-      <c r="G11" s="161"/>
-      <c r="H11" s="161"/>
-      <c r="I11" s="161"/>
-      <c r="J11" s="162"/>
+      <c r="A11" s="165"/>
+      <c r="B11" s="165"/>
+      <c r="C11" s="165"/>
+      <c r="D11" s="165"/>
+      <c r="E11" s="165"/>
+      <c r="F11" s="165"/>
+      <c r="G11" s="165"/>
+      <c r="H11" s="165"/>
+      <c r="I11" s="165"/>
+      <c r="J11" s="166"/>
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A12" s="150" t="s">
-        <v>127</v>
-      </c>
-      <c r="B12" s="151"/>
-      <c r="C12" s="151"/>
-      <c r="D12" s="151"/>
-      <c r="E12" s="151"/>
-      <c r="F12" s="151"/>
-      <c r="G12" s="151"/>
-      <c r="H12" s="151"/>
-      <c r="I12" s="151"/>
-      <c r="J12" s="152"/>
+      <c r="A12" s="145" t="s">
+        <v>122</v>
+      </c>
+      <c r="B12" s="146"/>
+      <c r="C12" s="146"/>
+      <c r="D12" s="146"/>
+      <c r="E12" s="146"/>
+      <c r="F12" s="146"/>
+      <c r="G12" s="146"/>
+      <c r="H12" s="146"/>
+      <c r="I12" s="146"/>
+      <c r="J12" s="158"/>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" ht="102.75" customHeight="1" outlineLevel="1">
       <c r="A13" s="77" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="81" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C13" s="76" t="s">
-        <v>165</v>
-      </c>
-      <c r="D13" s="138" t="s">
-        <v>166</v>
-      </c>
-      <c r="E13" s="139"/>
-      <c r="F13" s="139"/>
+        <v>160</v>
+      </c>
+      <c r="D13" s="131" t="s">
+        <v>161</v>
+      </c>
+      <c r="E13" s="132"/>
+      <c r="F13" s="132"/>
       <c r="G13" s="75"/>
       <c r="H13" s="89"/>
       <c r="I13" s="76"/>
@@ -8104,16 +8492,16 @@
         <v>1</v>
       </c>
       <c r="B14" s="81" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C14" s="76" t="s">
-        <v>169</v>
-      </c>
-      <c r="D14" s="138" t="s">
-        <v>170</v>
-      </c>
-      <c r="E14" s="139"/>
-      <c r="F14" s="139"/>
+        <v>164</v>
+      </c>
+      <c r="D14" s="131" t="s">
+        <v>165</v>
+      </c>
+      <c r="E14" s="132"/>
+      <c r="F14" s="132"/>
       <c r="G14" s="75"/>
       <c r="H14" s="89"/>
       <c r="I14" s="76"/>
@@ -8124,27 +8512,27 @@
         <v>2</v>
       </c>
       <c r="B15" s="81" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C15" s="76" t="s">
-        <v>172</v>
-      </c>
-      <c r="D15" s="138" t="s">
-        <v>173</v>
-      </c>
-      <c r="E15" s="139"/>
-      <c r="F15" s="139"/>
+        <v>167</v>
+      </c>
+      <c r="D15" s="131" t="s">
+        <v>168</v>
+      </c>
+      <c r="E15" s="132"/>
+      <c r="F15" s="132"/>
       <c r="G15" s="75"/>
       <c r="H15" s="89"/>
       <c r="I15" s="76"/>
       <c r="J15" s="74"/>
     </row>
     <row r="16" spans="1:11" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A16" s="150" t="s">
-        <v>128</v>
-      </c>
-      <c r="B16" s="151"/>
-      <c r="C16" s="151"/>
+      <c r="A16" s="145" t="s">
+        <v>123</v>
+      </c>
+      <c r="B16" s="146"/>
+      <c r="C16" s="146"/>
       <c r="D16" s="87"/>
       <c r="E16" s="87"/>
       <c r="F16" s="87"/>
@@ -8158,13 +8546,13 @@
         <v>0</v>
       </c>
       <c r="B17" s="85" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C17" s="86" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D17" s="173" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E17" s="174"/>
       <c r="F17" s="174"/>
@@ -8178,13 +8566,13 @@
         <v>1</v>
       </c>
       <c r="B18" s="85" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C18" s="86" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D18" s="173" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E18" s="174"/>
       <c r="F18" s="174"/>
@@ -8198,13 +8586,13 @@
         <v>2</v>
       </c>
       <c r="B19" s="85" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C19" s="86" t="s">
+        <v>131</v>
+      </c>
+      <c r="D19" s="173" t="s">
         <v>136</v>
-      </c>
-      <c r="D19" s="173" t="s">
-        <v>141</v>
       </c>
       <c r="E19" s="174"/>
       <c r="F19" s="174"/>
@@ -8214,11 +8602,11 @@
       <c r="J19" s="96"/>
     </row>
     <row r="20" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A20" s="150" t="s">
-        <v>145</v>
-      </c>
-      <c r="B20" s="151"/>
-      <c r="C20" s="151"/>
+      <c r="A20" s="145" t="s">
+        <v>140</v>
+      </c>
+      <c r="B20" s="146"/>
+      <c r="C20" s="146"/>
       <c r="D20" s="87"/>
       <c r="E20" s="87"/>
       <c r="F20" s="87"/>
@@ -8232,16 +8620,16 @@
         <v>0</v>
       </c>
       <c r="B21" s="92" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C21" s="76" t="s">
-        <v>149</v>
-      </c>
-      <c r="D21" s="138" t="s">
-        <v>147</v>
-      </c>
-      <c r="E21" s="139"/>
-      <c r="F21" s="139"/>
+        <v>144</v>
+      </c>
+      <c r="D21" s="131" t="s">
+        <v>142</v>
+      </c>
+      <c r="E21" s="132"/>
+      <c r="F21" s="132"/>
       <c r="G21" s="75"/>
       <c r="H21" s="82"/>
       <c r="I21" s="76"/>
@@ -8252,16 +8640,16 @@
         <v>1</v>
       </c>
       <c r="B22" s="92" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C22" s="76" t="s">
-        <v>150</v>
-      </c>
-      <c r="D22" s="138" t="s">
-        <v>151</v>
-      </c>
-      <c r="E22" s="139"/>
-      <c r="F22" s="139"/>
+        <v>145</v>
+      </c>
+      <c r="D22" s="131" t="s">
+        <v>146</v>
+      </c>
+      <c r="E22" s="132"/>
+      <c r="F22" s="132"/>
       <c r="G22" s="75"/>
       <c r="H22" s="82"/>
       <c r="I22" s="76"/>
@@ -8272,16 +8660,16 @@
         <v>2</v>
       </c>
       <c r="B23" s="92" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C23" s="76" t="s">
-        <v>153</v>
-      </c>
-      <c r="D23" s="138" t="s">
-        <v>154</v>
-      </c>
-      <c r="E23" s="139"/>
-      <c r="F23" s="139"/>
+        <v>148</v>
+      </c>
+      <c r="D23" s="131" t="s">
+        <v>149</v>
+      </c>
+      <c r="E23" s="132"/>
+      <c r="F23" s="132"/>
       <c r="G23" s="75"/>
       <c r="H23" s="82"/>
       <c r="I23" s="76"/>
@@ -8292,25 +8680,25 @@
         <v>49</v>
       </c>
       <c r="B24" s="92" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C24" s="76" t="s">
-        <v>156</v>
-      </c>
-      <c r="D24" s="138" t="s">
-        <v>157</v>
-      </c>
-      <c r="E24" s="139"/>
-      <c r="F24" s="139"/>
+        <v>151</v>
+      </c>
+      <c r="D24" s="131" t="s">
+        <v>152</v>
+      </c>
+      <c r="E24" s="132"/>
+      <c r="F24" s="132"/>
       <c r="G24" s="75"/>
       <c r="H24" s="82"/>
       <c r="I24" s="76"/>
       <c r="J24" s="74"/>
     </row>
     <row r="25" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A25" s="133"/>
-      <c r="B25" s="134"/>
-      <c r="C25" s="134"/>
+      <c r="A25" s="134"/>
+      <c r="B25" s="135"/>
+      <c r="C25" s="135"/>
       <c r="D25" s="97"/>
       <c r="E25" s="97"/>
       <c r="F25" s="97"/>
@@ -8323,9 +8711,9 @@
       <c r="A26" s="77"/>
       <c r="B26" s="92"/>
       <c r="C26" s="76"/>
-      <c r="D26" s="131"/>
-      <c r="E26" s="132"/>
-      <c r="F26" s="132"/>
+      <c r="D26" s="147"/>
+      <c r="E26" s="148"/>
+      <c r="F26" s="148"/>
       <c r="G26" s="75"/>
       <c r="H26" s="82"/>
       <c r="I26" s="76"/>
@@ -8335,9 +8723,9 @@
       <c r="A27" s="77"/>
       <c r="B27" s="92"/>
       <c r="C27" s="76"/>
-      <c r="D27" s="131"/>
-      <c r="E27" s="132"/>
-      <c r="F27" s="132"/>
+      <c r="D27" s="147"/>
+      <c r="E27" s="148"/>
+      <c r="F27" s="148"/>
       <c r="G27" s="75"/>
       <c r="H27" s="82"/>
       <c r="I27" s="76"/>
@@ -8347,9 +8735,9 @@
       <c r="A28" s="77"/>
       <c r="B28" s="92"/>
       <c r="C28" s="76"/>
-      <c r="D28" s="131"/>
-      <c r="E28" s="132"/>
-      <c r="F28" s="132"/>
+      <c r="D28" s="147"/>
+      <c r="E28" s="148"/>
+      <c r="F28" s="148"/>
       <c r="G28" s="75"/>
       <c r="H28" s="82"/>
       <c r="I28" s="76"/>
@@ -8359,9 +8747,9 @@
       <c r="A29" s="77"/>
       <c r="B29" s="92"/>
       <c r="C29" s="76"/>
-      <c r="D29" s="131"/>
-      <c r="E29" s="132"/>
-      <c r="F29" s="132"/>
+      <c r="D29" s="147"/>
+      <c r="E29" s="148"/>
+      <c r="F29" s="148"/>
       <c r="G29" s="75"/>
       <c r="H29" s="82"/>
       <c r="I29" s="76"/>
@@ -8371,9 +8759,9 @@
       <c r="A30" s="77"/>
       <c r="B30" s="92"/>
       <c r="C30" s="76"/>
-      <c r="D30" s="131"/>
-      <c r="E30" s="132"/>
-      <c r="F30" s="132"/>
+      <c r="D30" s="147"/>
+      <c r="E30" s="148"/>
+      <c r="F30" s="148"/>
       <c r="G30" s="75"/>
       <c r="H30" s="82"/>
       <c r="I30" s="76"/>
@@ -8383,18 +8771,18 @@
       <c r="A31" s="77"/>
       <c r="B31" s="92"/>
       <c r="C31" s="76"/>
-      <c r="D31" s="131"/>
-      <c r="E31" s="132"/>
-      <c r="F31" s="132"/>
+      <c r="D31" s="147"/>
+      <c r="E31" s="148"/>
+      <c r="F31" s="148"/>
       <c r="G31" s="75"/>
       <c r="H31" s="82"/>
       <c r="I31" s="76"/>
       <c r="J31" s="74"/>
     </row>
     <row r="32" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A32" s="133"/>
-      <c r="B32" s="134"/>
-      <c r="C32" s="134"/>
+      <c r="A32" s="134"/>
+      <c r="B32" s="135"/>
+      <c r="C32" s="135"/>
       <c r="D32" s="97"/>
       <c r="E32" s="97"/>
       <c r="F32" s="97"/>
@@ -8407,9 +8795,9 @@
       <c r="A33" s="77"/>
       <c r="B33" s="92"/>
       <c r="C33" s="76"/>
-      <c r="D33" s="131"/>
-      <c r="E33" s="132"/>
-      <c r="F33" s="132"/>
+      <c r="D33" s="147"/>
+      <c r="E33" s="148"/>
+      <c r="F33" s="148"/>
       <c r="G33" s="75"/>
       <c r="H33" s="82"/>
       <c r="I33" s="76"/>
@@ -8545,6 +8933,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:G10"/>
     <mergeCell ref="D19:F19"/>
     <mergeCell ref="B1:D2"/>
     <mergeCell ref="B3:D3"/>
@@ -8561,30 +8973,6 @@
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="H6:J6"/>
     <mergeCell ref="H7:J7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -8619,9 +9007,9 @@
       <c r="A1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="144"/>
-      <c r="C1" s="144"/>
-      <c r="D1" s="144"/>
+      <c r="B1" s="152"/>
+      <c r="C1" s="152"/>
+      <c r="D1" s="152"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -8632,9 +9020,9 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="145"/>
-      <c r="C2" s="145"/>
-      <c r="D2" s="145"/>
+      <c r="B2" s="153"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -8655,43 +9043,43 @@
       <c r="E3" s="60"/>
       <c r="F3" s="60"/>
       <c r="G3" s="60"/>
-      <c r="H3" s="154"/>
-      <c r="I3" s="154"/>
-      <c r="J3" s="154"/>
+      <c r="H3" s="160"/>
+      <c r="I3" s="160"/>
+      <c r="J3" s="160"/>
       <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="12.75">
       <c r="A4" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="156" t="s">
-        <v>248</v>
-      </c>
-      <c r="C4" s="157"/>
-      <c r="D4" s="158"/>
+      <c r="B4" s="161" t="s">
+        <v>243</v>
+      </c>
+      <c r="C4" s="162"/>
+      <c r="D4" s="163"/>
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
       <c r="G4" s="60"/>
-      <c r="H4" s="154"/>
-      <c r="I4" s="154"/>
-      <c r="J4" s="154"/>
+      <c r="H4" s="160"/>
+      <c r="I4" s="160"/>
+      <c r="J4" s="160"/>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" s="70" customFormat="1" ht="25.5">
       <c r="A5" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="147" t="s">
+      <c r="B5" s="155" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="148"/>
-      <c r="D5" s="149"/>
+      <c r="C5" s="156"/>
+      <c r="D5" s="157"/>
       <c r="E5" s="68"/>
       <c r="F5" s="68"/>
       <c r="G5" s="68"/>
-      <c r="H5" s="153"/>
-      <c r="I5" s="153"/>
-      <c r="J5" s="153"/>
+      <c r="H5" s="159"/>
+      <c r="I5" s="159"/>
+      <c r="J5" s="159"/>
       <c r="K5" s="69"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
@@ -8712,9 +9100,9 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="154"/>
-      <c r="I6" s="154"/>
-      <c r="J6" s="154"/>
+      <c r="H6" s="160"/>
+      <c r="I6" s="160"/>
+      <c r="J6" s="160"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -8735,16 +9123,16 @@
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
       <c r="G7" s="61"/>
-      <c r="H7" s="154"/>
-      <c r="I7" s="154"/>
-      <c r="J7" s="154"/>
+      <c r="H7" s="160"/>
+      <c r="I7" s="160"/>
+      <c r="J7" s="160"/>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="146"/>
-      <c r="B8" s="146"/>
-      <c r="C8" s="146"/>
-      <c r="D8" s="146"/>
+      <c r="A8" s="154"/>
+      <c r="B8" s="154"/>
+      <c r="C8" s="154"/>
+      <c r="D8" s="154"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -8754,84 +9142,84 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" s="72" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="163" t="s">
+      <c r="A9" s="138" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="164" t="s">
+      <c r="B9" s="167" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="163" t="s">
+      <c r="C9" s="138" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="168" t="s">
+      <c r="D9" s="139" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="169"/>
-      <c r="F9" s="169"/>
-      <c r="G9" s="170"/>
-      <c r="H9" s="159" t="s">
+      <c r="E9" s="140"/>
+      <c r="F9" s="140"/>
+      <c r="G9" s="141"/>
+      <c r="H9" s="164" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="155" t="s">
+      <c r="I9" s="133" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="155" t="s">
+      <c r="J9" s="133" t="s">
         <v>32</v>
       </c>
       <c r="K9" s="71"/>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="155"/>
-      <c r="B10" s="165"/>
-      <c r="C10" s="155"/>
-      <c r="D10" s="160"/>
-      <c r="E10" s="171"/>
-      <c r="F10" s="171"/>
-      <c r="G10" s="172"/>
-      <c r="H10" s="160"/>
-      <c r="I10" s="155"/>
-      <c r="J10" s="155"/>
+      <c r="A10" s="133"/>
+      <c r="B10" s="168"/>
+      <c r="C10" s="133"/>
+      <c r="D10" s="142"/>
+      <c r="E10" s="143"/>
+      <c r="F10" s="143"/>
+      <c r="G10" s="144"/>
+      <c r="H10" s="142"/>
+      <c r="I10" s="133"/>
+      <c r="J10" s="133"/>
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" s="73" customFormat="1" ht="15">
-      <c r="A11" s="161"/>
-      <c r="B11" s="161"/>
-      <c r="C11" s="161"/>
-      <c r="D11" s="161"/>
-      <c r="E11" s="161"/>
-      <c r="F11" s="161"/>
-      <c r="G11" s="161"/>
-      <c r="H11" s="161"/>
-      <c r="I11" s="161"/>
-      <c r="J11" s="162"/>
+      <c r="A11" s="165"/>
+      <c r="B11" s="165"/>
+      <c r="C11" s="165"/>
+      <c r="D11" s="165"/>
+      <c r="E11" s="165"/>
+      <c r="F11" s="165"/>
+      <c r="G11" s="165"/>
+      <c r="H11" s="165"/>
+      <c r="I11" s="165"/>
+      <c r="J11" s="166"/>
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A12" s="150" t="s">
-        <v>278</v>
-      </c>
-      <c r="B12" s="151"/>
-      <c r="C12" s="151"/>
-      <c r="D12" s="151"/>
-      <c r="E12" s="151"/>
-      <c r="F12" s="151"/>
-      <c r="G12" s="151"/>
-      <c r="H12" s="151"/>
-      <c r="I12" s="151"/>
-      <c r="J12" s="152"/>
+      <c r="A12" s="145" t="s">
+        <v>273</v>
+      </c>
+      <c r="B12" s="146"/>
+      <c r="C12" s="146"/>
+      <c r="D12" s="146"/>
+      <c r="E12" s="146"/>
+      <c r="F12" s="146"/>
+      <c r="G12" s="146"/>
+      <c r="H12" s="146"/>
+      <c r="I12" s="146"/>
+      <c r="J12" s="158"/>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" ht="132.75" customHeight="1" outlineLevel="1">
       <c r="A13" s="77" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="81" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C13" s="122" t="s">
-        <v>251</v>
-      </c>
-      <c r="D13" s="138"/>
-      <c r="E13" s="139"/>
-      <c r="F13" s="139"/>
+        <v>246</v>
+      </c>
+      <c r="D13" s="131"/>
+      <c r="E13" s="132"/>
+      <c r="F13" s="132"/>
       <c r="G13" s="75"/>
       <c r="H13" s="89"/>
       <c r="I13" s="76"/>
@@ -8842,14 +9230,14 @@
         <v>1</v>
       </c>
       <c r="B14" s="81" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="C14" s="122" t="s">
-        <v>252</v>
-      </c>
-      <c r="D14" s="138"/>
-      <c r="E14" s="139"/>
-      <c r="F14" s="139"/>
+        <v>247</v>
+      </c>
+      <c r="D14" s="131"/>
+      <c r="E14" s="132"/>
+      <c r="F14" s="132"/>
       <c r="G14" s="75"/>
       <c r="H14" s="89"/>
       <c r="I14" s="76"/>
@@ -8860,25 +9248,25 @@
         <v>2</v>
       </c>
       <c r="B15" s="81" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="C15" s="76" t="s">
-        <v>260</v>
-      </c>
-      <c r="D15" s="138"/>
-      <c r="E15" s="139"/>
-      <c r="F15" s="139"/>
+        <v>255</v>
+      </c>
+      <c r="D15" s="131"/>
+      <c r="E15" s="132"/>
+      <c r="F15" s="132"/>
       <c r="G15" s="75"/>
       <c r="H15" s="89"/>
       <c r="I15" s="76"/>
       <c r="J15" s="74"/>
     </row>
     <row r="16" spans="1:11" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A16" s="150" t="s">
-        <v>279</v>
-      </c>
-      <c r="B16" s="151"/>
-      <c r="C16" s="151"/>
+      <c r="A16" s="145" t="s">
+        <v>274</v>
+      </c>
+      <c r="B16" s="146"/>
+      <c r="C16" s="146"/>
       <c r="D16" s="87"/>
       <c r="E16" s="87"/>
       <c r="F16" s="87"/>
@@ -8892,10 +9280,10 @@
         <v>0</v>
       </c>
       <c r="B17" s="85" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="C17" s="86" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="D17" s="173"/>
       <c r="E17" s="174"/>
@@ -8910,10 +9298,10 @@
         <v>1</v>
       </c>
       <c r="B18" s="85" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="C18" s="86" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="D18" s="173"/>
       <c r="E18" s="174"/>
@@ -8928,10 +9316,10 @@
         <v>2</v>
       </c>
       <c r="B19" s="92" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C19" s="76" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="D19" s="173"/>
       <c r="E19" s="174"/>
@@ -8946,10 +9334,10 @@
         <v>49</v>
       </c>
       <c r="B20" s="85" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="C20" s="86" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D20" s="173"/>
       <c r="E20" s="174"/>
@@ -8964,10 +9352,10 @@
         <v>52</v>
       </c>
       <c r="B21" s="85" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="C21" s="123" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D21" s="173"/>
       <c r="E21" s="174"/>
@@ -8978,11 +9366,11 @@
       <c r="J21" s="96"/>
     </row>
     <row r="22" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A22" s="150" t="s">
-        <v>255</v>
-      </c>
-      <c r="B22" s="151"/>
-      <c r="C22" s="151"/>
+      <c r="A22" s="145" t="s">
+        <v>250</v>
+      </c>
+      <c r="B22" s="146"/>
+      <c r="C22" s="146"/>
       <c r="D22" s="87"/>
       <c r="E22" s="87"/>
       <c r="F22" s="87"/>
@@ -8996,14 +9384,14 @@
         <v>0</v>
       </c>
       <c r="B23" s="92" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="C23" s="76" t="s">
-        <v>258</v>
-      </c>
-      <c r="D23" s="138"/>
-      <c r="E23" s="139"/>
-      <c r="F23" s="139"/>
+        <v>253</v>
+      </c>
+      <c r="D23" s="131"/>
+      <c r="E23" s="132"/>
+      <c r="F23" s="132"/>
       <c r="G23" s="75"/>
       <c r="H23" s="82"/>
       <c r="I23" s="76"/>
@@ -9014,14 +9402,14 @@
         <v>1</v>
       </c>
       <c r="B24" s="92" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C24" s="76" t="s">
-        <v>260</v>
-      </c>
-      <c r="D24" s="138"/>
-      <c r="E24" s="139"/>
-      <c r="F24" s="139"/>
+        <v>255</v>
+      </c>
+      <c r="D24" s="131"/>
+      <c r="E24" s="132"/>
+      <c r="F24" s="132"/>
       <c r="G24" s="75"/>
       <c r="H24" s="82"/>
       <c r="I24" s="76"/>
@@ -9032,14 +9420,14 @@
         <v>2</v>
       </c>
       <c r="B25" s="92" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="C25" s="76" t="s">
-        <v>269</v>
-      </c>
-      <c r="D25" s="138"/>
-      <c r="E25" s="139"/>
-      <c r="F25" s="139"/>
+        <v>264</v>
+      </c>
+      <c r="D25" s="131"/>
+      <c r="E25" s="132"/>
+      <c r="F25" s="132"/>
       <c r="G25" s="75"/>
       <c r="H25" s="82"/>
       <c r="I25" s="76"/>
@@ -9050,23 +9438,23 @@
         <v>49</v>
       </c>
       <c r="B26" s="92" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="C26" s="76" t="s">
-        <v>266</v>
-      </c>
-      <c r="D26" s="138"/>
-      <c r="E26" s="139"/>
-      <c r="F26" s="139"/>
+        <v>261</v>
+      </c>
+      <c r="D26" s="131"/>
+      <c r="E26" s="132"/>
+      <c r="F26" s="132"/>
       <c r="G26" s="75"/>
       <c r="H26" s="82"/>
       <c r="I26" s="76"/>
       <c r="J26" s="74"/>
     </row>
     <row r="27" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A27" s="133"/>
-      <c r="B27" s="134"/>
-      <c r="C27" s="134"/>
+      <c r="A27" s="134"/>
+      <c r="B27" s="135"/>
+      <c r="C27" s="135"/>
       <c r="D27" s="97"/>
       <c r="E27" s="97"/>
       <c r="F27" s="97"/>
@@ -9079,9 +9467,9 @@
       <c r="A28" s="77"/>
       <c r="B28" s="92"/>
       <c r="C28" s="76"/>
-      <c r="D28" s="131"/>
-      <c r="E28" s="132"/>
-      <c r="F28" s="132"/>
+      <c r="D28" s="147"/>
+      <c r="E28" s="148"/>
+      <c r="F28" s="148"/>
       <c r="G28" s="75"/>
       <c r="H28" s="82"/>
       <c r="I28" s="76"/>
@@ -9091,9 +9479,9 @@
       <c r="A29" s="77"/>
       <c r="B29" s="92"/>
       <c r="C29" s="76"/>
-      <c r="D29" s="131"/>
-      <c r="E29" s="132"/>
-      <c r="F29" s="132"/>
+      <c r="D29" s="147"/>
+      <c r="E29" s="148"/>
+      <c r="F29" s="148"/>
       <c r="G29" s="75"/>
       <c r="H29" s="82"/>
       <c r="I29" s="76"/>
@@ -9103,9 +9491,9 @@
       <c r="A30" s="77"/>
       <c r="B30" s="92"/>
       <c r="C30" s="76"/>
-      <c r="D30" s="131"/>
-      <c r="E30" s="132"/>
-      <c r="F30" s="132"/>
+      <c r="D30" s="147"/>
+      <c r="E30" s="148"/>
+      <c r="F30" s="148"/>
       <c r="G30" s="75"/>
       <c r="H30" s="82"/>
       <c r="I30" s="76"/>
@@ -9115,9 +9503,9 @@
       <c r="A31" s="77"/>
       <c r="B31" s="92"/>
       <c r="C31" s="76"/>
-      <c r="D31" s="131"/>
-      <c r="E31" s="132"/>
-      <c r="F31" s="132"/>
+      <c r="D31" s="147"/>
+      <c r="E31" s="148"/>
+      <c r="F31" s="148"/>
       <c r="G31" s="75"/>
       <c r="H31" s="82"/>
       <c r="I31" s="76"/>
@@ -9127,9 +9515,9 @@
       <c r="A32" s="77"/>
       <c r="B32" s="92"/>
       <c r="C32" s="76"/>
-      <c r="D32" s="131"/>
-      <c r="E32" s="132"/>
-      <c r="F32" s="132"/>
+      <c r="D32" s="147"/>
+      <c r="E32" s="148"/>
+      <c r="F32" s="148"/>
       <c r="G32" s="75"/>
       <c r="H32" s="82"/>
       <c r="I32" s="76"/>
@@ -9139,18 +9527,18 @@
       <c r="A33" s="77"/>
       <c r="B33" s="92"/>
       <c r="C33" s="76"/>
-      <c r="D33" s="131"/>
-      <c r="E33" s="132"/>
-      <c r="F33" s="132"/>
+      <c r="D33" s="147"/>
+      <c r="E33" s="148"/>
+      <c r="F33" s="148"/>
       <c r="G33" s="75"/>
       <c r="H33" s="82"/>
       <c r="I33" s="76"/>
       <c r="J33" s="74"/>
     </row>
     <row r="34" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A34" s="133"/>
-      <c r="B34" s="134"/>
-      <c r="C34" s="134"/>
+      <c r="A34" s="134"/>
+      <c r="B34" s="135"/>
+      <c r="C34" s="135"/>
       <c r="D34" s="97"/>
       <c r="E34" s="97"/>
       <c r="F34" s="97"/>
@@ -9163,9 +9551,9 @@
       <c r="A35" s="77"/>
       <c r="B35" s="92"/>
       <c r="C35" s="76"/>
-      <c r="D35" s="131"/>
-      <c r="E35" s="132"/>
-      <c r="F35" s="132"/>
+      <c r="D35" s="147"/>
+      <c r="E35" s="148"/>
+      <c r="F35" s="148"/>
       <c r="G35" s="75"/>
       <c r="H35" s="82"/>
       <c r="I35" s="76"/>
@@ -9301,6 +9689,32 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="D13:F13"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="D14:F14"/>
@@ -9317,32 +9731,6 @@
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:G10"/>
     <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="D21:F21"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -9456,7 +9844,7 @@
       </c>
       <c r="D8" s="66">
         <f>Samples!B6</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E8" s="65">
         <f>Samples!B7</f>
@@ -9531,7 +9919,7 @@
       </c>
       <c r="D11" s="53">
         <f>SUM(D6:D10)</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E11" s="53">
         <f>SUM(E6:E10)</f>
@@ -9564,7 +9952,7 @@
       <c r="D13" s="19"/>
       <c r="E13" s="23">
         <f>(D11+E11)*100/G11</f>
-        <v>32.8125</v>
+        <v>39.0625</v>
       </c>
       <c r="F13" s="19" t="s">
         <v>22</v>
@@ -9580,7 +9968,7 @@
       <c r="D14" s="19"/>
       <c r="E14" s="23">
         <f>D11*100/G11</f>
-        <v>20.3125</v>
+        <v>26.5625</v>
       </c>
       <c r="F14" s="19" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
up test tao sk bs
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University_IT\Tam\KiemThuPhanMem\event-manager-javafx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83F7218-54A3-4EF1-A5DB-8F5F7324834E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC09A14-4A0B-47CD-8254-930C51622FD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="821" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="343">
   <si>
     <t>TC1</t>
   </si>
@@ -1350,6 +1350,46 @@
   </si>
   <si>
     <t>3.0</t>
+  </si>
+  <si>
+    <t>Kiểm tra sự trùng lặp sự kiện được tổ chức tại cùng một địa điểm nhưng có thời gian trùng lặp một phần</t>
+  </si>
+  <si>
+    <t>Sự kiện không được tạo khi trùng thời gian một phần và địa điểm với sự kiện khác</t>
+  </si>
+  <si>
+    <t>1: Đăng nhập với tư cách là admin
+2: Truy cập vào trang quản trị, chọn mục sự kiện
+3: Tạo một sự kiện mới trùng địa điểm và thời gian một phần(trong khung giờ một phần khi sự kiện đó đang diễn ra, cận thời gian) với sự kiện đã có sẵn
+4: Nhấn nút Thêm sự kiện
+6: Hiển thị thông báo Lỗi: Trùng địa điểm và giờ với sự kiện khác!</t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra sự trùng lặp sự kiện được tổ chức tại cùng một địa điểm nhưng có thời gian trùng lặp một phần</t>
+  </si>
+  <si>
+    <t>Test TC Kiểm tra sự trùng lặp sự kiện được tổ chức tại cùng một địa điểm nhưng có thời gian trùng lặp một phần</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng xử lý lỗi trong quá trình tạo sự kiện</t>
+  </si>
+  <si>
+    <t>Khi ngắt kết nối database hệ thống có thể duy trì nhiều kết nối mở sẵn đến database. Khi đóng MySQL server, các kết nối đã được thiết lập từ trước có thể vẫn còn hoạt động trong một khoảng thời gian ngắn trước khi timeout. Vậy nên sự kiện vẫn được tạo thành công và lưu vào database</t>
+  </si>
+  <si>
+    <t>Viết TC Kiểm tra chức năng xử lý lỗi trong quá trình tạo sự kiện</t>
+  </si>
+  <si>
+    <t>Test TC Kiểm tra chức năng xử lý lỗi trong quá trình tạo sự kiện</t>
+  </si>
+  <si>
+    <t>1: Đăng nhập với tư cách là admin
+2: Truy cập vào trang quản trị, chọn mục sự kiện
+3: Nhập đầy đủ thông tin hợp lệ của các trường bắt buộc.
+4: Giả lập lỗi tạo sự kiện(Vd: Ngắt kết nối database)
+5: Nhấn nút Thêm sự kiện 
+6: Hệ thống hiển thị thông báo Thêm sự kiện thành công và sự kiện được lưu vào trong danh sách sự kiện
+7: Khôi phục lại kết nối database thì sự kiện vẫn được tạo và lưu vào</t>
   </si>
 </sst>
 </file>
@@ -2425,18 +2465,60 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2446,11 +2528,56 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2463,93 +2590,6 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4178,8 +4218,8 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>-1</xdr:rowOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>2531961</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4208,58 +4248,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5784022" y="55507283"/>
-          <a:ext cx="3147391" cy="2539999"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="Picture 22">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{336B5F8C-B96F-575C-2054-A520A149CB37}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5784022" y="59234457"/>
-          <a:ext cx="3147391" cy="2540000"/>
+          <a:off x="5787342" y="55425854"/>
+          <a:ext cx="3146867" cy="2531961"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4295,7 +4285,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -4322,13 +4312,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>1402621</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4345,7 +4335,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -4372,13 +4362,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>1357313</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1797843</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>2774157</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4395,7 +4385,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -4422,13 +4412,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>2703607</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4445,7 +4435,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -4472,13 +4462,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>1512093</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4495,7 +4485,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -4522,13 +4512,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>1516221</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>2986985</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4545,7 +4535,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -4572,13 +4562,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>2988467</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4595,7 +4585,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -4622,13 +4612,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>3203863</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>1563419</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4645,7 +4635,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -4672,13 +4662,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>1587500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>2962257</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4695,7 +4685,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -4722,13 +4712,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>2949086</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>3809999</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4745,7 +4735,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -4760,6 +4750,356 @@
         <a:xfrm>
           <a:off x="5779111" y="70036225"/>
           <a:ext cx="3159735" cy="860913"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>2531961</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>1929114</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD46916A-3F32-087D-87BE-F7999D089775}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5787343" y="60489777"/>
+          <a:ext cx="3146866" cy="1929115"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>1929114</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30557F45-21F2-159D-D975-E7EA956474B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5787342" y="62418892"/>
+          <a:ext cx="3146867" cy="1880886"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7B8E7FD-E2C3-4CE9-AA26-7F54447572EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5787342" y="68109778"/>
+          <a:ext cx="3146867" cy="2531963"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>2530378</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>1799166</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="47" name="Picture 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{038C746D-6DE8-60B9-2EA1-744A78E8253B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5791971" y="66848181"/>
+          <a:ext cx="3146135" cy="1799167"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>1799166</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>3280832</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="49" name="Picture 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D925759-F3E3-E502-CF50-955299F35AE8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5791970" y="68647348"/>
+          <a:ext cx="3146136" cy="1481666"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>3290453</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>4185226</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="54" name="Picture 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{393D21A4-F4FF-1C9B-6425-53A72647BBD9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5791970" y="70138635"/>
+          <a:ext cx="3146136" cy="894773"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>4146743</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="59" name="Picture 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{675E678E-D2AE-B5AB-1626-09EF1D0C4F1F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5791971" y="70994925"/>
+          <a:ext cx="3146135" cy="933258"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5073,8 +5413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H146"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A114" zoomScale="85" workbookViewId="0">
-      <selection activeCell="D122" sqref="D122"/>
+    <sheetView showGridLines="0" topLeftCell="A119" zoomScale="85" workbookViewId="0">
+      <selection activeCell="G129" sqref="G129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -7180,39 +7520,71 @@
       <c r="G127" s="99"/>
       <c r="H127" s="105"/>
     </row>
-    <row r="128" spans="2:8" s="33" customFormat="1">
-      <c r="B128" s="118"/>
-      <c r="C128" s="119"/>
+    <row r="128" spans="2:8" s="33" customFormat="1" ht="38.25">
+      <c r="B128" s="118">
+        <v>45739</v>
+      </c>
+      <c r="C128" s="119" t="s">
+        <v>40</v>
+      </c>
       <c r="D128" s="99"/>
-      <c r="E128" s="104"/>
-      <c r="F128" s="120"/>
+      <c r="E128" s="104" t="s">
+        <v>336</v>
+      </c>
+      <c r="F128" s="110" t="s">
+        <v>44</v>
+      </c>
       <c r="G128" s="99"/>
       <c r="H128" s="105"/>
     </row>
-    <row r="129" spans="2:8" s="33" customFormat="1">
-      <c r="B129" s="118"/>
-      <c r="C129" s="119"/>
+    <row r="129" spans="2:8" s="33" customFormat="1" ht="38.25">
+      <c r="B129" s="118">
+        <v>45739</v>
+      </c>
+      <c r="C129" s="119" t="s">
+        <v>40</v>
+      </c>
       <c r="D129" s="99"/>
-      <c r="E129" s="104"/>
-      <c r="F129" s="120"/>
+      <c r="E129" s="104" t="s">
+        <v>337</v>
+      </c>
+      <c r="F129" s="110" t="s">
+        <v>44</v>
+      </c>
       <c r="G129" s="99"/>
       <c r="H129" s="105"/>
     </row>
-    <row r="130" spans="2:8" s="33" customFormat="1">
-      <c r="B130" s="118"/>
-      <c r="C130" s="119"/>
+    <row r="130" spans="2:8" s="33" customFormat="1" ht="25.5">
+      <c r="B130" s="118">
+        <v>45739</v>
+      </c>
+      <c r="C130" s="119" t="s">
+        <v>40</v>
+      </c>
       <c r="D130" s="99"/>
-      <c r="E130" s="104"/>
-      <c r="F130" s="120"/>
+      <c r="E130" s="104" t="s">
+        <v>340</v>
+      </c>
+      <c r="F130" s="110" t="s">
+        <v>44</v>
+      </c>
       <c r="G130" s="99"/>
       <c r="H130" s="105"/>
     </row>
-    <row r="131" spans="2:8" s="33" customFormat="1">
-      <c r="B131" s="118"/>
-      <c r="C131" s="119"/>
+    <row r="131" spans="2:8" s="33" customFormat="1" ht="25.5">
+      <c r="B131" s="118">
+        <v>45739</v>
+      </c>
+      <c r="C131" s="119" t="s">
+        <v>40</v>
+      </c>
       <c r="D131" s="99"/>
-      <c r="E131" s="104"/>
-      <c r="F131" s="120"/>
+      <c r="E131" s="104" t="s">
+        <v>341</v>
+      </c>
+      <c r="F131" s="110" t="s">
+        <v>44</v>
+      </c>
       <c r="G131" s="99"/>
       <c r="H131" s="105"/>
     </row>
@@ -7366,7 +7738,7 @@
     <oddFooter>&amp;L&amp;"Tahoma,Regular"&amp;8 02ae-BM/PM/HDCV/FSOFT v1/0&amp;R&amp;"Tahoma,Regular"&amp;10&amp;P/&amp;N</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="C12:C28 C41 C34:C40 C42:C47 C48:C49 C51:C53 C50 C54:C57 C58:C60 C29:C33 C61:C83 C84:C92 C93:C94 C95:C102 C103:C105 C106:C110 C115:C116 C118 C112:C113 C111 C114 C119:C127 C117" numberStoredAsText="1"/>
+    <ignoredError sqref="C12:C28 C41 C34:C40 C42:C47 C48:C49 C51:C53 C50 C54:C57 C58:C60 C29:C33 C61:C83 C84:C92 C93:C94 C95:C102 C103:C105 C106:C110 C115:C116 C118 C112:C113 C111 C114 C119:C127 C117 C128:C131" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -7376,10 +7748,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K100"/>
+  <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A45" zoomScale="70" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B44" zoomScale="99" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" outlineLevelRow="1"/>
@@ -7398,9 +7770,9 @@
       <c r="A1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
+      <c r="B1" s="153"/>
+      <c r="C1" s="153"/>
+      <c r="D1" s="153"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -7411,9 +7783,9 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="146"/>
-      <c r="C2" s="146"/>
-      <c r="D2" s="146"/>
+      <c r="B2" s="154"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -7434,43 +7806,43 @@
       <c r="E3" s="60"/>
       <c r="F3" s="60"/>
       <c r="G3" s="60"/>
-      <c r="H3" s="155"/>
-      <c r="I3" s="155"/>
-      <c r="J3" s="155"/>
+      <c r="H3" s="161"/>
+      <c r="I3" s="161"/>
+      <c r="J3" s="161"/>
       <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="12.75">
       <c r="A4" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="157" t="s">
+      <c r="B4" s="162" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="158"/>
-      <c r="D4" s="159"/>
+      <c r="C4" s="163"/>
+      <c r="D4" s="164"/>
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
       <c r="G4" s="60"/>
-      <c r="H4" s="155"/>
-      <c r="I4" s="155"/>
-      <c r="J4" s="155"/>
+      <c r="H4" s="161"/>
+      <c r="I4" s="161"/>
+      <c r="J4" s="161"/>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" s="70" customFormat="1" ht="25.5">
       <c r="A5" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="148" t="s">
+      <c r="B5" s="156" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="149"/>
-      <c r="D5" s="150"/>
+      <c r="C5" s="157"/>
+      <c r="D5" s="158"/>
       <c r="E5" s="68"/>
       <c r="F5" s="68"/>
       <c r="G5" s="68"/>
-      <c r="H5" s="154"/>
-      <c r="I5" s="154"/>
-      <c r="J5" s="154"/>
+      <c r="H5" s="160"/>
+      <c r="I5" s="160"/>
+      <c r="J5" s="160"/>
       <c r="K5" s="69"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
@@ -7478,22 +7850,22 @@
         <v>38</v>
       </c>
       <c r="B6" s="79">
-        <f>COUNTIF(I12:I63,"Pass")</f>
-        <v>21</v>
+        <f>COUNTIF(I12:I65,"Pass")</f>
+        <v>23</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>39</v>
       </c>
       <c r="D6" s="13">
-        <f>COUNTIF(I10:I765,"Pending")</f>
+        <f>COUNTIF(I10:I767,"Pending")</f>
         <v>0</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="155"/>
-      <c r="I6" s="155"/>
-      <c r="J6" s="155"/>
+      <c r="H6" s="161"/>
+      <c r="I6" s="161"/>
+      <c r="J6" s="161"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -7501,29 +7873,29 @@
         <v>3</v>
       </c>
       <c r="B7" s="80">
-        <f>COUNTIF(I12:I63,"Fail")</f>
+        <f>COUNTIF(I12:I65,"Fail")</f>
         <v>8</v>
       </c>
       <c r="C7" s="29" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="58">
-        <f>COUNTA(A12:A63) -9</f>
-        <v>43</v>
+        <f>COUNTA(A12:A65) -9</f>
+        <v>45</v>
       </c>
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
       <c r="G7" s="61"/>
-      <c r="H7" s="155"/>
-      <c r="I7" s="155"/>
-      <c r="J7" s="155"/>
+      <c r="H7" s="161"/>
+      <c r="I7" s="161"/>
+      <c r="J7" s="161"/>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="147"/>
-      <c r="B8" s="147"/>
-      <c r="C8" s="147"/>
-      <c r="D8" s="147"/>
+      <c r="A8" s="155"/>
+      <c r="B8" s="155"/>
+      <c r="C8" s="155"/>
+      <c r="D8" s="155"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -7533,70 +7905,70 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" s="72" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="164" t="s">
+      <c r="A9" s="139" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="165" t="s">
+      <c r="B9" s="168" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="164" t="s">
+      <c r="C9" s="139" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="169" t="s">
+      <c r="D9" s="140" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="170"/>
-      <c r="F9" s="170"/>
-      <c r="G9" s="171"/>
-      <c r="H9" s="160" t="s">
+      <c r="E9" s="141"/>
+      <c r="F9" s="141"/>
+      <c r="G9" s="142"/>
+      <c r="H9" s="165" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="156" t="s">
+      <c r="I9" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="156" t="s">
+      <c r="J9" s="134" t="s">
         <v>32</v>
       </c>
       <c r="K9" s="71"/>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="156"/>
-      <c r="B10" s="166"/>
-      <c r="C10" s="156"/>
-      <c r="D10" s="161"/>
-      <c r="E10" s="172"/>
-      <c r="F10" s="172"/>
-      <c r="G10" s="173"/>
-      <c r="H10" s="161"/>
-      <c r="I10" s="156"/>
-      <c r="J10" s="156"/>
+      <c r="A10" s="134"/>
+      <c r="B10" s="169"/>
+      <c r="C10" s="134"/>
+      <c r="D10" s="143"/>
+      <c r="E10" s="144"/>
+      <c r="F10" s="144"/>
+      <c r="G10" s="145"/>
+      <c r="H10" s="143"/>
+      <c r="I10" s="134"/>
+      <c r="J10" s="134"/>
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" s="73" customFormat="1" ht="15">
-      <c r="A11" s="162"/>
-      <c r="B11" s="162"/>
-      <c r="C11" s="162"/>
-      <c r="D11" s="162"/>
-      <c r="E11" s="162"/>
-      <c r="F11" s="162"/>
-      <c r="G11" s="162"/>
-      <c r="H11" s="162"/>
-      <c r="I11" s="162"/>
-      <c r="J11" s="163"/>
+      <c r="A11" s="166"/>
+      <c r="B11" s="166"/>
+      <c r="C11" s="166"/>
+      <c r="D11" s="166"/>
+      <c r="E11" s="166"/>
+      <c r="F11" s="166"/>
+      <c r="G11" s="166"/>
+      <c r="H11" s="166"/>
+      <c r="I11" s="166"/>
+      <c r="J11" s="167"/>
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A12" s="151" t="s">
+      <c r="A12" s="146" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="152"/>
-      <c r="C12" s="152"/>
-      <c r="D12" s="152"/>
-      <c r="E12" s="152"/>
-      <c r="F12" s="152"/>
-      <c r="G12" s="152"/>
-      <c r="H12" s="152"/>
-      <c r="I12" s="152"/>
-      <c r="J12" s="153"/>
+      <c r="B12" s="147"/>
+      <c r="C12" s="147"/>
+      <c r="D12" s="147"/>
+      <c r="E12" s="147"/>
+      <c r="F12" s="147"/>
+      <c r="G12" s="147"/>
+      <c r="H12" s="147"/>
+      <c r="I12" s="147"/>
+      <c r="J12" s="159"/>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" ht="350.1" customHeight="1" outlineLevel="1">
       <c r="A13" s="77" t="s">
@@ -7608,9 +7980,9 @@
       <c r="C13" s="76" t="s">
         <v>193</v>
       </c>
-      <c r="D13" s="139"/>
-      <c r="E13" s="140"/>
-      <c r="F13" s="140"/>
+      <c r="D13" s="132"/>
+      <c r="E13" s="133"/>
+      <c r="F13" s="133"/>
       <c r="G13" s="75"/>
       <c r="H13" s="116">
         <v>45755</v>
@@ -7630,9 +8002,9 @@
       <c r="C14" s="76" t="s">
         <v>192</v>
       </c>
-      <c r="D14" s="139"/>
-      <c r="E14" s="140"/>
-      <c r="F14" s="140"/>
+      <c r="D14" s="132"/>
+      <c r="E14" s="133"/>
+      <c r="F14" s="133"/>
       <c r="G14" s="75"/>
       <c r="H14" s="116">
         <v>45755</v>
@@ -7652,9 +8024,9 @@
       <c r="C15" s="76" t="s">
         <v>191</v>
       </c>
-      <c r="D15" s="139"/>
-      <c r="E15" s="140"/>
-      <c r="F15" s="140"/>
+      <c r="D15" s="132"/>
+      <c r="E15" s="133"/>
+      <c r="F15" s="133"/>
       <c r="G15" s="75"/>
       <c r="H15" s="116">
         <v>45755</v>
@@ -7676,9 +8048,9 @@
       <c r="C16" s="76" t="s">
         <v>190</v>
       </c>
-      <c r="D16" s="139"/>
-      <c r="E16" s="140"/>
-      <c r="F16" s="140"/>
+      <c r="D16" s="132"/>
+      <c r="E16" s="133"/>
+      <c r="F16" s="133"/>
       <c r="G16" s="75"/>
       <c r="H16" s="116">
         <v>45755</v>
@@ -7698,9 +8070,9 @@
       <c r="C17" s="76" t="s">
         <v>189</v>
       </c>
-      <c r="D17" s="139"/>
-      <c r="E17" s="140"/>
-      <c r="F17" s="140"/>
+      <c r="D17" s="132"/>
+      <c r="E17" s="133"/>
+      <c r="F17" s="133"/>
       <c r="G17" s="75"/>
       <c r="H17" s="116">
         <v>45755</v>
@@ -7720,9 +8092,9 @@
       <c r="C18" s="86" t="s">
         <v>188</v>
       </c>
-      <c r="D18" s="139"/>
-      <c r="E18" s="140"/>
-      <c r="F18" s="140"/>
+      <c r="D18" s="132"/>
+      <c r="E18" s="133"/>
+      <c r="F18" s="133"/>
       <c r="G18" s="75"/>
       <c r="H18" s="116">
         <v>45755</v>
@@ -7744,9 +8116,9 @@
       <c r="C19" s="86" t="s">
         <v>187</v>
       </c>
-      <c r="D19" s="139"/>
-      <c r="E19" s="140"/>
-      <c r="F19" s="140"/>
+      <c r="D19" s="132"/>
+      <c r="E19" s="133"/>
+      <c r="F19" s="133"/>
       <c r="G19" s="75"/>
       <c r="H19" s="116">
         <v>45755</v>
@@ -7768,9 +8140,9 @@
       <c r="C20" s="76" t="s">
         <v>185</v>
       </c>
-      <c r="D20" s="139"/>
-      <c r="E20" s="140"/>
-      <c r="F20" s="140"/>
+      <c r="D20" s="132"/>
+      <c r="E20" s="133"/>
+      <c r="F20" s="133"/>
       <c r="G20" s="75"/>
       <c r="H20" s="116">
         <v>45755</v>
@@ -7792,9 +8164,9 @@
       <c r="C21" s="76" t="s">
         <v>184</v>
       </c>
-      <c r="D21" s="139"/>
-      <c r="E21" s="140"/>
-      <c r="F21" s="140"/>
+      <c r="D21" s="132"/>
+      <c r="E21" s="133"/>
+      <c r="F21" s="133"/>
       <c r="G21" s="75"/>
       <c r="H21" s="116">
         <v>45755</v>
@@ -7816,9 +8188,9 @@
       <c r="C22" s="86" t="s">
         <v>186</v>
       </c>
-      <c r="D22" s="139"/>
-      <c r="E22" s="140"/>
-      <c r="F22" s="140"/>
+      <c r="D22" s="132"/>
+      <c r="E22" s="133"/>
+      <c r="F22" s="133"/>
       <c r="G22" s="75"/>
       <c r="H22" s="116">
         <v>45755</v>
@@ -7831,11 +8203,11 @@
       </c>
     </row>
     <row r="23" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A23" s="151" t="s">
+      <c r="A23" s="146" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="152"/>
-      <c r="C23" s="152"/>
+      <c r="B23" s="147"/>
+      <c r="C23" s="147"/>
       <c r="D23" s="87"/>
       <c r="E23" s="87"/>
       <c r="F23" s="87"/>
@@ -7854,9 +8226,9 @@
       <c r="C24" s="86" t="s">
         <v>221</v>
       </c>
-      <c r="D24" s="167"/>
-      <c r="E24" s="168"/>
-      <c r="F24" s="168"/>
+      <c r="D24" s="137"/>
+      <c r="E24" s="138"/>
+      <c r="F24" s="138"/>
       <c r="G24" s="94"/>
       <c r="H24" s="115">
         <v>45756</v>
@@ -7876,9 +8248,9 @@
       <c r="C25" s="86" t="s">
         <v>220</v>
       </c>
-      <c r="D25" s="167"/>
-      <c r="E25" s="168"/>
-      <c r="F25" s="168"/>
+      <c r="D25" s="137"/>
+      <c r="E25" s="138"/>
+      <c r="F25" s="138"/>
       <c r="G25" s="94"/>
       <c r="H25" s="115">
         <v>45755</v>
@@ -7900,9 +8272,9 @@
       <c r="C26" s="86" t="s">
         <v>225</v>
       </c>
-      <c r="D26" s="132"/>
-      <c r="E26" s="133"/>
-      <c r="F26" s="133"/>
+      <c r="D26" s="148"/>
+      <c r="E26" s="149"/>
+      <c r="F26" s="149"/>
       <c r="G26" s="94"/>
       <c r="H26" s="115">
         <v>45756</v>
@@ -7922,9 +8294,9 @@
       <c r="C27" s="86" t="s">
         <v>226</v>
       </c>
-      <c r="D27" s="136"/>
-      <c r="E27" s="137"/>
-      <c r="F27" s="138"/>
+      <c r="D27" s="150"/>
+      <c r="E27" s="151"/>
+      <c r="F27" s="152"/>
       <c r="G27" s="94"/>
       <c r="H27" s="115">
         <v>45755</v>
@@ -7944,9 +8316,9 @@
       <c r="C28" s="86" t="s">
         <v>230</v>
       </c>
-      <c r="D28" s="136"/>
-      <c r="E28" s="137"/>
-      <c r="F28" s="138"/>
+      <c r="D28" s="150"/>
+      <c r="E28" s="151"/>
+      <c r="F28" s="152"/>
       <c r="G28" s="94"/>
       <c r="H28" s="115">
         <v>45756</v>
@@ -7968,9 +8340,9 @@
       <c r="C29" s="86" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="136"/>
-      <c r="E29" s="137"/>
-      <c r="F29" s="138"/>
+      <c r="D29" s="150"/>
+      <c r="E29" s="151"/>
+      <c r="F29" s="152"/>
       <c r="G29" s="94"/>
       <c r="H29" s="115">
         <v>45756</v>
@@ -7992,9 +8364,9 @@
       <c r="C30" s="86" t="s">
         <v>227</v>
       </c>
-      <c r="D30" s="136"/>
-      <c r="E30" s="137"/>
-      <c r="F30" s="138"/>
+      <c r="D30" s="150"/>
+      <c r="E30" s="151"/>
+      <c r="F30" s="152"/>
       <c r="G30" s="94"/>
       <c r="H30" s="115">
         <v>45755</v>
@@ -8014,9 +8386,9 @@
       <c r="C31" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="136"/>
-      <c r="E31" s="137"/>
-      <c r="F31" s="138"/>
+      <c r="D31" s="150"/>
+      <c r="E31" s="151"/>
+      <c r="F31" s="152"/>
       <c r="G31" s="94"/>
       <c r="H31" s="115">
         <v>45756</v>
@@ -8038,9 +8410,9 @@
       <c r="C32" s="86" t="s">
         <v>70</v>
       </c>
-      <c r="D32" s="136"/>
-      <c r="E32" s="137"/>
-      <c r="F32" s="138"/>
+      <c r="D32" s="150"/>
+      <c r="E32" s="151"/>
+      <c r="F32" s="152"/>
       <c r="G32" s="94"/>
       <c r="H32" s="115">
         <v>45756</v>
@@ -8062,9 +8434,9 @@
       <c r="C33" s="86" t="s">
         <v>234</v>
       </c>
-      <c r="D33" s="139"/>
-      <c r="E33" s="140"/>
-      <c r="F33" s="141"/>
+      <c r="D33" s="132"/>
+      <c r="E33" s="133"/>
+      <c r="F33" s="170"/>
       <c r="G33" s="94"/>
       <c r="H33" s="115">
         <v>45755</v>
@@ -8084,9 +8456,9 @@
       <c r="C34" s="86" t="s">
         <v>194</v>
       </c>
-      <c r="D34" s="142"/>
-      <c r="E34" s="143"/>
-      <c r="F34" s="144"/>
+      <c r="D34" s="171"/>
+      <c r="E34" s="172"/>
+      <c r="F34" s="173"/>
       <c r="G34" s="94"/>
       <c r="H34" s="115">
         <v>45755</v>
@@ -8097,11 +8469,11 @@
       <c r="J34" s="96"/>
     </row>
     <row r="35" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A35" s="151" t="s">
+      <c r="A35" s="146" t="s">
         <v>71</v>
       </c>
-      <c r="B35" s="152"/>
-      <c r="C35" s="152"/>
+      <c r="B35" s="147"/>
+      <c r="C35" s="147"/>
       <c r="D35" s="87"/>
       <c r="E35" s="87"/>
       <c r="F35" s="87"/>
@@ -8120,20 +8492,20 @@
       <c r="C36" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="D36" s="132"/>
-      <c r="E36" s="133"/>
-      <c r="F36" s="133"/>
+      <c r="D36" s="148"/>
+      <c r="E36" s="149"/>
+      <c r="F36" s="149"/>
       <c r="G36" s="75"/>
       <c r="H36" s="82"/>
       <c r="I36" s="76"/>
       <c r="J36" s="74"/>
     </row>
     <row r="37" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A37" s="134" t="s">
+      <c r="A37" s="135" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="135"/>
-      <c r="C37" s="135"/>
+      <c r="B37" s="136"/>
+      <c r="C37" s="136"/>
       <c r="D37" s="97"/>
       <c r="E37" s="97"/>
       <c r="F37" s="97"/>
@@ -8152,9 +8524,9 @@
       <c r="C38" s="76" t="s">
         <v>302</v>
       </c>
-      <c r="D38" s="132"/>
-      <c r="E38" s="133"/>
-      <c r="F38" s="133"/>
+      <c r="D38" s="148"/>
+      <c r="E38" s="149"/>
+      <c r="F38" s="149"/>
       <c r="G38" s="75"/>
       <c r="H38" s="129">
         <v>45768</v>
@@ -8174,9 +8546,9 @@
       <c r="C39" s="76" t="s">
         <v>306</v>
       </c>
-      <c r="D39" s="132"/>
-      <c r="E39" s="133"/>
-      <c r="F39" s="133"/>
+      <c r="D39" s="148"/>
+      <c r="E39" s="149"/>
+      <c r="F39" s="149"/>
       <c r="G39" s="75"/>
       <c r="H39" s="129">
         <v>45768</v>
@@ -8198,9 +8570,9 @@
       <c r="C40" s="76" t="s">
         <v>308</v>
       </c>
-      <c r="D40" s="132"/>
-      <c r="E40" s="133"/>
-      <c r="F40" s="133"/>
+      <c r="D40" s="148"/>
+      <c r="E40" s="149"/>
+      <c r="F40" s="149"/>
       <c r="G40" s="75"/>
       <c r="H40" s="129">
         <v>45768</v>
@@ -8222,9 +8594,9 @@
       <c r="C41" s="76" t="s">
         <v>313</v>
       </c>
-      <c r="D41" s="132"/>
-      <c r="E41" s="133"/>
-      <c r="F41" s="133"/>
+      <c r="D41" s="148"/>
+      <c r="E41" s="149"/>
+      <c r="F41" s="149"/>
       <c r="G41" s="75"/>
       <c r="H41" s="129">
         <v>45769</v>
@@ -8236,224 +8608,240 @@
         <v>315</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="4" customFormat="1" ht="200.1" customHeight="1" outlineLevel="1">
+    <row r="42" spans="1:10" s="4" customFormat="1" ht="300" customHeight="1" outlineLevel="1">
       <c r="A42" s="77" t="s">
         <v>52</v>
       </c>
       <c r="B42" s="92" t="s">
-        <v>112</v>
+        <v>333</v>
       </c>
       <c r="C42" s="76" t="s">
-        <v>311</v>
-      </c>
-      <c r="D42" s="132"/>
-      <c r="E42" s="133"/>
-      <c r="F42" s="133"/>
+        <v>335</v>
+      </c>
+      <c r="D42" s="148"/>
+      <c r="E42" s="149"/>
+      <c r="F42" s="149"/>
       <c r="G42" s="75"/>
       <c r="H42" s="129">
-        <v>45768</v>
+        <v>45770</v>
       </c>
       <c r="I42" s="76" t="s">
         <v>38</v>
       </c>
       <c r="J42" s="74" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="4" customFormat="1" ht="200.1" customHeight="1" outlineLevel="1">
+      <c r="A43" s="77" t="s">
+        <v>53</v>
+      </c>
+      <c r="B43" s="92" t="s">
+        <v>112</v>
+      </c>
+      <c r="C43" s="76" t="s">
+        <v>311</v>
+      </c>
+      <c r="D43" s="148"/>
+      <c r="E43" s="149"/>
+      <c r="F43" s="149"/>
+      <c r="G43" s="75"/>
+      <c r="H43" s="129">
+        <v>45768</v>
+      </c>
+      <c r="I43" s="76" t="s">
+        <v>38</v>
+      </c>
+      <c r="J43" s="74" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A43" s="134" t="s">
-        <v>88</v>
-      </c>
-      <c r="B43" s="135"/>
-      <c r="C43" s="135"/>
-      <c r="D43" s="97"/>
-      <c r="E43" s="97"/>
-      <c r="F43" s="97"/>
-      <c r="G43" s="97"/>
-      <c r="H43" s="97"/>
-      <c r="I43" s="97"/>
-      <c r="J43" s="98"/>
-    </row>
-    <row r="44" spans="1:10" s="4" customFormat="1" ht="300" customHeight="1" outlineLevel="1">
+    <row r="44" spans="1:10" s="4" customFormat="1" ht="399.95" customHeight="1" outlineLevel="1">
       <c r="A44" s="77" t="s">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="B44" s="92" t="s">
-        <v>89</v>
+        <v>338</v>
       </c>
       <c r="C44" s="76" t="s">
-        <v>326</v>
-      </c>
-      <c r="D44" s="132"/>
-      <c r="E44" s="133"/>
-      <c r="F44" s="133"/>
+        <v>342</v>
+      </c>
+      <c r="D44" s="148"/>
+      <c r="E44" s="149"/>
+      <c r="F44" s="149"/>
       <c r="G44" s="75"/>
       <c r="H44" s="129">
-        <v>45769</v>
+        <v>45770</v>
       </c>
       <c r="I44" s="76" t="s">
         <v>38</v>
       </c>
-      <c r="J44" s="74"/>
-    </row>
-    <row r="45" spans="1:10" s="4" customFormat="1" ht="300" customHeight="1" outlineLevel="1">
-      <c r="A45" s="77" t="s">
+      <c r="J44" s="74" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
+      <c r="A45" s="135" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" s="136"/>
+      <c r="C45" s="136"/>
+      <c r="D45" s="97"/>
+      <c r="E45" s="97"/>
+      <c r="F45" s="97"/>
+      <c r="G45" s="97"/>
+      <c r="H45" s="97"/>
+      <c r="I45" s="97"/>
+      <c r="J45" s="98"/>
+    </row>
+    <row r="46" spans="1:10" s="4" customFormat="1" ht="300" customHeight="1" outlineLevel="1">
+      <c r="A46" s="77" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" s="92" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" s="76" t="s">
+        <v>326</v>
+      </c>
+      <c r="D46" s="148"/>
+      <c r="E46" s="149"/>
+      <c r="F46" s="149"/>
+      <c r="G46" s="75"/>
+      <c r="H46" s="129">
+        <v>45769</v>
+      </c>
+      <c r="I46" s="76" t="s">
+        <v>38</v>
+      </c>
+      <c r="J46" s="74"/>
+    </row>
+    <row r="47" spans="1:10" s="4" customFormat="1" ht="300" customHeight="1" outlineLevel="1">
+      <c r="A47" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="B45" s="92" t="s">
+      <c r="B47" s="92" t="s">
         <v>90</v>
       </c>
-      <c r="C45" s="76" t="s">
+      <c r="C47" s="76" t="s">
         <v>327</v>
       </c>
-      <c r="D45" s="132"/>
-      <c r="E45" s="133"/>
-      <c r="F45" s="133"/>
-      <c r="G45" s="75"/>
-      <c r="H45" s="129">
+      <c r="D47" s="148"/>
+      <c r="E47" s="149"/>
+      <c r="F47" s="149"/>
+      <c r="G47" s="75"/>
+      <c r="H47" s="129">
         <v>45769</v>
       </c>
-      <c r="I45" s="76" t="s">
+      <c r="I47" s="76" t="s">
         <v>38</v>
       </c>
-      <c r="J45" s="74" t="s">
+      <c r="J47" s="74" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="4" customFormat="1" ht="79.5" customHeight="1" outlineLevel="1">
-      <c r="A46" s="77" t="s">
+    <row r="48" spans="1:10" s="4" customFormat="1" ht="79.5" customHeight="1" outlineLevel="1">
+      <c r="A48" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="92" t="s">
+      <c r="B48" s="92" t="s">
         <v>93</v>
       </c>
-      <c r="C46" s="76" t="s">
+      <c r="C48" s="76" t="s">
         <v>95</v>
       </c>
-      <c r="D46" s="132"/>
-      <c r="E46" s="133"/>
-      <c r="F46" s="133"/>
-      <c r="G46" s="75"/>
-      <c r="H46" s="82"/>
-      <c r="I46" s="76"/>
-      <c r="J46" s="74"/>
-    </row>
-    <row r="47" spans="1:10" s="4" customFormat="1" ht="79.5" customHeight="1" outlineLevel="1">
-      <c r="A47" s="77" t="s">
-        <v>49</v>
-      </c>
-      <c r="B47" s="92" t="s">
-        <v>94</v>
-      </c>
-      <c r="C47" s="76" t="s">
-        <v>96</v>
-      </c>
-      <c r="D47" s="132"/>
-      <c r="E47" s="133"/>
-      <c r="F47" s="133"/>
-      <c r="G47" s="75"/>
-      <c r="H47" s="82"/>
-      <c r="I47" s="76"/>
-      <c r="J47" s="74"/>
-    </row>
-    <row r="48" spans="1:10" s="4" customFormat="1" ht="91.5" customHeight="1" outlineLevel="1">
-      <c r="A48" s="77" t="s">
-        <v>52</v>
-      </c>
-      <c r="B48" s="92" t="s">
-        <v>97</v>
-      </c>
-      <c r="C48" s="76" t="s">
-        <v>98</v>
-      </c>
-      <c r="D48" s="132"/>
-      <c r="E48" s="133"/>
-      <c r="F48" s="133"/>
+      <c r="D48" s="148"/>
+      <c r="E48" s="149"/>
+      <c r="F48" s="149"/>
       <c r="G48" s="75"/>
       <c r="H48" s="82"/>
       <c r="I48" s="76"/>
       <c r="J48" s="74"/>
     </row>
-    <row r="49" spans="1:10" s="4" customFormat="1" ht="67.5" customHeight="1" outlineLevel="1">
+    <row r="49" spans="1:10" s="4" customFormat="1" ht="79.5" customHeight="1" outlineLevel="1">
       <c r="A49" s="77" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B49" s="92" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C49" s="76" t="s">
-        <v>92</v>
-      </c>
-      <c r="D49" s="132"/>
-      <c r="E49" s="133"/>
-      <c r="F49" s="133"/>
+        <v>96</v>
+      </c>
+      <c r="D49" s="148"/>
+      <c r="E49" s="149"/>
+      <c r="F49" s="149"/>
       <c r="G49" s="75"/>
       <c r="H49" s="82"/>
       <c r="I49" s="76"/>
       <c r="J49" s="74"/>
     </row>
-    <row r="50" spans="1:10" s="4" customFormat="1" ht="300" customHeight="1" outlineLevel="1">
+    <row r="50" spans="1:10" s="4" customFormat="1" ht="91.5" customHeight="1" outlineLevel="1">
       <c r="A50" s="77" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" s="92" t="s">
+        <v>97</v>
+      </c>
+      <c r="C50" s="76" t="s">
+        <v>98</v>
+      </c>
+      <c r="D50" s="148"/>
+      <c r="E50" s="149"/>
+      <c r="F50" s="149"/>
+      <c r="G50" s="75"/>
+      <c r="H50" s="82"/>
+      <c r="I50" s="76"/>
+      <c r="J50" s="74"/>
+    </row>
+    <row r="51" spans="1:10" s="4" customFormat="1" ht="67.5" customHeight="1" outlineLevel="1">
+      <c r="A51" s="77" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51" s="92" t="s">
+        <v>91</v>
+      </c>
+      <c r="C51" s="76" t="s">
+        <v>92</v>
+      </c>
+      <c r="D51" s="148"/>
+      <c r="E51" s="149"/>
+      <c r="F51" s="149"/>
+      <c r="G51" s="75"/>
+      <c r="H51" s="82"/>
+      <c r="I51" s="76"/>
+      <c r="J51" s="74"/>
+    </row>
+    <row r="52" spans="1:10" s="4" customFormat="1" ht="300" customHeight="1" outlineLevel="1">
+      <c r="A52" s="77" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="92" t="s">
+      <c r="B52" s="92" t="s">
         <v>317</v>
       </c>
-      <c r="C50" s="76" t="s">
+      <c r="C52" s="76" t="s">
         <v>318</v>
       </c>
-      <c r="D50" s="132"/>
-      <c r="E50" s="133"/>
-      <c r="F50" s="133"/>
-      <c r="G50" s="75"/>
-      <c r="H50" s="129">
+      <c r="D52" s="148"/>
+      <c r="E52" s="149"/>
+      <c r="F52" s="149"/>
+      <c r="G52" s="75"/>
+      <c r="H52" s="129">
         <v>45769</v>
       </c>
-      <c r="I50" s="76" t="s">
+      <c r="I52" s="76" t="s">
         <v>38</v>
       </c>
-      <c r="J50" s="74" t="s">
+      <c r="J52" s="74" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="51" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A51" s="134" t="s">
+    <row r="53" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
+      <c r="A53" s="135" t="s">
         <v>99</v>
       </c>
-      <c r="B51" s="135"/>
-      <c r="C51" s="135"/>
-      <c r="D51" s="97"/>
-      <c r="E51" s="97"/>
-      <c r="F51" s="97"/>
-      <c r="G51" s="97"/>
-      <c r="H51" s="97"/>
-      <c r="I51" s="97"/>
-      <c r="J51" s="98"/>
-    </row>
-    <row r="52" spans="1:10" s="4" customFormat="1" ht="47.25" customHeight="1" outlineLevel="1">
-      <c r="A52" s="77" t="s">
-        <v>0</v>
-      </c>
-      <c r="B52" s="92" t="s">
-        <v>123</v>
-      </c>
-      <c r="C52" s="76" t="s">
-        <v>100</v>
-      </c>
-      <c r="D52" s="132"/>
-      <c r="E52" s="133"/>
-      <c r="F52" s="133"/>
-      <c r="G52" s="75"/>
-      <c r="H52" s="82"/>
-      <c r="I52" s="76"/>
-      <c r="J52" s="74"/>
-    </row>
-    <row r="53" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A53" s="134" t="s">
-        <v>258</v>
-      </c>
-      <c r="B53" s="135"/>
-      <c r="C53" s="135"/>
+      <c r="B53" s="136"/>
+      <c r="C53" s="136"/>
       <c r="D53" s="97"/>
       <c r="E53" s="97"/>
       <c r="F53" s="97"/>
@@ -8462,206 +8850,214 @@
       <c r="I53" s="97"/>
       <c r="J53" s="98"/>
     </row>
-    <row r="54" spans="1:10" s="4" customFormat="1" ht="144" customHeight="1" outlineLevel="1">
+    <row r="54" spans="1:10" s="4" customFormat="1" ht="47.25" customHeight="1" outlineLevel="1">
       <c r="A54" s="77" t="s">
         <v>0</v>
       </c>
       <c r="B54" s="92" t="s">
-        <v>260</v>
+        <v>123</v>
       </c>
       <c r="C54" s="76" t="s">
-        <v>257</v>
-      </c>
-      <c r="D54" s="132"/>
-      <c r="E54" s="133"/>
-      <c r="F54" s="133"/>
+        <v>100</v>
+      </c>
+      <c r="D54" s="148"/>
+      <c r="E54" s="149"/>
+      <c r="F54" s="149"/>
       <c r="G54" s="75"/>
       <c r="H54" s="82"/>
       <c r="I54" s="76"/>
       <c r="J54" s="74"/>
     </row>
-    <row r="55" spans="1:10" s="4" customFormat="1" ht="123" customHeight="1" outlineLevel="1">
-      <c r="A55" s="77" t="s">
+    <row r="55" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
+      <c r="A55" s="135" t="s">
+        <v>258</v>
+      </c>
+      <c r="B55" s="136"/>
+      <c r="C55" s="136"/>
+      <c r="D55" s="97"/>
+      <c r="E55" s="97"/>
+      <c r="F55" s="97"/>
+      <c r="G55" s="97"/>
+      <c r="H55" s="97"/>
+      <c r="I55" s="97"/>
+      <c r="J55" s="98"/>
+    </row>
+    <row r="56" spans="1:10" s="4" customFormat="1" ht="144" customHeight="1" outlineLevel="1">
+      <c r="A56" s="77" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" s="92" t="s">
+        <v>260</v>
+      </c>
+      <c r="C56" s="76" t="s">
+        <v>257</v>
+      </c>
+      <c r="D56" s="148"/>
+      <c r="E56" s="149"/>
+      <c r="F56" s="149"/>
+      <c r="G56" s="75"/>
+      <c r="H56" s="82"/>
+      <c r="I56" s="76"/>
+      <c r="J56" s="74"/>
+    </row>
+    <row r="57" spans="1:10" s="4" customFormat="1" ht="123" customHeight="1" outlineLevel="1">
+      <c r="A57" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="B55" s="92" t="s">
+      <c r="B57" s="92" t="s">
         <v>261</v>
       </c>
-      <c r="C55" s="76" t="s">
+      <c r="C57" s="76" t="s">
         <v>262</v>
       </c>
-      <c r="D55" s="132"/>
-      <c r="E55" s="133"/>
-      <c r="F55" s="133"/>
-      <c r="G55" s="75"/>
-      <c r="H55" s="82"/>
-      <c r="I55" s="76"/>
-      <c r="J55" s="74"/>
-    </row>
-    <row r="56" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A56" s="134" t="s">
-        <v>285</v>
-      </c>
-      <c r="B56" s="135"/>
-      <c r="C56" s="135"/>
-      <c r="D56" s="97"/>
-      <c r="E56" s="97"/>
-      <c r="F56" s="97"/>
-      <c r="G56" s="97"/>
-      <c r="H56" s="97"/>
-      <c r="I56" s="97"/>
-      <c r="J56" s="98"/>
-    </row>
-    <row r="57" spans="1:10" s="4" customFormat="1" ht="98.25" customHeight="1" outlineLevel="1">
-      <c r="A57" s="77" t="s">
-        <v>0</v>
-      </c>
-      <c r="B57" s="92" t="s">
-        <v>301</v>
-      </c>
-      <c r="C57" s="76" t="s">
-        <v>296</v>
-      </c>
-      <c r="D57" s="132"/>
-      <c r="E57" s="133"/>
-      <c r="F57" s="133"/>
+      <c r="D57" s="148"/>
+      <c r="E57" s="149"/>
+      <c r="F57" s="149"/>
       <c r="G57" s="75"/>
       <c r="H57" s="82"/>
       <c r="I57" s="76"/>
       <c r="J57" s="74"/>
     </row>
-    <row r="58" spans="1:10" s="4" customFormat="1" ht="160.5" customHeight="1" outlineLevel="1">
-      <c r="A58" s="77" t="s">
+    <row r="58" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
+      <c r="A58" s="135" t="s">
+        <v>285</v>
+      </c>
+      <c r="B58" s="136"/>
+      <c r="C58" s="136"/>
+      <c r="D58" s="97"/>
+      <c r="E58" s="97"/>
+      <c r="F58" s="97"/>
+      <c r="G58" s="97"/>
+      <c r="H58" s="97"/>
+      <c r="I58" s="97"/>
+      <c r="J58" s="98"/>
+    </row>
+    <row r="59" spans="1:10" s="4" customFormat="1" ht="98.25" customHeight="1" outlineLevel="1">
+      <c r="A59" s="77" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="92" t="s">
+        <v>301</v>
+      </c>
+      <c r="C59" s="76" t="s">
+        <v>296</v>
+      </c>
+      <c r="D59" s="148"/>
+      <c r="E59" s="149"/>
+      <c r="F59" s="149"/>
+      <c r="G59" s="75"/>
+      <c r="H59" s="82"/>
+      <c r="I59" s="76"/>
+      <c r="J59" s="74"/>
+    </row>
+    <row r="60" spans="1:10" s="4" customFormat="1" ht="160.5" customHeight="1" outlineLevel="1">
+      <c r="A60" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="B58" s="92" t="s">
+      <c r="B60" s="92" t="s">
         <v>297</v>
       </c>
-      <c r="C58" s="76" t="s">
+      <c r="C60" s="76" t="s">
         <v>300</v>
       </c>
-      <c r="D58" s="132"/>
-      <c r="E58" s="133"/>
-      <c r="F58" s="133"/>
-      <c r="G58" s="75"/>
-      <c r="H58" s="82"/>
-      <c r="I58" s="76"/>
-      <c r="J58" s="74"/>
-    </row>
-    <row r="59" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A59" s="134" t="s">
-        <v>286</v>
-      </c>
-      <c r="B59" s="135"/>
-      <c r="C59" s="135"/>
-      <c r="D59" s="97"/>
-      <c r="E59" s="97"/>
-      <c r="F59" s="97"/>
-      <c r="G59" s="97"/>
-      <c r="H59" s="97"/>
-      <c r="I59" s="97"/>
-      <c r="J59" s="98"/>
-    </row>
-    <row r="60" spans="1:10" s="4" customFormat="1" ht="136.5" customHeight="1" outlineLevel="1">
-      <c r="A60" s="77" t="s">
-        <v>0</v>
-      </c>
-      <c r="B60" s="92" t="s">
-        <v>287</v>
-      </c>
-      <c r="C60" s="76" t="s">
-        <v>288</v>
-      </c>
-      <c r="D60" s="132"/>
-      <c r="E60" s="133"/>
-      <c r="F60" s="133"/>
+      <c r="D60" s="148"/>
+      <c r="E60" s="149"/>
+      <c r="F60" s="149"/>
       <c r="G60" s="75"/>
       <c r="H60" s="82"/>
       <c r="I60" s="76"/>
       <c r="J60" s="74"/>
     </row>
-    <row r="61" spans="1:10" s="4" customFormat="1" ht="136.5" customHeight="1" outlineLevel="1">
-      <c r="A61" s="77" t="s">
-        <v>1</v>
-      </c>
-      <c r="B61" s="92" t="s">
+    <row r="61" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
+      <c r="A61" s="135" t="s">
+        <v>286</v>
+      </c>
+      <c r="B61" s="136"/>
+      <c r="C61" s="136"/>
+      <c r="D61" s="97"/>
+      <c r="E61" s="97"/>
+      <c r="F61" s="97"/>
+      <c r="G61" s="97"/>
+      <c r="H61" s="97"/>
+      <c r="I61" s="97"/>
+      <c r="J61" s="98"/>
+    </row>
+    <row r="62" spans="1:10" s="4" customFormat="1" ht="136.5" customHeight="1" outlineLevel="1">
+      <c r="A62" s="77" t="s">
+        <v>0</v>
+      </c>
+      <c r="B62" s="92" t="s">
         <v>287</v>
       </c>
-      <c r="C61" s="76" t="s">
-        <v>289</v>
-      </c>
-      <c r="D61" s="132"/>
-      <c r="E61" s="133"/>
-      <c r="F61" s="133"/>
-      <c r="G61" s="75"/>
-      <c r="H61" s="82"/>
-      <c r="I61" s="76"/>
-      <c r="J61" s="74"/>
-    </row>
-    <row r="62" spans="1:10" s="4" customFormat="1" ht="148.5" customHeight="1" outlineLevel="1">
-      <c r="A62" s="77" t="s">
-        <v>2</v>
-      </c>
-      <c r="B62" s="92" t="s">
-        <v>290</v>
-      </c>
       <c r="C62" s="76" t="s">
-        <v>291</v>
-      </c>
-      <c r="D62" s="132"/>
-      <c r="E62" s="133"/>
-      <c r="F62" s="133"/>
+        <v>288</v>
+      </c>
+      <c r="D62" s="148"/>
+      <c r="E62" s="149"/>
+      <c r="F62" s="149"/>
       <c r="G62" s="75"/>
       <c r="H62" s="82"/>
       <c r="I62" s="76"/>
       <c r="J62" s="74"/>
     </row>
-    <row r="63" spans="1:10" s="4" customFormat="1" ht="146.25" customHeight="1" outlineLevel="1">
+    <row r="63" spans="1:10" s="4" customFormat="1" ht="136.5" customHeight="1" outlineLevel="1">
       <c r="A63" s="77" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="B63" s="92" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="C63" s="76" t="s">
-        <v>298</v>
-      </c>
-      <c r="D63" s="132"/>
-      <c r="E63" s="133"/>
-      <c r="F63" s="133"/>
+        <v>289</v>
+      </c>
+      <c r="D63" s="148"/>
+      <c r="E63" s="149"/>
+      <c r="F63" s="149"/>
       <c r="G63" s="75"/>
       <c r="H63" s="82"/>
       <c r="I63" s="76"/>
       <c r="J63" s="74"/>
     </row>
-    <row r="64" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A64" s="134"/>
-      <c r="B64" s="135"/>
-      <c r="C64" s="135"/>
-      <c r="D64" s="97"/>
-      <c r="E64" s="97"/>
-      <c r="F64" s="97"/>
-      <c r="G64" s="97"/>
-      <c r="H64" s="97"/>
-      <c r="I64" s="97"/>
-      <c r="J64" s="98"/>
-    </row>
-    <row r="65" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
-      <c r="A65" s="77"/>
-      <c r="B65" s="92"/>
-      <c r="C65" s="76"/>
-      <c r="D65" s="132"/>
-      <c r="E65" s="133"/>
-      <c r="F65" s="133"/>
+    <row r="64" spans="1:10" s="4" customFormat="1" ht="148.5" customHeight="1" outlineLevel="1">
+      <c r="A64" s="77" t="s">
+        <v>2</v>
+      </c>
+      <c r="B64" s="92" t="s">
+        <v>290</v>
+      </c>
+      <c r="C64" s="76" t="s">
+        <v>291</v>
+      </c>
+      <c r="D64" s="148"/>
+      <c r="E64" s="149"/>
+      <c r="F64" s="149"/>
+      <c r="G64" s="75"/>
+      <c r="H64" s="82"/>
+      <c r="I64" s="76"/>
+      <c r="J64" s="74"/>
+    </row>
+    <row r="65" spans="1:10" s="4" customFormat="1" ht="146.25" customHeight="1" outlineLevel="1">
+      <c r="A65" s="77" t="s">
+        <v>49</v>
+      </c>
+      <c r="B65" s="92" t="s">
+        <v>292</v>
+      </c>
+      <c r="C65" s="76" t="s">
+        <v>298</v>
+      </c>
+      <c r="D65" s="148"/>
+      <c r="E65" s="149"/>
+      <c r="F65" s="149"/>
       <c r="G65" s="75"/>
       <c r="H65" s="82"/>
       <c r="I65" s="76"/>
       <c r="J65" s="74"/>
     </row>
     <row r="66" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A66" s="134"/>
-      <c r="B66" s="135"/>
-      <c r="C66" s="135"/>
+      <c r="A66" s="135"/>
+      <c r="B66" s="136"/>
+      <c r="C66" s="136"/>
       <c r="D66" s="97"/>
       <c r="E66" s="97"/>
       <c r="F66" s="97"/>
@@ -8674,33 +9070,49 @@
       <c r="A67" s="77"/>
       <c r="B67" s="92"/>
       <c r="C67" s="76"/>
-      <c r="D67" s="132"/>
-      <c r="E67" s="133"/>
-      <c r="F67" s="133"/>
+      <c r="D67" s="148"/>
+      <c r="E67" s="149"/>
+      <c r="F67" s="149"/>
       <c r="G67" s="75"/>
       <c r="H67" s="82"/>
       <c r="I67" s="76"/>
       <c r="J67" s="74"/>
     </row>
-    <row r="68" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
-      <c r="A68" s="124"/>
-      <c r="B68" s="125"/>
-      <c r="C68" s="126"/>
-      <c r="D68" s="127"/>
-      <c r="E68" s="127"/>
-      <c r="F68" s="127"/>
-      <c r="G68" s="126"/>
-      <c r="H68" s="126"/>
-      <c r="I68" s="126"/>
-      <c r="J68" s="128"/>
-    </row>
-    <row r="69" spans="1:10" ht="12" customHeight="1">
-      <c r="I69"/>
-      <c r="J69"/>
-    </row>
-    <row r="70" spans="1:10" ht="12" customHeight="1">
-      <c r="I70"/>
-      <c r="J70"/>
+    <row r="68" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
+      <c r="A68" s="135"/>
+      <c r="B68" s="136"/>
+      <c r="C68" s="136"/>
+      <c r="D68" s="97"/>
+      <c r="E68" s="97"/>
+      <c r="F68" s="97"/>
+      <c r="G68" s="97"/>
+      <c r="H68" s="97"/>
+      <c r="I68" s="97"/>
+      <c r="J68" s="98"/>
+    </row>
+    <row r="69" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A69" s="77"/>
+      <c r="B69" s="92"/>
+      <c r="C69" s="76"/>
+      <c r="D69" s="148"/>
+      <c r="E69" s="149"/>
+      <c r="F69" s="149"/>
+      <c r="G69" s="75"/>
+      <c r="H69" s="82"/>
+      <c r="I69" s="76"/>
+      <c r="J69" s="74"/>
+    </row>
+    <row r="70" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A70" s="124"/>
+      <c r="B70" s="125"/>
+      <c r="C70" s="126"/>
+      <c r="D70" s="127"/>
+      <c r="E70" s="127"/>
+      <c r="F70" s="127"/>
+      <c r="G70" s="126"/>
+      <c r="H70" s="126"/>
+      <c r="I70" s="126"/>
+      <c r="J70" s="128"/>
     </row>
     <row r="71" spans="1:10" ht="12" customHeight="1">
       <c r="I71"/>
@@ -8758,12 +9170,12 @@
       <c r="I84"/>
       <c r="J84"/>
     </row>
-    <row r="85" spans="9:10">
-      <c r="I85" s="19"/>
+    <row r="85" spans="9:10" ht="12" customHeight="1">
+      <c r="I85"/>
       <c r="J85"/>
     </row>
-    <row r="86" spans="9:10">
-      <c r="I86" s="19"/>
+    <row r="86" spans="9:10" ht="12" customHeight="1">
+      <c r="I86"/>
       <c r="J86"/>
     </row>
     <row r="87" spans="9:10">
@@ -8822,13 +9234,71 @@
       <c r="I100" s="19"/>
       <c r="J100"/>
     </row>
+    <row r="101" spans="9:10">
+      <c r="I101" s="19"/>
+      <c r="J101"/>
+    </row>
+    <row r="102" spans="9:10">
+      <c r="I102" s="19"/>
+      <c r="J102"/>
+    </row>
   </sheetData>
-  <mergeCells count="74">
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D17:F17"/>
+  <mergeCells count="76">
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="D69:F69"/>
+    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="D64:F64"/>
+    <mergeCell ref="D62:F62"/>
+    <mergeCell ref="D63:F63"/>
+    <mergeCell ref="D60:F60"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="D65:F65"/>
+    <mergeCell ref="A66:C66"/>
+    <mergeCell ref="D67:F67"/>
+    <mergeCell ref="A68:C68"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="D57:F57"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="D54:F54"/>
+    <mergeCell ref="D52:F52"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="D50:F50"/>
+    <mergeCell ref="D56:F56"/>
+    <mergeCell ref="D51:F51"/>
+    <mergeCell ref="B1:D2"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="A37:C37"/>
     <mergeCell ref="D24:F24"/>
@@ -8845,59 +9315,11 @@
     <mergeCell ref="D20:F20"/>
     <mergeCell ref="D18:F18"/>
     <mergeCell ref="D22:F22"/>
-    <mergeCell ref="B1:D2"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="A53:C53"/>
-    <mergeCell ref="D55:F55"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="D52:F52"/>
-    <mergeCell ref="D50:F50"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="D48:F48"/>
-    <mergeCell ref="D54:F54"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="A59:C59"/>
-    <mergeCell ref="D63:F63"/>
-    <mergeCell ref="A64:C64"/>
-    <mergeCell ref="D65:F65"/>
-    <mergeCell ref="A66:C66"/>
-    <mergeCell ref="D67:F67"/>
-    <mergeCell ref="D57:F57"/>
-    <mergeCell ref="D62:F62"/>
-    <mergeCell ref="D60:F60"/>
-    <mergeCell ref="D61:F61"/>
-    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D17:F17"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8914,7 +9336,7 @@
   </sheetPr>
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="82" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="82" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -8934,9 +9356,9 @@
       <c r="A1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
+      <c r="B1" s="153"/>
+      <c r="C1" s="153"/>
+      <c r="D1" s="153"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -8947,9 +9369,9 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="146"/>
-      <c r="C2" s="146"/>
-      <c r="D2" s="146"/>
+      <c r="B2" s="154"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -8970,43 +9392,43 @@
       <c r="E3" s="60"/>
       <c r="F3" s="60"/>
       <c r="G3" s="60"/>
-      <c r="H3" s="155"/>
-      <c r="I3" s="155"/>
-      <c r="J3" s="155"/>
+      <c r="H3" s="161"/>
+      <c r="I3" s="161"/>
+      <c r="J3" s="161"/>
       <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="12.75">
       <c r="A4" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="157" t="s">
+      <c r="B4" s="162" t="s">
         <v>119</v>
       </c>
-      <c r="C4" s="158"/>
-      <c r="D4" s="159"/>
+      <c r="C4" s="163"/>
+      <c r="D4" s="164"/>
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
       <c r="G4" s="60"/>
-      <c r="H4" s="155"/>
-      <c r="I4" s="155"/>
-      <c r="J4" s="155"/>
+      <c r="H4" s="161"/>
+      <c r="I4" s="161"/>
+      <c r="J4" s="161"/>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" s="70" customFormat="1" ht="25.5">
       <c r="A5" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="148" t="s">
+      <c r="B5" s="156" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="149"/>
-      <c r="D5" s="150"/>
+      <c r="C5" s="157"/>
+      <c r="D5" s="158"/>
       <c r="E5" s="68"/>
       <c r="F5" s="68"/>
       <c r="G5" s="68"/>
-      <c r="H5" s="154"/>
-      <c r="I5" s="154"/>
-      <c r="J5" s="154"/>
+      <c r="H5" s="160"/>
+      <c r="I5" s="160"/>
+      <c r="J5" s="160"/>
       <c r="K5" s="69"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
@@ -9027,9 +9449,9 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="155"/>
-      <c r="I6" s="155"/>
-      <c r="J6" s="155"/>
+      <c r="H6" s="161"/>
+      <c r="I6" s="161"/>
+      <c r="J6" s="161"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -9050,16 +9472,16 @@
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
       <c r="G7" s="61"/>
-      <c r="H7" s="155"/>
-      <c r="I7" s="155"/>
-      <c r="J7" s="155"/>
+      <c r="H7" s="161"/>
+      <c r="I7" s="161"/>
+      <c r="J7" s="161"/>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="147"/>
-      <c r="B8" s="147"/>
-      <c r="C8" s="147"/>
-      <c r="D8" s="147"/>
+      <c r="A8" s="155"/>
+      <c r="B8" s="155"/>
+      <c r="C8" s="155"/>
+      <c r="D8" s="155"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -9069,70 +9491,70 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" s="72" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="164" t="s">
+      <c r="A9" s="139" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="165" t="s">
+      <c r="B9" s="168" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="164" t="s">
+      <c r="C9" s="139" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="169" t="s">
+      <c r="D9" s="140" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="170"/>
-      <c r="F9" s="170"/>
-      <c r="G9" s="171"/>
-      <c r="H9" s="160" t="s">
+      <c r="E9" s="141"/>
+      <c r="F9" s="141"/>
+      <c r="G9" s="142"/>
+      <c r="H9" s="165" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="156" t="s">
+      <c r="I9" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="156" t="s">
+      <c r="J9" s="134" t="s">
         <v>32</v>
       </c>
       <c r="K9" s="71"/>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="156"/>
-      <c r="B10" s="166"/>
-      <c r="C10" s="156"/>
-      <c r="D10" s="161"/>
-      <c r="E10" s="172"/>
-      <c r="F10" s="172"/>
-      <c r="G10" s="173"/>
-      <c r="H10" s="161"/>
-      <c r="I10" s="156"/>
-      <c r="J10" s="156"/>
+      <c r="A10" s="134"/>
+      <c r="B10" s="169"/>
+      <c r="C10" s="134"/>
+      <c r="D10" s="143"/>
+      <c r="E10" s="144"/>
+      <c r="F10" s="144"/>
+      <c r="G10" s="145"/>
+      <c r="H10" s="143"/>
+      <c r="I10" s="134"/>
+      <c r="J10" s="134"/>
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" s="73" customFormat="1" ht="15">
-      <c r="A11" s="162"/>
-      <c r="B11" s="162"/>
-      <c r="C11" s="162"/>
-      <c r="D11" s="162"/>
-      <c r="E11" s="162"/>
-      <c r="F11" s="162"/>
-      <c r="G11" s="162"/>
-      <c r="H11" s="162"/>
-      <c r="I11" s="162"/>
-      <c r="J11" s="163"/>
+      <c r="A11" s="166"/>
+      <c r="B11" s="166"/>
+      <c r="C11" s="166"/>
+      <c r="D11" s="166"/>
+      <c r="E11" s="166"/>
+      <c r="F11" s="166"/>
+      <c r="G11" s="166"/>
+      <c r="H11" s="166"/>
+      <c r="I11" s="166"/>
+      <c r="J11" s="167"/>
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A12" s="151" t="s">
+      <c r="A12" s="146" t="s">
         <v>120</v>
       </c>
-      <c r="B12" s="152"/>
-      <c r="C12" s="152"/>
-      <c r="D12" s="152"/>
-      <c r="E12" s="152"/>
-      <c r="F12" s="152"/>
-      <c r="G12" s="152"/>
-      <c r="H12" s="152"/>
-      <c r="I12" s="152"/>
-      <c r="J12" s="153"/>
+      <c r="B12" s="147"/>
+      <c r="C12" s="147"/>
+      <c r="D12" s="147"/>
+      <c r="E12" s="147"/>
+      <c r="F12" s="147"/>
+      <c r="G12" s="147"/>
+      <c r="H12" s="147"/>
+      <c r="I12" s="147"/>
+      <c r="J12" s="159"/>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" ht="102.75" customHeight="1" outlineLevel="1">
       <c r="A13" s="77" t="s">
@@ -9144,11 +9566,11 @@
       <c r="C13" s="76" t="s">
         <v>158</v>
       </c>
-      <c r="D13" s="139" t="s">
+      <c r="D13" s="132" t="s">
         <v>159</v>
       </c>
-      <c r="E13" s="140"/>
-      <c r="F13" s="140"/>
+      <c r="E13" s="133"/>
+      <c r="F13" s="133"/>
       <c r="G13" s="75"/>
       <c r="H13" s="89"/>
       <c r="I13" s="76"/>
@@ -9164,11 +9586,11 @@
       <c r="C14" s="76" t="s">
         <v>162</v>
       </c>
-      <c r="D14" s="139" t="s">
+      <c r="D14" s="132" t="s">
         <v>163</v>
       </c>
-      <c r="E14" s="140"/>
-      <c r="F14" s="140"/>
+      <c r="E14" s="133"/>
+      <c r="F14" s="133"/>
       <c r="G14" s="75"/>
       <c r="H14" s="89"/>
       <c r="I14" s="76"/>
@@ -9184,22 +9606,22 @@
       <c r="C15" s="76" t="s">
         <v>165</v>
       </c>
-      <c r="D15" s="139" t="s">
+      <c r="D15" s="132" t="s">
         <v>166</v>
       </c>
-      <c r="E15" s="140"/>
-      <c r="F15" s="140"/>
+      <c r="E15" s="133"/>
+      <c r="F15" s="133"/>
       <c r="G15" s="75"/>
       <c r="H15" s="89"/>
       <c r="I15" s="76"/>
       <c r="J15" s="74"/>
     </row>
     <row r="16" spans="1:11" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A16" s="151" t="s">
+      <c r="A16" s="146" t="s">
         <v>121</v>
       </c>
-      <c r="B16" s="152"/>
-      <c r="C16" s="152"/>
+      <c r="B16" s="147"/>
+      <c r="C16" s="147"/>
       <c r="D16" s="87"/>
       <c r="E16" s="87"/>
       <c r="F16" s="87"/>
@@ -9269,11 +9691,11 @@
       <c r="J19" s="96"/>
     </row>
     <row r="20" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A20" s="151" t="s">
+      <c r="A20" s="146" t="s">
         <v>138</v>
       </c>
-      <c r="B20" s="152"/>
-      <c r="C20" s="152"/>
+      <c r="B20" s="147"/>
+      <c r="C20" s="147"/>
       <c r="D20" s="87"/>
       <c r="E20" s="87"/>
       <c r="F20" s="87"/>
@@ -9292,11 +9714,11 @@
       <c r="C21" s="76" t="s">
         <v>142</v>
       </c>
-      <c r="D21" s="139" t="s">
+      <c r="D21" s="132" t="s">
         <v>140</v>
       </c>
-      <c r="E21" s="140"/>
-      <c r="F21" s="140"/>
+      <c r="E21" s="133"/>
+      <c r="F21" s="133"/>
       <c r="G21" s="75"/>
       <c r="H21" s="82"/>
       <c r="I21" s="76"/>
@@ -9312,11 +9734,11 @@
       <c r="C22" s="76" t="s">
         <v>143</v>
       </c>
-      <c r="D22" s="139" t="s">
+      <c r="D22" s="132" t="s">
         <v>144</v>
       </c>
-      <c r="E22" s="140"/>
-      <c r="F22" s="140"/>
+      <c r="E22" s="133"/>
+      <c r="F22" s="133"/>
       <c r="G22" s="75"/>
       <c r="H22" s="82"/>
       <c r="I22" s="76"/>
@@ -9332,11 +9754,11 @@
       <c r="C23" s="76" t="s">
         <v>146</v>
       </c>
-      <c r="D23" s="139" t="s">
+      <c r="D23" s="132" t="s">
         <v>147</v>
       </c>
-      <c r="E23" s="140"/>
-      <c r="F23" s="140"/>
+      <c r="E23" s="133"/>
+      <c r="F23" s="133"/>
       <c r="G23" s="75"/>
       <c r="H23" s="82"/>
       <c r="I23" s="76"/>
@@ -9352,20 +9774,20 @@
       <c r="C24" s="76" t="s">
         <v>149</v>
       </c>
-      <c r="D24" s="139" t="s">
+      <c r="D24" s="132" t="s">
         <v>150</v>
       </c>
-      <c r="E24" s="140"/>
-      <c r="F24" s="140"/>
+      <c r="E24" s="133"/>
+      <c r="F24" s="133"/>
       <c r="G24" s="75"/>
       <c r="H24" s="82"/>
       <c r="I24" s="76"/>
       <c r="J24" s="74"/>
     </row>
     <row r="25" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A25" s="134"/>
-      <c r="B25" s="135"/>
-      <c r="C25" s="135"/>
+      <c r="A25" s="135"/>
+      <c r="B25" s="136"/>
+      <c r="C25" s="136"/>
       <c r="D25" s="97"/>
       <c r="E25" s="97"/>
       <c r="F25" s="97"/>
@@ -9378,9 +9800,9 @@
       <c r="A26" s="77"/>
       <c r="B26" s="92"/>
       <c r="C26" s="76"/>
-      <c r="D26" s="132"/>
-      <c r="E26" s="133"/>
-      <c r="F26" s="133"/>
+      <c r="D26" s="148"/>
+      <c r="E26" s="149"/>
+      <c r="F26" s="149"/>
       <c r="G26" s="75"/>
       <c r="H26" s="82"/>
       <c r="I26" s="76"/>
@@ -9390,9 +9812,9 @@
       <c r="A27" s="77"/>
       <c r="B27" s="92"/>
       <c r="C27" s="76"/>
-      <c r="D27" s="132"/>
-      <c r="E27" s="133"/>
-      <c r="F27" s="133"/>
+      <c r="D27" s="148"/>
+      <c r="E27" s="149"/>
+      <c r="F27" s="149"/>
       <c r="G27" s="75"/>
       <c r="H27" s="82"/>
       <c r="I27" s="76"/>
@@ -9402,9 +9824,9 @@
       <c r="A28" s="77"/>
       <c r="B28" s="92"/>
       <c r="C28" s="76"/>
-      <c r="D28" s="132"/>
-      <c r="E28" s="133"/>
-      <c r="F28" s="133"/>
+      <c r="D28" s="148"/>
+      <c r="E28" s="149"/>
+      <c r="F28" s="149"/>
       <c r="G28" s="75"/>
       <c r="H28" s="82"/>
       <c r="I28" s="76"/>
@@ -9414,9 +9836,9 @@
       <c r="A29" s="77"/>
       <c r="B29" s="92"/>
       <c r="C29" s="76"/>
-      <c r="D29" s="132"/>
-      <c r="E29" s="133"/>
-      <c r="F29" s="133"/>
+      <c r="D29" s="148"/>
+      <c r="E29" s="149"/>
+      <c r="F29" s="149"/>
       <c r="G29" s="75"/>
       <c r="H29" s="82"/>
       <c r="I29" s="76"/>
@@ -9426,9 +9848,9 @@
       <c r="A30" s="77"/>
       <c r="B30" s="92"/>
       <c r="C30" s="76"/>
-      <c r="D30" s="132"/>
-      <c r="E30" s="133"/>
-      <c r="F30" s="133"/>
+      <c r="D30" s="148"/>
+      <c r="E30" s="149"/>
+      <c r="F30" s="149"/>
       <c r="G30" s="75"/>
       <c r="H30" s="82"/>
       <c r="I30" s="76"/>
@@ -9438,18 +9860,18 @@
       <c r="A31" s="77"/>
       <c r="B31" s="92"/>
       <c r="C31" s="76"/>
-      <c r="D31" s="132"/>
-      <c r="E31" s="133"/>
-      <c r="F31" s="133"/>
+      <c r="D31" s="148"/>
+      <c r="E31" s="149"/>
+      <c r="F31" s="149"/>
       <c r="G31" s="75"/>
       <c r="H31" s="82"/>
       <c r="I31" s="76"/>
       <c r="J31" s="74"/>
     </row>
     <row r="32" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A32" s="134"/>
-      <c r="B32" s="135"/>
-      <c r="C32" s="135"/>
+      <c r="A32" s="135"/>
+      <c r="B32" s="136"/>
+      <c r="C32" s="136"/>
       <c r="D32" s="97"/>
       <c r="E32" s="97"/>
       <c r="F32" s="97"/>
@@ -9462,9 +9884,9 @@
       <c r="A33" s="77"/>
       <c r="B33" s="92"/>
       <c r="C33" s="76"/>
-      <c r="D33" s="132"/>
-      <c r="E33" s="133"/>
-      <c r="F33" s="133"/>
+      <c r="D33" s="148"/>
+      <c r="E33" s="149"/>
+      <c r="F33" s="149"/>
       <c r="G33" s="75"/>
       <c r="H33" s="82"/>
       <c r="I33" s="76"/>
@@ -9600,6 +10022,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:G10"/>
     <mergeCell ref="D19:F19"/>
     <mergeCell ref="B1:D2"/>
     <mergeCell ref="B3:D3"/>
@@ -9616,30 +10062,6 @@
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="H6:J6"/>
     <mergeCell ref="H7:J7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -9654,7 +10076,7 @@
   </sheetPr>
   <dimension ref="A1:K67"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="80" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="80" workbookViewId="0">
       <selection activeCell="D21" sqref="D21:F21"/>
     </sheetView>
   </sheetViews>
@@ -9674,9 +10096,9 @@
       <c r="A1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
+      <c r="B1" s="153"/>
+      <c r="C1" s="153"/>
+      <c r="D1" s="153"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -9687,9 +10109,9 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="146"/>
-      <c r="C2" s="146"/>
-      <c r="D2" s="146"/>
+      <c r="B2" s="154"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -9710,43 +10132,43 @@
       <c r="E3" s="60"/>
       <c r="F3" s="60"/>
       <c r="G3" s="60"/>
-      <c r="H3" s="155"/>
-      <c r="I3" s="155"/>
-      <c r="J3" s="155"/>
+      <c r="H3" s="161"/>
+      <c r="I3" s="161"/>
+      <c r="J3" s="161"/>
       <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="12.75">
       <c r="A4" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="157" t="s">
+      <c r="B4" s="162" t="s">
         <v>241</v>
       </c>
-      <c r="C4" s="158"/>
-      <c r="D4" s="159"/>
+      <c r="C4" s="163"/>
+      <c r="D4" s="164"/>
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
       <c r="G4" s="60"/>
-      <c r="H4" s="155"/>
-      <c r="I4" s="155"/>
-      <c r="J4" s="155"/>
+      <c r="H4" s="161"/>
+      <c r="I4" s="161"/>
+      <c r="J4" s="161"/>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" s="70" customFormat="1" ht="25.5">
       <c r="A5" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="148" t="s">
+      <c r="B5" s="156" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="149"/>
-      <c r="D5" s="150"/>
+      <c r="C5" s="157"/>
+      <c r="D5" s="158"/>
       <c r="E5" s="68"/>
       <c r="F5" s="68"/>
       <c r="G5" s="68"/>
-      <c r="H5" s="154"/>
-      <c r="I5" s="154"/>
-      <c r="J5" s="154"/>
+      <c r="H5" s="160"/>
+      <c r="I5" s="160"/>
+      <c r="J5" s="160"/>
       <c r="K5" s="69"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
@@ -9767,9 +10189,9 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="155"/>
-      <c r="I6" s="155"/>
-      <c r="J6" s="155"/>
+      <c r="H6" s="161"/>
+      <c r="I6" s="161"/>
+      <c r="J6" s="161"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -9790,16 +10212,16 @@
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
       <c r="G7" s="61"/>
-      <c r="H7" s="155"/>
-      <c r="I7" s="155"/>
-      <c r="J7" s="155"/>
+      <c r="H7" s="161"/>
+      <c r="I7" s="161"/>
+      <c r="J7" s="161"/>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="147"/>
-      <c r="B8" s="147"/>
-      <c r="C8" s="147"/>
-      <c r="D8" s="147"/>
+      <c r="A8" s="155"/>
+      <c r="B8" s="155"/>
+      <c r="C8" s="155"/>
+      <c r="D8" s="155"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -9809,70 +10231,70 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" s="72" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="164" t="s">
+      <c r="A9" s="139" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="165" t="s">
+      <c r="B9" s="168" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="164" t="s">
+      <c r="C9" s="139" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="169" t="s">
+      <c r="D9" s="140" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="170"/>
-      <c r="F9" s="170"/>
-      <c r="G9" s="171"/>
-      <c r="H9" s="160" t="s">
+      <c r="E9" s="141"/>
+      <c r="F9" s="141"/>
+      <c r="G9" s="142"/>
+      <c r="H9" s="165" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="156" t="s">
+      <c r="I9" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="156" t="s">
+      <c r="J9" s="134" t="s">
         <v>32</v>
       </c>
       <c r="K9" s="71"/>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="156"/>
-      <c r="B10" s="166"/>
-      <c r="C10" s="156"/>
-      <c r="D10" s="161"/>
-      <c r="E10" s="172"/>
-      <c r="F10" s="172"/>
-      <c r="G10" s="173"/>
-      <c r="H10" s="161"/>
-      <c r="I10" s="156"/>
-      <c r="J10" s="156"/>
+      <c r="A10" s="134"/>
+      <c r="B10" s="169"/>
+      <c r="C10" s="134"/>
+      <c r="D10" s="143"/>
+      <c r="E10" s="144"/>
+      <c r="F10" s="144"/>
+      <c r="G10" s="145"/>
+      <c r="H10" s="143"/>
+      <c r="I10" s="134"/>
+      <c r="J10" s="134"/>
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" s="73" customFormat="1" ht="15">
-      <c r="A11" s="162"/>
-      <c r="B11" s="162"/>
-      <c r="C11" s="162"/>
-      <c r="D11" s="162"/>
-      <c r="E11" s="162"/>
-      <c r="F11" s="162"/>
-      <c r="G11" s="162"/>
-      <c r="H11" s="162"/>
-      <c r="I11" s="162"/>
-      <c r="J11" s="163"/>
+      <c r="A11" s="166"/>
+      <c r="B11" s="166"/>
+      <c r="C11" s="166"/>
+      <c r="D11" s="166"/>
+      <c r="E11" s="166"/>
+      <c r="F11" s="166"/>
+      <c r="G11" s="166"/>
+      <c r="H11" s="166"/>
+      <c r="I11" s="166"/>
+      <c r="J11" s="167"/>
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A12" s="151" t="s">
+      <c r="A12" s="146" t="s">
         <v>271</v>
       </c>
-      <c r="B12" s="152"/>
-      <c r="C12" s="152"/>
-      <c r="D12" s="152"/>
-      <c r="E12" s="152"/>
-      <c r="F12" s="152"/>
-      <c r="G12" s="152"/>
-      <c r="H12" s="152"/>
-      <c r="I12" s="152"/>
-      <c r="J12" s="153"/>
+      <c r="B12" s="147"/>
+      <c r="C12" s="147"/>
+      <c r="D12" s="147"/>
+      <c r="E12" s="147"/>
+      <c r="F12" s="147"/>
+      <c r="G12" s="147"/>
+      <c r="H12" s="147"/>
+      <c r="I12" s="147"/>
+      <c r="J12" s="159"/>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" ht="132.75" customHeight="1" outlineLevel="1">
       <c r="A13" s="77" t="s">
@@ -9884,9 +10306,9 @@
       <c r="C13" s="122" t="s">
         <v>244</v>
       </c>
-      <c r="D13" s="139"/>
-      <c r="E13" s="140"/>
-      <c r="F13" s="140"/>
+      <c r="D13" s="132"/>
+      <c r="E13" s="133"/>
+      <c r="F13" s="133"/>
       <c r="G13" s="75"/>
       <c r="H13" s="89"/>
       <c r="I13" s="76"/>
@@ -9902,9 +10324,9 @@
       <c r="C14" s="122" t="s">
         <v>245</v>
       </c>
-      <c r="D14" s="139"/>
-      <c r="E14" s="140"/>
-      <c r="F14" s="140"/>
+      <c r="D14" s="132"/>
+      <c r="E14" s="133"/>
+      <c r="F14" s="133"/>
       <c r="G14" s="75"/>
       <c r="H14" s="89"/>
       <c r="I14" s="76"/>
@@ -9920,20 +10342,20 @@
       <c r="C15" s="76" t="s">
         <v>253</v>
       </c>
-      <c r="D15" s="139"/>
-      <c r="E15" s="140"/>
-      <c r="F15" s="140"/>
+      <c r="D15" s="132"/>
+      <c r="E15" s="133"/>
+      <c r="F15" s="133"/>
       <c r="G15" s="75"/>
       <c r="H15" s="89"/>
       <c r="I15" s="76"/>
       <c r="J15" s="74"/>
     </row>
     <row r="16" spans="1:11" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A16" s="151" t="s">
+      <c r="A16" s="146" t="s">
         <v>272</v>
       </c>
-      <c r="B16" s="152"/>
-      <c r="C16" s="152"/>
+      <c r="B16" s="147"/>
+      <c r="C16" s="147"/>
       <c r="D16" s="87"/>
       <c r="E16" s="87"/>
       <c r="F16" s="87"/>
@@ -10033,11 +10455,11 @@
       <c r="J21" s="96"/>
     </row>
     <row r="22" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A22" s="151" t="s">
+      <c r="A22" s="146" t="s">
         <v>248</v>
       </c>
-      <c r="B22" s="152"/>
-      <c r="C22" s="152"/>
+      <c r="B22" s="147"/>
+      <c r="C22" s="147"/>
       <c r="D22" s="87"/>
       <c r="E22" s="87"/>
       <c r="F22" s="87"/>
@@ -10056,9 +10478,9 @@
       <c r="C23" s="76" t="s">
         <v>251</v>
       </c>
-      <c r="D23" s="139"/>
-      <c r="E23" s="140"/>
-      <c r="F23" s="140"/>
+      <c r="D23" s="132"/>
+      <c r="E23" s="133"/>
+      <c r="F23" s="133"/>
       <c r="G23" s="75"/>
       <c r="H23" s="82"/>
       <c r="I23" s="76"/>
@@ -10074,9 +10496,9 @@
       <c r="C24" s="76" t="s">
         <v>253</v>
       </c>
-      <c r="D24" s="139"/>
-      <c r="E24" s="140"/>
-      <c r="F24" s="140"/>
+      <c r="D24" s="132"/>
+      <c r="E24" s="133"/>
+      <c r="F24" s="133"/>
       <c r="G24" s="75"/>
       <c r="H24" s="82"/>
       <c r="I24" s="76"/>
@@ -10092,9 +10514,9 @@
       <c r="C25" s="76" t="s">
         <v>262</v>
       </c>
-      <c r="D25" s="139"/>
-      <c r="E25" s="140"/>
-      <c r="F25" s="140"/>
+      <c r="D25" s="132"/>
+      <c r="E25" s="133"/>
+      <c r="F25" s="133"/>
       <c r="G25" s="75"/>
       <c r="H25" s="82"/>
       <c r="I25" s="76"/>
@@ -10110,18 +10532,18 @@
       <c r="C26" s="76" t="s">
         <v>259</v>
       </c>
-      <c r="D26" s="139"/>
-      <c r="E26" s="140"/>
-      <c r="F26" s="140"/>
+      <c r="D26" s="132"/>
+      <c r="E26" s="133"/>
+      <c r="F26" s="133"/>
       <c r="G26" s="75"/>
       <c r="H26" s="82"/>
       <c r="I26" s="76"/>
       <c r="J26" s="74"/>
     </row>
     <row r="27" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A27" s="134"/>
-      <c r="B27" s="135"/>
-      <c r="C27" s="135"/>
+      <c r="A27" s="135"/>
+      <c r="B27" s="136"/>
+      <c r="C27" s="136"/>
       <c r="D27" s="97"/>
       <c r="E27" s="97"/>
       <c r="F27" s="97"/>
@@ -10134,9 +10556,9 @@
       <c r="A28" s="77"/>
       <c r="B28" s="92"/>
       <c r="C28" s="76"/>
-      <c r="D28" s="132"/>
-      <c r="E28" s="133"/>
-      <c r="F28" s="133"/>
+      <c r="D28" s="148"/>
+      <c r="E28" s="149"/>
+      <c r="F28" s="149"/>
       <c r="G28" s="75"/>
       <c r="H28" s="82"/>
       <c r="I28" s="76"/>
@@ -10146,9 +10568,9 @@
       <c r="A29" s="77"/>
       <c r="B29" s="92"/>
       <c r="C29" s="76"/>
-      <c r="D29" s="132"/>
-      <c r="E29" s="133"/>
-      <c r="F29" s="133"/>
+      <c r="D29" s="148"/>
+      <c r="E29" s="149"/>
+      <c r="F29" s="149"/>
       <c r="G29" s="75"/>
       <c r="H29" s="82"/>
       <c r="I29" s="76"/>
@@ -10158,9 +10580,9 @@
       <c r="A30" s="77"/>
       <c r="B30" s="92"/>
       <c r="C30" s="76"/>
-      <c r="D30" s="132"/>
-      <c r="E30" s="133"/>
-      <c r="F30" s="133"/>
+      <c r="D30" s="148"/>
+      <c r="E30" s="149"/>
+      <c r="F30" s="149"/>
       <c r="G30" s="75"/>
       <c r="H30" s="82"/>
       <c r="I30" s="76"/>
@@ -10170,9 +10592,9 @@
       <c r="A31" s="77"/>
       <c r="B31" s="92"/>
       <c r="C31" s="76"/>
-      <c r="D31" s="132"/>
-      <c r="E31" s="133"/>
-      <c r="F31" s="133"/>
+      <c r="D31" s="148"/>
+      <c r="E31" s="149"/>
+      <c r="F31" s="149"/>
       <c r="G31" s="75"/>
       <c r="H31" s="82"/>
       <c r="I31" s="76"/>
@@ -10182,9 +10604,9 @@
       <c r="A32" s="77"/>
       <c r="B32" s="92"/>
       <c r="C32" s="76"/>
-      <c r="D32" s="132"/>
-      <c r="E32" s="133"/>
-      <c r="F32" s="133"/>
+      <c r="D32" s="148"/>
+      <c r="E32" s="149"/>
+      <c r="F32" s="149"/>
       <c r="G32" s="75"/>
       <c r="H32" s="82"/>
       <c r="I32" s="76"/>
@@ -10194,18 +10616,18 @@
       <c r="A33" s="77"/>
       <c r="B33" s="92"/>
       <c r="C33" s="76"/>
-      <c r="D33" s="132"/>
-      <c r="E33" s="133"/>
-      <c r="F33" s="133"/>
+      <c r="D33" s="148"/>
+      <c r="E33" s="149"/>
+      <c r="F33" s="149"/>
       <c r="G33" s="75"/>
       <c r="H33" s="82"/>
       <c r="I33" s="76"/>
       <c r="J33" s="74"/>
     </row>
     <row r="34" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A34" s="134"/>
-      <c r="B34" s="135"/>
-      <c r="C34" s="135"/>
+      <c r="A34" s="135"/>
+      <c r="B34" s="136"/>
+      <c r="C34" s="136"/>
       <c r="D34" s="97"/>
       <c r="E34" s="97"/>
       <c r="F34" s="97"/>
@@ -10218,9 +10640,9 @@
       <c r="A35" s="77"/>
       <c r="B35" s="92"/>
       <c r="C35" s="76"/>
-      <c r="D35" s="132"/>
-      <c r="E35" s="133"/>
-      <c r="F35" s="133"/>
+      <c r="D35" s="148"/>
+      <c r="E35" s="149"/>
+      <c r="F35" s="149"/>
       <c r="G35" s="75"/>
       <c r="H35" s="82"/>
       <c r="I35" s="76"/>
@@ -10356,6 +10778,32 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="D13:F13"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="D14:F14"/>
@@ -10372,32 +10820,6 @@
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:G10"/>
     <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="D21:F21"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -10511,7 +10933,7 @@
       </c>
       <c r="D8" s="66">
         <f>Samples!B6</f>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E8" s="65">
         <f>Samples!B7</f>
@@ -10523,7 +10945,7 @@
       </c>
       <c r="G8" s="66">
         <f>Samples!D7</f>
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="59" customFormat="1" ht="14.25">
@@ -10586,7 +11008,7 @@
       </c>
       <c r="D11" s="53">
         <f>SUM(D6:D10)</f>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E11" s="53">
         <f>SUM(E6:E10)</f>
@@ -10598,7 +11020,7 @@
       </c>
       <c r="G11" s="54">
         <f>SUM(G6:G10)</f>
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14.25">
@@ -10619,7 +11041,7 @@
       <c r="D13" s="19"/>
       <c r="E13" s="23">
         <f>(D11+E11)*100/G11</f>
-        <v>44.615384615384613</v>
+        <v>46.268656716417908</v>
       </c>
       <c r="F13" s="19" t="s">
         <v>22</v>
@@ -10635,7 +11057,7 @@
       <c r="D14" s="19"/>
       <c r="E14" s="23">
         <f>D11*100/G11</f>
-        <v>32.307692307692307</v>
+        <v>34.328358208955223</v>
       </c>
       <c r="F14" s="19" t="s">
         <v>22</v>

</xml_diff>